<commit_message>
Implemented basic version of the EuTaxonomy Assurance FormField for the new dev-tools.
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/euTaxonomyNonFinancials/EutaxonomyNonFinancials.xlsx
+++ b/dataland-framework-toolbox/inputs/euTaxonomyNonFinancials/EutaxonomyNonFinancials.xlsx
@@ -1,67 +1,51 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d92928\Documents\Projects\Dataland\Dataland\dataland-framework-toolbox\inputs\euTaxonomyNonFinancials\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAFE234B-272E-494C-9ABE-ABAE40182351}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{F6C97AD1-BE88-460E-8FB2-9D06955DFA3F}"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Framework Data Model" sheetId="1" r:id="rId1"/>
+    <sheet name="Framework Data Model" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="IQ_CH">110000</definedName>
-    <definedName name="IQ_CQ">5000</definedName>
-    <definedName name="IQ_CY">10000</definedName>
-    <definedName name="IQ_DAILY">500000</definedName>
-    <definedName name="IQ_DNTM" hidden="1">700000</definedName>
-    <definedName name="IQ_FH">100000</definedName>
-    <definedName name="IQ_FQ">500</definedName>
-    <definedName name="IQ_FWD_CY" hidden="1">10001</definedName>
-    <definedName name="IQ_FWD_CY1" hidden="1">10002</definedName>
-    <definedName name="IQ_FWD_CY2" hidden="1">10003</definedName>
-    <definedName name="IQ_FWD_FY" hidden="1">1001</definedName>
-    <definedName name="IQ_FWD_FY1" hidden="1">1002</definedName>
-    <definedName name="IQ_FWD_FY2" hidden="1">1003</definedName>
-    <definedName name="IQ_FWD_Q" hidden="1">501</definedName>
-    <definedName name="IQ_FWD_Q1" hidden="1">502</definedName>
-    <definedName name="IQ_FWD_Q2" hidden="1">503</definedName>
-    <definedName name="IQ_FY">1000</definedName>
-    <definedName name="IQ_LATESTK" hidden="1">1000</definedName>
-    <definedName name="IQ_LATESTQ" hidden="1">500</definedName>
-    <definedName name="IQ_LTM">2000</definedName>
-    <definedName name="IQ_LTMMONTH" hidden="1">120000</definedName>
-    <definedName name="IQ_MONTH">15000</definedName>
-    <definedName name="IQ_MTD" hidden="1">800000</definedName>
-    <definedName name="IQ_NAMES_REVISION_DATE_" hidden="1">"08/31/2022 13:06:56"</definedName>
-    <definedName name="IQ_NTM">6000</definedName>
-    <definedName name="IQ_QTD" hidden="1">750000</definedName>
-    <definedName name="IQ_TODAY" hidden="1">0</definedName>
-    <definedName name="IQ_WEEK">50000</definedName>
-    <definedName name="IQ_YTD">3000</definedName>
-    <definedName name="IQ_YTDMONTH" hidden="1">130000</definedName>
+    <definedName function="false" hidden="false" name="IQ_CH" vbProcedure="false">110000</definedName>
+    <definedName function="false" hidden="false" name="IQ_CQ" vbProcedure="false">5000</definedName>
+    <definedName function="false" hidden="false" name="IQ_CY" vbProcedure="false">10000</definedName>
+    <definedName function="false" hidden="false" name="IQ_DAILY" vbProcedure="false">500000</definedName>
+    <definedName function="false" hidden="false" name="IQ_DNTM" vbProcedure="false">700000</definedName>
+    <definedName function="false" hidden="false" name="IQ_FH" vbProcedure="false">100000</definedName>
+    <definedName function="false" hidden="false" name="IQ_FQ" vbProcedure="false">500</definedName>
+    <definedName function="false" hidden="false" name="IQ_FWD_CY" vbProcedure="false">10001</definedName>
+    <definedName function="false" hidden="false" name="IQ_FWD_CY1" vbProcedure="false">10002</definedName>
+    <definedName function="false" hidden="false" name="IQ_FWD_CY2" vbProcedure="false">10003</definedName>
+    <definedName function="false" hidden="false" name="IQ_FWD_FY" vbProcedure="false">1001</definedName>
+    <definedName function="false" hidden="false" name="IQ_FWD_FY1" vbProcedure="false">1002</definedName>
+    <definedName function="false" hidden="false" name="IQ_FWD_FY2" vbProcedure="false">1003</definedName>
+    <definedName function="false" hidden="false" name="IQ_FWD_Q" vbProcedure="false">501</definedName>
+    <definedName function="false" hidden="false" name="IQ_FWD_Q1" vbProcedure="false">502</definedName>
+    <definedName function="false" hidden="false" name="IQ_FWD_Q2" vbProcedure="false">503</definedName>
+    <definedName function="false" hidden="false" name="IQ_FY" vbProcedure="false">1000</definedName>
+    <definedName function="false" hidden="false" name="IQ_LATESTK" vbProcedure="false">1000</definedName>
+    <definedName function="false" hidden="false" name="IQ_LATESTQ" vbProcedure="false">500</definedName>
+    <definedName function="false" hidden="false" name="IQ_LTM" vbProcedure="false">2000</definedName>
+    <definedName function="false" hidden="false" name="IQ_LTMMONTH" vbProcedure="false">120000</definedName>
+    <definedName function="false" hidden="false" name="IQ_MONTH" vbProcedure="false">15000</definedName>
+    <definedName function="false" hidden="false" name="IQ_MTD" vbProcedure="false">800000</definedName>
+    <definedName function="false" hidden="false" name="IQ_NAMES_REVISION_DATE_" vbProcedure="false">"08/31/2022 13:06:56"</definedName>
+    <definedName function="false" hidden="false" name="IQ_NTM" vbProcedure="false">6000</definedName>
+    <definedName function="false" hidden="false" name="IQ_QTD" vbProcedure="false">750000</definedName>
+    <definedName function="false" hidden="false" name="IQ_TODAY" vbProcedure="false">0</definedName>
+    <definedName function="false" hidden="false" name="IQ_WEEK" vbProcedure="false">50000</definedName>
+    <definedName function="false" hidden="false" name="IQ_YTD" vbProcedure="false">3000</definedName>
+    <definedName function="false" hidden="false" name="IQ_YTDMONTH" vbProcedure="false">130000</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
   </extLst>
 </workbook>
@@ -70,529 +54,548 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="148">
   <si>
-    <t>Field Identifier</t>
-  </si>
-  <si>
-    <t>Category</t>
-  </si>
-  <si>
-    <t>Sub-Category</t>
-  </si>
-  <si>
-    <t>Field Name</t>
-  </si>
-  <si>
-    <t>Tooltip</t>
-  </si>
-  <si>
-    <t>Component</t>
-  </si>
-  <si>
-    <t>Options</t>
-  </si>
-  <si>
-    <t>Unit</t>
-  </si>
-  <si>
-    <t>Document-Support</t>
-  </si>
-  <si>
-    <t>Dependency</t>
-  </si>
-  <si>
-    <t>Show when value is</t>
-  </si>
-  <si>
-    <t>Mandatory Field</t>
-  </si>
-  <si>
-    <t>Expected value</t>
-  </si>
-  <si>
-    <t>Guidance/Comment</t>
-  </si>
-  <si>
-    <t>Cross-check indicators</t>
-  </si>
-  <si>
-    <t>checks when uploading data</t>
-  </si>
-  <si>
-    <t>Optional/Required</t>
-  </si>
-  <si>
-    <t>API Name</t>
-  </si>
-  <si>
-    <t>Uploading screens</t>
-  </si>
-  <si>
-    <t>Display screens</t>
-  </si>
-  <si>
-    <t>General</t>
-  </si>
-  <si>
-    <t>Reporting period</t>
-  </si>
-  <si>
-    <t>The reporting period the dataset belongs to (e.g. fiscal year).</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t> </t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>YYYY</t>
-  </si>
-  <si>
-    <t>Required</t>
-  </si>
-  <si>
-    <t>+</t>
-  </si>
-  <si>
-    <t>Fiscal Year Deviation</t>
-  </si>
-  <si>
-    <t>Does the fiscal year deviate from the calendar year?</t>
-  </si>
-  <si>
-    <t>Single-Select Radio Button</t>
-  </si>
-  <si>
-    <t>Deviation| No Deviation</t>
-  </si>
-  <si>
-    <t>Text: Deviation or No Deviation</t>
-  </si>
-  <si>
-    <t>Optional</t>
-  </si>
-  <si>
-    <t>Fiscal Year End</t>
-  </si>
-  <si>
-    <t>The date at which the fiscal year ends.</t>
-  </si>
-  <si>
-    <t>YYYY-MM-DD</t>
-  </si>
-  <si>
-    <t>Referenced Reports</t>
-  </si>
-  <si>
-    <t>Please upload all relevant reports for this dataset in the PDF format.</t>
-  </si>
-  <si>
-    <t>Report Preupload</t>
-  </si>
-  <si>
-    <t>Scope Of Entities</t>
-  </si>
-  <si>
-    <t>Are all Group legal entities covered in the reports?</t>
-  </si>
-  <si>
-    <t>Yes/No/NA</t>
-  </si>
-  <si>
-    <t>Simple</t>
-  </si>
-  <si>
-    <t>Text: Yes, No, N/A</t>
+    <t xml:space="preserve">Field Identifier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sub-Category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Field Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tooltip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Component</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Options</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Document-Support</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dependency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Show when value is</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mandatory Field</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expected value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Guidance/Comment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cross-check indicators</t>
+  </si>
+  <si>
+    <t xml:space="preserve">checks when uploading data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Optional/Required</t>
+  </si>
+  <si>
+    <t xml:space="preserve">API Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uploading screens</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Display screens</t>
+  </si>
+  <si>
+    <t xml:space="preserve">General</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reporting period</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The reporting period the dataset belongs to (e.g. fiscal year).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YYYY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Required</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fiscal Year Deviation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Does the fiscal year deviate from the calendar year?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Single-Select Radio Button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deviation| No Deviation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Text: Deviation or No Deviation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Optional</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fiscal Year End</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The date at which the fiscal year ends.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YYYY-MM-DD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Referenced Reports</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please upload all relevant reports for this dataset in the PDF format.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Report Preupload</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scope Of Entities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Are all Group legal entities covered in the reports?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes/No/NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Simple</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Text: Yes, No, N/A</t>
   </si>
   <si>
     <t xml:space="preserve">We expect that in the most cases Value should be "Yes". </t>
   </si>
   <si>
-    <t>EU Taxonomy Activity Level Reporting</t>
-  </si>
-  <si>
-    <t>Activity level disclosure</t>
-  </si>
-  <si>
-    <t>Yes/No</t>
-  </si>
-  <si>
-    <t>Text: Yes or No</t>
-  </si>
-  <si>
-    <t>Number Of Employees</t>
-  </si>
-  <si>
-    <t>Total number of employees (including temporary workers with assignment duration &gt;6 months)</t>
-  </si>
-  <si>
-    <t>Percentage</t>
-  </si>
-  <si>
-    <t>Integer</t>
-  </si>
-  <si>
-    <t>integer, positive</t>
-  </si>
-  <si>
-    <t>NFRD Mandatory</t>
-  </si>
-  <si>
-    <t>Is the NFRD mandatory for your company?</t>
-  </si>
-  <si>
-    <t>Number of employees &gt;=500</t>
-  </si>
-  <si>
-    <t>Assurance</t>
-  </si>
-  <si>
-    <t>Level of assurance of the EU Taxonomy disclosure (Reasonable Assurance, Limited Assurance, None)</t>
-  </si>
-  <si>
-    <t>AssuranceFormField</t>
-  </si>
-  <si>
-    <t>Text: Reasonable Assurance or Limited Assurance or None</t>
-  </si>
-  <si>
-    <t>Revenue</t>
-  </si>
-  <si>
-    <t>Total Revenue</t>
-  </si>
-  <si>
-    <t>Total revenue per annum</t>
-  </si>
-  <si>
-    <t>Number</t>
-  </si>
-  <si>
-    <t>The primary way of aggregating from an economic activity to a company level. Some companies may need to aggregate from asset to economic activity level.</t>
-  </si>
-  <si>
-    <t>a) check with the value of Revenue line from Profit and Loss Consolidated Financial Statement b) check with the value from other source/database (Capital IQ) c) find the same value in the other report of a company (Annual report, Integrated report, Sustainablity report) d) avarage revenue growth for the last 3-5 years in comparison with the reporting period growth (historical revenue for calculation are taken from third-party source/database (Capital IQ)</t>
-  </si>
-  <si>
-    <t>float, allow negative</t>
-  </si>
-  <si>
-    <t>totalAmount</t>
-  </si>
-  <si>
-    <t>Eligible Revenue</t>
-  </si>
-  <si>
-    <t>Absolute value and share of the total eligible revenue in same currency than total revenue. Is part of the total revenue where the economic activity meets taxonomy criteria for substantial contribution to climate change mitigation and does no serious harm to the other environmental objectives (DNSH criteria).</t>
-  </si>
-  <si>
-    <t>Percentage: Numerator - Revenues derived from products and/or services associated with EU taxonomy eligible activities. Denominator- Revenues accounted for in the Consolidated Income Statement under IFRS.</t>
+    <t xml:space="preserve">EU Taxonomy Activity Level Reporting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Activity level disclosure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes/No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Text: Yes or No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number Of Employees</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total number of employees (including temporary workers with assignment duration &gt;6 months)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percentage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Integer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">integer, positive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NFRD Mandatory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is the NFRD mandatory for your company?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of employees &gt;=500</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assurance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Level of assurance of the EU Taxonomy disclosure (Reasonable Assurance, Limited Assurance, None)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Custom – EuTaxonomyAssuranceComponent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Text: Reasonable Assurance or Limited Assurance or None</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Revenue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Revenue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total revenue per annum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The primary way of aggregating from an economic activity to a company level. Some companies may need to aggregate from asset to economic activity level.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a) check with the value of Revenue line from Profit and Loss Consolidated Financial Statement b) check with the value from other source/database (Capital IQ) c) find the same value in the other report of a company (Annual report, Integrated report, Sustainablity report) d) avarage revenue growth for the last 3-5 years in comparison with the reporting period growth (historical revenue for calculation are taken from third-party source/database (Capital IQ)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">float, allow negative</t>
+  </si>
+  <si>
+    <t xml:space="preserve">totalAmount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eligible Revenue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Absolute value and share of the total eligible revenue in same currency than total revenue. Is part of the total revenue where the economic activity meets taxonomy criteria for substantial contribution to climate change mitigation and does no serious harm to the other environmental objectives (DNSH criteria).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percentage: Numerator - Revenues derived from products and/or services associated with EU taxonomy eligible activities. Denominator- Revenues accounted for in the Consolidated Income Statement under IFRS.</t>
   </si>
   <si>
     <t xml:space="preserve">&gt;= Aligned Revenue, &lt;= Total Revenue, for NACE codes listed below eligible revenue (%) &gt;=90%:  C25,C28,C27, C29.1, C30.1, C30.2, C30.9, C33.15, C33.17, D35.11, F42.22, D35.30, E38.11, F42.11, F42.12, F42.13, F43.21, F711, F71.20, F42, F43, M71, C16, C17, C22, C23, C25, M71 </t>
   </si>
   <si>
-    <t>percentage is float, between 0 and 100</t>
-  </si>
-  <si>
-    <t>eligibleShare</t>
-  </si>
-  <si>
-    <t>Aligned Revenue</t>
-  </si>
-  <si>
-    <t>Absolute value and share of the total eligible revenue that is taxonomy-aligned, i.e., generated by an eligible economic activity that is making a substantial contribution to at least one of the climate and environmental objectives, while also doing no significant harm to the remaining objectives and meeting minimum standards on human rights and labour standards. In same currency than total revenue.</t>
-  </si>
-  <si>
-    <t>&lt;= Eligible Revenue, &lt;= Total Revenue, &lt;= Use of Proceeds (Green Bond Principles)</t>
-  </si>
-  <si>
-    <t>alignedShare</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to Climate Change Mitigation</t>
-  </si>
-  <si>
-    <t>Grade of the substantial contribution criterion fulfillment</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to Climate Change Adaptation</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to Sustainable Use and Protection of Water and Marine Resources</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to Transition to a Circular Economy</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to Pollution Prevention and Control</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to Protection and Restoration of Biodiversity and Ecosystems</t>
-  </si>
-  <si>
-    <t>Aligned Revenue per Activity</t>
-  </si>
-  <si>
-    <t>Absolute value and share of the revenue per activity that is taxonomy-aligned, i.e., generated by an eligible economic activity that is making a substantial contribution to at least one of the climate and environmental objectives, while also doing no significant harm to the remaining objectives and meeting minimum standards on human rights and labour standards</t>
-  </si>
-  <si>
-    <t>AlignedActivitiesFormField</t>
-  </si>
-  <si>
-    <t>Extended</t>
-  </si>
-  <si>
-    <t>alignedActivities</t>
-  </si>
-  <si>
-    <t>Non-Aligned Revenue</t>
-  </si>
-  <si>
-    <t>Absolute value and share of the revenue that is associated with non taxonomy-aligned but eligible activities</t>
-  </si>
-  <si>
-    <t>nonAlignedShare</t>
-  </si>
-  <si>
-    <t>Non-Aligned Revenue per Activity</t>
-  </si>
-  <si>
-    <t>Absolute value and share of the revenue per activity that is not taxonomy-aligned but eligible</t>
-  </si>
-  <si>
-    <t>NonAlignedActivitiesFormField</t>
-  </si>
-  <si>
-    <t>nonAlignedActivities</t>
-  </si>
-  <si>
-    <t>Non-Eligible Revenue</t>
-  </si>
-  <si>
-    <t>Absolute value and share of the revenue that is not part of a plan to meet the DNSH criteria and make substantial contribution to any environmental objective</t>
-  </si>
-  <si>
-    <t>nonEligibleShare</t>
-  </si>
-  <si>
-    <t>Enabling Revenue</t>
-  </si>
-  <si>
-    <t>Share of the taxonomy-aligned revenue from total aligned revenue that is linked to activities that enable reduction of GHG in other sectors</t>
-  </si>
-  <si>
-    <t>enablingShareInPercent</t>
-  </si>
-  <si>
-    <t>Transitional Revenue</t>
-  </si>
-  <si>
-    <t>Share of the taxonomy-aligned revenue from total aligned revenue that is linked to activities with significantly lower GHG emissions than the sector or industry average</t>
-  </si>
-  <si>
-    <t>transitionalShareInPercent</t>
-  </si>
-  <si>
-    <t>CapEx</t>
-  </si>
-  <si>
-    <t>Total CapEx</t>
+    <t xml:space="preserve">percentage is float, between 0 and 100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eligibleShare</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aligned Revenue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Absolute value and share of the total eligible revenue that is taxonomy-aligned, i.e., generated by an eligible economic activity that is making a substantial contribution to at least one of the climate and environmental objectives, while also doing no significant harm to the remaining objectives and meeting minimum standards on human rights and labour standards. In same currency than total revenue.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;= Eligible Revenue, &lt;= Total Revenue, &lt;= Use of Proceeds (Green Bond Principles)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">alignedShare</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Substantial Contribution to Climate Change Mitigation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grade of the substantial contribution criterion fulfillment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Substantial Contribution to Climate Change Adaptation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Substantial Contribution to Sustainable Use and Protection of Water and Marine Resources</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Substantial Contribution to Transition to a Circular Economy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Substantial Contribution to Pollution Prevention and Control</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Substantial Contribution to Protection and Restoration of Biodiversity and Ecosystems</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aligned Revenue per Activity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Absolute value and share of the revenue per activity that is taxonomy-aligned, i.e., generated by an eligible economic activity that is making a substantial contribution to at least one of the climate and environmental objectives, while also doing no significant harm to the remaining objectives and meeting minimum standards on human rights and labour standards</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AlignedActivitiesFormField</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extended</t>
+  </si>
+  <si>
+    <t xml:space="preserve">alignedActivities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non-Aligned Revenue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Absolute value and share of the revenue that is associated with non taxonomy-aligned but eligible activities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nonAlignedShare</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non-Aligned Revenue per Activity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Absolute value and share of the revenue per activity that is not taxonomy-aligned but eligible</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NonAlignedActivitiesFormField</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nonAlignedActivities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non-Eligible Revenue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Absolute value and share of the revenue that is not part of a plan to meet the DNSH criteria and make substantial contribution to any environmental objective</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nonEligibleShare</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enabling Revenue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Share of the taxonomy-aligned revenue from total aligned revenue that is linked to activities that enable reduction of GHG in other sectors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">enablingShareInPercent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transitional Revenue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Share of the taxonomy-aligned revenue from total aligned revenue that is linked to activities with significantly lower GHG emissions than the sector or industry average</t>
+  </si>
+  <si>
+    <t xml:space="preserve">transitionalShareInPercent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CapEx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total CapEx</t>
   </si>
   <si>
     <t xml:space="preserve">Total CapEx for the reported year. Capital expenditures are non-consumable investments, e.g. for acquiring, upgrading, and maintaining physical assets such as property, plants, buildings, technology </t>
   </si>
   <si>
-    <t>Eligible CapEx</t>
-  </si>
-  <si>
-    <t>Absolute value and share of the total CapEx where the economic activity meets taxonomy criteria for substantial contribution to climate change mitigation and does no serious harm to the other environmental objectives (DNSH criteria)</t>
-  </si>
-  <si>
-    <t>Aligned CapEx</t>
-  </si>
-  <si>
-    <t>Absolute value and share of CapEx that is taxonomy-aligned, i.e., generated by an eligible economic activity that is making a substantial contribution to at least one of the climate and environmental objectives, while also doing no significant harm to the remaining objectives and meeting minimum standards on human rights and labour standards.</t>
-  </si>
-  <si>
-    <t>Aligned CapEx per Activity</t>
-  </si>
-  <si>
-    <t>Absolute value and share of the CapEx per activity that is taxonomy-aligned, i.e., generated by an eligible economic activity that is making a substantial contribution to at least one of the climate and environmental objectives, while also doing no significant harm to the remaining objectives and meeting minimum standards on human rights and labour standards</t>
-  </si>
-  <si>
-    <t>Allowed Range: [0, 100]</t>
-  </si>
-  <si>
-    <t>Non-Aligned CapEx</t>
-  </si>
-  <si>
-    <t>Absolute value and share of the CapEx that is associated with non taxonomy-aligned but eligible activities</t>
-  </si>
-  <si>
-    <t>Non-Aligned CapEx per Activity</t>
-  </si>
-  <si>
-    <t>Absolute value and share of the CapEx per activity that is not taxonomy-aligned but eligible</t>
-  </si>
-  <si>
-    <t>Non-Eligible CapEx</t>
-  </si>
-  <si>
-    <t>Absolute value and share of the CapEx that is not part of a plan to meet the DNSH criteria and make substantial contribution to any environmental objective</t>
-  </si>
-  <si>
-    <t>Enabling CapEx</t>
-  </si>
-  <si>
-    <t>Share of the taxonomy-aligned CapEx from total aligned CapEx that is linked to activities that enable reduction of GHG in other sectors</t>
-  </si>
-  <si>
-    <t>Transitional CapEx</t>
-  </si>
-  <si>
-    <t>Share of the taxonomy-aligned CapEx from total aligned CapEx that is linked to activities with significantly lower GHG emissions than the sector or industry average</t>
-  </si>
-  <si>
-    <t>OpEx</t>
-  </si>
-  <si>
-    <t>Total OpEx</t>
-  </si>
-  <si>
-    <t>Total OpEx for the financial year. Operating expenses (OpEx) are shorter term expenses required to meet the ongoing operational costs of running a business.</t>
-  </si>
-  <si>
-    <t>Eligible OpEx</t>
-  </si>
-  <si>
-    <t>Absolute value and share of the OpEx that is part of a plan to meet the DNSH criteria and make substantial contribution to any environmental objective</t>
-  </si>
-  <si>
-    <t>Aligned OpEx</t>
-  </si>
-  <si>
-    <t>Absolute value and share of the OpEx that is associated with taxonomy-aligned activities. i.e., for an eligible economic activity that is making a substantial contribution to at least one of the climate and environmental objectives, while also doing no significant harm to the remaining objectives and meeting minimum standards on human rights and labour standards</t>
-  </si>
-  <si>
-    <t>Aligned OpEx per Activity</t>
+    <t xml:space="preserve">Eligible CapEx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Absolute value and share of the total CapEx where the economic activity meets taxonomy criteria for substantial contribution to climate change mitigation and does no serious harm to the other environmental objectives (DNSH criteria)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aligned CapEx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Absolute value and share of CapEx that is taxonomy-aligned, i.e., generated by an eligible economic activity that is making a substantial contribution to at least one of the climate and environmental objectives, while also doing no significant harm to the remaining objectives and meeting minimum standards on human rights and labour standards.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aligned CapEx per Activity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Absolute value and share of the CapEx per activity that is taxonomy-aligned, i.e., generated by an eligible economic activity that is making a substantial contribution to at least one of the climate and environmental objectives, while also doing no significant harm to the remaining objectives and meeting minimum standards on human rights and labour standards</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allowed Range: [0, 100]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non-Aligned CapEx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Absolute value and share of the CapEx that is associated with non taxonomy-aligned but eligible activities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non-Aligned CapEx per Activity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Absolute value and share of the CapEx per activity that is not taxonomy-aligned but eligible</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non-Eligible CapEx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Absolute value and share of the CapEx that is not part of a plan to meet the DNSH criteria and make substantial contribution to any environmental objective</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enabling CapEx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Share of the taxonomy-aligned CapEx from total aligned CapEx that is linked to activities that enable reduction of GHG in other sectors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transitional CapEx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Share of the taxonomy-aligned CapEx from total aligned CapEx that is linked to activities with significantly lower GHG emissions than the sector or industry average</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OpEx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total OpEx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total OpEx for the financial year. Operating expenses (OpEx) are shorter term expenses required to meet the ongoing operational costs of running a business.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eligible OpEx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Absolute value and share of the OpEx that is part of a plan to meet the DNSH criteria and make substantial contribution to any environmental objective</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aligned OpEx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Absolute value and share of the OpEx that is associated with taxonomy-aligned activities. i.e., for an eligible economic activity that is making a substantial contribution to at least one of the climate and environmental objectives, while also doing no significant harm to the remaining objectives and meeting minimum standards on human rights and labour standards</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aligned OpEx per Activity</t>
   </si>
   <si>
     <t xml:space="preserve">Absolute value and share of taxonomy-aligned OpEx for the activity from total OpEx. </t>
   </si>
   <si>
-    <t>Non-Aligned OpEx</t>
-  </si>
-  <si>
-    <t>Absolute value and share of the OpEx that is associated with non taxonomy-aligned but eligible activities</t>
-  </si>
-  <si>
-    <t>Non-Aligned OpEx per Activity</t>
-  </si>
-  <si>
-    <t>Absolute value and share of the OpEx per activity that is not taxonomy-aligned but eligible</t>
-  </si>
-  <si>
-    <t>Non-Eligible OpEx</t>
-  </si>
-  <si>
-    <t>Absolute value and share of the OpEx that is not part of a plan to meet the DNSH criteria and make substantial contribution to any environmental objective</t>
-  </si>
-  <si>
-    <t>Enabling OpEx</t>
-  </si>
-  <si>
-    <t>Share of the taxonomy-aligned OpEx from total aligned OpEx that is linked to activities that enable reduction of GHG in other sectors</t>
-  </si>
-  <si>
-    <t>Transitional OpEx</t>
-  </si>
-  <si>
-    <t>Share of the taxonomy-aligned OpEx from total aligned OpEx that is linked to activities with significantly lower GHG emissions than the sector or industry average</t>
+    <t xml:space="preserve">Non-Aligned OpEx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Absolute value and share of the OpEx that is associated with non taxonomy-aligned but eligible activities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non-Aligned OpEx per Activity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Absolute value and share of the OpEx per activity that is not taxonomy-aligned but eligible</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non-Eligible OpEx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Absolute value and share of the OpEx that is not part of a plan to meet the DNSH criteria and make substantial contribution to any environmental objective</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enabling OpEx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Share of the taxonomy-aligned OpEx from total aligned OpEx that is linked to activities that enable reduction of GHG in other sectors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transitional OpEx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Share of the taxonomy-aligned OpEx from total aligned OpEx that is linked to activities with significantly lower GHG emissions than the sector or industry average</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="General"/>
+  </numFmts>
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <scheme val="minor"/>
+      <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="9"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="9"/>
       <color rgb="FF3F3F3F"/>
       <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="8"/>
       <color rgb="FF3F3F3F"/>
       <name val="Roboto"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="9"/>
       <color rgb="FF3F3F3F"/>
       <name val="Roboto"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
-      <b/>
+      <b val="true"/>
       <sz val="9"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -602,61 +605,100 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF434343"/>
-        <bgColor rgb="FF434343"/>
+        <bgColor rgb="FF3F3F3F"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFBFBFBF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF434343"/>
-        <bgColor rgb="FF000000"/>
+        <bgColor rgb="FFCCCCCC"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF7F7F7F"/>
-        <bgColor rgb="FF7F7F7F"/>
+        <bgColor rgb="FF969696"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
-        <bgColor rgb="FFF2F2F2"/>
+        <bgColor rgb="FFEFEFEF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor rgb="FF000000"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFEFEFEF"/>
-        <bgColor rgb="FFEFEFEF"/>
+        <bgColor rgb="FFF2F2F2"/>
       </patternFill>
     </fill>
   </fills>
   <borders count="15">
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="thin"/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="thin"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -671,92 +713,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right style="thin">
         <color rgb="FF3F3F3F"/>
@@ -767,7 +724,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right style="thin">
         <color rgb="FF3F3F3F"/>
@@ -780,20 +737,14 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
       <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -806,304 +757,368 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
       <bottom/>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+  <cellStyleXfs count="21">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="40">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="13" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="14" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="14" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+  <cellXfs count="38">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="3" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="3" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="7" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="7" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="7" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="5" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="7" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="5" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="7" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="7" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="5" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="7" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="7" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{49FDFDEC-F4AA-4DD2-90E4-0B6C182B275F}"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Normal 3" xfId="20"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFBFBFBF"/>
+      <rgbColor rgb="FF7F7F7F"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFF2F2F2"/>
+      <rgbColor rgb="FFEFEFEF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCCC"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF434343"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF3F3F3F"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:srgbClr val="ffffff"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="44546a"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="e7e6e6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4472c4"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="ed7d31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="a5a5a5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="ffc000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="5b9bd5"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="70ad47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0563c1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="954f72"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204" pitchFamily="0" charset="1"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="0" charset="1"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme>
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
                 <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
                 <a:tint val="67000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="50000">
               <a:schemeClr val="phClr">
                 <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
                 <a:tint val="73000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
                 <a:tint val="81000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
                 <a:lumMod val="102000"/>
                 <a:tint val="94000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
                 <a:lumMod val="100000"/>
                 <a:shade val="100000"/>
               </a:schemeClr>
@@ -1111,33 +1126,24 @@
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
                 <a:shade val="78000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
         <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
@@ -1150,13 +1156,7 @@
           <a:effectLst/>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
+          <a:effectLst/>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
@@ -1166,15 +1166,13 @@
         <a:solidFill>
           <a:schemeClr val="phClr">
             <a:tint val="95000"/>
-            <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
                 <a:tint val="93000"/>
-                <a:satMod val="150000"/>
                 <a:shade val="98000"/>
                 <a:lumMod val="102000"/>
               </a:schemeClr>
@@ -1182,7 +1180,6 @@
             <a:gs pos="50000">
               <a:schemeClr val="phClr">
                 <a:tint val="98000"/>
-                <a:satMod val="130000"/>
                 <a:shade val="90000"/>
                 <a:lumMod val="103000"/>
               </a:schemeClr>
@@ -1190,110 +1187,106 @@
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:shade val="63000"/>
-                <a:satMod val="120000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{535E0EDD-39B9-4B5D-8666-66CC7B300147}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:T55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="4" max="4" width="70.33203125" customWidth="1"/>
-    <col min="5" max="5" width="77.88671875" customWidth="1"/>
-    <col min="6" max="6" width="21.33203125" customWidth="1"/>
-    <col min="8" max="12" width="14.33203125" customWidth="1"/>
-    <col min="13" max="13" width="19.5546875" customWidth="1"/>
-    <col min="14" max="14" width="19.109375" customWidth="1"/>
-    <col min="15" max="15" width="20.88671875" customWidth="1"/>
-    <col min="16" max="16" width="50.6640625" customWidth="1"/>
-    <col min="17" max="17" width="14.5546875" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="70.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="77.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="21.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="8" style="1" width="14.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="19.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="19.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="20.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="50.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="14.56"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="O1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="P1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="Q1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="8" t="s">
+      <c r="R1" s="6" t="s">
         <v>17</v>
       </c>
       <c r="S1" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A2" s="10">
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="10" t="n">
         <v>0</v>
       </c>
       <c r="B2" s="11" t="s">
@@ -1338,8 +1331,8 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A3" s="10">
+    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="10" t="n">
         <v>1</v>
       </c>
       <c r="B3" s="11" t="s">
@@ -1382,8 +1375,8 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A4" s="10">
+    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="10" t="n">
         <v>2</v>
       </c>
       <c r="B4" s="11" t="s">
@@ -1424,10 +1417,10 @@
       <c r="S4" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="T4" s="26"/>
-    </row>
-    <row r="5" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A5" s="22">
+      <c r="T4" s="20"/>
+    </row>
+    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="22" t="n">
         <v>3</v>
       </c>
       <c r="B5" s="22" t="s">
@@ -1452,15 +1445,15 @@
       <c r="J5" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="Q5" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="S5" s="28" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A6" s="10">
+      <c r="Q5" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="S5" s="27" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="10" t="n">
         <v>4</v>
       </c>
       <c r="B6" s="11" t="s">
@@ -1503,10 +1496,10 @@
       <c r="S6" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="T6" s="26"/>
-    </row>
-    <row r="7" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A7" s="10">
+      <c r="T6" s="20"/>
+    </row>
+    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="10" t="n">
         <v>5</v>
       </c>
       <c r="B7" s="11" t="s">
@@ -1547,10 +1540,10 @@
       <c r="S7" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="T7" s="26"/>
-    </row>
-    <row r="8" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A8" s="10">
+      <c r="T7" s="20"/>
+    </row>
+    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="10" t="n">
         <v>6</v>
       </c>
       <c r="B8" s="11" t="s">
@@ -1593,8 +1586,8 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A9" s="10">
+    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="10" t="n">
         <v>7</v>
       </c>
       <c r="B9" s="11" t="s">
@@ -1639,8 +1632,8 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A10" s="10">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="10" t="n">
         <v>8</v>
       </c>
       <c r="B10" s="11" t="s">
@@ -1655,7 +1648,7 @@
       <c r="E10" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="F10" s="14" t="s">
+      <c r="F10" s="16" t="s">
         <v>61</v>
       </c>
       <c r="G10" s="14" t="s">
@@ -1683,8 +1676,8 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A11" s="10">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="10" t="n">
         <v>9</v>
       </c>
       <c r="B11" s="11" t="s">
@@ -1693,14 +1686,14 @@
       <c r="C11" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="D11" s="29" t="s">
+      <c r="D11" s="28" t="s">
         <v>64</v>
       </c>
       <c r="E11" s="25" t="s">
         <v>65</v>
       </c>
       <c r="F11" s="16" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="G11" s="22"/>
       <c r="H11" s="16"/>
@@ -1723,18 +1716,18 @@
       <c r="Q11" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="R11" s="30" t="s">
+      <c r="R11" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="S11" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="T11" s="32" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A12" s="10">
+      <c r="S11" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="T11" s="30" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="10" t="n">
         <v>10</v>
       </c>
       <c r="B12" s="11" t="s">
@@ -1743,14 +1736,14 @@
       <c r="C12" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="D12" s="29" t="s">
+      <c r="D12" s="28" t="s">
         <v>71</v>
       </c>
       <c r="E12" s="16" t="s">
         <v>72</v>
       </c>
       <c r="F12" s="16" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="G12" s="22"/>
       <c r="H12" s="16"/>
@@ -1773,18 +1766,18 @@
       <c r="Q12" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="R12" s="33" t="s">
+      <c r="R12" s="31" t="s">
         <v>76</v>
       </c>
-      <c r="S12" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="T12" s="35" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A13" s="10">
+      <c r="S12" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="T12" s="33" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="10" t="n">
         <v>11</v>
       </c>
       <c r="B13" s="11" t="s">
@@ -1793,14 +1786,14 @@
       <c r="C13" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="D13" s="29" t="s">
+      <c r="D13" s="28" t="s">
         <v>77</v>
       </c>
       <c r="E13" s="16" t="s">
         <v>78</v>
       </c>
       <c r="F13" s="16" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="G13" s="22"/>
       <c r="H13" s="16"/>
@@ -1821,18 +1814,18 @@
       <c r="Q13" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="R13" s="33" t="s">
+      <c r="R13" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="S13" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="T13" s="35" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A14" s="10">
+      <c r="S13" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="T13" s="33" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="10" t="n">
         <v>12</v>
       </c>
       <c r="B14" s="11" t="s">
@@ -1841,7 +1834,7 @@
       <c r="C14" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="D14" s="29" t="s">
+      <c r="D14" s="28" t="s">
         <v>81</v>
       </c>
       <c r="E14" s="16" t="s">
@@ -1867,16 +1860,16 @@
       <c r="Q14" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="R14" s="33"/>
-      <c r="S14" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="T14" s="35" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A15" s="10">
+      <c r="R14" s="31"/>
+      <c r="S14" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="T14" s="33" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="10" t="n">
         <v>13</v>
       </c>
       <c r="B15" s="11" t="s">
@@ -1885,7 +1878,7 @@
       <c r="C15" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="D15" s="29" t="s">
+      <c r="D15" s="28" t="s">
         <v>83</v>
       </c>
       <c r="E15" s="16" t="s">
@@ -1911,16 +1904,16 @@
       <c r="Q15" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="R15" s="33"/>
-      <c r="S15" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="T15" s="35" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A16" s="10">
+      <c r="R15" s="31"/>
+      <c r="S15" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="T15" s="33" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="10" t="n">
         <v>14</v>
       </c>
       <c r="B16" s="11" t="s">
@@ -1929,7 +1922,7 @@
       <c r="C16" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="D16" s="29" t="s">
+      <c r="D16" s="28" t="s">
         <v>84</v>
       </c>
       <c r="E16" s="16" t="s">
@@ -1955,16 +1948,16 @@
       <c r="Q16" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="R16" s="33"/>
-      <c r="S16" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="T16" s="35" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A17" s="10">
+      <c r="R16" s="31"/>
+      <c r="S16" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="T16" s="33" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="10" t="n">
         <v>15</v>
       </c>
       <c r="B17" s="11" t="s">
@@ -1973,7 +1966,7 @@
       <c r="C17" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="D17" s="29" t="s">
+      <c r="D17" s="28" t="s">
         <v>85</v>
       </c>
       <c r="E17" s="16" t="s">
@@ -1999,16 +1992,16 @@
       <c r="Q17" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="R17" s="33"/>
-      <c r="S17" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="T17" s="35" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A18" s="10">
+      <c r="R17" s="31"/>
+      <c r="S17" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="T17" s="33" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="10" t="n">
         <v>16</v>
       </c>
       <c r="B18" s="11" t="s">
@@ -2017,7 +2010,7 @@
       <c r="C18" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="D18" s="29" t="s">
+      <c r="D18" s="28" t="s">
         <v>86</v>
       </c>
       <c r="E18" s="16" t="s">
@@ -2043,16 +2036,16 @@
       <c r="Q18" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="R18" s="33"/>
-      <c r="S18" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="T18" s="35" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A19" s="10">
+      <c r="R18" s="31"/>
+      <c r="S18" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="T18" s="33" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="10" t="n">
         <v>17</v>
       </c>
       <c r="B19" s="11" t="s">
@@ -2061,7 +2054,7 @@
       <c r="C19" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="D19" s="29" t="s">
+      <c r="D19" s="28" t="s">
         <v>87</v>
       </c>
       <c r="E19" s="16" t="s">
@@ -2087,16 +2080,16 @@
       <c r="Q19" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="R19" s="33"/>
-      <c r="S19" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="T19" s="35" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A20" s="10">
+      <c r="R19" s="31"/>
+      <c r="S19" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="T19" s="33" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="10" t="n">
         <v>18</v>
       </c>
       <c r="B20" s="11" t="s">
@@ -2105,7 +2098,7 @@
       <c r="C20" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="D20" s="29" t="s">
+      <c r="D20" s="28" t="s">
         <v>88</v>
       </c>
       <c r="E20" s="16" t="s">
@@ -2131,18 +2124,18 @@
       <c r="Q20" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="R20" s="33" t="s">
+      <c r="R20" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="S20" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="T20" s="35" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A21" s="10">
+      <c r="S20" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="T20" s="33" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="10" t="n">
         <v>19</v>
       </c>
       <c r="B21" s="11" t="s">
@@ -2151,7 +2144,7 @@
       <c r="C21" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="D21" s="29" t="s">
+      <c r="D21" s="28" t="s">
         <v>93</v>
       </c>
       <c r="E21" s="16" t="s">
@@ -2177,18 +2170,18 @@
       <c r="Q21" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="R21" s="33" t="s">
+      <c r="R21" s="31" t="s">
         <v>95</v>
       </c>
-      <c r="S21" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="T21" s="35" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A22" s="10">
+      <c r="S21" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="T21" s="33" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="10" t="n">
         <v>20</v>
       </c>
       <c r="B22" s="11" t="s">
@@ -2197,7 +2190,7 @@
       <c r="C22" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="D22" s="29" t="s">
+      <c r="D22" s="28" t="s">
         <v>96</v>
       </c>
       <c r="E22" s="16" t="s">
@@ -2223,18 +2216,18 @@
       <c r="Q22" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="R22" s="33" t="s">
+      <c r="R22" s="31" t="s">
         <v>99</v>
       </c>
-      <c r="S22" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="T22" s="35" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A23" s="10">
+      <c r="S22" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="T22" s="33" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="10" t="n">
         <v>21</v>
       </c>
       <c r="B23" s="11" t="s">
@@ -2243,7 +2236,7 @@
       <c r="C23" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="D23" s="29" t="s">
+      <c r="D23" s="28" t="s">
         <v>100</v>
       </c>
       <c r="E23" s="16" t="s">
@@ -2269,27 +2262,27 @@
       <c r="Q23" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="R23" s="33" t="s">
+      <c r="R23" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="S23" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="T23" s="35" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A24" s="10">
+      <c r="S23" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="T23" s="33" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="10" t="n">
         <v>22</v>
       </c>
-      <c r="B24" s="36" t="s">
+      <c r="B24" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="C24" s="36" t="s">
+      <c r="C24" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="D24" s="37" t="s">
+      <c r="D24" s="35" t="s">
         <v>103</v>
       </c>
       <c r="E24" s="16" t="s">
@@ -2307,35 +2300,35 @@
       <c r="M24" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="N24" s="33"/>
-      <c r="O24" s="33"/>
-      <c r="P24" s="33" t="s">
+      <c r="N24" s="31"/>
+      <c r="O24" s="31"/>
+      <c r="P24" s="31" t="s">
         <v>75</v>
       </c>
       <c r="Q24" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="R24" s="33" t="s">
+      <c r="R24" s="31" t="s">
         <v>105</v>
       </c>
-      <c r="S24" s="38" t="s">
-        <v>28</v>
-      </c>
-      <c r="T24" s="39" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="25" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A25" s="10">
+      <c r="S24" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="T24" s="37" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="10" t="n">
         <v>23</v>
       </c>
-      <c r="B25" s="36" t="s">
+      <c r="B25" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="C25" s="36" t="s">
+      <c r="C25" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="D25" s="37" t="s">
+      <c r="D25" s="35" t="s">
         <v>106</v>
       </c>
       <c r="E25" s="16" t="s">
@@ -2353,26 +2346,26 @@
       <c r="M25" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="N25" s="33"/>
-      <c r="O25" s="33"/>
-      <c r="P25" s="33" t="s">
+      <c r="N25" s="31"/>
+      <c r="O25" s="31"/>
+      <c r="P25" s="31" t="s">
         <v>75</v>
       </c>
       <c r="Q25" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="R25" s="33" t="s">
+      <c r="R25" s="31" t="s">
         <v>108</v>
       </c>
-      <c r="S25" s="38" t="s">
-        <v>28</v>
-      </c>
-      <c r="T25" s="39" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="26" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A26" s="10">
+      <c r="S25" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="T25" s="37" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="10" t="n">
         <v>24</v>
       </c>
       <c r="B26" s="11" t="s">
@@ -2381,7 +2374,7 @@
       <c r="C26" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="D26" s="29" t="s">
+      <c r="D26" s="28" t="s">
         <v>110</v>
       </c>
       <c r="E26" s="16" t="s">
@@ -2407,18 +2400,18 @@
       <c r="Q26" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="R26" s="30" t="s">
+      <c r="R26" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="S26" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="T26" s="35" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="27" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A27" s="10">
+      <c r="S26" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="T26" s="33" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="10" t="n">
         <v>25</v>
       </c>
       <c r="B27" s="11" t="s">
@@ -2427,7 +2420,7 @@
       <c r="C27" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="D27" s="29" t="s">
+      <c r="D27" s="28" t="s">
         <v>112</v>
       </c>
       <c r="E27" s="16" t="s">
@@ -2453,18 +2446,18 @@
       <c r="Q27" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="R27" s="33" t="s">
+      <c r="R27" s="31" t="s">
         <v>76</v>
       </c>
-      <c r="S27" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="T27" s="35" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="28" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A28" s="10">
+      <c r="S27" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="T27" s="33" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="10" t="n">
         <v>26</v>
       </c>
       <c r="B28" s="11" t="s">
@@ -2473,7 +2466,7 @@
       <c r="C28" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="D28" s="29" t="s">
+      <c r="D28" s="28" t="s">
         <v>114</v>
       </c>
       <c r="E28" s="16" t="s">
@@ -2499,18 +2492,18 @@
       <c r="Q28" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="R28" s="33" t="s">
+      <c r="R28" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="S28" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="T28" s="35" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="29" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A29" s="10">
+      <c r="S28" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="T28" s="33" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="10" t="n">
         <v>27</v>
       </c>
       <c r="B29" s="11" t="s">
@@ -2519,7 +2512,7 @@
       <c r="C29" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="D29" s="29" t="s">
+      <c r="D29" s="28" t="s">
         <v>81</v>
       </c>
       <c r="E29" s="16" t="s">
@@ -2545,16 +2538,16 @@
       <c r="Q29" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="R29" s="33"/>
-      <c r="S29" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="T29" s="35" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="30" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A30" s="10">
+      <c r="R29" s="31"/>
+      <c r="S29" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="T29" s="33" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="10" t="n">
         <v>28</v>
       </c>
       <c r="B30" s="11" t="s">
@@ -2563,7 +2556,7 @@
       <c r="C30" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="D30" s="29" t="s">
+      <c r="D30" s="28" t="s">
         <v>83</v>
       </c>
       <c r="E30" s="16" t="s">
@@ -2589,16 +2582,16 @@
       <c r="Q30" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="R30" s="33"/>
-      <c r="S30" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="T30" s="35" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="31" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A31" s="10">
+      <c r="R30" s="31"/>
+      <c r="S30" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="T30" s="33" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="10" t="n">
         <v>29</v>
       </c>
       <c r="B31" s="11" t="s">
@@ -2607,7 +2600,7 @@
       <c r="C31" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="D31" s="29" t="s">
+      <c r="D31" s="28" t="s">
         <v>84</v>
       </c>
       <c r="E31" s="16" t="s">
@@ -2633,16 +2626,16 @@
       <c r="Q31" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="R31" s="33"/>
-      <c r="S31" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="T31" s="35" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="32" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A32" s="10">
+      <c r="R31" s="31"/>
+      <c r="S31" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="T31" s="33" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="10" t="n">
         <v>30</v>
       </c>
       <c r="B32" s="11" t="s">
@@ -2651,7 +2644,7 @@
       <c r="C32" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="D32" s="29" t="s">
+      <c r="D32" s="28" t="s">
         <v>85</v>
       </c>
       <c r="E32" s="16" t="s">
@@ -2677,16 +2670,16 @@
       <c r="Q32" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="R32" s="33"/>
-      <c r="S32" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="T32" s="35" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="33" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A33" s="10">
+      <c r="R32" s="31"/>
+      <c r="S32" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="T32" s="33" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="10" t="n">
         <v>31</v>
       </c>
       <c r="B33" s="11" t="s">
@@ -2695,7 +2688,7 @@
       <c r="C33" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="D33" s="29" t="s">
+      <c r="D33" s="28" t="s">
         <v>86</v>
       </c>
       <c r="E33" s="16" t="s">
@@ -2721,16 +2714,16 @@
       <c r="Q33" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="R33" s="33"/>
-      <c r="S33" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="T33" s="35" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="34" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A34" s="10">
+      <c r="R33" s="31"/>
+      <c r="S33" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="T33" s="33" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="10" t="n">
         <v>32</v>
       </c>
       <c r="B34" s="11" t="s">
@@ -2739,7 +2732,7 @@
       <c r="C34" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="D34" s="29" t="s">
+      <c r="D34" s="28" t="s">
         <v>87</v>
       </c>
       <c r="E34" s="16" t="s">
@@ -2765,16 +2758,16 @@
       <c r="Q34" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="R34" s="33"/>
-      <c r="S34" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="T34" s="35" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="35" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A35" s="10">
+      <c r="R34" s="31"/>
+      <c r="S34" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="T34" s="33" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="10" t="n">
         <v>33</v>
       </c>
       <c r="B35" s="11" t="s">
@@ -2783,7 +2776,7 @@
       <c r="C35" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="D35" s="29" t="s">
+      <c r="D35" s="28" t="s">
         <v>116</v>
       </c>
       <c r="E35" s="16" t="s">
@@ -2811,18 +2804,18 @@
       <c r="Q35" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="R35" s="33" t="s">
+      <c r="R35" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="S35" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="T35" s="35" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="36" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A36" s="10">
+      <c r="S35" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="T35" s="33" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="10" t="n">
         <v>34</v>
       </c>
       <c r="B36" s="11" t="s">
@@ -2831,7 +2824,7 @@
       <c r="C36" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="D36" s="29" t="s">
+      <c r="D36" s="28" t="s">
         <v>119</v>
       </c>
       <c r="E36" s="16" t="s">
@@ -2857,18 +2850,18 @@
       <c r="Q36" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="R36" s="33" t="s">
+      <c r="R36" s="31" t="s">
         <v>95</v>
       </c>
-      <c r="S36" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="T36" s="35" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="37" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A37" s="10">
+      <c r="S36" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="T36" s="33" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="10" t="n">
         <v>35</v>
       </c>
       <c r="B37" s="11" t="s">
@@ -2877,7 +2870,7 @@
       <c r="C37" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="D37" s="29" t="s">
+      <c r="D37" s="28" t="s">
         <v>121</v>
       </c>
       <c r="E37" s="16" t="s">
@@ -2905,18 +2898,18 @@
       <c r="Q37" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="R37" s="33" t="s">
+      <c r="R37" s="31" t="s">
         <v>99</v>
       </c>
-      <c r="S37" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="T37" s="35" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="38" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A38" s="10">
+      <c r="S37" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="T37" s="33" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="10" t="n">
         <v>36</v>
       </c>
       <c r="B38" s="11" t="s">
@@ -2925,7 +2918,7 @@
       <c r="C38" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="D38" s="29" t="s">
+      <c r="D38" s="28" t="s">
         <v>123</v>
       </c>
       <c r="E38" s="16" t="s">
@@ -2951,18 +2944,18 @@
       <c r="Q38" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="R38" s="33" t="s">
+      <c r="R38" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="S38" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="T38" s="35" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="39" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A39" s="10">
+      <c r="S38" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="T38" s="33" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="10" t="n">
         <v>37</v>
       </c>
       <c r="B39" s="11" t="s">
@@ -2971,7 +2964,7 @@
       <c r="C39" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="D39" s="37" t="s">
+      <c r="D39" s="35" t="s">
         <v>125</v>
       </c>
       <c r="E39" s="16" t="s">
@@ -2989,26 +2982,26 @@
       <c r="M39" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="N39" s="33"/>
-      <c r="O39" s="33"/>
-      <c r="P39" s="33" t="s">
+      <c r="N39" s="31"/>
+      <c r="O39" s="31"/>
+      <c r="P39" s="31" t="s">
         <v>75</v>
       </c>
       <c r="Q39" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="R39" s="33" t="s">
+      <c r="R39" s="31" t="s">
         <v>105</v>
       </c>
-      <c r="S39" s="38" t="s">
-        <v>28</v>
-      </c>
-      <c r="T39" s="39" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="40" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A40" s="10">
+      <c r="S39" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="T39" s="37" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="10" t="n">
         <v>38</v>
       </c>
       <c r="B40" s="11" t="s">
@@ -3017,7 +3010,7 @@
       <c r="C40" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="D40" s="37" t="s">
+      <c r="D40" s="35" t="s">
         <v>127</v>
       </c>
       <c r="E40" s="16" t="s">
@@ -3035,26 +3028,26 @@
       <c r="M40" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="N40" s="33"/>
-      <c r="O40" s="33"/>
-      <c r="P40" s="33" t="s">
+      <c r="N40" s="31"/>
+      <c r="O40" s="31"/>
+      <c r="P40" s="31" t="s">
         <v>75</v>
       </c>
       <c r="Q40" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="R40" s="33" t="s">
+      <c r="R40" s="31" t="s">
         <v>108</v>
       </c>
-      <c r="S40" s="38" t="s">
-        <v>28</v>
-      </c>
-      <c r="T40" s="39" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="41" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A41" s="10">
+      <c r="S40" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="T40" s="37" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="10" t="n">
         <v>39</v>
       </c>
       <c r="B41" s="11" t="s">
@@ -3063,7 +3056,7 @@
       <c r="C41" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="D41" s="29" t="s">
+      <c r="D41" s="28" t="s">
         <v>130</v>
       </c>
       <c r="E41" s="16" t="s">
@@ -3089,18 +3082,18 @@
       <c r="Q41" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="R41" s="30" t="s">
+      <c r="R41" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="S41" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="T41" s="35" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="42" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A42" s="10">
+      <c r="S41" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="T41" s="33" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="10" t="n">
         <v>40</v>
       </c>
       <c r="B42" s="11" t="s">
@@ -3109,7 +3102,7 @@
       <c r="C42" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="D42" s="29" t="s">
+      <c r="D42" s="28" t="s">
         <v>132</v>
       </c>
       <c r="E42" s="16" t="s">
@@ -3135,18 +3128,18 @@
       <c r="Q42" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="R42" s="33" t="s">
+      <c r="R42" s="31" t="s">
         <v>76</v>
       </c>
-      <c r="S42" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="T42" s="35" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="43" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A43" s="10">
+      <c r="S42" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="T42" s="33" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="10" t="n">
         <v>41</v>
       </c>
       <c r="B43" s="11" t="s">
@@ -3155,7 +3148,7 @@
       <c r="C43" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="D43" s="29" t="s">
+      <c r="D43" s="28" t="s">
         <v>134</v>
       </c>
       <c r="E43" s="16" t="s">
@@ -3181,18 +3174,18 @@
       <c r="Q43" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="R43" s="33" t="s">
+      <c r="R43" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="S43" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="T43" s="35" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="44" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A44" s="10">
+      <c r="S43" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="T43" s="33" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="10" t="n">
         <v>42</v>
       </c>
       <c r="B44" s="11" t="s">
@@ -3201,7 +3194,7 @@
       <c r="C44" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="D44" s="29" t="s">
+      <c r="D44" s="28" t="s">
         <v>81</v>
       </c>
       <c r="E44" s="16" t="s">
@@ -3227,16 +3220,16 @@
       <c r="Q44" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="R44" s="33"/>
-      <c r="S44" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="T44" s="35" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="45" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A45" s="10">
+      <c r="R44" s="31"/>
+      <c r="S44" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="T44" s="33" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="10" t="n">
         <v>43</v>
       </c>
       <c r="B45" s="11" t="s">
@@ -3245,7 +3238,7 @@
       <c r="C45" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="D45" s="29" t="s">
+      <c r="D45" s="28" t="s">
         <v>83</v>
       </c>
       <c r="E45" s="16" t="s">
@@ -3271,16 +3264,16 @@
       <c r="Q45" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="R45" s="33"/>
-      <c r="S45" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="T45" s="35" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="46" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A46" s="10">
+      <c r="R45" s="31"/>
+      <c r="S45" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="T45" s="33" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="10" t="n">
         <v>44</v>
       </c>
       <c r="B46" s="11" t="s">
@@ -3289,7 +3282,7 @@
       <c r="C46" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="D46" s="29" t="s">
+      <c r="D46" s="28" t="s">
         <v>84</v>
       </c>
       <c r="E46" s="16" t="s">
@@ -3315,16 +3308,16 @@
       <c r="Q46" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="R46" s="33"/>
-      <c r="S46" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="T46" s="35" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="47" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A47" s="10">
+      <c r="R46" s="31"/>
+      <c r="S46" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="T46" s="33" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="10" t="n">
         <v>45</v>
       </c>
       <c r="B47" s="11" t="s">
@@ -3333,7 +3326,7 @@
       <c r="C47" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="D47" s="29" t="s">
+      <c r="D47" s="28" t="s">
         <v>85</v>
       </c>
       <c r="E47" s="16" t="s">
@@ -3359,16 +3352,16 @@
       <c r="Q47" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="R47" s="33"/>
-      <c r="S47" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="T47" s="35" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="48" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A48" s="10">
+      <c r="R47" s="31"/>
+      <c r="S47" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="T47" s="33" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="10" t="n">
         <v>46</v>
       </c>
       <c r="B48" s="11" t="s">
@@ -3377,7 +3370,7 @@
       <c r="C48" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="D48" s="29" t="s">
+      <c r="D48" s="28" t="s">
         <v>86</v>
       </c>
       <c r="E48" s="16" t="s">
@@ -3403,16 +3396,16 @@
       <c r="Q48" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="R48" s="33"/>
-      <c r="S48" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="T48" s="35" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="49" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A49" s="10">
+      <c r="R48" s="31"/>
+      <c r="S48" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="T48" s="33" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="10" t="n">
         <v>47</v>
       </c>
       <c r="B49" s="11" t="s">
@@ -3421,7 +3414,7 @@
       <c r="C49" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="D49" s="29" t="s">
+      <c r="D49" s="28" t="s">
         <v>87</v>
       </c>
       <c r="E49" s="16" t="s">
@@ -3447,16 +3440,16 @@
       <c r="Q49" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="R49" s="33"/>
-      <c r="S49" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="T49" s="35" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="50" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A50" s="10">
+      <c r="R49" s="31"/>
+      <c r="S49" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="T49" s="33" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="10" t="n">
         <v>48</v>
       </c>
       <c r="B50" s="11" t="s">
@@ -3465,7 +3458,7 @@
       <c r="C50" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="D50" s="29" t="s">
+      <c r="D50" s="28" t="s">
         <v>136</v>
       </c>
       <c r="E50" s="16" t="s">
@@ -3493,18 +3486,18 @@
       <c r="Q50" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="R50" s="33" t="s">
+      <c r="R50" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="S50" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="T50" s="35" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="51" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A51" s="10">
+      <c r="S50" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="T50" s="33" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="10" t="n">
         <v>49</v>
       </c>
       <c r="B51" s="11" t="s">
@@ -3513,7 +3506,7 @@
       <c r="C51" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="D51" s="29" t="s">
+      <c r="D51" s="28" t="s">
         <v>138</v>
       </c>
       <c r="E51" s="16" t="s">
@@ -3539,18 +3532,18 @@
       <c r="Q51" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="R51" s="33" t="s">
+      <c r="R51" s="31" t="s">
         <v>95</v>
       </c>
-      <c r="S51" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="T51" s="35" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="52" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A52" s="10">
+      <c r="S51" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="T51" s="33" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="10" t="n">
         <v>50</v>
       </c>
       <c r="B52" s="11" t="s">
@@ -3559,7 +3552,7 @@
       <c r="C52" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="D52" s="29" t="s">
+      <c r="D52" s="28" t="s">
         <v>140</v>
       </c>
       <c r="E52" s="16" t="s">
@@ -3587,18 +3580,18 @@
       <c r="Q52" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="R52" s="33" t="s">
+      <c r="R52" s="31" t="s">
         <v>99</v>
       </c>
-      <c r="S52" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="T52" s="35" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="53" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A53" s="10">
+      <c r="S52" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="T52" s="33" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="10" t="n">
         <v>51</v>
       </c>
       <c r="B53" s="11" t="s">
@@ -3607,7 +3600,7 @@
       <c r="C53" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="D53" s="29" t="s">
+      <c r="D53" s="28" t="s">
         <v>142</v>
       </c>
       <c r="E53" s="16" t="s">
@@ -3632,18 +3625,18 @@
       <c r="Q53" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="R53" s="33" t="s">
+      <c r="R53" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="S53" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="T53" s="35" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="54" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A54" s="10">
+      <c r="S53" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="T53" s="33" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="10" t="n">
         <v>52</v>
       </c>
       <c r="B54" s="11" t="s">
@@ -3652,7 +3645,7 @@
       <c r="C54" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="D54" s="37" t="s">
+      <c r="D54" s="35" t="s">
         <v>144</v>
       </c>
       <c r="E54" s="16" t="s">
@@ -3670,26 +3663,26 @@
       <c r="M54" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="N54" s="33"/>
-      <c r="O54" s="33"/>
-      <c r="P54" s="33" t="s">
+      <c r="N54" s="31"/>
+      <c r="O54" s="31"/>
+      <c r="P54" s="31" t="s">
         <v>75</v>
       </c>
       <c r="Q54" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="R54" s="33" t="s">
+      <c r="R54" s="31" t="s">
         <v>105</v>
       </c>
-      <c r="S54" s="38" t="s">
-        <v>28</v>
-      </c>
-      <c r="T54" s="39" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="55" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A55" s="10">
+      <c r="S54" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="T54" s="37" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="10" t="n">
         <v>53</v>
       </c>
       <c r="B55" s="11" t="s">
@@ -3698,7 +3691,7 @@
       <c r="C55" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="D55" s="37" t="s">
+      <c r="D55" s="35" t="s">
         <v>146</v>
       </c>
       <c r="E55" s="16" t="s">
@@ -3716,26 +3709,31 @@
       <c r="M55" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="N55" s="33"/>
-      <c r="O55" s="33"/>
-      <c r="P55" s="33" t="s">
+      <c r="N55" s="31"/>
+      <c r="O55" s="31"/>
+      <c r="P55" s="31" t="s">
         <v>75</v>
       </c>
       <c r="Q55" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="R55" s="33" t="s">
+      <c r="R55" s="31" t="s">
         <v>108</v>
       </c>
-      <c r="S55" s="38" t="s">
-        <v>28</v>
-      </c>
-      <c r="T55" s="39" t="s">
+      <c r="S55" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="T55" s="37" t="s">
         <v>28</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Migrated to no-subcategory model
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/euTaxonomyNonFinancials/EutaxonomyNonFinancials.xlsx
+++ b/dataland-framework-toolbox/inputs/euTaxonomyNonFinancials/EutaxonomyNonFinancials.xlsx
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="148">
   <si>
     <t xml:space="preserve">Field Identifier</t>
   </si>
@@ -1207,7 +1207,7 @@
   <dimension ref="A1:T55"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+      <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1292,9 +1292,7 @@
       <c r="B2" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="11" t="s">
-        <v>20</v>
-      </c>
+      <c r="C2" s="11"/>
       <c r="D2" s="12" t="s">
         <v>21</v>
       </c>
@@ -1338,9 +1336,7 @@
       <c r="B3" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="11" t="s">
-        <v>20</v>
-      </c>
+      <c r="C3" s="11"/>
       <c r="D3" s="12" t="s">
         <v>29</v>
       </c>
@@ -1382,9 +1378,7 @@
       <c r="B4" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="11" t="s">
-        <v>20</v>
-      </c>
+      <c r="C4" s="11"/>
       <c r="D4" s="24" t="s">
         <v>35</v>
       </c>
@@ -1426,9 +1420,7 @@
       <c r="B5" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="22" t="s">
-        <v>20</v>
-      </c>
+      <c r="C5" s="22"/>
       <c r="D5" s="22" t="s">
         <v>38</v>
       </c>
@@ -1452,16 +1444,14 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="10" t="n">
         <v>4</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="11" t="s">
-        <v>20</v>
-      </c>
+      <c r="C6" s="11"/>
       <c r="D6" s="24" t="s">
         <v>41</v>
       </c>
@@ -1498,16 +1488,14 @@
       </c>
       <c r="T6" s="20"/>
     </row>
-    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="10" t="n">
         <v>5</v>
       </c>
       <c r="B7" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="11" t="s">
-        <v>20</v>
-      </c>
+      <c r="C7" s="11"/>
       <c r="D7" s="24" t="s">
         <v>47</v>
       </c>
@@ -1549,9 +1537,7 @@
       <c r="B8" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="11" t="s">
-        <v>20</v>
-      </c>
+      <c r="C8" s="11"/>
       <c r="D8" s="24" t="s">
         <v>51</v>
       </c>
@@ -1586,16 +1572,14 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="10" t="n">
         <v>7</v>
       </c>
       <c r="B9" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="11" t="s">
-        <v>20</v>
-      </c>
+      <c r="C9" s="11"/>
       <c r="D9" s="24" t="s">
         <v>56</v>
       </c>
@@ -1639,9 +1623,7 @@
       <c r="B10" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="11" t="s">
-        <v>20</v>
-      </c>
+      <c r="C10" s="11"/>
       <c r="D10" s="24" t="s">
         <v>59</v>
       </c>
@@ -1683,9 +1665,7 @@
       <c r="B11" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="C11" s="11" t="s">
-        <v>63</v>
-      </c>
+      <c r="C11" s="11"/>
       <c r="D11" s="28" t="s">
         <v>64</v>
       </c>
@@ -1726,16 +1706,14 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="10" t="n">
         <v>10</v>
       </c>
       <c r="B12" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="C12" s="11" t="s">
-        <v>63</v>
-      </c>
+      <c r="C12" s="11"/>
       <c r="D12" s="28" t="s">
         <v>71</v>
       </c>
@@ -1776,16 +1754,14 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="10" t="n">
         <v>11</v>
       </c>
       <c r="B13" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="C13" s="11" t="s">
-        <v>63</v>
-      </c>
+      <c r="C13" s="11"/>
       <c r="D13" s="28" t="s">
         <v>77</v>
       </c>
@@ -1824,16 +1800,14 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="10" t="n">
         <v>12</v>
       </c>
       <c r="B14" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="C14" s="11" t="s">
-        <v>63</v>
-      </c>
+      <c r="C14" s="11"/>
       <c r="D14" s="28" t="s">
         <v>81</v>
       </c>
@@ -1868,16 +1842,14 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="10" t="n">
         <v>13</v>
       </c>
       <c r="B15" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="C15" s="11" t="s">
-        <v>63</v>
-      </c>
+      <c r="C15" s="11"/>
       <c r="D15" s="28" t="s">
         <v>83</v>
       </c>
@@ -1912,16 +1884,14 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="10" t="n">
         <v>14</v>
       </c>
       <c r="B16" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="C16" s="11" t="s">
-        <v>63</v>
-      </c>
+      <c r="C16" s="11"/>
       <c r="D16" s="28" t="s">
         <v>84</v>
       </c>
@@ -1956,16 +1926,14 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="10" t="n">
         <v>15</v>
       </c>
       <c r="B17" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="C17" s="11" t="s">
-        <v>63</v>
-      </c>
+      <c r="C17" s="11"/>
       <c r="D17" s="28" t="s">
         <v>85</v>
       </c>
@@ -2000,16 +1968,14 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="10" t="n">
         <v>16</v>
       </c>
       <c r="B18" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="C18" s="11" t="s">
-        <v>63</v>
-      </c>
+      <c r="C18" s="11"/>
       <c r="D18" s="28" t="s">
         <v>86</v>
       </c>
@@ -2044,16 +2010,14 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="10" t="n">
         <v>17</v>
       </c>
       <c r="B19" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="C19" s="11" t="s">
-        <v>63</v>
-      </c>
+      <c r="C19" s="11"/>
       <c r="D19" s="28" t="s">
         <v>87</v>
       </c>
@@ -2088,16 +2052,14 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="10" t="n">
         <v>18</v>
       </c>
       <c r="B20" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="C20" s="11" t="s">
-        <v>63</v>
-      </c>
+      <c r="C20" s="11"/>
       <c r="D20" s="28" t="s">
         <v>88</v>
       </c>
@@ -2134,16 +2096,14 @@
         <v>28</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="10" t="n">
         <v>19</v>
       </c>
       <c r="B21" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="C21" s="11" t="s">
-        <v>63</v>
-      </c>
+      <c r="C21" s="11"/>
       <c r="D21" s="28" t="s">
         <v>93</v>
       </c>
@@ -2180,16 +2140,14 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="10" t="n">
         <v>20</v>
       </c>
       <c r="B22" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="C22" s="11" t="s">
-        <v>63</v>
-      </c>
+      <c r="C22" s="11"/>
       <c r="D22" s="28" t="s">
         <v>96</v>
       </c>
@@ -2226,16 +2184,14 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="10" t="n">
         <v>21</v>
       </c>
       <c r="B23" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="C23" s="11" t="s">
-        <v>63</v>
-      </c>
+      <c r="C23" s="11"/>
       <c r="D23" s="28" t="s">
         <v>100</v>
       </c>
@@ -2272,16 +2228,14 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="10" t="n">
         <v>22</v>
       </c>
       <c r="B24" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="C24" s="34" t="s">
-        <v>63</v>
-      </c>
+      <c r="C24" s="34"/>
       <c r="D24" s="35" t="s">
         <v>103</v>
       </c>
@@ -2318,16 +2272,14 @@
         <v>28</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="10" t="n">
         <v>23</v>
       </c>
       <c r="B25" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="C25" s="34" t="s">
-        <v>63</v>
-      </c>
+      <c r="C25" s="34"/>
       <c r="D25" s="35" t="s">
         <v>106</v>
       </c>
@@ -2364,16 +2316,14 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="10" t="n">
         <v>24</v>
       </c>
       <c r="B26" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="C26" s="11" t="s">
-        <v>109</v>
-      </c>
+      <c r="C26" s="11"/>
       <c r="D26" s="28" t="s">
         <v>110</v>
       </c>
@@ -2410,16 +2360,14 @@
         <v>28</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="10" t="n">
         <v>25</v>
       </c>
       <c r="B27" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="C27" s="11" t="s">
-        <v>109</v>
-      </c>
+      <c r="C27" s="11"/>
       <c r="D27" s="28" t="s">
         <v>112</v>
       </c>
@@ -2456,16 +2404,14 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="10" t="n">
         <v>26</v>
       </c>
       <c r="B28" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="C28" s="11" t="s">
-        <v>109</v>
-      </c>
+      <c r="C28" s="11"/>
       <c r="D28" s="28" t="s">
         <v>114</v>
       </c>
@@ -2502,16 +2448,14 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="10" t="n">
         <v>27</v>
       </c>
       <c r="B29" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="C29" s="11" t="s">
-        <v>109</v>
-      </c>
+      <c r="C29" s="11"/>
       <c r="D29" s="28" t="s">
         <v>81</v>
       </c>
@@ -2546,16 +2490,14 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="10" t="n">
         <v>28</v>
       </c>
       <c r="B30" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="C30" s="11" t="s">
-        <v>109</v>
-      </c>
+      <c r="C30" s="11"/>
       <c r="D30" s="28" t="s">
         <v>83</v>
       </c>
@@ -2590,16 +2532,14 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="10" t="n">
         <v>29</v>
       </c>
       <c r="B31" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="C31" s="11" t="s">
-        <v>109</v>
-      </c>
+      <c r="C31" s="11"/>
       <c r="D31" s="28" t="s">
         <v>84</v>
       </c>
@@ -2634,16 +2574,14 @@
         <v>28</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="10" t="n">
         <v>30</v>
       </c>
       <c r="B32" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="C32" s="11" t="s">
-        <v>109</v>
-      </c>
+      <c r="C32" s="11"/>
       <c r="D32" s="28" t="s">
         <v>85</v>
       </c>
@@ -2678,16 +2616,14 @@
         <v>28</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="10" t="n">
         <v>31</v>
       </c>
       <c r="B33" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="C33" s="11" t="s">
-        <v>109</v>
-      </c>
+      <c r="C33" s="11"/>
       <c r="D33" s="28" t="s">
         <v>86</v>
       </c>
@@ -2722,16 +2658,14 @@
         <v>28</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="10" t="n">
         <v>32</v>
       </c>
       <c r="B34" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="C34" s="11" t="s">
-        <v>109</v>
-      </c>
+      <c r="C34" s="11"/>
       <c r="D34" s="28" t="s">
         <v>87</v>
       </c>
@@ -2766,16 +2700,14 @@
         <v>28</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="10" t="n">
         <v>33</v>
       </c>
       <c r="B35" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="C35" s="11" t="s">
-        <v>109</v>
-      </c>
+      <c r="C35" s="11"/>
       <c r="D35" s="28" t="s">
         <v>116</v>
       </c>
@@ -2814,16 +2746,14 @@
         <v>28</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="10" t="n">
         <v>34</v>
       </c>
       <c r="B36" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="C36" s="11" t="s">
-        <v>109</v>
-      </c>
+      <c r="C36" s="11"/>
       <c r="D36" s="28" t="s">
         <v>119</v>
       </c>
@@ -2860,16 +2790,14 @@
         <v>28</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="10" t="n">
         <v>35</v>
       </c>
       <c r="B37" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="C37" s="11" t="s">
-        <v>109</v>
-      </c>
+      <c r="C37" s="11"/>
       <c r="D37" s="28" t="s">
         <v>121</v>
       </c>
@@ -2908,16 +2836,14 @@
         <v>28</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="10" t="n">
         <v>36</v>
       </c>
       <c r="B38" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="C38" s="11" t="s">
-        <v>109</v>
-      </c>
+      <c r="C38" s="11"/>
       <c r="D38" s="28" t="s">
         <v>123</v>
       </c>
@@ -2954,16 +2880,14 @@
         <v>28</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="10" t="n">
         <v>37</v>
       </c>
       <c r="B39" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="C39" s="11" t="s">
-        <v>109</v>
-      </c>
+      <c r="C39" s="11"/>
       <c r="D39" s="35" t="s">
         <v>125</v>
       </c>
@@ -3000,16 +2924,14 @@
         <v>28</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="10" t="n">
         <v>38</v>
       </c>
       <c r="B40" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="C40" s="11" t="s">
-        <v>109</v>
-      </c>
+      <c r="C40" s="11"/>
       <c r="D40" s="35" t="s">
         <v>127</v>
       </c>
@@ -3046,16 +2968,14 @@
         <v>28</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="10" t="n">
         <v>39</v>
       </c>
       <c r="B41" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="C41" s="11" t="s">
-        <v>129</v>
-      </c>
+      <c r="C41" s="11"/>
       <c r="D41" s="28" t="s">
         <v>130</v>
       </c>
@@ -3092,16 +3012,14 @@
         <v>28</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="10" t="n">
         <v>40</v>
       </c>
       <c r="B42" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="C42" s="11" t="s">
-        <v>129</v>
-      </c>
+      <c r="C42" s="11"/>
       <c r="D42" s="28" t="s">
         <v>132</v>
       </c>
@@ -3138,16 +3056,14 @@
         <v>28</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="10" t="n">
         <v>41</v>
       </c>
       <c r="B43" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="C43" s="11" t="s">
-        <v>129</v>
-      </c>
+      <c r="C43" s="11"/>
       <c r="D43" s="28" t="s">
         <v>134</v>
       </c>
@@ -3184,16 +3100,14 @@
         <v>28</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="10" t="n">
         <v>42</v>
       </c>
       <c r="B44" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="C44" s="11" t="s">
-        <v>129</v>
-      </c>
+      <c r="C44" s="11"/>
       <c r="D44" s="28" t="s">
         <v>81</v>
       </c>
@@ -3228,16 +3142,14 @@
         <v>28</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="10" t="n">
         <v>43</v>
       </c>
       <c r="B45" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="C45" s="11" t="s">
-        <v>129</v>
-      </c>
+      <c r="C45" s="11"/>
       <c r="D45" s="28" t="s">
         <v>83</v>
       </c>
@@ -3272,16 +3184,14 @@
         <v>28</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="10" t="n">
         <v>44</v>
       </c>
       <c r="B46" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="C46" s="11" t="s">
-        <v>129</v>
-      </c>
+      <c r="C46" s="11"/>
       <c r="D46" s="28" t="s">
         <v>84</v>
       </c>
@@ -3316,16 +3226,14 @@
         <v>28</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="10" t="n">
         <v>45</v>
       </c>
       <c r="B47" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="C47" s="11" t="s">
-        <v>129</v>
-      </c>
+      <c r="C47" s="11"/>
       <c r="D47" s="28" t="s">
         <v>85</v>
       </c>
@@ -3360,16 +3268,14 @@
         <v>28</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="10" t="n">
         <v>46</v>
       </c>
       <c r="B48" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="C48" s="11" t="s">
-        <v>129</v>
-      </c>
+      <c r="C48" s="11"/>
       <c r="D48" s="28" t="s">
         <v>86</v>
       </c>
@@ -3404,16 +3310,14 @@
         <v>28</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="10" t="n">
         <v>47</v>
       </c>
       <c r="B49" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="C49" s="11" t="s">
-        <v>129</v>
-      </c>
+      <c r="C49" s="11"/>
       <c r="D49" s="28" t="s">
         <v>87</v>
       </c>
@@ -3448,16 +3352,14 @@
         <v>28</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="10" t="n">
         <v>48</v>
       </c>
       <c r="B50" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="C50" s="11" t="s">
-        <v>129</v>
-      </c>
+      <c r="C50" s="11"/>
       <c r="D50" s="28" t="s">
         <v>136</v>
       </c>
@@ -3496,16 +3398,14 @@
         <v>28</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="10" t="n">
         <v>49</v>
       </c>
       <c r="B51" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="C51" s="11" t="s">
-        <v>129</v>
-      </c>
+      <c r="C51" s="11"/>
       <c r="D51" s="28" t="s">
         <v>138</v>
       </c>
@@ -3542,16 +3442,14 @@
         <v>28</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="10" t="n">
         <v>50</v>
       </c>
       <c r="B52" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="C52" s="11" t="s">
-        <v>129</v>
-      </c>
+      <c r="C52" s="11"/>
       <c r="D52" s="28" t="s">
         <v>140</v>
       </c>
@@ -3590,16 +3488,14 @@
         <v>28</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="10" t="n">
         <v>51</v>
       </c>
       <c r="B53" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="C53" s="11" t="s">
-        <v>129</v>
-      </c>
+      <c r="C53" s="11"/>
       <c r="D53" s="28" t="s">
         <v>142</v>
       </c>
@@ -3635,16 +3531,14 @@
         <v>28</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="10" t="n">
         <v>52</v>
       </c>
       <c r="B54" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="C54" s="11" t="s">
-        <v>129</v>
-      </c>
+      <c r="C54" s="11"/>
       <c r="D54" s="35" t="s">
         <v>144</v>
       </c>
@@ -3681,16 +3575,14 @@
         <v>28</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="10" t="n">
         <v>53</v>
       </c>
       <c r="B55" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="C55" s="11" t="s">
-        <v>129</v>
-      </c>
+      <c r="C55" s="11"/>
       <c r="D55" s="35" t="s">
         <v>146</v>
       </c>

</xml_diff>

<commit_message>
further progress on excel
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/euTaxonomyNonFinancials/EutaxonomyNonFinancials.xlsx
+++ b/dataland-framework-toolbox/inputs/euTaxonomyNonFinancials/EutaxonomyNonFinancials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d92432\Documents\Projekte\02-Dataland\Dataland\dataland-framework-toolbox\inputs\euTaxonomyNonFinancials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA0EC660-67D9-486A-BBF9-111EDB31EBCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{760E8EE2-5509-4F1E-8774-0D2E6C82F2FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="38640" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="158">
   <si>
     <t>Field Identifier</t>
   </si>
@@ -299,9 +299,6 @@
     <t>Substantial Contribution to Protection and Restoration of Biodiversity and Ecosystems</t>
   </si>
   <si>
-    <t>Aligned Revenue per Activity</t>
-  </si>
-  <si>
     <t>Absolute value and share of the revenue per activity that is taxonomy-aligned, i.e., generated by an eligible economic activity that is making a substantial contribution to at least one of the climate and environmental objectives, while also doing no significant harm to the remaining objectives and meeting minimum standards on human rights and labour standards</t>
   </si>
   <si>
@@ -314,48 +311,24 @@
     <t>alignedActivities</t>
   </si>
   <si>
-    <t>Non-Aligned Revenue</t>
-  </si>
-  <si>
-    <t>Absolute value and share of the revenue that is associated with non taxonomy-aligned but eligible activities</t>
-  </si>
-  <si>
     <t>nonAlignedShare</t>
   </si>
   <si>
-    <t>Non-Aligned Revenue per Activity</t>
-  </si>
-  <si>
-    <t>Absolute value and share of the revenue per activity that is not taxonomy-aligned but eligible</t>
-  </si>
-  <si>
     <t>NonAlignedActivitiesFormField</t>
   </si>
   <si>
     <t>nonAlignedActivities</t>
   </si>
   <si>
-    <t>Non-Eligible Revenue</t>
-  </si>
-  <si>
-    <t>Absolute value and share of the revenue that is not part of a plan to meet the DNSH criteria and make substantial contribution to any environmental objective</t>
-  </si>
-  <si>
     <t>nonEligibleShare</t>
   </si>
   <si>
-    <t>Enabling Revenue</t>
-  </si>
-  <si>
     <t>Share of the taxonomy-aligned revenue from total aligned revenue that is linked to activities that enable reduction of GHG in other sectors</t>
   </si>
   <si>
     <t>enablingShareInPercent</t>
   </si>
   <si>
-    <t>Transitional Revenue</t>
-  </si>
-  <si>
     <t>Share of the taxonomy-aligned revenue from total aligned revenue that is linked to activities with significantly lower GHG emissions than the sector or industry average</t>
   </si>
   <si>
@@ -510,6 +483,54 @@
   </si>
   <si>
     <t>11.2</t>
+  </si>
+  <si>
+    <t>Non-Aligned Activities</t>
+  </si>
+  <si>
+    <t>Custom - List of EuTaxonomyActivity</t>
+  </si>
+  <si>
+    <t>Aligned Share</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Climate Change Mitigation In Percent</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Climate Change Adaptation In Percent</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Sustainable Use and Protection of Water and Marine Resources In Percent</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Transition to a Circular Economy In Percent</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Pollution Prevention and Control In Percent</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Protection and Restoration of Biodiversity and Ecosystems In Percent</t>
+  </si>
+  <si>
+    <t>Aligned Activities</t>
+  </si>
+  <si>
+    <t>Custom - AlignedActivitiesFormField</t>
+  </si>
+  <si>
+    <t>Enabling Share In Percent</t>
+  </si>
+  <si>
+    <t>Transitional Share In Percent</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>13.1</t>
+  </si>
+  <si>
+    <t>13.2</t>
   </si>
 </sst>
 </file>
@@ -1209,7 +1230,7 @@
   <dimension ref="A1:T58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1639,18 +1660,18 @@
       </c>
       <c r="C10" s="11"/>
       <c r="D10" s="24" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="E10" s="36" t="s">
         <v>61</v>
       </c>
       <c r="F10" s="38" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="G10" s="40"/>
       <c r="H10" s="15"/>
       <c r="I10" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J10" s="15"/>
       <c r="K10" s="15"/>
@@ -1682,16 +1703,16 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A11" s="34" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="E11" s="36"/>
       <c r="F11" s="38" t="s">
@@ -1714,20 +1735,20 @@
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A12" s="34" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="B12" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="D12" s="24" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="E12" s="36"/>
       <c r="F12" s="38" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="G12" s="40"/>
       <c r="H12" s="15"/>
@@ -1746,16 +1767,16 @@
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A13" s="34" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="B13" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="D13" s="24" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="E13" s="15"/>
       <c r="F13" s="38" t="s">
@@ -1794,20 +1815,20 @@
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A14" s="34" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="B14" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="D14" s="24" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="E14" s="15"/>
       <c r="F14" s="38" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="G14" s="40"/>
       <c r="H14" s="15"/>
@@ -1826,16 +1847,16 @@
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A15" s="34" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="B15" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="D15" s="24" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="E15" s="15"/>
       <c r="F15" s="38" t="s">
@@ -1858,20 +1879,20 @@
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A16" s="34" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B16" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="D16" s="24" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="E16" s="15"/>
       <c r="F16" s="38" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="G16" s="40"/>
       <c r="H16" s="15"/>
@@ -1903,21 +1924,19 @@
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A17" s="10">
-        <v>12</v>
+      <c r="A17" s="34" t="s">
+        <v>155</v>
       </c>
       <c r="B17" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C17" s="11"/>
       <c r="D17" s="24" t="s">
-        <v>73</v>
-      </c>
-      <c r="E17" s="15" t="s">
-        <v>74</v>
-      </c>
+        <v>142</v>
+      </c>
+      <c r="E17" s="15"/>
       <c r="F17" s="38" t="s">
-        <v>50</v>
+        <v>143</v>
       </c>
       <c r="G17" s="40"/>
       <c r="H17" s="15"/>
@@ -1925,39 +1944,29 @@
       <c r="J17" s="15"/>
       <c r="K17" s="15"/>
       <c r="L17" s="15"/>
-      <c r="M17" s="15" t="s">
-        <v>62</v>
-      </c>
+      <c r="M17" s="15"/>
       <c r="N17" s="15"/>
       <c r="O17" s="15"/>
-      <c r="P17" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q17" s="13" t="s">
-        <v>34</v>
-      </c>
+      <c r="P17" s="15"/>
+      <c r="Q17" s="13"/>
       <c r="R17" s="27"/>
-      <c r="S17" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="T17" s="29" t="s">
-        <v>28</v>
-      </c>
+      <c r="S17" s="28"/>
+      <c r="T17" s="29"/>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A18" s="10">
-        <v>13</v>
+      <c r="A18" s="34" t="s">
+        <v>156</v>
       </c>
       <c r="B18" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="C18" s="11"/>
+      <c r="C18" s="11" t="s">
+        <v>144</v>
+      </c>
       <c r="D18" s="24" t="s">
-        <v>75</v>
-      </c>
-      <c r="E18" s="15" t="s">
-        <v>74</v>
-      </c>
+        <v>132</v>
+      </c>
+      <c r="E18" s="15"/>
       <c r="F18" s="38" t="s">
         <v>50</v>
       </c>
@@ -1967,41 +1976,31 @@
       <c r="J18" s="15"/>
       <c r="K18" s="15"/>
       <c r="L18" s="15"/>
-      <c r="M18" s="15" t="s">
-        <v>62</v>
-      </c>
+      <c r="M18" s="15"/>
       <c r="N18" s="15"/>
       <c r="O18" s="15"/>
-      <c r="P18" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q18" s="13" t="s">
-        <v>34</v>
-      </c>
+      <c r="P18" s="15"/>
+      <c r="Q18" s="13"/>
       <c r="R18" s="27"/>
-      <c r="S18" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="T18" s="29" t="s">
-        <v>28</v>
-      </c>
+      <c r="S18" s="28"/>
+      <c r="T18" s="29"/>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A19" s="10">
-        <v>14</v>
+      <c r="A19" s="34" t="s">
+        <v>157</v>
       </c>
       <c r="B19" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="C19" s="11"/>
+      <c r="C19" s="11" t="s">
+        <v>144</v>
+      </c>
       <c r="D19" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="E19" s="15" t="s">
-        <v>74</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="E19" s="15"/>
       <c r="F19" s="38" t="s">
-        <v>50</v>
+        <v>129</v>
       </c>
       <c r="G19" s="40"/>
       <c r="H19" s="15"/>
@@ -2009,35 +2008,25 @@
       <c r="J19" s="15"/>
       <c r="K19" s="15"/>
       <c r="L19" s="15"/>
-      <c r="M19" s="15" t="s">
-        <v>62</v>
-      </c>
+      <c r="M19" s="15"/>
       <c r="N19" s="15"/>
       <c r="O19" s="15"/>
-      <c r="P19" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q19" s="13" t="s">
-        <v>34</v>
-      </c>
+      <c r="P19" s="15"/>
+      <c r="Q19" s="13"/>
       <c r="R19" s="27"/>
-      <c r="S19" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="T19" s="29" t="s">
-        <v>28</v>
-      </c>
+      <c r="S19" s="28"/>
+      <c r="T19" s="29"/>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A20" s="10">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B20" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C20" s="11"/>
       <c r="D20" s="24" t="s">
-        <v>77</v>
+        <v>145</v>
       </c>
       <c r="E20" s="15" t="s">
         <v>74</v>
@@ -2072,14 +2061,14 @@
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A21" s="10">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B21" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C21" s="11"/>
       <c r="D21" s="24" t="s">
-        <v>78</v>
+        <v>146</v>
       </c>
       <c r="E21" s="15" t="s">
         <v>74</v>
@@ -2114,14 +2103,14 @@
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A22" s="10">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B22" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C22" s="11"/>
       <c r="D22" s="24" t="s">
-        <v>79</v>
+        <v>147</v>
       </c>
       <c r="E22" s="15" t="s">
         <v>74</v>
@@ -2156,20 +2145,20 @@
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A23" s="10">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B23" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C23" s="11"/>
       <c r="D23" s="24" t="s">
-        <v>80</v>
+        <v>148</v>
       </c>
       <c r="E23" s="15" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="F23" s="38" t="s">
-        <v>82</v>
+        <v>50</v>
       </c>
       <c r="G23" s="40"/>
       <c r="H23" s="15"/>
@@ -2177,7 +2166,9 @@
       <c r="J23" s="15"/>
       <c r="K23" s="15"/>
       <c r="L23" s="15"/>
-      <c r="M23" s="15"/>
+      <c r="M23" s="15" t="s">
+        <v>62</v>
+      </c>
       <c r="N23" s="15"/>
       <c r="O23" s="15"/>
       <c r="P23" s="15" t="s">
@@ -2186,9 +2177,7 @@
       <c r="Q23" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="R23" s="27" t="s">
-        <v>84</v>
-      </c>
+      <c r="R23" s="27"/>
       <c r="S23" s="28" t="s">
         <v>28</v>
       </c>
@@ -2198,20 +2187,20 @@
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A24" s="10">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B24" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C24" s="11"/>
       <c r="D24" s="24" t="s">
-        <v>85</v>
+        <v>149</v>
       </c>
       <c r="E24" s="15" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="F24" s="38" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="G24" s="40"/>
       <c r="H24" s="15"/>
@@ -2230,9 +2219,7 @@
       <c r="Q24" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="R24" s="27" t="s">
-        <v>87</v>
-      </c>
+      <c r="R24" s="27"/>
       <c r="S24" s="28" t="s">
         <v>28</v>
       </c>
@@ -2242,20 +2229,20 @@
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A25" s="10">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B25" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C25" s="11"/>
       <c r="D25" s="24" t="s">
-        <v>88</v>
+        <v>150</v>
       </c>
       <c r="E25" s="15" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="F25" s="38" t="s">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="G25" s="40"/>
       <c r="H25" s="15"/>
@@ -2263,7 +2250,9 @@
       <c r="J25" s="15"/>
       <c r="K25" s="15"/>
       <c r="L25" s="15"/>
-      <c r="M25" s="15"/>
+      <c r="M25" s="15" t="s">
+        <v>62</v>
+      </c>
       <c r="N25" s="15"/>
       <c r="O25" s="15"/>
       <c r="P25" s="15" t="s">
@@ -2272,9 +2261,7 @@
       <c r="Q25" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="R25" s="27" t="s">
-        <v>91</v>
-      </c>
+      <c r="R25" s="27"/>
       <c r="S25" s="28" t="s">
         <v>28</v>
       </c>
@@ -2284,20 +2271,20 @@
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A26" s="10">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B26" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C26" s="11"/>
       <c r="D26" s="24" t="s">
-        <v>92</v>
+        <v>151</v>
       </c>
       <c r="E26" s="15" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="F26" s="38" t="s">
-        <v>50</v>
+        <v>152</v>
       </c>
       <c r="G26" s="40"/>
       <c r="H26" s="15"/>
@@ -2305,9 +2292,7 @@
       <c r="J26" s="15"/>
       <c r="K26" s="15"/>
       <c r="L26" s="15"/>
-      <c r="M26" s="15" t="s">
-        <v>62</v>
-      </c>
+      <c r="M26" s="15"/>
       <c r="N26" s="15"/>
       <c r="O26" s="15"/>
       <c r="P26" s="15" t="s">
@@ -2317,7 +2302,7 @@
         <v>34</v>
       </c>
       <c r="R26" s="27" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="S26" s="28" t="s">
         <v>28</v>
@@ -2328,17 +2313,17 @@
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A27" s="10">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B27" s="30" t="s">
         <v>60</v>
       </c>
       <c r="C27" s="30"/>
       <c r="D27" s="31" t="s">
-        <v>95</v>
+        <v>153</v>
       </c>
       <c r="E27" s="15" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="F27" s="38" t="s">
         <v>50</v>
@@ -2361,7 +2346,7 @@
         <v>34</v>
       </c>
       <c r="R27" s="27" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="S27" s="32" t="s">
         <v>28</v>
@@ -2372,17 +2357,17 @@
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A28" s="10">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B28" s="30" t="s">
         <v>60</v>
       </c>
       <c r="C28" s="30"/>
       <c r="D28" s="31" t="s">
-        <v>98</v>
+        <v>154</v>
       </c>
       <c r="E28" s="15" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="F28" s="38" t="s">
         <v>50</v>
@@ -2405,7 +2390,7 @@
         <v>34</v>
       </c>
       <c r="R28" s="27" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="S28" s="32" t="s">
         <v>28</v>
@@ -2419,14 +2404,14 @@
         <v>24</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="C29" s="11"/>
       <c r="D29" s="24" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="E29" s="15" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="F29" s="38" t="s">
         <v>50</v>
@@ -2463,14 +2448,14 @@
         <v>25</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="C30" s="11"/>
       <c r="D30" s="24" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="E30" s="15" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="F30" s="38" t="s">
         <v>50</v>
@@ -2507,14 +2492,14 @@
         <v>26</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="C31" s="11"/>
       <c r="D31" s="24" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="E31" s="15" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="F31" s="38" t="s">
         <v>50</v>
@@ -2551,7 +2536,7 @@
         <v>27</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="C32" s="11"/>
       <c r="D32" s="24" t="s">
@@ -2593,7 +2578,7 @@
         <v>28</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="C33" s="11"/>
       <c r="D33" s="24" t="s">
@@ -2635,7 +2620,7 @@
         <v>29</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="C34" s="11"/>
       <c r="D34" s="24" t="s">
@@ -2677,7 +2662,7 @@
         <v>30</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="C35" s="11"/>
       <c r="D35" s="24" t="s">
@@ -2719,7 +2704,7 @@
         <v>31</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="C36" s="11"/>
       <c r="D36" s="24" t="s">
@@ -2761,7 +2746,7 @@
         <v>32</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="C37" s="11"/>
       <c r="D37" s="24" t="s">
@@ -2803,20 +2788,20 @@
         <v>33</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="C38" s="11"/>
       <c r="D38" s="24" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="E38" s="15" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="F38" s="38" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G38" s="40" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="H38" s="15"/>
       <c r="I38" s="15"/>
@@ -2833,7 +2818,7 @@
         <v>34</v>
       </c>
       <c r="R38" s="27" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="S38" s="28" t="s">
         <v>28</v>
@@ -2847,14 +2832,14 @@
         <v>34</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="C39" s="11"/>
       <c r="D39" s="24" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="E39" s="15" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="F39" s="38" t="s">
         <v>50</v>
@@ -2877,7 +2862,7 @@
         <v>34</v>
       </c>
       <c r="R39" s="27" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="S39" s="28" t="s">
         <v>28</v>
@@ -2891,20 +2876,20 @@
         <v>35</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="C40" s="11"/>
       <c r="D40" s="24" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="E40" s="15" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="F40" s="38" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="G40" s="40" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="H40" s="15"/>
       <c r="I40" s="15"/>
@@ -2921,7 +2906,7 @@
         <v>34</v>
       </c>
       <c r="R40" s="27" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="S40" s="28" t="s">
         <v>28</v>
@@ -2935,14 +2920,14 @@
         <v>36</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="C41" s="11"/>
       <c r="D41" s="24" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="E41" s="15" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="F41" s="38" t="s">
         <v>50</v>
@@ -2965,7 +2950,7 @@
         <v>34</v>
       </c>
       <c r="R41" s="27" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="S41" s="28" t="s">
         <v>28</v>
@@ -2979,14 +2964,14 @@
         <v>37</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="C42" s="11"/>
       <c r="D42" s="31" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="E42" s="15" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="F42" s="38" t="s">
         <v>50</v>
@@ -3009,7 +2994,7 @@
         <v>34</v>
       </c>
       <c r="R42" s="27" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="S42" s="32" t="s">
         <v>28</v>
@@ -3023,14 +3008,14 @@
         <v>38</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="C43" s="11"/>
       <c r="D43" s="31" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="E43" s="15" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="F43" s="38" t="s">
         <v>50</v>
@@ -3053,7 +3038,7 @@
         <v>34</v>
       </c>
       <c r="R43" s="27" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="S43" s="32" t="s">
         <v>28</v>
@@ -3067,14 +3052,14 @@
         <v>39</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="C44" s="11"/>
       <c r="D44" s="24" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="E44" s="15" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="F44" s="38" t="s">
         <v>62</v>
@@ -3111,14 +3096,14 @@
         <v>40</v>
       </c>
       <c r="B45" s="11" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="C45" s="11"/>
       <c r="D45" s="24" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="E45" s="15" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="F45" s="38" t="s">
         <v>50</v>
@@ -3155,14 +3140,14 @@
         <v>41</v>
       </c>
       <c r="B46" s="11" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="C46" s="11"/>
       <c r="D46" s="24" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="E46" s="15" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="F46" s="38" t="s">
         <v>50</v>
@@ -3199,7 +3184,7 @@
         <v>42</v>
       </c>
       <c r="B47" s="11" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="C47" s="11"/>
       <c r="D47" s="24" t="s">
@@ -3241,7 +3226,7 @@
         <v>43</v>
       </c>
       <c r="B48" s="11" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="C48" s="11"/>
       <c r="D48" s="24" t="s">
@@ -3283,7 +3268,7 @@
         <v>44</v>
       </c>
       <c r="B49" s="11" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="C49" s="11"/>
       <c r="D49" s="24" t="s">
@@ -3325,7 +3310,7 @@
         <v>45</v>
       </c>
       <c r="B50" s="11" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="C50" s="11"/>
       <c r="D50" s="24" t="s">
@@ -3367,7 +3352,7 @@
         <v>46</v>
       </c>
       <c r="B51" s="11" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="C51" s="11"/>
       <c r="D51" s="24" t="s">
@@ -3409,7 +3394,7 @@
         <v>47</v>
       </c>
       <c r="B52" s="11" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="C52" s="11"/>
       <c r="D52" s="24" t="s">
@@ -3451,20 +3436,20 @@
         <v>48</v>
       </c>
       <c r="B53" s="11" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="C53" s="11"/>
       <c r="D53" s="24" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="E53" s="15" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="F53" s="38" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G53" s="40" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="H53" s="15"/>
       <c r="I53" s="15"/>
@@ -3481,7 +3466,7 @@
         <v>34</v>
       </c>
       <c r="R53" s="27" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="S53" s="28" t="s">
         <v>28</v>
@@ -3495,14 +3480,14 @@
         <v>49</v>
       </c>
       <c r="B54" s="11" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="C54" s="11"/>
       <c r="D54" s="24" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="E54" s="15" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="F54" s="38" t="s">
         <v>50</v>
@@ -3525,7 +3510,7 @@
         <v>34</v>
       </c>
       <c r="R54" s="27" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="S54" s="28" t="s">
         <v>28</v>
@@ -3539,20 +3524,20 @@
         <v>50</v>
       </c>
       <c r="B55" s="11" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="C55" s="11"/>
       <c r="D55" s="24" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="E55" s="15" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="F55" s="38" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="G55" s="40" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="H55" s="15"/>
       <c r="I55" s="15"/>
@@ -3569,7 +3554,7 @@
         <v>34</v>
       </c>
       <c r="R55" s="27" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="S55" s="28" t="s">
         <v>28</v>
@@ -3583,14 +3568,14 @@
         <v>51</v>
       </c>
       <c r="B56" s="11" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="C56" s="11"/>
       <c r="D56" s="24" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="E56" s="15" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="F56" s="38" t="s">
         <v>50</v>
@@ -3613,7 +3598,7 @@
         <v>34</v>
       </c>
       <c r="R56" s="27" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="S56" s="28" t="s">
         <v>28</v>
@@ -3627,14 +3612,14 @@
         <v>52</v>
       </c>
       <c r="B57" s="11" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="C57" s="11"/>
       <c r="D57" s="31" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="E57" s="15" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="F57" s="38" t="s">
         <v>50</v>
@@ -3657,7 +3642,7 @@
         <v>34</v>
       </c>
       <c r="R57" s="27" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="S57" s="32" t="s">
         <v>28</v>
@@ -3671,14 +3656,14 @@
         <v>53</v>
       </c>
       <c r="B58" s="11" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="C58" s="11"/>
       <c r="D58" s="31" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="E58" s="15" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="F58" s="38" t="s">
         <v>50</v>
@@ -3701,7 +3686,7 @@
         <v>34</v>
       </c>
       <c r="R58" s="27" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="S58" s="32" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
more and more progress on excel
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/euTaxonomyNonFinancials/EutaxonomyNonFinancials.xlsx
+++ b/dataland-framework-toolbox/inputs/euTaxonomyNonFinancials/EutaxonomyNonFinancials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d92432\Documents\Projekte\02-Dataland\Dataland\dataland-framework-toolbox\inputs\euTaxonomyNonFinancials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{760E8EE2-5509-4F1E-8774-0D2E6C82F2FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C7CA0C9-4CB5-4B28-968D-EE6EBCED466D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="38640" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="129">
   <si>
     <t>Field Identifier</t>
   </si>
@@ -242,9 +242,6 @@
     <t>Revenue</t>
   </si>
   <si>
-    <t>Total revenue per annum</t>
-  </si>
-  <si>
     <t>Number</t>
   </si>
   <si>
@@ -278,33 +275,9 @@
     <t>alignedShare</t>
   </si>
   <si>
-    <t>Substantial Contribution to Climate Change Mitigation</t>
-  </si>
-  <si>
     <t>Grade of the substantial contribution criterion fulfillment</t>
   </si>
   <si>
-    <t>Substantial Contribution to Climate Change Adaptation</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to Sustainable Use and Protection of Water and Marine Resources</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to Transition to a Circular Economy</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to Pollution Prevention and Control</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to Protection and Restoration of Biodiversity and Ecosystems</t>
-  </si>
-  <si>
-    <t>Absolute value and share of the revenue per activity that is taxonomy-aligned, i.e., generated by an eligible economic activity that is making a substantial contribution to at least one of the climate and environmental objectives, while also doing no significant harm to the remaining objectives and meeting minimum standards on human rights and labour standards</t>
-  </si>
-  <si>
-    <t>AlignedActivitiesFormField</t>
-  </si>
-  <si>
     <t>Extended</t>
   </si>
   <si>
@@ -314,138 +287,24 @@
     <t>nonAlignedShare</t>
   </si>
   <si>
-    <t>NonAlignedActivitiesFormField</t>
-  </si>
-  <si>
     <t>nonAlignedActivities</t>
   </si>
   <si>
     <t>nonEligibleShare</t>
   </si>
   <si>
-    <t>Share of the taxonomy-aligned revenue from total aligned revenue that is linked to activities that enable reduction of GHG in other sectors</t>
-  </si>
-  <si>
     <t>enablingShareInPercent</t>
   </si>
   <si>
-    <t>Share of the taxonomy-aligned revenue from total aligned revenue that is linked to activities with significantly lower GHG emissions than the sector or industry average</t>
-  </si>
-  <si>
     <t>transitionalShareInPercent</t>
   </si>
   <si>
     <t>CapEx</t>
   </si>
   <si>
-    <t xml:space="preserve">Total CapEx for the reported year. Capital expenditures are non-consumable investments, e.g. for acquiring, upgrading, and maintaining physical assets such as property, plants, buildings, technology </t>
-  </si>
-  <si>
-    <t>Eligible CapEx</t>
-  </si>
-  <si>
-    <t>Absolute value and share of the total CapEx where the economic activity meets taxonomy criteria for substantial contribution to climate change mitigation and does no serious harm to the other environmental objectives (DNSH criteria)</t>
-  </si>
-  <si>
-    <t>Aligned CapEx</t>
-  </si>
-  <si>
-    <t>Absolute value and share of CapEx that is taxonomy-aligned, i.e., generated by an eligible economic activity that is making a substantial contribution to at least one of the climate and environmental objectives, while also doing no significant harm to the remaining objectives and meeting minimum standards on human rights and labour standards.</t>
-  </si>
-  <si>
-    <t>Aligned CapEx per Activity</t>
-  </si>
-  <si>
-    <t>Absolute value and share of the CapEx per activity that is taxonomy-aligned, i.e., generated by an eligible economic activity that is making a substantial contribution to at least one of the climate and environmental objectives, while also doing no significant harm to the remaining objectives and meeting minimum standards on human rights and labour standards</t>
-  </si>
-  <si>
-    <t>Allowed Range: [0, 100]</t>
-  </si>
-  <si>
-    <t>Non-Aligned CapEx</t>
-  </si>
-  <si>
-    <t>Absolute value and share of the CapEx that is associated with non taxonomy-aligned but eligible activities</t>
-  </si>
-  <si>
-    <t>Non-Aligned CapEx per Activity</t>
-  </si>
-  <si>
-    <t>Absolute value and share of the CapEx per activity that is not taxonomy-aligned but eligible</t>
-  </si>
-  <si>
-    <t>Non-Eligible CapEx</t>
-  </si>
-  <si>
-    <t>Absolute value and share of the CapEx that is not part of a plan to meet the DNSH criteria and make substantial contribution to any environmental objective</t>
-  </si>
-  <si>
-    <t>Enabling CapEx</t>
-  </si>
-  <si>
-    <t>Share of the taxonomy-aligned CapEx from total aligned CapEx that is linked to activities that enable reduction of GHG in other sectors</t>
-  </si>
-  <si>
-    <t>Transitional CapEx</t>
-  </si>
-  <si>
-    <t>Share of the taxonomy-aligned CapEx from total aligned CapEx that is linked to activities with significantly lower GHG emissions than the sector or industry average</t>
-  </si>
-  <si>
     <t>OpEx</t>
   </si>
   <si>
-    <t>Total OpEx for the financial year. Operating expenses (OpEx) are shorter term expenses required to meet the ongoing operational costs of running a business.</t>
-  </si>
-  <si>
-    <t>Eligible OpEx</t>
-  </si>
-  <si>
-    <t>Absolute value and share of the OpEx that is part of a plan to meet the DNSH criteria and make substantial contribution to any environmental objective</t>
-  </si>
-  <si>
-    <t>Aligned OpEx</t>
-  </si>
-  <si>
-    <t>Absolute value and share of the OpEx that is associated with taxonomy-aligned activities. i.e., for an eligible economic activity that is making a substantial contribution to at least one of the climate and environmental objectives, while also doing no significant harm to the remaining objectives and meeting minimum standards on human rights and labour standards</t>
-  </si>
-  <si>
-    <t>Aligned OpEx per Activity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Absolute value and share of taxonomy-aligned OpEx for the activity from total OpEx. </t>
-  </si>
-  <si>
-    <t>Non-Aligned OpEx</t>
-  </si>
-  <si>
-    <t>Absolute value and share of the OpEx that is associated with non taxonomy-aligned but eligible activities</t>
-  </si>
-  <si>
-    <t>Non-Aligned OpEx per Activity</t>
-  </si>
-  <si>
-    <t>Absolute value and share of the OpEx per activity that is not taxonomy-aligned but eligible</t>
-  </si>
-  <si>
-    <t>Non-Eligible OpEx</t>
-  </si>
-  <si>
-    <t>Absolute value and share of the OpEx that is not part of a plan to meet the DNSH criteria and make substantial contribution to any environmental objective</t>
-  </si>
-  <si>
-    <t>Enabling OpEx</t>
-  </si>
-  <si>
-    <t>Share of the taxonomy-aligned OpEx from total aligned OpEx that is linked to activities that enable reduction of GHG in other sectors</t>
-  </si>
-  <si>
-    <t>Transitional OpEx</t>
-  </si>
-  <si>
-    <t>Share of the taxonomy-aligned OpEx from total aligned OpEx that is linked to activities with significantly lower GHG emissions than the sector or industry average</t>
-  </si>
-  <si>
     <t>Currency</t>
   </si>
   <si>
@@ -531,6 +390,60 @@
   </si>
   <si>
     <t>13.2</t>
+  </si>
+  <si>
+    <t>25.1</t>
+  </si>
+  <si>
+    <t>25.2</t>
+  </si>
+  <si>
+    <t>24.1</t>
+  </si>
+  <si>
+    <t>24.2</t>
+  </si>
+  <si>
+    <t>26.1</t>
+  </si>
+  <si>
+    <t>26.2</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>28.1</t>
+  </si>
+  <si>
+    <t>28.2</t>
+  </si>
+  <si>
+    <t>39.1</t>
+  </si>
+  <si>
+    <t>39.2</t>
+  </si>
+  <si>
+    <t>40.1</t>
+  </si>
+  <si>
+    <t>40.2</t>
+  </si>
+  <si>
+    <t>41.1</t>
+  </si>
+  <si>
+    <t>41.2</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>43.1</t>
+  </si>
+  <si>
+    <t>43.2</t>
   </si>
 </sst>
 </file>
@@ -618,7 +531,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -647,12 +560,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor rgb="FFEFEFEF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
     <fill>
@@ -896,7 +803,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -929,29 +836,28 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="1" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment readingOrder="1"/>
     </xf>
@@ -959,12 +865,12 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1227,10 +1133,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T58"/>
+  <dimension ref="A1:T66"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1320,10 +1226,10 @@
       <c r="D2" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="35" t="s">
+      <c r="E2" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="39" t="s">
+      <c r="F2" s="38" t="s">
         <v>23</v>
       </c>
       <c r="G2" s="13" t="s">
@@ -1364,10 +1270,10 @@
       <c r="D3" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="42" t="s">
+      <c r="E3" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="F3" s="43" t="s">
+      <c r="F3" s="42" t="s">
         <v>31</v>
       </c>
       <c r="G3" s="16" t="s">
@@ -1406,7 +1312,7 @@
       <c r="D4" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="36" t="s">
+      <c r="E4" s="35" t="s">
         <v>36</v>
       </c>
       <c r="F4" s="13" t="s">
@@ -1448,7 +1354,7 @@
       <c r="D5" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="E5" s="36" t="s">
+      <c r="E5" s="35" t="s">
         <v>39</v>
       </c>
       <c r="F5" s="13" t="s">
@@ -1492,13 +1398,13 @@
       <c r="D6" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="E6" s="36" t="s">
+      <c r="E6" s="35" t="s">
         <v>45</v>
       </c>
       <c r="F6" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="G6" s="39" t="s">
+      <c r="G6" s="38" t="s">
         <v>24</v>
       </c>
       <c r="H6" s="15"/>
@@ -1537,10 +1443,10 @@
       <c r="E7" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="F7" s="37" t="s">
+      <c r="F7" s="36" t="s">
         <v>50</v>
       </c>
-      <c r="G7" s="40"/>
+      <c r="G7" s="39"/>
       <c r="H7" s="15"/>
       <c r="I7" s="15"/>
       <c r="J7" s="15"/>
@@ -1579,10 +1485,10 @@
       <c r="E8" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="F8" s="37" t="s">
+      <c r="F8" s="36" t="s">
         <v>46</v>
       </c>
-      <c r="G8" s="41" t="s">
+      <c r="G8" s="40" t="s">
         <v>24</v>
       </c>
       <c r="H8" s="15"/>
@@ -1620,13 +1526,13 @@
       <c r="D9" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="E9" s="36" t="s">
+      <c r="E9" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="F9" s="38" t="s">
+      <c r="F9" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="G9" s="41" t="s">
+      <c r="G9" s="40" t="s">
         <v>24</v>
       </c>
       <c r="H9" s="15"/>
@@ -1659,66 +1565,64 @@
         <v>60</v>
       </c>
       <c r="C10" s="11"/>
-      <c r="D10" s="24" t="s">
-        <v>130</v>
-      </c>
-      <c r="E10" s="36" t="s">
-        <v>61</v>
-      </c>
-      <c r="F10" s="38" t="s">
-        <v>129</v>
-      </c>
-      <c r="G10" s="40"/>
+      <c r="D10" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="E10" s="35"/>
+      <c r="F10" s="37" t="s">
+        <v>82</v>
+      </c>
+      <c r="G10" s="39"/>
       <c r="H10" s="15"/>
       <c r="I10" s="15" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="J10" s="15"/>
       <c r="K10" s="15"/>
       <c r="L10" s="15"/>
       <c r="M10" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="N10" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="N10" s="15" t="s">
+      <c r="O10" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="O10" s="15" t="s">
+      <c r="P10" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="P10" s="13" t="s">
+      <c r="Q10" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="R10" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="Q10" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="R10" s="25" t="s">
-        <v>66</v>
-      </c>
-      <c r="S10" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="T10" s="26" t="s">
+      <c r="S10" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="T10" s="25" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A11" s="34" t="s">
-        <v>134</v>
+      <c r="A11" s="33" t="s">
+        <v>87</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="D11" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="E11" s="36"/>
-      <c r="F11" s="38" t="s">
+        <v>84</v>
+      </c>
+      <c r="D11" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="E11" s="35"/>
+      <c r="F11" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="G11" s="40"/>
+      <c r="G11" s="39"/>
       <c r="H11" s="15"/>
       <c r="I11" s="15"/>
       <c r="J11" s="15"/>
@@ -1729,28 +1633,28 @@
       <c r="O11" s="15"/>
       <c r="P11" s="13"/>
       <c r="Q11" s="13"/>
-      <c r="R11" s="25"/>
-      <c r="S11" s="23"/>
-      <c r="T11" s="26"/>
+      <c r="R11" s="24"/>
+      <c r="S11" s="22"/>
+      <c r="T11" s="25"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A12" s="34" t="s">
-        <v>135</v>
+      <c r="A12" s="33" t="s">
+        <v>88</v>
       </c>
       <c r="B12" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="D12" s="24" t="s">
-        <v>133</v>
-      </c>
-      <c r="E12" s="36"/>
-      <c r="F12" s="38" t="s">
-        <v>129</v>
-      </c>
-      <c r="G12" s="40"/>
+        <v>84</v>
+      </c>
+      <c r="D12" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="E12" s="35"/>
+      <c r="F12" s="37" t="s">
+        <v>82</v>
+      </c>
+      <c r="G12" s="39"/>
       <c r="H12" s="15"/>
       <c r="I12" s="15"/>
       <c r="J12" s="15"/>
@@ -1761,76 +1665,76 @@
       <c r="O12" s="15"/>
       <c r="P12" s="13"/>
       <c r="Q12" s="13"/>
-      <c r="R12" s="25"/>
-      <c r="S12" s="23"/>
-      <c r="T12" s="26"/>
+      <c r="R12" s="24"/>
+      <c r="S12" s="22"/>
+      <c r="T12" s="25"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A13" s="34" t="s">
-        <v>137</v>
+      <c r="A13" s="33" t="s">
+        <v>90</v>
       </c>
       <c r="B13" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="D13" s="24" t="s">
-        <v>132</v>
+        <v>89</v>
+      </c>
+      <c r="D13" s="23" t="s">
+        <v>85</v>
       </c>
       <c r="E13" s="15"/>
-      <c r="F13" s="38" t="s">
+      <c r="F13" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="G13" s="40"/>
+      <c r="G13" s="39"/>
       <c r="H13" s="15"/>
       <c r="I13" s="15"/>
       <c r="J13" s="15"/>
       <c r="K13" s="15"/>
       <c r="L13" s="15"/>
       <c r="M13" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N13" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="O13" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="O13" s="15" t="s">
+      <c r="P13" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="P13" s="15" t="s">
+      <c r="Q13" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="R13" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="Q13" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="R13" s="27" t="s">
-        <v>70</v>
-      </c>
-      <c r="S13" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="T13" s="29" t="s">
+      <c r="S13" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="T13" s="28" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A14" s="34" t="s">
-        <v>138</v>
+      <c r="A14" s="33" t="s">
+        <v>91</v>
       </c>
       <c r="B14" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="D14" s="24" t="s">
-        <v>133</v>
+        <v>89</v>
+      </c>
+      <c r="D14" s="23" t="s">
+        <v>86</v>
       </c>
       <c r="E14" s="15"/>
-      <c r="F14" s="38" t="s">
-        <v>129</v>
-      </c>
-      <c r="G14" s="40"/>
+      <c r="F14" s="37" t="s">
+        <v>82</v>
+      </c>
+      <c r="G14" s="39"/>
       <c r="H14" s="15"/>
       <c r="I14" s="15"/>
       <c r="J14" s="15"/>
@@ -1841,28 +1745,28 @@
       <c r="O14" s="15"/>
       <c r="P14" s="15"/>
       <c r="Q14" s="13"/>
-      <c r="R14" s="27"/>
-      <c r="S14" s="28"/>
-      <c r="T14" s="29"/>
+      <c r="R14" s="26"/>
+      <c r="S14" s="27"/>
+      <c r="T14" s="28"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A15" s="34" t="s">
-        <v>140</v>
+      <c r="A15" s="33" t="s">
+        <v>93</v>
       </c>
       <c r="B15" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>139</v>
-      </c>
-      <c r="D15" s="24" t="s">
-        <v>132</v>
+        <v>92</v>
+      </c>
+      <c r="D15" s="23" t="s">
+        <v>85</v>
       </c>
       <c r="E15" s="15"/>
-      <c r="F15" s="38" t="s">
+      <c r="F15" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="G15" s="40"/>
+      <c r="G15" s="39"/>
       <c r="H15" s="15"/>
       <c r="I15" s="15"/>
       <c r="J15" s="15"/>
@@ -1873,72 +1777,72 @@
       <c r="O15" s="15"/>
       <c r="P15" s="15"/>
       <c r="Q15" s="13"/>
-      <c r="R15" s="27"/>
-      <c r="S15" s="28"/>
-      <c r="T15" s="29"/>
+      <c r="R15" s="26"/>
+      <c r="S15" s="27"/>
+      <c r="T15" s="28"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A16" s="34" t="s">
-        <v>141</v>
+      <c r="A16" s="33" t="s">
+        <v>94</v>
       </c>
       <c r="B16" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>139</v>
-      </c>
-      <c r="D16" s="24" t="s">
-        <v>133</v>
+        <v>92</v>
+      </c>
+      <c r="D16" s="23" t="s">
+        <v>86</v>
       </c>
       <c r="E16" s="15"/>
-      <c r="F16" s="38" t="s">
-        <v>129</v>
-      </c>
-      <c r="G16" s="40"/>
+      <c r="F16" s="37" t="s">
+        <v>82</v>
+      </c>
+      <c r="G16" s="39"/>
       <c r="H16" s="15"/>
       <c r="I16" s="15"/>
       <c r="J16" s="15"/>
       <c r="K16" s="15"/>
       <c r="L16" s="15"/>
       <c r="M16" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N16" s="15"/>
       <c r="O16" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="P16" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q16" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="R16" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="P16" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q16" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="R16" s="27" t="s">
-        <v>72</v>
-      </c>
-      <c r="S16" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="T16" s="29" t="s">
+      <c r="S16" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="T16" s="28" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A17" s="34" t="s">
-        <v>155</v>
+      <c r="A17" s="33" t="s">
+        <v>108</v>
       </c>
       <c r="B17" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C17" s="11"/>
-      <c r="D17" s="24" t="s">
-        <v>142</v>
+      <c r="D17" s="23" t="s">
+        <v>95</v>
       </c>
       <c r="E17" s="15"/>
-      <c r="F17" s="38" t="s">
-        <v>143</v>
-      </c>
-      <c r="G17" s="40"/>
+      <c r="F17" s="37" t="s">
+        <v>96</v>
+      </c>
+      <c r="G17" s="39"/>
       <c r="H17" s="15"/>
       <c r="I17" s="15"/>
       <c r="J17" s="15"/>
@@ -1949,28 +1853,28 @@
       <c r="O17" s="15"/>
       <c r="P17" s="15"/>
       <c r="Q17" s="13"/>
-      <c r="R17" s="27"/>
-      <c r="S17" s="28"/>
-      <c r="T17" s="29"/>
+      <c r="R17" s="26"/>
+      <c r="S17" s="27"/>
+      <c r="T17" s="28"/>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A18" s="34" t="s">
-        <v>156</v>
+      <c r="A18" s="33" t="s">
+        <v>109</v>
       </c>
       <c r="B18" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>144</v>
-      </c>
-      <c r="D18" s="24" t="s">
-        <v>132</v>
+        <v>97</v>
+      </c>
+      <c r="D18" s="23" t="s">
+        <v>85</v>
       </c>
       <c r="E18" s="15"/>
-      <c r="F18" s="38" t="s">
+      <c r="F18" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="G18" s="40"/>
+      <c r="G18" s="39"/>
       <c r="H18" s="15"/>
       <c r="I18" s="15"/>
       <c r="J18" s="15"/>
@@ -1981,28 +1885,28 @@
       <c r="O18" s="15"/>
       <c r="P18" s="15"/>
       <c r="Q18" s="13"/>
-      <c r="R18" s="27"/>
-      <c r="S18" s="28"/>
-      <c r="T18" s="29"/>
+      <c r="R18" s="26"/>
+      <c r="S18" s="27"/>
+      <c r="T18" s="28"/>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A19" s="34" t="s">
-        <v>157</v>
+      <c r="A19" s="33" t="s">
+        <v>110</v>
       </c>
       <c r="B19" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>144</v>
-      </c>
-      <c r="D19" s="24" t="s">
-        <v>133</v>
+        <v>97</v>
+      </c>
+      <c r="D19" s="23" t="s">
+        <v>86</v>
       </c>
       <c r="E19" s="15"/>
-      <c r="F19" s="38" t="s">
-        <v>129</v>
-      </c>
-      <c r="G19" s="40"/>
+      <c r="F19" s="37" t="s">
+        <v>82</v>
+      </c>
+      <c r="G19" s="39"/>
       <c r="H19" s="15"/>
       <c r="I19" s="15"/>
       <c r="J19" s="15"/>
@@ -2013,9 +1917,9 @@
       <c r="O19" s="15"/>
       <c r="P19" s="15"/>
       <c r="Q19" s="13"/>
-      <c r="R19" s="27"/>
-      <c r="S19" s="28"/>
-      <c r="T19" s="29"/>
+      <c r="R19" s="26"/>
+      <c r="S19" s="27"/>
+      <c r="T19" s="28"/>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A20" s="10">
@@ -2025,37 +1929,37 @@
         <v>60</v>
       </c>
       <c r="C20" s="11"/>
-      <c r="D20" s="24" t="s">
-        <v>145</v>
+      <c r="D20" s="23" t="s">
+        <v>98</v>
       </c>
       <c r="E20" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="F20" s="38" t="s">
+        <v>72</v>
+      </c>
+      <c r="F20" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="G20" s="40"/>
+      <c r="G20" s="39"/>
       <c r="H20" s="15"/>
       <c r="I20" s="15"/>
       <c r="J20" s="15"/>
       <c r="K20" s="15"/>
       <c r="L20" s="15"/>
       <c r="M20" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N20" s="15"/>
       <c r="O20" s="15"/>
       <c r="P20" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="Q20" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="R20" s="27"/>
-      <c r="S20" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="T20" s="29" t="s">
+      <c r="R20" s="26"/>
+      <c r="S20" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="T20" s="28" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2067,37 +1971,37 @@
         <v>60</v>
       </c>
       <c r="C21" s="11"/>
-      <c r="D21" s="24" t="s">
-        <v>146</v>
+      <c r="D21" s="23" t="s">
+        <v>99</v>
       </c>
       <c r="E21" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="F21" s="38" t="s">
+        <v>72</v>
+      </c>
+      <c r="F21" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="G21" s="40"/>
+      <c r="G21" s="39"/>
       <c r="H21" s="15"/>
       <c r="I21" s="15"/>
       <c r="J21" s="15"/>
       <c r="K21" s="15"/>
       <c r="L21" s="15"/>
       <c r="M21" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N21" s="15"/>
       <c r="O21" s="15"/>
       <c r="P21" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="Q21" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="R21" s="27"/>
-      <c r="S21" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="T21" s="29" t="s">
+      <c r="R21" s="26"/>
+      <c r="S21" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="T21" s="28" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2109,37 +2013,37 @@
         <v>60</v>
       </c>
       <c r="C22" s="11"/>
-      <c r="D22" s="24" t="s">
-        <v>147</v>
+      <c r="D22" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="E22" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="F22" s="38" t="s">
+        <v>72</v>
+      </c>
+      <c r="F22" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="G22" s="40"/>
+      <c r="G22" s="39"/>
       <c r="H22" s="15"/>
       <c r="I22" s="15"/>
       <c r="J22" s="15"/>
       <c r="K22" s="15"/>
       <c r="L22" s="15"/>
       <c r="M22" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N22" s="15"/>
       <c r="O22" s="15"/>
       <c r="P22" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="Q22" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="R22" s="27"/>
-      <c r="S22" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="T22" s="29" t="s">
+      <c r="R22" s="26"/>
+      <c r="S22" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="T22" s="28" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2151,37 +2055,37 @@
         <v>60</v>
       </c>
       <c r="C23" s="11"/>
-      <c r="D23" s="24" t="s">
-        <v>148</v>
+      <c r="D23" s="23" t="s">
+        <v>101</v>
       </c>
       <c r="E23" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="F23" s="38" t="s">
+        <v>72</v>
+      </c>
+      <c r="F23" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="G23" s="40"/>
+      <c r="G23" s="39"/>
       <c r="H23" s="15"/>
       <c r="I23" s="15"/>
       <c r="J23" s="15"/>
       <c r="K23" s="15"/>
       <c r="L23" s="15"/>
       <c r="M23" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N23" s="15"/>
       <c r="O23" s="15"/>
       <c r="P23" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="Q23" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="R23" s="27"/>
-      <c r="S23" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="T23" s="29" t="s">
+      <c r="R23" s="26"/>
+      <c r="S23" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="T23" s="28" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2193,37 +2097,37 @@
         <v>60</v>
       </c>
       <c r="C24" s="11"/>
-      <c r="D24" s="24" t="s">
-        <v>149</v>
+      <c r="D24" s="23" t="s">
+        <v>102</v>
       </c>
       <c r="E24" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="F24" s="38" t="s">
+        <v>72</v>
+      </c>
+      <c r="F24" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="G24" s="40"/>
+      <c r="G24" s="39"/>
       <c r="H24" s="15"/>
       <c r="I24" s="15"/>
       <c r="J24" s="15"/>
       <c r="K24" s="15"/>
       <c r="L24" s="15"/>
       <c r="M24" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N24" s="15"/>
       <c r="O24" s="15"/>
       <c r="P24" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="Q24" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="R24" s="27"/>
-      <c r="S24" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="T24" s="29" t="s">
+      <c r="R24" s="26"/>
+      <c r="S24" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="T24" s="28" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2235,37 +2139,37 @@
         <v>60</v>
       </c>
       <c r="C25" s="11"/>
-      <c r="D25" s="24" t="s">
-        <v>150</v>
+      <c r="D25" s="23" t="s">
+        <v>103</v>
       </c>
       <c r="E25" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="F25" s="38" t="s">
+        <v>72</v>
+      </c>
+      <c r="F25" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="G25" s="40"/>
+      <c r="G25" s="39"/>
       <c r="H25" s="15"/>
       <c r="I25" s="15"/>
       <c r="J25" s="15"/>
       <c r="K25" s="15"/>
       <c r="L25" s="15"/>
       <c r="M25" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N25" s="15"/>
       <c r="O25" s="15"/>
       <c r="P25" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="Q25" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="R25" s="27"/>
-      <c r="S25" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="T25" s="29" t="s">
+      <c r="R25" s="26"/>
+      <c r="S25" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="T25" s="28" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2277,16 +2181,14 @@
         <v>60</v>
       </c>
       <c r="C26" s="11"/>
-      <c r="D26" s="24" t="s">
-        <v>151</v>
-      </c>
-      <c r="E26" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="F26" s="38" t="s">
-        <v>152</v>
-      </c>
-      <c r="G26" s="40"/>
+      <c r="D26" s="23" t="s">
+        <v>104</v>
+      </c>
+      <c r="E26" s="15"/>
+      <c r="F26" s="37" t="s">
+        <v>105</v>
+      </c>
+      <c r="G26" s="39"/>
       <c r="H26" s="15"/>
       <c r="I26" s="15"/>
       <c r="J26" s="15"/>
@@ -2296,18 +2198,18 @@
       <c r="N26" s="15"/>
       <c r="O26" s="15"/>
       <c r="P26" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="Q26" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="R26" s="27" t="s">
-        <v>83</v>
-      </c>
-      <c r="S26" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="T26" s="29" t="s">
+      <c r="R26" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="S26" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="T26" s="28" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2315,43 +2217,41 @@
       <c r="A27" s="10">
         <v>21</v>
       </c>
-      <c r="B27" s="30" t="s">
+      <c r="B27" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="C27" s="30"/>
-      <c r="D27" s="31" t="s">
-        <v>153</v>
-      </c>
-      <c r="E27" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="F27" s="38" t="s">
+      <c r="C27" s="29"/>
+      <c r="D27" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="E27" s="15"/>
+      <c r="F27" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="G27" s="40"/>
+      <c r="G27" s="39"/>
       <c r="H27" s="15"/>
       <c r="I27" s="15"/>
       <c r="J27" s="15"/>
       <c r="K27" s="15"/>
       <c r="L27" s="15"/>
       <c r="M27" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="N27" s="27"/>
-      <c r="O27" s="27"/>
-      <c r="P27" s="27" t="s">
-        <v>69</v>
+        <v>61</v>
+      </c>
+      <c r="N27" s="26"/>
+      <c r="O27" s="26"/>
+      <c r="P27" s="26" t="s">
+        <v>68</v>
       </c>
       <c r="Q27" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="R27" s="27" t="s">
-        <v>89</v>
-      </c>
-      <c r="S27" s="32" t="s">
-        <v>28</v>
-      </c>
-      <c r="T27" s="33" t="s">
+      <c r="R27" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="S27" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="T27" s="32" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2359,1339 +2259,1563 @@
       <c r="A28" s="10">
         <v>22</v>
       </c>
-      <c r="B28" s="30" t="s">
+      <c r="B28" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="C28" s="30"/>
-      <c r="D28" s="31" t="s">
-        <v>154</v>
-      </c>
-      <c r="E28" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="F28" s="38" t="s">
+      <c r="C28" s="29"/>
+      <c r="D28" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="E28" s="15"/>
+      <c r="F28" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="G28" s="40"/>
+      <c r="G28" s="39"/>
       <c r="H28" s="15"/>
       <c r="I28" s="15"/>
       <c r="J28" s="15"/>
       <c r="K28" s="15"/>
       <c r="L28" s="15"/>
       <c r="M28" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="N28" s="27"/>
-      <c r="O28" s="27"/>
-      <c r="P28" s="27" t="s">
-        <v>69</v>
+        <v>61</v>
+      </c>
+      <c r="N28" s="26"/>
+      <c r="O28" s="26"/>
+      <c r="P28" s="26" t="s">
+        <v>68</v>
       </c>
       <c r="Q28" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="R28" s="27" t="s">
-        <v>91</v>
-      </c>
-      <c r="S28" s="32" t="s">
-        <v>28</v>
-      </c>
-      <c r="T28" s="33" t="s">
+      <c r="R28" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="S28" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="T28" s="32" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A29" s="10">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="C29" s="11"/>
-      <c r="D29" s="24" t="s">
-        <v>130</v>
-      </c>
-      <c r="E29" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="F29" s="38" t="s">
-        <v>50</v>
-      </c>
-      <c r="G29" s="40"/>
+      <c r="D29" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="E29" s="35"/>
+      <c r="F29" s="37" t="s">
+        <v>82</v>
+      </c>
+      <c r="G29" s="39"/>
       <c r="H29" s="15"/>
       <c r="I29" s="15"/>
       <c r="J29" s="15"/>
       <c r="K29" s="15"/>
       <c r="L29" s="15"/>
       <c r="M29" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N29" s="15"/>
       <c r="O29" s="15"/>
       <c r="P29" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q29" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="R29" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="Q29" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="R29" s="25" t="s">
-        <v>66</v>
-      </c>
-      <c r="S29" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="T29" s="29" t="s">
+      <c r="S29" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="T29" s="28" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A30" s="10">
-        <v>25</v>
+      <c r="A30" s="33" t="s">
+        <v>113</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="C30" s="11"/>
-      <c r="D30" s="24" t="s">
-        <v>94</v>
-      </c>
-      <c r="E30" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="F30" s="38" t="s">
+        <v>80</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="D30" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="E30" s="35"/>
+      <c r="F30" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="G30" s="40"/>
+      <c r="G30" s="39"/>
       <c r="H30" s="15"/>
       <c r="I30" s="15"/>
       <c r="J30" s="15"/>
       <c r="K30" s="15"/>
       <c r="L30" s="15"/>
-      <c r="M30" s="15" t="s">
-        <v>62</v>
-      </c>
+      <c r="M30" s="15"/>
       <c r="N30" s="15"/>
       <c r="O30" s="15"/>
-      <c r="P30" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q30" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="R30" s="27" t="s">
-        <v>70</v>
-      </c>
-      <c r="S30" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="T30" s="29" t="s">
-        <v>28</v>
-      </c>
+      <c r="P30" s="13"/>
+      <c r="Q30" s="13"/>
+      <c r="R30" s="24"/>
+      <c r="S30" s="27"/>
+      <c r="T30" s="28"/>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A31" s="10">
-        <v>26</v>
+      <c r="A31" s="33" t="s">
+        <v>114</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="C31" s="11"/>
-      <c r="D31" s="24" t="s">
-        <v>96</v>
-      </c>
-      <c r="E31" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="F31" s="38" t="s">
-        <v>50</v>
-      </c>
-      <c r="G31" s="40"/>
+        <v>80</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="D31" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="E31" s="35"/>
+      <c r="F31" s="37" t="s">
+        <v>82</v>
+      </c>
+      <c r="G31" s="39"/>
       <c r="H31" s="15"/>
       <c r="I31" s="15"/>
       <c r="J31" s="15"/>
       <c r="K31" s="15"/>
       <c r="L31" s="15"/>
       <c r="M31" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N31" s="15"/>
       <c r="O31" s="15"/>
       <c r="P31" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q31" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="R31" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="Q31" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="R31" s="27" t="s">
-        <v>72</v>
-      </c>
-      <c r="S31" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="T31" s="29" t="s">
+      <c r="S31" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="T31" s="28" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A32" s="10">
-        <v>27</v>
+      <c r="A32" s="33" t="s">
+        <v>111</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="C32" s="11"/>
-      <c r="D32" s="24" t="s">
-        <v>73</v>
-      </c>
-      <c r="E32" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="F32" s="38" t="s">
+        <v>80</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D32" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="E32" s="15"/>
+      <c r="F32" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="G32" s="40"/>
+      <c r="G32" s="39"/>
       <c r="H32" s="15"/>
       <c r="I32" s="15"/>
       <c r="J32" s="15"/>
       <c r="K32" s="15"/>
       <c r="L32" s="15"/>
       <c r="M32" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N32" s="15"/>
       <c r="O32" s="15"/>
       <c r="P32" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="Q32" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="R32" s="27"/>
-      <c r="S32" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="T32" s="29" t="s">
+      <c r="R32" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="S32" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="T32" s="28" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A33" s="10">
-        <v>28</v>
+      <c r="A33" s="33" t="s">
+        <v>112</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="C33" s="11"/>
-      <c r="D33" s="24" t="s">
-        <v>75</v>
-      </c>
-      <c r="E33" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="F33" s="38" t="s">
-        <v>50</v>
-      </c>
-      <c r="G33" s="40"/>
+        <v>80</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D33" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="E33" s="15"/>
+      <c r="F33" s="37" t="s">
+        <v>82</v>
+      </c>
+      <c r="G33" s="39"/>
       <c r="H33" s="15"/>
       <c r="I33" s="15"/>
       <c r="J33" s="15"/>
       <c r="K33" s="15"/>
       <c r="L33" s="15"/>
       <c r="M33" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N33" s="15"/>
       <c r="O33" s="15"/>
       <c r="P33" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="Q33" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="R33" s="27"/>
-      <c r="S33" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="T33" s="29" t="s">
+      <c r="R33" s="26"/>
+      <c r="S33" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="T33" s="28" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A34" s="10">
-        <v>29</v>
+      <c r="A34" s="33" t="s">
+        <v>115</v>
       </c>
       <c r="B34" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="C34" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="C34" s="11"/>
-      <c r="D34" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="E34" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="F34" s="38" t="s">
+      <c r="D34" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="E34" s="15"/>
+      <c r="F34" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="G34" s="40"/>
+      <c r="G34" s="39"/>
       <c r="H34" s="15"/>
       <c r="I34" s="15"/>
       <c r="J34" s="15"/>
       <c r="K34" s="15"/>
       <c r="L34" s="15"/>
       <c r="M34" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N34" s="15"/>
       <c r="O34" s="15"/>
       <c r="P34" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="Q34" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="R34" s="27"/>
-      <c r="S34" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="T34" s="29" t="s">
+      <c r="R34" s="26"/>
+      <c r="S34" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="T34" s="28" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A35" s="10">
-        <v>30</v>
+      <c r="A35" s="33" t="s">
+        <v>116</v>
       </c>
       <c r="B35" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="C35" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="C35" s="11"/>
-      <c r="D35" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="E35" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="F35" s="38" t="s">
-        <v>50</v>
-      </c>
-      <c r="G35" s="40"/>
+      <c r="D35" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="E35" s="15"/>
+      <c r="F35" s="37" t="s">
+        <v>82</v>
+      </c>
+      <c r="G35" s="39"/>
       <c r="H35" s="15"/>
       <c r="I35" s="15"/>
       <c r="J35" s="15"/>
       <c r="K35" s="15"/>
       <c r="L35" s="15"/>
       <c r="M35" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N35" s="15"/>
       <c r="O35" s="15"/>
       <c r="P35" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="Q35" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="R35" s="27"/>
-      <c r="S35" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="T35" s="29" t="s">
+      <c r="R35" s="26"/>
+      <c r="S35" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="T35" s="28" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A36" s="10">
-        <v>31</v>
+      <c r="A36" s="33" t="s">
+        <v>117</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="C36" s="11"/>
-      <c r="D36" s="24" t="s">
-        <v>78</v>
-      </c>
-      <c r="E36" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="F36" s="38" t="s">
-        <v>50</v>
-      </c>
-      <c r="G36" s="40"/>
+      <c r="D36" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="E36" s="15"/>
+      <c r="F36" s="37" t="s">
+        <v>96</v>
+      </c>
+      <c r="G36" s="39"/>
       <c r="H36" s="15"/>
       <c r="I36" s="15"/>
       <c r="J36" s="15"/>
       <c r="K36" s="15"/>
       <c r="L36" s="15"/>
       <c r="M36" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N36" s="15"/>
       <c r="O36" s="15"/>
       <c r="P36" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="Q36" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="R36" s="27"/>
-      <c r="S36" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="T36" s="29" t="s">
+      <c r="R36" s="26"/>
+      <c r="S36" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="T36" s="28" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A37" s="10">
-        <v>32</v>
+      <c r="A37" s="33" t="s">
+        <v>118</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="C37" s="11"/>
-      <c r="D37" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="E37" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="F37" s="38" t="s">
+        <v>80</v>
+      </c>
+      <c r="C37" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="D37" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="E37" s="15"/>
+      <c r="F37" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="G37" s="40"/>
+      <c r="G37" s="39"/>
       <c r="H37" s="15"/>
       <c r="I37" s="15"/>
       <c r="J37" s="15"/>
       <c r="K37" s="15"/>
       <c r="L37" s="15"/>
       <c r="M37" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N37" s="15"/>
       <c r="O37" s="15"/>
       <c r="P37" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="Q37" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="R37" s="27"/>
-      <c r="S37" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="T37" s="29" t="s">
+      <c r="R37" s="26"/>
+      <c r="S37" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="T37" s="28" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A38" s="10">
-        <v>33</v>
+      <c r="A38" s="33" t="s">
+        <v>119</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="C38" s="11"/>
-      <c r="D38" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="E38" s="15" t="s">
-        <v>99</v>
-      </c>
-      <c r="F38" s="38" t="s">
-        <v>81</v>
-      </c>
-      <c r="G38" s="40" t="s">
-        <v>100</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="D38" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="E38" s="15"/>
+      <c r="F38" s="37" t="s">
+        <v>82</v>
+      </c>
+      <c r="G38" s="39"/>
       <c r="H38" s="15"/>
       <c r="I38" s="15"/>
       <c r="J38" s="15"/>
       <c r="K38" s="15"/>
       <c r="L38" s="15"/>
-      <c r="M38" s="15"/>
+      <c r="M38" s="15" t="s">
+        <v>61</v>
+      </c>
       <c r="N38" s="15"/>
       <c r="O38" s="15"/>
       <c r="P38" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="Q38" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="R38" s="27" t="s">
-        <v>83</v>
-      </c>
-      <c r="S38" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="T38" s="29" t="s">
+      <c r="R38" s="26"/>
+      <c r="S38" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="T38" s="28" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A39" s="10">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="C39" s="11"/>
-      <c r="D39" s="24" t="s">
-        <v>101</v>
+      <c r="D39" s="23" t="s">
+        <v>98</v>
       </c>
       <c r="E39" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="F39" s="38" t="s">
+        <v>72</v>
+      </c>
+      <c r="F39" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="G39" s="40"/>
+      <c r="G39" s="39"/>
       <c r="H39" s="15"/>
       <c r="I39" s="15"/>
       <c r="J39" s="15"/>
       <c r="K39" s="15"/>
       <c r="L39" s="15"/>
-      <c r="M39" s="15" t="s">
-        <v>62</v>
-      </c>
+      <c r="M39" s="15"/>
       <c r="N39" s="15"/>
       <c r="O39" s="15"/>
       <c r="P39" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="Q39" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="R39" s="27" t="s">
-        <v>84</v>
-      </c>
-      <c r="S39" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="T39" s="29" t="s">
+      <c r="R39" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="S39" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="T39" s="28" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A40" s="10">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="C40" s="11"/>
-      <c r="D40" s="24" t="s">
-        <v>103</v>
+      <c r="D40" s="23" t="s">
+        <v>99</v>
       </c>
       <c r="E40" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="F40" s="38" t="s">
-        <v>85</v>
-      </c>
-      <c r="G40" s="40" t="s">
-        <v>100</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="F40" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="G40" s="39"/>
       <c r="H40" s="15"/>
       <c r="I40" s="15"/>
       <c r="J40" s="15"/>
       <c r="K40" s="15"/>
       <c r="L40" s="15"/>
-      <c r="M40" s="15"/>
+      <c r="M40" s="15" t="s">
+        <v>61</v>
+      </c>
       <c r="N40" s="15"/>
       <c r="O40" s="15"/>
       <c r="P40" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="Q40" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="R40" s="27" t="s">
-        <v>86</v>
-      </c>
-      <c r="S40" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="T40" s="29" t="s">
+      <c r="R40" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="S40" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="T40" s="28" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A41" s="10">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="C41" s="11"/>
-      <c r="D41" s="24" t="s">
-        <v>105</v>
+      <c r="D41" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="E41" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="F41" s="38" t="s">
+        <v>72</v>
+      </c>
+      <c r="F41" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="G41" s="40"/>
+      <c r="G41" s="39"/>
       <c r="H41" s="15"/>
       <c r="I41" s="15"/>
       <c r="J41" s="15"/>
       <c r="K41" s="15"/>
       <c r="L41" s="15"/>
-      <c r="M41" s="15" t="s">
-        <v>62</v>
-      </c>
+      <c r="M41" s="15"/>
       <c r="N41" s="15"/>
       <c r="O41" s="15"/>
       <c r="P41" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="Q41" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="R41" s="27" t="s">
-        <v>87</v>
-      </c>
-      <c r="S41" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="T41" s="29" t="s">
+      <c r="R41" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="S41" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="T41" s="28" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A42" s="10">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="C42" s="11"/>
-      <c r="D42" s="31" t="s">
-        <v>107</v>
+      <c r="D42" s="23" t="s">
+        <v>101</v>
       </c>
       <c r="E42" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="F42" s="38" t="s">
+        <v>72</v>
+      </c>
+      <c r="F42" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="G42" s="40"/>
+      <c r="G42" s="39"/>
       <c r="H42" s="15"/>
       <c r="I42" s="15"/>
       <c r="J42" s="15"/>
       <c r="K42" s="15"/>
       <c r="L42" s="15"/>
       <c r="M42" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="N42" s="27"/>
-      <c r="O42" s="27"/>
-      <c r="P42" s="27" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q42" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="R42" s="27" t="s">
-        <v>89</v>
-      </c>
-      <c r="S42" s="32" t="s">
-        <v>28</v>
-      </c>
-      <c r="T42" s="33" t="s">
+        <v>61</v>
+      </c>
+      <c r="N42" s="15"/>
+      <c r="O42" s="15"/>
+      <c r="P42" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q42" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="R42" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="S42" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="T42" s="28" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A43" s="10">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="C43" s="11"/>
-      <c r="D43" s="31" t="s">
-        <v>109</v>
+      <c r="D43" s="23" t="s">
+        <v>102</v>
       </c>
       <c r="E43" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="F43" s="38" t="s">
+        <v>72</v>
+      </c>
+      <c r="F43" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="G43" s="40"/>
+      <c r="G43" s="39"/>
       <c r="H43" s="15"/>
       <c r="I43" s="15"/>
       <c r="J43" s="15"/>
       <c r="K43" s="15"/>
       <c r="L43" s="15"/>
       <c r="M43" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="N43" s="27"/>
-      <c r="O43" s="27"/>
-      <c r="P43" s="27" t="s">
-        <v>69</v>
+        <v>61</v>
+      </c>
+      <c r="N43" s="26"/>
+      <c r="O43" s="26"/>
+      <c r="P43" s="26" t="s">
+        <v>68</v>
       </c>
       <c r="Q43" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="R43" s="27" t="s">
-        <v>91</v>
-      </c>
-      <c r="S43" s="32" t="s">
-        <v>28</v>
-      </c>
-      <c r="T43" s="33" t="s">
+      <c r="R43" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="S43" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="T43" s="32" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A44" s="10">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>111</v>
+        <v>80</v>
       </c>
       <c r="C44" s="11"/>
-      <c r="D44" s="24" t="s">
-        <v>130</v>
+      <c r="D44" s="23" t="s">
+        <v>103</v>
       </c>
       <c r="E44" s="15" t="s">
-        <v>112</v>
-      </c>
-      <c r="F44" s="38" t="s">
-        <v>62</v>
-      </c>
-      <c r="G44" s="40"/>
+        <v>72</v>
+      </c>
+      <c r="F44" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="G44" s="39"/>
       <c r="H44" s="15"/>
       <c r="I44" s="15"/>
       <c r="J44" s="15"/>
       <c r="K44" s="15"/>
       <c r="L44" s="15"/>
       <c r="M44" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="N44" s="15"/>
-      <c r="O44" s="15"/>
-      <c r="P44" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q44" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="R44" s="25" t="s">
-        <v>66</v>
-      </c>
-      <c r="S44" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="T44" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="N44" s="26"/>
+      <c r="O44" s="26"/>
+      <c r="P44" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q44" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="R44" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="S44" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="T44" s="32" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A45" s="10">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B45" s="11" t="s">
-        <v>111</v>
+        <v>80</v>
       </c>
       <c r="C45" s="11"/>
-      <c r="D45" s="24" t="s">
-        <v>113</v>
-      </c>
-      <c r="E45" s="15" t="s">
-        <v>114</v>
-      </c>
-      <c r="F45" s="38" t="s">
-        <v>50</v>
-      </c>
-      <c r="G45" s="40"/>
+      <c r="D45" s="23" t="s">
+        <v>104</v>
+      </c>
+      <c r="E45" s="15"/>
+      <c r="F45" s="37" t="s">
+        <v>105</v>
+      </c>
+      <c r="G45" s="39"/>
       <c r="H45" s="15"/>
       <c r="I45" s="15"/>
       <c r="J45" s="15"/>
       <c r="K45" s="15"/>
       <c r="L45" s="15"/>
       <c r="M45" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N45" s="15"/>
       <c r="O45" s="15"/>
-      <c r="P45" s="15" t="s">
-        <v>69</v>
+      <c r="P45" s="13" t="s">
+        <v>64</v>
       </c>
       <c r="Q45" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="R45" s="27" t="s">
-        <v>70</v>
-      </c>
-      <c r="S45" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="T45" s="29" t="s">
+      <c r="R45" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="S45" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="T45" s="28" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="46" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A46" s="10">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B46" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="C46" s="11"/>
-      <c r="D46" s="24" t="s">
-        <v>115</v>
-      </c>
-      <c r="E46" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="F46" s="38" t="s">
+        <v>80</v>
+      </c>
+      <c r="C46" s="29"/>
+      <c r="D46" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="E46" s="15"/>
+      <c r="F46" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="G46" s="40"/>
+      <c r="G46" s="39"/>
       <c r="H46" s="15"/>
       <c r="I46" s="15"/>
       <c r="J46" s="15"/>
       <c r="K46" s="15"/>
       <c r="L46" s="15"/>
       <c r="M46" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N46" s="15"/>
       <c r="O46" s="15"/>
       <c r="P46" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q46" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="R46" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="Q46" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="R46" s="27" t="s">
-        <v>72</v>
-      </c>
-      <c r="S46" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="T46" s="29" t="s">
+      <c r="S46" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="T46" s="28" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="47" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A47" s="10">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B47" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="C47" s="11"/>
-      <c r="D47" s="24" t="s">
-        <v>73</v>
-      </c>
-      <c r="E47" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="F47" s="38" t="s">
+        <v>80</v>
+      </c>
+      <c r="C47" s="29"/>
+      <c r="D47" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="E47" s="15"/>
+      <c r="F47" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="G47" s="40"/>
+      <c r="G47" s="39"/>
       <c r="H47" s="15"/>
       <c r="I47" s="15"/>
       <c r="J47" s="15"/>
       <c r="K47" s="15"/>
       <c r="L47" s="15"/>
       <c r="M47" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N47" s="15"/>
       <c r="O47" s="15"/>
       <c r="P47" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="Q47" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="R47" s="27"/>
-      <c r="S47" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="T47" s="29" t="s">
+      <c r="R47" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="S47" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="T47" s="28" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A48" s="10">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B48" s="11" t="s">
-        <v>111</v>
+        <v>81</v>
       </c>
       <c r="C48" s="11"/>
-      <c r="D48" s="24" t="s">
-        <v>75</v>
-      </c>
-      <c r="E48" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="F48" s="38" t="s">
-        <v>50</v>
-      </c>
-      <c r="G48" s="40"/>
+      <c r="D48" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="E48" s="35"/>
+      <c r="F48" s="37" t="s">
+        <v>82</v>
+      </c>
+      <c r="G48" s="39"/>
       <c r="H48" s="15"/>
       <c r="I48" s="15"/>
       <c r="J48" s="15"/>
       <c r="K48" s="15"/>
       <c r="L48" s="15"/>
       <c r="M48" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N48" s="15"/>
       <c r="O48" s="15"/>
       <c r="P48" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="Q48" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="R48" s="27"/>
-      <c r="S48" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="T48" s="29" t="s">
+      <c r="R48" s="26"/>
+      <c r="S48" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="T48" s="28" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="49" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A49" s="10">
-        <v>44</v>
+      <c r="A49" s="33" t="s">
+        <v>120</v>
       </c>
       <c r="B49" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="C49" s="11"/>
-      <c r="D49" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="E49" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="F49" s="38" t="s">
+        <v>80</v>
+      </c>
+      <c r="C49" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="D49" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="E49" s="35"/>
+      <c r="F49" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="G49" s="40"/>
+      <c r="G49" s="39"/>
       <c r="H49" s="15"/>
       <c r="I49" s="15"/>
       <c r="J49" s="15"/>
       <c r="K49" s="15"/>
       <c r="L49" s="15"/>
       <c r="M49" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N49" s="15"/>
       <c r="O49" s="15"/>
       <c r="P49" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="Q49" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="R49" s="27"/>
-      <c r="S49" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="T49" s="29" t="s">
+      <c r="R49" s="26"/>
+      <c r="S49" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="T49" s="28" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="50" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A50" s="10">
-        <v>45</v>
+      <c r="A50" s="33" t="s">
+        <v>121</v>
       </c>
       <c r="B50" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="C50" s="11"/>
-      <c r="D50" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="E50" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="F50" s="38" t="s">
-        <v>50</v>
-      </c>
-      <c r="G50" s="40"/>
+        <v>80</v>
+      </c>
+      <c r="C50" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="D50" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="E50" s="35"/>
+      <c r="F50" s="37" t="s">
+        <v>82</v>
+      </c>
+      <c r="G50" s="39"/>
       <c r="H50" s="15"/>
       <c r="I50" s="15"/>
       <c r="J50" s="15"/>
       <c r="K50" s="15"/>
       <c r="L50" s="15"/>
       <c r="M50" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N50" s="15"/>
       <c r="O50" s="15"/>
       <c r="P50" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="Q50" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="R50" s="27"/>
-      <c r="S50" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="T50" s="29" t="s">
+      <c r="R50" s="26"/>
+      <c r="S50" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="T50" s="28" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="51" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A51" s="10">
-        <v>46</v>
+      <c r="A51" s="33" t="s">
+        <v>122</v>
       </c>
       <c r="B51" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="C51" s="11"/>
-      <c r="D51" s="24" t="s">
-        <v>78</v>
-      </c>
-      <c r="E51" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="F51" s="38" t="s">
+        <v>80</v>
+      </c>
+      <c r="C51" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D51" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="E51" s="15"/>
+      <c r="F51" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="G51" s="40"/>
+      <c r="G51" s="39"/>
       <c r="H51" s="15"/>
       <c r="I51" s="15"/>
       <c r="J51" s="15"/>
       <c r="K51" s="15"/>
       <c r="L51" s="15"/>
       <c r="M51" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N51" s="15"/>
       <c r="O51" s="15"/>
       <c r="P51" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="Q51" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="R51" s="27"/>
-      <c r="S51" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="T51" s="29" t="s">
+      <c r="R51" s="26"/>
+      <c r="S51" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="T51" s="28" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="52" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A52" s="10">
-        <v>47</v>
+      <c r="A52" s="33" t="s">
+        <v>123</v>
       </c>
       <c r="B52" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="C52" s="11"/>
-      <c r="D52" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="E52" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="F52" s="38" t="s">
-        <v>50</v>
-      </c>
-      <c r="G52" s="40"/>
+        <v>80</v>
+      </c>
+      <c r="C52" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D52" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="E52" s="15"/>
+      <c r="F52" s="37" t="s">
+        <v>82</v>
+      </c>
+      <c r="G52" s="39"/>
       <c r="H52" s="15"/>
       <c r="I52" s="15"/>
       <c r="J52" s="15"/>
       <c r="K52" s="15"/>
       <c r="L52" s="15"/>
       <c r="M52" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N52" s="15"/>
       <c r="O52" s="15"/>
       <c r="P52" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="Q52" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="R52" s="27"/>
-      <c r="S52" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="T52" s="29" t="s">
+      <c r="R52" s="26"/>
+      <c r="S52" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="T52" s="28" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="53" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A53" s="10">
-        <v>48</v>
+      <c r="A53" s="33" t="s">
+        <v>124</v>
       </c>
       <c r="B53" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="C53" s="11"/>
-      <c r="D53" s="24" t="s">
-        <v>117</v>
-      </c>
-      <c r="E53" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="F53" s="38" t="s">
-        <v>81</v>
-      </c>
-      <c r="G53" s="40" t="s">
-        <v>100</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="C53" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="D53" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="E53" s="15"/>
+      <c r="F53" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="G53" s="39"/>
       <c r="H53" s="15"/>
       <c r="I53" s="15"/>
       <c r="J53" s="15"/>
       <c r="K53" s="15"/>
       <c r="L53" s="15"/>
-      <c r="M53" s="15"/>
+      <c r="M53" s="15" t="s">
+        <v>61</v>
+      </c>
       <c r="N53" s="15"/>
       <c r="O53" s="15"/>
       <c r="P53" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="Q53" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="R53" s="27" t="s">
-        <v>83</v>
-      </c>
-      <c r="S53" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="T53" s="29" t="s">
+      <c r="R53" s="26"/>
+      <c r="S53" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="T53" s="28" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="54" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A54" s="10">
-        <v>49</v>
+      <c r="A54" s="33" t="s">
+        <v>125</v>
       </c>
       <c r="B54" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="C54" s="11"/>
-      <c r="D54" s="24" t="s">
-        <v>119</v>
-      </c>
-      <c r="E54" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="F54" s="38" t="s">
-        <v>50</v>
-      </c>
-      <c r="G54" s="40"/>
+        <v>80</v>
+      </c>
+      <c r="C54" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="D54" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="E54" s="15"/>
+      <c r="F54" s="37" t="s">
+        <v>82</v>
+      </c>
+      <c r="G54" s="39"/>
       <c r="H54" s="15"/>
       <c r="I54" s="15"/>
       <c r="J54" s="15"/>
       <c r="K54" s="15"/>
       <c r="L54" s="15"/>
-      <c r="M54" s="15" t="s">
-        <v>62</v>
-      </c>
+      <c r="M54" s="15"/>
       <c r="N54" s="15"/>
       <c r="O54" s="15"/>
       <c r="P54" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="Q54" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="R54" s="27" t="s">
-        <v>84</v>
-      </c>
-      <c r="S54" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="T54" s="29" t="s">
+      <c r="R54" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="S54" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="T54" s="28" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="55" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A55" s="10">
-        <v>50</v>
+      <c r="A55" s="33" t="s">
+        <v>126</v>
       </c>
       <c r="B55" s="11" t="s">
-        <v>111</v>
+        <v>80</v>
       </c>
       <c r="C55" s="11"/>
-      <c r="D55" s="24" t="s">
-        <v>121</v>
-      </c>
-      <c r="E55" s="15" t="s">
-        <v>122</v>
-      </c>
-      <c r="F55" s="38" t="s">
-        <v>85</v>
-      </c>
-      <c r="G55" s="40" t="s">
-        <v>100</v>
-      </c>
+      <c r="D55" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="E55" s="15"/>
+      <c r="F55" s="37" t="s">
+        <v>96</v>
+      </c>
+      <c r="G55" s="39"/>
       <c r="H55" s="15"/>
       <c r="I55" s="15"/>
       <c r="J55" s="15"/>
       <c r="K55" s="15"/>
       <c r="L55" s="15"/>
-      <c r="M55" s="15"/>
+      <c r="M55" s="15" t="s">
+        <v>61</v>
+      </c>
       <c r="N55" s="15"/>
       <c r="O55" s="15"/>
       <c r="P55" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="Q55" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="R55" s="27" t="s">
-        <v>86</v>
-      </c>
-      <c r="S55" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="T55" s="29" t="s">
+      <c r="R55" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="S55" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="T55" s="28" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="56" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A56" s="10">
-        <v>51</v>
+      <c r="A56" s="33" t="s">
+        <v>127</v>
       </c>
       <c r="B56" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="C56" s="11"/>
-      <c r="D56" s="24" t="s">
-        <v>123</v>
-      </c>
-      <c r="E56" s="15" t="s">
-        <v>124</v>
-      </c>
-      <c r="F56" s="38" t="s">
+        <v>80</v>
+      </c>
+      <c r="C56" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="D56" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="E56" s="15"/>
+      <c r="F56" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="G56" s="40"/>
+      <c r="G56" s="39"/>
       <c r="H56" s="15"/>
       <c r="I56" s="15"/>
       <c r="J56" s="15"/>
       <c r="K56" s="15"/>
       <c r="L56" s="15"/>
-      <c r="M56" s="15" t="s">
-        <v>62</v>
-      </c>
+      <c r="M56" s="15"/>
       <c r="N56" s="15"/>
       <c r="O56" s="15"/>
       <c r="P56" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="Q56" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="R56" s="27" t="s">
-        <v>87</v>
-      </c>
-      <c r="S56" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="T56" s="29" t="s">
+      <c r="R56" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="S56" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="T56" s="28" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="57" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A57" s="10">
-        <v>52</v>
+      <c r="A57" s="33" t="s">
+        <v>128</v>
       </c>
       <c r="B57" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="C57" s="11"/>
-      <c r="D57" s="31" t="s">
-        <v>125</v>
-      </c>
-      <c r="E57" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="F57" s="38" t="s">
-        <v>50</v>
-      </c>
-      <c r="G57" s="40"/>
-      <c r="H57" s="22"/>
-      <c r="I57" s="22"/>
-      <c r="J57" s="22"/>
-      <c r="K57" s="22"/>
-      <c r="L57" s="22"/>
-      <c r="M57" s="22" t="s">
-        <v>62</v>
-      </c>
-      <c r="N57" s="27"/>
-      <c r="O57" s="27"/>
-      <c r="P57" s="27" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q57" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="R57" s="27" t="s">
-        <v>89</v>
-      </c>
-      <c r="S57" s="32" t="s">
-        <v>28</v>
-      </c>
-      <c r="T57" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="C57" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="D57" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="E57" s="15"/>
+      <c r="F57" s="37" t="s">
+        <v>82</v>
+      </c>
+      <c r="G57" s="39"/>
+      <c r="H57" s="15"/>
+      <c r="I57" s="15"/>
+      <c r="J57" s="15"/>
+      <c r="K57" s="15"/>
+      <c r="L57" s="15"/>
+      <c r="M57" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="N57" s="15"/>
+      <c r="O57" s="15"/>
+      <c r="P57" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q57" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="R57" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="S57" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="T57" s="28" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="58" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A58" s="10">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="B58" s="11" t="s">
-        <v>111</v>
+        <v>80</v>
       </c>
       <c r="C58" s="11"/>
-      <c r="D58" s="31" t="s">
-        <v>127</v>
+      <c r="D58" s="23" t="s">
+        <v>98</v>
       </c>
       <c r="E58" s="15" t="s">
-        <v>128</v>
-      </c>
-      <c r="F58" s="38" t="s">
+        <v>72</v>
+      </c>
+      <c r="F58" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="G58" s="40"/>
-      <c r="H58" s="22"/>
-      <c r="I58" s="22"/>
-      <c r="J58" s="22"/>
-      <c r="K58" s="22"/>
-      <c r="L58" s="22"/>
-      <c r="M58" s="22" t="s">
-        <v>62</v>
-      </c>
-      <c r="N58" s="27"/>
-      <c r="O58" s="27"/>
-      <c r="P58" s="27" t="s">
-        <v>69</v>
+      <c r="G58" s="39"/>
+      <c r="H58" s="35"/>
+      <c r="I58" s="35"/>
+      <c r="J58" s="35"/>
+      <c r="K58" s="35"/>
+      <c r="L58" s="35"/>
+      <c r="M58" s="35" t="s">
+        <v>61</v>
+      </c>
+      <c r="N58" s="26"/>
+      <c r="O58" s="26"/>
+      <c r="P58" s="26" t="s">
+        <v>68</v>
       </c>
       <c r="Q58" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="R58" s="27" t="s">
-        <v>91</v>
-      </c>
-      <c r="S58" s="32" t="s">
-        <v>28</v>
-      </c>
-      <c r="T58" s="33" t="s">
+      <c r="R58" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="S58" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="T58" s="32" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="59" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A59" s="10">
+        <v>45</v>
+      </c>
+      <c r="B59" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="C59" s="11"/>
+      <c r="D59" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="E59" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="F59" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="G59" s="39"/>
+      <c r="H59" s="35"/>
+      <c r="I59" s="35"/>
+      <c r="J59" s="35"/>
+      <c r="K59" s="35"/>
+      <c r="L59" s="35"/>
+      <c r="M59" s="35"/>
+      <c r="N59" s="26"/>
+      <c r="O59" s="26"/>
+      <c r="P59" s="26"/>
+      <c r="Q59" s="17"/>
+      <c r="R59" s="26"/>
+      <c r="S59" s="31"/>
+      <c r="T59" s="32"/>
+    </row>
+    <row r="60" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A60" s="10">
+        <v>46</v>
+      </c>
+      <c r="B60" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="C60" s="11"/>
+      <c r="D60" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="E60" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="F60" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="G60" s="39"/>
+      <c r="H60" s="35"/>
+      <c r="I60" s="35"/>
+      <c r="J60" s="35"/>
+      <c r="K60" s="35"/>
+      <c r="L60" s="35"/>
+      <c r="M60" s="35"/>
+      <c r="N60" s="26"/>
+      <c r="O60" s="26"/>
+      <c r="P60" s="26"/>
+      <c r="Q60" s="17"/>
+      <c r="R60" s="26"/>
+      <c r="S60" s="31"/>
+      <c r="T60" s="32"/>
+    </row>
+    <row r="61" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A61" s="10">
+        <v>47</v>
+      </c>
+      <c r="B61" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="C61" s="11"/>
+      <c r="D61" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="E61" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="F61" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="G61" s="39"/>
+      <c r="H61" s="35"/>
+      <c r="I61" s="35"/>
+      <c r="J61" s="35"/>
+      <c r="K61" s="35"/>
+      <c r="L61" s="35"/>
+      <c r="M61" s="35"/>
+      <c r="N61" s="26"/>
+      <c r="O61" s="26"/>
+      <c r="P61" s="26"/>
+      <c r="Q61" s="17"/>
+      <c r="R61" s="26"/>
+      <c r="S61" s="31"/>
+      <c r="T61" s="32"/>
+    </row>
+    <row r="62" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A62" s="10">
+        <v>48</v>
+      </c>
+      <c r="B62" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="C62" s="11"/>
+      <c r="D62" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="E62" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="F62" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="G62" s="39"/>
+      <c r="H62" s="35"/>
+      <c r="I62" s="35"/>
+      <c r="J62" s="35"/>
+      <c r="K62" s="35"/>
+      <c r="L62" s="35"/>
+      <c r="M62" s="35"/>
+      <c r="N62" s="26"/>
+      <c r="O62" s="26"/>
+      <c r="P62" s="26"/>
+      <c r="Q62" s="17"/>
+      <c r="R62" s="26"/>
+      <c r="S62" s="31"/>
+      <c r="T62" s="32"/>
+    </row>
+    <row r="63" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A63" s="10">
+        <v>49</v>
+      </c>
+      <c r="B63" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="C63" s="11"/>
+      <c r="D63" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="E63" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="F63" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="G63" s="39"/>
+      <c r="H63" s="35"/>
+      <c r="I63" s="35"/>
+      <c r="J63" s="35"/>
+      <c r="K63" s="35"/>
+      <c r="L63" s="35"/>
+      <c r="M63" s="35"/>
+      <c r="N63" s="26"/>
+      <c r="O63" s="26"/>
+      <c r="P63" s="26"/>
+      <c r="Q63" s="17"/>
+      <c r="R63" s="26"/>
+      <c r="S63" s="31"/>
+      <c r="T63" s="32"/>
+    </row>
+    <row r="64" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A64" s="10">
+        <v>50</v>
+      </c>
+      <c r="B64" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="C64" s="11"/>
+      <c r="D64" s="23" t="s">
+        <v>104</v>
+      </c>
+      <c r="E64" s="15"/>
+      <c r="F64" s="37" t="s">
+        <v>105</v>
+      </c>
+      <c r="G64" s="39"/>
+      <c r="H64" s="35"/>
+      <c r="I64" s="35"/>
+      <c r="J64" s="35"/>
+      <c r="K64" s="35"/>
+      <c r="L64" s="35"/>
+      <c r="M64" s="35"/>
+      <c r="N64" s="26"/>
+      <c r="O64" s="26"/>
+      <c r="P64" s="26"/>
+      <c r="Q64" s="17"/>
+      <c r="R64" s="26"/>
+      <c r="S64" s="31"/>
+      <c r="T64" s="32"/>
+    </row>
+    <row r="65" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A65" s="10">
+        <v>51</v>
+      </c>
+      <c r="B65" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="C65" s="29"/>
+      <c r="D65" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="E65" s="15"/>
+      <c r="F65" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="G65" s="39"/>
+      <c r="H65" s="35"/>
+      <c r="I65" s="35"/>
+      <c r="J65" s="35"/>
+      <c r="K65" s="35"/>
+      <c r="L65" s="35"/>
+      <c r="M65" s="35"/>
+      <c r="N65" s="26"/>
+      <c r="O65" s="26"/>
+      <c r="P65" s="26"/>
+      <c r="Q65" s="17"/>
+      <c r="R65" s="26"/>
+      <c r="S65" s="31"/>
+      <c r="T65" s="32"/>
+    </row>
+    <row r="66" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A66" s="10">
+        <v>52</v>
+      </c>
+      <c r="B66" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="C66" s="29"/>
+      <c r="D66" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="E66" s="15"/>
+      <c r="F66" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="G66" s="39"/>
+      <c r="H66" s="35"/>
+      <c r="I66" s="35"/>
+      <c r="J66" s="35"/>
+      <c r="K66" s="35"/>
+      <c r="L66" s="35"/>
+      <c r="M66" s="35"/>
+      <c r="N66" s="26"/>
+      <c r="O66" s="26"/>
+      <c r="P66" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q66" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="R66" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="S66" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="T66" s="32" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix mistake in excel
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/euTaxonomyNonFinancials/EutaxonomyNonFinancials.xlsx
+++ b/dataland-framework-toolbox/inputs/euTaxonomyNonFinancials/EutaxonomyNonFinancials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d92432\Documents\Projekte\02-Dataland\Dataland\dataland-framework-toolbox\inputs\euTaxonomyNonFinancials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C7CA0C9-4CB5-4B28-968D-EE6EBCED466D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE8FB046-8FE1-4533-91F9-DE0EE1B43E09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="38640" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1135,8 +1135,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3140,7 +3140,7 @@
         <v>120</v>
       </c>
       <c r="B49" s="11" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C49" s="11" t="s">
         <v>84</v>
@@ -3182,7 +3182,7 @@
         <v>121</v>
       </c>
       <c r="B50" s="11" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C50" s="11" t="s">
         <v>84</v>
@@ -3224,7 +3224,7 @@
         <v>122</v>
       </c>
       <c r="B51" s="11" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C51" s="11" t="s">
         <v>89</v>
@@ -3266,7 +3266,7 @@
         <v>123</v>
       </c>
       <c r="B52" s="11" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C52" s="11" t="s">
         <v>89</v>
@@ -3308,7 +3308,7 @@
         <v>124</v>
       </c>
       <c r="B53" s="11" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C53" s="11" t="s">
         <v>92</v>
@@ -3350,7 +3350,7 @@
         <v>125</v>
       </c>
       <c r="B54" s="11" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C54" s="11" t="s">
         <v>92</v>
@@ -3392,7 +3392,7 @@
         <v>126</v>
       </c>
       <c r="B55" s="11" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C55" s="11"/>
       <c r="D55" s="23" t="s">
@@ -3434,7 +3434,7 @@
         <v>127</v>
       </c>
       <c r="B56" s="11" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C56" s="11" t="s">
         <v>97</v>
@@ -3476,7 +3476,7 @@
         <v>128</v>
       </c>
       <c r="B57" s="11" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C57" s="11" t="s">
         <v>97</v>
@@ -3520,7 +3520,7 @@
         <v>44</v>
       </c>
       <c r="B58" s="11" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C58" s="11"/>
       <c r="D58" s="23" t="s">
@@ -3564,7 +3564,7 @@
         <v>45</v>
       </c>
       <c r="B59" s="11" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C59" s="11"/>
       <c r="D59" s="23" t="s">
@@ -3596,7 +3596,7 @@
         <v>46</v>
       </c>
       <c r="B60" s="11" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C60" s="11"/>
       <c r="D60" s="23" t="s">
@@ -3628,7 +3628,7 @@
         <v>47</v>
       </c>
       <c r="B61" s="11" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C61" s="11"/>
       <c r="D61" s="23" t="s">
@@ -3660,7 +3660,7 @@
         <v>48</v>
       </c>
       <c r="B62" s="11" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C62" s="11"/>
       <c r="D62" s="23" t="s">
@@ -3692,7 +3692,7 @@
         <v>49</v>
       </c>
       <c r="B63" s="11" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C63" s="11"/>
       <c r="D63" s="23" t="s">
@@ -3724,7 +3724,7 @@
         <v>50</v>
       </c>
       <c r="B64" s="11" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C64" s="11"/>
       <c r="D64" s="23" t="s">
@@ -3754,7 +3754,7 @@
         <v>51</v>
       </c>
       <c r="B65" s="11" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C65" s="29"/>
       <c r="D65" s="30" t="s">
@@ -3784,7 +3784,7 @@
         <v>52</v>
       </c>
       <c r="B66" s="11" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C66" s="29"/>
       <c r="D66" s="30" t="s">

</xml_diff>

<commit_message>
another update that makes everything nullable in "General"
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/euTaxonomyNonFinancials/EutaxonomyNonFinancials.xlsx
+++ b/dataland-framework-toolbox/inputs/euTaxonomyNonFinancials/EutaxonomyNonFinancials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d92432\Documents\Projekte\02-Dataland\Dataland\dataland-framework-toolbox\inputs\euTaxonomyNonFinancials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F0BD13F-0D85-461C-8768-60C5C37D39EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{726DAF2C-5FF6-44E1-8DCC-62D0C182EB89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="38640" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="90">
   <si>
     <t>Field Identifier</t>
   </si>
@@ -102,9 +102,6 @@
   </si>
   <si>
     <t> </t>
-  </si>
-  <si>
-    <t>Yes</t>
   </si>
   <si>
     <t>Fiscal Year Deviation</t>
@@ -923,7 +920,7 @@
   <dimension ref="A1:L66"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -983,16 +980,16 @@
       </c>
       <c r="C2" s="8"/>
       <c r="D2" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="24" t="s">
+      <c r="F2" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="25" t="s">
-        <v>18</v>
-      </c>
       <c r="G2" s="13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H2" s="11"/>
       <c r="I2" s="12"/>
@@ -1007,10 +1004,10 @@
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="19" t="s">
         <v>19</v>
-      </c>
-      <c r="E3" s="19" t="s">
-        <v>20</v>
       </c>
       <c r="F3" s="10" t="s">
         <v>13</v>
@@ -1020,9 +1017,7 @@
       <c r="I3" s="12"/>
       <c r="J3" s="12"/>
       <c r="K3" s="12"/>
-      <c r="L3" s="12" t="s">
-        <v>15</v>
-      </c>
+      <c r="L3" s="12"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="7">
@@ -1033,13 +1028,13 @@
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="19" t="s">
+      <c r="F4" s="10" t="s">
         <v>22</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>23</v>
       </c>
       <c r="G4" s="10" t="s">
         <v>14</v>
@@ -1059,13 +1054,13 @@
       </c>
       <c r="C5" s="8"/>
       <c r="D5" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="12" t="s">
-        <v>31</v>
-      </c>
       <c r="F5" s="20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G5" s="23" t="s">
         <v>14</v>
@@ -1085,13 +1080,13 @@
       </c>
       <c r="C6" s="8"/>
       <c r="D6" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="19" t="s">
+      <c r="F6" s="20" t="s">
         <v>25</v>
-      </c>
-      <c r="F6" s="20" t="s">
-        <v>26</v>
       </c>
       <c r="G6" s="26" t="s">
         <v>14</v>
@@ -1111,13 +1106,13 @@
       </c>
       <c r="C7" s="8"/>
       <c r="D7" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="E7" s="19" t="s">
+      <c r="F7" s="21" t="s">
         <v>33</v>
-      </c>
-      <c r="F7" s="21" t="s">
-        <v>34</v>
       </c>
       <c r="G7" s="26" t="s">
         <v>14</v>
@@ -1126,9 +1121,7 @@
       <c r="I7" s="12"/>
       <c r="J7" s="12"/>
       <c r="K7" s="12"/>
-      <c r="L7" s="12" t="s">
-        <v>15</v>
-      </c>
+      <c r="L7" s="12"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="7">
@@ -1139,13 +1132,13 @@
       </c>
       <c r="C8" s="8"/>
       <c r="D8" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="12" t="s">
-        <v>28</v>
-      </c>
       <c r="F8" s="20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G8" s="22"/>
       <c r="H8" s="12"/>
@@ -1163,11 +1156,11 @@
       </c>
       <c r="C9" s="8"/>
       <c r="D9" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E9" s="12"/>
       <c r="F9" s="20" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G9" s="23" t="s">
         <v>14</v>
@@ -1183,20 +1176,20 @@
         <v>8</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C10" s="8"/>
       <c r="D10" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E10" s="19"/>
       <c r="F10" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G10" s="22"/>
       <c r="H10" s="12"/>
       <c r="I10" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J10" s="12"/>
       <c r="K10" s="12"/>
@@ -1204,20 +1197,20 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" s="18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C11" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="15" t="s">
         <v>42</v>
-      </c>
-      <c r="D11" s="15" t="s">
-        <v>43</v>
       </c>
       <c r="E11" s="19"/>
       <c r="F11" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G11" s="22"/>
       <c r="H11" s="12"/>
@@ -1228,20 +1221,20 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" s="18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E12" s="19"/>
       <c r="F12" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G12" s="22"/>
       <c r="H12" s="12"/>
@@ -1252,20 +1245,20 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" s="18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E13" s="12"/>
       <c r="F13" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G13" s="22"/>
       <c r="H13" s="12"/>
@@ -1276,20 +1269,20 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" s="18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E14" s="12"/>
       <c r="F14" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G14" s="22"/>
       <c r="H14" s="12"/>
@@ -1300,20 +1293,20 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" s="18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E15" s="12"/>
       <c r="F15" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G15" s="22"/>
       <c r="H15" s="12"/>
@@ -1324,20 +1317,20 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" s="18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E16" s="12"/>
       <c r="F16" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G16" s="22"/>
       <c r="H16" s="12"/>
@@ -1348,18 +1341,18 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C17" s="8"/>
       <c r="D17" s="15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E17" s="12"/>
       <c r="F17" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G17" s="22"/>
       <c r="H17" s="12"/>
@@ -1370,20 +1363,20 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18" s="18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E18" s="12"/>
       <c r="F18" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G18" s="22"/>
       <c r="H18" s="12"/>
@@ -1394,20 +1387,20 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E19" s="12"/>
       <c r="F19" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G19" s="22"/>
       <c r="H19" s="12"/>
@@ -1421,17 +1414,17 @@
         <v>14</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C20" s="8"/>
       <c r="D20" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F20" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G20" s="22"/>
       <c r="H20" s="12"/>
@@ -1445,17 +1438,17 @@
         <v>15</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C21" s="8"/>
       <c r="D21" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F21" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G21" s="22"/>
       <c r="H21" s="12"/>
@@ -1469,17 +1462,17 @@
         <v>16</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C22" s="8"/>
       <c r="D22" s="15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F22" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G22" s="22"/>
       <c r="H22" s="12"/>
@@ -1493,17 +1486,17 @@
         <v>17</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C23" s="8"/>
       <c r="D23" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F23" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G23" s="22"/>
       <c r="H23" s="12"/>
@@ -1517,17 +1510,17 @@
         <v>18</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C24" s="8"/>
       <c r="D24" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F24" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G24" s="22"/>
       <c r="H24" s="12"/>
@@ -1541,17 +1534,17 @@
         <v>19</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C25" s="8"/>
       <c r="D25" s="15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F25" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G25" s="22"/>
       <c r="H25" s="12"/>
@@ -1565,15 +1558,15 @@
         <v>20</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C26" s="8"/>
       <c r="D26" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E26" s="12"/>
       <c r="F26" s="21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G26" s="22"/>
       <c r="H26" s="12"/>
@@ -1587,15 +1580,15 @@
         <v>21</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C27" s="16"/>
       <c r="D27" s="17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E27" s="12"/>
       <c r="F27" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G27" s="22"/>
       <c r="H27" s="12"/>
@@ -1609,15 +1602,15 @@
         <v>22</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C28" s="16"/>
       <c r="D28" s="17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E28" s="12"/>
       <c r="F28" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G28" s="22"/>
       <c r="H28" s="12"/>
@@ -1631,15 +1624,15 @@
         <v>23</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C29" s="8"/>
       <c r="D29" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E29" s="19"/>
       <c r="F29" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G29" s="22"/>
       <c r="H29" s="12"/>
@@ -1650,20 +1643,20 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A30" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C30" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D30" s="15" t="s">
         <v>42</v>
-      </c>
-      <c r="D30" s="15" t="s">
-        <v>43</v>
       </c>
       <c r="E30" s="19"/>
       <c r="F30" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G30" s="22"/>
       <c r="H30" s="12"/>
@@ -1674,20 +1667,20 @@
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A31" s="18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D31" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E31" s="19"/>
       <c r="F31" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G31" s="22"/>
       <c r="H31" s="12"/>
@@ -1698,20 +1691,20 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A32" s="18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D32" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E32" s="12"/>
       <c r="F32" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G32" s="22"/>
       <c r="H32" s="12"/>
@@ -1722,20 +1715,20 @@
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A33" s="18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D33" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E33" s="12"/>
       <c r="F33" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G33" s="22"/>
       <c r="H33" s="12"/>
@@ -1746,20 +1739,20 @@
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A34" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D34" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E34" s="12"/>
       <c r="F34" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G34" s="22"/>
       <c r="H34" s="12"/>
@@ -1770,20 +1763,20 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A35" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D35" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E35" s="12"/>
       <c r="F35" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G35" s="22"/>
       <c r="H35" s="12"/>
@@ -1794,18 +1787,18 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A36" s="18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C36" s="8"/>
       <c r="D36" s="15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E36" s="12"/>
       <c r="F36" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G36" s="22"/>
       <c r="H36" s="12"/>
@@ -1816,20 +1809,20 @@
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A37" s="18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D37" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E37" s="12"/>
       <c r="F37" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G37" s="22"/>
       <c r="H37" s="12"/>
@@ -1840,20 +1833,20 @@
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A38" s="18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D38" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E38" s="12"/>
       <c r="F38" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G38" s="22"/>
       <c r="H38" s="12"/>
@@ -1867,17 +1860,17 @@
         <v>29</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C39" s="8"/>
       <c r="D39" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E39" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F39" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G39" s="22"/>
       <c r="H39" s="12"/>
@@ -1891,17 +1884,17 @@
         <v>30</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C40" s="8"/>
       <c r="D40" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E40" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F40" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G40" s="22"/>
       <c r="H40" s="12"/>
@@ -1915,17 +1908,17 @@
         <v>31</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C41" s="8"/>
       <c r="D41" s="15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E41" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F41" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G41" s="22"/>
       <c r="H41" s="12"/>
@@ -1939,17 +1932,17 @@
         <v>32</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C42" s="8"/>
       <c r="D42" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E42" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F42" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G42" s="22"/>
       <c r="H42" s="12"/>
@@ -1963,17 +1956,17 @@
         <v>33</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C43" s="8"/>
       <c r="D43" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E43" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F43" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G43" s="22"/>
       <c r="H43" s="12"/>
@@ -1987,17 +1980,17 @@
         <v>34</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C44" s="8"/>
       <c r="D44" s="15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E44" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F44" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G44" s="22"/>
       <c r="H44" s="12"/>
@@ -2011,15 +2004,15 @@
         <v>35</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C45" s="8"/>
       <c r="D45" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E45" s="12"/>
       <c r="F45" s="21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G45" s="22"/>
       <c r="H45" s="12"/>
@@ -2033,15 +2026,15 @@
         <v>36</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C46" s="16"/>
       <c r="D46" s="17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E46" s="12"/>
       <c r="F46" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G46" s="22"/>
       <c r="H46" s="12"/>
@@ -2055,15 +2048,15 @@
         <v>37</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C47" s="16"/>
       <c r="D47" s="17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E47" s="12"/>
       <c r="F47" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G47" s="22"/>
       <c r="H47" s="12"/>
@@ -2077,15 +2070,15 @@
         <v>38</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C48" s="8"/>
       <c r="D48" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E48" s="19"/>
       <c r="F48" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G48" s="22"/>
       <c r="H48" s="12"/>
@@ -2096,20 +2089,20 @@
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A49" s="18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C49" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D49" s="15" t="s">
         <v>42</v>
-      </c>
-      <c r="D49" s="15" t="s">
-        <v>43</v>
       </c>
       <c r="E49" s="19"/>
       <c r="F49" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G49" s="22"/>
       <c r="H49" s="12"/>
@@ -2120,20 +2113,20 @@
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A50" s="18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D50" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E50" s="19"/>
       <c r="F50" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G50" s="22"/>
       <c r="H50" s="12"/>
@@ -2144,20 +2137,20 @@
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A51" s="18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D51" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E51" s="12"/>
       <c r="F51" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G51" s="22"/>
       <c r="H51" s="12"/>
@@ -2168,20 +2161,20 @@
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A52" s="18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D52" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E52" s="12"/>
       <c r="F52" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G52" s="22"/>
       <c r="H52" s="12"/>
@@ -2192,20 +2185,20 @@
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A53" s="18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D53" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E53" s="12"/>
       <c r="F53" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G53" s="22"/>
       <c r="H53" s="12"/>
@@ -2216,20 +2209,20 @@
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A54" s="18" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D54" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E54" s="12"/>
       <c r="F54" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G54" s="22"/>
       <c r="H54" s="12"/>
@@ -2240,18 +2233,18 @@
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A55" s="18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C55" s="8"/>
       <c r="D55" s="15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E55" s="12"/>
       <c r="F55" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G55" s="22"/>
       <c r="H55" s="12"/>
@@ -2262,20 +2255,20 @@
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A56" s="18" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D56" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E56" s="12"/>
       <c r="F56" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G56" s="22"/>
       <c r="H56" s="12"/>
@@ -2286,20 +2279,20 @@
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A57" s="18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D57" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E57" s="12"/>
       <c r="F57" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G57" s="22"/>
       <c r="H57" s="12"/>
@@ -2313,17 +2306,17 @@
         <v>44</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C58" s="8"/>
       <c r="D58" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E58" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F58" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G58" s="22"/>
       <c r="H58" s="19"/>
@@ -2337,17 +2330,17 @@
         <v>45</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C59" s="8"/>
       <c r="D59" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E59" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F59" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G59" s="22"/>
       <c r="H59" s="19"/>
@@ -2361,17 +2354,17 @@
         <v>46</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C60" s="8"/>
       <c r="D60" s="15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E60" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F60" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G60" s="22"/>
       <c r="H60" s="19"/>
@@ -2385,17 +2378,17 @@
         <v>47</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C61" s="8"/>
       <c r="D61" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E61" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F61" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G61" s="22"/>
       <c r="H61" s="19"/>
@@ -2409,17 +2402,17 @@
         <v>48</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C62" s="8"/>
       <c r="D62" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E62" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F62" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G62" s="22"/>
       <c r="H62" s="19"/>
@@ -2433,17 +2426,17 @@
         <v>49</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C63" s="8"/>
       <c r="D63" s="15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E63" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F63" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G63" s="22"/>
       <c r="H63" s="19"/>
@@ -2457,15 +2450,15 @@
         <v>50</v>
       </c>
       <c r="B64" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C64" s="8"/>
       <c r="D64" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E64" s="12"/>
       <c r="F64" s="21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G64" s="22"/>
       <c r="H64" s="19"/>
@@ -2479,15 +2472,15 @@
         <v>51</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C65" s="16"/>
       <c r="D65" s="17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E65" s="12"/>
       <c r="F65" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G65" s="22"/>
       <c r="H65" s="19"/>
@@ -2501,15 +2494,15 @@
         <v>52</v>
       </c>
       <c r="B66" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C66" s="16"/>
       <c r="D66" s="17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E66" s="12"/>
       <c r="F66" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G66" s="22"/>
       <c r="H66" s="19"/>

</xml_diff>

<commit_message>
revive the "CurrencyDataPoint" component + use it for totalAmounts only
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/euTaxonomyNonFinancials/EutaxonomyNonFinancials.xlsx
+++ b/dataland-framework-toolbox/inputs/euTaxonomyNonFinancials/EutaxonomyNonFinancials.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d92432\Documents\Projekte\02-Dataland\Dataland\dataland-framework-toolbox\inputs\euTaxonomyNonFinancials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{726DAF2C-5FF6-44E1-8DCC-62D0C182EB89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62C78E3A-6442-4458-B05F-FC66F185D6D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="38640" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="38620" windowHeight="21220" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Framework Data Model" sheetId="1" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="91">
   <si>
     <t>Field Identifier</t>
   </si>
@@ -327,6 +327,9 @@
   </si>
   <si>
     <t>Report Preupload</t>
+  </si>
+  <si>
+    <t>AmountWithCurrency</t>
   </si>
 </sst>
 </file>
@@ -919,8 +922,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1234,7 +1237,7 @@
       </c>
       <c r="E12" s="19"/>
       <c r="F12" s="21" t="s">
-        <v>39</v>
+        <v>90</v>
       </c>
       <c r="G12" s="22"/>
       <c r="H12" s="12"/>
@@ -1282,7 +1285,7 @@
       </c>
       <c r="E14" s="12"/>
       <c r="F14" s="21" t="s">
-        <v>39</v>
+        <v>90</v>
       </c>
       <c r="G14" s="22"/>
       <c r="H14" s="12"/>
@@ -1330,7 +1333,7 @@
       </c>
       <c r="E16" s="12"/>
       <c r="F16" s="21" t="s">
-        <v>39</v>
+        <v>90</v>
       </c>
       <c r="G16" s="22"/>
       <c r="H16" s="12"/>
@@ -1400,7 +1403,7 @@
       </c>
       <c r="E19" s="12"/>
       <c r="F19" s="21" t="s">
-        <v>39</v>
+        <v>90</v>
       </c>
       <c r="G19" s="22"/>
       <c r="H19" s="12"/>
@@ -1636,7 +1639,9 @@
       </c>
       <c r="G29" s="22"/>
       <c r="H29" s="12"/>
-      <c r="I29" s="12"/>
+      <c r="I29" s="12" t="s">
+        <v>36</v>
+      </c>
       <c r="J29" s="12"/>
       <c r="K29" s="12"/>
       <c r="L29" s="12"/>
@@ -1680,7 +1685,7 @@
       </c>
       <c r="E31" s="19"/>
       <c r="F31" s="21" t="s">
-        <v>39</v>
+        <v>90</v>
       </c>
       <c r="G31" s="22"/>
       <c r="H31" s="12"/>
@@ -1728,7 +1733,7 @@
       </c>
       <c r="E33" s="12"/>
       <c r="F33" s="21" t="s">
-        <v>39</v>
+        <v>90</v>
       </c>
       <c r="G33" s="22"/>
       <c r="H33" s="12"/>
@@ -1776,7 +1781,7 @@
       </c>
       <c r="E35" s="12"/>
       <c r="F35" s="21" t="s">
-        <v>39</v>
+        <v>90</v>
       </c>
       <c r="G35" s="22"/>
       <c r="H35" s="12"/>
@@ -1846,7 +1851,7 @@
       </c>
       <c r="E38" s="12"/>
       <c r="F38" s="21" t="s">
-        <v>39</v>
+        <v>90</v>
       </c>
       <c r="G38" s="22"/>
       <c r="H38" s="12"/>
@@ -2082,7 +2087,9 @@
       </c>
       <c r="G48" s="22"/>
       <c r="H48" s="12"/>
-      <c r="I48" s="12"/>
+      <c r="I48" s="12" t="s">
+        <v>36</v>
+      </c>
       <c r="J48" s="12"/>
       <c r="K48" s="12"/>
       <c r="L48" s="12"/>
@@ -2126,7 +2133,7 @@
       </c>
       <c r="E50" s="19"/>
       <c r="F50" s="21" t="s">
-        <v>39</v>
+        <v>90</v>
       </c>
       <c r="G50" s="22"/>
       <c r="H50" s="12"/>
@@ -2174,7 +2181,7 @@
       </c>
       <c r="E52" s="12"/>
       <c r="F52" s="21" t="s">
-        <v>39</v>
+        <v>90</v>
       </c>
       <c r="G52" s="22"/>
       <c r="H52" s="12"/>
@@ -2222,7 +2229,7 @@
       </c>
       <c r="E54" s="12"/>
       <c r="F54" s="21" t="s">
-        <v>39</v>
+        <v>90</v>
       </c>
       <c r="G54" s="22"/>
       <c r="H54" s="12"/>
@@ -2292,7 +2299,7 @@
       </c>
       <c r="E57" s="12"/>
       <c r="F57" s="21" t="s">
-        <v>39</v>
+        <v>90</v>
       </c>
       <c r="G57" s="22"/>
       <c r="H57" s="12"/>

</xml_diff>

<commit_message>
progress in currency points
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/euTaxonomyNonFinancials/EutaxonomyNonFinancials.xlsx
+++ b/dataland-framework-toolbox/inputs/euTaxonomyNonFinancials/EutaxonomyNonFinancials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d92432\Documents\Projekte\02-Dataland\Dataland\dataland-framework-toolbox\inputs\euTaxonomyNonFinancials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62C78E3A-6442-4458-B05F-FC66F185D6D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBB2E4E2-B174-4FC7-8C49-EDF4F1150C49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-110" windowWidth="38620" windowHeight="21220" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -329,7 +329,7 @@
     <t>Report Preupload</t>
   </si>
   <si>
-    <t>AmountWithCurrency</t>
+    <t>Custom – AmountWithCurrency</t>
   </si>
 </sst>
 </file>
@@ -923,7 +923,7 @@
   <dimension ref="A1:L66"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
exclude old data model wip
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/euTaxonomyNonFinancials/EutaxonomyNonFinancials.xlsx
+++ b/dataland-framework-toolbox/inputs/euTaxonomyNonFinancials/EutaxonomyNonFinancials.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d92432\Documents\Projekte\02-Dataland\Dataland\dataland-framework-toolbox\inputs\euTaxonomyNonFinancials\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d92928\Documents\Projects\Dataland\Dataland\dataland-framework-toolbox\inputs\euTaxonomyNonFinancials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBB2E4E2-B174-4FC7-8C49-EDF4F1150C49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5699FD66-CA24-4395-9BC8-29E3D2EFAB1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="38620" windowHeight="21220" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Framework Data Model" sheetId="1" r:id="rId1"/>
@@ -218,9 +218,6 @@
     <t>Non-Aligned Activities</t>
   </si>
   <si>
-    <t>Custom - List of EuTaxonomyActivity</t>
-  </si>
-  <si>
     <t>Aligned Share</t>
   </si>
   <si>
@@ -245,9 +242,6 @@
     <t>Aligned Activities</t>
   </si>
   <si>
-    <t>Custom - AlignedActivitiesFormField</t>
-  </si>
-  <si>
     <t>Enabling Share In Percent</t>
   </si>
   <si>
@@ -330,6 +324,12 @@
   </si>
   <si>
     <t>Custom – AmountWithCurrency</t>
+  </si>
+  <si>
+    <t>Custom – AlignedActivitiesFormField</t>
+  </si>
+  <si>
+    <t>Custom – List of EuTaxonomyActivity</t>
   </si>
 </sst>
 </file>
@@ -922,21 +922,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="20.26953125" customWidth="1"/>
-    <col min="4" max="4" width="70.36328125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="77.90625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="28.1796875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="26.26953125" customWidth="1"/>
-    <col min="8" max="12" width="14.36328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.21875" customWidth="1"/>
+    <col min="4" max="4" width="70.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="77.88671875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="28.21875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="26.21875" customWidth="1"/>
+    <col min="8" max="12" width="14.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -974,7 +974,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="7">
         <v>0</v>
       </c>
@@ -992,7 +992,7 @@
         <v>17</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H2" s="11"/>
       <c r="I2" s="12"/>
@@ -1000,7 +1000,7 @@
       <c r="K2" s="12"/>
       <c r="L2" s="12"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="7"/>
       <c r="B3" s="8" t="s">
         <v>12</v>
@@ -1022,7 +1022,7 @@
       <c r="K3" s="12"/>
       <c r="L3" s="12"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>1</v>
       </c>
@@ -1048,7 +1048,7 @@
       <c r="K4" s="11"/>
       <c r="L4" s="12"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>2</v>
       </c>
@@ -1074,7 +1074,7 @@
       <c r="K5" s="12"/>
       <c r="L5" s="12"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>3</v>
       </c>
@@ -1100,7 +1100,7 @@
       <c r="K6" s="12"/>
       <c r="L6" s="12"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>4</v>
       </c>
@@ -1126,7 +1126,7 @@
       <c r="K7" s="12"/>
       <c r="L7" s="12"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>5</v>
       </c>
@@ -1141,7 +1141,7 @@
         <v>27</v>
       </c>
       <c r="F8" s="20" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G8" s="22"/>
       <c r="H8" s="12"/>
@@ -1150,7 +1150,7 @@
       <c r="K8" s="12"/>
       <c r="L8" s="12"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>6</v>
       </c>
@@ -1159,11 +1159,11 @@
       </c>
       <c r="C9" s="8"/>
       <c r="D9" s="14" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E9" s="12"/>
       <c r="F9" s="20" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G9" s="23" t="s">
         <v>14</v>
@@ -1174,7 +1174,7 @@
       <c r="K9" s="12"/>
       <c r="L9" s="12"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>8</v>
       </c>
@@ -1198,7 +1198,7 @@
       <c r="K10" s="12"/>
       <c r="L10" s="12"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="18" t="s">
         <v>44</v>
       </c>
@@ -1222,7 +1222,7 @@
       <c r="K11" s="12"/>
       <c r="L11" s="12"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="18" t="s">
         <v>45</v>
       </c>
@@ -1237,7 +1237,7 @@
       </c>
       <c r="E12" s="19"/>
       <c r="F12" s="21" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G12" s="22"/>
       <c r="H12" s="12"/>
@@ -1246,7 +1246,7 @@
       <c r="K12" s="12"/>
       <c r="L12" s="12"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="18" t="s">
         <v>47</v>
       </c>
@@ -1270,7 +1270,7 @@
       <c r="K13" s="12"/>
       <c r="L13" s="12"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="18" t="s">
         <v>48</v>
       </c>
@@ -1285,7 +1285,7 @@
       </c>
       <c r="E14" s="12"/>
       <c r="F14" s="21" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G14" s="22"/>
       <c r="H14" s="12"/>
@@ -1294,7 +1294,7 @@
       <c r="K14" s="12"/>
       <c r="L14" s="12"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="18" t="s">
         <v>50</v>
       </c>
@@ -1318,7 +1318,7 @@
       <c r="K15" s="12"/>
       <c r="L15" s="12"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="18" t="s">
         <v>51</v>
       </c>
@@ -1333,7 +1333,7 @@
       </c>
       <c r="E16" s="12"/>
       <c r="F16" s="21" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G16" s="22"/>
       <c r="H16" s="12"/>
@@ -1342,9 +1342,9 @@
       <c r="K16" s="12"/>
       <c r="L16" s="12"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="18" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>34</v>
@@ -1355,7 +1355,7 @@
       </c>
       <c r="E17" s="12"/>
       <c r="F17" s="21" t="s">
-        <v>53</v>
+        <v>90</v>
       </c>
       <c r="G17" s="22"/>
       <c r="H17" s="12"/>
@@ -1364,15 +1364,15 @@
       <c r="K17" s="12"/>
       <c r="L17" s="12"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="18" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B18" s="8" t="s">
         <v>34</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D18" s="15" t="s">
         <v>42</v>
@@ -1388,22 +1388,22 @@
       <c r="K18" s="12"/>
       <c r="L18" s="12"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="18" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>34</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D19" s="15" t="s">
         <v>43</v>
       </c>
       <c r="E19" s="12"/>
       <c r="F19" s="21" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G19" s="22"/>
       <c r="H19" s="12"/>
@@ -1412,7 +1412,7 @@
       <c r="K19" s="12"/>
       <c r="L19" s="12"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="7">
         <v>14</v>
       </c>
@@ -1421,7 +1421,7 @@
       </c>
       <c r="C20" s="8"/>
       <c r="D20" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E20" s="12" t="s">
         <v>35</v>
@@ -1436,7 +1436,7 @@
       <c r="K20" s="12"/>
       <c r="L20" s="12"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="7">
         <v>15</v>
       </c>
@@ -1445,7 +1445,7 @@
       </c>
       <c r="C21" s="8"/>
       <c r="D21" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E21" s="12" t="s">
         <v>35</v>
@@ -1460,7 +1460,7 @@
       <c r="K21" s="12"/>
       <c r="L21" s="12"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="7">
         <v>16</v>
       </c>
@@ -1469,7 +1469,7 @@
       </c>
       <c r="C22" s="8"/>
       <c r="D22" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E22" s="12" t="s">
         <v>35</v>
@@ -1484,7 +1484,7 @@
       <c r="K22" s="12"/>
       <c r="L22" s="12"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="7">
         <v>17</v>
       </c>
@@ -1493,7 +1493,7 @@
       </c>
       <c r="C23" s="8"/>
       <c r="D23" s="15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E23" s="12" t="s">
         <v>35</v>
@@ -1508,7 +1508,7 @@
       <c r="K23" s="12"/>
       <c r="L23" s="12"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="7">
         <v>18</v>
       </c>
@@ -1517,7 +1517,7 @@
       </c>
       <c r="C24" s="8"/>
       <c r="D24" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E24" s="12" t="s">
         <v>35</v>
@@ -1532,7 +1532,7 @@
       <c r="K24" s="12"/>
       <c r="L24" s="12"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="7">
         <v>19</v>
       </c>
@@ -1541,7 +1541,7 @@
       </c>
       <c r="C25" s="8"/>
       <c r="D25" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E25" s="12" t="s">
         <v>35</v>
@@ -1556,7 +1556,7 @@
       <c r="K25" s="12"/>
       <c r="L25" s="12"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="7">
         <v>20</v>
       </c>
@@ -1565,11 +1565,11 @@
       </c>
       <c r="C26" s="8"/>
       <c r="D26" s="15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E26" s="12"/>
       <c r="F26" s="21" t="s">
-        <v>62</v>
+        <v>89</v>
       </c>
       <c r="G26" s="22"/>
       <c r="H26" s="12"/>
@@ -1578,7 +1578,7 @@
       <c r="K26" s="12"/>
       <c r="L26" s="12"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="7">
         <v>21</v>
       </c>
@@ -1587,7 +1587,7 @@
       </c>
       <c r="C27" s="16"/>
       <c r="D27" s="17" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E27" s="12"/>
       <c r="F27" s="21" t="s">
@@ -1600,7 +1600,7 @@
       <c r="K27" s="12"/>
       <c r="L27" s="12"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="7">
         <v>22</v>
       </c>
@@ -1609,7 +1609,7 @@
       </c>
       <c r="C28" s="16"/>
       <c r="D28" s="17" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E28" s="12"/>
       <c r="F28" s="21" t="s">
@@ -1622,7 +1622,7 @@
       <c r="K28" s="12"/>
       <c r="L28" s="12"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="7">
         <v>23</v>
       </c>
@@ -1646,9 +1646,9 @@
       <c r="K29" s="12"/>
       <c r="L29" s="12"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B30" s="8" t="s">
         <v>37</v>
@@ -1670,9 +1670,9 @@
       <c r="K30" s="12"/>
       <c r="L30" s="12"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="18" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B31" s="8" t="s">
         <v>37</v>
@@ -1685,7 +1685,7 @@
       </c>
       <c r="E31" s="19"/>
       <c r="F31" s="21" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G31" s="22"/>
       <c r="H31" s="12"/>
@@ -1694,9 +1694,9 @@
       <c r="K31" s="12"/>
       <c r="L31" s="12"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B32" s="8" t="s">
         <v>37</v>
@@ -1718,9 +1718,9 @@
       <c r="K32" s="12"/>
       <c r="L32" s="12"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" s="18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B33" s="8" t="s">
         <v>37</v>
@@ -1733,7 +1733,7 @@
       </c>
       <c r="E33" s="12"/>
       <c r="F33" s="21" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G33" s="22"/>
       <c r="H33" s="12"/>
@@ -1742,9 +1742,9 @@
       <c r="K33" s="12"/>
       <c r="L33" s="12"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" s="18" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B34" s="8" t="s">
         <v>37</v>
@@ -1766,9 +1766,9 @@
       <c r="K34" s="12"/>
       <c r="L34" s="12"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B35" s="8" t="s">
         <v>37</v>
@@ -1781,7 +1781,7 @@
       </c>
       <c r="E35" s="12"/>
       <c r="F35" s="21" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G35" s="22"/>
       <c r="H35" s="12"/>
@@ -1790,9 +1790,9 @@
       <c r="K35" s="12"/>
       <c r="L35" s="12"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" s="18" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B36" s="8" t="s">
         <v>37</v>
@@ -1803,7 +1803,7 @@
       </c>
       <c r="E36" s="12"/>
       <c r="F36" s="21" t="s">
-        <v>53</v>
+        <v>90</v>
       </c>
       <c r="G36" s="22"/>
       <c r="H36" s="12"/>
@@ -1812,15 +1812,15 @@
       <c r="K36" s="12"/>
       <c r="L36" s="12"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" s="18" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B37" s="8" t="s">
         <v>37</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D37" s="15" t="s">
         <v>42</v>
@@ -1836,22 +1836,22 @@
       <c r="K37" s="12"/>
       <c r="L37" s="12"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" s="18" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B38" s="8" t="s">
         <v>37</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D38" s="15" t="s">
         <v>43</v>
       </c>
       <c r="E38" s="12"/>
       <c r="F38" s="21" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G38" s="22"/>
       <c r="H38" s="12"/>
@@ -1860,7 +1860,7 @@
       <c r="K38" s="12"/>
       <c r="L38" s="12"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" s="7">
         <v>29</v>
       </c>
@@ -1869,7 +1869,7 @@
       </c>
       <c r="C39" s="8"/>
       <c r="D39" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E39" s="12" t="s">
         <v>35</v>
@@ -1884,7 +1884,7 @@
       <c r="K39" s="12"/>
       <c r="L39" s="12"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" s="7">
         <v>30</v>
       </c>
@@ -1893,7 +1893,7 @@
       </c>
       <c r="C40" s="8"/>
       <c r="D40" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E40" s="12" t="s">
         <v>35</v>
@@ -1908,7 +1908,7 @@
       <c r="K40" s="12"/>
       <c r="L40" s="12"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" s="7">
         <v>31</v>
       </c>
@@ -1917,7 +1917,7 @@
       </c>
       <c r="C41" s="8"/>
       <c r="D41" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E41" s="12" t="s">
         <v>35</v>
@@ -1932,7 +1932,7 @@
       <c r="K41" s="12"/>
       <c r="L41" s="12"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" s="7">
         <v>32</v>
       </c>
@@ -1941,7 +1941,7 @@
       </c>
       <c r="C42" s="8"/>
       <c r="D42" s="15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E42" s="12" t="s">
         <v>35</v>
@@ -1956,7 +1956,7 @@
       <c r="K42" s="12"/>
       <c r="L42" s="12"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" s="7">
         <v>33</v>
       </c>
@@ -1965,7 +1965,7 @@
       </c>
       <c r="C43" s="8"/>
       <c r="D43" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E43" s="12" t="s">
         <v>35</v>
@@ -1980,7 +1980,7 @@
       <c r="K43" s="12"/>
       <c r="L43" s="12"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" s="7">
         <v>34</v>
       </c>
@@ -1989,7 +1989,7 @@
       </c>
       <c r="C44" s="8"/>
       <c r="D44" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E44" s="12" t="s">
         <v>35</v>
@@ -2004,7 +2004,7 @@
       <c r="K44" s="12"/>
       <c r="L44" s="12"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" s="7">
         <v>35</v>
       </c>
@@ -2013,11 +2013,11 @@
       </c>
       <c r="C45" s="8"/>
       <c r="D45" s="15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E45" s="12"/>
       <c r="F45" s="21" t="s">
-        <v>62</v>
+        <v>89</v>
       </c>
       <c r="G45" s="22"/>
       <c r="H45" s="12"/>
@@ -2026,7 +2026,7 @@
       <c r="K45" s="12"/>
       <c r="L45" s="12"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" s="7">
         <v>36</v>
       </c>
@@ -2035,7 +2035,7 @@
       </c>
       <c r="C46" s="16"/>
       <c r="D46" s="17" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E46" s="12"/>
       <c r="F46" s="21" t="s">
@@ -2048,7 +2048,7 @@
       <c r="K46" s="12"/>
       <c r="L46" s="12"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" s="7">
         <v>37</v>
       </c>
@@ -2057,7 +2057,7 @@
       </c>
       <c r="C47" s="16"/>
       <c r="D47" s="17" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E47" s="12"/>
       <c r="F47" s="21" t="s">
@@ -2070,7 +2070,7 @@
       <c r="K47" s="12"/>
       <c r="L47" s="12"/>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48" s="7">
         <v>38</v>
       </c>
@@ -2094,9 +2094,9 @@
       <c r="K48" s="12"/>
       <c r="L48" s="12"/>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" s="18" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B49" s="8" t="s">
         <v>38</v>
@@ -2118,9 +2118,9 @@
       <c r="K49" s="12"/>
       <c r="L49" s="12"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" s="18" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B50" s="8" t="s">
         <v>38</v>
@@ -2133,7 +2133,7 @@
       </c>
       <c r="E50" s="19"/>
       <c r="F50" s="21" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G50" s="22"/>
       <c r="H50" s="12"/>
@@ -2142,9 +2142,9 @@
       <c r="K50" s="12"/>
       <c r="L50" s="12"/>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" s="18" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B51" s="8" t="s">
         <v>38</v>
@@ -2166,9 +2166,9 @@
       <c r="K51" s="12"/>
       <c r="L51" s="12"/>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52" s="18" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B52" s="8" t="s">
         <v>38</v>
@@ -2181,7 +2181,7 @@
       </c>
       <c r="E52" s="12"/>
       <c r="F52" s="21" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G52" s="22"/>
       <c r="H52" s="12"/>
@@ -2190,9 +2190,9 @@
       <c r="K52" s="12"/>
       <c r="L52" s="12"/>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53" s="18" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B53" s="8" t="s">
         <v>38</v>
@@ -2214,9 +2214,9 @@
       <c r="K53" s="12"/>
       <c r="L53" s="12"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" s="18" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B54" s="8" t="s">
         <v>38</v>
@@ -2229,7 +2229,7 @@
       </c>
       <c r="E54" s="12"/>
       <c r="F54" s="21" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G54" s="22"/>
       <c r="H54" s="12"/>
@@ -2238,9 +2238,9 @@
       <c r="K54" s="12"/>
       <c r="L54" s="12"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55" s="18" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B55" s="8" t="s">
         <v>38</v>
@@ -2251,7 +2251,7 @@
       </c>
       <c r="E55" s="12"/>
       <c r="F55" s="21" t="s">
-        <v>53</v>
+        <v>90</v>
       </c>
       <c r="G55" s="22"/>
       <c r="H55" s="12"/>
@@ -2260,15 +2260,15 @@
       <c r="K55" s="12"/>
       <c r="L55" s="12"/>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56" s="18" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B56" s="8" t="s">
         <v>38</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D56" s="15" t="s">
         <v>42</v>
@@ -2284,22 +2284,22 @@
       <c r="K56" s="12"/>
       <c r="L56" s="12"/>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57" s="18" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B57" s="8" t="s">
         <v>38</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D57" s="15" t="s">
         <v>43</v>
       </c>
       <c r="E57" s="12"/>
       <c r="F57" s="21" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G57" s="22"/>
       <c r="H57" s="12"/>
@@ -2308,7 +2308,7 @@
       <c r="K57" s="12"/>
       <c r="L57" s="12"/>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58" s="7">
         <v>44</v>
       </c>
@@ -2317,7 +2317,7 @@
       </c>
       <c r="C58" s="8"/>
       <c r="D58" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E58" s="12" t="s">
         <v>35</v>
@@ -2332,7 +2332,7 @@
       <c r="K58" s="19"/>
       <c r="L58" s="19"/>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59" s="7">
         <v>45</v>
       </c>
@@ -2341,7 +2341,7 @@
       </c>
       <c r="C59" s="8"/>
       <c r="D59" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E59" s="12" t="s">
         <v>35</v>
@@ -2356,7 +2356,7 @@
       <c r="K59" s="19"/>
       <c r="L59" s="19"/>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60" s="7">
         <v>46</v>
       </c>
@@ -2365,7 +2365,7 @@
       </c>
       <c r="C60" s="8"/>
       <c r="D60" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E60" s="12" t="s">
         <v>35</v>
@@ -2380,7 +2380,7 @@
       <c r="K60" s="19"/>
       <c r="L60" s="19"/>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61" s="7">
         <v>47</v>
       </c>
@@ -2389,7 +2389,7 @@
       </c>
       <c r="C61" s="8"/>
       <c r="D61" s="15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E61" s="12" t="s">
         <v>35</v>
@@ -2404,7 +2404,7 @@
       <c r="K61" s="19"/>
       <c r="L61" s="19"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62" s="7">
         <v>48</v>
       </c>
@@ -2413,7 +2413,7 @@
       </c>
       <c r="C62" s="8"/>
       <c r="D62" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E62" s="12" t="s">
         <v>35</v>
@@ -2428,7 +2428,7 @@
       <c r="K62" s="19"/>
       <c r="L62" s="19"/>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63" s="7">
         <v>49</v>
       </c>
@@ -2437,7 +2437,7 @@
       </c>
       <c r="C63" s="8"/>
       <c r="D63" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E63" s="12" t="s">
         <v>35</v>
@@ -2452,7 +2452,7 @@
       <c r="K63" s="19"/>
       <c r="L63" s="19"/>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64" s="7">
         <v>50</v>
       </c>
@@ -2461,11 +2461,11 @@
       </c>
       <c r="C64" s="8"/>
       <c r="D64" s="15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E64" s="12"/>
       <c r="F64" s="21" t="s">
-        <v>62</v>
+        <v>89</v>
       </c>
       <c r="G64" s="22"/>
       <c r="H64" s="19"/>
@@ -2474,7 +2474,7 @@
       <c r="K64" s="19"/>
       <c r="L64" s="19"/>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A65" s="7">
         <v>51</v>
       </c>
@@ -2483,7 +2483,7 @@
       </c>
       <c r="C65" s="16"/>
       <c r="D65" s="17" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E65" s="12"/>
       <c r="F65" s="21" t="s">
@@ -2496,7 +2496,7 @@
       <c r="K65" s="19"/>
       <c r="L65" s="19"/>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A66" s="7">
         <v>52</v>
       </c>
@@ -2505,7 +2505,7 @@
       </c>
       <c r="C66" s="16"/>
       <c r="D66" s="17" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E66" s="12"/>
       <c r="F66" s="21" t="s">

</xml_diff>

<commit_message>
upload config and fix
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/euTaxonomyNonFinancials/EutaxonomyNonFinancials.xlsx
+++ b/dataland-framework-toolbox/inputs/euTaxonomyNonFinancials/EutaxonomyNonFinancials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d92928\Documents\Projects\Dataland\Dataland\dataland-framework-toolbox\inputs\euTaxonomyNonFinancials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5699FD66-CA24-4395-9BC8-29E3D2EFAB1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{426B5BC0-BD5A-4F95-97FE-ACC2B6BDB794}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -47,7 +47,7 @@
     <definedName name="IQ_YTD">3000</definedName>
     <definedName name="IQ_YTDMONTH">130000</definedName>
   </definedNames>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -158,9 +158,6 @@
     <t>Level of assurance of the EU Taxonomy disclosure (Reasonable Assurance, Limited Assurance, None)</t>
   </si>
   <si>
-    <t>Custom – EuTaxonomyAssuranceComponent</t>
-  </si>
-  <si>
     <t>Revenue</t>
   </si>
   <si>
@@ -323,20 +320,23 @@
     <t>Report Preupload</t>
   </si>
   <si>
-    <t>Custom – AmountWithCurrency</t>
-  </si>
-  <si>
-    <t>Custom – AlignedActivitiesFormField</t>
-  </si>
-  <si>
-    <t>Custom – List of EuTaxonomyActivity</t>
+    <t>Custom AmountWithCurrency</t>
+  </si>
+  <si>
+    <t>Custom List of EuTaxonomyActivity</t>
+  </si>
+  <si>
+    <t>Custom AlignedActivitiesFormField</t>
+  </si>
+  <si>
+    <t>Custom EuTaxonomyAssuranceComponent</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -399,6 +399,12 @@
     <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -612,7 +618,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -658,6 +664,7 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -922,8 +929,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="B19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -931,7 +938,7 @@
     <col min="3" max="3" width="20.21875" customWidth="1"/>
     <col min="4" max="4" width="70.33203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="77.88671875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="28.21875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="38.88671875" style="1" customWidth="1"/>
     <col min="7" max="7" width="26.21875" customWidth="1"/>
     <col min="8" max="12" width="14.33203125" style="1" customWidth="1"/>
   </cols>
@@ -992,7 +999,7 @@
         <v>17</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H2" s="11"/>
       <c r="I2" s="12"/>
@@ -1114,8 +1121,8 @@
       <c r="E7" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="F7" s="21" t="s">
-        <v>33</v>
+      <c r="F7" s="27" t="s">
+        <v>90</v>
       </c>
       <c r="G7" s="26" t="s">
         <v>14</v>
@@ -1141,7 +1148,7 @@
         <v>27</v>
       </c>
       <c r="F8" s="20" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G8" s="22"/>
       <c r="H8" s="12"/>
@@ -1159,11 +1166,11 @@
       </c>
       <c r="C9" s="8"/>
       <c r="D9" s="14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E9" s="12"/>
       <c r="F9" s="20" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G9" s="23" t="s">
         <v>14</v>
@@ -1179,20 +1186,20 @@
         <v>8</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C10" s="8"/>
       <c r="D10" s="15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E10" s="19"/>
       <c r="F10" s="21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G10" s="22"/>
       <c r="H10" s="12"/>
       <c r="I10" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J10" s="12"/>
       <c r="K10" s="12"/>
@@ -1200,16 +1207,16 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C11" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="15" t="s">
         <v>41</v>
-      </c>
-      <c r="D11" s="15" t="s">
-        <v>42</v>
       </c>
       <c r="E11" s="19"/>
       <c r="F11" s="21" t="s">
@@ -1224,20 +1231,20 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E12" s="19"/>
       <c r="F12" s="21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G12" s="22"/>
       <c r="H12" s="12"/>
@@ -1248,16 +1255,16 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E13" s="12"/>
       <c r="F13" s="21" t="s">
@@ -1272,20 +1279,20 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E14" s="12"/>
       <c r="F14" s="21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G14" s="22"/>
       <c r="H14" s="12"/>
@@ -1296,16 +1303,16 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E15" s="12"/>
       <c r="F15" s="21" t="s">
@@ -1320,20 +1327,20 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E16" s="12"/>
       <c r="F16" s="21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G16" s="22"/>
       <c r="H16" s="12"/>
@@ -1344,18 +1351,18 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C17" s="8"/>
       <c r="D17" s="15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E17" s="12"/>
       <c r="F17" s="21" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G17" s="22"/>
       <c r="H17" s="12"/>
@@ -1366,16 +1373,16 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E18" s="12"/>
       <c r="F18" s="21" t="s">
@@ -1390,20 +1397,20 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E19" s="12"/>
       <c r="F19" s="21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G19" s="22"/>
       <c r="H19" s="12"/>
@@ -1417,14 +1424,14 @@
         <v>14</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C20" s="8"/>
       <c r="D20" s="15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F20" s="21" t="s">
         <v>28</v>
@@ -1441,14 +1448,14 @@
         <v>15</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C21" s="8"/>
       <c r="D21" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F21" s="21" t="s">
         <v>28</v>
@@ -1465,14 +1472,14 @@
         <v>16</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C22" s="8"/>
       <c r="D22" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F22" s="21" t="s">
         <v>28</v>
@@ -1489,14 +1496,14 @@
         <v>17</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C23" s="8"/>
       <c r="D23" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F23" s="21" t="s">
         <v>28</v>
@@ -1513,14 +1520,14 @@
         <v>18</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C24" s="8"/>
       <c r="D24" s="15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F24" s="21" t="s">
         <v>28</v>
@@ -1537,14 +1544,14 @@
         <v>19</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C25" s="8"/>
       <c r="D25" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F25" s="21" t="s">
         <v>28</v>
@@ -1561,11 +1568,11 @@
         <v>20</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C26" s="8"/>
       <c r="D26" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E26" s="12"/>
       <c r="F26" s="21" t="s">
@@ -1583,11 +1590,11 @@
         <v>21</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C27" s="16"/>
       <c r="D27" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E27" s="12"/>
       <c r="F27" s="21" t="s">
@@ -1605,11 +1612,11 @@
         <v>22</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C28" s="16"/>
       <c r="D28" s="17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E28" s="12"/>
       <c r="F28" s="21" t="s">
@@ -1627,20 +1634,20 @@
         <v>23</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C29" s="8"/>
       <c r="D29" s="15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E29" s="19"/>
       <c r="F29" s="21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G29" s="22"/>
       <c r="H29" s="12"/>
       <c r="I29" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J29" s="12"/>
       <c r="K29" s="12"/>
@@ -1648,16 +1655,16 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C30" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D30" s="15" t="s">
         <v>41</v>
-      </c>
-      <c r="D30" s="15" t="s">
-        <v>42</v>
       </c>
       <c r="E30" s="19"/>
       <c r="F30" s="21" t="s">
@@ -1672,20 +1679,20 @@
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D31" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E31" s="19"/>
       <c r="F31" s="21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G31" s="22"/>
       <c r="H31" s="12"/>
@@ -1696,16 +1703,16 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D32" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E32" s="12"/>
       <c r="F32" s="21" t="s">
@@ -1720,20 +1727,20 @@
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" s="18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D33" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E33" s="12"/>
       <c r="F33" s="21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G33" s="22"/>
       <c r="H33" s="12"/>
@@ -1744,16 +1751,16 @@
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" s="18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D34" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E34" s="12"/>
       <c r="F34" s="21" t="s">
@@ -1768,20 +1775,20 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D35" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E35" s="12"/>
       <c r="F35" s="21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G35" s="22"/>
       <c r="H35" s="12"/>
@@ -1792,18 +1799,18 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" s="18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C36" s="8"/>
       <c r="D36" s="15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E36" s="12"/>
       <c r="F36" s="21" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G36" s="22"/>
       <c r="H36" s="12"/>
@@ -1814,16 +1821,16 @@
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D37" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E37" s="12"/>
       <c r="F37" s="21" t="s">
@@ -1838,20 +1845,20 @@
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D38" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E38" s="12"/>
       <c r="F38" s="21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G38" s="22"/>
       <c r="H38" s="12"/>
@@ -1865,14 +1872,14 @@
         <v>29</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C39" s="8"/>
       <c r="D39" s="15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E39" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F39" s="21" t="s">
         <v>28</v>
@@ -1889,14 +1896,14 @@
         <v>30</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C40" s="8"/>
       <c r="D40" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E40" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F40" s="21" t="s">
         <v>28</v>
@@ -1913,14 +1920,14 @@
         <v>31</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C41" s="8"/>
       <c r="D41" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E41" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F41" s="21" t="s">
         <v>28</v>
@@ -1937,14 +1944,14 @@
         <v>32</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C42" s="8"/>
       <c r="D42" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E42" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F42" s="21" t="s">
         <v>28</v>
@@ -1961,14 +1968,14 @@
         <v>33</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C43" s="8"/>
       <c r="D43" s="15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E43" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F43" s="21" t="s">
         <v>28</v>
@@ -1985,14 +1992,14 @@
         <v>34</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C44" s="8"/>
       <c r="D44" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E44" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F44" s="21" t="s">
         <v>28</v>
@@ -2009,11 +2016,11 @@
         <v>35</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C45" s="8"/>
       <c r="D45" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E45" s="12"/>
       <c r="F45" s="21" t="s">
@@ -2031,11 +2038,11 @@
         <v>36</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C46" s="16"/>
       <c r="D46" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E46" s="12"/>
       <c r="F46" s="21" t="s">
@@ -2053,11 +2060,11 @@
         <v>37</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C47" s="16"/>
       <c r="D47" s="17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E47" s="12"/>
       <c r="F47" s="21" t="s">
@@ -2075,20 +2082,20 @@
         <v>38</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C48" s="8"/>
       <c r="D48" s="15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E48" s="19"/>
       <c r="F48" s="21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G48" s="22"/>
       <c r="H48" s="12"/>
       <c r="I48" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J48" s="12"/>
       <c r="K48" s="12"/>
@@ -2096,16 +2103,16 @@
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" s="18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C49" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D49" s="15" t="s">
         <v>41</v>
-      </c>
-      <c r="D49" s="15" t="s">
-        <v>42</v>
       </c>
       <c r="E49" s="19"/>
       <c r="F49" s="21" t="s">
@@ -2120,20 +2127,20 @@
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" s="18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D50" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E50" s="19"/>
       <c r="F50" s="21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G50" s="22"/>
       <c r="H50" s="12"/>
@@ -2144,16 +2151,16 @@
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" s="18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D51" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E51" s="12"/>
       <c r="F51" s="21" t="s">
@@ -2168,20 +2175,20 @@
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52" s="18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D52" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E52" s="12"/>
       <c r="F52" s="21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G52" s="22"/>
       <c r="H52" s="12"/>
@@ -2192,16 +2199,16 @@
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53" s="18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D53" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E53" s="12"/>
       <c r="F53" s="21" t="s">
@@ -2216,20 +2223,20 @@
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" s="18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D54" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E54" s="12"/>
       <c r="F54" s="21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G54" s="22"/>
       <c r="H54" s="12"/>
@@ -2240,18 +2247,18 @@
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55" s="18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C55" s="8"/>
       <c r="D55" s="15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E55" s="12"/>
       <c r="F55" s="21" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G55" s="22"/>
       <c r="H55" s="12"/>
@@ -2262,16 +2269,16 @@
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56" s="18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D56" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E56" s="12"/>
       <c r="F56" s="21" t="s">
@@ -2286,20 +2293,20 @@
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57" s="18" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D57" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E57" s="12"/>
       <c r="F57" s="21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G57" s="22"/>
       <c r="H57" s="12"/>
@@ -2313,14 +2320,14 @@
         <v>44</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C58" s="8"/>
       <c r="D58" s="15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E58" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F58" s="21" t="s">
         <v>28</v>
@@ -2337,14 +2344,14 @@
         <v>45</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C59" s="8"/>
       <c r="D59" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E59" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F59" s="21" t="s">
         <v>28</v>
@@ -2361,14 +2368,14 @@
         <v>46</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C60" s="8"/>
       <c r="D60" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E60" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F60" s="21" t="s">
         <v>28</v>
@@ -2385,14 +2392,14 @@
         <v>47</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C61" s="8"/>
       <c r="D61" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E61" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F61" s="21" t="s">
         <v>28</v>
@@ -2409,14 +2416,14 @@
         <v>48</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C62" s="8"/>
       <c r="D62" s="15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E62" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F62" s="21" t="s">
         <v>28</v>
@@ -2433,14 +2440,14 @@
         <v>49</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C63" s="8"/>
       <c r="D63" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E63" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F63" s="21" t="s">
         <v>28</v>
@@ -2457,11 +2464,11 @@
         <v>50</v>
       </c>
       <c r="B64" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C64" s="8"/>
       <c r="D64" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E64" s="12"/>
       <c r="F64" s="21" t="s">
@@ -2479,11 +2486,11 @@
         <v>51</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C65" s="16"/>
       <c r="D65" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E65" s="12"/>
       <c r="F65" s="21" t="s">
@@ -2501,11 +2508,11 @@
         <v>52</v>
       </c>
       <c r="B66" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C66" s="16"/>
       <c r="D66" s="17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E66" s="12"/>
       <c r="F66" s="21" t="s">

</xml_diff>

<commit_message>
take care of one TODO
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/euTaxonomyNonFinancials/EutaxonomyNonFinancials.xlsx
+++ b/dataland-framework-toolbox/inputs/euTaxonomyNonFinancials/EutaxonomyNonFinancials.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d92928\Documents\Projects\Dataland\Dataland\dataland-framework-toolbox\inputs\euTaxonomyNonFinancials\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d92432\Documents\Projekte\02-Dataland\Dataland\dataland-framework-toolbox\inputs\euTaxonomyNonFinancials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BE35C43-0F19-409E-8183-DEC5B64EF4B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D5C2100-E386-44BC-ACBE-73E594D0D808}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Framework Data Model" sheetId="1" r:id="rId1"/>
@@ -320,9 +320,6 @@
     <t>Report Preupload</t>
   </si>
   <si>
-    <t>Custom AmountWithCurrency</t>
-  </si>
-  <si>
     <t>Custom List of EuTaxonomyActivity</t>
   </si>
   <si>
@@ -444,6 +441,9 @@
   </si>
   <si>
     <t>Relative share of the OpEx that is associated with taxonomy-aligned activities. i.e., for an eligible economic activity that is making a substantial contribution to at least one of the climate and environmental objectives, while also doing no significant harm to the remaining objectives and meeting minimum standards on human rights and labour standards</t>
+  </si>
+  <si>
+    <t>Custom EuTaxonomyAmountWithCurrencyComponent</t>
   </si>
 </sst>
 </file>
@@ -1064,21 +1064,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E65" sqref="E65"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="20.21875" customWidth="1"/>
-    <col min="4" max="4" width="70.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="77.88671875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="38.88671875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="26.21875" customWidth="1"/>
-    <col min="8" max="12" width="14.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.1796875" customWidth="1"/>
+    <col min="4" max="4" width="70.36328125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="77.90625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="44.6328125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="26.1796875" customWidth="1"/>
+    <col min="8" max="12" width="14.36328125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1116,7 +1116,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="7">
         <v>0</v>
       </c>
@@ -1142,7 +1142,7 @@
       <c r="K2" s="12"/>
       <c r="L2" s="12"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="7"/>
       <c r="B3" s="8" t="s">
         <v>12</v>
@@ -1164,7 +1164,7 @@
       <c r="K3" s="12"/>
       <c r="L3" s="12"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="7">
         <v>1</v>
       </c>
@@ -1190,7 +1190,7 @@
       <c r="K4" s="11"/>
       <c r="L4" s="12"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="7">
         <v>2</v>
       </c>
@@ -1216,7 +1216,7 @@
       <c r="K5" s="12"/>
       <c r="L5" s="12"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="7">
         <v>3</v>
       </c>
@@ -1242,7 +1242,7 @@
       <c r="K6" s="12"/>
       <c r="L6" s="12"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="7">
         <v>4</v>
       </c>
@@ -1257,7 +1257,7 @@
         <v>32</v>
       </c>
       <c r="F7" s="27" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G7" s="26" t="s">
         <v>14</v>
@@ -1268,7 +1268,7 @@
       <c r="K7" s="12"/>
       <c r="L7" s="12"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="7">
         <v>5</v>
       </c>
@@ -1292,7 +1292,7 @@
       <c r="K8" s="12"/>
       <c r="L8" s="12"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" s="7">
         <v>6</v>
       </c>
@@ -1316,7 +1316,7 @@
       <c r="K9" s="12"/>
       <c r="L9" s="12"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" s="7">
         <v>8</v>
       </c>
@@ -1328,7 +1328,7 @@
         <v>39</v>
       </c>
       <c r="E10" s="19" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F10" s="21" t="s">
         <v>38</v>
@@ -1342,7 +1342,7 @@
       <c r="K10" s="12"/>
       <c r="L10" s="12"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" s="18" t="s">
         <v>43</v>
       </c>
@@ -1366,7 +1366,7 @@
       <c r="K11" s="12"/>
       <c r="L11" s="12"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" s="18" t="s">
         <v>44</v>
       </c>
@@ -1380,10 +1380,10 @@
         <v>42</v>
       </c>
       <c r="E12" s="28" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F12" s="21" t="s">
-        <v>87</v>
+        <v>128</v>
       </c>
       <c r="G12" s="22"/>
       <c r="H12" s="12"/>
@@ -1392,7 +1392,7 @@
       <c r="K12" s="12"/>
       <c r="L12" s="12"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" s="18" t="s">
         <v>46</v>
       </c>
@@ -1406,7 +1406,7 @@
         <v>41</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F13" s="21" t="s">
         <v>28</v>
@@ -1418,7 +1418,7 @@
       <c r="K13" s="12"/>
       <c r="L13" s="12"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" s="18" t="s">
         <v>47</v>
       </c>
@@ -1432,10 +1432,10 @@
         <v>42</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F14" s="21" t="s">
-        <v>87</v>
+        <v>128</v>
       </c>
       <c r="G14" s="22"/>
       <c r="H14" s="12"/>
@@ -1444,7 +1444,7 @@
       <c r="K14" s="12"/>
       <c r="L14" s="12"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" s="18" t="s">
         <v>49</v>
       </c>
@@ -1458,7 +1458,7 @@
         <v>41</v>
       </c>
       <c r="E15" s="28" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F15" s="21" t="s">
         <v>28</v>
@@ -1470,7 +1470,7 @@
       <c r="K15" s="12"/>
       <c r="L15" s="12"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" s="18" t="s">
         <v>50</v>
       </c>
@@ -1484,10 +1484,10 @@
         <v>42</v>
       </c>
       <c r="E16" s="28" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F16" s="21" t="s">
-        <v>87</v>
+        <v>128</v>
       </c>
       <c r="G16" s="22"/>
       <c r="H16" s="12"/>
@@ -1496,7 +1496,7 @@
       <c r="K16" s="12"/>
       <c r="L16" s="12"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" s="18" t="s">
         <v>62</v>
       </c>
@@ -1508,10 +1508,10 @@
         <v>51</v>
       </c>
       <c r="E17" s="28" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F17" s="21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G17" s="22"/>
       <c r="H17" s="12"/>
@@ -1520,7 +1520,7 @@
       <c r="K17" s="12"/>
       <c r="L17" s="12"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18" s="18" t="s">
         <v>63</v>
       </c>
@@ -1534,7 +1534,7 @@
         <v>41</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F18" s="21" t="s">
         <v>28</v>
@@ -1546,7 +1546,7 @@
       <c r="K18" s="12"/>
       <c r="L18" s="12"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19" s="18" t="s">
         <v>64</v>
       </c>
@@ -1560,10 +1560,10 @@
         <v>42</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F19" s="21" t="s">
-        <v>87</v>
+        <v>128</v>
       </c>
       <c r="G19" s="22"/>
       <c r="H19" s="12"/>
@@ -1572,7 +1572,7 @@
       <c r="K19" s="12"/>
       <c r="L19" s="12"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20" s="7">
         <v>14</v>
       </c>
@@ -1596,7 +1596,7 @@
       <c r="K20" s="12"/>
       <c r="L20" s="12"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A21" s="7">
         <v>15</v>
       </c>
@@ -1620,7 +1620,7 @@
       <c r="K21" s="12"/>
       <c r="L21" s="12"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A22" s="7">
         <v>16</v>
       </c>
@@ -1644,7 +1644,7 @@
       <c r="K22" s="12"/>
       <c r="L22" s="12"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A23" s="7">
         <v>17</v>
       </c>
@@ -1668,7 +1668,7 @@
       <c r="K23" s="12"/>
       <c r="L23" s="12"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A24" s="7">
         <v>18</v>
       </c>
@@ -1692,7 +1692,7 @@
       <c r="K24" s="12"/>
       <c r="L24" s="12"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A25" s="7">
         <v>19</v>
       </c>
@@ -1716,7 +1716,7 @@
       <c r="K25" s="12"/>
       <c r="L25" s="12"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A26" s="7">
         <v>20</v>
       </c>
@@ -1728,10 +1728,10 @@
         <v>59</v>
       </c>
       <c r="E26" s="28" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F26" s="21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G26" s="22"/>
       <c r="H26" s="12"/>
@@ -1740,7 +1740,7 @@
       <c r="K26" s="12"/>
       <c r="L26" s="12"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A27" s="7">
         <v>21</v>
       </c>
@@ -1752,7 +1752,7 @@
         <v>60</v>
       </c>
       <c r="E27" s="28" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F27" s="21" t="s">
         <v>28</v>
@@ -1764,7 +1764,7 @@
       <c r="K27" s="12"/>
       <c r="L27" s="12"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A28" s="7">
         <v>22</v>
       </c>
@@ -1776,7 +1776,7 @@
         <v>61</v>
       </c>
       <c r="E28" s="28" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F28" s="21" t="s">
         <v>28</v>
@@ -1788,7 +1788,7 @@
       <c r="K28" s="12"/>
       <c r="L28" s="12"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A29" s="7">
         <v>23</v>
       </c>
@@ -1800,7 +1800,7 @@
         <v>39</v>
       </c>
       <c r="E29" s="28" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F29" s="21" t="s">
         <v>38</v>
@@ -1814,7 +1814,7 @@
       <c r="K29" s="12"/>
       <c r="L29" s="12"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A30" s="18" t="s">
         <v>67</v>
       </c>
@@ -1828,7 +1828,7 @@
         <v>41</v>
       </c>
       <c r="E30" s="29" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F30" s="21" t="s">
         <v>28</v>
@@ -1840,7 +1840,7 @@
       <c r="K30" s="12"/>
       <c r="L30" s="12"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A31" s="18" t="s">
         <v>68</v>
       </c>
@@ -1854,10 +1854,10 @@
         <v>42</v>
       </c>
       <c r="E31" s="29" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F31" s="21" t="s">
-        <v>87</v>
+        <v>128</v>
       </c>
       <c r="G31" s="22"/>
       <c r="H31" s="12"/>
@@ -1866,7 +1866,7 @@
       <c r="K31" s="12"/>
       <c r="L31" s="12"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A32" s="18" t="s">
         <v>65</v>
       </c>
@@ -1880,7 +1880,7 @@
         <v>41</v>
       </c>
       <c r="E32" s="28" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F32" s="21" t="s">
         <v>28</v>
@@ -1892,7 +1892,7 @@
       <c r="K32" s="12"/>
       <c r="L32" s="12"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A33" s="18" t="s">
         <v>66</v>
       </c>
@@ -1906,10 +1906,10 @@
         <v>42</v>
       </c>
       <c r="E33" s="28" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F33" s="21" t="s">
-        <v>87</v>
+        <v>128</v>
       </c>
       <c r="G33" s="22"/>
       <c r="H33" s="12"/>
@@ -1918,7 +1918,7 @@
       <c r="K33" s="12"/>
       <c r="L33" s="12"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A34" s="18" t="s">
         <v>69</v>
       </c>
@@ -1932,7 +1932,7 @@
         <v>41</v>
       </c>
       <c r="E34" s="29" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F34" s="21" t="s">
         <v>28</v>
@@ -1944,7 +1944,7 @@
       <c r="K34" s="12"/>
       <c r="L34" s="12"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A35" s="18" t="s">
         <v>70</v>
       </c>
@@ -1958,10 +1958,10 @@
         <v>42</v>
       </c>
       <c r="E35" s="29" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F35" s="21" t="s">
-        <v>87</v>
+        <v>128</v>
       </c>
       <c r="G35" s="22"/>
       <c r="H35" s="12"/>
@@ -1970,7 +1970,7 @@
       <c r="K35" s="12"/>
       <c r="L35" s="12"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A36" s="18" t="s">
         <v>71</v>
       </c>
@@ -1982,10 +1982,10 @@
         <v>51</v>
       </c>
       <c r="E36" s="29" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F36" s="21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G36" s="22"/>
       <c r="H36" s="12"/>
@@ -1994,7 +1994,7 @@
       <c r="K36" s="12"/>
       <c r="L36" s="12"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A37" s="18" t="s">
         <v>72</v>
       </c>
@@ -2008,7 +2008,7 @@
         <v>41</v>
       </c>
       <c r="E37" s="29" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F37" s="21" t="s">
         <v>28</v>
@@ -2020,7 +2020,7 @@
       <c r="K37" s="12"/>
       <c r="L37" s="12"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A38" s="18" t="s">
         <v>73</v>
       </c>
@@ -2034,10 +2034,10 @@
         <v>42</v>
       </c>
       <c r="E38" s="29" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F38" s="21" t="s">
-        <v>87</v>
+        <v>128</v>
       </c>
       <c r="G38" s="22"/>
       <c r="H38" s="12"/>
@@ -2046,7 +2046,7 @@
       <c r="K38" s="12"/>
       <c r="L38" s="12"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A39" s="7">
         <v>29</v>
       </c>
@@ -2070,7 +2070,7 @@
       <c r="K39" s="12"/>
       <c r="L39" s="12"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A40" s="7">
         <v>30</v>
       </c>
@@ -2094,7 +2094,7 @@
       <c r="K40" s="12"/>
       <c r="L40" s="12"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A41" s="7">
         <v>31</v>
       </c>
@@ -2118,7 +2118,7 @@
       <c r="K41" s="12"/>
       <c r="L41" s="12"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A42" s="7">
         <v>32</v>
       </c>
@@ -2142,7 +2142,7 @@
       <c r="K42" s="12"/>
       <c r="L42" s="12"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A43" s="7">
         <v>33</v>
       </c>
@@ -2166,7 +2166,7 @@
       <c r="K43" s="12"/>
       <c r="L43" s="12"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A44" s="7">
         <v>34</v>
       </c>
@@ -2190,7 +2190,7 @@
       <c r="K44" s="12"/>
       <c r="L44" s="12"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A45" s="7">
         <v>35</v>
       </c>
@@ -2202,10 +2202,10 @@
         <v>59</v>
       </c>
       <c r="E45" s="29" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F45" s="21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G45" s="22"/>
       <c r="H45" s="12"/>
@@ -2214,7 +2214,7 @@
       <c r="K45" s="12"/>
       <c r="L45" s="12"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A46" s="7">
         <v>36</v>
       </c>
@@ -2226,7 +2226,7 @@
         <v>60</v>
       </c>
       <c r="E46" s="28" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F46" s="21" t="s">
         <v>28</v>
@@ -2238,7 +2238,7 @@
       <c r="K46" s="12"/>
       <c r="L46" s="12"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A47" s="7">
         <v>37</v>
       </c>
@@ -2250,7 +2250,7 @@
         <v>61</v>
       </c>
       <c r="E47" s="28" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F47" s="21" t="s">
         <v>28</v>
@@ -2262,7 +2262,7 @@
       <c r="K47" s="12"/>
       <c r="L47" s="12"/>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A48" s="7">
         <v>38</v>
       </c>
@@ -2274,7 +2274,7 @@
         <v>39</v>
       </c>
       <c r="E48" s="28" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F48" s="21" t="s">
         <v>38</v>
@@ -2288,7 +2288,7 @@
       <c r="K48" s="12"/>
       <c r="L48" s="12"/>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A49" s="18" t="s">
         <v>74</v>
       </c>
@@ -2302,7 +2302,7 @@
         <v>41</v>
       </c>
       <c r="E49" s="28" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F49" s="21" t="s">
         <v>28</v>
@@ -2314,7 +2314,7 @@
       <c r="K49" s="12"/>
       <c r="L49" s="12"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A50" s="18" t="s">
         <v>75</v>
       </c>
@@ -2328,10 +2328,10 @@
         <v>42</v>
       </c>
       <c r="E50" s="28" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F50" s="21" t="s">
-        <v>87</v>
+        <v>128</v>
       </c>
       <c r="G50" s="22"/>
       <c r="H50" s="12"/>
@@ -2340,7 +2340,7 @@
       <c r="K50" s="12"/>
       <c r="L50" s="12"/>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A51" s="18" t="s">
         <v>76</v>
       </c>
@@ -2354,7 +2354,7 @@
         <v>41</v>
       </c>
       <c r="E51" s="28" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F51" s="21" t="s">
         <v>28</v>
@@ -2366,7 +2366,7 @@
       <c r="K51" s="12"/>
       <c r="L51" s="12"/>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A52" s="18" t="s">
         <v>77</v>
       </c>
@@ -2380,10 +2380,10 @@
         <v>42</v>
       </c>
       <c r="E52" s="28" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F52" s="21" t="s">
-        <v>87</v>
+        <v>128</v>
       </c>
       <c r="G52" s="22"/>
       <c r="H52" s="12"/>
@@ -2392,7 +2392,7 @@
       <c r="K52" s="12"/>
       <c r="L52" s="12"/>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A53" s="18" t="s">
         <v>78</v>
       </c>
@@ -2406,7 +2406,7 @@
         <v>41</v>
       </c>
       <c r="E53" s="28" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F53" s="21" t="s">
         <v>28</v>
@@ -2418,7 +2418,7 @@
       <c r="K53" s="12"/>
       <c r="L53" s="12"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A54" s="18" t="s">
         <v>79</v>
       </c>
@@ -2432,10 +2432,10 @@
         <v>42</v>
       </c>
       <c r="E54" s="28" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F54" s="21" t="s">
-        <v>87</v>
+        <v>128</v>
       </c>
       <c r="G54" s="22"/>
       <c r="H54" s="12"/>
@@ -2444,7 +2444,7 @@
       <c r="K54" s="12"/>
       <c r="L54" s="12"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A55" s="18" t="s">
         <v>80</v>
       </c>
@@ -2456,10 +2456,10 @@
         <v>51</v>
       </c>
       <c r="E55" s="28" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F55" s="21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G55" s="22"/>
       <c r="H55" s="12"/>
@@ -2468,7 +2468,7 @@
       <c r="K55" s="12"/>
       <c r="L55" s="12"/>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A56" s="18" t="s">
         <v>81</v>
       </c>
@@ -2482,7 +2482,7 @@
         <v>41</v>
       </c>
       <c r="E56" s="28" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F56" s="21" t="s">
         <v>28</v>
@@ -2494,7 +2494,7 @@
       <c r="K56" s="12"/>
       <c r="L56" s="12"/>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A57" s="18" t="s">
         <v>82</v>
       </c>
@@ -2508,10 +2508,10 @@
         <v>42</v>
       </c>
       <c r="E57" s="28" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F57" s="21" t="s">
-        <v>87</v>
+        <v>128</v>
       </c>
       <c r="G57" s="22"/>
       <c r="H57" s="12"/>
@@ -2520,7 +2520,7 @@
       <c r="K57" s="12"/>
       <c r="L57" s="12"/>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A58" s="7">
         <v>44</v>
       </c>
@@ -2544,7 +2544,7 @@
       <c r="K58" s="19"/>
       <c r="L58" s="19"/>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A59" s="7">
         <v>45</v>
       </c>
@@ -2568,7 +2568,7 @@
       <c r="K59" s="19"/>
       <c r="L59" s="19"/>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A60" s="7">
         <v>46</v>
       </c>
@@ -2592,7 +2592,7 @@
       <c r="K60" s="19"/>
       <c r="L60" s="19"/>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A61" s="7">
         <v>47</v>
       </c>
@@ -2616,7 +2616,7 @@
       <c r="K61" s="19"/>
       <c r="L61" s="19"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A62" s="7">
         <v>48</v>
       </c>
@@ -2640,7 +2640,7 @@
       <c r="K62" s="19"/>
       <c r="L62" s="19"/>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A63" s="7">
         <v>49</v>
       </c>
@@ -2664,7 +2664,7 @@
       <c r="K63" s="19"/>
       <c r="L63" s="19"/>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A64" s="7">
         <v>50</v>
       </c>
@@ -2676,10 +2676,10 @@
         <v>59</v>
       </c>
       <c r="E64" s="28" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F64" s="21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G64" s="22"/>
       <c r="H64" s="19"/>
@@ -2688,7 +2688,7 @@
       <c r="K64" s="19"/>
       <c r="L64" s="19"/>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A65" s="7">
         <v>51</v>
       </c>
@@ -2700,7 +2700,7 @@
         <v>60</v>
       </c>
       <c r="E65" s="28" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F65" s="21" t="s">
         <v>28</v>
@@ -2712,7 +2712,7 @@
       <c r="K65" s="19"/>
       <c r="L65" s="19"/>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A66" s="7">
         <v>52</v>
       </c>
@@ -2724,7 +2724,7 @@
         <v>61</v>
       </c>
       <c r="E66" s="28" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F66" s="21" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
some refactoring related to TODO
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/euTaxonomyNonFinancials/EutaxonomyNonFinancials.xlsx
+++ b/dataland-framework-toolbox/inputs/euTaxonomyNonFinancials/EutaxonomyNonFinancials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d92432\Documents\Projekte\02-Dataland\Dataland\dataland-framework-toolbox\inputs\euTaxonomyNonFinancials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D5C2100-E386-44BC-ACBE-73E594D0D808}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF86820C-6993-48EB-BEFD-3A27DED127E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -320,12 +320,6 @@
     <t>Report Preupload</t>
   </si>
   <si>
-    <t>Custom List of EuTaxonomyActivity</t>
-  </si>
-  <si>
-    <t>Custom AlignedActivitiesFormField</t>
-  </si>
-  <si>
     <t>Custom EuTaxonomyAssuranceComponent</t>
   </si>
   <si>
@@ -444,6 +438,12 @@
   </si>
   <si>
     <t>Custom EuTaxonomyAmountWithCurrencyComponent</t>
+  </si>
+  <si>
+    <t>Custom EuTaxonomyNonAlignedActivitiesComponent</t>
+  </si>
+  <si>
+    <t>Custom EuTaxonomyAlignedActivitiesComponent</t>
   </si>
 </sst>
 </file>
@@ -1064,8 +1064,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="D50" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E71" sqref="E71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1257,7 +1257,7 @@
         <v>32</v>
       </c>
       <c r="F7" s="27" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G7" s="26" t="s">
         <v>14</v>
@@ -1328,7 +1328,7 @@
         <v>39</v>
       </c>
       <c r="E10" s="19" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F10" s="21" t="s">
         <v>38</v>
@@ -1380,10 +1380,10 @@
         <v>42</v>
       </c>
       <c r="E12" s="28" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F12" s="21" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G12" s="22"/>
       <c r="H12" s="12"/>
@@ -1406,7 +1406,7 @@
         <v>41</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F13" s="21" t="s">
         <v>28</v>
@@ -1432,10 +1432,10 @@
         <v>42</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F14" s="21" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G14" s="22"/>
       <c r="H14" s="12"/>
@@ -1458,7 +1458,7 @@
         <v>41</v>
       </c>
       <c r="E15" s="28" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F15" s="21" t="s">
         <v>28</v>
@@ -1484,10 +1484,10 @@
         <v>42</v>
       </c>
       <c r="E16" s="28" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F16" s="21" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G16" s="22"/>
       <c r="H16" s="12"/>
@@ -1508,10 +1508,10 @@
         <v>51</v>
       </c>
       <c r="E17" s="28" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F17" s="21" t="s">
-        <v>87</v>
+        <v>127</v>
       </c>
       <c r="G17" s="22"/>
       <c r="H17" s="12"/>
@@ -1534,7 +1534,7 @@
         <v>41</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F18" s="21" t="s">
         <v>28</v>
@@ -1560,10 +1560,10 @@
         <v>42</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F19" s="21" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G19" s="22"/>
       <c r="H19" s="12"/>
@@ -1728,10 +1728,10 @@
         <v>59</v>
       </c>
       <c r="E26" s="28" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F26" s="21" t="s">
-        <v>88</v>
+        <v>128</v>
       </c>
       <c r="G26" s="22"/>
       <c r="H26" s="12"/>
@@ -1752,7 +1752,7 @@
         <v>60</v>
       </c>
       <c r="E27" s="28" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F27" s="21" t="s">
         <v>28</v>
@@ -1776,7 +1776,7 @@
         <v>61</v>
       </c>
       <c r="E28" s="28" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F28" s="21" t="s">
         <v>28</v>
@@ -1800,7 +1800,7 @@
         <v>39</v>
       </c>
       <c r="E29" s="28" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F29" s="21" t="s">
         <v>38</v>
@@ -1828,7 +1828,7 @@
         <v>41</v>
       </c>
       <c r="E30" s="29" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F30" s="21" t="s">
         <v>28</v>
@@ -1854,10 +1854,10 @@
         <v>42</v>
       </c>
       <c r="E31" s="29" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F31" s="21" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G31" s="22"/>
       <c r="H31" s="12"/>
@@ -1880,7 +1880,7 @@
         <v>41</v>
       </c>
       <c r="E32" s="28" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F32" s="21" t="s">
         <v>28</v>
@@ -1906,10 +1906,10 @@
         <v>42</v>
       </c>
       <c r="E33" s="28" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F33" s="21" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G33" s="22"/>
       <c r="H33" s="12"/>
@@ -1932,7 +1932,7 @@
         <v>41</v>
       </c>
       <c r="E34" s="29" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F34" s="21" t="s">
         <v>28</v>
@@ -1958,10 +1958,10 @@
         <v>42</v>
       </c>
       <c r="E35" s="29" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F35" s="21" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G35" s="22"/>
       <c r="H35" s="12"/>
@@ -1982,10 +1982,10 @@
         <v>51</v>
       </c>
       <c r="E36" s="29" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F36" s="21" t="s">
-        <v>87</v>
+        <v>127</v>
       </c>
       <c r="G36" s="22"/>
       <c r="H36" s="12"/>
@@ -2008,7 +2008,7 @@
         <v>41</v>
       </c>
       <c r="E37" s="29" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F37" s="21" t="s">
         <v>28</v>
@@ -2034,10 +2034,10 @@
         <v>42</v>
       </c>
       <c r="E38" s="29" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F38" s="21" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G38" s="22"/>
       <c r="H38" s="12"/>
@@ -2202,10 +2202,10 @@
         <v>59</v>
       </c>
       <c r="E45" s="29" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F45" s="21" t="s">
-        <v>88</v>
+        <v>128</v>
       </c>
       <c r="G45" s="22"/>
       <c r="H45" s="12"/>
@@ -2226,7 +2226,7 @@
         <v>60</v>
       </c>
       <c r="E46" s="28" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F46" s="21" t="s">
         <v>28</v>
@@ -2250,7 +2250,7 @@
         <v>61</v>
       </c>
       <c r="E47" s="28" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F47" s="21" t="s">
         <v>28</v>
@@ -2274,7 +2274,7 @@
         <v>39</v>
       </c>
       <c r="E48" s="28" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F48" s="21" t="s">
         <v>38</v>
@@ -2302,7 +2302,7 @@
         <v>41</v>
       </c>
       <c r="E49" s="28" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F49" s="21" t="s">
         <v>28</v>
@@ -2328,10 +2328,10 @@
         <v>42</v>
       </c>
       <c r="E50" s="28" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F50" s="21" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G50" s="22"/>
       <c r="H50" s="12"/>
@@ -2354,7 +2354,7 @@
         <v>41</v>
       </c>
       <c r="E51" s="28" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F51" s="21" t="s">
         <v>28</v>
@@ -2380,10 +2380,10 @@
         <v>42</v>
       </c>
       <c r="E52" s="28" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F52" s="21" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G52" s="22"/>
       <c r="H52" s="12"/>
@@ -2406,7 +2406,7 @@
         <v>41</v>
       </c>
       <c r="E53" s="28" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F53" s="21" t="s">
         <v>28</v>
@@ -2432,10 +2432,10 @@
         <v>42</v>
       </c>
       <c r="E54" s="28" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F54" s="21" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G54" s="22"/>
       <c r="H54" s="12"/>
@@ -2456,10 +2456,10 @@
         <v>51</v>
       </c>
       <c r="E55" s="28" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F55" s="21" t="s">
-        <v>87</v>
+        <v>127</v>
       </c>
       <c r="G55" s="22"/>
       <c r="H55" s="12"/>
@@ -2482,7 +2482,7 @@
         <v>41</v>
       </c>
       <c r="E56" s="28" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F56" s="21" t="s">
         <v>28</v>
@@ -2508,10 +2508,10 @@
         <v>42</v>
       </c>
       <c r="E57" s="28" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F57" s="21" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G57" s="22"/>
       <c r="H57" s="12"/>
@@ -2676,10 +2676,10 @@
         <v>59</v>
       </c>
       <c r="E64" s="28" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F64" s="21" t="s">
-        <v>88</v>
+        <v>128</v>
       </c>
       <c r="G64" s="22"/>
       <c r="H64" s="19"/>
@@ -2700,7 +2700,7 @@
         <v>60</v>
       </c>
       <c r="E65" s="28" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F65" s="21" t="s">
         <v>28</v>
@@ -2724,7 +2724,7 @@
         <v>61</v>
       </c>
       <c r="E66" s="28" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F66" s="21" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
refactors ValueWithCurrency and AmountWithCurrency in lksg and EutaxonomyNonFinancials and repairs swaggerUi example
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/euTaxonomyNonFinancials/EutaxonomyNonFinancials.xlsx
+++ b/dataland-framework-toolbox/inputs/euTaxonomyNonFinancials/EutaxonomyNonFinancials.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d92432\Documents\Projekte\02-Dataland\Dataland\dataland-framework-toolbox\inputs\euTaxonomyNonFinancials\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d92048\IdeaProjects\Dataland5\dataland-framework-toolbox\inputs\euTaxonomyNonFinancials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF86820C-6993-48EB-BEFD-3A27DED127E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9190097E-1C69-4385-816A-3AC5DD386F05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -437,13 +437,13 @@
     <t>Relative share of the OpEx that is associated with taxonomy-aligned activities. i.e., for an eligible economic activity that is making a substantial contribution to at least one of the climate and environmental objectives, while also doing no significant harm to the remaining objectives and meeting minimum standards on human rights and labour standards</t>
   </si>
   <si>
-    <t>Custom EuTaxonomyAmountWithCurrencyComponent</t>
-  </si>
-  <si>
     <t>Custom EuTaxonomyNonAlignedActivitiesComponent</t>
   </si>
   <si>
     <t>Custom EuTaxonomyAlignedActivitiesComponent</t>
+  </si>
+  <si>
+    <t>AmountWithCurrencyComponent</t>
   </si>
 </sst>
 </file>
@@ -1064,8 +1064,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D50" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E71" sqref="E71"/>
+    <sheetView tabSelected="1" topLeftCell="D46" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F57" sqref="F57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1383,7 +1383,7 @@
         <v>91</v>
       </c>
       <c r="F12" s="21" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="G12" s="22"/>
       <c r="H12" s="12"/>
@@ -1435,7 +1435,7 @@
         <v>114</v>
       </c>
       <c r="F14" s="21" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="G14" s="22"/>
       <c r="H14" s="12"/>
@@ -1487,7 +1487,7 @@
         <v>113</v>
       </c>
       <c r="F16" s="21" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="G16" s="22"/>
       <c r="H16" s="12"/>
@@ -1511,7 +1511,7 @@
         <v>90</v>
       </c>
       <c r="F17" s="21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G17" s="22"/>
       <c r="H17" s="12"/>
@@ -1563,7 +1563,7 @@
         <v>112</v>
       </c>
       <c r="F19" s="21" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="G19" s="22"/>
       <c r="H19" s="12"/>
@@ -1731,7 +1731,7 @@
         <v>89</v>
       </c>
       <c r="F26" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G26" s="22"/>
       <c r="H26" s="12"/>
@@ -1857,7 +1857,7 @@
         <v>107</v>
       </c>
       <c r="F31" s="21" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="G31" s="22"/>
       <c r="H31" s="12"/>
@@ -1909,7 +1909,7 @@
         <v>102</v>
       </c>
       <c r="F33" s="21" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="G33" s="22"/>
       <c r="H33" s="12"/>
@@ -1961,7 +1961,7 @@
         <v>106</v>
       </c>
       <c r="F35" s="21" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="G35" s="22"/>
       <c r="H35" s="12"/>
@@ -1985,7 +1985,7 @@
         <v>105</v>
       </c>
       <c r="F36" s="21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G36" s="22"/>
       <c r="H36" s="12"/>
@@ -2037,7 +2037,7 @@
         <v>103</v>
       </c>
       <c r="F38" s="21" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="G38" s="22"/>
       <c r="H38" s="12"/>
@@ -2205,7 +2205,7 @@
         <v>104</v>
       </c>
       <c r="F45" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G45" s="22"/>
       <c r="H45" s="12"/>
@@ -2331,7 +2331,7 @@
         <v>108</v>
       </c>
       <c r="F50" s="21" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="G50" s="22"/>
       <c r="H50" s="12"/>
@@ -2383,7 +2383,7 @@
         <v>109</v>
       </c>
       <c r="F52" s="21" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="G52" s="22"/>
       <c r="H52" s="12"/>
@@ -2435,7 +2435,7 @@
         <v>110</v>
       </c>
       <c r="F54" s="21" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="G54" s="22"/>
       <c r="H54" s="12"/>
@@ -2459,7 +2459,7 @@
         <v>99</v>
       </c>
       <c r="F55" s="21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G55" s="22"/>
       <c r="H55" s="12"/>
@@ -2511,7 +2511,7 @@
         <v>111</v>
       </c>
       <c r="F57" s="21" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="G57" s="22"/>
       <c r="H57" s="12"/>
@@ -2679,7 +2679,7 @@
         <v>98</v>
       </c>
       <c r="F64" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G64" s="22"/>
       <c r="H64" s="19"/>

</xml_diff>

<commit_message>
Dala 3260 update lksg (#445)
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/euTaxonomyNonFinancials/EutaxonomyNonFinancials.xlsx
+++ b/dataland-framework-toolbox/inputs/euTaxonomyNonFinancials/EutaxonomyNonFinancials.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d92432\Documents\Projekte\02-Dataland\Dataland\dataland-framework-toolbox\inputs\euTaxonomyNonFinancials\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d92048\IdeaProjects\Dataland5\dataland-framework-toolbox\inputs\euTaxonomyNonFinancials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF86820C-6993-48EB-BEFD-3A27DED127E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9190097E-1C69-4385-816A-3AC5DD386F05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -437,13 +437,13 @@
     <t>Relative share of the OpEx that is associated with taxonomy-aligned activities. i.e., for an eligible economic activity that is making a substantial contribution to at least one of the climate and environmental objectives, while also doing no significant harm to the remaining objectives and meeting minimum standards on human rights and labour standards</t>
   </si>
   <si>
-    <t>Custom EuTaxonomyAmountWithCurrencyComponent</t>
-  </si>
-  <si>
     <t>Custom EuTaxonomyNonAlignedActivitiesComponent</t>
   </si>
   <si>
     <t>Custom EuTaxonomyAlignedActivitiesComponent</t>
+  </si>
+  <si>
+    <t>AmountWithCurrencyComponent</t>
   </si>
 </sst>
 </file>
@@ -1064,8 +1064,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D50" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E71" sqref="E71"/>
+    <sheetView tabSelected="1" topLeftCell="D46" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F57" sqref="F57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1383,7 +1383,7 @@
         <v>91</v>
       </c>
       <c r="F12" s="21" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="G12" s="22"/>
       <c r="H12" s="12"/>
@@ -1435,7 +1435,7 @@
         <v>114</v>
       </c>
       <c r="F14" s="21" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="G14" s="22"/>
       <c r="H14" s="12"/>
@@ -1487,7 +1487,7 @@
         <v>113</v>
       </c>
       <c r="F16" s="21" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="G16" s="22"/>
       <c r="H16" s="12"/>
@@ -1511,7 +1511,7 @@
         <v>90</v>
       </c>
       <c r="F17" s="21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G17" s="22"/>
       <c r="H17" s="12"/>
@@ -1563,7 +1563,7 @@
         <v>112</v>
       </c>
       <c r="F19" s="21" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="G19" s="22"/>
       <c r="H19" s="12"/>
@@ -1731,7 +1731,7 @@
         <v>89</v>
       </c>
       <c r="F26" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G26" s="22"/>
       <c r="H26" s="12"/>
@@ -1857,7 +1857,7 @@
         <v>107</v>
       </c>
       <c r="F31" s="21" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="G31" s="22"/>
       <c r="H31" s="12"/>
@@ -1909,7 +1909,7 @@
         <v>102</v>
       </c>
       <c r="F33" s="21" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="G33" s="22"/>
       <c r="H33" s="12"/>
@@ -1961,7 +1961,7 @@
         <v>106</v>
       </c>
       <c r="F35" s="21" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="G35" s="22"/>
       <c r="H35" s="12"/>
@@ -1985,7 +1985,7 @@
         <v>105</v>
       </c>
       <c r="F36" s="21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G36" s="22"/>
       <c r="H36" s="12"/>
@@ -2037,7 +2037,7 @@
         <v>103</v>
       </c>
       <c r="F38" s="21" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="G38" s="22"/>
       <c r="H38" s="12"/>
@@ -2205,7 +2205,7 @@
         <v>104</v>
       </c>
       <c r="F45" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G45" s="22"/>
       <c r="H45" s="12"/>
@@ -2331,7 +2331,7 @@
         <v>108</v>
       </c>
       <c r="F50" s="21" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="G50" s="22"/>
       <c r="H50" s="12"/>
@@ -2383,7 +2383,7 @@
         <v>109</v>
       </c>
       <c r="F52" s="21" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="G52" s="22"/>
       <c r="H52" s="12"/>
@@ -2435,7 +2435,7 @@
         <v>110</v>
       </c>
       <c r="F54" s="21" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="G54" s="22"/>
       <c r="H54" s="12"/>
@@ -2459,7 +2459,7 @@
         <v>99</v>
       </c>
       <c r="F55" s="21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G55" s="22"/>
       <c r="H55" s="12"/>
@@ -2511,7 +2511,7 @@
         <v>111</v>
       </c>
       <c r="F57" s="21" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="G57" s="22"/>
       <c r="H57" s="12"/>
@@ -2679,7 +2679,7 @@
         <v>98</v>
       </c>
       <c r="F64" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G64" s="22"/>
       <c r="H64" s="19"/>

</xml_diff>

<commit_message>
Set Percentage field to "Extended"
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/euTaxonomyNonFinancials/EutaxonomyNonFinancials.xlsx
+++ b/dataland-framework-toolbox/inputs/euTaxonomyNonFinancials/EutaxonomyNonFinancials.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d92048\IdeaProjects\Dataland5\dataland-framework-toolbox\inputs\euTaxonomyNonFinancials\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d93476\Dataland\dataland-framework-toolbox\inputs\euTaxonomyNonFinancials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9190097E-1C69-4385-816A-3AC5DD386F05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14D3C2D5-6DFE-455A-908F-947CE39F3735}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Framework Data Model" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Framework Data Model'!$A$1:$L$66</definedName>
     <definedName name="IQ_CH">110000</definedName>
     <definedName name="IQ_CQ">5000</definedName>
     <definedName name="IQ_CY">10000</definedName>
@@ -57,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="129">
   <si>
     <t>Field Identifier</t>
   </si>
@@ -750,7 +751,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -800,6 +801,7 @@
     <xf numFmtId="0" fontId="10" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1064,21 +1066,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D46" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F57" sqref="F57"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="20.1796875" customWidth="1"/>
-    <col min="4" max="4" width="70.36328125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="77.90625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="44.6328125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="26.1796875" customWidth="1"/>
-    <col min="8" max="12" width="14.36328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.21875" customWidth="1"/>
+    <col min="4" max="4" width="70.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="77.88671875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="44.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="26.21875" customWidth="1"/>
+    <col min="8" max="12" width="14.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1116,7 +1118,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="7">
         <v>0</v>
       </c>
@@ -1142,7 +1144,7 @@
       <c r="K2" s="12"/>
       <c r="L2" s="12"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="7"/>
       <c r="B3" s="8" t="s">
         <v>12</v>
@@ -1164,7 +1166,7 @@
       <c r="K3" s="12"/>
       <c r="L3" s="12"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>1</v>
       </c>
@@ -1190,7 +1192,7 @@
       <c r="K4" s="11"/>
       <c r="L4" s="12"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>2</v>
       </c>
@@ -1216,7 +1218,7 @@
       <c r="K5" s="12"/>
       <c r="L5" s="12"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>3</v>
       </c>
@@ -1242,7 +1244,7 @@
       <c r="K6" s="12"/>
       <c r="L6" s="12"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>4</v>
       </c>
@@ -1268,7 +1270,7 @@
       <c r="K7" s="12"/>
       <c r="L7" s="12"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>5</v>
       </c>
@@ -1292,7 +1294,7 @@
       <c r="K8" s="12"/>
       <c r="L8" s="12"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>6</v>
       </c>
@@ -1316,7 +1318,7 @@
       <c r="K9" s="12"/>
       <c r="L9" s="12"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>8</v>
       </c>
@@ -1342,7 +1344,7 @@
       <c r="K10" s="12"/>
       <c r="L10" s="12"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="18" t="s">
         <v>43</v>
       </c>
@@ -1361,12 +1363,14 @@
       </c>
       <c r="G11" s="22"/>
       <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
+      <c r="I11" s="31" t="s">
+        <v>35</v>
+      </c>
       <c r="J11" s="12"/>
       <c r="K11" s="12"/>
       <c r="L11" s="12"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="18" t="s">
         <v>44</v>
       </c>
@@ -1392,7 +1396,7 @@
       <c r="K12" s="12"/>
       <c r="L12" s="12"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="18" t="s">
         <v>46</v>
       </c>
@@ -1413,12 +1417,14 @@
       </c>
       <c r="G13" s="22"/>
       <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
+      <c r="I13" s="31" t="s">
+        <v>35</v>
+      </c>
       <c r="J13" s="12"/>
       <c r="K13" s="12"/>
       <c r="L13" s="12"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="18" t="s">
         <v>47</v>
       </c>
@@ -1444,7 +1450,7 @@
       <c r="K14" s="12"/>
       <c r="L14" s="12"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="18" t="s">
         <v>49</v>
       </c>
@@ -1465,12 +1471,14 @@
       </c>
       <c r="G15" s="22"/>
       <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
+      <c r="I15" s="31" t="s">
+        <v>35</v>
+      </c>
       <c r="J15" s="12"/>
       <c r="K15" s="12"/>
       <c r="L15" s="12"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="18" t="s">
         <v>50</v>
       </c>
@@ -1496,7 +1504,7 @@
       <c r="K16" s="12"/>
       <c r="L16" s="12"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="18" t="s">
         <v>62</v>
       </c>
@@ -1520,7 +1528,7 @@
       <c r="K17" s="12"/>
       <c r="L17" s="12"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="18" t="s">
         <v>63</v>
       </c>
@@ -1541,12 +1549,14 @@
       </c>
       <c r="G18" s="22"/>
       <c r="H18" s="12"/>
-      <c r="I18" s="12"/>
+      <c r="I18" s="31" t="s">
+        <v>35</v>
+      </c>
       <c r="J18" s="12"/>
       <c r="K18" s="12"/>
       <c r="L18" s="12"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="18" t="s">
         <v>64</v>
       </c>
@@ -1572,7 +1582,7 @@
       <c r="K19" s="12"/>
       <c r="L19" s="12"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="7">
         <v>14</v>
       </c>
@@ -1591,12 +1601,14 @@
       </c>
       <c r="G20" s="22"/>
       <c r="H20" s="12"/>
-      <c r="I20" s="12"/>
+      <c r="I20" s="31" t="s">
+        <v>35</v>
+      </c>
       <c r="J20" s="12"/>
       <c r="K20" s="12"/>
       <c r="L20" s="12"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="7">
         <v>15</v>
       </c>
@@ -1615,12 +1627,14 @@
       </c>
       <c r="G21" s="22"/>
       <c r="H21" s="12"/>
-      <c r="I21" s="12"/>
+      <c r="I21" s="31" t="s">
+        <v>35</v>
+      </c>
       <c r="J21" s="12"/>
       <c r="K21" s="12"/>
       <c r="L21" s="12"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="7">
         <v>16</v>
       </c>
@@ -1639,12 +1653,14 @@
       </c>
       <c r="G22" s="22"/>
       <c r="H22" s="12"/>
-      <c r="I22" s="12"/>
+      <c r="I22" s="31" t="s">
+        <v>35</v>
+      </c>
       <c r="J22" s="12"/>
       <c r="K22" s="12"/>
       <c r="L22" s="12"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="7">
         <v>17</v>
       </c>
@@ -1663,12 +1679,14 @@
       </c>
       <c r="G23" s="22"/>
       <c r="H23" s="12"/>
-      <c r="I23" s="12"/>
+      <c r="I23" s="31" t="s">
+        <v>35</v>
+      </c>
       <c r="J23" s="12"/>
       <c r="K23" s="12"/>
       <c r="L23" s="12"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="7">
         <v>18</v>
       </c>
@@ -1687,12 +1705,14 @@
       </c>
       <c r="G24" s="22"/>
       <c r="H24" s="12"/>
-      <c r="I24" s="12"/>
+      <c r="I24" s="31" t="s">
+        <v>35</v>
+      </c>
       <c r="J24" s="12"/>
       <c r="K24" s="12"/>
       <c r="L24" s="12"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="7">
         <v>19</v>
       </c>
@@ -1711,12 +1731,14 @@
       </c>
       <c r="G25" s="22"/>
       <c r="H25" s="12"/>
-      <c r="I25" s="12"/>
+      <c r="I25" s="31" t="s">
+        <v>35</v>
+      </c>
       <c r="J25" s="12"/>
       <c r="K25" s="12"/>
       <c r="L25" s="12"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="7">
         <v>20</v>
       </c>
@@ -1740,7 +1762,7 @@
       <c r="K26" s="12"/>
       <c r="L26" s="12"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="7">
         <v>21</v>
       </c>
@@ -1759,12 +1781,14 @@
       </c>
       <c r="G27" s="22"/>
       <c r="H27" s="12"/>
-      <c r="I27" s="12"/>
+      <c r="I27" s="31" t="s">
+        <v>35</v>
+      </c>
       <c r="J27" s="12"/>
       <c r="K27" s="12"/>
       <c r="L27" s="12"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="7">
         <v>22</v>
       </c>
@@ -1783,12 +1807,14 @@
       </c>
       <c r="G28" s="22"/>
       <c r="H28" s="12"/>
-      <c r="I28" s="12"/>
+      <c r="I28" s="31" t="s">
+        <v>35</v>
+      </c>
       <c r="J28" s="12"/>
       <c r="K28" s="12"/>
       <c r="L28" s="12"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="7">
         <v>23</v>
       </c>
@@ -1814,7 +1840,7 @@
       <c r="K29" s="12"/>
       <c r="L29" s="12"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="18" t="s">
         <v>67</v>
       </c>
@@ -1835,12 +1861,14 @@
       </c>
       <c r="G30" s="22"/>
       <c r="H30" s="12"/>
-      <c r="I30" s="12"/>
+      <c r="I30" s="31" t="s">
+        <v>35</v>
+      </c>
       <c r="J30" s="12"/>
       <c r="K30" s="12"/>
       <c r="L30" s="12"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="18" t="s">
         <v>68</v>
       </c>
@@ -1866,7 +1894,7 @@
       <c r="K31" s="12"/>
       <c r="L31" s="12"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="18" t="s">
         <v>65</v>
       </c>
@@ -1887,12 +1915,14 @@
       </c>
       <c r="G32" s="22"/>
       <c r="H32" s="12"/>
-      <c r="I32" s="12"/>
+      <c r="I32" s="31" t="s">
+        <v>35</v>
+      </c>
       <c r="J32" s="12"/>
       <c r="K32" s="12"/>
       <c r="L32" s="12"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" s="18" t="s">
         <v>66</v>
       </c>
@@ -1918,7 +1948,7 @@
       <c r="K33" s="12"/>
       <c r="L33" s="12"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" s="18" t="s">
         <v>69</v>
       </c>
@@ -1939,12 +1969,14 @@
       </c>
       <c r="G34" s="22"/>
       <c r="H34" s="12"/>
-      <c r="I34" s="12"/>
+      <c r="I34" s="31" t="s">
+        <v>35</v>
+      </c>
       <c r="J34" s="12"/>
       <c r="K34" s="12"/>
       <c r="L34" s="12"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" s="18" t="s">
         <v>70</v>
       </c>
@@ -1970,7 +2002,7 @@
       <c r="K35" s="12"/>
       <c r="L35" s="12"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" s="18" t="s">
         <v>71</v>
       </c>
@@ -1994,7 +2026,7 @@
       <c r="K36" s="12"/>
       <c r="L36" s="12"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" s="18" t="s">
         <v>72</v>
       </c>
@@ -2015,12 +2047,14 @@
       </c>
       <c r="G37" s="22"/>
       <c r="H37" s="12"/>
-      <c r="I37" s="12"/>
+      <c r="I37" s="31" t="s">
+        <v>35</v>
+      </c>
       <c r="J37" s="12"/>
       <c r="K37" s="12"/>
       <c r="L37" s="12"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" s="18" t="s">
         <v>73</v>
       </c>
@@ -2046,7 +2080,7 @@
       <c r="K38" s="12"/>
       <c r="L38" s="12"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" s="7">
         <v>29</v>
       </c>
@@ -2065,12 +2099,14 @@
       </c>
       <c r="G39" s="22"/>
       <c r="H39" s="12"/>
-      <c r="I39" s="12"/>
+      <c r="I39" s="31" t="s">
+        <v>35</v>
+      </c>
       <c r="J39" s="12"/>
       <c r="K39" s="12"/>
       <c r="L39" s="12"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" s="7">
         <v>30</v>
       </c>
@@ -2089,12 +2125,14 @@
       </c>
       <c r="G40" s="22"/>
       <c r="H40" s="12"/>
-      <c r="I40" s="12"/>
+      <c r="I40" s="31" t="s">
+        <v>35</v>
+      </c>
       <c r="J40" s="12"/>
       <c r="K40" s="12"/>
       <c r="L40" s="12"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" s="7">
         <v>31</v>
       </c>
@@ -2113,12 +2151,14 @@
       </c>
       <c r="G41" s="22"/>
       <c r="H41" s="12"/>
-      <c r="I41" s="12"/>
+      <c r="I41" s="31" t="s">
+        <v>35</v>
+      </c>
       <c r="J41" s="12"/>
       <c r="K41" s="12"/>
       <c r="L41" s="12"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" s="7">
         <v>32</v>
       </c>
@@ -2137,12 +2177,14 @@
       </c>
       <c r="G42" s="22"/>
       <c r="H42" s="12"/>
-      <c r="I42" s="12"/>
+      <c r="I42" s="31" t="s">
+        <v>35</v>
+      </c>
       <c r="J42" s="12"/>
       <c r="K42" s="12"/>
       <c r="L42" s="12"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" s="7">
         <v>33</v>
       </c>
@@ -2161,12 +2203,14 @@
       </c>
       <c r="G43" s="22"/>
       <c r="H43" s="12"/>
-      <c r="I43" s="12"/>
+      <c r="I43" s="31" t="s">
+        <v>35</v>
+      </c>
       <c r="J43" s="12"/>
       <c r="K43" s="12"/>
       <c r="L43" s="12"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" s="7">
         <v>34</v>
       </c>
@@ -2185,12 +2229,14 @@
       </c>
       <c r="G44" s="22"/>
       <c r="H44" s="12"/>
-      <c r="I44" s="12"/>
+      <c r="I44" s="31" t="s">
+        <v>35</v>
+      </c>
       <c r="J44" s="12"/>
       <c r="K44" s="12"/>
       <c r="L44" s="12"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" s="7">
         <v>35</v>
       </c>
@@ -2214,7 +2260,7 @@
       <c r="K45" s="12"/>
       <c r="L45" s="12"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" s="7">
         <v>36</v>
       </c>
@@ -2233,12 +2279,14 @@
       </c>
       <c r="G46" s="22"/>
       <c r="H46" s="12"/>
-      <c r="I46" s="12"/>
+      <c r="I46" s="31" t="s">
+        <v>35</v>
+      </c>
       <c r="J46" s="12"/>
       <c r="K46" s="12"/>
       <c r="L46" s="12"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" s="7">
         <v>37</v>
       </c>
@@ -2257,12 +2305,14 @@
       </c>
       <c r="G47" s="22"/>
       <c r="H47" s="12"/>
-      <c r="I47" s="12"/>
+      <c r="I47" s="31" t="s">
+        <v>35</v>
+      </c>
       <c r="J47" s="12"/>
       <c r="K47" s="12"/>
       <c r="L47" s="12"/>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48" s="7">
         <v>38</v>
       </c>
@@ -2288,7 +2338,7 @@
       <c r="K48" s="12"/>
       <c r="L48" s="12"/>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" s="18" t="s">
         <v>74</v>
       </c>
@@ -2309,12 +2359,14 @@
       </c>
       <c r="G49" s="22"/>
       <c r="H49" s="12"/>
-      <c r="I49" s="12"/>
+      <c r="I49" s="31" t="s">
+        <v>35</v>
+      </c>
       <c r="J49" s="12"/>
       <c r="K49" s="12"/>
       <c r="L49" s="12"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" s="18" t="s">
         <v>75</v>
       </c>
@@ -2340,7 +2392,7 @@
       <c r="K50" s="12"/>
       <c r="L50" s="12"/>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" s="18" t="s">
         <v>76</v>
       </c>
@@ -2361,12 +2413,14 @@
       </c>
       <c r="G51" s="22"/>
       <c r="H51" s="12"/>
-      <c r="I51" s="12"/>
+      <c r="I51" s="31" t="s">
+        <v>35</v>
+      </c>
       <c r="J51" s="12"/>
       <c r="K51" s="12"/>
       <c r="L51" s="12"/>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52" s="18" t="s">
         <v>77</v>
       </c>
@@ -2392,7 +2446,7 @@
       <c r="K52" s="12"/>
       <c r="L52" s="12"/>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53" s="18" t="s">
         <v>78</v>
       </c>
@@ -2413,12 +2467,14 @@
       </c>
       <c r="G53" s="22"/>
       <c r="H53" s="12"/>
-      <c r="I53" s="12"/>
+      <c r="I53" s="31" t="s">
+        <v>35</v>
+      </c>
       <c r="J53" s="12"/>
       <c r="K53" s="12"/>
       <c r="L53" s="12"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" s="18" t="s">
         <v>79</v>
       </c>
@@ -2444,7 +2500,7 @@
       <c r="K54" s="12"/>
       <c r="L54" s="12"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55" s="18" t="s">
         <v>80</v>
       </c>
@@ -2468,7 +2524,7 @@
       <c r="K55" s="12"/>
       <c r="L55" s="12"/>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56" s="18" t="s">
         <v>81</v>
       </c>
@@ -2489,12 +2545,14 @@
       </c>
       <c r="G56" s="22"/>
       <c r="H56" s="12"/>
-      <c r="I56" s="12"/>
+      <c r="I56" s="31" t="s">
+        <v>35</v>
+      </c>
       <c r="J56" s="12"/>
       <c r="K56" s="12"/>
       <c r="L56" s="12"/>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57" s="18" t="s">
         <v>82</v>
       </c>
@@ -2520,7 +2578,7 @@
       <c r="K57" s="12"/>
       <c r="L57" s="12"/>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58" s="7">
         <v>44</v>
       </c>
@@ -2539,12 +2597,14 @@
       </c>
       <c r="G58" s="22"/>
       <c r="H58" s="19"/>
-      <c r="I58" s="19"/>
+      <c r="I58" s="31" t="s">
+        <v>35</v>
+      </c>
       <c r="J58" s="19"/>
       <c r="K58" s="19"/>
       <c r="L58" s="19"/>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59" s="7">
         <v>45</v>
       </c>
@@ -2563,12 +2623,14 @@
       </c>
       <c r="G59" s="22"/>
       <c r="H59" s="19"/>
-      <c r="I59" s="19"/>
+      <c r="I59" s="31" t="s">
+        <v>35</v>
+      </c>
       <c r="J59" s="19"/>
       <c r="K59" s="19"/>
       <c r="L59" s="19"/>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60" s="7">
         <v>46</v>
       </c>
@@ -2587,12 +2649,14 @@
       </c>
       <c r="G60" s="22"/>
       <c r="H60" s="19"/>
-      <c r="I60" s="19"/>
+      <c r="I60" s="31" t="s">
+        <v>35</v>
+      </c>
       <c r="J60" s="19"/>
       <c r="K60" s="19"/>
       <c r="L60" s="19"/>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61" s="7">
         <v>47</v>
       </c>
@@ -2611,12 +2675,14 @@
       </c>
       <c r="G61" s="22"/>
       <c r="H61" s="19"/>
-      <c r="I61" s="19"/>
+      <c r="I61" s="31" t="s">
+        <v>35</v>
+      </c>
       <c r="J61" s="19"/>
       <c r="K61" s="19"/>
       <c r="L61" s="19"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62" s="7">
         <v>48</v>
       </c>
@@ -2635,12 +2701,14 @@
       </c>
       <c r="G62" s="22"/>
       <c r="H62" s="19"/>
-      <c r="I62" s="19"/>
+      <c r="I62" s="31" t="s">
+        <v>35</v>
+      </c>
       <c r="J62" s="19"/>
       <c r="K62" s="19"/>
       <c r="L62" s="19"/>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63" s="7">
         <v>49</v>
       </c>
@@ -2659,12 +2727,14 @@
       </c>
       <c r="G63" s="22"/>
       <c r="H63" s="19"/>
-      <c r="I63" s="19"/>
+      <c r="I63" s="31" t="s">
+        <v>35</v>
+      </c>
       <c r="J63" s="19"/>
       <c r="K63" s="19"/>
       <c r="L63" s="19"/>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64" s="7">
         <v>50</v>
       </c>
@@ -2688,7 +2758,7 @@
       <c r="K64" s="19"/>
       <c r="L64" s="19"/>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A65" s="7">
         <v>51</v>
       </c>
@@ -2707,12 +2777,14 @@
       </c>
       <c r="G65" s="22"/>
       <c r="H65" s="19"/>
-      <c r="I65" s="19"/>
+      <c r="I65" s="31" t="s">
+        <v>35</v>
+      </c>
       <c r="J65" s="19"/>
       <c r="K65" s="19"/>
       <c r="L65" s="19"/>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A66" s="7">
         <v>52</v>
       </c>
@@ -2731,12 +2803,15 @@
       </c>
       <c r="G66" s="22"/>
       <c r="H66" s="19"/>
-      <c r="I66" s="19"/>
+      <c r="I66" s="31" t="s">
+        <v>35</v>
+      </c>
       <c r="J66" s="19"/>
       <c r="K66" s="19"/>
       <c r="L66" s="19"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:L66" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Enabled "ExtendedDataPoint" for YesNoNaComponent
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/euTaxonomyNonFinancials/EutaxonomyNonFinancials.xlsx
+++ b/dataland-framework-toolbox/inputs/euTaxonomyNonFinancials/EutaxonomyNonFinancials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d93476\Dataland\dataland-framework-toolbox\inputs\euTaxonomyNonFinancials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14D3C2D5-6DFE-455A-908F-947CE39F3735}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65447D9B-8421-407A-9A4B-2BE49E2034F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="128">
   <si>
     <t>Field Identifier</t>
   </si>
@@ -442,9 +442,6 @@
   </si>
   <si>
     <t>Custom EuTaxonomyAlignedActivitiesComponent</t>
-  </si>
-  <si>
-    <t>AmountWithCurrencyComponent</t>
   </si>
 </sst>
 </file>
@@ -751,7 +748,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -801,7 +798,6 @@
     <xf numFmtId="0" fontId="10" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1064,10 +1060,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:L66"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1118,7 +1115,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7">
         <v>0</v>
       </c>
@@ -1144,7 +1141,7 @@
       <c r="K2" s="12"/>
       <c r="L2" s="12"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7"/>
       <c r="B3" s="8" t="s">
         <v>12</v>
@@ -1187,7 +1184,9 @@
         <v>14</v>
       </c>
       <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
+      <c r="I4" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="J4" s="11"/>
       <c r="K4" s="11"/>
       <c r="L4" s="12"/>
@@ -1213,7 +1212,9 @@
         <v>14</v>
       </c>
       <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
+      <c r="I5" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="J5" s="12"/>
       <c r="K5" s="12"/>
       <c r="L5" s="12"/>
@@ -1239,12 +1240,14 @@
         <v>14</v>
       </c>
       <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
+      <c r="I6" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="J6" s="12"/>
       <c r="K6" s="12"/>
       <c r="L6" s="12"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>4</v>
       </c>
@@ -1289,12 +1292,14 @@
       </c>
       <c r="G8" s="22"/>
       <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
+      <c r="I8" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="J8" s="12"/>
       <c r="K8" s="12"/>
       <c r="L8" s="12"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>6</v>
       </c>
@@ -1363,7 +1368,7 @@
       </c>
       <c r="G11" s="22"/>
       <c r="H11" s="12"/>
-      <c r="I11" s="31" t="s">
+      <c r="I11" s="12" t="s">
         <v>35</v>
       </c>
       <c r="J11" s="12"/>
@@ -1387,11 +1392,13 @@
         <v>91</v>
       </c>
       <c r="F12" s="21" t="s">
-        <v>128</v>
+        <v>38</v>
       </c>
       <c r="G12" s="22"/>
       <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
+      <c r="I12" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="J12" s="12"/>
       <c r="K12" s="12"/>
       <c r="L12" s="12"/>
@@ -1417,7 +1424,7 @@
       </c>
       <c r="G13" s="22"/>
       <c r="H13" s="12"/>
-      <c r="I13" s="31" t="s">
+      <c r="I13" s="12" t="s">
         <v>35</v>
       </c>
       <c r="J13" s="12"/>
@@ -1441,11 +1448,13 @@
         <v>114</v>
       </c>
       <c r="F14" s="21" t="s">
-        <v>128</v>
+        <v>38</v>
       </c>
       <c r="G14" s="22"/>
       <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
+      <c r="I14" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="J14" s="12"/>
       <c r="K14" s="12"/>
       <c r="L14" s="12"/>
@@ -1471,7 +1480,7 @@
       </c>
       <c r="G15" s="22"/>
       <c r="H15" s="12"/>
-      <c r="I15" s="31" t="s">
+      <c r="I15" s="12" t="s">
         <v>35</v>
       </c>
       <c r="J15" s="12"/>
@@ -1495,16 +1504,18 @@
         <v>113</v>
       </c>
       <c r="F16" s="21" t="s">
-        <v>128</v>
+        <v>38</v>
       </c>
       <c r="G16" s="22"/>
       <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
+      <c r="I16" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="J16" s="12"/>
       <c r="K16" s="12"/>
       <c r="L16" s="12"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" s="18" t="s">
         <v>62</v>
       </c>
@@ -1549,7 +1560,7 @@
       </c>
       <c r="G18" s="22"/>
       <c r="H18" s="12"/>
-      <c r="I18" s="31" t="s">
+      <c r="I18" s="12" t="s">
         <v>35</v>
       </c>
       <c r="J18" s="12"/>
@@ -1573,11 +1584,13 @@
         <v>112</v>
       </c>
       <c r="F19" s="21" t="s">
-        <v>128</v>
+        <v>38</v>
       </c>
       <c r="G19" s="22"/>
       <c r="H19" s="12"/>
-      <c r="I19" s="12"/>
+      <c r="I19" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="J19" s="12"/>
       <c r="K19" s="12"/>
       <c r="L19" s="12"/>
@@ -1601,7 +1614,7 @@
       </c>
       <c r="G20" s="22"/>
       <c r="H20" s="12"/>
-      <c r="I20" s="31" t="s">
+      <c r="I20" s="12" t="s">
         <v>35</v>
       </c>
       <c r="J20" s="12"/>
@@ -1627,7 +1640,7 @@
       </c>
       <c r="G21" s="22"/>
       <c r="H21" s="12"/>
-      <c r="I21" s="31" t="s">
+      <c r="I21" s="12" t="s">
         <v>35</v>
       </c>
       <c r="J21" s="12"/>
@@ -1653,7 +1666,7 @@
       </c>
       <c r="G22" s="22"/>
       <c r="H22" s="12"/>
-      <c r="I22" s="31" t="s">
+      <c r="I22" s="12" t="s">
         <v>35</v>
       </c>
       <c r="J22" s="12"/>
@@ -1679,7 +1692,7 @@
       </c>
       <c r="G23" s="22"/>
       <c r="H23" s="12"/>
-      <c r="I23" s="31" t="s">
+      <c r="I23" s="12" t="s">
         <v>35</v>
       </c>
       <c r="J23" s="12"/>
@@ -1705,7 +1718,7 @@
       </c>
       <c r="G24" s="22"/>
       <c r="H24" s="12"/>
-      <c r="I24" s="31" t="s">
+      <c r="I24" s="12" t="s">
         <v>35</v>
       </c>
       <c r="J24" s="12"/>
@@ -1731,14 +1744,14 @@
       </c>
       <c r="G25" s="22"/>
       <c r="H25" s="12"/>
-      <c r="I25" s="31" t="s">
+      <c r="I25" s="12" t="s">
         <v>35</v>
       </c>
       <c r="J25" s="12"/>
       <c r="K25" s="12"/>
       <c r="L25" s="12"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" s="7">
         <v>20</v>
       </c>
@@ -1781,7 +1794,7 @@
       </c>
       <c r="G27" s="22"/>
       <c r="H27" s="12"/>
-      <c r="I27" s="31" t="s">
+      <c r="I27" s="12" t="s">
         <v>35</v>
       </c>
       <c r="J27" s="12"/>
@@ -1807,7 +1820,7 @@
       </c>
       <c r="G28" s="22"/>
       <c r="H28" s="12"/>
-      <c r="I28" s="31" t="s">
+      <c r="I28" s="12" t="s">
         <v>35</v>
       </c>
       <c r="J28" s="12"/>
@@ -1861,7 +1874,7 @@
       </c>
       <c r="G30" s="22"/>
       <c r="H30" s="12"/>
-      <c r="I30" s="31" t="s">
+      <c r="I30" s="12" t="s">
         <v>35</v>
       </c>
       <c r="J30" s="12"/>
@@ -1885,11 +1898,13 @@
         <v>107</v>
       </c>
       <c r="F31" s="21" t="s">
-        <v>128</v>
+        <v>38</v>
       </c>
       <c r="G31" s="22"/>
       <c r="H31" s="12"/>
-      <c r="I31" s="12"/>
+      <c r="I31" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="J31" s="12"/>
       <c r="K31" s="12"/>
       <c r="L31" s="12"/>
@@ -1915,7 +1930,7 @@
       </c>
       <c r="G32" s="22"/>
       <c r="H32" s="12"/>
-      <c r="I32" s="31" t="s">
+      <c r="I32" s="12" t="s">
         <v>35</v>
       </c>
       <c r="J32" s="12"/>
@@ -1939,11 +1954,13 @@
         <v>102</v>
       </c>
       <c r="F33" s="21" t="s">
-        <v>128</v>
+        <v>38</v>
       </c>
       <c r="G33" s="22"/>
       <c r="H33" s="12"/>
-      <c r="I33" s="12"/>
+      <c r="I33" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="J33" s="12"/>
       <c r="K33" s="12"/>
       <c r="L33" s="12"/>
@@ -1969,7 +1986,7 @@
       </c>
       <c r="G34" s="22"/>
       <c r="H34" s="12"/>
-      <c r="I34" s="31" t="s">
+      <c r="I34" s="12" t="s">
         <v>35</v>
       </c>
       <c r="J34" s="12"/>
@@ -1993,16 +2010,18 @@
         <v>106</v>
       </c>
       <c r="F35" s="21" t="s">
-        <v>128</v>
+        <v>38</v>
       </c>
       <c r="G35" s="22"/>
       <c r="H35" s="12"/>
-      <c r="I35" s="12"/>
+      <c r="I35" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="J35" s="12"/>
       <c r="K35" s="12"/>
       <c r="L35" s="12"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" s="18" t="s">
         <v>71</v>
       </c>
@@ -2047,7 +2066,7 @@
       </c>
       <c r="G37" s="22"/>
       <c r="H37" s="12"/>
-      <c r="I37" s="31" t="s">
+      <c r="I37" s="12" t="s">
         <v>35</v>
       </c>
       <c r="J37" s="12"/>
@@ -2071,11 +2090,13 @@
         <v>103</v>
       </c>
       <c r="F38" s="21" t="s">
-        <v>128</v>
+        <v>38</v>
       </c>
       <c r="G38" s="22"/>
       <c r="H38" s="12"/>
-      <c r="I38" s="12"/>
+      <c r="I38" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="J38" s="12"/>
       <c r="K38" s="12"/>
       <c r="L38" s="12"/>
@@ -2099,7 +2120,7 @@
       </c>
       <c r="G39" s="22"/>
       <c r="H39" s="12"/>
-      <c r="I39" s="31" t="s">
+      <c r="I39" s="12" t="s">
         <v>35</v>
       </c>
       <c r="J39" s="12"/>
@@ -2125,7 +2146,7 @@
       </c>
       <c r="G40" s="22"/>
       <c r="H40" s="12"/>
-      <c r="I40" s="31" t="s">
+      <c r="I40" s="12" t="s">
         <v>35</v>
       </c>
       <c r="J40" s="12"/>
@@ -2151,7 +2172,7 @@
       </c>
       <c r="G41" s="22"/>
       <c r="H41" s="12"/>
-      <c r="I41" s="31" t="s">
+      <c r="I41" s="12" t="s">
         <v>35</v>
       </c>
       <c r="J41" s="12"/>
@@ -2177,7 +2198,7 @@
       </c>
       <c r="G42" s="22"/>
       <c r="H42" s="12"/>
-      <c r="I42" s="31" t="s">
+      <c r="I42" s="12" t="s">
         <v>35</v>
       </c>
       <c r="J42" s="12"/>
@@ -2203,7 +2224,7 @@
       </c>
       <c r="G43" s="22"/>
       <c r="H43" s="12"/>
-      <c r="I43" s="31" t="s">
+      <c r="I43" s="12" t="s">
         <v>35</v>
       </c>
       <c r="J43" s="12"/>
@@ -2229,14 +2250,14 @@
       </c>
       <c r="G44" s="22"/>
       <c r="H44" s="12"/>
-      <c r="I44" s="31" t="s">
+      <c r="I44" s="12" t="s">
         <v>35</v>
       </c>
       <c r="J44" s="12"/>
       <c r="K44" s="12"/>
       <c r="L44" s="12"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" s="7">
         <v>35</v>
       </c>
@@ -2279,7 +2300,7 @@
       </c>
       <c r="G46" s="22"/>
       <c r="H46" s="12"/>
-      <c r="I46" s="31" t="s">
+      <c r="I46" s="12" t="s">
         <v>35</v>
       </c>
       <c r="J46" s="12"/>
@@ -2305,7 +2326,7 @@
       </c>
       <c r="G47" s="22"/>
       <c r="H47" s="12"/>
-      <c r="I47" s="31" t="s">
+      <c r="I47" s="12" t="s">
         <v>35</v>
       </c>
       <c r="J47" s="12"/>
@@ -2359,7 +2380,7 @@
       </c>
       <c r="G49" s="22"/>
       <c r="H49" s="12"/>
-      <c r="I49" s="31" t="s">
+      <c r="I49" s="12" t="s">
         <v>35</v>
       </c>
       <c r="J49" s="12"/>
@@ -2383,11 +2404,13 @@
         <v>108</v>
       </c>
       <c r="F50" s="21" t="s">
-        <v>128</v>
+        <v>38</v>
       </c>
       <c r="G50" s="22"/>
       <c r="H50" s="12"/>
-      <c r="I50" s="12"/>
+      <c r="I50" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="J50" s="12"/>
       <c r="K50" s="12"/>
       <c r="L50" s="12"/>
@@ -2413,7 +2436,7 @@
       </c>
       <c r="G51" s="22"/>
       <c r="H51" s="12"/>
-      <c r="I51" s="31" t="s">
+      <c r="I51" s="12" t="s">
         <v>35</v>
       </c>
       <c r="J51" s="12"/>
@@ -2437,11 +2460,13 @@
         <v>109</v>
       </c>
       <c r="F52" s="21" t="s">
-        <v>128</v>
+        <v>38</v>
       </c>
       <c r="G52" s="22"/>
       <c r="H52" s="12"/>
-      <c r="I52" s="12"/>
+      <c r="I52" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="J52" s="12"/>
       <c r="K52" s="12"/>
       <c r="L52" s="12"/>
@@ -2467,7 +2492,7 @@
       </c>
       <c r="G53" s="22"/>
       <c r="H53" s="12"/>
-      <c r="I53" s="31" t="s">
+      <c r="I53" s="12" t="s">
         <v>35</v>
       </c>
       <c r="J53" s="12"/>
@@ -2491,16 +2516,18 @@
         <v>110</v>
       </c>
       <c r="F54" s="21" t="s">
-        <v>128</v>
+        <v>38</v>
       </c>
       <c r="G54" s="22"/>
       <c r="H54" s="12"/>
-      <c r="I54" s="12"/>
+      <c r="I54" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="J54" s="12"/>
       <c r="K54" s="12"/>
       <c r="L54" s="12"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" s="18" t="s">
         <v>80</v>
       </c>
@@ -2545,7 +2572,7 @@
       </c>
       <c r="G56" s="22"/>
       <c r="H56" s="12"/>
-      <c r="I56" s="31" t="s">
+      <c r="I56" s="12" t="s">
         <v>35</v>
       </c>
       <c r="J56" s="12"/>
@@ -2569,11 +2596,13 @@
         <v>111</v>
       </c>
       <c r="F57" s="21" t="s">
-        <v>128</v>
+        <v>38</v>
       </c>
       <c r="G57" s="22"/>
       <c r="H57" s="12"/>
-      <c r="I57" s="12"/>
+      <c r="I57" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="J57" s="12"/>
       <c r="K57" s="12"/>
       <c r="L57" s="12"/>
@@ -2597,7 +2626,7 @@
       </c>
       <c r="G58" s="22"/>
       <c r="H58" s="19"/>
-      <c r="I58" s="31" t="s">
+      <c r="I58" s="12" t="s">
         <v>35</v>
       </c>
       <c r="J58" s="19"/>
@@ -2623,7 +2652,7 @@
       </c>
       <c r="G59" s="22"/>
       <c r="H59" s="19"/>
-      <c r="I59" s="31" t="s">
+      <c r="I59" s="12" t="s">
         <v>35</v>
       </c>
       <c r="J59" s="19"/>
@@ -2649,7 +2678,7 @@
       </c>
       <c r="G60" s="22"/>
       <c r="H60" s="19"/>
-      <c r="I60" s="31" t="s">
+      <c r="I60" s="12" t="s">
         <v>35</v>
       </c>
       <c r="J60" s="19"/>
@@ -2675,7 +2704,7 @@
       </c>
       <c r="G61" s="22"/>
       <c r="H61" s="19"/>
-      <c r="I61" s="31" t="s">
+      <c r="I61" s="12" t="s">
         <v>35</v>
       </c>
       <c r="J61" s="19"/>
@@ -2701,7 +2730,7 @@
       </c>
       <c r="G62" s="22"/>
       <c r="H62" s="19"/>
-      <c r="I62" s="31" t="s">
+      <c r="I62" s="12" t="s">
         <v>35</v>
       </c>
       <c r="J62" s="19"/>
@@ -2727,14 +2756,14 @@
       </c>
       <c r="G63" s="22"/>
       <c r="H63" s="19"/>
-      <c r="I63" s="31" t="s">
+      <c r="I63" s="12" t="s">
         <v>35</v>
       </c>
       <c r="J63" s="19"/>
       <c r="K63" s="19"/>
       <c r="L63" s="19"/>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64" s="7">
         <v>50</v>
       </c>
@@ -2753,7 +2782,7 @@
       </c>
       <c r="G64" s="22"/>
       <c r="H64" s="19"/>
-      <c r="I64" s="19"/>
+      <c r="I64" s="12"/>
       <c r="J64" s="19"/>
       <c r="K64" s="19"/>
       <c r="L64" s="19"/>
@@ -2777,7 +2806,7 @@
       </c>
       <c r="G65" s="22"/>
       <c r="H65" s="19"/>
-      <c r="I65" s="31" t="s">
+      <c r="I65" s="12" t="s">
         <v>35</v>
       </c>
       <c r="J65" s="19"/>
@@ -2803,7 +2832,7 @@
       </c>
       <c r="G66" s="22"/>
       <c r="H66" s="19"/>
-      <c r="I66" s="31" t="s">
+      <c r="I66" s="12" t="s">
         <v>35</v>
       </c>
       <c r="J66" s="19"/>
@@ -2811,7 +2840,13 @@
       <c r="L66" s="19"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L66" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:L66" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="8">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Created BaseExpectedInput.json and BaseInput.json
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/euTaxonomyNonFinancials/EutaxonomyNonFinancials.xlsx
+++ b/dataland-framework-toolbox/inputs/euTaxonomyNonFinancials/EutaxonomyNonFinancials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d93476\Dataland\dataland-framework-toolbox\inputs\euTaxonomyNonFinancials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D52CD9D2-00C2-4CF3-8F7D-5C82E77CF2DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00A3FA48-BAA2-4D94-9D7C-689D0975D370}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1063,7 +1063,7 @@
   <dimension ref="A1:L66"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="F55" sqref="F55:F64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Created first working test for V19_Migration
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/euTaxonomyNonFinancials/EutaxonomyNonFinancials.xlsx
+++ b/dataland-framework-toolbox/inputs/euTaxonomyNonFinancials/EutaxonomyNonFinancials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d93476\Dataland\dataland-framework-toolbox\inputs\euTaxonomyNonFinancials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00A3FA48-BAA2-4D94-9D7C-689D0975D370}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6884C855-0BA1-4207-96C7-75ADBC295737}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1060,9 +1060,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:L66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="F55" sqref="F55:F64"/>
     </sheetView>
   </sheetViews>
@@ -1114,7 +1115,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7">
         <v>0</v>
       </c>
@@ -1140,7 +1141,7 @@
       <c r="K2" s="12"/>
       <c r="L2" s="12"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7"/>
       <c r="B3" s="8" t="s">
         <v>12</v>
@@ -1246,7 +1247,7 @@
       <c r="K6" s="12"/>
       <c r="L6" s="12"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>4</v>
       </c>
@@ -1298,7 +1299,7 @@
       <c r="K8" s="12"/>
       <c r="L8" s="12"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>6</v>
       </c>
@@ -1514,7 +1515,7 @@
       <c r="K16" s="12"/>
       <c r="L16" s="12"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" s="18" t="s">
         <v>62</v>
       </c>
@@ -1750,7 +1751,7 @@
       <c r="K25" s="12"/>
       <c r="L25" s="12"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" s="7">
         <v>20</v>
       </c>
@@ -2020,7 +2021,7 @@
       <c r="K35" s="12"/>
       <c r="L35" s="12"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" s="18" t="s">
         <v>71</v>
       </c>
@@ -2256,7 +2257,7 @@
       <c r="K44" s="12"/>
       <c r="L44" s="12"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" s="7">
         <v>35</v>
       </c>
@@ -2526,7 +2527,7 @@
       <c r="K54" s="12"/>
       <c r="L54" s="12"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" s="18" t="s">
         <v>80</v>
       </c>
@@ -2762,7 +2763,7 @@
       <c r="K63" s="19"/>
       <c r="L63" s="19"/>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64" s="7">
         <v>50</v>
       </c>
@@ -2839,7 +2840,13 @@
       <c r="L66" s="19"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L66" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:L66" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="8">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Made "Date" to ExtendedDataPoint
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/euTaxonomyNonFinancials/EutaxonomyNonFinancials.xlsx
+++ b/dataland-framework-toolbox/inputs/euTaxonomyNonFinancials/EutaxonomyNonFinancials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d93476\Dataland\dataland-framework-toolbox\inputs\euTaxonomyNonFinancials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{626F09FB-0630-4554-A75A-35EA748AF4CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9121EED6-7DC9-4447-8611-DF94F6EECA44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="128">
   <si>
     <t>Field Identifier</t>
   </si>
@@ -1060,11 +1060,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:L66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F55" sqref="F55:F64"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1115,7 +1114,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="7">
         <v>0</v>
       </c>
@@ -1141,7 +1140,7 @@
       <c r="K2" s="12"/>
       <c r="L2" s="12"/>
     </row>
-    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="7"/>
       <c r="B3" s="8" t="s">
         <v>12</v>
@@ -1158,7 +1157,9 @@
       </c>
       <c r="G3" s="10"/>
       <c r="H3" s="11"/>
-      <c r="I3" s="12"/>
+      <c r="I3" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="J3" s="12"/>
       <c r="K3" s="12"/>
       <c r="L3" s="12"/>
@@ -1247,7 +1248,7 @@
       <c r="K6" s="12"/>
       <c r="L6" s="12"/>
     </row>
-    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>4</v>
       </c>
@@ -1299,7 +1300,7 @@
       <c r="K8" s="12"/>
       <c r="L8" s="12"/>
     </row>
-    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>6</v>
       </c>
@@ -1515,7 +1516,7 @@
       <c r="K16" s="12"/>
       <c r="L16" s="12"/>
     </row>
-    <row r="17" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="18" t="s">
         <v>62</v>
       </c>
@@ -1751,7 +1752,7 @@
       <c r="K25" s="12"/>
       <c r="L25" s="12"/>
     </row>
-    <row r="26" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="7">
         <v>20</v>
       </c>
@@ -2021,7 +2022,7 @@
       <c r="K35" s="12"/>
       <c r="L35" s="12"/>
     </row>
-    <row r="36" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" s="18" t="s">
         <v>71</v>
       </c>
@@ -2257,7 +2258,7 @@
       <c r="K44" s="12"/>
       <c r="L44" s="12"/>
     </row>
-    <row r="45" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" s="7">
         <v>35</v>
       </c>
@@ -2527,7 +2528,7 @@
       <c r="K54" s="12"/>
       <c r="L54" s="12"/>
     </row>
-    <row r="55" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55" s="18" t="s">
         <v>80</v>
       </c>
@@ -2763,7 +2764,7 @@
       <c r="K63" s="19"/>
       <c r="L63" s="19"/>
     </row>
-    <row r="64" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64" s="7">
         <v>50</v>
       </c>
@@ -2840,13 +2841,7 @@
       <c r="L66" s="19"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L66" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="8">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:L66" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Made "Date" to ExtendedDataPoint and tested it
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/euTaxonomyNonFinancials/EutaxonomyNonFinancials.xlsx
+++ b/dataland-framework-toolbox/inputs/euTaxonomyNonFinancials/EutaxonomyNonFinancials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d93476\Dataland\dataland-framework-toolbox\inputs\euTaxonomyNonFinancials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9121EED6-7DC9-4447-8611-DF94F6EECA44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00DD5139-EC54-4ADB-A218-4569D6BF6AF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1063,7 +1063,7 @@
   <dimension ref="A1:L66"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Changed Excel File EutaxonomyNonFinancials.xlsx to the newewst Version.
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/euTaxonomyNonFinancials/EutaxonomyNonFinancials.xlsx
+++ b/dataland-framework-toolbox/inputs/euTaxonomyNonFinancials/EutaxonomyNonFinancials.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d92048\IdeaProjects\Dataland5\dataland-framework-toolbox\inputs\euTaxonomyNonFinancials\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d93369\Documents\Projekte\Dataland\Repos\Dataland\dataland-framework-toolbox\inputs\euTaxonomyNonFinancials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9190097E-1C69-4385-816A-3AC5DD386F05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AD449AF-6DDA-4D38-8046-160256CB1462}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Framework Data Model" sheetId="1" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="235">
   <si>
     <t>Field Identifier</t>
   </si>
@@ -161,9 +161,6 @@
     <t>Revenue</t>
   </si>
   <si>
-    <t>Grade of the substantial contribution criterion fulfillment</t>
-  </si>
-  <si>
     <t>Extended</t>
   </si>
   <si>
@@ -218,24 +215,6 @@
     <t>Aligned Share</t>
   </si>
   <si>
-    <t>Substantial Contribution to Climate Change Mitigation In Percent</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to Climate Change Adaptation In Percent</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to Sustainable Use and Protection of Water and Marine Resources In Percent</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to Transition to a Circular Economy In Percent</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to Pollution Prevention and Control In Percent</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to Protection and Restoration of Biodiversity and Ecosystems In Percent</t>
-  </si>
-  <si>
     <t>Aligned Activities</t>
   </si>
   <si>
@@ -444,13 +423,352 @@
   </si>
   <si>
     <t>AmountWithCurrencyComponent</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Climate Change Mitigation In Percent - Eligible</t>
+  </si>
+  <si>
+    <t>Taxonomy-eligible proportion of revenue substantially contributing to climate change mitigation</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Climate Change Mitigation In Percent - Aligned</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned proportion of revenue substantially contributing to climate change mitigation</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Climate Change Mitigation In Percent - Of which use of proceeds</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned use of proceeds share substantially contributing to climate change mitigation</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Climate Change Mitigation In Percent - Enabling Share</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned and enabling proportion of revenue substantially contributing to climate change mitigation</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Climate Change Mitigation In Percent - Transitional Share</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned and transitional proportion of revenue substantially contributing to climate change mitigation</t>
+  </si>
+  <si>
+    <t>14.1</t>
+  </si>
+  <si>
+    <t>14.1.1</t>
+  </si>
+  <si>
+    <t>14.1.2</t>
+  </si>
+  <si>
+    <t>14.1.3</t>
+  </si>
+  <si>
+    <t>15.1</t>
+  </si>
+  <si>
+    <t>15.1.1</t>
+  </si>
+  <si>
+    <t>15.1.2</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Climate Change Adaptation In Percent - Eligible</t>
+  </si>
+  <si>
+    <t>Taxonomy-eligible proportion of revenue substantially contributing to climate change adaptation</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Climate Change Adaptation In Percent - Aligned</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned proportion of revenue substantially contributing to climate change adaptation</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Climate Change Adaptation In Percent - Of which use of proceeds</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned use of proceeds share substantially contributing to climate change adaptation</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Climate Change Adaptation In Percent - Enabling Share</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned and enabling proportion of revenue substantially contributing to climate change adaptation</t>
+  </si>
+  <si>
+    <t>16.1</t>
+  </si>
+  <si>
+    <t>16.1.1</t>
+  </si>
+  <si>
+    <t>16.1.2</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Sustainable Use and Protection of Water and Marine Resources In Percent - Eligible</t>
+  </si>
+  <si>
+    <t>Taxonomy-eligible proportion of revenue substantially contributing to sustainable use and protection of water and marine resources</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Sustainable Use and Protection of Water and Marine Resources In Percent - Aligned</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned proportion of revenue substantially contributing to sustainable use and protection of water and marine resources</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Sustainable Use and Protection of Water and Marine Resources In Percent - Of which use of proceeds</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned use of proceeds share substantially contributing to sustainable use and protection of water and marine resources</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Sustainable Use and Protection of Water and Marine Resources In Percent - Enabling Share</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned and enabling proportion of revenue substantially contributing to sustainable use and protection of water and marine resources</t>
+  </si>
+  <si>
+    <t>17.1</t>
+  </si>
+  <si>
+    <t>17.1.1</t>
+  </si>
+  <si>
+    <t>17.1.2</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Transition to a Circular Economy In Percent - Eligible</t>
+  </si>
+  <si>
+    <t>Taxonomy-eligible proportion of revenue substantially contributing to circular economy</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Transition to a Circular Economy In Percent - Aligned</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned proportion of revenue substantially contributing to circular economy</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Transition to a Circular Economy In Percent - Of which use of proceeds</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned use of proceeds share substantially contributing to circular economy</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Transition to a Circular Economy In Percent - Enabling Share</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned and enabling proportion of revenue substantially contributing to circular economy</t>
+  </si>
+  <si>
+    <t>18.1</t>
+  </si>
+  <si>
+    <t>18.1.1</t>
+  </si>
+  <si>
+    <t>18.1.2</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Pollution Prevention and Control In Percent - Eligible</t>
+  </si>
+  <si>
+    <t>Taxonomy-eligible proportion of revenue substantially contributing to pollution prevention and control</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Pollution Prevention and Control In Percent - Aligned</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned proportion of revenue substantially contributing to pollution prevention and control</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Pollution Prevention and Control In Percent - Of which use of proceeds</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned use of proceeds share substantially contributing to pollution prevention and control</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Pollution Prevention and Control In Percent - Enabling Share</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned and enabling proportion of revenue substantially contributing to pollution prevention and control</t>
+  </si>
+  <si>
+    <t>19.1</t>
+  </si>
+  <si>
+    <t>19.1.1</t>
+  </si>
+  <si>
+    <t>19.1.2</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Protection and Restoration of Biodiversity and Ecosystems In Percent - Eligible</t>
+  </si>
+  <si>
+    <t>Taxonomy-eligible proportion of revenue substantially contributing to protection and restoration of biodiversity and ecosystems</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Protection and Restoration of Biodiversity and Ecosystems In Percent - Aligned</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned proportion of revenue substantially contributing to protection and restoration of biodiversity and ecosystems</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Protection and Restoration of Biodiversity and Ecosystems In Percent - Of which use of proceeds</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned use of proceeds share substantially contributing to protection and restoration of biodiversity and ecosystems</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Protection and Restoration of Biodiversity and Ecosystems In Percent - Enabling Share</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned and enabling proportion of revenue substantially contributing to protection and restoration of biodiversity and ecosystems</t>
+  </si>
+  <si>
+    <t>29.1</t>
+  </si>
+  <si>
+    <t>29.1.1</t>
+  </si>
+  <si>
+    <t>29.1.2</t>
+  </si>
+  <si>
+    <t>29.1.3</t>
+  </si>
+  <si>
+    <t>Taxonomy-eligible proportion of CapEx substantially contributing to climate change mitigation</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned proportion of CapEx substantially contributing to climate change mitigation</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned and enabling proportion of CapEx substantially contributing to climate change mitigation</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned and transitional proportion of CapEx substantially contributing to climate change mitigation</t>
+  </si>
+  <si>
+    <t>30.1</t>
+  </si>
+  <si>
+    <t>30.1.1</t>
+  </si>
+  <si>
+    <t>30.1.2</t>
+  </si>
+  <si>
+    <t>Taxonomy-eligible proportion of CapEx substantially contributing to climate change adaptation</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned proportion of CapEx substantially contributing to climate change adaptation</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned and enabling proportion of CapEx substantially contributing to climate change adaptation</t>
+  </si>
+  <si>
+    <t>31.1</t>
+  </si>
+  <si>
+    <t>31.1.1</t>
+  </si>
+  <si>
+    <t>31.1.2</t>
+  </si>
+  <si>
+    <t>Taxonomy-eligible proportion of CapEx substantially contributing to sustainable use and protection of water and marine resources</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned proportion of CapEx substantially contributing to sustainable use and protection of water and marine resources</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned and enabling proportion of CapEx substantially contributing to sustainable use and protection of water and marine resources</t>
+  </si>
+  <si>
+    <t>32.1</t>
+  </si>
+  <si>
+    <t>32.1.1</t>
+  </si>
+  <si>
+    <t>32.1.2</t>
+  </si>
+  <si>
+    <t>Taxonomy-eligible proportion of CapEx substantially contributing to circular economy</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned proportion of CapEx substantially contributing to circular economy</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned and enabling proportion of CapEx substantially contributing to circular economy</t>
+  </si>
+  <si>
+    <t>Taxonomy-eligible proportion of CapEx substantially contributing to pollution prevention and control</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned proportion of CapEx substantially contributing to pollution prevention and control</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned and enabling proportion of CapEx substantially contributing to pollution prevention and control</t>
+  </si>
+  <si>
+    <t>Taxonomy-eligible proportion of CapEx substantially contributing to protection and restoration of biodiversity and ecosystems</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned proportion of CapEx substantially contributing to protection and restoration of biodiversity and ecosystems</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned and enabling proportion of CapEx substantially contributing to protection and restoration of biodiversity and ecosystems</t>
+  </si>
+  <si>
+    <t>33.1</t>
+  </si>
+  <si>
+    <t>33.1.1</t>
+  </si>
+  <si>
+    <t>33.1.2</t>
+  </si>
+  <si>
+    <t>34.1</t>
+  </si>
+  <si>
+    <t>34.1.1</t>
+  </si>
+  <si>
+    <t>34.1.2</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned proportion of OpEx substantially contributing to climate change mitigation</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned proportion of OpEx substantially contributing to climate change adaptation</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned proportion of OpEx substantially contributing to sustainable use and protection of water and marine resources</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned proportion of OpEx substantially contributing to circular economy</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned proportion of OpEx substantially contributing to pollution prevention and control</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned proportion of OpEx substantially contributing to protection and restoration of biodiversity and ecosystems</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -522,8 +840,18 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -580,14 +908,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor rgb="FFF2F2F2"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor rgb="FFEFEFEF"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -750,7 +1072,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -798,8 +1120,10 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="10" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -874,6 +1198,10 @@
       <rgbColor rgb="00333399"/>
       <rgbColor rgb="00333333"/>
     </indexedColors>
+    <mruColors>
+      <color rgb="FFF2F2F2"/>
+      <color rgb="FFF2FFFF"/>
+    </mruColors>
   </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1062,23 +1390,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L66"/>
+  <dimension ref="A1:L104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D46" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F57" sqref="F57"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="20.1796875" customWidth="1"/>
-    <col min="4" max="4" width="70.36328125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="77.90625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="44.6328125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="26.1796875" customWidth="1"/>
-    <col min="8" max="12" width="14.36328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.21875" customWidth="1"/>
+    <col min="4" max="4" width="95.109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="77.88671875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="44.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="26.21875" customWidth="1"/>
+    <col min="8" max="12" width="14.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1116,7 +1444,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="7">
         <v>0</v>
       </c>
@@ -1134,7 +1462,7 @@
         <v>17</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="H2" s="11"/>
       <c r="I2" s="12"/>
@@ -1142,7 +1470,7 @@
       <c r="K2" s="12"/>
       <c r="L2" s="12"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="7"/>
       <c r="B3" s="8" t="s">
         <v>12</v>
@@ -1164,7 +1492,7 @@
       <c r="K3" s="12"/>
       <c r="L3" s="12"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>1</v>
       </c>
@@ -1190,7 +1518,7 @@
       <c r="K4" s="11"/>
       <c r="L4" s="12"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>2</v>
       </c>
@@ -1216,7 +1544,7 @@
       <c r="K5" s="12"/>
       <c r="L5" s="12"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>3</v>
       </c>
@@ -1242,7 +1570,7 @@
       <c r="K6" s="12"/>
       <c r="L6" s="12"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>4</v>
       </c>
@@ -1257,7 +1585,7 @@
         <v>32</v>
       </c>
       <c r="F7" s="27" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="G7" s="26" t="s">
         <v>14</v>
@@ -1268,7 +1596,7 @@
       <c r="K7" s="12"/>
       <c r="L7" s="12"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>5</v>
       </c>
@@ -1283,7 +1611,7 @@
         <v>27</v>
       </c>
       <c r="F8" s="20" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="G8" s="22"/>
       <c r="H8" s="12"/>
@@ -1292,7 +1620,7 @@
       <c r="K8" s="12"/>
       <c r="L8" s="12"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>6</v>
       </c>
@@ -1301,11 +1629,11 @@
       </c>
       <c r="C9" s="8"/>
       <c r="D9" s="14" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="E9" s="12"/>
       <c r="F9" s="20" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="G9" s="23" t="s">
         <v>14</v>
@@ -1316,7 +1644,7 @@
       <c r="K9" s="12"/>
       <c r="L9" s="12"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>8</v>
       </c>
@@ -1325,35 +1653,35 @@
       </c>
       <c r="C10" s="8"/>
       <c r="D10" s="15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E10" s="19" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="F10" s="21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G10" s="22"/>
       <c r="H10" s="12"/>
       <c r="I10" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J10" s="12"/>
       <c r="K10" s="12"/>
       <c r="L10" s="12"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C11" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="15" t="s">
         <v>40</v>
-      </c>
-      <c r="D11" s="15" t="s">
-        <v>41</v>
       </c>
       <c r="E11" s="19"/>
       <c r="F11" s="21" t="s">
@@ -1366,24 +1694,24 @@
       <c r="K11" s="12"/>
       <c r="L11" s="12"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E12" s="28" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="F12" s="21" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="G12" s="22"/>
       <c r="H12" s="12"/>
@@ -1392,21 +1720,21 @@
       <c r="K12" s="12"/>
       <c r="L12" s="12"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="F13" s="21" t="s">
         <v>28</v>
@@ -1418,24 +1746,24 @@
       <c r="K13" s="12"/>
       <c r="L13" s="12"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="F14" s="21" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="G14" s="22"/>
       <c r="H14" s="12"/>
@@ -1444,21 +1772,21 @@
       <c r="K14" s="12"/>
       <c r="L14" s="12"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B15" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E15" s="28" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="F15" s="21" t="s">
         <v>28</v>
@@ -1470,24 +1798,24 @@
       <c r="K15" s="12"/>
       <c r="L15" s="12"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E16" s="28" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="F16" s="21" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="G16" s="22"/>
       <c r="H16" s="12"/>
@@ -1496,22 +1824,22 @@
       <c r="K16" s="12"/>
       <c r="L16" s="12"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="18" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C17" s="8"/>
       <c r="D17" s="15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E17" s="28" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="F17" s="21" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="G17" s="22"/>
       <c r="H17" s="12"/>
@@ -1520,21 +1848,21 @@
       <c r="K17" s="12"/>
       <c r="L17" s="12"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="18" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="B18" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="F18" s="21" t="s">
         <v>28</v>
@@ -1546,24 +1874,24 @@
       <c r="K18" s="12"/>
       <c r="L18" s="12"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="18" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="F19" s="21" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="G19" s="22"/>
       <c r="H19" s="12"/>
@@ -1572,7 +1900,7 @@
       <c r="K19" s="12"/>
       <c r="L19" s="12"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="7">
         <v>14</v>
       </c>
@@ -1580,11 +1908,11 @@
         <v>33</v>
       </c>
       <c r="C20" s="8"/>
-      <c r="D20" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="E20" s="12" t="s">
-        <v>34</v>
+      <c r="D20" s="29" t="s">
+        <v>122</v>
+      </c>
+      <c r="E20" s="30" t="s">
+        <v>123</v>
       </c>
       <c r="F20" s="21" t="s">
         <v>28</v>
@@ -1596,19 +1924,19 @@
       <c r="K20" s="12"/>
       <c r="L20" s="12"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A21" s="7">
-        <v>15</v>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A21" s="18" t="s">
+        <v>132</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C21" s="8"/>
-      <c r="D21" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="E21" s="12" t="s">
-        <v>34</v>
+      <c r="D21" s="29" t="s">
+        <v>124</v>
+      </c>
+      <c r="E21" s="30" t="s">
+        <v>125</v>
       </c>
       <c r="F21" s="21" t="s">
         <v>28</v>
@@ -1620,19 +1948,19 @@
       <c r="K21" s="12"/>
       <c r="L21" s="12"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A22" s="7">
-        <v>16</v>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A22" s="18" t="s">
+        <v>133</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C22" s="8"/>
-      <c r="D22" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="E22" s="12" t="s">
-        <v>34</v>
+      <c r="D22" s="31" t="s">
+        <v>126</v>
+      </c>
+      <c r="E22" s="30" t="s">
+        <v>127</v>
       </c>
       <c r="F22" s="21" t="s">
         <v>28</v>
@@ -1644,19 +1972,19 @@
       <c r="K22" s="12"/>
       <c r="L22" s="12"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A23" s="7">
-        <v>17</v>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A23" s="18" t="s">
+        <v>134</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C23" s="8"/>
-      <c r="D23" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="E23" s="12" t="s">
-        <v>34</v>
+      <c r="D23" s="29" t="s">
+        <v>128</v>
+      </c>
+      <c r="E23" s="30" t="s">
+        <v>129</v>
       </c>
       <c r="F23" s="21" t="s">
         <v>28</v>
@@ -1668,19 +1996,19 @@
       <c r="K23" s="12"/>
       <c r="L23" s="12"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A24" s="7">
-        <v>18</v>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A24" s="18" t="s">
+        <v>135</v>
       </c>
       <c r="B24" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C24" s="8"/>
-      <c r="D24" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="E24" s="12" t="s">
-        <v>34</v>
+      <c r="D24" s="29" t="s">
+        <v>130</v>
+      </c>
+      <c r="E24" s="30" t="s">
+        <v>131</v>
       </c>
       <c r="F24" s="21" t="s">
         <v>28</v>
@@ -1692,19 +2020,19 @@
       <c r="K24" s="12"/>
       <c r="L24" s="12"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="7">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B25" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C25" s="8"/>
-      <c r="D25" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="E25" s="12" t="s">
-        <v>34</v>
+      <c r="D25" s="32" t="s">
+        <v>139</v>
+      </c>
+      <c r="E25" s="30" t="s">
+        <v>140</v>
       </c>
       <c r="F25" s="21" t="s">
         <v>28</v>
@@ -1716,22 +2044,22 @@
       <c r="K25" s="12"/>
       <c r="L25" s="12"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A26" s="7">
-        <v>20</v>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A26" s="18" t="s">
+        <v>136</v>
       </c>
       <c r="B26" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C26" s="8"/>
-      <c r="D26" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="E26" s="28" t="s">
-        <v>89</v>
+      <c r="D26" s="32" t="s">
+        <v>141</v>
+      </c>
+      <c r="E26" s="30" t="s">
+        <v>142</v>
       </c>
       <c r="F26" s="21" t="s">
-        <v>127</v>
+        <v>28</v>
       </c>
       <c r="G26" s="22"/>
       <c r="H26" s="12"/>
@@ -1740,19 +2068,19 @@
       <c r="K26" s="12"/>
       <c r="L26" s="12"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A27" s="7">
-        <v>21</v>
-      </c>
-      <c r="B27" s="16" t="s">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A27" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="B27" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C27" s="16"/>
-      <c r="D27" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="E27" s="28" t="s">
-        <v>92</v>
+      <c r="C27" s="8"/>
+      <c r="D27" s="31" t="s">
+        <v>143</v>
+      </c>
+      <c r="E27" s="30" t="s">
+        <v>144</v>
       </c>
       <c r="F27" s="21" t="s">
         <v>28</v>
@@ -1764,19 +2092,19 @@
       <c r="K27" s="12"/>
       <c r="L27" s="12"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A28" s="7">
-        <v>22</v>
-      </c>
-      <c r="B28" s="16" t="s">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A28" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="B28" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C28" s="16"/>
-      <c r="D28" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="E28" s="28" t="s">
-        <v>93</v>
+      <c r="C28" s="8"/>
+      <c r="D28" s="31" t="s">
+        <v>145</v>
+      </c>
+      <c r="E28" s="30" t="s">
+        <v>146</v>
       </c>
       <c r="F28" s="21" t="s">
         <v>28</v>
@@ -1788,47 +2116,43 @@
       <c r="K28" s="12"/>
       <c r="L28" s="12"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="7">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C29" s="8"/>
-      <c r="D29" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="E29" s="28" t="s">
-        <v>94</v>
+      <c r="D29" s="31" t="s">
+        <v>150</v>
+      </c>
+      <c r="E29" s="30" t="s">
+        <v>151</v>
       </c>
       <c r="F29" s="21" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="G29" s="22"/>
       <c r="H29" s="12"/>
-      <c r="I29" s="12" t="s">
-        <v>35</v>
-      </c>
+      <c r="I29" s="12"/>
       <c r="J29" s="12"/>
       <c r="K29" s="12"/>
       <c r="L29" s="12"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="18" t="s">
-        <v>67</v>
+        <v>147</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C30" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="D30" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="E30" s="29" t="s">
-        <v>118</v>
+        <v>33</v>
+      </c>
+      <c r="C30" s="8"/>
+      <c r="D30" s="31" t="s">
+        <v>152</v>
+      </c>
+      <c r="E30" s="30" t="s">
+        <v>153</v>
       </c>
       <c r="F30" s="21" t="s">
         <v>28</v>
@@ -1840,24 +2164,22 @@
       <c r="K30" s="12"/>
       <c r="L30" s="12"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="18" t="s">
-        <v>68</v>
+        <v>148</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C31" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="D31" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="E31" s="29" t="s">
-        <v>107</v>
+        <v>33</v>
+      </c>
+      <c r="C31" s="8"/>
+      <c r="D31" s="31" t="s">
+        <v>154</v>
+      </c>
+      <c r="E31" s="30" t="s">
+        <v>155</v>
       </c>
       <c r="F31" s="21" t="s">
-        <v>128</v>
+        <v>28</v>
       </c>
       <c r="G31" s="22"/>
       <c r="H31" s="12"/>
@@ -1866,21 +2188,19 @@
       <c r="K31" s="12"/>
       <c r="L31" s="12"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="18" t="s">
-        <v>65</v>
+        <v>149</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C32" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="D32" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="E32" s="28" t="s">
-        <v>119</v>
+        <v>33</v>
+      </c>
+      <c r="C32" s="8"/>
+      <c r="D32" s="31" t="s">
+        <v>156</v>
+      </c>
+      <c r="E32" s="30" t="s">
+        <v>157</v>
       </c>
       <c r="F32" s="21" t="s">
         <v>28</v>
@@ -1892,24 +2212,22 @@
       <c r="K32" s="12"/>
       <c r="L32" s="12"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A33" s="18" t="s">
-        <v>66</v>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A33" s="7">
+        <v>17</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C33" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="D33" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="E33" s="28" t="s">
-        <v>102</v>
+        <v>33</v>
+      </c>
+      <c r="C33" s="8"/>
+      <c r="D33" s="31" t="s">
+        <v>161</v>
+      </c>
+      <c r="E33" s="30" t="s">
+        <v>162</v>
       </c>
       <c r="F33" s="21" t="s">
-        <v>128</v>
+        <v>28</v>
       </c>
       <c r="G33" s="22"/>
       <c r="H33" s="12"/>
@@ -1918,21 +2236,19 @@
       <c r="K33" s="12"/>
       <c r="L33" s="12"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" s="18" t="s">
-        <v>69</v>
+        <v>158</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C34" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="D34" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="E34" s="29" t="s">
-        <v>120</v>
+        <v>33</v>
+      </c>
+      <c r="C34" s="8"/>
+      <c r="D34" s="31" t="s">
+        <v>163</v>
+      </c>
+      <c r="E34" s="30" t="s">
+        <v>164</v>
       </c>
       <c r="F34" s="21" t="s">
         <v>28</v>
@@ -1944,24 +2260,22 @@
       <c r="K34" s="12"/>
       <c r="L34" s="12"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" s="18" t="s">
-        <v>70</v>
+        <v>159</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C35" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="D35" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="E35" s="29" t="s">
-        <v>106</v>
+        <v>33</v>
+      </c>
+      <c r="C35" s="8"/>
+      <c r="D35" s="31" t="s">
+        <v>165</v>
+      </c>
+      <c r="E35" s="30" t="s">
+        <v>166</v>
       </c>
       <c r="F35" s="21" t="s">
-        <v>128</v>
+        <v>28</v>
       </c>
       <c r="G35" s="22"/>
       <c r="H35" s="12"/>
@@ -1970,22 +2284,22 @@
       <c r="K35" s="12"/>
       <c r="L35" s="12"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" s="18" t="s">
-        <v>71</v>
+        <v>160</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C36" s="8"/>
-      <c r="D36" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="E36" s="29" t="s">
-        <v>105</v>
+      <c r="D36" s="31" t="s">
+        <v>167</v>
+      </c>
+      <c r="E36" s="30" t="s">
+        <v>168</v>
       </c>
       <c r="F36" s="21" t="s">
-        <v>126</v>
+        <v>28</v>
       </c>
       <c r="G36" s="22"/>
       <c r="H36" s="12"/>
@@ -1994,21 +2308,19 @@
       <c r="K36" s="12"/>
       <c r="L36" s="12"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A37" s="18" t="s">
-        <v>72</v>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A37" s="7">
+        <v>18</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C37" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="D37" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="E37" s="29" t="s">
-        <v>121</v>
+        <v>33</v>
+      </c>
+      <c r="C37" s="8"/>
+      <c r="D37" s="31" t="s">
+        <v>172</v>
+      </c>
+      <c r="E37" s="30" t="s">
+        <v>173</v>
       </c>
       <c r="F37" s="21" t="s">
         <v>28</v>
@@ -2020,24 +2332,22 @@
       <c r="K37" s="12"/>
       <c r="L37" s="12"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" s="18" t="s">
-        <v>73</v>
+        <v>169</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C38" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="D38" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="E38" s="29" t="s">
-        <v>103</v>
+        <v>33</v>
+      </c>
+      <c r="C38" s="8"/>
+      <c r="D38" s="31" t="s">
+        <v>174</v>
+      </c>
+      <c r="E38" s="30" t="s">
+        <v>175</v>
       </c>
       <c r="F38" s="21" t="s">
-        <v>128</v>
+        <v>28</v>
       </c>
       <c r="G38" s="22"/>
       <c r="H38" s="12"/>
@@ -2046,19 +2356,19 @@
       <c r="K38" s="12"/>
       <c r="L38" s="12"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A39" s="7">
-        <v>29</v>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A39" s="18" t="s">
+        <v>170</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C39" s="8"/>
-      <c r="D39" s="15" t="s">
-        <v>53</v>
+      <c r="D39" s="31" t="s">
+        <v>176</v>
       </c>
       <c r="E39" s="30" t="s">
-        <v>34</v>
+        <v>177</v>
       </c>
       <c r="F39" s="21" t="s">
         <v>28</v>
@@ -2070,19 +2380,19 @@
       <c r="K39" s="12"/>
       <c r="L39" s="12"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A40" s="7">
-        <v>30</v>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A40" s="18" t="s">
+        <v>171</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C40" s="8"/>
-      <c r="D40" s="15" t="s">
-        <v>54</v>
+      <c r="D40" s="31" t="s">
+        <v>178</v>
       </c>
       <c r="E40" s="30" t="s">
-        <v>34</v>
+        <v>179</v>
       </c>
       <c r="F40" s="21" t="s">
         <v>28</v>
@@ -2094,19 +2404,19 @@
       <c r="K40" s="12"/>
       <c r="L40" s="12"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" s="7">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C41" s="8"/>
-      <c r="D41" s="15" t="s">
-        <v>55</v>
+      <c r="D41" s="31" t="s">
+        <v>183</v>
       </c>
       <c r="E41" s="30" t="s">
-        <v>34</v>
+        <v>184</v>
       </c>
       <c r="F41" s="21" t="s">
         <v>28</v>
@@ -2118,19 +2428,19 @@
       <c r="K41" s="12"/>
       <c r="L41" s="12"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A42" s="7">
-        <v>32</v>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A42" s="18" t="s">
+        <v>180</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C42" s="8"/>
-      <c r="D42" s="15" t="s">
-        <v>56</v>
+      <c r="D42" s="31" t="s">
+        <v>185</v>
       </c>
       <c r="E42" s="30" t="s">
-        <v>34</v>
+        <v>186</v>
       </c>
       <c r="F42" s="21" t="s">
         <v>28</v>
@@ -2142,19 +2452,19 @@
       <c r="K42" s="12"/>
       <c r="L42" s="12"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A43" s="7">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A43" s="18" t="s">
+        <v>181</v>
+      </c>
+      <c r="B43" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B43" s="8" t="s">
-        <v>36</v>
-      </c>
       <c r="C43" s="8"/>
-      <c r="D43" s="15" t="s">
-        <v>57</v>
+      <c r="D43" s="31" t="s">
+        <v>187</v>
       </c>
       <c r="E43" s="30" t="s">
-        <v>34</v>
+        <v>188</v>
       </c>
       <c r="F43" s="21" t="s">
         <v>28</v>
@@ -2166,19 +2476,19 @@
       <c r="K43" s="12"/>
       <c r="L43" s="12"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A44" s="7">
-        <v>34</v>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A44" s="18" t="s">
+        <v>182</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C44" s="8"/>
-      <c r="D44" s="15" t="s">
-        <v>58</v>
+      <c r="D44" s="31" t="s">
+        <v>189</v>
       </c>
       <c r="E44" s="30" t="s">
-        <v>34</v>
+        <v>190</v>
       </c>
       <c r="F44" s="21" t="s">
         <v>28</v>
@@ -2190,22 +2500,22 @@
       <c r="K44" s="12"/>
       <c r="L44" s="12"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" s="7">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C45" s="8"/>
       <c r="D45" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="E45" s="29" t="s">
-        <v>104</v>
+        <v>52</v>
+      </c>
+      <c r="E45" s="28" t="s">
+        <v>82</v>
       </c>
       <c r="F45" s="21" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="G45" s="22"/>
       <c r="H45" s="12"/>
@@ -2214,19 +2524,19 @@
       <c r="K45" s="12"/>
       <c r="L45" s="12"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" s="7">
-        <v>36</v>
-      </c>
-      <c r="B46" s="8" t="s">
-        <v>36</v>
+        <v>21</v>
+      </c>
+      <c r="B46" s="16" t="s">
+        <v>33</v>
       </c>
       <c r="C46" s="16"/>
       <c r="D46" s="17" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="E46" s="28" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="F46" s="21" t="s">
         <v>28</v>
@@ -2238,19 +2548,19 @@
       <c r="K46" s="12"/>
       <c r="L46" s="12"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" s="7">
-        <v>37</v>
-      </c>
-      <c r="B47" s="8" t="s">
-        <v>36</v>
+        <v>22</v>
+      </c>
+      <c r="B47" s="16" t="s">
+        <v>33</v>
       </c>
       <c r="C47" s="16"/>
       <c r="D47" s="17" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="E47" s="28" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="F47" s="21" t="s">
         <v>28</v>
@@ -2262,47 +2572,47 @@
       <c r="K47" s="12"/>
       <c r="L47" s="12"/>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48" s="7">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C48" s="8"/>
       <c r="D48" s="15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E48" s="28" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="F48" s="21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G48" s="22"/>
       <c r="H48" s="12"/>
       <c r="I48" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J48" s="12"/>
       <c r="K48" s="12"/>
       <c r="L48" s="12"/>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" s="18" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C49" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D49" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="D49" s="15" t="s">
-        <v>41</v>
-      </c>
       <c r="E49" s="28" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="F49" s="21" t="s">
         <v>28</v>
@@ -2314,24 +2624,24 @@
       <c r="K49" s="12"/>
       <c r="L49" s="12"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" s="18" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D50" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E50" s="28" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="F50" s="21" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="G50" s="22"/>
       <c r="H50" s="12"/>
@@ -2340,21 +2650,21 @@
       <c r="K50" s="12"/>
       <c r="L50" s="12"/>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" s="18" t="s">
-        <v>76</v>
+        <v>58</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D51" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E51" s="28" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="F51" s="21" t="s">
         <v>28</v>
@@ -2366,24 +2676,24 @@
       <c r="K51" s="12"/>
       <c r="L51" s="12"/>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52" s="18" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D52" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E52" s="28" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="F52" s="21" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="G52" s="22"/>
       <c r="H52" s="12"/>
@@ -2392,21 +2702,21 @@
       <c r="K52" s="12"/>
       <c r="L52" s="12"/>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53" s="18" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D53" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E53" s="28" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="F53" s="21" t="s">
         <v>28</v>
@@ -2418,24 +2728,24 @@
       <c r="K53" s="12"/>
       <c r="L53" s="12"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" s="18" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D54" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E54" s="28" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="F54" s="21" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="G54" s="22"/>
       <c r="H54" s="12"/>
@@ -2444,22 +2754,22 @@
       <c r="K54" s="12"/>
       <c r="L54" s="12"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55" s="18" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C55" s="8"/>
       <c r="D55" s="15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E55" s="28" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F55" s="21" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="G55" s="22"/>
       <c r="H55" s="12"/>
@@ -2468,21 +2778,21 @@
       <c r="K55" s="12"/>
       <c r="L55" s="12"/>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56" s="18" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D56" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E56" s="28" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="F56" s="21" t="s">
         <v>28</v>
@@ -2494,24 +2804,24 @@
       <c r="K56" s="12"/>
       <c r="L56" s="12"/>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57" s="18" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D57" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E57" s="28" t="s">
-        <v>111</v>
+        <v>96</v>
       </c>
       <c r="F57" s="21" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="G57" s="22"/>
       <c r="H57" s="12"/>
@@ -2520,223 +2830,1154 @@
       <c r="K57" s="12"/>
       <c r="L57" s="12"/>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58" s="7">
+        <v>29</v>
+      </c>
+      <c r="B58" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C58" s="8"/>
+      <c r="D58" s="29" t="s">
+        <v>122</v>
+      </c>
+      <c r="E58" s="30" t="s">
+        <v>195</v>
+      </c>
+      <c r="F58" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G58" s="22"/>
+      <c r="H58" s="12"/>
+      <c r="I58" s="12"/>
+      <c r="J58" s="12"/>
+      <c r="K58" s="12"/>
+      <c r="L58" s="12"/>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A59" s="18" t="s">
+        <v>191</v>
+      </c>
+      <c r="B59" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C59" s="8"/>
+      <c r="D59" s="29" t="s">
+        <v>124</v>
+      </c>
+      <c r="E59" s="30" t="s">
+        <v>196</v>
+      </c>
+      <c r="F59" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G59" s="22"/>
+      <c r="H59" s="12"/>
+      <c r="I59" s="12"/>
+      <c r="J59" s="12"/>
+      <c r="K59" s="12"/>
+      <c r="L59" s="12"/>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A60" s="18" t="s">
+        <v>192</v>
+      </c>
+      <c r="B60" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C60" s="8"/>
+      <c r="D60" s="31" t="s">
+        <v>126</v>
+      </c>
+      <c r="E60" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="F60" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G60" s="22"/>
+      <c r="H60" s="12"/>
+      <c r="I60" s="12"/>
+      <c r="J60" s="12"/>
+      <c r="K60" s="12"/>
+      <c r="L60" s="12"/>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A61" s="18" t="s">
+        <v>193</v>
+      </c>
+      <c r="B61" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C61" s="8"/>
+      <c r="D61" s="29" t="s">
+        <v>128</v>
+      </c>
+      <c r="E61" s="30" t="s">
+        <v>197</v>
+      </c>
+      <c r="F61" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G61" s="22"/>
+      <c r="H61" s="12"/>
+      <c r="I61" s="12"/>
+      <c r="J61" s="12"/>
+      <c r="K61" s="12"/>
+      <c r="L61" s="12"/>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A62" s="18" t="s">
+        <v>194</v>
+      </c>
+      <c r="B62" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C62" s="8"/>
+      <c r="D62" s="29" t="s">
+        <v>130</v>
+      </c>
+      <c r="E62" s="30" t="s">
+        <v>198</v>
+      </c>
+      <c r="F62" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G62" s="22"/>
+      <c r="H62" s="12"/>
+      <c r="I62" s="12"/>
+      <c r="J62" s="12"/>
+      <c r="K62" s="12"/>
+      <c r="L62" s="12"/>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A63" s="7">
+        <v>30</v>
+      </c>
+      <c r="B63" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C63" s="8"/>
+      <c r="D63" s="32" t="s">
+        <v>139</v>
+      </c>
+      <c r="E63" s="30" t="s">
+        <v>202</v>
+      </c>
+      <c r="F63" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G63" s="22"/>
+      <c r="H63" s="12"/>
+      <c r="I63" s="12"/>
+      <c r="J63" s="12"/>
+      <c r="K63" s="12"/>
+      <c r="L63" s="12"/>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A64" s="18" t="s">
+        <v>199</v>
+      </c>
+      <c r="B64" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C64" s="8"/>
+      <c r="D64" s="32" t="s">
+        <v>141</v>
+      </c>
+      <c r="E64" s="30" t="s">
+        <v>203</v>
+      </c>
+      <c r="F64" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G64" s="22"/>
+      <c r="H64" s="12"/>
+      <c r="I64" s="12"/>
+      <c r="J64" s="12"/>
+      <c r="K64" s="12"/>
+      <c r="L64" s="12"/>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A65" s="18" t="s">
+        <v>200</v>
+      </c>
+      <c r="B65" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C65" s="8"/>
+      <c r="D65" s="31" t="s">
+        <v>143</v>
+      </c>
+      <c r="E65" s="30" t="s">
+        <v>144</v>
+      </c>
+      <c r="F65" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G65" s="22"/>
+      <c r="H65" s="12"/>
+      <c r="I65" s="12"/>
+      <c r="J65" s="12"/>
+      <c r="K65" s="12"/>
+      <c r="L65" s="12"/>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A66" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="B66" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C66" s="8"/>
+      <c r="D66" s="31" t="s">
+        <v>145</v>
+      </c>
+      <c r="E66" s="30" t="s">
+        <v>204</v>
+      </c>
+      <c r="F66" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G66" s="22"/>
+      <c r="H66" s="12"/>
+      <c r="I66" s="12"/>
+      <c r="J66" s="12"/>
+      <c r="K66" s="12"/>
+      <c r="L66" s="12"/>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A67" s="7">
+        <v>31</v>
+      </c>
+      <c r="B67" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C67" s="8"/>
+      <c r="D67" s="31" t="s">
+        <v>150</v>
+      </c>
+      <c r="E67" s="30" t="s">
+        <v>208</v>
+      </c>
+      <c r="F67" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G67" s="22"/>
+      <c r="H67" s="12"/>
+      <c r="I67" s="12"/>
+      <c r="J67" s="12"/>
+      <c r="K67" s="12"/>
+      <c r="L67" s="12"/>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A68" s="18" t="s">
+        <v>205</v>
+      </c>
+      <c r="B68" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C68" s="8"/>
+      <c r="D68" s="31" t="s">
+        <v>152</v>
+      </c>
+      <c r="E68" s="30" t="s">
+        <v>209</v>
+      </c>
+      <c r="F68" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G68" s="22"/>
+      <c r="H68" s="12"/>
+      <c r="I68" s="12"/>
+      <c r="J68" s="12"/>
+      <c r="K68" s="12"/>
+      <c r="L68" s="12"/>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A69" s="18" t="s">
+        <v>206</v>
+      </c>
+      <c r="B69" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C69" s="8"/>
+      <c r="D69" s="31" t="s">
+        <v>154</v>
+      </c>
+      <c r="E69" s="30" t="s">
+        <v>155</v>
+      </c>
+      <c r="F69" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G69" s="22"/>
+      <c r="H69" s="12"/>
+      <c r="I69" s="12"/>
+      <c r="J69" s="12"/>
+      <c r="K69" s="12"/>
+      <c r="L69" s="12"/>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A70" s="18" t="s">
+        <v>207</v>
+      </c>
+      <c r="B70" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C70" s="8"/>
+      <c r="D70" s="31" t="s">
+        <v>156</v>
+      </c>
+      <c r="E70" s="30" t="s">
+        <v>210</v>
+      </c>
+      <c r="F70" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G70" s="22"/>
+      <c r="H70" s="12"/>
+      <c r="I70" s="12"/>
+      <c r="J70" s="12"/>
+      <c r="K70" s="12"/>
+      <c r="L70" s="12"/>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A71" s="7">
+        <v>32</v>
+      </c>
+      <c r="B71" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C71" s="8"/>
+      <c r="D71" s="31" t="s">
+        <v>161</v>
+      </c>
+      <c r="E71" s="30" t="s">
+        <v>214</v>
+      </c>
+      <c r="F71" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G71" s="22"/>
+      <c r="H71" s="12"/>
+      <c r="I71" s="12"/>
+      <c r="J71" s="12"/>
+      <c r="K71" s="12"/>
+      <c r="L71" s="12"/>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A72" s="18" t="s">
+        <v>211</v>
+      </c>
+      <c r="B72" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C72" s="8"/>
+      <c r="D72" s="31" t="s">
+        <v>163</v>
+      </c>
+      <c r="E72" s="30" t="s">
+        <v>215</v>
+      </c>
+      <c r="F72" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G72" s="22"/>
+      <c r="H72" s="12"/>
+      <c r="I72" s="12"/>
+      <c r="J72" s="12"/>
+      <c r="K72" s="12"/>
+      <c r="L72" s="12"/>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A73" s="18" t="s">
+        <v>212</v>
+      </c>
+      <c r="B73" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C73" s="8"/>
+      <c r="D73" s="31" t="s">
+        <v>165</v>
+      </c>
+      <c r="E73" s="30" t="s">
+        <v>166</v>
+      </c>
+      <c r="F73" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G73" s="22"/>
+      <c r="H73" s="12"/>
+      <c r="I73" s="12"/>
+      <c r="J73" s="12"/>
+      <c r="K73" s="12"/>
+      <c r="L73" s="12"/>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A74" s="18" t="s">
+        <v>213</v>
+      </c>
+      <c r="B74" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C74" s="8"/>
+      <c r="D74" s="31" t="s">
+        <v>167</v>
+      </c>
+      <c r="E74" s="30" t="s">
+        <v>216</v>
+      </c>
+      <c r="F74" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G74" s="22"/>
+      <c r="H74" s="12"/>
+      <c r="I74" s="12"/>
+      <c r="J74" s="12"/>
+      <c r="K74" s="12"/>
+      <c r="L74" s="12"/>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A75" s="7">
+        <v>33</v>
+      </c>
+      <c r="B75" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C75" s="8"/>
+      <c r="D75" s="31" t="s">
+        <v>172</v>
+      </c>
+      <c r="E75" s="30" t="s">
+        <v>217</v>
+      </c>
+      <c r="F75" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G75" s="22"/>
+      <c r="H75" s="12"/>
+      <c r="I75" s="12"/>
+      <c r="J75" s="12"/>
+      <c r="K75" s="12"/>
+      <c r="L75" s="12"/>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A76" s="18" t="s">
+        <v>223</v>
+      </c>
+      <c r="B76" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C76" s="8"/>
+      <c r="D76" s="31" t="s">
+        <v>174</v>
+      </c>
+      <c r="E76" s="30" t="s">
+        <v>218</v>
+      </c>
+      <c r="F76" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G76" s="22"/>
+      <c r="H76" s="12"/>
+      <c r="I76" s="12"/>
+      <c r="J76" s="12"/>
+      <c r="K76" s="12"/>
+      <c r="L76" s="12"/>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A77" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="B77" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C77" s="8"/>
+      <c r="D77" s="31" t="s">
+        <v>176</v>
+      </c>
+      <c r="E77" s="30" t="s">
+        <v>177</v>
+      </c>
+      <c r="F77" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G77" s="22"/>
+      <c r="H77" s="12"/>
+      <c r="I77" s="12"/>
+      <c r="J77" s="12"/>
+      <c r="K77" s="12"/>
+      <c r="L77" s="12"/>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A78" s="18" t="s">
+        <v>225</v>
+      </c>
+      <c r="B78" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C78" s="8"/>
+      <c r="D78" s="31" t="s">
+        <v>178</v>
+      </c>
+      <c r="E78" s="30" t="s">
+        <v>219</v>
+      </c>
+      <c r="F78" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G78" s="22"/>
+      <c r="H78" s="12"/>
+      <c r="I78" s="12"/>
+      <c r="J78" s="12"/>
+      <c r="K78" s="12"/>
+      <c r="L78" s="12"/>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A79" s="7">
+        <v>34</v>
+      </c>
+      <c r="B79" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C79" s="8"/>
+      <c r="D79" s="31" t="s">
+        <v>183</v>
+      </c>
+      <c r="E79" s="30" t="s">
+        <v>220</v>
+      </c>
+      <c r="F79" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G79" s="22"/>
+      <c r="H79" s="12"/>
+      <c r="I79" s="12"/>
+      <c r="J79" s="12"/>
+      <c r="K79" s="12"/>
+      <c r="L79" s="12"/>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A80" s="18" t="s">
+        <v>226</v>
+      </c>
+      <c r="B80" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C80" s="8"/>
+      <c r="D80" s="31" t="s">
+        <v>185</v>
+      </c>
+      <c r="E80" s="30" t="s">
+        <v>221</v>
+      </c>
+      <c r="F80" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G80" s="22"/>
+      <c r="H80" s="12"/>
+      <c r="I80" s="12"/>
+      <c r="J80" s="12"/>
+      <c r="K80" s="12"/>
+      <c r="L80" s="12"/>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A81" s="18" t="s">
+        <v>227</v>
+      </c>
+      <c r="B81" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C81" s="8"/>
+      <c r="D81" s="31" t="s">
+        <v>187</v>
+      </c>
+      <c r="E81" s="30" t="s">
+        <v>188</v>
+      </c>
+      <c r="F81" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G81" s="22"/>
+      <c r="H81" s="12"/>
+      <c r="I81" s="12"/>
+      <c r="J81" s="12"/>
+      <c r="K81" s="12"/>
+      <c r="L81" s="12"/>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A82" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="B82" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C82" s="8"/>
+      <c r="D82" s="31" t="s">
+        <v>189</v>
+      </c>
+      <c r="E82" s="30" t="s">
+        <v>222</v>
+      </c>
+      <c r="F82" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G82" s="22"/>
+      <c r="H82" s="12"/>
+      <c r="I82" s="12"/>
+      <c r="J82" s="12"/>
+      <c r="K82" s="12"/>
+      <c r="L82" s="12"/>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A83" s="7">
+        <v>35</v>
+      </c>
+      <c r="B83" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C83" s="8"/>
+      <c r="D83" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="E83" s="28" t="s">
+        <v>97</v>
+      </c>
+      <c r="F83" s="21" t="s">
+        <v>120</v>
+      </c>
+      <c r="G83" s="22"/>
+      <c r="H83" s="12"/>
+      <c r="I83" s="12"/>
+      <c r="J83" s="12"/>
+      <c r="K83" s="12"/>
+      <c r="L83" s="12"/>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A84" s="7">
+        <v>36</v>
+      </c>
+      <c r="B84" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C84" s="16"/>
+      <c r="D84" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="E84" s="28" t="s">
+        <v>88</v>
+      </c>
+      <c r="F84" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G84" s="22"/>
+      <c r="H84" s="12"/>
+      <c r="I84" s="12"/>
+      <c r="J84" s="12"/>
+      <c r="K84" s="12"/>
+      <c r="L84" s="12"/>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A85" s="7">
+        <v>37</v>
+      </c>
+      <c r="B85" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C85" s="16"/>
+      <c r="D85" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="E85" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="F85" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G85" s="22"/>
+      <c r="H85" s="12"/>
+      <c r="I85" s="12"/>
+      <c r="J85" s="12"/>
+      <c r="K85" s="12"/>
+      <c r="L85" s="12"/>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A86" s="7">
+        <v>38</v>
+      </c>
+      <c r="B86" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C86" s="8"/>
+      <c r="D86" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="E86" s="28" t="s">
+        <v>90</v>
+      </c>
+      <c r="F86" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="G86" s="22"/>
+      <c r="H86" s="12"/>
+      <c r="I86" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="J86" s="12"/>
+      <c r="K86" s="12"/>
+      <c r="L86" s="12"/>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A87" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B87" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C87" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D87" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="E87" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="F87" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G87" s="22"/>
+      <c r="H87" s="12"/>
+      <c r="I87" s="12"/>
+      <c r="J87" s="12"/>
+      <c r="K87" s="12"/>
+      <c r="L87" s="12"/>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A88" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="B88" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C88" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D88" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="E88" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="F88" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="G88" s="22"/>
+      <c r="H88" s="12"/>
+      <c r="I88" s="12"/>
+      <c r="J88" s="12"/>
+      <c r="K88" s="12"/>
+      <c r="L88" s="12"/>
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A89" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="B89" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C89" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="B58" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C58" s="8"/>
-      <c r="D58" s="15" t="s">
+      <c r="D89" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="E89" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="F89" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G89" s="22"/>
+      <c r="H89" s="12"/>
+      <c r="I89" s="12"/>
+      <c r="J89" s="12"/>
+      <c r="K89" s="12"/>
+      <c r="L89" s="12"/>
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A90" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="B90" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C90" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D90" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="E90" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="F90" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="G90" s="22"/>
+      <c r="H90" s="12"/>
+      <c r="I90" s="12"/>
+      <c r="J90" s="12"/>
+      <c r="K90" s="12"/>
+      <c r="L90" s="12"/>
+    </row>
+    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A91" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="B91" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C91" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D91" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="E91" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="F91" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G91" s="22"/>
+      <c r="H91" s="12"/>
+      <c r="I91" s="12"/>
+      <c r="J91" s="12"/>
+      <c r="K91" s="12"/>
+      <c r="L91" s="12"/>
+    </row>
+    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A92" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="B92" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C92" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D92" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="E92" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="F92" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="G92" s="22"/>
+      <c r="H92" s="12"/>
+      <c r="I92" s="12"/>
+      <c r="J92" s="12"/>
+      <c r="K92" s="12"/>
+      <c r="L92" s="12"/>
+    </row>
+    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A93" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="B93" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C93" s="8"/>
+      <c r="D93" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="E93" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="F93" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="G93" s="22"/>
+      <c r="H93" s="12"/>
+      <c r="I93" s="12"/>
+      <c r="J93" s="12"/>
+      <c r="K93" s="12"/>
+      <c r="L93" s="12"/>
+    </row>
+    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A94" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="B94" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C94" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D94" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="E94" s="28" t="s">
+        <v>118</v>
+      </c>
+      <c r="F94" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G94" s="22"/>
+      <c r="H94" s="12"/>
+      <c r="I94" s="12"/>
+      <c r="J94" s="12"/>
+      <c r="K94" s="12"/>
+      <c r="L94" s="12"/>
+    </row>
+    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A95" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="B95" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C95" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D95" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="E95" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="F95" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="G95" s="22"/>
+      <c r="H95" s="12"/>
+      <c r="I95" s="12"/>
+      <c r="J95" s="12"/>
+      <c r="K95" s="12"/>
+      <c r="L95" s="12"/>
+    </row>
+    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A96" s="7">
+        <v>44</v>
+      </c>
+      <c r="B96" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C96" s="8"/>
+      <c r="D96" s="29" t="s">
+        <v>124</v>
+      </c>
+      <c r="E96" s="30" t="s">
+        <v>229</v>
+      </c>
+      <c r="F96" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G96" s="22"/>
+      <c r="H96" s="19"/>
+      <c r="I96" s="19"/>
+      <c r="J96" s="19"/>
+      <c r="K96" s="19"/>
+      <c r="L96" s="19"/>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A97" s="7">
+        <v>45</v>
+      </c>
+      <c r="B97" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C97" s="8"/>
+      <c r="D97" s="32" t="s">
+        <v>141</v>
+      </c>
+      <c r="E97" s="30" t="s">
+        <v>230</v>
+      </c>
+      <c r="F97" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G97" s="22"/>
+      <c r="H97" s="19"/>
+      <c r="I97" s="19"/>
+      <c r="J97" s="19"/>
+      <c r="K97" s="19"/>
+      <c r="L97" s="19"/>
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A98" s="7">
+        <v>46</v>
+      </c>
+      <c r="B98" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C98" s="8"/>
+      <c r="D98" s="31" t="s">
+        <v>152</v>
+      </c>
+      <c r="E98" s="30" t="s">
+        <v>231</v>
+      </c>
+      <c r="F98" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G98" s="22"/>
+      <c r="H98" s="19"/>
+      <c r="I98" s="19"/>
+      <c r="J98" s="19"/>
+      <c r="K98" s="19"/>
+      <c r="L98" s="19"/>
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A99" s="7">
+        <v>47</v>
+      </c>
+      <c r="B99" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C99" s="8"/>
+      <c r="D99" s="31" t="s">
+        <v>163</v>
+      </c>
+      <c r="E99" s="30" t="s">
+        <v>232</v>
+      </c>
+      <c r="F99" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G99" s="22"/>
+      <c r="H99" s="19"/>
+      <c r="I99" s="19"/>
+      <c r="J99" s="19"/>
+      <c r="K99" s="19"/>
+      <c r="L99" s="19"/>
+    </row>
+    <row r="100" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A100" s="7">
+        <v>48</v>
+      </c>
+      <c r="B100" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C100" s="8"/>
+      <c r="D100" s="31" t="s">
+        <v>174</v>
+      </c>
+      <c r="E100" s="30" t="s">
+        <v>233</v>
+      </c>
+      <c r="F100" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G100" s="22"/>
+      <c r="H100" s="19"/>
+      <c r="I100" s="19"/>
+      <c r="J100" s="19"/>
+      <c r="K100" s="19"/>
+      <c r="L100" s="19"/>
+    </row>
+    <row r="101" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A101" s="7">
+        <v>49</v>
+      </c>
+      <c r="B101" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C101" s="8"/>
+      <c r="D101" s="31" t="s">
+        <v>185</v>
+      </c>
+      <c r="E101" s="30" t="s">
+        <v>234</v>
+      </c>
+      <c r="F101" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G101" s="22"/>
+      <c r="H101" s="19"/>
+      <c r="I101" s="19"/>
+      <c r="J101" s="19"/>
+      <c r="K101" s="19"/>
+      <c r="L101" s="19"/>
+    </row>
+    <row r="102" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A102" s="7">
+        <v>50</v>
+      </c>
+      <c r="B102" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C102" s="8"/>
+      <c r="D102" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="E102" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="F102" s="21" t="s">
+        <v>120</v>
+      </c>
+      <c r="G102" s="22"/>
+      <c r="H102" s="19"/>
+      <c r="I102" s="19"/>
+      <c r="J102" s="19"/>
+      <c r="K102" s="19"/>
+      <c r="L102" s="19"/>
+    </row>
+    <row r="103" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A103" s="7">
+        <v>51</v>
+      </c>
+      <c r="B103" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C103" s="16"/>
+      <c r="D103" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="E58" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="F58" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="G58" s="22"/>
-      <c r="H58" s="19"/>
-      <c r="I58" s="19"/>
-      <c r="J58" s="19"/>
-      <c r="K58" s="19"/>
-      <c r="L58" s="19"/>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A59" s="7">
-        <v>45</v>
-      </c>
-      <c r="B59" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C59" s="8"/>
-      <c r="D59" s="15" t="s">
+      <c r="E103" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="F103" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G103" s="22"/>
+      <c r="H103" s="19"/>
+      <c r="I103" s="19"/>
+      <c r="J103" s="19"/>
+      <c r="K103" s="19"/>
+      <c r="L103" s="19"/>
+    </row>
+    <row r="104" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A104" s="7">
+        <v>52</v>
+      </c>
+      <c r="B104" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C104" s="16"/>
+      <c r="D104" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="E59" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="F59" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="G59" s="22"/>
-      <c r="H59" s="19"/>
-      <c r="I59" s="19"/>
-      <c r="J59" s="19"/>
-      <c r="K59" s="19"/>
-      <c r="L59" s="19"/>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A60" s="7">
-        <v>46</v>
-      </c>
-      <c r="B60" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C60" s="8"/>
-      <c r="D60" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="E60" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="F60" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="G60" s="22"/>
-      <c r="H60" s="19"/>
-      <c r="I60" s="19"/>
-      <c r="J60" s="19"/>
-      <c r="K60" s="19"/>
-      <c r="L60" s="19"/>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A61" s="7">
-        <v>47</v>
-      </c>
-      <c r="B61" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C61" s="8"/>
-      <c r="D61" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="E61" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="F61" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="G61" s="22"/>
-      <c r="H61" s="19"/>
-      <c r="I61" s="19"/>
-      <c r="J61" s="19"/>
-      <c r="K61" s="19"/>
-      <c r="L61" s="19"/>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A62" s="7">
-        <v>48</v>
-      </c>
-      <c r="B62" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C62" s="8"/>
-      <c r="D62" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="E62" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="F62" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="G62" s="22"/>
-      <c r="H62" s="19"/>
-      <c r="I62" s="19"/>
-      <c r="J62" s="19"/>
-      <c r="K62" s="19"/>
-      <c r="L62" s="19"/>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A63" s="7">
-        <v>49</v>
-      </c>
-      <c r="B63" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C63" s="8"/>
-      <c r="D63" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="E63" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="F63" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="G63" s="22"/>
-      <c r="H63" s="19"/>
-      <c r="I63" s="19"/>
-      <c r="J63" s="19"/>
-      <c r="K63" s="19"/>
-      <c r="L63" s="19"/>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A64" s="7">
-        <v>50</v>
-      </c>
-      <c r="B64" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C64" s="8"/>
-      <c r="D64" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="E64" s="28" t="s">
-        <v>98</v>
-      </c>
-      <c r="F64" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="G64" s="22"/>
-      <c r="H64" s="19"/>
-      <c r="I64" s="19"/>
-      <c r="J64" s="19"/>
-      <c r="K64" s="19"/>
-      <c r="L64" s="19"/>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A65" s="7">
-        <v>51</v>
-      </c>
-      <c r="B65" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C65" s="16"/>
-      <c r="D65" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="E65" s="28" t="s">
-        <v>100</v>
-      </c>
-      <c r="F65" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="G65" s="22"/>
-      <c r="H65" s="19"/>
-      <c r="I65" s="19"/>
-      <c r="J65" s="19"/>
-      <c r="K65" s="19"/>
-      <c r="L65" s="19"/>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A66" s="7">
-        <v>52</v>
-      </c>
-      <c r="B66" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C66" s="16"/>
-      <c r="D66" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="E66" s="28" t="s">
-        <v>101</v>
-      </c>
-      <c r="F66" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="G66" s="22"/>
-      <c r="H66" s="19"/>
-      <c r="I66" s="19"/>
-      <c r="J66" s="19"/>
-      <c r="K66" s="19"/>
-      <c r="L66" s="19"/>
+      <c r="E104" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="F104" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G104" s="22"/>
+      <c r="H104" s="19"/>
+      <c r="I104" s="19"/>
+      <c r="J104" s="19"/>
+      <c r="K104" s="19"/>
+      <c r="L104" s="19"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Tested changes in SingleSelectComponent.kt
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/euTaxonomyNonFinancials/EutaxonomyNonFinancials.xlsx
+++ b/dataland-framework-toolbox/inputs/euTaxonomyNonFinancials/EutaxonomyNonFinancials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d93476\Dataland\dataland-framework-toolbox\inputs\euTaxonomyNonFinancials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74961600-956F-455B-B137-8E5A191190B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7387AC29-C78D-42C7-81C5-A3856B3BB672}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="128">
   <si>
     <t>Field Identifier</t>
   </si>
@@ -1063,7 +1063,7 @@
   <dimension ref="A1:L66"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1135,7 +1135,9 @@
         <v>85</v>
       </c>
       <c r="H2" s="11"/>
-      <c r="I2" s="12"/>
+      <c r="I2" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="J2" s="12"/>
       <c r="K2" s="12"/>
       <c r="L2" s="12"/>

</xml_diff>

<commit_message>
Dala 4606 adapt eu taxonomy model (#638)
Introduce extended data points for EU-Taxonomy non-financials

Co-authored-by: d93476 <jakob.kraus@d-fine.com>
Co-authored-by: swaldow <stephan.waldow@d-fine.de>
Co-authored-by: MarcTM01 <marc@marctm.com>
Co-authored-by: SiegfriedSobkowiak <siegfried.sobkowiak@d-fine.de>
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/euTaxonomyNonFinancials/EutaxonomyNonFinancials.xlsx
+++ b/dataland-framework-toolbox/inputs/euTaxonomyNonFinancials/EutaxonomyNonFinancials.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d92048\IdeaProjects\Dataland5\dataland-framework-toolbox\inputs\euTaxonomyNonFinancials\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d93476\Dataland\dataland-framework-toolbox\inputs\euTaxonomyNonFinancials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9190097E-1C69-4385-816A-3AC5DD386F05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7387AC29-C78D-42C7-81C5-A3856B3BB672}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Framework Data Model" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Framework Data Model'!$A$1:$L$66</definedName>
     <definedName name="IQ_CH">110000</definedName>
     <definedName name="IQ_CQ">5000</definedName>
     <definedName name="IQ_CY">10000</definedName>
@@ -57,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="128">
   <si>
     <t>Field Identifier</t>
   </si>
@@ -441,9 +442,6 @@
   </si>
   <si>
     <t>Custom EuTaxonomyAlignedActivitiesComponent</t>
-  </si>
-  <si>
-    <t>AmountWithCurrencyComponent</t>
   </si>
 </sst>
 </file>
@@ -1064,21 +1062,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D46" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F57" sqref="F57"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="20.1796875" customWidth="1"/>
-    <col min="4" max="4" width="70.36328125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="77.90625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="44.6328125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="26.1796875" customWidth="1"/>
-    <col min="8" max="12" width="14.36328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.21875" customWidth="1"/>
+    <col min="4" max="4" width="70.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="77.88671875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="44.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="26.21875" customWidth="1"/>
+    <col min="8" max="12" width="14.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1116,7 +1114,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="7">
         <v>0</v>
       </c>
@@ -1137,12 +1135,14 @@
         <v>85</v>
       </c>
       <c r="H2" s="11"/>
-      <c r="I2" s="12"/>
+      <c r="I2" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="J2" s="12"/>
       <c r="K2" s="12"/>
       <c r="L2" s="12"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="7"/>
       <c r="B3" s="8" t="s">
         <v>12</v>
@@ -1159,12 +1159,14 @@
       </c>
       <c r="G3" s="10"/>
       <c r="H3" s="11"/>
-      <c r="I3" s="12"/>
+      <c r="I3" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="J3" s="12"/>
       <c r="K3" s="12"/>
       <c r="L3" s="12"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>1</v>
       </c>
@@ -1185,12 +1187,14 @@
         <v>14</v>
       </c>
       <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
+      <c r="I4" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="J4" s="11"/>
       <c r="K4" s="11"/>
       <c r="L4" s="12"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>2</v>
       </c>
@@ -1211,12 +1215,14 @@
         <v>14</v>
       </c>
       <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
+      <c r="I5" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="J5" s="12"/>
       <c r="K5" s="12"/>
       <c r="L5" s="12"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>3</v>
       </c>
@@ -1237,12 +1243,14 @@
         <v>14</v>
       </c>
       <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
+      <c r="I6" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="J6" s="12"/>
       <c r="K6" s="12"/>
       <c r="L6" s="12"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>4</v>
       </c>
@@ -1268,7 +1276,7 @@
       <c r="K7" s="12"/>
       <c r="L7" s="12"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>5</v>
       </c>
@@ -1287,12 +1295,14 @@
       </c>
       <c r="G8" s="22"/>
       <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
+      <c r="I8" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="J8" s="12"/>
       <c r="K8" s="12"/>
       <c r="L8" s="12"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>6</v>
       </c>
@@ -1316,7 +1326,7 @@
       <c r="K9" s="12"/>
       <c r="L9" s="12"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>8</v>
       </c>
@@ -1342,7 +1352,7 @@
       <c r="K10" s="12"/>
       <c r="L10" s="12"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="18" t="s">
         <v>43</v>
       </c>
@@ -1361,12 +1371,14 @@
       </c>
       <c r="G11" s="22"/>
       <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
+      <c r="I11" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="J11" s="12"/>
       <c r="K11" s="12"/>
       <c r="L11" s="12"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="18" t="s">
         <v>44</v>
       </c>
@@ -1383,16 +1395,18 @@
         <v>91</v>
       </c>
       <c r="F12" s="21" t="s">
-        <v>128</v>
+        <v>38</v>
       </c>
       <c r="G12" s="22"/>
       <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
+      <c r="I12" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="J12" s="12"/>
       <c r="K12" s="12"/>
       <c r="L12" s="12"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="18" t="s">
         <v>46</v>
       </c>
@@ -1413,12 +1427,14 @@
       </c>
       <c r="G13" s="22"/>
       <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
+      <c r="I13" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="J13" s="12"/>
       <c r="K13" s="12"/>
       <c r="L13" s="12"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="18" t="s">
         <v>47</v>
       </c>
@@ -1435,16 +1451,18 @@
         <v>114</v>
       </c>
       <c r="F14" s="21" t="s">
-        <v>128</v>
+        <v>38</v>
       </c>
       <c r="G14" s="22"/>
       <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
+      <c r="I14" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="J14" s="12"/>
       <c r="K14" s="12"/>
       <c r="L14" s="12"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="18" t="s">
         <v>49</v>
       </c>
@@ -1465,12 +1483,14 @@
       </c>
       <c r="G15" s="22"/>
       <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
+      <c r="I15" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="J15" s="12"/>
       <c r="K15" s="12"/>
       <c r="L15" s="12"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="18" t="s">
         <v>50</v>
       </c>
@@ -1487,16 +1507,18 @@
         <v>113</v>
       </c>
       <c r="F16" s="21" t="s">
-        <v>128</v>
+        <v>38</v>
       </c>
       <c r="G16" s="22"/>
       <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
+      <c r="I16" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="J16" s="12"/>
       <c r="K16" s="12"/>
       <c r="L16" s="12"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="18" t="s">
         <v>62</v>
       </c>
@@ -1520,7 +1542,7 @@
       <c r="K17" s="12"/>
       <c r="L17" s="12"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="18" t="s">
         <v>63</v>
       </c>
@@ -1541,12 +1563,14 @@
       </c>
       <c r="G18" s="22"/>
       <c r="H18" s="12"/>
-      <c r="I18" s="12"/>
+      <c r="I18" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="J18" s="12"/>
       <c r="K18" s="12"/>
       <c r="L18" s="12"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="18" t="s">
         <v>64</v>
       </c>
@@ -1563,16 +1587,18 @@
         <v>112</v>
       </c>
       <c r="F19" s="21" t="s">
-        <v>128</v>
+        <v>38</v>
       </c>
       <c r="G19" s="22"/>
       <c r="H19" s="12"/>
-      <c r="I19" s="12"/>
+      <c r="I19" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="J19" s="12"/>
       <c r="K19" s="12"/>
       <c r="L19" s="12"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="7">
         <v>14</v>
       </c>
@@ -1591,12 +1617,14 @@
       </c>
       <c r="G20" s="22"/>
       <c r="H20" s="12"/>
-      <c r="I20" s="12"/>
+      <c r="I20" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="J20" s="12"/>
       <c r="K20" s="12"/>
       <c r="L20" s="12"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="7">
         <v>15</v>
       </c>
@@ -1615,12 +1643,14 @@
       </c>
       <c r="G21" s="22"/>
       <c r="H21" s="12"/>
-      <c r="I21" s="12"/>
+      <c r="I21" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="J21" s="12"/>
       <c r="K21" s="12"/>
       <c r="L21" s="12"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="7">
         <v>16</v>
       </c>
@@ -1639,12 +1669,14 @@
       </c>
       <c r="G22" s="22"/>
       <c r="H22" s="12"/>
-      <c r="I22" s="12"/>
+      <c r="I22" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="J22" s="12"/>
       <c r="K22" s="12"/>
       <c r="L22" s="12"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="7">
         <v>17</v>
       </c>
@@ -1663,12 +1695,14 @@
       </c>
       <c r="G23" s="22"/>
       <c r="H23" s="12"/>
-      <c r="I23" s="12"/>
+      <c r="I23" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="J23" s="12"/>
       <c r="K23" s="12"/>
       <c r="L23" s="12"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="7">
         <v>18</v>
       </c>
@@ -1687,12 +1721,14 @@
       </c>
       <c r="G24" s="22"/>
       <c r="H24" s="12"/>
-      <c r="I24" s="12"/>
+      <c r="I24" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="J24" s="12"/>
       <c r="K24" s="12"/>
       <c r="L24" s="12"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="7">
         <v>19</v>
       </c>
@@ -1711,12 +1747,14 @@
       </c>
       <c r="G25" s="22"/>
       <c r="H25" s="12"/>
-      <c r="I25" s="12"/>
+      <c r="I25" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="J25" s="12"/>
       <c r="K25" s="12"/>
       <c r="L25" s="12"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="7">
         <v>20</v>
       </c>
@@ -1740,7 +1778,7 @@
       <c r="K26" s="12"/>
       <c r="L26" s="12"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="7">
         <v>21</v>
       </c>
@@ -1759,12 +1797,14 @@
       </c>
       <c r="G27" s="22"/>
       <c r="H27" s="12"/>
-      <c r="I27" s="12"/>
+      <c r="I27" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="J27" s="12"/>
       <c r="K27" s="12"/>
       <c r="L27" s="12"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="7">
         <v>22</v>
       </c>
@@ -1783,12 +1823,14 @@
       </c>
       <c r="G28" s="22"/>
       <c r="H28" s="12"/>
-      <c r="I28" s="12"/>
+      <c r="I28" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="J28" s="12"/>
       <c r="K28" s="12"/>
       <c r="L28" s="12"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="7">
         <v>23</v>
       </c>
@@ -1814,7 +1856,7 @@
       <c r="K29" s="12"/>
       <c r="L29" s="12"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="18" t="s">
         <v>67</v>
       </c>
@@ -1835,12 +1877,14 @@
       </c>
       <c r="G30" s="22"/>
       <c r="H30" s="12"/>
-      <c r="I30" s="12"/>
+      <c r="I30" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="J30" s="12"/>
       <c r="K30" s="12"/>
       <c r="L30" s="12"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="18" t="s">
         <v>68</v>
       </c>
@@ -1857,16 +1901,18 @@
         <v>107</v>
       </c>
       <c r="F31" s="21" t="s">
-        <v>128</v>
+        <v>38</v>
       </c>
       <c r="G31" s="22"/>
       <c r="H31" s="12"/>
-      <c r="I31" s="12"/>
+      <c r="I31" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="J31" s="12"/>
       <c r="K31" s="12"/>
       <c r="L31" s="12"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="18" t="s">
         <v>65</v>
       </c>
@@ -1887,12 +1933,14 @@
       </c>
       <c r="G32" s="22"/>
       <c r="H32" s="12"/>
-      <c r="I32" s="12"/>
+      <c r="I32" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="J32" s="12"/>
       <c r="K32" s="12"/>
       <c r="L32" s="12"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" s="18" t="s">
         <v>66</v>
       </c>
@@ -1909,16 +1957,18 @@
         <v>102</v>
       </c>
       <c r="F33" s="21" t="s">
-        <v>128</v>
+        <v>38</v>
       </c>
       <c r="G33" s="22"/>
       <c r="H33" s="12"/>
-      <c r="I33" s="12"/>
+      <c r="I33" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="J33" s="12"/>
       <c r="K33" s="12"/>
       <c r="L33" s="12"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" s="18" t="s">
         <v>69</v>
       </c>
@@ -1939,12 +1989,14 @@
       </c>
       <c r="G34" s="22"/>
       <c r="H34" s="12"/>
-      <c r="I34" s="12"/>
+      <c r="I34" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="J34" s="12"/>
       <c r="K34" s="12"/>
       <c r="L34" s="12"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" s="18" t="s">
         <v>70</v>
       </c>
@@ -1961,16 +2013,18 @@
         <v>106</v>
       </c>
       <c r="F35" s="21" t="s">
-        <v>128</v>
+        <v>38</v>
       </c>
       <c r="G35" s="22"/>
       <c r="H35" s="12"/>
-      <c r="I35" s="12"/>
+      <c r="I35" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="J35" s="12"/>
       <c r="K35" s="12"/>
       <c r="L35" s="12"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" s="18" t="s">
         <v>71</v>
       </c>
@@ -1994,7 +2048,7 @@
       <c r="K36" s="12"/>
       <c r="L36" s="12"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" s="18" t="s">
         <v>72</v>
       </c>
@@ -2015,12 +2069,14 @@
       </c>
       <c r="G37" s="22"/>
       <c r="H37" s="12"/>
-      <c r="I37" s="12"/>
+      <c r="I37" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="J37" s="12"/>
       <c r="K37" s="12"/>
       <c r="L37" s="12"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" s="18" t="s">
         <v>73</v>
       </c>
@@ -2037,16 +2093,18 @@
         <v>103</v>
       </c>
       <c r="F38" s="21" t="s">
-        <v>128</v>
+        <v>38</v>
       </c>
       <c r="G38" s="22"/>
       <c r="H38" s="12"/>
-      <c r="I38" s="12"/>
+      <c r="I38" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="J38" s="12"/>
       <c r="K38" s="12"/>
       <c r="L38" s="12"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" s="7">
         <v>29</v>
       </c>
@@ -2065,12 +2123,14 @@
       </c>
       <c r="G39" s="22"/>
       <c r="H39" s="12"/>
-      <c r="I39" s="12"/>
+      <c r="I39" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="J39" s="12"/>
       <c r="K39" s="12"/>
       <c r="L39" s="12"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" s="7">
         <v>30</v>
       </c>
@@ -2089,12 +2149,14 @@
       </c>
       <c r="G40" s="22"/>
       <c r="H40" s="12"/>
-      <c r="I40" s="12"/>
+      <c r="I40" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="J40" s="12"/>
       <c r="K40" s="12"/>
       <c r="L40" s="12"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" s="7">
         <v>31</v>
       </c>
@@ -2113,12 +2175,14 @@
       </c>
       <c r="G41" s="22"/>
       <c r="H41" s="12"/>
-      <c r="I41" s="12"/>
+      <c r="I41" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="J41" s="12"/>
       <c r="K41" s="12"/>
       <c r="L41" s="12"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" s="7">
         <v>32</v>
       </c>
@@ -2137,12 +2201,14 @@
       </c>
       <c r="G42" s="22"/>
       <c r="H42" s="12"/>
-      <c r="I42" s="12"/>
+      <c r="I42" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="J42" s="12"/>
       <c r="K42" s="12"/>
       <c r="L42" s="12"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" s="7">
         <v>33</v>
       </c>
@@ -2161,12 +2227,14 @@
       </c>
       <c r="G43" s="22"/>
       <c r="H43" s="12"/>
-      <c r="I43" s="12"/>
+      <c r="I43" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="J43" s="12"/>
       <c r="K43" s="12"/>
       <c r="L43" s="12"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" s="7">
         <v>34</v>
       </c>
@@ -2185,12 +2253,14 @@
       </c>
       <c r="G44" s="22"/>
       <c r="H44" s="12"/>
-      <c r="I44" s="12"/>
+      <c r="I44" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="J44" s="12"/>
       <c r="K44" s="12"/>
       <c r="L44" s="12"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" s="7">
         <v>35</v>
       </c>
@@ -2214,7 +2284,7 @@
       <c r="K45" s="12"/>
       <c r="L45" s="12"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" s="7">
         <v>36</v>
       </c>
@@ -2233,12 +2303,14 @@
       </c>
       <c r="G46" s="22"/>
       <c r="H46" s="12"/>
-      <c r="I46" s="12"/>
+      <c r="I46" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="J46" s="12"/>
       <c r="K46" s="12"/>
       <c r="L46" s="12"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" s="7">
         <v>37</v>
       </c>
@@ -2257,12 +2329,14 @@
       </c>
       <c r="G47" s="22"/>
       <c r="H47" s="12"/>
-      <c r="I47" s="12"/>
+      <c r="I47" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="J47" s="12"/>
       <c r="K47" s="12"/>
       <c r="L47" s="12"/>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48" s="7">
         <v>38</v>
       </c>
@@ -2288,7 +2362,7 @@
       <c r="K48" s="12"/>
       <c r="L48" s="12"/>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" s="18" t="s">
         <v>74</v>
       </c>
@@ -2309,12 +2383,14 @@
       </c>
       <c r="G49" s="22"/>
       <c r="H49" s="12"/>
-      <c r="I49" s="12"/>
+      <c r="I49" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="J49" s="12"/>
       <c r="K49" s="12"/>
       <c r="L49" s="12"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" s="18" t="s">
         <v>75</v>
       </c>
@@ -2331,16 +2407,18 @@
         <v>108</v>
       </c>
       <c r="F50" s="21" t="s">
-        <v>128</v>
+        <v>38</v>
       </c>
       <c r="G50" s="22"/>
       <c r="H50" s="12"/>
-      <c r="I50" s="12"/>
+      <c r="I50" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="J50" s="12"/>
       <c r="K50" s="12"/>
       <c r="L50" s="12"/>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" s="18" t="s">
         <v>76</v>
       </c>
@@ -2361,12 +2439,14 @@
       </c>
       <c r="G51" s="22"/>
       <c r="H51" s="12"/>
-      <c r="I51" s="12"/>
+      <c r="I51" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="J51" s="12"/>
       <c r="K51" s="12"/>
       <c r="L51" s="12"/>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52" s="18" t="s">
         <v>77</v>
       </c>
@@ -2383,16 +2463,18 @@
         <v>109</v>
       </c>
       <c r="F52" s="21" t="s">
-        <v>128</v>
+        <v>38</v>
       </c>
       <c r="G52" s="22"/>
       <c r="H52" s="12"/>
-      <c r="I52" s="12"/>
+      <c r="I52" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="J52" s="12"/>
       <c r="K52" s="12"/>
       <c r="L52" s="12"/>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53" s="18" t="s">
         <v>78</v>
       </c>
@@ -2413,12 +2495,14 @@
       </c>
       <c r="G53" s="22"/>
       <c r="H53" s="12"/>
-      <c r="I53" s="12"/>
+      <c r="I53" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="J53" s="12"/>
       <c r="K53" s="12"/>
       <c r="L53" s="12"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" s="18" t="s">
         <v>79</v>
       </c>
@@ -2435,16 +2519,18 @@
         <v>110</v>
       </c>
       <c r="F54" s="21" t="s">
-        <v>128</v>
+        <v>38</v>
       </c>
       <c r="G54" s="22"/>
       <c r="H54" s="12"/>
-      <c r="I54" s="12"/>
+      <c r="I54" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="J54" s="12"/>
       <c r="K54" s="12"/>
       <c r="L54" s="12"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55" s="18" t="s">
         <v>80</v>
       </c>
@@ -2468,7 +2554,7 @@
       <c r="K55" s="12"/>
       <c r="L55" s="12"/>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56" s="18" t="s">
         <v>81</v>
       </c>
@@ -2489,12 +2575,14 @@
       </c>
       <c r="G56" s="22"/>
       <c r="H56" s="12"/>
-      <c r="I56" s="12"/>
+      <c r="I56" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="J56" s="12"/>
       <c r="K56" s="12"/>
       <c r="L56" s="12"/>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57" s="18" t="s">
         <v>82</v>
       </c>
@@ -2511,16 +2599,18 @@
         <v>111</v>
       </c>
       <c r="F57" s="21" t="s">
-        <v>128</v>
+        <v>38</v>
       </c>
       <c r="G57" s="22"/>
       <c r="H57" s="12"/>
-      <c r="I57" s="12"/>
+      <c r="I57" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="J57" s="12"/>
       <c r="K57" s="12"/>
       <c r="L57" s="12"/>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58" s="7">
         <v>44</v>
       </c>
@@ -2539,12 +2629,14 @@
       </c>
       <c r="G58" s="22"/>
       <c r="H58" s="19"/>
-      <c r="I58" s="19"/>
+      <c r="I58" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="J58" s="19"/>
       <c r="K58" s="19"/>
       <c r="L58" s="19"/>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59" s="7">
         <v>45</v>
       </c>
@@ -2563,12 +2655,14 @@
       </c>
       <c r="G59" s="22"/>
       <c r="H59" s="19"/>
-      <c r="I59" s="19"/>
+      <c r="I59" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="J59" s="19"/>
       <c r="K59" s="19"/>
       <c r="L59" s="19"/>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60" s="7">
         <v>46</v>
       </c>
@@ -2587,12 +2681,14 @@
       </c>
       <c r="G60" s="22"/>
       <c r="H60" s="19"/>
-      <c r="I60" s="19"/>
+      <c r="I60" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="J60" s="19"/>
       <c r="K60" s="19"/>
       <c r="L60" s="19"/>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61" s="7">
         <v>47</v>
       </c>
@@ -2611,12 +2707,14 @@
       </c>
       <c r="G61" s="22"/>
       <c r="H61" s="19"/>
-      <c r="I61" s="19"/>
+      <c r="I61" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="J61" s="19"/>
       <c r="K61" s="19"/>
       <c r="L61" s="19"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62" s="7">
         <v>48</v>
       </c>
@@ -2635,12 +2733,14 @@
       </c>
       <c r="G62" s="22"/>
       <c r="H62" s="19"/>
-      <c r="I62" s="19"/>
+      <c r="I62" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="J62" s="19"/>
       <c r="K62" s="19"/>
       <c r="L62" s="19"/>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63" s="7">
         <v>49</v>
       </c>
@@ -2659,12 +2759,14 @@
       </c>
       <c r="G63" s="22"/>
       <c r="H63" s="19"/>
-      <c r="I63" s="19"/>
+      <c r="I63" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="J63" s="19"/>
       <c r="K63" s="19"/>
       <c r="L63" s="19"/>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64" s="7">
         <v>50</v>
       </c>
@@ -2683,12 +2785,12 @@
       </c>
       <c r="G64" s="22"/>
       <c r="H64" s="19"/>
-      <c r="I64" s="19"/>
+      <c r="I64" s="12"/>
       <c r="J64" s="19"/>
       <c r="K64" s="19"/>
       <c r="L64" s="19"/>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A65" s="7">
         <v>51</v>
       </c>
@@ -2707,12 +2809,14 @@
       </c>
       <c r="G65" s="22"/>
       <c r="H65" s="19"/>
-      <c r="I65" s="19"/>
+      <c r="I65" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="J65" s="19"/>
       <c r="K65" s="19"/>
       <c r="L65" s="19"/>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A66" s="7">
         <v>52</v>
       </c>
@@ -2731,12 +2835,15 @@
       </c>
       <c r="G66" s="22"/>
       <c r="H66" s="19"/>
-      <c r="I66" s="19"/>
+      <c r="I66" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="J66" s="19"/>
       <c r="K66" s="19"/>
       <c r="L66" s="19"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:L66" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
changes after merge to main
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/euTaxonomyNonFinancials/EutaxonomyNonFinancials.xlsx
+++ b/dataland-framework-toolbox/inputs/euTaxonomyNonFinancials/EutaxonomyNonFinancials.xlsx
@@ -5,17 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d93369\Documents\Projekte\Dataland\Repos\Dataland\dataland-framework-toolbox\inputs\euTaxonomyNonFinancials\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dataland\dataland_alternative\dataland-framework-toolbox\inputs\euTaxonomyNonFinancials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AD449AF-6DDA-4D38-8046-160256CB1462}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E51E730-3590-4F62-A449-A34DD2DB217B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57490" yWindow="-10800" windowWidth="38620" windowHeight="21220" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Framework Data Model" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Framework Data Model'!$A$1:$L$104</definedName>
     <definedName name="IQ_CH">110000</definedName>
     <definedName name="IQ_CQ">5000</definedName>
     <definedName name="IQ_CY">10000</definedName>
@@ -57,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="234">
   <si>
     <t>Field Identifier</t>
   </si>
@@ -420,9 +421,6 @@
   </si>
   <si>
     <t>Custom EuTaxonomyAlignedActivitiesComponent</t>
-  </si>
-  <si>
-    <t>AmountWithCurrencyComponent</t>
   </si>
   <si>
     <t>Substantial Contribution to Climate Change Mitigation In Percent - Eligible</t>
@@ -1392,21 +1390,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D57" sqref="D57"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14:F95"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="20.21875" customWidth="1"/>
-    <col min="4" max="4" width="95.109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="77.88671875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="44.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="26.21875" customWidth="1"/>
-    <col min="8" max="12" width="14.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" customWidth="1"/>
+    <col min="4" max="4" width="95.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="77.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="44.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="26.28515625" customWidth="1"/>
+    <col min="8" max="12" width="14.28515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1444,7 +1442,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
         <v>0</v>
       </c>
@@ -1465,12 +1463,14 @@
         <v>78</v>
       </c>
       <c r="H2" s="11"/>
-      <c r="I2" s="12"/>
+      <c r="I2" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J2" s="12"/>
       <c r="K2" s="12"/>
       <c r="L2" s="12"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
       <c r="B3" s="8" t="s">
         <v>12</v>
@@ -1487,12 +1487,14 @@
       </c>
       <c r="G3" s="10"/>
       <c r="H3" s="11"/>
-      <c r="I3" s="12"/>
+      <c r="I3" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J3" s="12"/>
       <c r="K3" s="12"/>
       <c r="L3" s="12"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>1</v>
       </c>
@@ -1513,12 +1515,14 @@
         <v>14</v>
       </c>
       <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
+      <c r="I4" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J4" s="11"/>
       <c r="K4" s="11"/>
       <c r="L4" s="12"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>2</v>
       </c>
@@ -1539,12 +1543,14 @@
         <v>14</v>
       </c>
       <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
+      <c r="I5" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J5" s="12"/>
       <c r="K5" s="12"/>
       <c r="L5" s="12"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>3</v>
       </c>
@@ -1565,12 +1571,14 @@
         <v>14</v>
       </c>
       <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
+      <c r="I6" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J6" s="12"/>
       <c r="K6" s="12"/>
       <c r="L6" s="12"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>4</v>
       </c>
@@ -1596,7 +1604,7 @@
       <c r="K7" s="12"/>
       <c r="L7" s="12"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>5</v>
       </c>
@@ -1615,12 +1623,14 @@
       </c>
       <c r="G8" s="22"/>
       <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
+      <c r="I8" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J8" s="12"/>
       <c r="K8" s="12"/>
       <c r="L8" s="12"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>6</v>
       </c>
@@ -1644,7 +1654,7 @@
       <c r="K9" s="12"/>
       <c r="L9" s="12"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>8</v>
       </c>
@@ -1670,7 +1680,7 @@
       <c r="K10" s="12"/>
       <c r="L10" s="12"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
         <v>42</v>
       </c>
@@ -1689,12 +1699,14 @@
       </c>
       <c r="G11" s="22"/>
       <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
+      <c r="I11" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J11" s="12"/>
       <c r="K11" s="12"/>
       <c r="L11" s="12"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
         <v>43</v>
       </c>
@@ -1711,16 +1723,18 @@
         <v>84</v>
       </c>
       <c r="F12" s="21" t="s">
-        <v>121</v>
+        <v>37</v>
       </c>
       <c r="G12" s="22"/>
       <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
+      <c r="I12" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J12" s="12"/>
       <c r="K12" s="12"/>
       <c r="L12" s="12"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
         <v>45</v>
       </c>
@@ -1741,12 +1755,14 @@
       </c>
       <c r="G13" s="22"/>
       <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
+      <c r="I13" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J13" s="12"/>
       <c r="K13" s="12"/>
       <c r="L13" s="12"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
         <v>46</v>
       </c>
@@ -1763,16 +1779,18 @@
         <v>107</v>
       </c>
       <c r="F14" s="21" t="s">
-        <v>121</v>
+        <v>37</v>
       </c>
       <c r="G14" s="22"/>
       <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
+      <c r="I14" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J14" s="12"/>
       <c r="K14" s="12"/>
       <c r="L14" s="12"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
         <v>48</v>
       </c>
@@ -1793,12 +1811,14 @@
       </c>
       <c r="G15" s="22"/>
       <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
+      <c r="I15" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J15" s="12"/>
       <c r="K15" s="12"/>
       <c r="L15" s="12"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
         <v>49</v>
       </c>
@@ -1815,16 +1835,18 @@
         <v>106</v>
       </c>
       <c r="F16" s="21" t="s">
-        <v>121</v>
+        <v>37</v>
       </c>
       <c r="G16" s="22"/>
       <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
+      <c r="I16" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J16" s="12"/>
       <c r="K16" s="12"/>
       <c r="L16" s="12"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
         <v>55</v>
       </c>
@@ -1848,7 +1870,7 @@
       <c r="K17" s="12"/>
       <c r="L17" s="12"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
         <v>56</v>
       </c>
@@ -1869,12 +1891,14 @@
       </c>
       <c r="G18" s="22"/>
       <c r="H18" s="12"/>
-      <c r="I18" s="12"/>
+      <c r="I18" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J18" s="12"/>
       <c r="K18" s="12"/>
       <c r="L18" s="12"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="18" t="s">
         <v>57</v>
       </c>
@@ -1891,16 +1915,18 @@
         <v>105</v>
       </c>
       <c r="F19" s="21" t="s">
-        <v>121</v>
+        <v>37</v>
       </c>
       <c r="G19" s="22"/>
       <c r="H19" s="12"/>
-      <c r="I19" s="12"/>
+      <c r="I19" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J19" s="12"/>
       <c r="K19" s="12"/>
       <c r="L19" s="12"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="7">
         <v>14</v>
       </c>
@@ -1909,118 +1935,128 @@
       </c>
       <c r="C20" s="8"/>
       <c r="D20" s="29" t="s">
+        <v>121</v>
+      </c>
+      <c r="E20" s="30" t="s">
         <v>122</v>
-      </c>
-      <c r="E20" s="30" t="s">
-        <v>123</v>
       </c>
       <c r="F20" s="21" t="s">
         <v>28</v>
       </c>
       <c r="G20" s="22"/>
       <c r="H20" s="12"/>
-      <c r="I20" s="12"/>
+      <c r="I20" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J20" s="12"/>
       <c r="K20" s="12"/>
       <c r="L20" s="12"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="18" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C21" s="8"/>
       <c r="D21" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="E21" s="30" t="s">
         <v>124</v>
-      </c>
-      <c r="E21" s="30" t="s">
-        <v>125</v>
       </c>
       <c r="F21" s="21" t="s">
         <v>28</v>
       </c>
       <c r="G21" s="22"/>
       <c r="H21" s="12"/>
-      <c r="I21" s="12"/>
+      <c r="I21" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J21" s="12"/>
       <c r="K21" s="12"/>
       <c r="L21" s="12"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C22" s="8"/>
       <c r="D22" s="31" t="s">
+        <v>125</v>
+      </c>
+      <c r="E22" s="30" t="s">
         <v>126</v>
-      </c>
-      <c r="E22" s="30" t="s">
-        <v>127</v>
       </c>
       <c r="F22" s="21" t="s">
         <v>28</v>
       </c>
       <c r="G22" s="22"/>
       <c r="H22" s="12"/>
-      <c r="I22" s="12"/>
+      <c r="I22" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J22" s="12"/>
       <c r="K22" s="12"/>
       <c r="L22" s="12"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="18" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C23" s="8"/>
       <c r="D23" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="E23" s="30" t="s">
         <v>128</v>
-      </c>
-      <c r="E23" s="30" t="s">
-        <v>129</v>
       </c>
       <c r="F23" s="21" t="s">
         <v>28</v>
       </c>
       <c r="G23" s="22"/>
       <c r="H23" s="12"/>
-      <c r="I23" s="12"/>
+      <c r="I23" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J23" s="12"/>
       <c r="K23" s="12"/>
       <c r="L23" s="12"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="18" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B24" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C24" s="8"/>
       <c r="D24" s="29" t="s">
+        <v>129</v>
+      </c>
+      <c r="E24" s="30" t="s">
         <v>130</v>
-      </c>
-      <c r="E24" s="30" t="s">
-        <v>131</v>
       </c>
       <c r="F24" s="21" t="s">
         <v>28</v>
       </c>
       <c r="G24" s="22"/>
       <c r="H24" s="12"/>
-      <c r="I24" s="12"/>
+      <c r="I24" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J24" s="12"/>
       <c r="K24" s="12"/>
       <c r="L24" s="12"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="7">
         <v>15</v>
       </c>
@@ -2029,94 +2065,102 @@
       </c>
       <c r="C25" s="8"/>
       <c r="D25" s="32" t="s">
+        <v>138</v>
+      </c>
+      <c r="E25" s="30" t="s">
         <v>139</v>
-      </c>
-      <c r="E25" s="30" t="s">
-        <v>140</v>
       </c>
       <c r="F25" s="21" t="s">
         <v>28</v>
       </c>
       <c r="G25" s="22"/>
       <c r="H25" s="12"/>
-      <c r="I25" s="12"/>
+      <c r="I25" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J25" s="12"/>
       <c r="K25" s="12"/>
       <c r="L25" s="12"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="18" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B26" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C26" s="8"/>
       <c r="D26" s="32" t="s">
+        <v>140</v>
+      </c>
+      <c r="E26" s="30" t="s">
         <v>141</v>
-      </c>
-      <c r="E26" s="30" t="s">
-        <v>142</v>
       </c>
       <c r="F26" s="21" t="s">
         <v>28</v>
       </c>
       <c r="G26" s="22"/>
       <c r="H26" s="12"/>
-      <c r="I26" s="12"/>
+      <c r="I26" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J26" s="12"/>
       <c r="K26" s="12"/>
       <c r="L26" s="12"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="18" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B27" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C27" s="8"/>
       <c r="D27" s="31" t="s">
+        <v>142</v>
+      </c>
+      <c r="E27" s="30" t="s">
         <v>143</v>
-      </c>
-      <c r="E27" s="30" t="s">
-        <v>144</v>
       </c>
       <c r="F27" s="21" t="s">
         <v>28</v>
       </c>
       <c r="G27" s="22"/>
       <c r="H27" s="12"/>
-      <c r="I27" s="12"/>
+      <c r="I27" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J27" s="12"/>
       <c r="K27" s="12"/>
       <c r="L27" s="12"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="18" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B28" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C28" s="8"/>
       <c r="D28" s="31" t="s">
+        <v>144</v>
+      </c>
+      <c r="E28" s="30" t="s">
         <v>145</v>
-      </c>
-      <c r="E28" s="30" t="s">
-        <v>146</v>
       </c>
       <c r="F28" s="21" t="s">
         <v>28</v>
       </c>
       <c r="G28" s="22"/>
       <c r="H28" s="12"/>
-      <c r="I28" s="12"/>
+      <c r="I28" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J28" s="12"/>
       <c r="K28" s="12"/>
       <c r="L28" s="12"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="7">
         <v>16</v>
       </c>
@@ -2125,94 +2169,102 @@
       </c>
       <c r="C29" s="8"/>
       <c r="D29" s="31" t="s">
+        <v>149</v>
+      </c>
+      <c r="E29" s="30" t="s">
         <v>150</v>
-      </c>
-      <c r="E29" s="30" t="s">
-        <v>151</v>
       </c>
       <c r="F29" s="21" t="s">
         <v>28</v>
       </c>
       <c r="G29" s="22"/>
       <c r="H29" s="12"/>
-      <c r="I29" s="12"/>
+      <c r="I29" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J29" s="12"/>
       <c r="K29" s="12"/>
       <c r="L29" s="12"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="18" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B30" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C30" s="8"/>
       <c r="D30" s="31" t="s">
+        <v>151</v>
+      </c>
+      <c r="E30" s="30" t="s">
         <v>152</v>
-      </c>
-      <c r="E30" s="30" t="s">
-        <v>153</v>
       </c>
       <c r="F30" s="21" t="s">
         <v>28</v>
       </c>
       <c r="G30" s="22"/>
       <c r="H30" s="12"/>
-      <c r="I30" s="12"/>
+      <c r="I30" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J30" s="12"/>
       <c r="K30" s="12"/>
       <c r="L30" s="12"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="18" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B31" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C31" s="8"/>
       <c r="D31" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="E31" s="30" t="s">
         <v>154</v>
-      </c>
-      <c r="E31" s="30" t="s">
-        <v>155</v>
       </c>
       <c r="F31" s="21" t="s">
         <v>28</v>
       </c>
       <c r="G31" s="22"/>
       <c r="H31" s="12"/>
-      <c r="I31" s="12"/>
+      <c r="I31" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J31" s="12"/>
       <c r="K31" s="12"/>
       <c r="L31" s="12"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="18" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B32" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C32" s="8"/>
       <c r="D32" s="31" t="s">
+        <v>155</v>
+      </c>
+      <c r="E32" s="30" t="s">
         <v>156</v>
-      </c>
-      <c r="E32" s="30" t="s">
-        <v>157</v>
       </c>
       <c r="F32" s="21" t="s">
         <v>28</v>
       </c>
       <c r="G32" s="22"/>
       <c r="H32" s="12"/>
-      <c r="I32" s="12"/>
+      <c r="I32" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J32" s="12"/>
       <c r="K32" s="12"/>
       <c r="L32" s="12"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="7">
         <v>17</v>
       </c>
@@ -2221,94 +2273,102 @@
       </c>
       <c r="C33" s="8"/>
       <c r="D33" s="31" t="s">
+        <v>160</v>
+      </c>
+      <c r="E33" s="30" t="s">
         <v>161</v>
-      </c>
-      <c r="E33" s="30" t="s">
-        <v>162</v>
       </c>
       <c r="F33" s="21" t="s">
         <v>28</v>
       </c>
       <c r="G33" s="22"/>
       <c r="H33" s="12"/>
-      <c r="I33" s="12"/>
+      <c r="I33" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J33" s="12"/>
       <c r="K33" s="12"/>
       <c r="L33" s="12"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="18" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B34" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C34" s="8"/>
       <c r="D34" s="31" t="s">
+        <v>162</v>
+      </c>
+      <c r="E34" s="30" t="s">
         <v>163</v>
-      </c>
-      <c r="E34" s="30" t="s">
-        <v>164</v>
       </c>
       <c r="F34" s="21" t="s">
         <v>28</v>
       </c>
       <c r="G34" s="22"/>
       <c r="H34" s="12"/>
-      <c r="I34" s="12"/>
+      <c r="I34" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J34" s="12"/>
       <c r="K34" s="12"/>
       <c r="L34" s="12"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="18" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B35" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C35" s="8"/>
       <c r="D35" s="31" t="s">
+        <v>164</v>
+      </c>
+      <c r="E35" s="30" t="s">
         <v>165</v>
-      </c>
-      <c r="E35" s="30" t="s">
-        <v>166</v>
       </c>
       <c r="F35" s="21" t="s">
         <v>28</v>
       </c>
       <c r="G35" s="22"/>
       <c r="H35" s="12"/>
-      <c r="I35" s="12"/>
+      <c r="I35" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J35" s="12"/>
       <c r="K35" s="12"/>
       <c r="L35" s="12"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="18" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B36" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C36" s="8"/>
       <c r="D36" s="31" t="s">
+        <v>166</v>
+      </c>
+      <c r="E36" s="30" t="s">
         <v>167</v>
-      </c>
-      <c r="E36" s="30" t="s">
-        <v>168</v>
       </c>
       <c r="F36" s="21" t="s">
         <v>28</v>
       </c>
       <c r="G36" s="22"/>
       <c r="H36" s="12"/>
-      <c r="I36" s="12"/>
+      <c r="I36" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J36" s="12"/>
       <c r="K36" s="12"/>
       <c r="L36" s="12"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="7">
         <v>18</v>
       </c>
@@ -2317,94 +2377,102 @@
       </c>
       <c r="C37" s="8"/>
       <c r="D37" s="31" t="s">
+        <v>171</v>
+      </c>
+      <c r="E37" s="30" t="s">
         <v>172</v>
-      </c>
-      <c r="E37" s="30" t="s">
-        <v>173</v>
       </c>
       <c r="F37" s="21" t="s">
         <v>28</v>
       </c>
       <c r="G37" s="22"/>
       <c r="H37" s="12"/>
-      <c r="I37" s="12"/>
+      <c r="I37" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J37" s="12"/>
       <c r="K37" s="12"/>
       <c r="L37" s="12"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="18" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B38" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C38" s="8"/>
       <c r="D38" s="31" t="s">
+        <v>173</v>
+      </c>
+      <c r="E38" s="30" t="s">
         <v>174</v>
-      </c>
-      <c r="E38" s="30" t="s">
-        <v>175</v>
       </c>
       <c r="F38" s="21" t="s">
         <v>28</v>
       </c>
       <c r="G38" s="22"/>
       <c r="H38" s="12"/>
-      <c r="I38" s="12"/>
+      <c r="I38" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J38" s="12"/>
       <c r="K38" s="12"/>
       <c r="L38" s="12"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="18" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B39" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C39" s="8"/>
       <c r="D39" s="31" t="s">
+        <v>175</v>
+      </c>
+      <c r="E39" s="30" t="s">
         <v>176</v>
-      </c>
-      <c r="E39" s="30" t="s">
-        <v>177</v>
       </c>
       <c r="F39" s="21" t="s">
         <v>28</v>
       </c>
       <c r="G39" s="22"/>
       <c r="H39" s="12"/>
-      <c r="I39" s="12"/>
+      <c r="I39" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J39" s="12"/>
       <c r="K39" s="12"/>
       <c r="L39" s="12"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B40" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C40" s="8"/>
       <c r="D40" s="31" t="s">
+        <v>177</v>
+      </c>
+      <c r="E40" s="30" t="s">
         <v>178</v>
-      </c>
-      <c r="E40" s="30" t="s">
-        <v>179</v>
       </c>
       <c r="F40" s="21" t="s">
         <v>28</v>
       </c>
       <c r="G40" s="22"/>
       <c r="H40" s="12"/>
-      <c r="I40" s="12"/>
+      <c r="I40" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J40" s="12"/>
       <c r="K40" s="12"/>
       <c r="L40" s="12"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="7">
         <v>19</v>
       </c>
@@ -2413,94 +2481,102 @@
       </c>
       <c r="C41" s="8"/>
       <c r="D41" s="31" t="s">
+        <v>182</v>
+      </c>
+      <c r="E41" s="30" t="s">
         <v>183</v>
-      </c>
-      <c r="E41" s="30" t="s">
-        <v>184</v>
       </c>
       <c r="F41" s="21" t="s">
         <v>28</v>
       </c>
       <c r="G41" s="22"/>
       <c r="H41" s="12"/>
-      <c r="I41" s="12"/>
+      <c r="I41" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J41" s="12"/>
       <c r="K41" s="12"/>
       <c r="L41" s="12"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="18" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B42" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C42" s="8"/>
       <c r="D42" s="31" t="s">
+        <v>184</v>
+      </c>
+      <c r="E42" s="30" t="s">
         <v>185</v>
-      </c>
-      <c r="E42" s="30" t="s">
-        <v>186</v>
       </c>
       <c r="F42" s="21" t="s">
         <v>28</v>
       </c>
       <c r="G42" s="22"/>
       <c r="H42" s="12"/>
-      <c r="I42" s="12"/>
+      <c r="I42" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J42" s="12"/>
       <c r="K42" s="12"/>
       <c r="L42" s="12"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="18" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B43" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C43" s="8"/>
       <c r="D43" s="31" t="s">
+        <v>186</v>
+      </c>
+      <c r="E43" s="30" t="s">
         <v>187</v>
-      </c>
-      <c r="E43" s="30" t="s">
-        <v>188</v>
       </c>
       <c r="F43" s="21" t="s">
         <v>28</v>
       </c>
       <c r="G43" s="22"/>
       <c r="H43" s="12"/>
-      <c r="I43" s="12"/>
+      <c r="I43" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J43" s="12"/>
       <c r="K43" s="12"/>
       <c r="L43" s="12"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="18" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B44" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C44" s="8"/>
       <c r="D44" s="31" t="s">
+        <v>188</v>
+      </c>
+      <c r="E44" s="30" t="s">
         <v>189</v>
-      </c>
-      <c r="E44" s="30" t="s">
-        <v>190</v>
       </c>
       <c r="F44" s="21" t="s">
         <v>28</v>
       </c>
       <c r="G44" s="22"/>
       <c r="H44" s="12"/>
-      <c r="I44" s="12"/>
+      <c r="I44" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J44" s="12"/>
       <c r="K44" s="12"/>
       <c r="L44" s="12"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="7">
         <v>20</v>
       </c>
@@ -2524,7 +2600,7 @@
       <c r="K45" s="12"/>
       <c r="L45" s="12"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="7">
         <v>21</v>
       </c>
@@ -2543,12 +2619,14 @@
       </c>
       <c r="G46" s="22"/>
       <c r="H46" s="12"/>
-      <c r="I46" s="12"/>
+      <c r="I46" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J46" s="12"/>
       <c r="K46" s="12"/>
       <c r="L46" s="12"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
         <v>22</v>
       </c>
@@ -2567,12 +2645,14 @@
       </c>
       <c r="G47" s="22"/>
       <c r="H47" s="12"/>
-      <c r="I47" s="12"/>
+      <c r="I47" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J47" s="12"/>
       <c r="K47" s="12"/>
       <c r="L47" s="12"/>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="7">
         <v>23</v>
       </c>
@@ -2598,7 +2678,7 @@
       <c r="K48" s="12"/>
       <c r="L48" s="12"/>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="18" t="s">
         <v>60</v>
       </c>
@@ -2619,12 +2699,14 @@
       </c>
       <c r="G49" s="22"/>
       <c r="H49" s="12"/>
-      <c r="I49" s="12"/>
+      <c r="I49" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J49" s="12"/>
       <c r="K49" s="12"/>
       <c r="L49" s="12"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="18" t="s">
         <v>61</v>
       </c>
@@ -2641,16 +2723,18 @@
         <v>100</v>
       </c>
       <c r="F50" s="21" t="s">
-        <v>121</v>
+        <v>37</v>
       </c>
       <c r="G50" s="22"/>
       <c r="H50" s="12"/>
-      <c r="I50" s="12"/>
+      <c r="I50" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J50" s="12"/>
       <c r="K50" s="12"/>
       <c r="L50" s="12"/>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="18" t="s">
         <v>58</v>
       </c>
@@ -2671,12 +2755,14 @@
       </c>
       <c r="G51" s="22"/>
       <c r="H51" s="12"/>
-      <c r="I51" s="12"/>
+      <c r="I51" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J51" s="12"/>
       <c r="K51" s="12"/>
       <c r="L51" s="12"/>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="18" t="s">
         <v>59</v>
       </c>
@@ -2693,16 +2779,18 @@
         <v>95</v>
       </c>
       <c r="F52" s="21" t="s">
-        <v>121</v>
+        <v>37</v>
       </c>
       <c r="G52" s="22"/>
       <c r="H52" s="12"/>
-      <c r="I52" s="12"/>
+      <c r="I52" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J52" s="12"/>
       <c r="K52" s="12"/>
       <c r="L52" s="12"/>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="18" t="s">
         <v>62</v>
       </c>
@@ -2723,12 +2811,14 @@
       </c>
       <c r="G53" s="22"/>
       <c r="H53" s="12"/>
-      <c r="I53" s="12"/>
+      <c r="I53" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J53" s="12"/>
       <c r="K53" s="12"/>
       <c r="L53" s="12"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="18" t="s">
         <v>63</v>
       </c>
@@ -2745,16 +2835,18 @@
         <v>99</v>
       </c>
       <c r="F54" s="21" t="s">
-        <v>121</v>
+        <v>37</v>
       </c>
       <c r="G54" s="22"/>
       <c r="H54" s="12"/>
-      <c r="I54" s="12"/>
+      <c r="I54" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J54" s="12"/>
       <c r="K54" s="12"/>
       <c r="L54" s="12"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="18" t="s">
         <v>64</v>
       </c>
@@ -2778,7 +2870,7 @@
       <c r="K55" s="12"/>
       <c r="L55" s="12"/>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="18" t="s">
         <v>65</v>
       </c>
@@ -2799,12 +2891,14 @@
       </c>
       <c r="G56" s="22"/>
       <c r="H56" s="12"/>
-      <c r="I56" s="12"/>
+      <c r="I56" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J56" s="12"/>
       <c r="K56" s="12"/>
       <c r="L56" s="12"/>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="18" t="s">
         <v>66</v>
       </c>
@@ -2821,16 +2915,18 @@
         <v>96</v>
       </c>
       <c r="F57" s="21" t="s">
-        <v>121</v>
+        <v>37</v>
       </c>
       <c r="G57" s="22"/>
       <c r="H57" s="12"/>
-      <c r="I57" s="12"/>
+      <c r="I57" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J57" s="12"/>
       <c r="K57" s="12"/>
       <c r="L57" s="12"/>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="7">
         <v>29</v>
       </c>
@@ -2839,118 +2935,128 @@
       </c>
       <c r="C58" s="8"/>
       <c r="D58" s="29" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E58" s="30" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F58" s="21" t="s">
         <v>28</v>
       </c>
       <c r="G58" s="22"/>
       <c r="H58" s="12"/>
-      <c r="I58" s="12"/>
+      <c r="I58" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J58" s="12"/>
       <c r="K58" s="12"/>
       <c r="L58" s="12"/>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B59" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C59" s="8"/>
       <c r="D59" s="29" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E59" s="30" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F59" s="21" t="s">
         <v>28</v>
       </c>
       <c r="G59" s="22"/>
       <c r="H59" s="12"/>
-      <c r="I59" s="12"/>
+      <c r="I59" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J59" s="12"/>
       <c r="K59" s="12"/>
       <c r="L59" s="12"/>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="18" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B60" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C60" s="8"/>
       <c r="D60" s="31" t="s">
+        <v>125</v>
+      </c>
+      <c r="E60" s="30" t="s">
         <v>126</v>
-      </c>
-      <c r="E60" s="30" t="s">
-        <v>127</v>
       </c>
       <c r="F60" s="21" t="s">
         <v>28</v>
       </c>
       <c r="G60" s="22"/>
       <c r="H60" s="12"/>
-      <c r="I60" s="12"/>
+      <c r="I60" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J60" s="12"/>
       <c r="K60" s="12"/>
       <c r="L60" s="12"/>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" s="18" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B61" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C61" s="8"/>
       <c r="D61" s="29" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E61" s="30" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F61" s="21" t="s">
         <v>28</v>
       </c>
       <c r="G61" s="22"/>
       <c r="H61" s="12"/>
-      <c r="I61" s="12"/>
+      <c r="I61" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J61" s="12"/>
       <c r="K61" s="12"/>
       <c r="L61" s="12"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" s="18" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B62" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C62" s="8"/>
       <c r="D62" s="29" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E62" s="30" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F62" s="21" t="s">
         <v>28</v>
       </c>
       <c r="G62" s="22"/>
       <c r="H62" s="12"/>
-      <c r="I62" s="12"/>
+      <c r="I62" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J62" s="12"/>
       <c r="K62" s="12"/>
       <c r="L62" s="12"/>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="7">
         <v>30</v>
       </c>
@@ -2959,94 +3065,102 @@
       </c>
       <c r="C63" s="8"/>
       <c r="D63" s="32" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E63" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F63" s="21" t="s">
         <v>28</v>
       </c>
       <c r="G63" s="22"/>
       <c r="H63" s="12"/>
-      <c r="I63" s="12"/>
+      <c r="I63" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J63" s="12"/>
       <c r="K63" s="12"/>
       <c r="L63" s="12"/>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="18" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B64" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C64" s="8"/>
       <c r="D64" s="32" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E64" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F64" s="21" t="s">
         <v>28</v>
       </c>
       <c r="G64" s="22"/>
       <c r="H64" s="12"/>
-      <c r="I64" s="12"/>
+      <c r="I64" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J64" s="12"/>
       <c r="K64" s="12"/>
       <c r="L64" s="12"/>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" s="18" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B65" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C65" s="8"/>
       <c r="D65" s="31" t="s">
+        <v>142</v>
+      </c>
+      <c r="E65" s="30" t="s">
         <v>143</v>
-      </c>
-      <c r="E65" s="30" t="s">
-        <v>144</v>
       </c>
       <c r="F65" s="21" t="s">
         <v>28</v>
       </c>
       <c r="G65" s="22"/>
       <c r="H65" s="12"/>
-      <c r="I65" s="12"/>
+      <c r="I65" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J65" s="12"/>
       <c r="K65" s="12"/>
       <c r="L65" s="12"/>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B66" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C66" s="8"/>
       <c r="D66" s="31" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E66" s="30" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F66" s="21" t="s">
         <v>28</v>
       </c>
       <c r="G66" s="22"/>
       <c r="H66" s="12"/>
-      <c r="I66" s="12"/>
+      <c r="I66" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J66" s="12"/>
       <c r="K66" s="12"/>
       <c r="L66" s="12"/>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" s="7">
         <v>31</v>
       </c>
@@ -3055,94 +3169,102 @@
       </c>
       <c r="C67" s="8"/>
       <c r="D67" s="31" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E67" s="30" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F67" s="21" t="s">
         <v>28</v>
       </c>
       <c r="G67" s="22"/>
       <c r="H67" s="12"/>
-      <c r="I67" s="12"/>
+      <c r="I67" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J67" s="12"/>
       <c r="K67" s="12"/>
       <c r="L67" s="12"/>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" s="18" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B68" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C68" s="8"/>
       <c r="D68" s="31" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E68" s="30" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F68" s="21" t="s">
         <v>28</v>
       </c>
       <c r="G68" s="22"/>
       <c r="H68" s="12"/>
-      <c r="I68" s="12"/>
+      <c r="I68" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J68" s="12"/>
       <c r="K68" s="12"/>
       <c r="L68" s="12"/>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" s="18" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B69" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C69" s="8"/>
       <c r="D69" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="E69" s="30" t="s">
         <v>154</v>
-      </c>
-      <c r="E69" s="30" t="s">
-        <v>155</v>
       </c>
       <c r="F69" s="21" t="s">
         <v>28</v>
       </c>
       <c r="G69" s="22"/>
       <c r="H69" s="12"/>
-      <c r="I69" s="12"/>
+      <c r="I69" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J69" s="12"/>
       <c r="K69" s="12"/>
       <c r="L69" s="12"/>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" s="18" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B70" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C70" s="8"/>
       <c r="D70" s="31" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E70" s="30" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F70" s="21" t="s">
         <v>28</v>
       </c>
       <c r="G70" s="22"/>
       <c r="H70" s="12"/>
-      <c r="I70" s="12"/>
+      <c r="I70" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J70" s="12"/>
       <c r="K70" s="12"/>
       <c r="L70" s="12"/>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" s="7">
         <v>32</v>
       </c>
@@ -3151,94 +3273,102 @@
       </c>
       <c r="C71" s="8"/>
       <c r="D71" s="31" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E71" s="30" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F71" s="21" t="s">
         <v>28</v>
       </c>
       <c r="G71" s="22"/>
       <c r="H71" s="12"/>
-      <c r="I71" s="12"/>
+      <c r="I71" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J71" s="12"/>
       <c r="K71" s="12"/>
       <c r="L71" s="12"/>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" s="18" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B72" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C72" s="8"/>
       <c r="D72" s="31" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E72" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F72" s="21" t="s">
         <v>28</v>
       </c>
       <c r="G72" s="22"/>
       <c r="H72" s="12"/>
-      <c r="I72" s="12"/>
+      <c r="I72" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J72" s="12"/>
       <c r="K72" s="12"/>
       <c r="L72" s="12"/>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" s="18" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B73" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C73" s="8"/>
       <c r="D73" s="31" t="s">
+        <v>164</v>
+      </c>
+      <c r="E73" s="30" t="s">
         <v>165</v>
-      </c>
-      <c r="E73" s="30" t="s">
-        <v>166</v>
       </c>
       <c r="F73" s="21" t="s">
         <v>28</v>
       </c>
       <c r="G73" s="22"/>
       <c r="H73" s="12"/>
-      <c r="I73" s="12"/>
+      <c r="I73" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J73" s="12"/>
       <c r="K73" s="12"/>
       <c r="L73" s="12"/>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74" s="18" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B74" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C74" s="8"/>
       <c r="D74" s="31" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E74" s="30" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F74" s="21" t="s">
         <v>28</v>
       </c>
       <c r="G74" s="22"/>
       <c r="H74" s="12"/>
-      <c r="I74" s="12"/>
+      <c r="I74" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J74" s="12"/>
       <c r="K74" s="12"/>
       <c r="L74" s="12"/>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75" s="7">
         <v>33</v>
       </c>
@@ -3247,94 +3377,102 @@
       </c>
       <c r="C75" s="8"/>
       <c r="D75" s="31" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E75" s="30" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F75" s="21" t="s">
         <v>28</v>
       </c>
       <c r="G75" s="22"/>
       <c r="H75" s="12"/>
-      <c r="I75" s="12"/>
+      <c r="I75" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J75" s="12"/>
       <c r="K75" s="12"/>
       <c r="L75" s="12"/>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76" s="18" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B76" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C76" s="8"/>
       <c r="D76" s="31" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E76" s="30" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F76" s="21" t="s">
         <v>28</v>
       </c>
       <c r="G76" s="22"/>
       <c r="H76" s="12"/>
-      <c r="I76" s="12"/>
+      <c r="I76" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J76" s="12"/>
       <c r="K76" s="12"/>
       <c r="L76" s="12"/>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" s="18" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B77" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C77" s="8"/>
       <c r="D77" s="31" t="s">
+        <v>175</v>
+      </c>
+      <c r="E77" s="30" t="s">
         <v>176</v>
-      </c>
-      <c r="E77" s="30" t="s">
-        <v>177</v>
       </c>
       <c r="F77" s="21" t="s">
         <v>28</v>
       </c>
       <c r="G77" s="22"/>
       <c r="H77" s="12"/>
-      <c r="I77" s="12"/>
+      <c r="I77" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J77" s="12"/>
       <c r="K77" s="12"/>
       <c r="L77" s="12"/>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78" s="18" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B78" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C78" s="8"/>
       <c r="D78" s="31" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E78" s="30" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F78" s="21" t="s">
         <v>28</v>
       </c>
       <c r="G78" s="22"/>
       <c r="H78" s="12"/>
-      <c r="I78" s="12"/>
+      <c r="I78" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J78" s="12"/>
       <c r="K78" s="12"/>
       <c r="L78" s="12"/>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79" s="7">
         <v>34</v>
       </c>
@@ -3343,94 +3481,102 @@
       </c>
       <c r="C79" s="8"/>
       <c r="D79" s="31" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E79" s="30" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F79" s="21" t="s">
         <v>28</v>
       </c>
       <c r="G79" s="22"/>
       <c r="H79" s="12"/>
-      <c r="I79" s="12"/>
+      <c r="I79" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J79" s="12"/>
       <c r="K79" s="12"/>
       <c r="L79" s="12"/>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80" s="18" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B80" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C80" s="8"/>
       <c r="D80" s="31" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E80" s="30" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F80" s="21" t="s">
         <v>28</v>
       </c>
       <c r="G80" s="22"/>
       <c r="H80" s="12"/>
-      <c r="I80" s="12"/>
+      <c r="I80" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J80" s="12"/>
       <c r="K80" s="12"/>
       <c r="L80" s="12"/>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81" s="18" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B81" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C81" s="8"/>
       <c r="D81" s="31" t="s">
+        <v>186</v>
+      </c>
+      <c r="E81" s="30" t="s">
         <v>187</v>
-      </c>
-      <c r="E81" s="30" t="s">
-        <v>188</v>
       </c>
       <c r="F81" s="21" t="s">
         <v>28</v>
       </c>
       <c r="G81" s="22"/>
       <c r="H81" s="12"/>
-      <c r="I81" s="12"/>
+      <c r="I81" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J81" s="12"/>
       <c r="K81" s="12"/>
       <c r="L81" s="12"/>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82" s="18" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B82" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C82" s="8"/>
       <c r="D82" s="31" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E82" s="30" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F82" s="21" t="s">
         <v>28</v>
       </c>
       <c r="G82" s="22"/>
       <c r="H82" s="12"/>
-      <c r="I82" s="12"/>
+      <c r="I82" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J82" s="12"/>
       <c r="K82" s="12"/>
       <c r="L82" s="12"/>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83" s="7">
         <v>35</v>
       </c>
@@ -3454,7 +3600,7 @@
       <c r="K83" s="12"/>
       <c r="L83" s="12"/>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84" s="7">
         <v>36</v>
       </c>
@@ -3473,12 +3619,14 @@
       </c>
       <c r="G84" s="22"/>
       <c r="H84" s="12"/>
-      <c r="I84" s="12"/>
+      <c r="I84" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J84" s="12"/>
       <c r="K84" s="12"/>
       <c r="L84" s="12"/>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A85" s="7">
         <v>37</v>
       </c>
@@ -3497,12 +3645,14 @@
       </c>
       <c r="G85" s="22"/>
       <c r="H85" s="12"/>
-      <c r="I85" s="12"/>
+      <c r="I85" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J85" s="12"/>
       <c r="K85" s="12"/>
       <c r="L85" s="12"/>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A86" s="7">
         <v>38</v>
       </c>
@@ -3528,7 +3678,7 @@
       <c r="K86" s="12"/>
       <c r="L86" s="12"/>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A87" s="18" t="s">
         <v>67</v>
       </c>
@@ -3549,12 +3699,14 @@
       </c>
       <c r="G87" s="22"/>
       <c r="H87" s="12"/>
-      <c r="I87" s="12"/>
+      <c r="I87" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J87" s="12"/>
       <c r="K87" s="12"/>
       <c r="L87" s="12"/>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A88" s="18" t="s">
         <v>68</v>
       </c>
@@ -3571,16 +3723,18 @@
         <v>101</v>
       </c>
       <c r="F88" s="21" t="s">
-        <v>121</v>
+        <v>37</v>
       </c>
       <c r="G88" s="22"/>
       <c r="H88" s="12"/>
-      <c r="I88" s="12"/>
+      <c r="I88" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J88" s="12"/>
       <c r="K88" s="12"/>
       <c r="L88" s="12"/>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A89" s="18" t="s">
         <v>69</v>
       </c>
@@ -3601,12 +3755,14 @@
       </c>
       <c r="G89" s="22"/>
       <c r="H89" s="12"/>
-      <c r="I89" s="12"/>
+      <c r="I89" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J89" s="12"/>
       <c r="K89" s="12"/>
       <c r="L89" s="12"/>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A90" s="18" t="s">
         <v>70</v>
       </c>
@@ -3623,16 +3779,18 @@
         <v>102</v>
       </c>
       <c r="F90" s="21" t="s">
-        <v>121</v>
+        <v>37</v>
       </c>
       <c r="G90" s="22"/>
       <c r="H90" s="12"/>
-      <c r="I90" s="12"/>
+      <c r="I90" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J90" s="12"/>
       <c r="K90" s="12"/>
       <c r="L90" s="12"/>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A91" s="18" t="s">
         <v>71</v>
       </c>
@@ -3653,12 +3811,14 @@
       </c>
       <c r="G91" s="22"/>
       <c r="H91" s="12"/>
-      <c r="I91" s="12"/>
+      <c r="I91" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J91" s="12"/>
       <c r="K91" s="12"/>
       <c r="L91" s="12"/>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A92" s="18" t="s">
         <v>72</v>
       </c>
@@ -3675,16 +3835,18 @@
         <v>103</v>
       </c>
       <c r="F92" s="21" t="s">
-        <v>121</v>
+        <v>37</v>
       </c>
       <c r="G92" s="22"/>
       <c r="H92" s="12"/>
-      <c r="I92" s="12"/>
+      <c r="I92" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J92" s="12"/>
       <c r="K92" s="12"/>
       <c r="L92" s="12"/>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A93" s="18" t="s">
         <v>73</v>
       </c>
@@ -3708,7 +3870,7 @@
       <c r="K93" s="12"/>
       <c r="L93" s="12"/>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A94" s="18" t="s">
         <v>74</v>
       </c>
@@ -3729,12 +3891,14 @@
       </c>
       <c r="G94" s="22"/>
       <c r="H94" s="12"/>
-      <c r="I94" s="12"/>
+      <c r="I94" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J94" s="12"/>
       <c r="K94" s="12"/>
       <c r="L94" s="12"/>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A95" s="18" t="s">
         <v>75</v>
       </c>
@@ -3751,16 +3915,18 @@
         <v>104</v>
       </c>
       <c r="F95" s="21" t="s">
-        <v>121</v>
+        <v>37</v>
       </c>
       <c r="G95" s="22"/>
       <c r="H95" s="12"/>
-      <c r="I95" s="12"/>
+      <c r="I95" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J95" s="12"/>
       <c r="K95" s="12"/>
       <c r="L95" s="12"/>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A96" s="7">
         <v>44</v>
       </c>
@@ -3769,22 +3935,24 @@
       </c>
       <c r="C96" s="8"/>
       <c r="D96" s="29" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E96" s="30" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F96" s="21" t="s">
         <v>28</v>
       </c>
       <c r="G96" s="22"/>
       <c r="H96" s="19"/>
-      <c r="I96" s="19"/>
+      <c r="I96" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J96" s="19"/>
       <c r="K96" s="19"/>
       <c r="L96" s="19"/>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A97" s="7">
         <v>45</v>
       </c>
@@ -3793,22 +3961,24 @@
       </c>
       <c r="C97" s="8"/>
       <c r="D97" s="32" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E97" s="30" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F97" s="21" t="s">
         <v>28</v>
       </c>
       <c r="G97" s="22"/>
       <c r="H97" s="19"/>
-      <c r="I97" s="19"/>
+      <c r="I97" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J97" s="19"/>
       <c r="K97" s="19"/>
       <c r="L97" s="19"/>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A98" s="7">
         <v>46</v>
       </c>
@@ -3817,22 +3987,24 @@
       </c>
       <c r="C98" s="8"/>
       <c r="D98" s="31" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E98" s="30" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F98" s="21" t="s">
         <v>28</v>
       </c>
       <c r="G98" s="22"/>
       <c r="H98" s="19"/>
-      <c r="I98" s="19"/>
+      <c r="I98" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J98" s="19"/>
       <c r="K98" s="19"/>
       <c r="L98" s="19"/>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A99" s="7">
         <v>47</v>
       </c>
@@ -3841,22 +4013,24 @@
       </c>
       <c r="C99" s="8"/>
       <c r="D99" s="31" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E99" s="30" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F99" s="21" t="s">
         <v>28</v>
       </c>
       <c r="G99" s="22"/>
       <c r="H99" s="19"/>
-      <c r="I99" s="19"/>
+      <c r="I99" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J99" s="19"/>
       <c r="K99" s="19"/>
       <c r="L99" s="19"/>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A100" s="7">
         <v>48</v>
       </c>
@@ -3865,22 +4039,24 @@
       </c>
       <c r="C100" s="8"/>
       <c r="D100" s="31" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E100" s="30" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F100" s="21" t="s">
         <v>28</v>
       </c>
       <c r="G100" s="22"/>
       <c r="H100" s="19"/>
-      <c r="I100" s="19"/>
+      <c r="I100" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J100" s="19"/>
       <c r="K100" s="19"/>
       <c r="L100" s="19"/>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A101" s="7">
         <v>49</v>
       </c>
@@ -3889,22 +4065,24 @@
       </c>
       <c r="C101" s="8"/>
       <c r="D101" s="31" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E101" s="30" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F101" s="21" t="s">
         <v>28</v>
       </c>
       <c r="G101" s="22"/>
       <c r="H101" s="19"/>
-      <c r="I101" s="19"/>
+      <c r="I101" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J101" s="19"/>
       <c r="K101" s="19"/>
       <c r="L101" s="19"/>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A102" s="7">
         <v>50</v>
       </c>
@@ -3928,7 +4106,7 @@
       <c r="K102" s="19"/>
       <c r="L102" s="19"/>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A103" s="7">
         <v>51</v>
       </c>
@@ -3947,12 +4125,14 @@
       </c>
       <c r="G103" s="22"/>
       <c r="H103" s="19"/>
-      <c r="I103" s="19"/>
+      <c r="I103" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J103" s="19"/>
       <c r="K103" s="19"/>
       <c r="L103" s="19"/>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A104" s="7">
         <v>52</v>
       </c>
@@ -3971,12 +4151,15 @@
       </c>
       <c r="G104" s="22"/>
       <c r="H104" s="19"/>
-      <c r="I104" s="19"/>
+      <c r="I104" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J104" s="19"/>
       <c r="K104" s="19"/>
       <c r="L104" s="19"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:L104" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Dala 4397 eu taxonomy data model update (#642)
Update EU Taxonomy non-financials model

Co-authored-by: Tayfun Dertsiz <Tayfun.Dertsiz@d-fine.com>
Co-authored-by: LaurinStrelow <1918073+LaurinStrelow@users.noreply.github.com>
Co-authored-by: Dennis Groh <dennis.groh@d-fine.com>
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/euTaxonomyNonFinancials/EutaxonomyNonFinancials.xlsx
+++ b/dataland-framework-toolbox/inputs/euTaxonomyNonFinancials/EutaxonomyNonFinancials.xlsx
@@ -5,18 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d93476\Dataland\dataland-framework-toolbox\inputs\euTaxonomyNonFinancials\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dataland\dataland_alternative\dataland-framework-toolbox\inputs\euTaxonomyNonFinancials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7387AC29-C78D-42C7-81C5-A3856B3BB672}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E51E730-3590-4F62-A449-A34DD2DB217B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57490" yWindow="-10800" windowWidth="38620" windowHeight="21220" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Framework Data Model" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Framework Data Model'!$A$1:$L$66</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Framework Data Model'!$A$1:$L$104</definedName>
     <definedName name="IQ_CH">110000</definedName>
     <definedName name="IQ_CQ">5000</definedName>
     <definedName name="IQ_CY">10000</definedName>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="234">
   <si>
     <t>Field Identifier</t>
   </si>
@@ -162,9 +162,6 @@
     <t>Revenue</t>
   </si>
   <si>
-    <t>Grade of the substantial contribution criterion fulfillment</t>
-  </si>
-  <si>
     <t>Extended</t>
   </si>
   <si>
@@ -219,24 +216,6 @@
     <t>Aligned Share</t>
   </si>
   <si>
-    <t>Substantial Contribution to Climate Change Mitigation In Percent</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to Climate Change Adaptation In Percent</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to Sustainable Use and Protection of Water and Marine Resources In Percent</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to Transition to a Circular Economy In Percent</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to Pollution Prevention and Control In Percent</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to Protection and Restoration of Biodiversity and Ecosystems In Percent</t>
-  </si>
-  <si>
     <t>Aligned Activities</t>
   </si>
   <si>
@@ -442,13 +421,352 @@
   </si>
   <si>
     <t>Custom EuTaxonomyAlignedActivitiesComponent</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Climate Change Mitigation In Percent - Eligible</t>
+  </si>
+  <si>
+    <t>Taxonomy-eligible proportion of revenue substantially contributing to climate change mitigation</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Climate Change Mitigation In Percent - Aligned</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned proportion of revenue substantially contributing to climate change mitigation</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Climate Change Mitigation In Percent - Of which use of proceeds</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned use of proceeds share substantially contributing to climate change mitigation</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Climate Change Mitigation In Percent - Enabling Share</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned and enabling proportion of revenue substantially contributing to climate change mitigation</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Climate Change Mitigation In Percent - Transitional Share</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned and transitional proportion of revenue substantially contributing to climate change mitigation</t>
+  </si>
+  <si>
+    <t>14.1</t>
+  </si>
+  <si>
+    <t>14.1.1</t>
+  </si>
+  <si>
+    <t>14.1.2</t>
+  </si>
+  <si>
+    <t>14.1.3</t>
+  </si>
+  <si>
+    <t>15.1</t>
+  </si>
+  <si>
+    <t>15.1.1</t>
+  </si>
+  <si>
+    <t>15.1.2</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Climate Change Adaptation In Percent - Eligible</t>
+  </si>
+  <si>
+    <t>Taxonomy-eligible proportion of revenue substantially contributing to climate change adaptation</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Climate Change Adaptation In Percent - Aligned</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned proportion of revenue substantially contributing to climate change adaptation</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Climate Change Adaptation In Percent - Of which use of proceeds</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned use of proceeds share substantially contributing to climate change adaptation</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Climate Change Adaptation In Percent - Enabling Share</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned and enabling proportion of revenue substantially contributing to climate change adaptation</t>
+  </si>
+  <si>
+    <t>16.1</t>
+  </si>
+  <si>
+    <t>16.1.1</t>
+  </si>
+  <si>
+    <t>16.1.2</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Sustainable Use and Protection of Water and Marine Resources In Percent - Eligible</t>
+  </si>
+  <si>
+    <t>Taxonomy-eligible proportion of revenue substantially contributing to sustainable use and protection of water and marine resources</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Sustainable Use and Protection of Water and Marine Resources In Percent - Aligned</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned proportion of revenue substantially contributing to sustainable use and protection of water and marine resources</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Sustainable Use and Protection of Water and Marine Resources In Percent - Of which use of proceeds</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned use of proceeds share substantially contributing to sustainable use and protection of water and marine resources</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Sustainable Use and Protection of Water and Marine Resources In Percent - Enabling Share</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned and enabling proportion of revenue substantially contributing to sustainable use and protection of water and marine resources</t>
+  </si>
+  <si>
+    <t>17.1</t>
+  </si>
+  <si>
+    <t>17.1.1</t>
+  </si>
+  <si>
+    <t>17.1.2</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Transition to a Circular Economy In Percent - Eligible</t>
+  </si>
+  <si>
+    <t>Taxonomy-eligible proportion of revenue substantially contributing to circular economy</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Transition to a Circular Economy In Percent - Aligned</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned proportion of revenue substantially contributing to circular economy</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Transition to a Circular Economy In Percent - Of which use of proceeds</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned use of proceeds share substantially contributing to circular economy</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Transition to a Circular Economy In Percent - Enabling Share</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned and enabling proportion of revenue substantially contributing to circular economy</t>
+  </si>
+  <si>
+    <t>18.1</t>
+  </si>
+  <si>
+    <t>18.1.1</t>
+  </si>
+  <si>
+    <t>18.1.2</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Pollution Prevention and Control In Percent - Eligible</t>
+  </si>
+  <si>
+    <t>Taxonomy-eligible proportion of revenue substantially contributing to pollution prevention and control</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Pollution Prevention and Control In Percent - Aligned</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned proportion of revenue substantially contributing to pollution prevention and control</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Pollution Prevention and Control In Percent - Of which use of proceeds</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned use of proceeds share substantially contributing to pollution prevention and control</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Pollution Prevention and Control In Percent - Enabling Share</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned and enabling proportion of revenue substantially contributing to pollution prevention and control</t>
+  </si>
+  <si>
+    <t>19.1</t>
+  </si>
+  <si>
+    <t>19.1.1</t>
+  </si>
+  <si>
+    <t>19.1.2</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Protection and Restoration of Biodiversity and Ecosystems In Percent - Eligible</t>
+  </si>
+  <si>
+    <t>Taxonomy-eligible proportion of revenue substantially contributing to protection and restoration of biodiversity and ecosystems</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Protection and Restoration of Biodiversity and Ecosystems In Percent - Aligned</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned proportion of revenue substantially contributing to protection and restoration of biodiversity and ecosystems</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Protection and Restoration of Biodiversity and Ecosystems In Percent - Of which use of proceeds</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned use of proceeds share substantially contributing to protection and restoration of biodiversity and ecosystems</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Protection and Restoration of Biodiversity and Ecosystems In Percent - Enabling Share</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned and enabling proportion of revenue substantially contributing to protection and restoration of biodiversity and ecosystems</t>
+  </si>
+  <si>
+    <t>29.1</t>
+  </si>
+  <si>
+    <t>29.1.1</t>
+  </si>
+  <si>
+    <t>29.1.2</t>
+  </si>
+  <si>
+    <t>29.1.3</t>
+  </si>
+  <si>
+    <t>Taxonomy-eligible proportion of CapEx substantially contributing to climate change mitigation</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned proportion of CapEx substantially contributing to climate change mitigation</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned and enabling proportion of CapEx substantially contributing to climate change mitigation</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned and transitional proportion of CapEx substantially contributing to climate change mitigation</t>
+  </si>
+  <si>
+    <t>30.1</t>
+  </si>
+  <si>
+    <t>30.1.1</t>
+  </si>
+  <si>
+    <t>30.1.2</t>
+  </si>
+  <si>
+    <t>Taxonomy-eligible proportion of CapEx substantially contributing to climate change adaptation</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned proportion of CapEx substantially contributing to climate change adaptation</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned and enabling proportion of CapEx substantially contributing to climate change adaptation</t>
+  </si>
+  <si>
+    <t>31.1</t>
+  </si>
+  <si>
+    <t>31.1.1</t>
+  </si>
+  <si>
+    <t>31.1.2</t>
+  </si>
+  <si>
+    <t>Taxonomy-eligible proportion of CapEx substantially contributing to sustainable use and protection of water and marine resources</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned proportion of CapEx substantially contributing to sustainable use and protection of water and marine resources</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned and enabling proportion of CapEx substantially contributing to sustainable use and protection of water and marine resources</t>
+  </si>
+  <si>
+    <t>32.1</t>
+  </si>
+  <si>
+    <t>32.1.1</t>
+  </si>
+  <si>
+    <t>32.1.2</t>
+  </si>
+  <si>
+    <t>Taxonomy-eligible proportion of CapEx substantially contributing to circular economy</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned proportion of CapEx substantially contributing to circular economy</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned and enabling proportion of CapEx substantially contributing to circular economy</t>
+  </si>
+  <si>
+    <t>Taxonomy-eligible proportion of CapEx substantially contributing to pollution prevention and control</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned proportion of CapEx substantially contributing to pollution prevention and control</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned and enabling proportion of CapEx substantially contributing to pollution prevention and control</t>
+  </si>
+  <si>
+    <t>Taxonomy-eligible proportion of CapEx substantially contributing to protection and restoration of biodiversity and ecosystems</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned proportion of CapEx substantially contributing to protection and restoration of biodiversity and ecosystems</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned and enabling proportion of CapEx substantially contributing to protection and restoration of biodiversity and ecosystems</t>
+  </si>
+  <si>
+    <t>33.1</t>
+  </si>
+  <si>
+    <t>33.1.1</t>
+  </si>
+  <si>
+    <t>33.1.2</t>
+  </si>
+  <si>
+    <t>34.1</t>
+  </si>
+  <si>
+    <t>34.1.1</t>
+  </si>
+  <si>
+    <t>34.1.2</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned proportion of OpEx substantially contributing to climate change mitigation</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned proportion of OpEx substantially contributing to climate change adaptation</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned proportion of OpEx substantially contributing to sustainable use and protection of water and marine resources</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned proportion of OpEx substantially contributing to circular economy</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned proportion of OpEx substantially contributing to pollution prevention and control</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned proportion of OpEx substantially contributing to protection and restoration of biodiversity and ecosystems</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -520,8 +838,18 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -578,14 +906,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor rgb="FFF2F2F2"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor rgb="FFEFEFEF"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -748,7 +1070,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -796,8 +1118,10 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="10" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -872,6 +1196,10 @@
       <rgbColor rgb="00333399"/>
       <rgbColor rgb="00333333"/>
     </indexedColors>
+    <mruColors>
+      <color rgb="FFF2F2F2"/>
+      <color rgb="FFF2FFFF"/>
+    </mruColors>
   </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1060,23 +1388,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L66"/>
+  <dimension ref="A1:L104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14:F95"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="20.21875" customWidth="1"/>
-    <col min="4" max="4" width="70.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="77.88671875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="44.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="26.21875" customWidth="1"/>
-    <col min="8" max="12" width="14.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" customWidth="1"/>
+    <col min="4" max="4" width="95.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="77.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="44.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="26.28515625" customWidth="1"/>
+    <col min="8" max="12" width="14.28515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1114,7 +1442,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
         <v>0</v>
       </c>
@@ -1132,17 +1460,17 @@
         <v>17</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="H2" s="11"/>
       <c r="I2" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J2" s="12"/>
       <c r="K2" s="12"/>
       <c r="L2" s="12"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
       <c r="B3" s="8" t="s">
         <v>12</v>
@@ -1160,13 +1488,13 @@
       <c r="G3" s="10"/>
       <c r="H3" s="11"/>
       <c r="I3" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J3" s="12"/>
       <c r="K3" s="12"/>
       <c r="L3" s="12"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>1</v>
       </c>
@@ -1188,13 +1516,13 @@
       </c>
       <c r="H4" s="12"/>
       <c r="I4" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J4" s="11"/>
       <c r="K4" s="11"/>
       <c r="L4" s="12"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>2</v>
       </c>
@@ -1216,13 +1544,13 @@
       </c>
       <c r="H5" s="12"/>
       <c r="I5" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J5" s="12"/>
       <c r="K5" s="12"/>
       <c r="L5" s="12"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>3</v>
       </c>
@@ -1244,13 +1572,13 @@
       </c>
       <c r="H6" s="12"/>
       <c r="I6" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J6" s="12"/>
       <c r="K6" s="12"/>
       <c r="L6" s="12"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>4</v>
       </c>
@@ -1265,7 +1593,7 @@
         <v>32</v>
       </c>
       <c r="F7" s="27" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="G7" s="26" t="s">
         <v>14</v>
@@ -1276,7 +1604,7 @@
       <c r="K7" s="12"/>
       <c r="L7" s="12"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>5</v>
       </c>
@@ -1291,18 +1619,18 @@
         <v>27</v>
       </c>
       <c r="F8" s="20" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="G8" s="22"/>
       <c r="H8" s="12"/>
       <c r="I8" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J8" s="12"/>
       <c r="K8" s="12"/>
       <c r="L8" s="12"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>6</v>
       </c>
@@ -1311,11 +1639,11 @@
       </c>
       <c r="C9" s="8"/>
       <c r="D9" s="14" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="E9" s="12"/>
       <c r="F9" s="20" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="G9" s="23" t="s">
         <v>14</v>
@@ -1326,7 +1654,7 @@
       <c r="K9" s="12"/>
       <c r="L9" s="12"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>8</v>
       </c>
@@ -1335,35 +1663,35 @@
       </c>
       <c r="C10" s="8"/>
       <c r="D10" s="15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E10" s="19" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="F10" s="21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G10" s="22"/>
       <c r="H10" s="12"/>
       <c r="I10" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J10" s="12"/>
       <c r="K10" s="12"/>
       <c r="L10" s="12"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C11" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="15" t="s">
         <v>40</v>
-      </c>
-      <c r="D11" s="15" t="s">
-        <v>41</v>
       </c>
       <c r="E11" s="19"/>
       <c r="F11" s="21" t="s">
@@ -1372,55 +1700,55 @@
       <c r="G11" s="22"/>
       <c r="H11" s="12"/>
       <c r="I11" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J11" s="12"/>
       <c r="K11" s="12"/>
       <c r="L11" s="12"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E12" s="28" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="F12" s="21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G12" s="22"/>
       <c r="H12" s="12"/>
       <c r="I12" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J12" s="12"/>
       <c r="K12" s="12"/>
       <c r="L12" s="12"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="F13" s="21" t="s">
         <v>28</v>
@@ -1428,55 +1756,55 @@
       <c r="G13" s="22"/>
       <c r="H13" s="12"/>
       <c r="I13" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J13" s="12"/>
       <c r="K13" s="12"/>
       <c r="L13" s="12"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="F14" s="21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G14" s="22"/>
       <c r="H14" s="12"/>
       <c r="I14" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J14" s="12"/>
       <c r="K14" s="12"/>
       <c r="L14" s="12"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B15" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E15" s="28" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="F15" s="21" t="s">
         <v>28</v>
@@ -1484,56 +1812,56 @@
       <c r="G15" s="22"/>
       <c r="H15" s="12"/>
       <c r="I15" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J15" s="12"/>
       <c r="K15" s="12"/>
       <c r="L15" s="12"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E16" s="28" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="F16" s="21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G16" s="22"/>
       <c r="H16" s="12"/>
       <c r="I16" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J16" s="12"/>
       <c r="K16" s="12"/>
       <c r="L16" s="12"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C17" s="8"/>
       <c r="D17" s="15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E17" s="28" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="F17" s="21" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="G17" s="22"/>
       <c r="H17" s="12"/>
@@ -1542,21 +1870,21 @@
       <c r="K17" s="12"/>
       <c r="L17" s="12"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="B18" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="F18" s="21" t="s">
         <v>28</v>
@@ -1564,41 +1892,41 @@
       <c r="G18" s="22"/>
       <c r="H18" s="12"/>
       <c r="I18" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J18" s="12"/>
       <c r="K18" s="12"/>
       <c r="L18" s="12"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="18" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="F19" s="21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G19" s="22"/>
       <c r="H19" s="12"/>
       <c r="I19" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J19" s="12"/>
       <c r="K19" s="12"/>
       <c r="L19" s="12"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="7">
         <v>14</v>
       </c>
@@ -1606,11 +1934,11 @@
         <v>33</v>
       </c>
       <c r="C20" s="8"/>
-      <c r="D20" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="E20" s="12" t="s">
-        <v>34</v>
+      <c r="D20" s="29" t="s">
+        <v>121</v>
+      </c>
+      <c r="E20" s="30" t="s">
+        <v>122</v>
       </c>
       <c r="F20" s="21" t="s">
         <v>28</v>
@@ -1618,25 +1946,25 @@
       <c r="G20" s="22"/>
       <c r="H20" s="12"/>
       <c r="I20" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J20" s="12"/>
       <c r="K20" s="12"/>
       <c r="L20" s="12"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A21" s="7">
-        <v>15</v>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="18" t="s">
+        <v>131</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C21" s="8"/>
-      <c r="D21" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="E21" s="12" t="s">
-        <v>34</v>
+      <c r="D21" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="E21" s="30" t="s">
+        <v>124</v>
       </c>
       <c r="F21" s="21" t="s">
         <v>28</v>
@@ -1644,25 +1972,25 @@
       <c r="G21" s="22"/>
       <c r="H21" s="12"/>
       <c r="I21" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J21" s="12"/>
       <c r="K21" s="12"/>
       <c r="L21" s="12"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A22" s="7">
-        <v>16</v>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="18" t="s">
+        <v>132</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C22" s="8"/>
-      <c r="D22" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="E22" s="12" t="s">
-        <v>34</v>
+      <c r="D22" s="31" t="s">
+        <v>125</v>
+      </c>
+      <c r="E22" s="30" t="s">
+        <v>126</v>
       </c>
       <c r="F22" s="21" t="s">
         <v>28</v>
@@ -1670,25 +1998,25 @@
       <c r="G22" s="22"/>
       <c r="H22" s="12"/>
       <c r="I22" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J22" s="12"/>
       <c r="K22" s="12"/>
       <c r="L22" s="12"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A23" s="7">
-        <v>17</v>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="18" t="s">
+        <v>133</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C23" s="8"/>
-      <c r="D23" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="E23" s="12" t="s">
-        <v>34</v>
+      <c r="D23" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="E23" s="30" t="s">
+        <v>128</v>
       </c>
       <c r="F23" s="21" t="s">
         <v>28</v>
@@ -1696,25 +2024,25 @@
       <c r="G23" s="22"/>
       <c r="H23" s="12"/>
       <c r="I23" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J23" s="12"/>
       <c r="K23" s="12"/>
       <c r="L23" s="12"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A24" s="7">
-        <v>18</v>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="18" t="s">
+        <v>134</v>
       </c>
       <c r="B24" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C24" s="8"/>
-      <c r="D24" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="E24" s="12" t="s">
-        <v>34</v>
+      <c r="D24" s="29" t="s">
+        <v>129</v>
+      </c>
+      <c r="E24" s="30" t="s">
+        <v>130</v>
       </c>
       <c r="F24" s="21" t="s">
         <v>28</v>
@@ -1722,25 +2050,25 @@
       <c r="G24" s="22"/>
       <c r="H24" s="12"/>
       <c r="I24" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J24" s="12"/>
       <c r="K24" s="12"/>
       <c r="L24" s="12"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="7">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B25" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C25" s="8"/>
-      <c r="D25" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="E25" s="12" t="s">
-        <v>34</v>
+      <c r="D25" s="32" t="s">
+        <v>138</v>
+      </c>
+      <c r="E25" s="30" t="s">
+        <v>139</v>
       </c>
       <c r="F25" s="21" t="s">
         <v>28</v>
@@ -1748,49 +2076,51 @@
       <c r="G25" s="22"/>
       <c r="H25" s="12"/>
       <c r="I25" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J25" s="12"/>
       <c r="K25" s="12"/>
       <c r="L25" s="12"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A26" s="7">
-        <v>20</v>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="18" t="s">
+        <v>135</v>
       </c>
       <c r="B26" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C26" s="8"/>
-      <c r="D26" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="E26" s="28" t="s">
-        <v>89</v>
+      <c r="D26" s="32" t="s">
+        <v>140</v>
+      </c>
+      <c r="E26" s="30" t="s">
+        <v>141</v>
       </c>
       <c r="F26" s="21" t="s">
-        <v>127</v>
+        <v>28</v>
       </c>
       <c r="G26" s="22"/>
       <c r="H26" s="12"/>
-      <c r="I26" s="12"/>
+      <c r="I26" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J26" s="12"/>
       <c r="K26" s="12"/>
       <c r="L26" s="12"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A27" s="7">
-        <v>21</v>
-      </c>
-      <c r="B27" s="16" t="s">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="B27" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C27" s="16"/>
-      <c r="D27" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="E27" s="28" t="s">
-        <v>92</v>
+      <c r="C27" s="8"/>
+      <c r="D27" s="31" t="s">
+        <v>142</v>
+      </c>
+      <c r="E27" s="30" t="s">
+        <v>143</v>
       </c>
       <c r="F27" s="21" t="s">
         <v>28</v>
@@ -1798,25 +2128,25 @@
       <c r="G27" s="22"/>
       <c r="H27" s="12"/>
       <c r="I27" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J27" s="12"/>
       <c r="K27" s="12"/>
       <c r="L27" s="12"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A28" s="7">
-        <v>22</v>
-      </c>
-      <c r="B28" s="16" t="s">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="B28" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C28" s="16"/>
-      <c r="D28" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="E28" s="28" t="s">
-        <v>93</v>
+      <c r="C28" s="8"/>
+      <c r="D28" s="31" t="s">
+        <v>144</v>
+      </c>
+      <c r="E28" s="30" t="s">
+        <v>145</v>
       </c>
       <c r="F28" s="21" t="s">
         <v>28</v>
@@ -1824,53 +2154,51 @@
       <c r="G28" s="22"/>
       <c r="H28" s="12"/>
       <c r="I28" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J28" s="12"/>
       <c r="K28" s="12"/>
       <c r="L28" s="12"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="7">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C29" s="8"/>
-      <c r="D29" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="E29" s="28" t="s">
-        <v>94</v>
+      <c r="D29" s="31" t="s">
+        <v>149</v>
+      </c>
+      <c r="E29" s="30" t="s">
+        <v>150</v>
       </c>
       <c r="F29" s="21" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="G29" s="22"/>
       <c r="H29" s="12"/>
       <c r="I29" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J29" s="12"/>
       <c r="K29" s="12"/>
       <c r="L29" s="12"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="18" t="s">
-        <v>67</v>
+        <v>146</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C30" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="D30" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="E30" s="29" t="s">
-        <v>118</v>
+        <v>33</v>
+      </c>
+      <c r="C30" s="8"/>
+      <c r="D30" s="31" t="s">
+        <v>151</v>
+      </c>
+      <c r="E30" s="30" t="s">
+        <v>152</v>
       </c>
       <c r="F30" s="21" t="s">
         <v>28</v>
@@ -1878,55 +2206,51 @@
       <c r="G30" s="22"/>
       <c r="H30" s="12"/>
       <c r="I30" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J30" s="12"/>
       <c r="K30" s="12"/>
       <c r="L30" s="12"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="18" t="s">
-        <v>68</v>
+        <v>147</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C31" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="D31" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="E31" s="29" t="s">
-        <v>107</v>
+        <v>33</v>
+      </c>
+      <c r="C31" s="8"/>
+      <c r="D31" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="E31" s="30" t="s">
+        <v>154</v>
       </c>
       <c r="F31" s="21" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="G31" s="22"/>
       <c r="H31" s="12"/>
       <c r="I31" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J31" s="12"/>
       <c r="K31" s="12"/>
       <c r="L31" s="12"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="18" t="s">
-        <v>65</v>
+        <v>148</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C32" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="D32" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="E32" s="28" t="s">
-        <v>119</v>
+        <v>33</v>
+      </c>
+      <c r="C32" s="8"/>
+      <c r="D32" s="31" t="s">
+        <v>155</v>
+      </c>
+      <c r="E32" s="30" t="s">
+        <v>156</v>
       </c>
       <c r="F32" s="21" t="s">
         <v>28</v>
@@ -1934,55 +2258,51 @@
       <c r="G32" s="22"/>
       <c r="H32" s="12"/>
       <c r="I32" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J32" s="12"/>
       <c r="K32" s="12"/>
       <c r="L32" s="12"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A33" s="18" t="s">
-        <v>66</v>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" s="7">
+        <v>17</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C33" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="D33" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="E33" s="28" t="s">
-        <v>102</v>
+        <v>33</v>
+      </c>
+      <c r="C33" s="8"/>
+      <c r="D33" s="31" t="s">
+        <v>160</v>
+      </c>
+      <c r="E33" s="30" t="s">
+        <v>161</v>
       </c>
       <c r="F33" s="21" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="G33" s="22"/>
       <c r="H33" s="12"/>
       <c r="I33" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J33" s="12"/>
       <c r="K33" s="12"/>
       <c r="L33" s="12"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="18" t="s">
-        <v>69</v>
+        <v>157</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C34" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="D34" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="E34" s="29" t="s">
-        <v>120</v>
+        <v>33</v>
+      </c>
+      <c r="C34" s="8"/>
+      <c r="D34" s="31" t="s">
+        <v>162</v>
+      </c>
+      <c r="E34" s="30" t="s">
+        <v>163</v>
       </c>
       <c r="F34" s="21" t="s">
         <v>28</v>
@@ -1990,79 +2310,77 @@
       <c r="G34" s="22"/>
       <c r="H34" s="12"/>
       <c r="I34" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J34" s="12"/>
       <c r="K34" s="12"/>
       <c r="L34" s="12"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="18" t="s">
-        <v>70</v>
+        <v>158</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C35" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="D35" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="E35" s="29" t="s">
-        <v>106</v>
+        <v>33</v>
+      </c>
+      <c r="C35" s="8"/>
+      <c r="D35" s="31" t="s">
+        <v>164</v>
+      </c>
+      <c r="E35" s="30" t="s">
+        <v>165</v>
       </c>
       <c r="F35" s="21" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="G35" s="22"/>
       <c r="H35" s="12"/>
       <c r="I35" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J35" s="12"/>
       <c r="K35" s="12"/>
       <c r="L35" s="12"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="18" t="s">
-        <v>71</v>
+        <v>159</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C36" s="8"/>
-      <c r="D36" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="E36" s="29" t="s">
-        <v>105</v>
+      <c r="D36" s="31" t="s">
+        <v>166</v>
+      </c>
+      <c r="E36" s="30" t="s">
+        <v>167</v>
       </c>
       <c r="F36" s="21" t="s">
-        <v>126</v>
+        <v>28</v>
       </c>
       <c r="G36" s="22"/>
       <c r="H36" s="12"/>
-      <c r="I36" s="12"/>
+      <c r="I36" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J36" s="12"/>
       <c r="K36" s="12"/>
       <c r="L36" s="12"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A37" s="18" t="s">
-        <v>72</v>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" s="7">
+        <v>18</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C37" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="D37" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="E37" s="29" t="s">
-        <v>121</v>
+        <v>33</v>
+      </c>
+      <c r="C37" s="8"/>
+      <c r="D37" s="31" t="s">
+        <v>171</v>
+      </c>
+      <c r="E37" s="30" t="s">
+        <v>172</v>
       </c>
       <c r="F37" s="21" t="s">
         <v>28</v>
@@ -2070,53 +2388,51 @@
       <c r="G37" s="22"/>
       <c r="H37" s="12"/>
       <c r="I37" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J37" s="12"/>
       <c r="K37" s="12"/>
       <c r="L37" s="12"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="18" t="s">
-        <v>73</v>
+        <v>168</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C38" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="D38" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="E38" s="29" t="s">
-        <v>103</v>
+        <v>33</v>
+      </c>
+      <c r="C38" s="8"/>
+      <c r="D38" s="31" t="s">
+        <v>173</v>
+      </c>
+      <c r="E38" s="30" t="s">
+        <v>174</v>
       </c>
       <c r="F38" s="21" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="G38" s="22"/>
       <c r="H38" s="12"/>
       <c r="I38" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J38" s="12"/>
       <c r="K38" s="12"/>
       <c r="L38" s="12"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A39" s="7">
-        <v>29</v>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" s="18" t="s">
+        <v>169</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C39" s="8"/>
-      <c r="D39" s="15" t="s">
-        <v>53</v>
+      <c r="D39" s="31" t="s">
+        <v>175</v>
       </c>
       <c r="E39" s="30" t="s">
-        <v>34</v>
+        <v>176</v>
       </c>
       <c r="F39" s="21" t="s">
         <v>28</v>
@@ -2124,25 +2440,25 @@
       <c r="G39" s="22"/>
       <c r="H39" s="12"/>
       <c r="I39" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J39" s="12"/>
       <c r="K39" s="12"/>
       <c r="L39" s="12"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A40" s="7">
-        <v>30</v>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40" s="18" t="s">
+        <v>170</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C40" s="8"/>
-      <c r="D40" s="15" t="s">
-        <v>54</v>
+      <c r="D40" s="31" t="s">
+        <v>177</v>
       </c>
       <c r="E40" s="30" t="s">
-        <v>34</v>
+        <v>178</v>
       </c>
       <c r="F40" s="21" t="s">
         <v>28</v>
@@ -2150,25 +2466,25 @@
       <c r="G40" s="22"/>
       <c r="H40" s="12"/>
       <c r="I40" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J40" s="12"/>
       <c r="K40" s="12"/>
       <c r="L40" s="12"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="7">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C41" s="8"/>
-      <c r="D41" s="15" t="s">
-        <v>55</v>
+      <c r="D41" s="31" t="s">
+        <v>182</v>
       </c>
       <c r="E41" s="30" t="s">
-        <v>34</v>
+        <v>183</v>
       </c>
       <c r="F41" s="21" t="s">
         <v>28</v>
@@ -2176,25 +2492,25 @@
       <c r="G41" s="22"/>
       <c r="H41" s="12"/>
       <c r="I41" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J41" s="12"/>
       <c r="K41" s="12"/>
       <c r="L41" s="12"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A42" s="7">
-        <v>32</v>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42" s="18" t="s">
+        <v>179</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C42" s="8"/>
-      <c r="D42" s="15" t="s">
-        <v>56</v>
+      <c r="D42" s="31" t="s">
+        <v>184</v>
       </c>
       <c r="E42" s="30" t="s">
-        <v>34</v>
+        <v>185</v>
       </c>
       <c r="F42" s="21" t="s">
         <v>28</v>
@@ -2202,25 +2518,25 @@
       <c r="G42" s="22"/>
       <c r="H42" s="12"/>
       <c r="I42" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J42" s="12"/>
       <c r="K42" s="12"/>
       <c r="L42" s="12"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A43" s="7">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43" s="18" t="s">
+        <v>180</v>
+      </c>
+      <c r="B43" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B43" s="8" t="s">
-        <v>36</v>
-      </c>
       <c r="C43" s="8"/>
-      <c r="D43" s="15" t="s">
-        <v>57</v>
+      <c r="D43" s="31" t="s">
+        <v>186</v>
       </c>
       <c r="E43" s="30" t="s">
-        <v>34</v>
+        <v>187</v>
       </c>
       <c r="F43" s="21" t="s">
         <v>28</v>
@@ -2228,25 +2544,25 @@
       <c r="G43" s="22"/>
       <c r="H43" s="12"/>
       <c r="I43" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J43" s="12"/>
       <c r="K43" s="12"/>
       <c r="L43" s="12"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A44" s="7">
-        <v>34</v>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A44" s="18" t="s">
+        <v>181</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C44" s="8"/>
-      <c r="D44" s="15" t="s">
-        <v>58</v>
+      <c r="D44" s="31" t="s">
+        <v>188</v>
       </c>
       <c r="E44" s="30" t="s">
-        <v>34</v>
+        <v>189</v>
       </c>
       <c r="F44" s="21" t="s">
         <v>28</v>
@@ -2254,28 +2570,28 @@
       <c r="G44" s="22"/>
       <c r="H44" s="12"/>
       <c r="I44" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J44" s="12"/>
       <c r="K44" s="12"/>
       <c r="L44" s="12"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="7">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C45" s="8"/>
       <c r="D45" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="E45" s="29" t="s">
-        <v>104</v>
+        <v>52</v>
+      </c>
+      <c r="E45" s="28" t="s">
+        <v>82</v>
       </c>
       <c r="F45" s="21" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="G45" s="22"/>
       <c r="H45" s="12"/>
@@ -2284,19 +2600,19 @@
       <c r="K45" s="12"/>
       <c r="L45" s="12"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="7">
-        <v>36</v>
-      </c>
-      <c r="B46" s="8" t="s">
-        <v>36</v>
+        <v>21</v>
+      </c>
+      <c r="B46" s="16" t="s">
+        <v>33</v>
       </c>
       <c r="C46" s="16"/>
       <c r="D46" s="17" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="E46" s="28" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="F46" s="21" t="s">
         <v>28</v>
@@ -2304,25 +2620,25 @@
       <c r="G46" s="22"/>
       <c r="H46" s="12"/>
       <c r="I46" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J46" s="12"/>
       <c r="K46" s="12"/>
       <c r="L46" s="12"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
-        <v>37</v>
-      </c>
-      <c r="B47" s="8" t="s">
-        <v>36</v>
+        <v>22</v>
+      </c>
+      <c r="B47" s="16" t="s">
+        <v>33</v>
       </c>
       <c r="C47" s="16"/>
       <c r="D47" s="17" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="E47" s="28" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="F47" s="21" t="s">
         <v>28</v>
@@ -2330,53 +2646,53 @@
       <c r="G47" s="22"/>
       <c r="H47" s="12"/>
       <c r="I47" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J47" s="12"/>
       <c r="K47" s="12"/>
       <c r="L47" s="12"/>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="7">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C48" s="8"/>
       <c r="D48" s="15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E48" s="28" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="F48" s="21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G48" s="22"/>
       <c r="H48" s="12"/>
       <c r="I48" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J48" s="12"/>
       <c r="K48" s="12"/>
       <c r="L48" s="12"/>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="18" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C49" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D49" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="D49" s="15" t="s">
-        <v>41</v>
-      </c>
       <c r="E49" s="28" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="F49" s="21" t="s">
         <v>28</v>
@@ -2384,55 +2700,55 @@
       <c r="G49" s="22"/>
       <c r="H49" s="12"/>
       <c r="I49" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J49" s="12"/>
       <c r="K49" s="12"/>
       <c r="L49" s="12"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="18" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="B50" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C50" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D50" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="E50" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="F50" s="21" t="s">
         <v>37</v>
-      </c>
-      <c r="C50" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="D50" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="E50" s="28" t="s">
-        <v>108</v>
-      </c>
-      <c r="F50" s="21" t="s">
-        <v>38</v>
       </c>
       <c r="G50" s="22"/>
       <c r="H50" s="12"/>
       <c r="I50" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J50" s="12"/>
       <c r="K50" s="12"/>
       <c r="L50" s="12"/>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="18" t="s">
-        <v>76</v>
+        <v>58</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D51" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E51" s="28" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="F51" s="21" t="s">
         <v>28</v>
@@ -2440,55 +2756,55 @@
       <c r="G51" s="22"/>
       <c r="H51" s="12"/>
       <c r="I51" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J51" s="12"/>
       <c r="K51" s="12"/>
       <c r="L51" s="12"/>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="18" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="B52" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C52" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D52" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="E52" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="F52" s="21" t="s">
         <v>37</v>
-      </c>
-      <c r="C52" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="D52" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="E52" s="28" t="s">
-        <v>109</v>
-      </c>
-      <c r="F52" s="21" t="s">
-        <v>38</v>
       </c>
       <c r="G52" s="22"/>
       <c r="H52" s="12"/>
       <c r="I52" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J52" s="12"/>
       <c r="K52" s="12"/>
       <c r="L52" s="12"/>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="18" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D53" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E53" s="28" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="F53" s="21" t="s">
         <v>28</v>
@@ -2496,56 +2812,56 @@
       <c r="G53" s="22"/>
       <c r="H53" s="12"/>
       <c r="I53" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J53" s="12"/>
       <c r="K53" s="12"/>
       <c r="L53" s="12"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="18" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="B54" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C54" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D54" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="E54" s="28" t="s">
+        <v>99</v>
+      </c>
+      <c r="F54" s="21" t="s">
         <v>37</v>
-      </c>
-      <c r="C54" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="D54" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="E54" s="28" t="s">
-        <v>110</v>
-      </c>
-      <c r="F54" s="21" t="s">
-        <v>38</v>
       </c>
       <c r="G54" s="22"/>
       <c r="H54" s="12"/>
       <c r="I54" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J54" s="12"/>
       <c r="K54" s="12"/>
       <c r="L54" s="12"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="18" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C55" s="8"/>
       <c r="D55" s="15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E55" s="28" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F55" s="21" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="G55" s="22"/>
       <c r="H55" s="12"/>
@@ -2554,21 +2870,21 @@
       <c r="K55" s="12"/>
       <c r="L55" s="12"/>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="18" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D56" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E56" s="28" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="F56" s="21" t="s">
         <v>28</v>
@@ -2576,274 +2892,1275 @@
       <c r="G56" s="22"/>
       <c r="H56" s="12"/>
       <c r="I56" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J56" s="12"/>
       <c r="K56" s="12"/>
       <c r="L56" s="12"/>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="18" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="B57" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C57" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D57" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="E57" s="28" t="s">
+        <v>96</v>
+      </c>
+      <c r="F57" s="21" t="s">
         <v>37</v>
-      </c>
-      <c r="C57" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="D57" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="E57" s="28" t="s">
-        <v>111</v>
-      </c>
-      <c r="F57" s="21" t="s">
-        <v>38</v>
       </c>
       <c r="G57" s="22"/>
       <c r="H57" s="12"/>
       <c r="I57" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J57" s="12"/>
       <c r="K57" s="12"/>
       <c r="L57" s="12"/>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="7">
+        <v>29</v>
+      </c>
+      <c r="B58" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C58" s="8"/>
+      <c r="D58" s="29" t="s">
+        <v>121</v>
+      </c>
+      <c r="E58" s="30" t="s">
+        <v>194</v>
+      </c>
+      <c r="F58" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G58" s="22"/>
+      <c r="H58" s="12"/>
+      <c r="I58" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="J58" s="12"/>
+      <c r="K58" s="12"/>
+      <c r="L58" s="12"/>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A59" s="18" t="s">
+        <v>190</v>
+      </c>
+      <c r="B59" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C59" s="8"/>
+      <c r="D59" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="E59" s="30" t="s">
+        <v>195</v>
+      </c>
+      <c r="F59" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G59" s="22"/>
+      <c r="H59" s="12"/>
+      <c r="I59" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="J59" s="12"/>
+      <c r="K59" s="12"/>
+      <c r="L59" s="12"/>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A60" s="18" t="s">
+        <v>191</v>
+      </c>
+      <c r="B60" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C60" s="8"/>
+      <c r="D60" s="31" t="s">
+        <v>125</v>
+      </c>
+      <c r="E60" s="30" t="s">
+        <v>126</v>
+      </c>
+      <c r="F60" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G60" s="22"/>
+      <c r="H60" s="12"/>
+      <c r="I60" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="J60" s="12"/>
+      <c r="K60" s="12"/>
+      <c r="L60" s="12"/>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A61" s="18" t="s">
+        <v>192</v>
+      </c>
+      <c r="B61" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C61" s="8"/>
+      <c r="D61" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="E61" s="30" t="s">
+        <v>196</v>
+      </c>
+      <c r="F61" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G61" s="22"/>
+      <c r="H61" s="12"/>
+      <c r="I61" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="J61" s="12"/>
+      <c r="K61" s="12"/>
+      <c r="L61" s="12"/>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A62" s="18" t="s">
+        <v>193</v>
+      </c>
+      <c r="B62" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C62" s="8"/>
+      <c r="D62" s="29" t="s">
+        <v>129</v>
+      </c>
+      <c r="E62" s="30" t="s">
+        <v>197</v>
+      </c>
+      <c r="F62" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G62" s="22"/>
+      <c r="H62" s="12"/>
+      <c r="I62" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="J62" s="12"/>
+      <c r="K62" s="12"/>
+      <c r="L62" s="12"/>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A63" s="7">
+        <v>30</v>
+      </c>
+      <c r="B63" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C63" s="8"/>
+      <c r="D63" s="32" t="s">
+        <v>138</v>
+      </c>
+      <c r="E63" s="30" t="s">
+        <v>201</v>
+      </c>
+      <c r="F63" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G63" s="22"/>
+      <c r="H63" s="12"/>
+      <c r="I63" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="J63" s="12"/>
+      <c r="K63" s="12"/>
+      <c r="L63" s="12"/>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A64" s="18" t="s">
+        <v>198</v>
+      </c>
+      <c r="B64" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C64" s="8"/>
+      <c r="D64" s="32" t="s">
+        <v>140</v>
+      </c>
+      <c r="E64" s="30" t="s">
+        <v>202</v>
+      </c>
+      <c r="F64" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G64" s="22"/>
+      <c r="H64" s="12"/>
+      <c r="I64" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="J64" s="12"/>
+      <c r="K64" s="12"/>
+      <c r="L64" s="12"/>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A65" s="18" t="s">
+        <v>199</v>
+      </c>
+      <c r="B65" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C65" s="8"/>
+      <c r="D65" s="31" t="s">
+        <v>142</v>
+      </c>
+      <c r="E65" s="30" t="s">
+        <v>143</v>
+      </c>
+      <c r="F65" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G65" s="22"/>
+      <c r="H65" s="12"/>
+      <c r="I65" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="J65" s="12"/>
+      <c r="K65" s="12"/>
+      <c r="L65" s="12"/>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A66" s="18" t="s">
+        <v>200</v>
+      </c>
+      <c r="B66" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C66" s="8"/>
+      <c r="D66" s="31" t="s">
+        <v>144</v>
+      </c>
+      <c r="E66" s="30" t="s">
+        <v>203</v>
+      </c>
+      <c r="F66" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G66" s="22"/>
+      <c r="H66" s="12"/>
+      <c r="I66" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="J66" s="12"/>
+      <c r="K66" s="12"/>
+      <c r="L66" s="12"/>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A67" s="7">
+        <v>31</v>
+      </c>
+      <c r="B67" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C67" s="8"/>
+      <c r="D67" s="31" t="s">
+        <v>149</v>
+      </c>
+      <c r="E67" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="F67" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G67" s="22"/>
+      <c r="H67" s="12"/>
+      <c r="I67" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="J67" s="12"/>
+      <c r="K67" s="12"/>
+      <c r="L67" s="12"/>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A68" s="18" t="s">
+        <v>204</v>
+      </c>
+      <c r="B68" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C68" s="8"/>
+      <c r="D68" s="31" t="s">
+        <v>151</v>
+      </c>
+      <c r="E68" s="30" t="s">
+        <v>208</v>
+      </c>
+      <c r="F68" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G68" s="22"/>
+      <c r="H68" s="12"/>
+      <c r="I68" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="J68" s="12"/>
+      <c r="K68" s="12"/>
+      <c r="L68" s="12"/>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A69" s="18" t="s">
+        <v>205</v>
+      </c>
+      <c r="B69" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C69" s="8"/>
+      <c r="D69" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="E69" s="30" t="s">
+        <v>154</v>
+      </c>
+      <c r="F69" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G69" s="22"/>
+      <c r="H69" s="12"/>
+      <c r="I69" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="J69" s="12"/>
+      <c r="K69" s="12"/>
+      <c r="L69" s="12"/>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A70" s="18" t="s">
+        <v>206</v>
+      </c>
+      <c r="B70" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C70" s="8"/>
+      <c r="D70" s="31" t="s">
+        <v>155</v>
+      </c>
+      <c r="E70" s="30" t="s">
+        <v>209</v>
+      </c>
+      <c r="F70" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G70" s="22"/>
+      <c r="H70" s="12"/>
+      <c r="I70" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="J70" s="12"/>
+      <c r="K70" s="12"/>
+      <c r="L70" s="12"/>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A71" s="7">
+        <v>32</v>
+      </c>
+      <c r="B71" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C71" s="8"/>
+      <c r="D71" s="31" t="s">
+        <v>160</v>
+      </c>
+      <c r="E71" s="30" t="s">
+        <v>213</v>
+      </c>
+      <c r="F71" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G71" s="22"/>
+      <c r="H71" s="12"/>
+      <c r="I71" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="J71" s="12"/>
+      <c r="K71" s="12"/>
+      <c r="L71" s="12"/>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A72" s="18" t="s">
+        <v>210</v>
+      </c>
+      <c r="B72" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C72" s="8"/>
+      <c r="D72" s="31" t="s">
+        <v>162</v>
+      </c>
+      <c r="E72" s="30" t="s">
+        <v>214</v>
+      </c>
+      <c r="F72" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G72" s="22"/>
+      <c r="H72" s="12"/>
+      <c r="I72" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="J72" s="12"/>
+      <c r="K72" s="12"/>
+      <c r="L72" s="12"/>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A73" s="18" t="s">
+        <v>211</v>
+      </c>
+      <c r="B73" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C73" s="8"/>
+      <c r="D73" s="31" t="s">
+        <v>164</v>
+      </c>
+      <c r="E73" s="30" t="s">
+        <v>165</v>
+      </c>
+      <c r="F73" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G73" s="22"/>
+      <c r="H73" s="12"/>
+      <c r="I73" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="J73" s="12"/>
+      <c r="K73" s="12"/>
+      <c r="L73" s="12"/>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A74" s="18" t="s">
+        <v>212</v>
+      </c>
+      <c r="B74" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C74" s="8"/>
+      <c r="D74" s="31" t="s">
+        <v>166</v>
+      </c>
+      <c r="E74" s="30" t="s">
+        <v>215</v>
+      </c>
+      <c r="F74" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G74" s="22"/>
+      <c r="H74" s="12"/>
+      <c r="I74" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="J74" s="12"/>
+      <c r="K74" s="12"/>
+      <c r="L74" s="12"/>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A75" s="7">
+        <v>33</v>
+      </c>
+      <c r="B75" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C75" s="8"/>
+      <c r="D75" s="31" t="s">
+        <v>171</v>
+      </c>
+      <c r="E75" s="30" t="s">
+        <v>216</v>
+      </c>
+      <c r="F75" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G75" s="22"/>
+      <c r="H75" s="12"/>
+      <c r="I75" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="J75" s="12"/>
+      <c r="K75" s="12"/>
+      <c r="L75" s="12"/>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A76" s="18" t="s">
+        <v>222</v>
+      </c>
+      <c r="B76" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C76" s="8"/>
+      <c r="D76" s="31" t="s">
+        <v>173</v>
+      </c>
+      <c r="E76" s="30" t="s">
+        <v>217</v>
+      </c>
+      <c r="F76" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G76" s="22"/>
+      <c r="H76" s="12"/>
+      <c r="I76" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="J76" s="12"/>
+      <c r="K76" s="12"/>
+      <c r="L76" s="12"/>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A77" s="18" t="s">
+        <v>223</v>
+      </c>
+      <c r="B77" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C77" s="8"/>
+      <c r="D77" s="31" t="s">
+        <v>175</v>
+      </c>
+      <c r="E77" s="30" t="s">
+        <v>176</v>
+      </c>
+      <c r="F77" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G77" s="22"/>
+      <c r="H77" s="12"/>
+      <c r="I77" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="J77" s="12"/>
+      <c r="K77" s="12"/>
+      <c r="L77" s="12"/>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A78" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="B78" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C78" s="8"/>
+      <c r="D78" s="31" t="s">
+        <v>177</v>
+      </c>
+      <c r="E78" s="30" t="s">
+        <v>218</v>
+      </c>
+      <c r="F78" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G78" s="22"/>
+      <c r="H78" s="12"/>
+      <c r="I78" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="J78" s="12"/>
+      <c r="K78" s="12"/>
+      <c r="L78" s="12"/>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A79" s="7">
+        <v>34</v>
+      </c>
+      <c r="B79" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C79" s="8"/>
+      <c r="D79" s="31" t="s">
+        <v>182</v>
+      </c>
+      <c r="E79" s="30" t="s">
+        <v>219</v>
+      </c>
+      <c r="F79" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G79" s="22"/>
+      <c r="H79" s="12"/>
+      <c r="I79" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="J79" s="12"/>
+      <c r="K79" s="12"/>
+      <c r="L79" s="12"/>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A80" s="18" t="s">
+        <v>225</v>
+      </c>
+      <c r="B80" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C80" s="8"/>
+      <c r="D80" s="31" t="s">
+        <v>184</v>
+      </c>
+      <c r="E80" s="30" t="s">
+        <v>220</v>
+      </c>
+      <c r="F80" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G80" s="22"/>
+      <c r="H80" s="12"/>
+      <c r="I80" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="J80" s="12"/>
+      <c r="K80" s="12"/>
+      <c r="L80" s="12"/>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A81" s="18" t="s">
+        <v>226</v>
+      </c>
+      <c r="B81" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C81" s="8"/>
+      <c r="D81" s="31" t="s">
+        <v>186</v>
+      </c>
+      <c r="E81" s="30" t="s">
+        <v>187</v>
+      </c>
+      <c r="F81" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G81" s="22"/>
+      <c r="H81" s="12"/>
+      <c r="I81" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="J81" s="12"/>
+      <c r="K81" s="12"/>
+      <c r="L81" s="12"/>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A82" s="18" t="s">
+        <v>227</v>
+      </c>
+      <c r="B82" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C82" s="8"/>
+      <c r="D82" s="31" t="s">
+        <v>188</v>
+      </c>
+      <c r="E82" s="30" t="s">
+        <v>221</v>
+      </c>
+      <c r="F82" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G82" s="22"/>
+      <c r="H82" s="12"/>
+      <c r="I82" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="J82" s="12"/>
+      <c r="K82" s="12"/>
+      <c r="L82" s="12"/>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A83" s="7">
+        <v>35</v>
+      </c>
+      <c r="B83" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C83" s="8"/>
+      <c r="D83" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="E83" s="28" t="s">
+        <v>97</v>
+      </c>
+      <c r="F83" s="21" t="s">
+        <v>120</v>
+      </c>
+      <c r="G83" s="22"/>
+      <c r="H83" s="12"/>
+      <c r="I83" s="12"/>
+      <c r="J83" s="12"/>
+      <c r="K83" s="12"/>
+      <c r="L83" s="12"/>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A84" s="7">
+        <v>36</v>
+      </c>
+      <c r="B84" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C84" s="16"/>
+      <c r="D84" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="E84" s="28" t="s">
+        <v>88</v>
+      </c>
+      <c r="F84" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G84" s="22"/>
+      <c r="H84" s="12"/>
+      <c r="I84" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="J84" s="12"/>
+      <c r="K84" s="12"/>
+      <c r="L84" s="12"/>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A85" s="7">
+        <v>37</v>
+      </c>
+      <c r="B85" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C85" s="16"/>
+      <c r="D85" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="E85" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="F85" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G85" s="22"/>
+      <c r="H85" s="12"/>
+      <c r="I85" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="J85" s="12"/>
+      <c r="K85" s="12"/>
+      <c r="L85" s="12"/>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A86" s="7">
+        <v>38</v>
+      </c>
+      <c r="B86" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C86" s="8"/>
+      <c r="D86" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="E86" s="28" t="s">
+        <v>90</v>
+      </c>
+      <c r="F86" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="G86" s="22"/>
+      <c r="H86" s="12"/>
+      <c r="I86" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="J86" s="12"/>
+      <c r="K86" s="12"/>
+      <c r="L86" s="12"/>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A87" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B87" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C87" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D87" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="E87" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="F87" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G87" s="22"/>
+      <c r="H87" s="12"/>
+      <c r="I87" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="J87" s="12"/>
+      <c r="K87" s="12"/>
+      <c r="L87" s="12"/>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A88" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="B88" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C88" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D88" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="E88" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="F88" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="G88" s="22"/>
+      <c r="H88" s="12"/>
+      <c r="I88" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="J88" s="12"/>
+      <c r="K88" s="12"/>
+      <c r="L88" s="12"/>
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A89" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="B89" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C89" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="B58" s="8" t="s">
+      <c r="D89" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="E89" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="F89" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G89" s="22"/>
+      <c r="H89" s="12"/>
+      <c r="I89" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="J89" s="12"/>
+      <c r="K89" s="12"/>
+      <c r="L89" s="12"/>
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A90" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="B90" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C90" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D90" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="E90" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="F90" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="C58" s="8"/>
-      <c r="D58" s="15" t="s">
+      <c r="G90" s="22"/>
+      <c r="H90" s="12"/>
+      <c r="I90" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="J90" s="12"/>
+      <c r="K90" s="12"/>
+      <c r="L90" s="12"/>
+    </row>
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A91" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="B91" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C91" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D91" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="E91" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="F91" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G91" s="22"/>
+      <c r="H91" s="12"/>
+      <c r="I91" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="J91" s="12"/>
+      <c r="K91" s="12"/>
+      <c r="L91" s="12"/>
+    </row>
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A92" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="B92" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C92" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D92" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="E92" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="F92" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="G92" s="22"/>
+      <c r="H92" s="12"/>
+      <c r="I92" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="J92" s="12"/>
+      <c r="K92" s="12"/>
+      <c r="L92" s="12"/>
+    </row>
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A93" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="B93" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C93" s="8"/>
+      <c r="D93" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="E93" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="F93" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="G93" s="22"/>
+      <c r="H93" s="12"/>
+      <c r="I93" s="12"/>
+      <c r="J93" s="12"/>
+      <c r="K93" s="12"/>
+      <c r="L93" s="12"/>
+    </row>
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A94" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="B94" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C94" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D94" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="E94" s="28" t="s">
+        <v>118</v>
+      </c>
+      <c r="F94" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G94" s="22"/>
+      <c r="H94" s="12"/>
+      <c r="I94" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="J94" s="12"/>
+      <c r="K94" s="12"/>
+      <c r="L94" s="12"/>
+    </row>
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A95" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="B95" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C95" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D95" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="E95" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="F95" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="G95" s="22"/>
+      <c r="H95" s="12"/>
+      <c r="I95" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="J95" s="12"/>
+      <c r="K95" s="12"/>
+      <c r="L95" s="12"/>
+    </row>
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A96" s="7">
+        <v>44</v>
+      </c>
+      <c r="B96" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C96" s="8"/>
+      <c r="D96" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="E96" s="30" t="s">
+        <v>228</v>
+      </c>
+      <c r="F96" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G96" s="22"/>
+      <c r="H96" s="19"/>
+      <c r="I96" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="J96" s="19"/>
+      <c r="K96" s="19"/>
+      <c r="L96" s="19"/>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A97" s="7">
+        <v>45</v>
+      </c>
+      <c r="B97" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C97" s="8"/>
+      <c r="D97" s="32" t="s">
+        <v>140</v>
+      </c>
+      <c r="E97" s="30" t="s">
+        <v>229</v>
+      </c>
+      <c r="F97" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G97" s="22"/>
+      <c r="H97" s="19"/>
+      <c r="I97" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="J97" s="19"/>
+      <c r="K97" s="19"/>
+      <c r="L97" s="19"/>
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A98" s="7">
+        <v>46</v>
+      </c>
+      <c r="B98" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C98" s="8"/>
+      <c r="D98" s="31" t="s">
+        <v>151</v>
+      </c>
+      <c r="E98" s="30" t="s">
+        <v>230</v>
+      </c>
+      <c r="F98" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G98" s="22"/>
+      <c r="H98" s="19"/>
+      <c r="I98" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="J98" s="19"/>
+      <c r="K98" s="19"/>
+      <c r="L98" s="19"/>
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A99" s="7">
+        <v>47</v>
+      </c>
+      <c r="B99" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C99" s="8"/>
+      <c r="D99" s="31" t="s">
+        <v>162</v>
+      </c>
+      <c r="E99" s="30" t="s">
+        <v>231</v>
+      </c>
+      <c r="F99" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G99" s="22"/>
+      <c r="H99" s="19"/>
+      <c r="I99" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="J99" s="19"/>
+      <c r="K99" s="19"/>
+      <c r="L99" s="19"/>
+    </row>
+    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A100" s="7">
+        <v>48</v>
+      </c>
+      <c r="B100" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C100" s="8"/>
+      <c r="D100" s="31" t="s">
+        <v>173</v>
+      </c>
+      <c r="E100" s="30" t="s">
+        <v>232</v>
+      </c>
+      <c r="F100" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G100" s="22"/>
+      <c r="H100" s="19"/>
+      <c r="I100" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="J100" s="19"/>
+      <c r="K100" s="19"/>
+      <c r="L100" s="19"/>
+    </row>
+    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A101" s="7">
+        <v>49</v>
+      </c>
+      <c r="B101" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C101" s="8"/>
+      <c r="D101" s="31" t="s">
+        <v>184</v>
+      </c>
+      <c r="E101" s="30" t="s">
+        <v>233</v>
+      </c>
+      <c r="F101" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G101" s="22"/>
+      <c r="H101" s="19"/>
+      <c r="I101" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="J101" s="19"/>
+      <c r="K101" s="19"/>
+      <c r="L101" s="19"/>
+    </row>
+    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A102" s="7">
+        <v>50</v>
+      </c>
+      <c r="B102" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C102" s="8"/>
+      <c r="D102" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="E102" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="F102" s="21" t="s">
+        <v>120</v>
+      </c>
+      <c r="G102" s="22"/>
+      <c r="H102" s="19"/>
+      <c r="I102" s="19"/>
+      <c r="J102" s="19"/>
+      <c r="K102" s="19"/>
+      <c r="L102" s="19"/>
+    </row>
+    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A103" s="7">
+        <v>51</v>
+      </c>
+      <c r="B103" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C103" s="16"/>
+      <c r="D103" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="E58" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="F58" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="G58" s="22"/>
-      <c r="H58" s="19"/>
-      <c r="I58" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="J58" s="19"/>
-      <c r="K58" s="19"/>
-      <c r="L58" s="19"/>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A59" s="7">
-        <v>45</v>
-      </c>
-      <c r="B59" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C59" s="8"/>
-      <c r="D59" s="15" t="s">
+      <c r="E103" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="F103" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G103" s="22"/>
+      <c r="H103" s="19"/>
+      <c r="I103" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="J103" s="19"/>
+      <c r="K103" s="19"/>
+      <c r="L103" s="19"/>
+    </row>
+    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A104" s="7">
+        <v>52</v>
+      </c>
+      <c r="B104" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C104" s="16"/>
+      <c r="D104" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="E59" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="F59" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="G59" s="22"/>
-      <c r="H59" s="19"/>
-      <c r="I59" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="J59" s="19"/>
-      <c r="K59" s="19"/>
-      <c r="L59" s="19"/>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A60" s="7">
-        <v>46</v>
-      </c>
-      <c r="B60" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C60" s="8"/>
-      <c r="D60" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="E60" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="F60" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="G60" s="22"/>
-      <c r="H60" s="19"/>
-      <c r="I60" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="J60" s="19"/>
-      <c r="K60" s="19"/>
-      <c r="L60" s="19"/>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A61" s="7">
-        <v>47</v>
-      </c>
-      <c r="B61" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C61" s="8"/>
-      <c r="D61" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="E61" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="F61" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="G61" s="22"/>
-      <c r="H61" s="19"/>
-      <c r="I61" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="J61" s="19"/>
-      <c r="K61" s="19"/>
-      <c r="L61" s="19"/>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A62" s="7">
-        <v>48</v>
-      </c>
-      <c r="B62" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C62" s="8"/>
-      <c r="D62" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="E62" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="F62" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="G62" s="22"/>
-      <c r="H62" s="19"/>
-      <c r="I62" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="J62" s="19"/>
-      <c r="K62" s="19"/>
-      <c r="L62" s="19"/>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A63" s="7">
-        <v>49</v>
-      </c>
-      <c r="B63" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C63" s="8"/>
-      <c r="D63" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="E63" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="F63" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="G63" s="22"/>
-      <c r="H63" s="19"/>
-      <c r="I63" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="J63" s="19"/>
-      <c r="K63" s="19"/>
-      <c r="L63" s="19"/>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A64" s="7">
-        <v>50</v>
-      </c>
-      <c r="B64" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C64" s="8"/>
-      <c r="D64" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="E64" s="28" t="s">
-        <v>98</v>
-      </c>
-      <c r="F64" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="G64" s="22"/>
-      <c r="H64" s="19"/>
-      <c r="I64" s="12"/>
-      <c r="J64" s="19"/>
-      <c r="K64" s="19"/>
-      <c r="L64" s="19"/>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A65" s="7">
-        <v>51</v>
-      </c>
-      <c r="B65" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C65" s="16"/>
-      <c r="D65" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="E65" s="28" t="s">
-        <v>100</v>
-      </c>
-      <c r="F65" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="G65" s="22"/>
-      <c r="H65" s="19"/>
-      <c r="I65" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="J65" s="19"/>
-      <c r="K65" s="19"/>
-      <c r="L65" s="19"/>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A66" s="7">
-        <v>52</v>
-      </c>
-      <c r="B66" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C66" s="16"/>
-      <c r="D66" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="E66" s="28" t="s">
-        <v>101</v>
-      </c>
-      <c r="F66" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="G66" s="22"/>
-      <c r="H66" s="19"/>
-      <c r="I66" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="J66" s="19"/>
-      <c r="K66" s="19"/>
-      <c r="L66" s="19"/>
+      <c r="E104" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="F104" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G104" s="22"/>
+      <c r="H104" s="19"/>
+      <c r="I104" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="J104" s="19"/>
+      <c r="K104" s="19"/>
+      <c r="L104" s="19"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L66" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:L104" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
eu taxo non financials data model update.
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/euTaxonomyNonFinancials/EutaxonomyNonFinancials.xlsx
+++ b/dataland-framework-toolbox/inputs/euTaxonomyNonFinancials/EutaxonomyNonFinancials.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dataland\dataland_alternative\dataland-framework-toolbox\inputs\euTaxonomyNonFinancials\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dataland\Dataland\dataland-framework-toolbox\inputs\euTaxonomyNonFinancials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E51E730-3590-4F62-A449-A34DD2DB217B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C67B78E9-299A-43AD-B2BD-B46716BA59B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57490" yWindow="-10800" windowWidth="38620" windowHeight="21220" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Framework Data Model" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Framework Data Model'!$A$1:$L$104</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Framework Data Model'!$A$1:$L$108</definedName>
     <definedName name="IQ_CH">110000</definedName>
     <definedName name="IQ_CQ">5000</definedName>
     <definedName name="IQ_CY">10000</definedName>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="242">
   <si>
     <t>Field Identifier</t>
   </si>
@@ -186,30 +186,12 @@
     <t>Absolute Share</t>
   </si>
   <si>
-    <t>9.1</t>
-  </si>
-  <si>
-    <t>9.2</t>
-  </si>
-  <si>
     <t>Eligible Share</t>
   </si>
   <si>
-    <t>10.1</t>
-  </si>
-  <si>
-    <t>10.2</t>
-  </si>
-  <si>
     <t>Non-Aligned Share</t>
   </si>
   <si>
-    <t>11.1</t>
-  </si>
-  <si>
-    <t>11.2</t>
-  </si>
-  <si>
     <t>Non-Aligned Activities</t>
   </si>
   <si>
@@ -225,548 +207,590 @@
     <t>Transitional Share In Percent</t>
   </si>
   <si>
-    <t>12</t>
-  </si>
-  <si>
     <t>13.1</t>
   </si>
   <si>
     <t>13.2</t>
   </si>
   <si>
-    <t>25.1</t>
-  </si>
-  <si>
-    <t>25.2</t>
-  </si>
-  <si>
-    <t>24.1</t>
-  </si>
-  <si>
-    <t>24.2</t>
-  </si>
-  <si>
-    <t>26.1</t>
-  </si>
-  <si>
-    <t>26.2</t>
-  </si>
-  <si>
-    <t>27</t>
-  </si>
-  <si>
     <t>28.1</t>
   </si>
   <si>
+    <t>43.1</t>
+  </si>
+  <si>
+    <t>43.2</t>
+  </si>
+  <si>
+    <t>Referenced Reports</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>Deviation | No Deviation</t>
+  </si>
+  <si>
+    <t>Report Preupload</t>
+  </si>
+  <si>
+    <t>Custom EuTaxonomyAssuranceComponent</t>
+  </si>
+  <si>
+    <t>Total revenue per annum</t>
+  </si>
+  <si>
+    <t>Absolute value and share of the revenue per activity that is taxonomy-aligned, i.e., generated by an eligible economic activity that is making a substantial contribution to at least one of the climate and environmental objectives, while also doing no significant harm to the remaining objectives and meeting minimum standards on human rights and labour standards</t>
+  </si>
+  <si>
+    <t>Absolute value and share of the revenue per activity that is not taxonomy-aligned but eligible</t>
+  </si>
+  <si>
+    <t>Absolute value and share of the revenue that is not part of a plan to meet the DNSH criteria and make substantial contribution to any environmental objective</t>
+  </si>
+  <si>
+    <t>Share of the taxonomy-aligned revenue from total aligned revenue that is linked to activities that enable reduction of GHG in other sectors</t>
+  </si>
+  <si>
+    <t>Share of the taxonomy-aligned revenue from total aligned revenue that is linked to activities with significantly lower GHG emissions than the sector or industry average</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total CapEx for the reported year. Capital expenditures are non-consumable investments, e.g. for acquiring, upgrading, and maintaining physical assets such as property, plants, buildings, technology </t>
+  </si>
+  <si>
+    <t>Share of the taxonomy-aligned CapEx from total aligned CapEx that is linked to activities that enable reduction of GHG in other sectors</t>
+  </si>
+  <si>
+    <t>Share of the taxonomy-aligned CapEx from total aligned CapEx that is linked to activities with significantly lower GHG emissions than the sector or industry average</t>
+  </si>
+  <si>
+    <t>Total OpEx for the financial year. Operating expenses (OpEx) are shorter term expenses required to meet the ongoing operational costs of running a business.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Absolute value and share of taxonomy-aligned OpEx for the activity from total OpEx. </t>
+  </si>
+  <si>
+    <t>Absolute value and share of the OpEx per activity that is not taxonomy-aligned but eligible</t>
+  </si>
+  <si>
+    <t>Share of the taxonomy-aligned OpEx from total aligned OpEx that is linked to activities that enable reduction of GHG in other sectors</t>
+  </si>
+  <si>
+    <t>Share of the taxonomy-aligned OpEx from total aligned OpEx that is linked to activities with significantly lower GHG emissions than the sector or industry average</t>
+  </si>
+  <si>
+    <t>Absolute value of the total CapEx where the economic activity meets taxonomy criteria for substantial contribution to climate change mitigation and does no serious harm to the other environmental objectives (DNSH criteria)</t>
+  </si>
+  <si>
+    <t>Absolute value of CapEx that is taxonomy-aligned, i.e., generated by an eligible economic activity that is making a substantial contribution to at least one of the climate and environmental objectives, while also doing no significant harm to the remaining objectives and meeting minimum standards on human rights and labour standards.</t>
+  </si>
+  <si>
+    <t>Absolute value and share of the CapEx per activity that is taxonomy-aligned, i.e., generated by an eligible economic activity that is making a substantial contribution to at least one of the climate and environmental objectives, while also doing no significant harm to the remaining objectives and meeting minimum standards on human rights and labour standards</t>
+  </si>
+  <si>
+    <t>Absolute value and share of the CapEx per activity that is not taxonomy-aligned but eligible</t>
+  </si>
+  <si>
+    <t>Absolute value of the CapEx that is associated with non taxonomy-aligned but eligible activities</t>
+  </si>
+  <si>
+    <t>Absolute value of the CapEx that is not part of a plan to meet the DNSH criteria and make substantial contribution to any environmental objective</t>
+  </si>
+  <si>
+    <t>Absolute value of the OpEx that is not part of a plan to meet the DNSH criteria and make substantial contribution to any environmental objective</t>
+  </si>
+  <si>
+    <t>Absolute value of the OpEx that is part of a plan to meet the DNSH criteria and make substantial contribution to any environmental objective</t>
+  </si>
+  <si>
+    <t>Absolute value of the OpEx that is associated with non taxonomy-aligned but eligible activities</t>
+  </si>
+  <si>
+    <t>Absolute value of the OpEx that is associated with taxonomy-aligned activities. i.e., for an eligible economic activity that is making a substantial contribution to at least one of the climate and environmental objectives, while also doing no significant harm to the remaining objectives and meeting minimum standards on human rights and labour standards</t>
+  </si>
+  <si>
+    <t>Absolute value of the total eligible revenue that is taxonomy-aligned, i.e., generated by an eligible economic activity that is making a substantial contribution to at least one of the climate and environmental objectives, while also doing no significant harm to the remaining objectives and meeting minimum standards on human rights and labour standards. In same currency than total revenue.</t>
+  </si>
+  <si>
+    <t>Absolute value of the revenue that is associated with non taxonomy-aligned but eligible activities</t>
+  </si>
+  <si>
+    <t>Absolute value of the total eligible revenue in same currency than total revenue. Is part of the total revenue where the economic activity meets taxonomy criteria for substantial contribution to climate change mitigation and does no serious harm to the other environmental objectives (DNSH criteria).</t>
+  </si>
+  <si>
+    <t>Relative share of the total eligible revenue in same currency than total revenue. Is part of the total revenue where the economic activity meets taxonomy criteria for substantial contribution to climate change mitigation and does no serious harm to the other environmental objectives (DNSH criteria).</t>
+  </si>
+  <si>
+    <t>Relative share of the revenue that is associated with non taxonomy-aligned but eligible activities</t>
+  </si>
+  <si>
+    <t>Relative share of the total eligible revenue that is taxonomy-aligned, i.e., generated by an eligible economic activity that is making a substantial contribution to at least one of the climate and environmental objectives, while also doing no significant harm to the remaining objectives and meeting minimum standards on human rights and labour standards. In same currency than total revenue.</t>
+  </si>
+  <si>
+    <t>Relative share of the CapEx that is not part of a plan to meet the DNSH criteria and make substantial contribution to any environmental objective</t>
+  </si>
+  <si>
+    <t>Relative share of the total CapEx where the economic activity meets taxonomy criteria for substantial contribution to climate change mitigation and does no serious harm to the other environmental objectives (DNSH criteria)</t>
+  </si>
+  <si>
+    <t>Relative share of the CapEx that is associated with non taxonomy-aligned but eligible activities</t>
+  </si>
+  <si>
+    <t>Relative share of CapEx that is taxonomy-aligned, i.e., generated by an eligible economic activity that is making a substantial contribution to at least one of the climate and environmental objectives, while also doing no significant harm to the remaining objectives and meeting minimum standards on human rights and labour standards.</t>
+  </si>
+  <si>
+    <t>Relative share of the OpEx that is not part of a plan to meet the DNSH criteria and make substantial contribution to any environmental objective</t>
+  </si>
+  <si>
+    <t>Relative share of the OpEx that is part of a plan to meet the DNSH criteria and make substantial contribution to any environmental objective</t>
+  </si>
+  <si>
+    <t>Relative share of the OpEx that is associated with non taxonomy-aligned but eligible activities</t>
+  </si>
+  <si>
+    <t>Relative share of the OpEx that is associated with taxonomy-aligned activities. i.e., for an eligible economic activity that is making a substantial contribution to at least one of the climate and environmental objectives, while also doing no significant harm to the remaining objectives and meeting minimum standards on human rights and labour standards</t>
+  </si>
+  <si>
+    <t>Custom EuTaxonomyNonAlignedActivitiesComponent</t>
+  </si>
+  <si>
+    <t>Custom EuTaxonomyAlignedActivitiesComponent</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Climate Change Mitigation In Percent - Eligible</t>
+  </si>
+  <si>
+    <t>Taxonomy-eligible proportion of revenue substantially contributing to climate change mitigation</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Climate Change Mitigation In Percent - Aligned</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned proportion of revenue substantially contributing to climate change mitigation</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Climate Change Mitigation In Percent - Of which use of proceeds</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned use of proceeds share substantially contributing to climate change mitigation</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Climate Change Mitigation In Percent - Enabling Share</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned and enabling proportion of revenue substantially contributing to climate change mitigation</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Climate Change Mitigation In Percent - Transitional Share</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned and transitional proportion of revenue substantially contributing to climate change mitigation</t>
+  </si>
+  <si>
+    <t>14.1</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Climate Change Adaptation In Percent - Eligible</t>
+  </si>
+  <si>
+    <t>Taxonomy-eligible proportion of revenue substantially contributing to climate change adaptation</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Climate Change Adaptation In Percent - Aligned</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned proportion of revenue substantially contributing to climate change adaptation</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Climate Change Adaptation In Percent - Of which use of proceeds</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned use of proceeds share substantially contributing to climate change adaptation</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Climate Change Adaptation In Percent - Enabling Share</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned and enabling proportion of revenue substantially contributing to climate change adaptation</t>
+  </si>
+  <si>
+    <t>16.1</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Sustainable Use and Protection of Water and Marine Resources In Percent - Eligible</t>
+  </si>
+  <si>
+    <t>Taxonomy-eligible proportion of revenue substantially contributing to sustainable use and protection of water and marine resources</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Sustainable Use and Protection of Water and Marine Resources In Percent - Aligned</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned proportion of revenue substantially contributing to sustainable use and protection of water and marine resources</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Sustainable Use and Protection of Water and Marine Resources In Percent - Of which use of proceeds</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned use of proceeds share substantially contributing to sustainable use and protection of water and marine resources</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Sustainable Use and Protection of Water and Marine Resources In Percent - Enabling Share</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned and enabling proportion of revenue substantially contributing to sustainable use and protection of water and marine resources</t>
+  </si>
+  <si>
+    <t>17.1</t>
+  </si>
+  <si>
+    <t>17.1.1</t>
+  </si>
+  <si>
+    <t>17.1.2</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Transition to a Circular Economy In Percent - Eligible</t>
+  </si>
+  <si>
+    <t>Taxonomy-eligible proportion of revenue substantially contributing to circular economy</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Transition to a Circular Economy In Percent - Aligned</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned proportion of revenue substantially contributing to circular economy</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Transition to a Circular Economy In Percent - Of which use of proceeds</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned use of proceeds share substantially contributing to circular economy</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Transition to a Circular Economy In Percent - Enabling Share</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned and enabling proportion of revenue substantially contributing to circular economy</t>
+  </si>
+  <si>
+    <t>18.1</t>
+  </si>
+  <si>
+    <t>18.1.1</t>
+  </si>
+  <si>
+    <t>18.1.2</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Pollution Prevention and Control In Percent - Eligible</t>
+  </si>
+  <si>
+    <t>Taxonomy-eligible proportion of revenue substantially contributing to pollution prevention and control</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Pollution Prevention and Control In Percent - Aligned</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned proportion of revenue substantially contributing to pollution prevention and control</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Pollution Prevention and Control In Percent - Of which use of proceeds</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned use of proceeds share substantially contributing to pollution prevention and control</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Pollution Prevention and Control In Percent - Enabling Share</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned and enabling proportion of revenue substantially contributing to pollution prevention and control</t>
+  </si>
+  <si>
+    <t>19.1</t>
+  </si>
+  <si>
+    <t>19.1.1</t>
+  </si>
+  <si>
+    <t>19.1.2</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Protection and Restoration of Biodiversity and Ecosystems In Percent - Eligible</t>
+  </si>
+  <si>
+    <t>Taxonomy-eligible proportion of revenue substantially contributing to protection and restoration of biodiversity and ecosystems</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Protection and Restoration of Biodiversity and Ecosystems In Percent - Aligned</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned proportion of revenue substantially contributing to protection and restoration of biodiversity and ecosystems</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Protection and Restoration of Biodiversity and Ecosystems In Percent - Of which use of proceeds</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned use of proceeds share substantially contributing to protection and restoration of biodiversity and ecosystems</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Protection and Restoration of Biodiversity and Ecosystems In Percent - Enabling Share</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned and enabling proportion of revenue substantially contributing to protection and restoration of biodiversity and ecosystems</t>
+  </si>
+  <si>
+    <t>29.1</t>
+  </si>
+  <si>
+    <t>Taxonomy-eligible proportion of CapEx substantially contributing to climate change mitigation</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned proportion of CapEx substantially contributing to climate change mitigation</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned and enabling proportion of CapEx substantially contributing to climate change mitigation</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned and transitional proportion of CapEx substantially contributing to climate change mitigation</t>
+  </si>
+  <si>
+    <t>Taxonomy-eligible proportion of CapEx substantially contributing to climate change adaptation</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned proportion of CapEx substantially contributing to climate change adaptation</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned and enabling proportion of CapEx substantially contributing to climate change adaptation</t>
+  </si>
+  <si>
+    <t>31.1</t>
+  </si>
+  <si>
+    <t>Taxonomy-eligible proportion of CapEx substantially contributing to sustainable use and protection of water and marine resources</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned proportion of CapEx substantially contributing to sustainable use and protection of water and marine resources</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned and enabling proportion of CapEx substantially contributing to sustainable use and protection of water and marine resources</t>
+  </si>
+  <si>
+    <t>32.1</t>
+  </si>
+  <si>
+    <t>32.1.1</t>
+  </si>
+  <si>
+    <t>32.1.2</t>
+  </si>
+  <si>
+    <t>Taxonomy-eligible proportion of CapEx substantially contributing to circular economy</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned proportion of CapEx substantially contributing to circular economy</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned and enabling proportion of CapEx substantially contributing to circular economy</t>
+  </si>
+  <si>
+    <t>Taxonomy-eligible proportion of CapEx substantially contributing to pollution prevention and control</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned proportion of CapEx substantially contributing to pollution prevention and control</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned and enabling proportion of CapEx substantially contributing to pollution prevention and control</t>
+  </si>
+  <si>
+    <t>Taxonomy-eligible proportion of CapEx substantially contributing to protection and restoration of biodiversity and ecosystems</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned proportion of CapEx substantially contributing to protection and restoration of biodiversity and ecosystems</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned and enabling proportion of CapEx substantially contributing to protection and restoration of biodiversity and ecosystems</t>
+  </si>
+  <si>
+    <t>33.1</t>
+  </si>
+  <si>
+    <t>33.1.1</t>
+  </si>
+  <si>
+    <t>33.1.2</t>
+  </si>
+  <si>
+    <t>34.1</t>
+  </si>
+  <si>
+    <t>34.1.1</t>
+  </si>
+  <si>
+    <t>34.1.2</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned proportion of OpEx substantially contributing to climate change mitigation</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned proportion of OpEx substantially contributing to climate change adaptation</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned proportion of OpEx substantially contributing to sustainable use and protection of water and marine resources</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned proportion of OpEx substantially contributing to circular economy</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned proportion of OpEx substantially contributing to pollution prevention and control</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned proportion of OpEx substantially contributing to protection and restoration of biodiversity and ecosystems</t>
+  </si>
+  <si>
+    <t>UN Global Compact Principles Compliance Policy</t>
+  </si>
+  <si>
+    <t>OECD Guidelines for Multinational Enterprises Compliance Policy</t>
+  </si>
+  <si>
+    <t>Existence of a policy to monitor compliance with the OECD Guidelines for Multinational Enterprises.</t>
+  </si>
+  <si>
+    <t>ILO Core Labour Standards</t>
+  </si>
+  <si>
+    <t>Abidance by the ILO Core Labour Standards.</t>
+  </si>
+  <si>
+    <t>Human Rights Due Diligence</t>
+  </si>
+  <si>
+    <t>Existence of due diligence processes to identify, prevent, mitigate and address adverse human rights impacts.</t>
+  </si>
+  <si>
+    <t>Existence of a policy to monitor compliance with the UNGC principles.</t>
+  </si>
+  <si>
+    <t>12.1</t>
+  </si>
+  <si>
+    <t>12.2</t>
+  </si>
+  <si>
+    <t>14.2</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>16.2</t>
+  </si>
+  <si>
+    <t>17.1.3</t>
+  </si>
+  <si>
+    <t>20.1</t>
+  </si>
+  <si>
+    <t>20.1.1</t>
+  </si>
+  <si>
+    <t>20.1.2</t>
+  </si>
+  <si>
+    <t>21.1</t>
+  </si>
+  <si>
+    <t>21.1.1</t>
+  </si>
+  <si>
+    <t>21.1.2</t>
+  </si>
+  <si>
+    <t>22.1</t>
+  </si>
+  <si>
+    <t>22.1.1</t>
+  </si>
+  <si>
+    <t>22.1.2</t>
+  </si>
+  <si>
+    <t>27.1</t>
+  </si>
+  <si>
+    <t>27.2</t>
+  </si>
+  <si>
+    <t>29.2</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>31.2</t>
+  </si>
+  <si>
+    <t>32.1.3</t>
+  </si>
+  <si>
+    <t>35.1</t>
+  </si>
+  <si>
+    <t>35.1.1</t>
+  </si>
+  <si>
+    <t>35.1.2</t>
+  </si>
+  <si>
+    <t>36.1</t>
+  </si>
+  <si>
+    <t>36.1.1</t>
+  </si>
+  <si>
+    <t>36.1.2</t>
+  </si>
+  <si>
+    <t>37.1</t>
+  </si>
+  <si>
+    <t>37.1.1</t>
+  </si>
+  <si>
+    <t>37.1.2</t>
+  </si>
+  <si>
+    <t>42.1</t>
+  </si>
+  <si>
+    <t>42.2</t>
+  </si>
+  <si>
+    <t>44.1</t>
+  </si>
+  <si>
+    <t>44.2</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>46.1</t>
+  </si>
+  <si>
+    <t>46.2</t>
+  </si>
+  <si>
     <t>28.2</t>
-  </si>
-  <si>
-    <t>39.1</t>
-  </si>
-  <si>
-    <t>39.2</t>
-  </si>
-  <si>
-    <t>40.1</t>
-  </si>
-  <si>
-    <t>40.2</t>
-  </si>
-  <si>
-    <t>41.1</t>
-  </si>
-  <si>
-    <t>41.2</t>
-  </si>
-  <si>
-    <t>42</t>
-  </si>
-  <si>
-    <t>43.1</t>
-  </si>
-  <si>
-    <t>43.2</t>
-  </si>
-  <si>
-    <t>Referenced Reports</t>
-  </si>
-  <si>
-    <t>Number</t>
-  </si>
-  <si>
-    <t>Deviation | No Deviation</t>
-  </si>
-  <si>
-    <t>Report Preupload</t>
-  </si>
-  <si>
-    <t>Custom EuTaxonomyAssuranceComponent</t>
-  </si>
-  <si>
-    <t>Total revenue per annum</t>
-  </si>
-  <si>
-    <t>Absolute value and share of the revenue per activity that is taxonomy-aligned, i.e., generated by an eligible economic activity that is making a substantial contribution to at least one of the climate and environmental objectives, while also doing no significant harm to the remaining objectives and meeting minimum standards on human rights and labour standards</t>
-  </si>
-  <si>
-    <t>Absolute value and share of the revenue per activity that is not taxonomy-aligned but eligible</t>
-  </si>
-  <si>
-    <t>Absolute value and share of the revenue that is not part of a plan to meet the DNSH criteria and make substantial contribution to any environmental objective</t>
-  </si>
-  <si>
-    <t>Share of the taxonomy-aligned revenue from total aligned revenue that is linked to activities that enable reduction of GHG in other sectors</t>
-  </si>
-  <si>
-    <t>Share of the taxonomy-aligned revenue from total aligned revenue that is linked to activities with significantly lower GHG emissions than the sector or industry average</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total CapEx for the reported year. Capital expenditures are non-consumable investments, e.g. for acquiring, upgrading, and maintaining physical assets such as property, plants, buildings, technology </t>
-  </si>
-  <si>
-    <t>Share of the taxonomy-aligned CapEx from total aligned CapEx that is linked to activities that enable reduction of GHG in other sectors</t>
-  </si>
-  <si>
-    <t>Share of the taxonomy-aligned CapEx from total aligned CapEx that is linked to activities with significantly lower GHG emissions than the sector or industry average</t>
-  </si>
-  <si>
-    <t>Total OpEx for the financial year. Operating expenses (OpEx) are shorter term expenses required to meet the ongoing operational costs of running a business.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Absolute value and share of taxonomy-aligned OpEx for the activity from total OpEx. </t>
-  </si>
-  <si>
-    <t>Absolute value and share of the OpEx per activity that is not taxonomy-aligned but eligible</t>
-  </si>
-  <si>
-    <t>Share of the taxonomy-aligned OpEx from total aligned OpEx that is linked to activities that enable reduction of GHG in other sectors</t>
-  </si>
-  <si>
-    <t>Share of the taxonomy-aligned OpEx from total aligned OpEx that is linked to activities with significantly lower GHG emissions than the sector or industry average</t>
-  </si>
-  <si>
-    <t>Absolute value of the total CapEx where the economic activity meets taxonomy criteria for substantial contribution to climate change mitigation and does no serious harm to the other environmental objectives (DNSH criteria)</t>
-  </si>
-  <si>
-    <t>Absolute value of CapEx that is taxonomy-aligned, i.e., generated by an eligible economic activity that is making a substantial contribution to at least one of the climate and environmental objectives, while also doing no significant harm to the remaining objectives and meeting minimum standards on human rights and labour standards.</t>
-  </si>
-  <si>
-    <t>Absolute value and share of the CapEx per activity that is taxonomy-aligned, i.e., generated by an eligible economic activity that is making a substantial contribution to at least one of the climate and environmental objectives, while also doing no significant harm to the remaining objectives and meeting minimum standards on human rights and labour standards</t>
-  </si>
-  <si>
-    <t>Absolute value and share of the CapEx per activity that is not taxonomy-aligned but eligible</t>
-  </si>
-  <si>
-    <t>Absolute value of the CapEx that is associated with non taxonomy-aligned but eligible activities</t>
-  </si>
-  <si>
-    <t>Absolute value of the CapEx that is not part of a plan to meet the DNSH criteria and make substantial contribution to any environmental objective</t>
-  </si>
-  <si>
-    <t>Absolute value of the OpEx that is not part of a plan to meet the DNSH criteria and make substantial contribution to any environmental objective</t>
-  </si>
-  <si>
-    <t>Absolute value of the OpEx that is part of a plan to meet the DNSH criteria and make substantial contribution to any environmental objective</t>
-  </si>
-  <si>
-    <t>Absolute value of the OpEx that is associated with non taxonomy-aligned but eligible activities</t>
-  </si>
-  <si>
-    <t>Absolute value of the OpEx that is associated with taxonomy-aligned activities. i.e., for an eligible economic activity that is making a substantial contribution to at least one of the climate and environmental objectives, while also doing no significant harm to the remaining objectives and meeting minimum standards on human rights and labour standards</t>
-  </si>
-  <si>
-    <t>Absolute value of the total eligible revenue that is taxonomy-aligned, i.e., generated by an eligible economic activity that is making a substantial contribution to at least one of the climate and environmental objectives, while also doing no significant harm to the remaining objectives and meeting minimum standards on human rights and labour standards. In same currency than total revenue.</t>
-  </si>
-  <si>
-    <t>Absolute value of the revenue that is associated with non taxonomy-aligned but eligible activities</t>
-  </si>
-  <si>
-    <t>Absolute value of the total eligible revenue in same currency than total revenue. Is part of the total revenue where the economic activity meets taxonomy criteria for substantial contribution to climate change mitigation and does no serious harm to the other environmental objectives (DNSH criteria).</t>
-  </si>
-  <si>
-    <t>Relative share of the total eligible revenue in same currency than total revenue. Is part of the total revenue where the economic activity meets taxonomy criteria for substantial contribution to climate change mitigation and does no serious harm to the other environmental objectives (DNSH criteria).</t>
-  </si>
-  <si>
-    <t>Relative share of the revenue that is associated with non taxonomy-aligned but eligible activities</t>
-  </si>
-  <si>
-    <t>Relative share of the total eligible revenue that is taxonomy-aligned, i.e., generated by an eligible economic activity that is making a substantial contribution to at least one of the climate and environmental objectives, while also doing no significant harm to the remaining objectives and meeting minimum standards on human rights and labour standards. In same currency than total revenue.</t>
-  </si>
-  <si>
-    <t>Relative share of the CapEx that is not part of a plan to meet the DNSH criteria and make substantial contribution to any environmental objective</t>
-  </si>
-  <si>
-    <t>Relative share of the total CapEx where the economic activity meets taxonomy criteria for substantial contribution to climate change mitigation and does no serious harm to the other environmental objectives (DNSH criteria)</t>
-  </si>
-  <si>
-    <t>Relative share of the CapEx that is associated with non taxonomy-aligned but eligible activities</t>
-  </si>
-  <si>
-    <t>Relative share of CapEx that is taxonomy-aligned, i.e., generated by an eligible economic activity that is making a substantial contribution to at least one of the climate and environmental objectives, while also doing no significant harm to the remaining objectives and meeting minimum standards on human rights and labour standards.</t>
-  </si>
-  <si>
-    <t>Relative share of the OpEx that is not part of a plan to meet the DNSH criteria and make substantial contribution to any environmental objective</t>
-  </si>
-  <si>
-    <t>Relative share of the OpEx that is part of a plan to meet the DNSH criteria and make substantial contribution to any environmental objective</t>
-  </si>
-  <si>
-    <t>Relative share of the OpEx that is associated with non taxonomy-aligned but eligible activities</t>
-  </si>
-  <si>
-    <t>Relative share of the OpEx that is associated with taxonomy-aligned activities. i.e., for an eligible economic activity that is making a substantial contribution to at least one of the climate and environmental objectives, while also doing no significant harm to the remaining objectives and meeting minimum standards on human rights and labour standards</t>
-  </si>
-  <si>
-    <t>Custom EuTaxonomyNonAlignedActivitiesComponent</t>
-  </si>
-  <si>
-    <t>Custom EuTaxonomyAlignedActivitiesComponent</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to Climate Change Mitigation In Percent - Eligible</t>
-  </si>
-  <si>
-    <t>Taxonomy-eligible proportion of revenue substantially contributing to climate change mitigation</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to Climate Change Mitigation In Percent - Aligned</t>
-  </si>
-  <si>
-    <t>Taxonomy-aligned proportion of revenue substantially contributing to climate change mitigation</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to Climate Change Mitigation In Percent - Of which use of proceeds</t>
-  </si>
-  <si>
-    <t>Taxonomy-aligned use of proceeds share substantially contributing to climate change mitigation</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to Climate Change Mitigation In Percent - Enabling Share</t>
-  </si>
-  <si>
-    <t>Taxonomy-aligned and enabling proportion of revenue substantially contributing to climate change mitigation</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to Climate Change Mitigation In Percent - Transitional Share</t>
-  </si>
-  <si>
-    <t>Taxonomy-aligned and transitional proportion of revenue substantially contributing to climate change mitigation</t>
-  </si>
-  <si>
-    <t>14.1</t>
-  </si>
-  <si>
-    <t>14.1.1</t>
-  </si>
-  <si>
-    <t>14.1.2</t>
-  </si>
-  <si>
-    <t>14.1.3</t>
-  </si>
-  <si>
-    <t>15.1</t>
-  </si>
-  <si>
-    <t>15.1.1</t>
-  </si>
-  <si>
-    <t>15.1.2</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to Climate Change Adaptation In Percent - Eligible</t>
-  </si>
-  <si>
-    <t>Taxonomy-eligible proportion of revenue substantially contributing to climate change adaptation</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to Climate Change Adaptation In Percent - Aligned</t>
-  </si>
-  <si>
-    <t>Taxonomy-aligned proportion of revenue substantially contributing to climate change adaptation</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to Climate Change Adaptation In Percent - Of which use of proceeds</t>
-  </si>
-  <si>
-    <t>Taxonomy-aligned use of proceeds share substantially contributing to climate change adaptation</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to Climate Change Adaptation In Percent - Enabling Share</t>
-  </si>
-  <si>
-    <t>Taxonomy-aligned and enabling proportion of revenue substantially contributing to climate change adaptation</t>
-  </si>
-  <si>
-    <t>16.1</t>
-  </si>
-  <si>
-    <t>16.1.1</t>
-  </si>
-  <si>
-    <t>16.1.2</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to Sustainable Use and Protection of Water and Marine Resources In Percent - Eligible</t>
-  </si>
-  <si>
-    <t>Taxonomy-eligible proportion of revenue substantially contributing to sustainable use and protection of water and marine resources</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to Sustainable Use and Protection of Water and Marine Resources In Percent - Aligned</t>
-  </si>
-  <si>
-    <t>Taxonomy-aligned proportion of revenue substantially contributing to sustainable use and protection of water and marine resources</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to Sustainable Use and Protection of Water and Marine Resources In Percent - Of which use of proceeds</t>
-  </si>
-  <si>
-    <t>Taxonomy-aligned use of proceeds share substantially contributing to sustainable use and protection of water and marine resources</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to Sustainable Use and Protection of Water and Marine Resources In Percent - Enabling Share</t>
-  </si>
-  <si>
-    <t>Taxonomy-aligned and enabling proportion of revenue substantially contributing to sustainable use and protection of water and marine resources</t>
-  </si>
-  <si>
-    <t>17.1</t>
-  </si>
-  <si>
-    <t>17.1.1</t>
-  </si>
-  <si>
-    <t>17.1.2</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to Transition to a Circular Economy In Percent - Eligible</t>
-  </si>
-  <si>
-    <t>Taxonomy-eligible proportion of revenue substantially contributing to circular economy</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to Transition to a Circular Economy In Percent - Aligned</t>
-  </si>
-  <si>
-    <t>Taxonomy-aligned proportion of revenue substantially contributing to circular economy</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to Transition to a Circular Economy In Percent - Of which use of proceeds</t>
-  </si>
-  <si>
-    <t>Taxonomy-aligned use of proceeds share substantially contributing to circular economy</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to Transition to a Circular Economy In Percent - Enabling Share</t>
-  </si>
-  <si>
-    <t>Taxonomy-aligned and enabling proportion of revenue substantially contributing to circular economy</t>
-  </si>
-  <si>
-    <t>18.1</t>
-  </si>
-  <si>
-    <t>18.1.1</t>
-  </si>
-  <si>
-    <t>18.1.2</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to Pollution Prevention and Control In Percent - Eligible</t>
-  </si>
-  <si>
-    <t>Taxonomy-eligible proportion of revenue substantially contributing to pollution prevention and control</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to Pollution Prevention and Control In Percent - Aligned</t>
-  </si>
-  <si>
-    <t>Taxonomy-aligned proportion of revenue substantially contributing to pollution prevention and control</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to Pollution Prevention and Control In Percent - Of which use of proceeds</t>
-  </si>
-  <si>
-    <t>Taxonomy-aligned use of proceeds share substantially contributing to pollution prevention and control</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to Pollution Prevention and Control In Percent - Enabling Share</t>
-  </si>
-  <si>
-    <t>Taxonomy-aligned and enabling proportion of revenue substantially contributing to pollution prevention and control</t>
-  </si>
-  <si>
-    <t>19.1</t>
-  </si>
-  <si>
-    <t>19.1.1</t>
-  </si>
-  <si>
-    <t>19.1.2</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to Protection and Restoration of Biodiversity and Ecosystems In Percent - Eligible</t>
-  </si>
-  <si>
-    <t>Taxonomy-eligible proportion of revenue substantially contributing to protection and restoration of biodiversity and ecosystems</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to Protection and Restoration of Biodiversity and Ecosystems In Percent - Aligned</t>
-  </si>
-  <si>
-    <t>Taxonomy-aligned proportion of revenue substantially contributing to protection and restoration of biodiversity and ecosystems</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to Protection and Restoration of Biodiversity and Ecosystems In Percent - Of which use of proceeds</t>
-  </si>
-  <si>
-    <t>Taxonomy-aligned use of proceeds share substantially contributing to protection and restoration of biodiversity and ecosystems</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to Protection and Restoration of Biodiversity and Ecosystems In Percent - Enabling Share</t>
-  </si>
-  <si>
-    <t>Taxonomy-aligned and enabling proportion of revenue substantially contributing to protection and restoration of biodiversity and ecosystems</t>
-  </si>
-  <si>
-    <t>29.1</t>
-  </si>
-  <si>
-    <t>29.1.1</t>
-  </si>
-  <si>
-    <t>29.1.2</t>
-  </si>
-  <si>
-    <t>29.1.3</t>
-  </si>
-  <si>
-    <t>Taxonomy-eligible proportion of CapEx substantially contributing to climate change mitigation</t>
-  </si>
-  <si>
-    <t>Taxonomy-aligned proportion of CapEx substantially contributing to climate change mitigation</t>
-  </si>
-  <si>
-    <t>Taxonomy-aligned and enabling proportion of CapEx substantially contributing to climate change mitigation</t>
-  </si>
-  <si>
-    <t>Taxonomy-aligned and transitional proportion of CapEx substantially contributing to climate change mitigation</t>
-  </si>
-  <si>
-    <t>30.1</t>
-  </si>
-  <si>
-    <t>30.1.1</t>
-  </si>
-  <si>
-    <t>30.1.2</t>
-  </si>
-  <si>
-    <t>Taxonomy-eligible proportion of CapEx substantially contributing to climate change adaptation</t>
-  </si>
-  <si>
-    <t>Taxonomy-aligned proportion of CapEx substantially contributing to climate change adaptation</t>
-  </si>
-  <si>
-    <t>Taxonomy-aligned and enabling proportion of CapEx substantially contributing to climate change adaptation</t>
-  </si>
-  <si>
-    <t>31.1</t>
-  </si>
-  <si>
-    <t>31.1.1</t>
-  </si>
-  <si>
-    <t>31.1.2</t>
-  </si>
-  <si>
-    <t>Taxonomy-eligible proportion of CapEx substantially contributing to sustainable use and protection of water and marine resources</t>
-  </si>
-  <si>
-    <t>Taxonomy-aligned proportion of CapEx substantially contributing to sustainable use and protection of water and marine resources</t>
-  </si>
-  <si>
-    <t>Taxonomy-aligned and enabling proportion of CapEx substantially contributing to sustainable use and protection of water and marine resources</t>
-  </si>
-  <si>
-    <t>32.1</t>
-  </si>
-  <si>
-    <t>32.1.1</t>
-  </si>
-  <si>
-    <t>32.1.2</t>
-  </si>
-  <si>
-    <t>Taxonomy-eligible proportion of CapEx substantially contributing to circular economy</t>
-  </si>
-  <si>
-    <t>Taxonomy-aligned proportion of CapEx substantially contributing to circular economy</t>
-  </si>
-  <si>
-    <t>Taxonomy-aligned and enabling proportion of CapEx substantially contributing to circular economy</t>
-  </si>
-  <si>
-    <t>Taxonomy-eligible proportion of CapEx substantially contributing to pollution prevention and control</t>
-  </si>
-  <si>
-    <t>Taxonomy-aligned proportion of CapEx substantially contributing to pollution prevention and control</t>
-  </si>
-  <si>
-    <t>Taxonomy-aligned and enabling proportion of CapEx substantially contributing to pollution prevention and control</t>
-  </si>
-  <si>
-    <t>Taxonomy-eligible proportion of CapEx substantially contributing to protection and restoration of biodiversity and ecosystems</t>
-  </si>
-  <si>
-    <t>Taxonomy-aligned proportion of CapEx substantially contributing to protection and restoration of biodiversity and ecosystems</t>
-  </si>
-  <si>
-    <t>Taxonomy-aligned and enabling proportion of CapEx substantially contributing to protection and restoration of biodiversity and ecosystems</t>
-  </si>
-  <si>
-    <t>33.1</t>
-  </si>
-  <si>
-    <t>33.1.1</t>
-  </si>
-  <si>
-    <t>33.1.2</t>
-  </si>
-  <si>
-    <t>34.1</t>
-  </si>
-  <si>
-    <t>34.1.1</t>
-  </si>
-  <si>
-    <t>34.1.2</t>
-  </si>
-  <si>
-    <t>Taxonomy-aligned proportion of OpEx substantially contributing to climate change mitigation</t>
-  </si>
-  <si>
-    <t>Taxonomy-aligned proportion of OpEx substantially contributing to climate change adaptation</t>
-  </si>
-  <si>
-    <t>Taxonomy-aligned proportion of OpEx substantially contributing to sustainable use and protection of water and marine resources</t>
-  </si>
-  <si>
-    <t>Taxonomy-aligned proportion of OpEx substantially contributing to circular economy</t>
-  </si>
-  <si>
-    <t>Taxonomy-aligned proportion of OpEx substantially contributing to pollution prevention and control</t>
-  </si>
-  <si>
-    <t>Taxonomy-aligned proportion of OpEx substantially contributing to protection and restoration of biodiversity and ecosystems</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -848,6 +872,18 @@
       <name val="Calibri"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="2" tint="-0.749992370372631"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="11">
     <fill>
@@ -911,7 +947,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -1065,12 +1101,44 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -1122,9 +1190,18 @@
     <xf numFmtId="0" fontId="11" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{438AC724-B8E1-4701-895E-04EF1113570C}"/>
     <cellStyle name="Normal 3" xfId="1" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1388,23 +1465,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L104"/>
+  <dimension ref="A1:L108"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14:F95"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="20.28515625" customWidth="1"/>
-    <col min="4" max="4" width="95.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="77.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="44.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="26.28515625" customWidth="1"/>
-    <col min="8" max="12" width="14.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.26953125" customWidth="1"/>
+    <col min="4" max="4" width="95.1796875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="77.81640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="44.7265625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="26.26953125" customWidth="1"/>
+    <col min="8" max="12" width="14.26953125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1442,7 +1519,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="7">
         <v>0</v>
       </c>
@@ -1460,7 +1537,7 @@
         <v>17</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="H2" s="11"/>
       <c r="I2" s="12" t="s">
@@ -1470,7 +1547,7 @@
       <c r="K2" s="12"/>
       <c r="L2" s="12"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="7"/>
       <c r="B3" s="8" t="s">
         <v>12</v>
@@ -1494,7 +1571,7 @@
       <c r="K3" s="12"/>
       <c r="L3" s="12"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="7">
         <v>1</v>
       </c>
@@ -1522,7 +1599,7 @@
       <c r="K4" s="11"/>
       <c r="L4" s="12"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="7">
         <v>2</v>
       </c>
@@ -1550,7 +1627,7 @@
       <c r="K5" s="12"/>
       <c r="L5" s="12"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="7">
         <v>3</v>
       </c>
@@ -1578,7 +1655,7 @@
       <c r="K6" s="12"/>
       <c r="L6" s="12"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="7">
         <v>4</v>
       </c>
@@ -1593,7 +1670,7 @@
         <v>32</v>
       </c>
       <c r="F7" s="27" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="G7" s="26" t="s">
         <v>14</v>
@@ -1604,7 +1681,7 @@
       <c r="K7" s="12"/>
       <c r="L7" s="12"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="7">
         <v>5</v>
       </c>
@@ -1612,14 +1689,14 @@
         <v>12</v>
       </c>
       <c r="C8" s="8"/>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="37" t="s">
         <v>26</v>
       </c>
       <c r="E8" s="12" t="s">
         <v>27</v>
       </c>
       <c r="F8" s="20" t="s">
-        <v>77</v>
+        <v>55</v>
       </c>
       <c r="G8" s="22"/>
       <c r="H8" s="12"/>
@@ -1630,7 +1707,7 @@
       <c r="K8" s="12"/>
       <c r="L8" s="12"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" s="7">
         <v>6</v>
       </c>
@@ -1638,38 +1715,40 @@
         <v>12</v>
       </c>
       <c r="C9" s="8"/>
-      <c r="D9" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="E9" s="12"/>
+      <c r="D9" s="38" t="s">
+        <v>196</v>
+      </c>
+      <c r="E9" s="34" t="s">
+        <v>203</v>
+      </c>
       <c r="F9" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="G9" s="23" t="s">
-        <v>14</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="G9" s="22"/>
       <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
+      <c r="I9" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J9" s="12"/>
       <c r="K9" s="12"/>
       <c r="L9" s="12"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" s="7">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="C10" s="8"/>
-      <c r="D10" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="E10" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="F10" s="21" t="s">
-        <v>37</v>
+      <c r="D10" s="33" t="s">
+        <v>197</v>
+      </c>
+      <c r="E10" s="35" t="s">
+        <v>198</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>25</v>
       </c>
       <c r="G10" s="22"/>
       <c r="H10" s="12"/>
@@ -1680,22 +1759,22 @@
       <c r="K10" s="12"/>
       <c r="L10" s="12"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="18" t="s">
-        <v>42</v>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A11" s="7">
+        <v>8</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="E11" s="19"/>
-      <c r="F11" s="21" t="s">
-        <v>28</v>
+        <v>12</v>
+      </c>
+      <c r="C11" s="8"/>
+      <c r="D11" s="38" t="s">
+        <v>199</v>
+      </c>
+      <c r="E11" s="36" t="s">
+        <v>200</v>
+      </c>
+      <c r="F11" s="20" t="s">
+        <v>25</v>
       </c>
       <c r="G11" s="22"/>
       <c r="H11" s="12"/>
@@ -1706,24 +1785,22 @@
       <c r="K11" s="12"/>
       <c r="L11" s="12"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="18" t="s">
-        <v>43</v>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A12" s="7">
+        <v>9</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D12" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="E12" s="28" t="s">
-        <v>84</v>
-      </c>
-      <c r="F12" s="21" t="s">
-        <v>37</v>
+        <v>12</v>
+      </c>
+      <c r="C12" s="8"/>
+      <c r="D12" s="38" t="s">
+        <v>201</v>
+      </c>
+      <c r="E12" s="35" t="s">
+        <v>202</v>
+      </c>
+      <c r="F12" s="20" t="s">
+        <v>25</v>
       </c>
       <c r="G12" s="22"/>
       <c r="H12" s="12"/>
@@ -1734,49 +1811,43 @@
       <c r="K12" s="12"/>
       <c r="L12" s="12"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="18" t="s">
-        <v>45</v>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A13" s="7">
+        <v>10</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="E13" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="F13" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="G13" s="22"/>
+        <v>12</v>
+      </c>
+      <c r="C13" s="8"/>
+      <c r="D13" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="E13" s="12"/>
+      <c r="F13" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="G13" s="23" t="s">
+        <v>14</v>
+      </c>
       <c r="H13" s="12"/>
-      <c r="I13" s="12" t="s">
-        <v>34</v>
-      </c>
+      <c r="I13" s="12"/>
       <c r="J13" s="12"/>
       <c r="K13" s="12"/>
       <c r="L13" s="12"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="18" t="s">
-        <v>46</v>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A14" s="7">
+        <v>11</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="8" t="s">
-        <v>44</v>
-      </c>
+      <c r="C14" s="8"/>
       <c r="D14" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="E14" s="12" t="s">
-        <v>107</v>
+        <v>38</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>59</v>
       </c>
       <c r="F14" s="21" t="s">
         <v>37</v>
@@ -1790,22 +1861,20 @@
       <c r="K14" s="12"/>
       <c r="L14" s="12"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" s="18" t="s">
-        <v>48</v>
+        <v>204</v>
       </c>
       <c r="B15" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="D15" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="E15" s="28" t="s">
-        <v>109</v>
-      </c>
+      <c r="E15" s="19"/>
       <c r="F15" s="21" t="s">
         <v>28</v>
       </c>
@@ -1818,21 +1887,21 @@
       <c r="K15" s="12"/>
       <c r="L15" s="12"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" s="18" t="s">
-        <v>49</v>
+        <v>205</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="D16" s="15" t="s">
         <v>41</v>
       </c>
       <c r="E16" s="28" t="s">
-        <v>106</v>
+        <v>62</v>
       </c>
       <c r="F16" s="21" t="s">
         <v>37</v>
@@ -1846,48 +1915,52 @@
       <c r="K16" s="12"/>
       <c r="L16" s="12"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" s="18" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="8"/>
+      <c r="C17" s="8" t="s">
+        <v>42</v>
+      </c>
       <c r="D17" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="E17" s="28" t="s">
-        <v>83</v>
+        <v>40</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>86</v>
       </c>
       <c r="F17" s="21" t="s">
-        <v>119</v>
+        <v>28</v>
       </c>
       <c r="G17" s="22"/>
       <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
+      <c r="I17" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J17" s="12"/>
       <c r="K17" s="12"/>
       <c r="L17" s="12"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18" s="18" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B18" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>110</v>
+        <v>85</v>
       </c>
       <c r="F18" s="21" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="G18" s="22"/>
       <c r="H18" s="12"/>
@@ -1898,24 +1971,24 @@
       <c r="K18" s="12"/>
       <c r="L18" s="12"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19" s="18" t="s">
-        <v>57</v>
+        <v>109</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="E19" s="12" t="s">
-        <v>105</v>
+        <v>40</v>
+      </c>
+      <c r="E19" s="28" t="s">
+        <v>87</v>
       </c>
       <c r="F19" s="21" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="G19" s="22"/>
       <c r="H19" s="12"/>
@@ -1926,22 +1999,24 @@
       <c r="K19" s="12"/>
       <c r="L19" s="12"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="7">
-        <v>14</v>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A20" s="18" t="s">
+        <v>206</v>
       </c>
       <c r="B20" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C20" s="8"/>
-      <c r="D20" s="29" t="s">
-        <v>121</v>
-      </c>
-      <c r="E20" s="30" t="s">
-        <v>122</v>
+      <c r="C20" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="E20" s="28" t="s">
+        <v>84</v>
       </c>
       <c r="F20" s="21" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="G20" s="22"/>
       <c r="H20" s="12"/>
@@ -1952,45 +2027,45 @@
       <c r="K20" s="12"/>
       <c r="L20" s="12"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A21" s="18" t="s">
-        <v>131</v>
+        <v>207</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C21" s="8"/>
-      <c r="D21" s="29" t="s">
-        <v>123</v>
-      </c>
-      <c r="E21" s="30" t="s">
-        <v>124</v>
+      <c r="D21" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="E21" s="28" t="s">
+        <v>61</v>
       </c>
       <c r="F21" s="21" t="s">
-        <v>28</v>
+        <v>97</v>
       </c>
       <c r="G21" s="22"/>
       <c r="H21" s="12"/>
-      <c r="I21" s="12" t="s">
-        <v>34</v>
-      </c>
+      <c r="I21" s="12"/>
       <c r="J21" s="12"/>
       <c r="K21" s="12"/>
       <c r="L21" s="12"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A22" s="18" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C22" s="8"/>
-      <c r="D22" s="31" t="s">
-        <v>125</v>
-      </c>
-      <c r="E22" s="30" t="s">
-        <v>126</v>
+      <c r="C22" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>88</v>
       </c>
       <c r="F22" s="21" t="s">
         <v>28</v>
@@ -2004,22 +2079,24 @@
       <c r="K22" s="12"/>
       <c r="L22" s="12"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A23" s="18" t="s">
-        <v>133</v>
+        <v>208</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C23" s="8"/>
-      <c r="D23" s="29" t="s">
-        <v>127</v>
-      </c>
-      <c r="E23" s="30" t="s">
-        <v>128</v>
+      <c r="C23" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>83</v>
       </c>
       <c r="F23" s="21" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="G23" s="22"/>
       <c r="H23" s="12"/>
@@ -2030,19 +2107,19 @@
       <c r="K23" s="12"/>
       <c r="L23" s="12"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="18" t="s">
-        <v>134</v>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A24" s="7">
+        <v>17</v>
       </c>
       <c r="B24" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C24" s="8"/>
       <c r="D24" s="29" t="s">
-        <v>129</v>
+        <v>99</v>
       </c>
       <c r="E24" s="30" t="s">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="F24" s="21" t="s">
         <v>28</v>
@@ -2056,19 +2133,19 @@
       <c r="K24" s="12"/>
       <c r="L24" s="12"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="7">
-        <v>15</v>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A25" s="18" t="s">
+        <v>127</v>
       </c>
       <c r="B25" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C25" s="8"/>
-      <c r="D25" s="32" t="s">
-        <v>138</v>
+      <c r="D25" s="29" t="s">
+        <v>101</v>
       </c>
       <c r="E25" s="30" t="s">
-        <v>139</v>
+        <v>102</v>
       </c>
       <c r="F25" s="21" t="s">
         <v>28</v>
@@ -2082,19 +2159,19 @@
       <c r="K25" s="12"/>
       <c r="L25" s="12"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A26" s="18" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="B26" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C26" s="8"/>
-      <c r="D26" s="32" t="s">
-        <v>140</v>
+      <c r="D26" s="31" t="s">
+        <v>103</v>
       </c>
       <c r="E26" s="30" t="s">
-        <v>141</v>
+        <v>104</v>
       </c>
       <c r="F26" s="21" t="s">
         <v>28</v>
@@ -2108,19 +2185,19 @@
       <c r="K26" s="12"/>
       <c r="L26" s="12"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A27" s="18" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="B27" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C27" s="8"/>
-      <c r="D27" s="31" t="s">
-        <v>142</v>
+      <c r="D27" s="29" t="s">
+        <v>105</v>
       </c>
       <c r="E27" s="30" t="s">
-        <v>143</v>
+        <v>106</v>
       </c>
       <c r="F27" s="21" t="s">
         <v>28</v>
@@ -2134,19 +2211,19 @@
       <c r="K27" s="12"/>
       <c r="L27" s="12"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A28" s="18" t="s">
-        <v>137</v>
+        <v>209</v>
       </c>
       <c r="B28" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C28" s="8"/>
-      <c r="D28" s="31" t="s">
-        <v>144</v>
+      <c r="D28" s="29" t="s">
+        <v>107</v>
       </c>
       <c r="E28" s="30" t="s">
-        <v>145</v>
+        <v>108</v>
       </c>
       <c r="F28" s="21" t="s">
         <v>28</v>
@@ -2160,19 +2237,19 @@
       <c r="K28" s="12"/>
       <c r="L28" s="12"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A29" s="7">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B29" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C29" s="8"/>
-      <c r="D29" s="31" t="s">
-        <v>149</v>
+      <c r="D29" s="32" t="s">
+        <v>110</v>
       </c>
       <c r="E29" s="30" t="s">
-        <v>150</v>
+        <v>111</v>
       </c>
       <c r="F29" s="21" t="s">
         <v>28</v>
@@ -2186,19 +2263,19 @@
       <c r="K29" s="12"/>
       <c r="L29" s="12"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A30" s="18" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="B30" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C30" s="8"/>
-      <c r="D30" s="31" t="s">
-        <v>151</v>
+      <c r="D30" s="32" t="s">
+        <v>112</v>
       </c>
       <c r="E30" s="30" t="s">
-        <v>152</v>
+        <v>113</v>
       </c>
       <c r="F30" s="21" t="s">
         <v>28</v>
@@ -2212,19 +2289,19 @@
       <c r="K30" s="12"/>
       <c r="L30" s="12"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A31" s="18" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="B31" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C31" s="8"/>
       <c r="D31" s="31" t="s">
-        <v>153</v>
+        <v>114</v>
       </c>
       <c r="E31" s="30" t="s">
-        <v>154</v>
+        <v>115</v>
       </c>
       <c r="F31" s="21" t="s">
         <v>28</v>
@@ -2238,19 +2315,19 @@
       <c r="K31" s="12"/>
       <c r="L31" s="12"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A32" s="18" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="B32" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C32" s="8"/>
       <c r="D32" s="31" t="s">
-        <v>155</v>
+        <v>116</v>
       </c>
       <c r="E32" s="30" t="s">
-        <v>156</v>
+        <v>117</v>
       </c>
       <c r="F32" s="21" t="s">
         <v>28</v>
@@ -2264,19 +2341,19 @@
       <c r="K32" s="12"/>
       <c r="L32" s="12"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A33" s="7">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B33" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C33" s="8"/>
       <c r="D33" s="31" t="s">
-        <v>160</v>
+        <v>119</v>
       </c>
       <c r="E33" s="30" t="s">
-        <v>161</v>
+        <v>120</v>
       </c>
       <c r="F33" s="21" t="s">
         <v>28</v>
@@ -2290,19 +2367,19 @@
       <c r="K33" s="12"/>
       <c r="L33" s="12"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A34" s="18" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="B34" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C34" s="8"/>
       <c r="D34" s="31" t="s">
-        <v>162</v>
+        <v>121</v>
       </c>
       <c r="E34" s="30" t="s">
-        <v>163</v>
+        <v>122</v>
       </c>
       <c r="F34" s="21" t="s">
         <v>28</v>
@@ -2316,19 +2393,19 @@
       <c r="K34" s="12"/>
       <c r="L34" s="12"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A35" s="18" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="B35" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C35" s="8"/>
       <c r="D35" s="31" t="s">
-        <v>164</v>
+        <v>123</v>
       </c>
       <c r="E35" s="30" t="s">
-        <v>165</v>
+        <v>124</v>
       </c>
       <c r="F35" s="21" t="s">
         <v>28</v>
@@ -2342,19 +2419,19 @@
       <c r="K35" s="12"/>
       <c r="L35" s="12"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A36" s="18" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B36" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C36" s="8"/>
       <c r="D36" s="31" t="s">
-        <v>166</v>
+        <v>125</v>
       </c>
       <c r="E36" s="30" t="s">
-        <v>167</v>
+        <v>126</v>
       </c>
       <c r="F36" s="21" t="s">
         <v>28</v>
@@ -2368,19 +2445,19 @@
       <c r="K36" s="12"/>
       <c r="L36" s="12"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A37" s="7">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B37" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C37" s="8"/>
       <c r="D37" s="31" t="s">
-        <v>171</v>
+        <v>130</v>
       </c>
       <c r="E37" s="30" t="s">
-        <v>172</v>
+        <v>131</v>
       </c>
       <c r="F37" s="21" t="s">
         <v>28</v>
@@ -2394,19 +2471,19 @@
       <c r="K37" s="12"/>
       <c r="L37" s="12"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A38" s="18" t="s">
-        <v>168</v>
+        <v>210</v>
       </c>
       <c r="B38" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C38" s="8"/>
       <c r="D38" s="31" t="s">
-        <v>173</v>
+        <v>132</v>
       </c>
       <c r="E38" s="30" t="s">
-        <v>174</v>
+        <v>133</v>
       </c>
       <c r="F38" s="21" t="s">
         <v>28</v>
@@ -2420,19 +2497,19 @@
       <c r="K38" s="12"/>
       <c r="L38" s="12"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A39" s="18" t="s">
-        <v>169</v>
+        <v>211</v>
       </c>
       <c r="B39" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C39" s="8"/>
       <c r="D39" s="31" t="s">
-        <v>175</v>
+        <v>134</v>
       </c>
       <c r="E39" s="30" t="s">
-        <v>176</v>
+        <v>135</v>
       </c>
       <c r="F39" s="21" t="s">
         <v>28</v>
@@ -2446,19 +2523,19 @@
       <c r="K39" s="12"/>
       <c r="L39" s="12"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A40" s="18" t="s">
-        <v>170</v>
+        <v>212</v>
       </c>
       <c r="B40" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C40" s="8"/>
       <c r="D40" s="31" t="s">
-        <v>177</v>
+        <v>136</v>
       </c>
       <c r="E40" s="30" t="s">
-        <v>178</v>
+        <v>137</v>
       </c>
       <c r="F40" s="21" t="s">
         <v>28</v>
@@ -2472,19 +2549,19 @@
       <c r="K40" s="12"/>
       <c r="L40" s="12"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A41" s="7">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B41" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C41" s="8"/>
       <c r="D41" s="31" t="s">
-        <v>182</v>
+        <v>141</v>
       </c>
       <c r="E41" s="30" t="s">
-        <v>183</v>
+        <v>142</v>
       </c>
       <c r="F41" s="21" t="s">
         <v>28</v>
@@ -2498,19 +2575,19 @@
       <c r="K41" s="12"/>
       <c r="L41" s="12"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A42" s="18" t="s">
-        <v>179</v>
+        <v>213</v>
       </c>
       <c r="B42" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C42" s="8"/>
       <c r="D42" s="31" t="s">
-        <v>184</v>
+        <v>143</v>
       </c>
       <c r="E42" s="30" t="s">
-        <v>185</v>
+        <v>144</v>
       </c>
       <c r="F42" s="21" t="s">
         <v>28</v>
@@ -2524,19 +2601,19 @@
       <c r="K42" s="12"/>
       <c r="L42" s="12"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A43" s="18" t="s">
-        <v>180</v>
+        <v>214</v>
       </c>
       <c r="B43" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C43" s="8"/>
       <c r="D43" s="31" t="s">
-        <v>186</v>
+        <v>145</v>
       </c>
       <c r="E43" s="30" t="s">
-        <v>187</v>
+        <v>146</v>
       </c>
       <c r="F43" s="21" t="s">
         <v>28</v>
@@ -2550,19 +2627,19 @@
       <c r="K43" s="12"/>
       <c r="L43" s="12"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A44" s="18" t="s">
-        <v>181</v>
+        <v>215</v>
       </c>
       <c r="B44" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C44" s="8"/>
       <c r="D44" s="31" t="s">
-        <v>188</v>
+        <v>147</v>
       </c>
       <c r="E44" s="30" t="s">
-        <v>189</v>
+        <v>148</v>
       </c>
       <c r="F44" s="21" t="s">
         <v>28</v>
@@ -2576,43 +2653,45 @@
       <c r="K44" s="12"/>
       <c r="L44" s="12"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A45" s="7">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B45" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C45" s="8"/>
-      <c r="D45" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="E45" s="28" t="s">
-        <v>82</v>
+      <c r="D45" s="31" t="s">
+        <v>152</v>
+      </c>
+      <c r="E45" s="30" t="s">
+        <v>153</v>
       </c>
       <c r="F45" s="21" t="s">
-        <v>120</v>
+        <v>28</v>
       </c>
       <c r="G45" s="22"/>
       <c r="H45" s="12"/>
-      <c r="I45" s="12"/>
+      <c r="I45" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J45" s="12"/>
       <c r="K45" s="12"/>
       <c r="L45" s="12"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A46" s="7">
-        <v>21</v>
-      </c>
-      <c r="B46" s="16" t="s">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A46" s="18" t="s">
+        <v>216</v>
+      </c>
+      <c r="B46" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C46" s="16"/>
-      <c r="D46" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="E46" s="28" t="s">
-        <v>85</v>
+      <c r="C46" s="8"/>
+      <c r="D46" s="31" t="s">
+        <v>154</v>
+      </c>
+      <c r="E46" s="30" t="s">
+        <v>155</v>
       </c>
       <c r="F46" s="21" t="s">
         <v>28</v>
@@ -2626,19 +2705,19 @@
       <c r="K46" s="12"/>
       <c r="L46" s="12"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A47" s="7">
-        <v>22</v>
-      </c>
-      <c r="B47" s="16" t="s">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A47" s="18" t="s">
+        <v>217</v>
+      </c>
+      <c r="B47" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C47" s="16"/>
-      <c r="D47" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="E47" s="28" t="s">
-        <v>86</v>
+      <c r="C47" s="8"/>
+      <c r="D47" s="31" t="s">
+        <v>156</v>
+      </c>
+      <c r="E47" s="30" t="s">
+        <v>157</v>
       </c>
       <c r="F47" s="21" t="s">
         <v>28</v>
@@ -2652,22 +2731,22 @@
       <c r="K47" s="12"/>
       <c r="L47" s="12"/>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A48" s="7">
-        <v>23</v>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A48" s="18" t="s">
+        <v>218</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C48" s="8"/>
-      <c r="D48" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="E48" s="28" t="s">
-        <v>87</v>
+      <c r="D48" s="31" t="s">
+        <v>158</v>
+      </c>
+      <c r="E48" s="30" t="s">
+        <v>159</v>
       </c>
       <c r="F48" s="21" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="G48" s="22"/>
       <c r="H48" s="12"/>
@@ -2678,52 +2757,46 @@
       <c r="K48" s="12"/>
       <c r="L48" s="12"/>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A49" s="18" t="s">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A49" s="7">
+        <v>23</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C49" s="8"/>
+      <c r="D49" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="E49" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="B49" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C49" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D49" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="E49" s="28" t="s">
-        <v>111</v>
-      </c>
       <c r="F49" s="21" t="s">
-        <v>28</v>
+        <v>98</v>
       </c>
       <c r="G49" s="22"/>
       <c r="H49" s="12"/>
-      <c r="I49" s="12" t="s">
-        <v>34</v>
-      </c>
+      <c r="I49" s="12"/>
       <c r="J49" s="12"/>
       <c r="K49" s="12"/>
       <c r="L49" s="12"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A50" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="B50" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C50" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D50" s="15" t="s">
-        <v>41</v>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A50" s="7">
+        <v>24</v>
+      </c>
+      <c r="B50" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C50" s="16"/>
+      <c r="D50" s="17" t="s">
+        <v>47</v>
       </c>
       <c r="E50" s="28" t="s">
-        <v>100</v>
+        <v>63</v>
       </c>
       <c r="F50" s="21" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="G50" s="22"/>
       <c r="H50" s="12"/>
@@ -2734,21 +2807,19 @@
       <c r="K50" s="12"/>
       <c r="L50" s="12"/>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A51" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="B51" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C51" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="D51" s="15" t="s">
-        <v>40</v>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A51" s="7">
+        <v>25</v>
+      </c>
+      <c r="B51" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C51" s="16"/>
+      <c r="D51" s="17" t="s">
+        <v>48</v>
       </c>
       <c r="E51" s="28" t="s">
-        <v>112</v>
+        <v>64</v>
       </c>
       <c r="F51" s="21" t="s">
         <v>28</v>
@@ -2762,21 +2833,19 @@
       <c r="K51" s="12"/>
       <c r="L51" s="12"/>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A52" s="18" t="s">
-        <v>59</v>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A52" s="7">
+        <v>26</v>
       </c>
       <c r="B52" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C52" s="8" t="s">
-        <v>44</v>
-      </c>
+      <c r="C52" s="8"/>
       <c r="D52" s="15" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E52" s="28" t="s">
-        <v>95</v>
+        <v>65</v>
       </c>
       <c r="F52" s="21" t="s">
         <v>37</v>
@@ -2790,21 +2859,21 @@
       <c r="K52" s="12"/>
       <c r="L52" s="12"/>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A53" s="18" t="s">
-        <v>62</v>
+        <v>219</v>
       </c>
       <c r="B53" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="D53" s="15" t="s">
         <v>40</v>
       </c>
       <c r="E53" s="28" t="s">
-        <v>113</v>
+        <v>89</v>
       </c>
       <c r="F53" s="21" t="s">
         <v>28</v>
@@ -2818,21 +2887,21 @@
       <c r="K53" s="12"/>
       <c r="L53" s="12"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A54" s="18" t="s">
-        <v>63</v>
+        <v>220</v>
       </c>
       <c r="B54" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="D54" s="15" t="s">
         <v>41</v>
       </c>
       <c r="E54" s="28" t="s">
-        <v>99</v>
+        <v>78</v>
       </c>
       <c r="F54" s="21" t="s">
         <v>37</v>
@@ -2846,48 +2915,52 @@
       <c r="K54" s="12"/>
       <c r="L54" s="12"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A55" s="18" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="B55" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C55" s="8"/>
+      <c r="C55" s="8" t="s">
+        <v>42</v>
+      </c>
       <c r="D55" s="15" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="E55" s="28" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="F55" s="21" t="s">
-        <v>119</v>
+        <v>28</v>
       </c>
       <c r="G55" s="22"/>
       <c r="H55" s="12"/>
-      <c r="I55" s="12"/>
+      <c r="I55" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J55" s="12"/>
       <c r="K55" s="12"/>
       <c r="L55" s="12"/>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A56" s="18" t="s">
-        <v>65</v>
+        <v>241</v>
       </c>
       <c r="B56" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="D56" s="15" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E56" s="28" t="s">
-        <v>114</v>
+        <v>73</v>
       </c>
       <c r="F56" s="21" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="G56" s="22"/>
       <c r="H56" s="12"/>
@@ -2898,24 +2971,24 @@
       <c r="K56" s="12"/>
       <c r="L56" s="12"/>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A57" s="18" t="s">
-        <v>66</v>
+        <v>160</v>
       </c>
       <c r="B57" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="D57" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E57" s="28" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="F57" s="21" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="G57" s="22"/>
       <c r="H57" s="12"/>
@@ -2926,22 +2999,24 @@
       <c r="K57" s="12"/>
       <c r="L57" s="12"/>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A58" s="7">
-        <v>29</v>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A58" s="18" t="s">
+        <v>221</v>
       </c>
       <c r="B58" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C58" s="8"/>
-      <c r="D58" s="29" t="s">
-        <v>121</v>
-      </c>
-      <c r="E58" s="30" t="s">
-        <v>194</v>
+      <c r="C58" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D58" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="E58" s="28" t="s">
+        <v>77</v>
       </c>
       <c r="F58" s="21" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="G58" s="22"/>
       <c r="H58" s="12"/>
@@ -2952,45 +3027,45 @@
       <c r="K58" s="12"/>
       <c r="L58" s="12"/>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A59" s="18" t="s">
-        <v>190</v>
+        <v>222</v>
       </c>
       <c r="B59" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C59" s="8"/>
-      <c r="D59" s="29" t="s">
-        <v>123</v>
-      </c>
-      <c r="E59" s="30" t="s">
-        <v>195</v>
+      <c r="D59" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="E59" s="28" t="s">
+        <v>76</v>
       </c>
       <c r="F59" s="21" t="s">
-        <v>28</v>
+        <v>97</v>
       </c>
       <c r="G59" s="22"/>
       <c r="H59" s="12"/>
-      <c r="I59" s="12" t="s">
-        <v>34</v>
-      </c>
+      <c r="I59" s="12"/>
       <c r="J59" s="12"/>
       <c r="K59" s="12"/>
       <c r="L59" s="12"/>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A60" s="18" t="s">
-        <v>191</v>
+        <v>168</v>
       </c>
       <c r="B60" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C60" s="8"/>
-      <c r="D60" s="31" t="s">
-        <v>125</v>
-      </c>
-      <c r="E60" s="30" t="s">
-        <v>126</v>
+      <c r="C60" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D60" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="E60" s="28" t="s">
+        <v>92</v>
       </c>
       <c r="F60" s="21" t="s">
         <v>28</v>
@@ -3004,22 +3079,24 @@
       <c r="K60" s="12"/>
       <c r="L60" s="12"/>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A61" s="18" t="s">
-        <v>192</v>
+        <v>223</v>
       </c>
       <c r="B61" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C61" s="8"/>
-      <c r="D61" s="29" t="s">
-        <v>127</v>
-      </c>
-      <c r="E61" s="30" t="s">
-        <v>196</v>
+      <c r="C61" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D61" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="E61" s="28" t="s">
+        <v>74</v>
       </c>
       <c r="F61" s="21" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="G61" s="22"/>
       <c r="H61" s="12"/>
@@ -3030,19 +3107,19 @@
       <c r="K61" s="12"/>
       <c r="L61" s="12"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A62" s="18" t="s">
-        <v>193</v>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A62" s="7">
+        <v>32</v>
       </c>
       <c r="B62" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C62" s="8"/>
       <c r="D62" s="29" t="s">
-        <v>129</v>
+        <v>99</v>
       </c>
       <c r="E62" s="30" t="s">
-        <v>197</v>
+        <v>161</v>
       </c>
       <c r="F62" s="21" t="s">
         <v>28</v>
@@ -3056,19 +3133,19 @@
       <c r="K62" s="12"/>
       <c r="L62" s="12"/>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A63" s="7">
-        <v>30</v>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A63" s="18" t="s">
+        <v>172</v>
       </c>
       <c r="B63" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C63" s="8"/>
-      <c r="D63" s="32" t="s">
-        <v>138</v>
+      <c r="D63" s="29" t="s">
+        <v>101</v>
       </c>
       <c r="E63" s="30" t="s">
-        <v>201</v>
+        <v>162</v>
       </c>
       <c r="F63" s="21" t="s">
         <v>28</v>
@@ -3082,19 +3159,19 @@
       <c r="K63" s="12"/>
       <c r="L63" s="12"/>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A64" s="18" t="s">
-        <v>198</v>
+        <v>173</v>
       </c>
       <c r="B64" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C64" s="8"/>
-      <c r="D64" s="32" t="s">
-        <v>140</v>
+      <c r="D64" s="31" t="s">
+        <v>103</v>
       </c>
       <c r="E64" s="30" t="s">
-        <v>202</v>
+        <v>104</v>
       </c>
       <c r="F64" s="21" t="s">
         <v>28</v>
@@ -3108,19 +3185,19 @@
       <c r="K64" s="12"/>
       <c r="L64" s="12"/>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A65" s="18" t="s">
-        <v>199</v>
+        <v>174</v>
       </c>
       <c r="B65" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C65" s="8"/>
-      <c r="D65" s="31" t="s">
-        <v>142</v>
+      <c r="D65" s="29" t="s">
+        <v>105</v>
       </c>
       <c r="E65" s="30" t="s">
-        <v>143</v>
+        <v>163</v>
       </c>
       <c r="F65" s="21" t="s">
         <v>28</v>
@@ -3134,19 +3211,19 @@
       <c r="K65" s="12"/>
       <c r="L65" s="12"/>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A66" s="18" t="s">
-        <v>200</v>
+        <v>224</v>
       </c>
       <c r="B66" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C66" s="8"/>
-      <c r="D66" s="31" t="s">
-        <v>144</v>
+      <c r="D66" s="29" t="s">
+        <v>107</v>
       </c>
       <c r="E66" s="30" t="s">
-        <v>203</v>
+        <v>164</v>
       </c>
       <c r="F66" s="21" t="s">
         <v>28</v>
@@ -3160,19 +3237,19 @@
       <c r="K66" s="12"/>
       <c r="L66" s="12"/>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A67" s="7">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B67" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C67" s="8"/>
-      <c r="D67" s="31" t="s">
-        <v>149</v>
+      <c r="D67" s="32" t="s">
+        <v>110</v>
       </c>
       <c r="E67" s="30" t="s">
-        <v>207</v>
+        <v>165</v>
       </c>
       <c r="F67" s="21" t="s">
         <v>28</v>
@@ -3186,19 +3263,19 @@
       <c r="K67" s="12"/>
       <c r="L67" s="12"/>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A68" s="18" t="s">
-        <v>204</v>
+        <v>184</v>
       </c>
       <c r="B68" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C68" s="8"/>
-      <c r="D68" s="31" t="s">
-        <v>151</v>
+      <c r="D68" s="32" t="s">
+        <v>112</v>
       </c>
       <c r="E68" s="30" t="s">
-        <v>208</v>
+        <v>166</v>
       </c>
       <c r="F68" s="21" t="s">
         <v>28</v>
@@ -3212,19 +3289,19 @@
       <c r="K68" s="12"/>
       <c r="L68" s="12"/>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A69" s="18" t="s">
-        <v>205</v>
+        <v>185</v>
       </c>
       <c r="B69" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C69" s="8"/>
       <c r="D69" s="31" t="s">
-        <v>153</v>
+        <v>114</v>
       </c>
       <c r="E69" s="30" t="s">
-        <v>154</v>
+        <v>115</v>
       </c>
       <c r="F69" s="21" t="s">
         <v>28</v>
@@ -3238,19 +3315,19 @@
       <c r="K69" s="12"/>
       <c r="L69" s="12"/>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A70" s="18" t="s">
-        <v>206</v>
+        <v>186</v>
       </c>
       <c r="B70" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C70" s="8"/>
       <c r="D70" s="31" t="s">
-        <v>155</v>
+        <v>116</v>
       </c>
       <c r="E70" s="30" t="s">
-        <v>209</v>
+        <v>167</v>
       </c>
       <c r="F70" s="21" t="s">
         <v>28</v>
@@ -3264,19 +3341,19 @@
       <c r="K70" s="12"/>
       <c r="L70" s="12"/>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A71" s="7">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B71" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C71" s="8"/>
       <c r="D71" s="31" t="s">
-        <v>160</v>
+        <v>119</v>
       </c>
       <c r="E71" s="30" t="s">
-        <v>213</v>
+        <v>169</v>
       </c>
       <c r="F71" s="21" t="s">
         <v>28</v>
@@ -3290,19 +3367,19 @@
       <c r="K71" s="12"/>
       <c r="L71" s="12"/>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A72" s="18" t="s">
-        <v>210</v>
+        <v>187</v>
       </c>
       <c r="B72" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C72" s="8"/>
       <c r="D72" s="31" t="s">
-        <v>162</v>
+        <v>121</v>
       </c>
       <c r="E72" s="30" t="s">
-        <v>214</v>
+        <v>170</v>
       </c>
       <c r="F72" s="21" t="s">
         <v>28</v>
@@ -3316,19 +3393,19 @@
       <c r="K72" s="12"/>
       <c r="L72" s="12"/>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A73" s="18" t="s">
-        <v>211</v>
+        <v>188</v>
       </c>
       <c r="B73" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C73" s="8"/>
       <c r="D73" s="31" t="s">
-        <v>164</v>
+        <v>123</v>
       </c>
       <c r="E73" s="30" t="s">
-        <v>165</v>
+        <v>124</v>
       </c>
       <c r="F73" s="21" t="s">
         <v>28</v>
@@ -3342,19 +3419,19 @@
       <c r="K73" s="12"/>
       <c r="L73" s="12"/>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A74" s="18" t="s">
-        <v>212</v>
+        <v>189</v>
       </c>
       <c r="B74" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C74" s="8"/>
       <c r="D74" s="31" t="s">
-        <v>166</v>
+        <v>125</v>
       </c>
       <c r="E74" s="30" t="s">
-        <v>215</v>
+        <v>171</v>
       </c>
       <c r="F74" s="21" t="s">
         <v>28</v>
@@ -3368,19 +3445,19 @@
       <c r="K74" s="12"/>
       <c r="L74" s="12"/>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A75" s="7">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B75" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C75" s="8"/>
       <c r="D75" s="31" t="s">
-        <v>171</v>
+        <v>130</v>
       </c>
       <c r="E75" s="30" t="s">
-        <v>216</v>
+        <v>175</v>
       </c>
       <c r="F75" s="21" t="s">
         <v>28</v>
@@ -3394,19 +3471,19 @@
       <c r="K75" s="12"/>
       <c r="L75" s="12"/>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A76" s="18" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="B76" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C76" s="8"/>
       <c r="D76" s="31" t="s">
-        <v>173</v>
+        <v>132</v>
       </c>
       <c r="E76" s="30" t="s">
-        <v>217</v>
+        <v>176</v>
       </c>
       <c r="F76" s="21" t="s">
         <v>28</v>
@@ -3420,19 +3497,19 @@
       <c r="K76" s="12"/>
       <c r="L76" s="12"/>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A77" s="18" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="B77" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C77" s="8"/>
       <c r="D77" s="31" t="s">
-        <v>175</v>
+        <v>134</v>
       </c>
       <c r="E77" s="30" t="s">
-        <v>176</v>
+        <v>135</v>
       </c>
       <c r="F77" s="21" t="s">
         <v>28</v>
@@ -3446,19 +3523,19 @@
       <c r="K77" s="12"/>
       <c r="L77" s="12"/>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A78" s="18" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="B78" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C78" s="8"/>
       <c r="D78" s="31" t="s">
+        <v>136</v>
+      </c>
+      <c r="E78" s="30" t="s">
         <v>177</v>
-      </c>
-      <c r="E78" s="30" t="s">
-        <v>218</v>
       </c>
       <c r="F78" s="21" t="s">
         <v>28</v>
@@ -3472,19 +3549,19 @@
       <c r="K78" s="12"/>
       <c r="L78" s="12"/>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A79" s="7">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B79" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C79" s="8"/>
       <c r="D79" s="31" t="s">
-        <v>182</v>
+        <v>141</v>
       </c>
       <c r="E79" s="30" t="s">
-        <v>219</v>
+        <v>178</v>
       </c>
       <c r="F79" s="21" t="s">
         <v>28</v>
@@ -3498,19 +3575,19 @@
       <c r="K79" s="12"/>
       <c r="L79" s="12"/>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A80" s="18" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="B80" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C80" s="8"/>
       <c r="D80" s="31" t="s">
-        <v>184</v>
+        <v>143</v>
       </c>
       <c r="E80" s="30" t="s">
-        <v>220</v>
+        <v>179</v>
       </c>
       <c r="F80" s="21" t="s">
         <v>28</v>
@@ -3524,19 +3601,19 @@
       <c r="K80" s="12"/>
       <c r="L80" s="12"/>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A81" s="18" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="B81" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C81" s="8"/>
       <c r="D81" s="31" t="s">
-        <v>186</v>
+        <v>145</v>
       </c>
       <c r="E81" s="30" t="s">
-        <v>187</v>
+        <v>146</v>
       </c>
       <c r="F81" s="21" t="s">
         <v>28</v>
@@ -3550,19 +3627,19 @@
       <c r="K81" s="12"/>
       <c r="L81" s="12"/>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A82" s="18" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="B82" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C82" s="8"/>
       <c r="D82" s="31" t="s">
-        <v>188</v>
+        <v>147</v>
       </c>
       <c r="E82" s="30" t="s">
-        <v>221</v>
+        <v>180</v>
       </c>
       <c r="F82" s="21" t="s">
         <v>28</v>
@@ -3576,43 +3653,45 @@
       <c r="K82" s="12"/>
       <c r="L82" s="12"/>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A83" s="7">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B83" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C83" s="8"/>
-      <c r="D83" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="E83" s="28" t="s">
-        <v>97</v>
+      <c r="D83" s="31" t="s">
+        <v>152</v>
+      </c>
+      <c r="E83" s="30" t="s">
+        <v>181</v>
       </c>
       <c r="F83" s="21" t="s">
-        <v>120</v>
+        <v>28</v>
       </c>
       <c r="G83" s="22"/>
       <c r="H83" s="12"/>
-      <c r="I83" s="12"/>
+      <c r="I83" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J83" s="12"/>
       <c r="K83" s="12"/>
       <c r="L83" s="12"/>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A84" s="7">
-        <v>36</v>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A84" s="18" t="s">
+        <v>231</v>
       </c>
       <c r="B84" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C84" s="16"/>
-      <c r="D84" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="E84" s="28" t="s">
-        <v>88</v>
+      <c r="C84" s="8"/>
+      <c r="D84" s="31" t="s">
+        <v>154</v>
+      </c>
+      <c r="E84" s="30" t="s">
+        <v>182</v>
       </c>
       <c r="F84" s="21" t="s">
         <v>28</v>
@@ -3626,19 +3705,19 @@
       <c r="K84" s="12"/>
       <c r="L84" s="12"/>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A85" s="7">
-        <v>37</v>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A85" s="18" t="s">
+        <v>232</v>
       </c>
       <c r="B85" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C85" s="16"/>
-      <c r="D85" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="E85" s="28" t="s">
-        <v>89</v>
+      <c r="C85" s="8"/>
+      <c r="D85" s="31" t="s">
+        <v>156</v>
+      </c>
+      <c r="E85" s="30" t="s">
+        <v>157</v>
       </c>
       <c r="F85" s="21" t="s">
         <v>28</v>
@@ -3652,22 +3731,22 @@
       <c r="K85" s="12"/>
       <c r="L85" s="12"/>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A86" s="7">
-        <v>38</v>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A86" s="18" t="s">
+        <v>233</v>
       </c>
       <c r="B86" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C86" s="8"/>
-      <c r="D86" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="E86" s="28" t="s">
-        <v>90</v>
+      <c r="D86" s="31" t="s">
+        <v>158</v>
+      </c>
+      <c r="E86" s="30" t="s">
+        <v>183</v>
       </c>
       <c r="F86" s="21" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="G86" s="22"/>
       <c r="H86" s="12"/>
@@ -3678,52 +3757,46 @@
       <c r="K86" s="12"/>
       <c r="L86" s="12"/>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A87" s="18" t="s">
-        <v>67</v>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A87" s="7">
+        <v>38</v>
       </c>
       <c r="B87" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C87" s="8" t="s">
-        <v>39</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="C87" s="8"/>
       <c r="D87" s="15" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="E87" s="28" t="s">
-        <v>115</v>
+        <v>75</v>
       </c>
       <c r="F87" s="21" t="s">
-        <v>28</v>
+        <v>98</v>
       </c>
       <c r="G87" s="22"/>
       <c r="H87" s="12"/>
-      <c r="I87" s="12" t="s">
-        <v>34</v>
-      </c>
+      <c r="I87" s="12"/>
       <c r="J87" s="12"/>
       <c r="K87" s="12"/>
       <c r="L87" s="12"/>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A88" s="18" t="s">
-        <v>68</v>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A88" s="7">
+        <v>39</v>
       </c>
       <c r="B88" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C88" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D88" s="15" t="s">
-        <v>41</v>
+        <v>35</v>
+      </c>
+      <c r="C88" s="16"/>
+      <c r="D88" s="17" t="s">
+        <v>47</v>
       </c>
       <c r="E88" s="28" t="s">
-        <v>101</v>
+        <v>66</v>
       </c>
       <c r="F88" s="21" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="G88" s="22"/>
       <c r="H88" s="12"/>
@@ -3734,21 +3807,19 @@
       <c r="K88" s="12"/>
       <c r="L88" s="12"/>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A89" s="18" t="s">
-        <v>69</v>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A89" s="7">
+        <v>40</v>
       </c>
       <c r="B89" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C89" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="D89" s="15" t="s">
-        <v>40</v>
+        <v>35</v>
+      </c>
+      <c r="C89" s="16"/>
+      <c r="D89" s="17" t="s">
+        <v>48</v>
       </c>
       <c r="E89" s="28" t="s">
-        <v>116</v>
+        <v>67</v>
       </c>
       <c r="F89" s="21" t="s">
         <v>28</v>
@@ -3762,21 +3833,19 @@
       <c r="K89" s="12"/>
       <c r="L89" s="12"/>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A90" s="18" t="s">
-        <v>70</v>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A90" s="7">
+        <v>41</v>
       </c>
       <c r="B90" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C90" s="8" t="s">
-        <v>44</v>
-      </c>
+      <c r="C90" s="8"/>
       <c r="D90" s="15" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E90" s="28" t="s">
-        <v>102</v>
+        <v>68</v>
       </c>
       <c r="F90" s="21" t="s">
         <v>37</v>
@@ -3790,21 +3859,21 @@
       <c r="K90" s="12"/>
       <c r="L90" s="12"/>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A91" s="18" t="s">
-        <v>71</v>
+        <v>234</v>
       </c>
       <c r="B91" s="8" t="s">
         <v>36</v>
       </c>
       <c r="C91" s="8" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="D91" s="15" t="s">
         <v>40</v>
       </c>
       <c r="E91" s="28" t="s">
-        <v>117</v>
+        <v>93</v>
       </c>
       <c r="F91" s="21" t="s">
         <v>28</v>
@@ -3818,21 +3887,21 @@
       <c r="K91" s="12"/>
       <c r="L91" s="12"/>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A92" s="18" t="s">
-        <v>72</v>
+        <v>235</v>
       </c>
       <c r="B92" s="8" t="s">
         <v>36</v>
       </c>
       <c r="C92" s="8" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="D92" s="15" t="s">
         <v>41</v>
       </c>
       <c r="E92" s="28" t="s">
-        <v>103</v>
+        <v>79</v>
       </c>
       <c r="F92" s="21" t="s">
         <v>37</v>
@@ -3846,48 +3915,52 @@
       <c r="K92" s="12"/>
       <c r="L92" s="12"/>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A93" s="18" t="s">
-        <v>73</v>
+        <v>52</v>
       </c>
       <c r="B93" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C93" s="8"/>
+      <c r="C93" s="8" t="s">
+        <v>42</v>
+      </c>
       <c r="D93" s="15" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="E93" s="28" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="F93" s="21" t="s">
-        <v>119</v>
+        <v>28</v>
       </c>
       <c r="G93" s="22"/>
       <c r="H93" s="12"/>
-      <c r="I93" s="12"/>
+      <c r="I93" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J93" s="12"/>
       <c r="K93" s="12"/>
       <c r="L93" s="12"/>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A94" s="18" t="s">
-        <v>74</v>
+        <v>53</v>
       </c>
       <c r="B94" s="8" t="s">
         <v>36</v>
       </c>
       <c r="C94" s="8" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="D94" s="15" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E94" s="28" t="s">
-        <v>118</v>
+        <v>80</v>
       </c>
       <c r="F94" s="21" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="G94" s="22"/>
       <c r="H94" s="12"/>
@@ -3898,24 +3971,24 @@
       <c r="K94" s="12"/>
       <c r="L94" s="12"/>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A95" s="18" t="s">
-        <v>75</v>
+        <v>236</v>
       </c>
       <c r="B95" s="8" t="s">
         <v>36</v>
       </c>
       <c r="C95" s="8" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="D95" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E95" s="28" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="F95" s="21" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="G95" s="22"/>
       <c r="H95" s="12"/>
@@ -3926,123 +3999,127 @@
       <c r="K95" s="12"/>
       <c r="L95" s="12"/>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A96" s="7">
-        <v>44</v>
+    <row r="96" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A96" s="18" t="s">
+        <v>237</v>
       </c>
       <c r="B96" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C96" s="8"/>
-      <c r="D96" s="29" t="s">
-        <v>123</v>
-      </c>
-      <c r="E96" s="30" t="s">
-        <v>228</v>
+      <c r="C96" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D96" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="E96" s="28" t="s">
+        <v>81</v>
       </c>
       <c r="F96" s="21" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="G96" s="22"/>
-      <c r="H96" s="19"/>
+      <c r="H96" s="12"/>
       <c r="I96" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="J96" s="19"/>
-      <c r="K96" s="19"/>
-      <c r="L96" s="19"/>
-    </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A97" s="7">
-        <v>45</v>
+      <c r="J96" s="12"/>
+      <c r="K96" s="12"/>
+      <c r="L96" s="12"/>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A97" s="18" t="s">
+        <v>238</v>
       </c>
       <c r="B97" s="8" t="s">
         <v>36</v>
       </c>
       <c r="C97" s="8"/>
-      <c r="D97" s="32" t="s">
-        <v>140</v>
-      </c>
-      <c r="E97" s="30" t="s">
-        <v>229</v>
+      <c r="D97" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="E97" s="28" t="s">
+        <v>70</v>
       </c>
       <c r="F97" s="21" t="s">
-        <v>28</v>
+        <v>97</v>
       </c>
       <c r="G97" s="22"/>
-      <c r="H97" s="19"/>
-      <c r="I97" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="J97" s="19"/>
-      <c r="K97" s="19"/>
-      <c r="L97" s="19"/>
-    </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A98" s="7">
-        <v>46</v>
+      <c r="H97" s="12"/>
+      <c r="I97" s="12"/>
+      <c r="J97" s="12"/>
+      <c r="K97" s="12"/>
+      <c r="L97" s="12"/>
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A98" s="18" t="s">
+        <v>239</v>
       </c>
       <c r="B98" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C98" s="8"/>
-      <c r="D98" s="31" t="s">
-        <v>151</v>
-      </c>
-      <c r="E98" s="30" t="s">
-        <v>230</v>
+      <c r="C98" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D98" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="E98" s="28" t="s">
+        <v>96</v>
       </c>
       <c r="F98" s="21" t="s">
         <v>28</v>
       </c>
       <c r="G98" s="22"/>
-      <c r="H98" s="19"/>
+      <c r="H98" s="12"/>
       <c r="I98" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="J98" s="19"/>
-      <c r="K98" s="19"/>
-      <c r="L98" s="19"/>
-    </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A99" s="7">
-        <v>47</v>
+      <c r="J98" s="12"/>
+      <c r="K98" s="12"/>
+      <c r="L98" s="12"/>
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A99" s="18" t="s">
+        <v>240</v>
       </c>
       <c r="B99" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C99" s="8"/>
-      <c r="D99" s="31" t="s">
-        <v>162</v>
-      </c>
-      <c r="E99" s="30" t="s">
-        <v>231</v>
+      <c r="C99" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D99" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="E99" s="28" t="s">
+        <v>82</v>
       </c>
       <c r="F99" s="21" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="G99" s="22"/>
-      <c r="H99" s="19"/>
+      <c r="H99" s="12"/>
       <c r="I99" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="J99" s="19"/>
-      <c r="K99" s="19"/>
-      <c r="L99" s="19"/>
-    </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J99" s="12"/>
+      <c r="K99" s="12"/>
+      <c r="L99" s="12"/>
+    </row>
+    <row r="100" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A100" s="7">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B100" s="8" t="s">
         <v>36</v>
       </c>
       <c r="C100" s="8"/>
-      <c r="D100" s="31" t="s">
-        <v>173</v>
+      <c r="D100" s="29" t="s">
+        <v>101</v>
       </c>
       <c r="E100" s="30" t="s">
-        <v>232</v>
+        <v>190</v>
       </c>
       <c r="F100" s="21" t="s">
         <v>28</v>
@@ -4056,19 +4133,19 @@
       <c r="K100" s="19"/>
       <c r="L100" s="19"/>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A101" s="7">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B101" s="8" t="s">
         <v>36</v>
       </c>
       <c r="C101" s="8"/>
-      <c r="D101" s="31" t="s">
-        <v>184</v>
+      <c r="D101" s="32" t="s">
+        <v>112</v>
       </c>
       <c r="E101" s="30" t="s">
-        <v>233</v>
+        <v>191</v>
       </c>
       <c r="F101" s="21" t="s">
         <v>28</v>
@@ -4082,43 +4159,45 @@
       <c r="K101" s="19"/>
       <c r="L101" s="19"/>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A102" s="7">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B102" s="8" t="s">
         <v>36</v>
       </c>
       <c r="C102" s="8"/>
-      <c r="D102" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="E102" s="28" t="s">
-        <v>91</v>
+      <c r="D102" s="31" t="s">
+        <v>121</v>
+      </c>
+      <c r="E102" s="30" t="s">
+        <v>192</v>
       </c>
       <c r="F102" s="21" t="s">
-        <v>120</v>
+        <v>28</v>
       </c>
       <c r="G102" s="22"/>
       <c r="H102" s="19"/>
-      <c r="I102" s="19"/>
+      <c r="I102" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J102" s="19"/>
       <c r="K102" s="19"/>
       <c r="L102" s="19"/>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A103" s="7">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B103" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C103" s="16"/>
-      <c r="D103" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="E103" s="28" t="s">
-        <v>93</v>
+      <c r="C103" s="8"/>
+      <c r="D103" s="31" t="s">
+        <v>132</v>
+      </c>
+      <c r="E103" s="30" t="s">
+        <v>193</v>
       </c>
       <c r="F103" s="21" t="s">
         <v>28</v>
@@ -4132,19 +4211,19 @@
       <c r="K103" s="19"/>
       <c r="L103" s="19"/>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A104" s="7">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B104" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C104" s="16"/>
-      <c r="D104" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="E104" s="28" t="s">
-        <v>94</v>
+      <c r="C104" s="8"/>
+      <c r="D104" s="31" t="s">
+        <v>143</v>
+      </c>
+      <c r="E104" s="30" t="s">
+        <v>194</v>
       </c>
       <c r="F104" s="21" t="s">
         <v>28</v>
@@ -4158,8 +4237,110 @@
       <c r="K104" s="19"/>
       <c r="L104" s="19"/>
     </row>
+    <row r="105" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A105" s="7">
+        <v>52</v>
+      </c>
+      <c r="B105" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C105" s="8"/>
+      <c r="D105" s="31" t="s">
+        <v>154</v>
+      </c>
+      <c r="E105" s="30" t="s">
+        <v>195</v>
+      </c>
+      <c r="F105" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G105" s="22"/>
+      <c r="H105" s="19"/>
+      <c r="I105" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="J105" s="19"/>
+      <c r="K105" s="19"/>
+      <c r="L105" s="19"/>
+    </row>
+    <row r="106" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A106" s="7">
+        <v>53</v>
+      </c>
+      <c r="B106" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C106" s="8"/>
+      <c r="D106" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="E106" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="F106" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="G106" s="22"/>
+      <c r="H106" s="19"/>
+      <c r="I106" s="19"/>
+      <c r="J106" s="19"/>
+      <c r="K106" s="19"/>
+      <c r="L106" s="19"/>
+    </row>
+    <row r="107" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A107" s="7">
+        <v>54</v>
+      </c>
+      <c r="B107" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C107" s="16"/>
+      <c r="D107" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="E107" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="F107" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G107" s="22"/>
+      <c r="H107" s="19"/>
+      <c r="I107" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="J107" s="19"/>
+      <c r="K107" s="19"/>
+      <c r="L107" s="19"/>
+    </row>
+    <row r="108" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A108" s="7">
+        <v>55</v>
+      </c>
+      <c r="B108" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C108" s="16"/>
+      <c r="D108" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="E108" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="F108" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G108" s="22"/>
+      <c r="H108" s="19"/>
+      <c r="I108" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="J108" s="19"/>
+      <c r="K108" s="19"/>
+      <c r="L108" s="19"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:L104" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:L108" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
DALA-5554_Expand EU Taxonomy Non-Financials Data Model by 4 fields (#1024)
Add new fields to EU Taxonomy Non-Financials

---------

Co-authored-by: SiegfriedSobkowiak <71646830+SiegfriedSobkowiak@users.noreply.github.com>
Co-authored-by: Stephan Wezorke <186339469+StephanWezorke@users.noreply.github.com>
Co-authored-by: MarcTM01 <108792843+MarcTM01@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/euTaxonomyNonFinancials/EutaxonomyNonFinancials.xlsx
+++ b/dataland-framework-toolbox/inputs/euTaxonomyNonFinancials/EutaxonomyNonFinancials.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dataland\dataland_alternative\dataland-framework-toolbox\inputs\euTaxonomyNonFinancials\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dataland\Dataland\dataland-framework-toolbox\inputs\euTaxonomyNonFinancials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E51E730-3590-4F62-A449-A34DD2DB217B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C67B78E9-299A-43AD-B2BD-B46716BA59B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57490" yWindow="-10800" windowWidth="38620" windowHeight="21220" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Framework Data Model" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Framework Data Model'!$A$1:$L$104</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Framework Data Model'!$A$1:$L$108</definedName>
     <definedName name="IQ_CH">110000</definedName>
     <definedName name="IQ_CQ">5000</definedName>
     <definedName name="IQ_CY">10000</definedName>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="242">
   <si>
     <t>Field Identifier</t>
   </si>
@@ -186,30 +186,12 @@
     <t>Absolute Share</t>
   </si>
   <si>
-    <t>9.1</t>
-  </si>
-  <si>
-    <t>9.2</t>
-  </si>
-  <si>
     <t>Eligible Share</t>
   </si>
   <si>
-    <t>10.1</t>
-  </si>
-  <si>
-    <t>10.2</t>
-  </si>
-  <si>
     <t>Non-Aligned Share</t>
   </si>
   <si>
-    <t>11.1</t>
-  </si>
-  <si>
-    <t>11.2</t>
-  </si>
-  <si>
     <t>Non-Aligned Activities</t>
   </si>
   <si>
@@ -225,548 +207,590 @@
     <t>Transitional Share In Percent</t>
   </si>
   <si>
-    <t>12</t>
-  </si>
-  <si>
     <t>13.1</t>
   </si>
   <si>
     <t>13.2</t>
   </si>
   <si>
-    <t>25.1</t>
-  </si>
-  <si>
-    <t>25.2</t>
-  </si>
-  <si>
-    <t>24.1</t>
-  </si>
-  <si>
-    <t>24.2</t>
-  </si>
-  <si>
-    <t>26.1</t>
-  </si>
-  <si>
-    <t>26.2</t>
-  </si>
-  <si>
-    <t>27</t>
-  </si>
-  <si>
     <t>28.1</t>
   </si>
   <si>
+    <t>43.1</t>
+  </si>
+  <si>
+    <t>43.2</t>
+  </si>
+  <si>
+    <t>Referenced Reports</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>Deviation | No Deviation</t>
+  </si>
+  <si>
+    <t>Report Preupload</t>
+  </si>
+  <si>
+    <t>Custom EuTaxonomyAssuranceComponent</t>
+  </si>
+  <si>
+    <t>Total revenue per annum</t>
+  </si>
+  <si>
+    <t>Absolute value and share of the revenue per activity that is taxonomy-aligned, i.e., generated by an eligible economic activity that is making a substantial contribution to at least one of the climate and environmental objectives, while also doing no significant harm to the remaining objectives and meeting minimum standards on human rights and labour standards</t>
+  </si>
+  <si>
+    <t>Absolute value and share of the revenue per activity that is not taxonomy-aligned but eligible</t>
+  </si>
+  <si>
+    <t>Absolute value and share of the revenue that is not part of a plan to meet the DNSH criteria and make substantial contribution to any environmental objective</t>
+  </si>
+  <si>
+    <t>Share of the taxonomy-aligned revenue from total aligned revenue that is linked to activities that enable reduction of GHG in other sectors</t>
+  </si>
+  <si>
+    <t>Share of the taxonomy-aligned revenue from total aligned revenue that is linked to activities with significantly lower GHG emissions than the sector or industry average</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total CapEx for the reported year. Capital expenditures are non-consumable investments, e.g. for acquiring, upgrading, and maintaining physical assets such as property, plants, buildings, technology </t>
+  </si>
+  <si>
+    <t>Share of the taxonomy-aligned CapEx from total aligned CapEx that is linked to activities that enable reduction of GHG in other sectors</t>
+  </si>
+  <si>
+    <t>Share of the taxonomy-aligned CapEx from total aligned CapEx that is linked to activities with significantly lower GHG emissions than the sector or industry average</t>
+  </si>
+  <si>
+    <t>Total OpEx for the financial year. Operating expenses (OpEx) are shorter term expenses required to meet the ongoing operational costs of running a business.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Absolute value and share of taxonomy-aligned OpEx for the activity from total OpEx. </t>
+  </si>
+  <si>
+    <t>Absolute value and share of the OpEx per activity that is not taxonomy-aligned but eligible</t>
+  </si>
+  <si>
+    <t>Share of the taxonomy-aligned OpEx from total aligned OpEx that is linked to activities that enable reduction of GHG in other sectors</t>
+  </si>
+  <si>
+    <t>Share of the taxonomy-aligned OpEx from total aligned OpEx that is linked to activities with significantly lower GHG emissions than the sector or industry average</t>
+  </si>
+  <si>
+    <t>Absolute value of the total CapEx where the economic activity meets taxonomy criteria for substantial contribution to climate change mitigation and does no serious harm to the other environmental objectives (DNSH criteria)</t>
+  </si>
+  <si>
+    <t>Absolute value of CapEx that is taxonomy-aligned, i.e., generated by an eligible economic activity that is making a substantial contribution to at least one of the climate and environmental objectives, while also doing no significant harm to the remaining objectives and meeting minimum standards on human rights and labour standards.</t>
+  </si>
+  <si>
+    <t>Absolute value and share of the CapEx per activity that is taxonomy-aligned, i.e., generated by an eligible economic activity that is making a substantial contribution to at least one of the climate and environmental objectives, while also doing no significant harm to the remaining objectives and meeting minimum standards on human rights and labour standards</t>
+  </si>
+  <si>
+    <t>Absolute value and share of the CapEx per activity that is not taxonomy-aligned but eligible</t>
+  </si>
+  <si>
+    <t>Absolute value of the CapEx that is associated with non taxonomy-aligned but eligible activities</t>
+  </si>
+  <si>
+    <t>Absolute value of the CapEx that is not part of a plan to meet the DNSH criteria and make substantial contribution to any environmental objective</t>
+  </si>
+  <si>
+    <t>Absolute value of the OpEx that is not part of a plan to meet the DNSH criteria and make substantial contribution to any environmental objective</t>
+  </si>
+  <si>
+    <t>Absolute value of the OpEx that is part of a plan to meet the DNSH criteria and make substantial contribution to any environmental objective</t>
+  </si>
+  <si>
+    <t>Absolute value of the OpEx that is associated with non taxonomy-aligned but eligible activities</t>
+  </si>
+  <si>
+    <t>Absolute value of the OpEx that is associated with taxonomy-aligned activities. i.e., for an eligible economic activity that is making a substantial contribution to at least one of the climate and environmental objectives, while also doing no significant harm to the remaining objectives and meeting minimum standards on human rights and labour standards</t>
+  </si>
+  <si>
+    <t>Absolute value of the total eligible revenue that is taxonomy-aligned, i.e., generated by an eligible economic activity that is making a substantial contribution to at least one of the climate and environmental objectives, while also doing no significant harm to the remaining objectives and meeting minimum standards on human rights and labour standards. In same currency than total revenue.</t>
+  </si>
+  <si>
+    <t>Absolute value of the revenue that is associated with non taxonomy-aligned but eligible activities</t>
+  </si>
+  <si>
+    <t>Absolute value of the total eligible revenue in same currency than total revenue. Is part of the total revenue where the economic activity meets taxonomy criteria for substantial contribution to climate change mitigation and does no serious harm to the other environmental objectives (DNSH criteria).</t>
+  </si>
+  <si>
+    <t>Relative share of the total eligible revenue in same currency than total revenue. Is part of the total revenue where the economic activity meets taxonomy criteria for substantial contribution to climate change mitigation and does no serious harm to the other environmental objectives (DNSH criteria).</t>
+  </si>
+  <si>
+    <t>Relative share of the revenue that is associated with non taxonomy-aligned but eligible activities</t>
+  </si>
+  <si>
+    <t>Relative share of the total eligible revenue that is taxonomy-aligned, i.e., generated by an eligible economic activity that is making a substantial contribution to at least one of the climate and environmental objectives, while also doing no significant harm to the remaining objectives and meeting minimum standards on human rights and labour standards. In same currency than total revenue.</t>
+  </si>
+  <si>
+    <t>Relative share of the CapEx that is not part of a plan to meet the DNSH criteria and make substantial contribution to any environmental objective</t>
+  </si>
+  <si>
+    <t>Relative share of the total CapEx where the economic activity meets taxonomy criteria for substantial contribution to climate change mitigation and does no serious harm to the other environmental objectives (DNSH criteria)</t>
+  </si>
+  <si>
+    <t>Relative share of the CapEx that is associated with non taxonomy-aligned but eligible activities</t>
+  </si>
+  <si>
+    <t>Relative share of CapEx that is taxonomy-aligned, i.e., generated by an eligible economic activity that is making a substantial contribution to at least one of the climate and environmental objectives, while also doing no significant harm to the remaining objectives and meeting minimum standards on human rights and labour standards.</t>
+  </si>
+  <si>
+    <t>Relative share of the OpEx that is not part of a plan to meet the DNSH criteria and make substantial contribution to any environmental objective</t>
+  </si>
+  <si>
+    <t>Relative share of the OpEx that is part of a plan to meet the DNSH criteria and make substantial contribution to any environmental objective</t>
+  </si>
+  <si>
+    <t>Relative share of the OpEx that is associated with non taxonomy-aligned but eligible activities</t>
+  </si>
+  <si>
+    <t>Relative share of the OpEx that is associated with taxonomy-aligned activities. i.e., for an eligible economic activity that is making a substantial contribution to at least one of the climate and environmental objectives, while also doing no significant harm to the remaining objectives and meeting minimum standards on human rights and labour standards</t>
+  </si>
+  <si>
+    <t>Custom EuTaxonomyNonAlignedActivitiesComponent</t>
+  </si>
+  <si>
+    <t>Custom EuTaxonomyAlignedActivitiesComponent</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Climate Change Mitigation In Percent - Eligible</t>
+  </si>
+  <si>
+    <t>Taxonomy-eligible proportion of revenue substantially contributing to climate change mitigation</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Climate Change Mitigation In Percent - Aligned</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned proportion of revenue substantially contributing to climate change mitigation</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Climate Change Mitigation In Percent - Of which use of proceeds</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned use of proceeds share substantially contributing to climate change mitigation</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Climate Change Mitigation In Percent - Enabling Share</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned and enabling proportion of revenue substantially contributing to climate change mitigation</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Climate Change Mitigation In Percent - Transitional Share</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned and transitional proportion of revenue substantially contributing to climate change mitigation</t>
+  </si>
+  <si>
+    <t>14.1</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Climate Change Adaptation In Percent - Eligible</t>
+  </si>
+  <si>
+    <t>Taxonomy-eligible proportion of revenue substantially contributing to climate change adaptation</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Climate Change Adaptation In Percent - Aligned</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned proportion of revenue substantially contributing to climate change adaptation</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Climate Change Adaptation In Percent - Of which use of proceeds</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned use of proceeds share substantially contributing to climate change adaptation</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Climate Change Adaptation In Percent - Enabling Share</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned and enabling proportion of revenue substantially contributing to climate change adaptation</t>
+  </si>
+  <si>
+    <t>16.1</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Sustainable Use and Protection of Water and Marine Resources In Percent - Eligible</t>
+  </si>
+  <si>
+    <t>Taxonomy-eligible proportion of revenue substantially contributing to sustainable use and protection of water and marine resources</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Sustainable Use and Protection of Water and Marine Resources In Percent - Aligned</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned proportion of revenue substantially contributing to sustainable use and protection of water and marine resources</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Sustainable Use and Protection of Water and Marine Resources In Percent - Of which use of proceeds</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned use of proceeds share substantially contributing to sustainable use and protection of water and marine resources</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Sustainable Use and Protection of Water and Marine Resources In Percent - Enabling Share</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned and enabling proportion of revenue substantially contributing to sustainable use and protection of water and marine resources</t>
+  </si>
+  <si>
+    <t>17.1</t>
+  </si>
+  <si>
+    <t>17.1.1</t>
+  </si>
+  <si>
+    <t>17.1.2</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Transition to a Circular Economy In Percent - Eligible</t>
+  </si>
+  <si>
+    <t>Taxonomy-eligible proportion of revenue substantially contributing to circular economy</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Transition to a Circular Economy In Percent - Aligned</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned proportion of revenue substantially contributing to circular economy</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Transition to a Circular Economy In Percent - Of which use of proceeds</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned use of proceeds share substantially contributing to circular economy</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Transition to a Circular Economy In Percent - Enabling Share</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned and enabling proportion of revenue substantially contributing to circular economy</t>
+  </si>
+  <si>
+    <t>18.1</t>
+  </si>
+  <si>
+    <t>18.1.1</t>
+  </si>
+  <si>
+    <t>18.1.2</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Pollution Prevention and Control In Percent - Eligible</t>
+  </si>
+  <si>
+    <t>Taxonomy-eligible proportion of revenue substantially contributing to pollution prevention and control</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Pollution Prevention and Control In Percent - Aligned</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned proportion of revenue substantially contributing to pollution prevention and control</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Pollution Prevention and Control In Percent - Of which use of proceeds</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned use of proceeds share substantially contributing to pollution prevention and control</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Pollution Prevention and Control In Percent - Enabling Share</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned and enabling proportion of revenue substantially contributing to pollution prevention and control</t>
+  </si>
+  <si>
+    <t>19.1</t>
+  </si>
+  <si>
+    <t>19.1.1</t>
+  </si>
+  <si>
+    <t>19.1.2</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Protection and Restoration of Biodiversity and Ecosystems In Percent - Eligible</t>
+  </si>
+  <si>
+    <t>Taxonomy-eligible proportion of revenue substantially contributing to protection and restoration of biodiversity and ecosystems</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Protection and Restoration of Biodiversity and Ecosystems In Percent - Aligned</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned proportion of revenue substantially contributing to protection and restoration of biodiversity and ecosystems</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Protection and Restoration of Biodiversity and Ecosystems In Percent - Of which use of proceeds</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned use of proceeds share substantially contributing to protection and restoration of biodiversity and ecosystems</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Protection and Restoration of Biodiversity and Ecosystems In Percent - Enabling Share</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned and enabling proportion of revenue substantially contributing to protection and restoration of biodiversity and ecosystems</t>
+  </si>
+  <si>
+    <t>29.1</t>
+  </si>
+  <si>
+    <t>Taxonomy-eligible proportion of CapEx substantially contributing to climate change mitigation</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned proportion of CapEx substantially contributing to climate change mitigation</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned and enabling proportion of CapEx substantially contributing to climate change mitigation</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned and transitional proportion of CapEx substantially contributing to climate change mitigation</t>
+  </si>
+  <si>
+    <t>Taxonomy-eligible proportion of CapEx substantially contributing to climate change adaptation</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned proportion of CapEx substantially contributing to climate change adaptation</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned and enabling proportion of CapEx substantially contributing to climate change adaptation</t>
+  </si>
+  <si>
+    <t>31.1</t>
+  </si>
+  <si>
+    <t>Taxonomy-eligible proportion of CapEx substantially contributing to sustainable use and protection of water and marine resources</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned proportion of CapEx substantially contributing to sustainable use and protection of water and marine resources</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned and enabling proportion of CapEx substantially contributing to sustainable use and protection of water and marine resources</t>
+  </si>
+  <si>
+    <t>32.1</t>
+  </si>
+  <si>
+    <t>32.1.1</t>
+  </si>
+  <si>
+    <t>32.1.2</t>
+  </si>
+  <si>
+    <t>Taxonomy-eligible proportion of CapEx substantially contributing to circular economy</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned proportion of CapEx substantially contributing to circular economy</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned and enabling proportion of CapEx substantially contributing to circular economy</t>
+  </si>
+  <si>
+    <t>Taxonomy-eligible proportion of CapEx substantially contributing to pollution prevention and control</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned proportion of CapEx substantially contributing to pollution prevention and control</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned and enabling proportion of CapEx substantially contributing to pollution prevention and control</t>
+  </si>
+  <si>
+    <t>Taxonomy-eligible proportion of CapEx substantially contributing to protection and restoration of biodiversity and ecosystems</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned proportion of CapEx substantially contributing to protection and restoration of biodiversity and ecosystems</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned and enabling proportion of CapEx substantially contributing to protection and restoration of biodiversity and ecosystems</t>
+  </si>
+  <si>
+    <t>33.1</t>
+  </si>
+  <si>
+    <t>33.1.1</t>
+  </si>
+  <si>
+    <t>33.1.2</t>
+  </si>
+  <si>
+    <t>34.1</t>
+  </si>
+  <si>
+    <t>34.1.1</t>
+  </si>
+  <si>
+    <t>34.1.2</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned proportion of OpEx substantially contributing to climate change mitigation</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned proportion of OpEx substantially contributing to climate change adaptation</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned proportion of OpEx substantially contributing to sustainable use and protection of water and marine resources</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned proportion of OpEx substantially contributing to circular economy</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned proportion of OpEx substantially contributing to pollution prevention and control</t>
+  </si>
+  <si>
+    <t>Taxonomy-aligned proportion of OpEx substantially contributing to protection and restoration of biodiversity and ecosystems</t>
+  </si>
+  <si>
+    <t>UN Global Compact Principles Compliance Policy</t>
+  </si>
+  <si>
+    <t>OECD Guidelines for Multinational Enterprises Compliance Policy</t>
+  </si>
+  <si>
+    <t>Existence of a policy to monitor compliance with the OECD Guidelines for Multinational Enterprises.</t>
+  </si>
+  <si>
+    <t>ILO Core Labour Standards</t>
+  </si>
+  <si>
+    <t>Abidance by the ILO Core Labour Standards.</t>
+  </si>
+  <si>
+    <t>Human Rights Due Diligence</t>
+  </si>
+  <si>
+    <t>Existence of due diligence processes to identify, prevent, mitigate and address adverse human rights impacts.</t>
+  </si>
+  <si>
+    <t>Existence of a policy to monitor compliance with the UNGC principles.</t>
+  </si>
+  <si>
+    <t>12.1</t>
+  </si>
+  <si>
+    <t>12.2</t>
+  </si>
+  <si>
+    <t>14.2</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>16.2</t>
+  </si>
+  <si>
+    <t>17.1.3</t>
+  </si>
+  <si>
+    <t>20.1</t>
+  </si>
+  <si>
+    <t>20.1.1</t>
+  </si>
+  <si>
+    <t>20.1.2</t>
+  </si>
+  <si>
+    <t>21.1</t>
+  </si>
+  <si>
+    <t>21.1.1</t>
+  </si>
+  <si>
+    <t>21.1.2</t>
+  </si>
+  <si>
+    <t>22.1</t>
+  </si>
+  <si>
+    <t>22.1.1</t>
+  </si>
+  <si>
+    <t>22.1.2</t>
+  </si>
+  <si>
+    <t>27.1</t>
+  </si>
+  <si>
+    <t>27.2</t>
+  </si>
+  <si>
+    <t>29.2</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>31.2</t>
+  </si>
+  <si>
+    <t>32.1.3</t>
+  </si>
+  <si>
+    <t>35.1</t>
+  </si>
+  <si>
+    <t>35.1.1</t>
+  </si>
+  <si>
+    <t>35.1.2</t>
+  </si>
+  <si>
+    <t>36.1</t>
+  </si>
+  <si>
+    <t>36.1.1</t>
+  </si>
+  <si>
+    <t>36.1.2</t>
+  </si>
+  <si>
+    <t>37.1</t>
+  </si>
+  <si>
+    <t>37.1.1</t>
+  </si>
+  <si>
+    <t>37.1.2</t>
+  </si>
+  <si>
+    <t>42.1</t>
+  </si>
+  <si>
+    <t>42.2</t>
+  </si>
+  <si>
+    <t>44.1</t>
+  </si>
+  <si>
+    <t>44.2</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>46.1</t>
+  </si>
+  <si>
+    <t>46.2</t>
+  </si>
+  <si>
     <t>28.2</t>
-  </si>
-  <si>
-    <t>39.1</t>
-  </si>
-  <si>
-    <t>39.2</t>
-  </si>
-  <si>
-    <t>40.1</t>
-  </si>
-  <si>
-    <t>40.2</t>
-  </si>
-  <si>
-    <t>41.1</t>
-  </si>
-  <si>
-    <t>41.2</t>
-  </si>
-  <si>
-    <t>42</t>
-  </si>
-  <si>
-    <t>43.1</t>
-  </si>
-  <si>
-    <t>43.2</t>
-  </si>
-  <si>
-    <t>Referenced Reports</t>
-  </si>
-  <si>
-    <t>Number</t>
-  </si>
-  <si>
-    <t>Deviation | No Deviation</t>
-  </si>
-  <si>
-    <t>Report Preupload</t>
-  </si>
-  <si>
-    <t>Custom EuTaxonomyAssuranceComponent</t>
-  </si>
-  <si>
-    <t>Total revenue per annum</t>
-  </si>
-  <si>
-    <t>Absolute value and share of the revenue per activity that is taxonomy-aligned, i.e., generated by an eligible economic activity that is making a substantial contribution to at least one of the climate and environmental objectives, while also doing no significant harm to the remaining objectives and meeting minimum standards on human rights and labour standards</t>
-  </si>
-  <si>
-    <t>Absolute value and share of the revenue per activity that is not taxonomy-aligned but eligible</t>
-  </si>
-  <si>
-    <t>Absolute value and share of the revenue that is not part of a plan to meet the DNSH criteria and make substantial contribution to any environmental objective</t>
-  </si>
-  <si>
-    <t>Share of the taxonomy-aligned revenue from total aligned revenue that is linked to activities that enable reduction of GHG in other sectors</t>
-  </si>
-  <si>
-    <t>Share of the taxonomy-aligned revenue from total aligned revenue that is linked to activities with significantly lower GHG emissions than the sector or industry average</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total CapEx for the reported year. Capital expenditures are non-consumable investments, e.g. for acquiring, upgrading, and maintaining physical assets such as property, plants, buildings, technology </t>
-  </si>
-  <si>
-    <t>Share of the taxonomy-aligned CapEx from total aligned CapEx that is linked to activities that enable reduction of GHG in other sectors</t>
-  </si>
-  <si>
-    <t>Share of the taxonomy-aligned CapEx from total aligned CapEx that is linked to activities with significantly lower GHG emissions than the sector or industry average</t>
-  </si>
-  <si>
-    <t>Total OpEx for the financial year. Operating expenses (OpEx) are shorter term expenses required to meet the ongoing operational costs of running a business.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Absolute value and share of taxonomy-aligned OpEx for the activity from total OpEx. </t>
-  </si>
-  <si>
-    <t>Absolute value and share of the OpEx per activity that is not taxonomy-aligned but eligible</t>
-  </si>
-  <si>
-    <t>Share of the taxonomy-aligned OpEx from total aligned OpEx that is linked to activities that enable reduction of GHG in other sectors</t>
-  </si>
-  <si>
-    <t>Share of the taxonomy-aligned OpEx from total aligned OpEx that is linked to activities with significantly lower GHG emissions than the sector or industry average</t>
-  </si>
-  <si>
-    <t>Absolute value of the total CapEx where the economic activity meets taxonomy criteria for substantial contribution to climate change mitigation and does no serious harm to the other environmental objectives (DNSH criteria)</t>
-  </si>
-  <si>
-    <t>Absolute value of CapEx that is taxonomy-aligned, i.e., generated by an eligible economic activity that is making a substantial contribution to at least one of the climate and environmental objectives, while also doing no significant harm to the remaining objectives and meeting minimum standards on human rights and labour standards.</t>
-  </si>
-  <si>
-    <t>Absolute value and share of the CapEx per activity that is taxonomy-aligned, i.e., generated by an eligible economic activity that is making a substantial contribution to at least one of the climate and environmental objectives, while also doing no significant harm to the remaining objectives and meeting minimum standards on human rights and labour standards</t>
-  </si>
-  <si>
-    <t>Absolute value and share of the CapEx per activity that is not taxonomy-aligned but eligible</t>
-  </si>
-  <si>
-    <t>Absolute value of the CapEx that is associated with non taxonomy-aligned but eligible activities</t>
-  </si>
-  <si>
-    <t>Absolute value of the CapEx that is not part of a plan to meet the DNSH criteria and make substantial contribution to any environmental objective</t>
-  </si>
-  <si>
-    <t>Absolute value of the OpEx that is not part of a plan to meet the DNSH criteria and make substantial contribution to any environmental objective</t>
-  </si>
-  <si>
-    <t>Absolute value of the OpEx that is part of a plan to meet the DNSH criteria and make substantial contribution to any environmental objective</t>
-  </si>
-  <si>
-    <t>Absolute value of the OpEx that is associated with non taxonomy-aligned but eligible activities</t>
-  </si>
-  <si>
-    <t>Absolute value of the OpEx that is associated with taxonomy-aligned activities. i.e., for an eligible economic activity that is making a substantial contribution to at least one of the climate and environmental objectives, while also doing no significant harm to the remaining objectives and meeting minimum standards on human rights and labour standards</t>
-  </si>
-  <si>
-    <t>Absolute value of the total eligible revenue that is taxonomy-aligned, i.e., generated by an eligible economic activity that is making a substantial contribution to at least one of the climate and environmental objectives, while also doing no significant harm to the remaining objectives and meeting minimum standards on human rights and labour standards. In same currency than total revenue.</t>
-  </si>
-  <si>
-    <t>Absolute value of the revenue that is associated with non taxonomy-aligned but eligible activities</t>
-  </si>
-  <si>
-    <t>Absolute value of the total eligible revenue in same currency than total revenue. Is part of the total revenue where the economic activity meets taxonomy criteria for substantial contribution to climate change mitigation and does no serious harm to the other environmental objectives (DNSH criteria).</t>
-  </si>
-  <si>
-    <t>Relative share of the total eligible revenue in same currency than total revenue. Is part of the total revenue where the economic activity meets taxonomy criteria for substantial contribution to climate change mitigation and does no serious harm to the other environmental objectives (DNSH criteria).</t>
-  </si>
-  <si>
-    <t>Relative share of the revenue that is associated with non taxonomy-aligned but eligible activities</t>
-  </si>
-  <si>
-    <t>Relative share of the total eligible revenue that is taxonomy-aligned, i.e., generated by an eligible economic activity that is making a substantial contribution to at least one of the climate and environmental objectives, while also doing no significant harm to the remaining objectives and meeting minimum standards on human rights and labour standards. In same currency than total revenue.</t>
-  </si>
-  <si>
-    <t>Relative share of the CapEx that is not part of a plan to meet the DNSH criteria and make substantial contribution to any environmental objective</t>
-  </si>
-  <si>
-    <t>Relative share of the total CapEx where the economic activity meets taxonomy criteria for substantial contribution to climate change mitigation and does no serious harm to the other environmental objectives (DNSH criteria)</t>
-  </si>
-  <si>
-    <t>Relative share of the CapEx that is associated with non taxonomy-aligned but eligible activities</t>
-  </si>
-  <si>
-    <t>Relative share of CapEx that is taxonomy-aligned, i.e., generated by an eligible economic activity that is making a substantial contribution to at least one of the climate and environmental objectives, while also doing no significant harm to the remaining objectives and meeting minimum standards on human rights and labour standards.</t>
-  </si>
-  <si>
-    <t>Relative share of the OpEx that is not part of a plan to meet the DNSH criteria and make substantial contribution to any environmental objective</t>
-  </si>
-  <si>
-    <t>Relative share of the OpEx that is part of a plan to meet the DNSH criteria and make substantial contribution to any environmental objective</t>
-  </si>
-  <si>
-    <t>Relative share of the OpEx that is associated with non taxonomy-aligned but eligible activities</t>
-  </si>
-  <si>
-    <t>Relative share of the OpEx that is associated with taxonomy-aligned activities. i.e., for an eligible economic activity that is making a substantial contribution to at least one of the climate and environmental objectives, while also doing no significant harm to the remaining objectives and meeting minimum standards on human rights and labour standards</t>
-  </si>
-  <si>
-    <t>Custom EuTaxonomyNonAlignedActivitiesComponent</t>
-  </si>
-  <si>
-    <t>Custom EuTaxonomyAlignedActivitiesComponent</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to Climate Change Mitigation In Percent - Eligible</t>
-  </si>
-  <si>
-    <t>Taxonomy-eligible proportion of revenue substantially contributing to climate change mitigation</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to Climate Change Mitigation In Percent - Aligned</t>
-  </si>
-  <si>
-    <t>Taxonomy-aligned proportion of revenue substantially contributing to climate change mitigation</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to Climate Change Mitigation In Percent - Of which use of proceeds</t>
-  </si>
-  <si>
-    <t>Taxonomy-aligned use of proceeds share substantially contributing to climate change mitigation</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to Climate Change Mitigation In Percent - Enabling Share</t>
-  </si>
-  <si>
-    <t>Taxonomy-aligned and enabling proportion of revenue substantially contributing to climate change mitigation</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to Climate Change Mitigation In Percent - Transitional Share</t>
-  </si>
-  <si>
-    <t>Taxonomy-aligned and transitional proportion of revenue substantially contributing to climate change mitigation</t>
-  </si>
-  <si>
-    <t>14.1</t>
-  </si>
-  <si>
-    <t>14.1.1</t>
-  </si>
-  <si>
-    <t>14.1.2</t>
-  </si>
-  <si>
-    <t>14.1.3</t>
-  </si>
-  <si>
-    <t>15.1</t>
-  </si>
-  <si>
-    <t>15.1.1</t>
-  </si>
-  <si>
-    <t>15.1.2</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to Climate Change Adaptation In Percent - Eligible</t>
-  </si>
-  <si>
-    <t>Taxonomy-eligible proportion of revenue substantially contributing to climate change adaptation</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to Climate Change Adaptation In Percent - Aligned</t>
-  </si>
-  <si>
-    <t>Taxonomy-aligned proportion of revenue substantially contributing to climate change adaptation</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to Climate Change Adaptation In Percent - Of which use of proceeds</t>
-  </si>
-  <si>
-    <t>Taxonomy-aligned use of proceeds share substantially contributing to climate change adaptation</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to Climate Change Adaptation In Percent - Enabling Share</t>
-  </si>
-  <si>
-    <t>Taxonomy-aligned and enabling proportion of revenue substantially contributing to climate change adaptation</t>
-  </si>
-  <si>
-    <t>16.1</t>
-  </si>
-  <si>
-    <t>16.1.1</t>
-  </si>
-  <si>
-    <t>16.1.2</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to Sustainable Use and Protection of Water and Marine Resources In Percent - Eligible</t>
-  </si>
-  <si>
-    <t>Taxonomy-eligible proportion of revenue substantially contributing to sustainable use and protection of water and marine resources</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to Sustainable Use and Protection of Water and Marine Resources In Percent - Aligned</t>
-  </si>
-  <si>
-    <t>Taxonomy-aligned proportion of revenue substantially contributing to sustainable use and protection of water and marine resources</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to Sustainable Use and Protection of Water and Marine Resources In Percent - Of which use of proceeds</t>
-  </si>
-  <si>
-    <t>Taxonomy-aligned use of proceeds share substantially contributing to sustainable use and protection of water and marine resources</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to Sustainable Use and Protection of Water and Marine Resources In Percent - Enabling Share</t>
-  </si>
-  <si>
-    <t>Taxonomy-aligned and enabling proportion of revenue substantially contributing to sustainable use and protection of water and marine resources</t>
-  </si>
-  <si>
-    <t>17.1</t>
-  </si>
-  <si>
-    <t>17.1.1</t>
-  </si>
-  <si>
-    <t>17.1.2</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to Transition to a Circular Economy In Percent - Eligible</t>
-  </si>
-  <si>
-    <t>Taxonomy-eligible proportion of revenue substantially contributing to circular economy</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to Transition to a Circular Economy In Percent - Aligned</t>
-  </si>
-  <si>
-    <t>Taxonomy-aligned proportion of revenue substantially contributing to circular economy</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to Transition to a Circular Economy In Percent - Of which use of proceeds</t>
-  </si>
-  <si>
-    <t>Taxonomy-aligned use of proceeds share substantially contributing to circular economy</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to Transition to a Circular Economy In Percent - Enabling Share</t>
-  </si>
-  <si>
-    <t>Taxonomy-aligned and enabling proportion of revenue substantially contributing to circular economy</t>
-  </si>
-  <si>
-    <t>18.1</t>
-  </si>
-  <si>
-    <t>18.1.1</t>
-  </si>
-  <si>
-    <t>18.1.2</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to Pollution Prevention and Control In Percent - Eligible</t>
-  </si>
-  <si>
-    <t>Taxonomy-eligible proportion of revenue substantially contributing to pollution prevention and control</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to Pollution Prevention and Control In Percent - Aligned</t>
-  </si>
-  <si>
-    <t>Taxonomy-aligned proportion of revenue substantially contributing to pollution prevention and control</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to Pollution Prevention and Control In Percent - Of which use of proceeds</t>
-  </si>
-  <si>
-    <t>Taxonomy-aligned use of proceeds share substantially contributing to pollution prevention and control</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to Pollution Prevention and Control In Percent - Enabling Share</t>
-  </si>
-  <si>
-    <t>Taxonomy-aligned and enabling proportion of revenue substantially contributing to pollution prevention and control</t>
-  </si>
-  <si>
-    <t>19.1</t>
-  </si>
-  <si>
-    <t>19.1.1</t>
-  </si>
-  <si>
-    <t>19.1.2</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to Protection and Restoration of Biodiversity and Ecosystems In Percent - Eligible</t>
-  </si>
-  <si>
-    <t>Taxonomy-eligible proportion of revenue substantially contributing to protection and restoration of biodiversity and ecosystems</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to Protection and Restoration of Biodiversity and Ecosystems In Percent - Aligned</t>
-  </si>
-  <si>
-    <t>Taxonomy-aligned proportion of revenue substantially contributing to protection and restoration of biodiversity and ecosystems</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to Protection and Restoration of Biodiversity and Ecosystems In Percent - Of which use of proceeds</t>
-  </si>
-  <si>
-    <t>Taxonomy-aligned use of proceeds share substantially contributing to protection and restoration of biodiversity and ecosystems</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to Protection and Restoration of Biodiversity and Ecosystems In Percent - Enabling Share</t>
-  </si>
-  <si>
-    <t>Taxonomy-aligned and enabling proportion of revenue substantially contributing to protection and restoration of biodiversity and ecosystems</t>
-  </si>
-  <si>
-    <t>29.1</t>
-  </si>
-  <si>
-    <t>29.1.1</t>
-  </si>
-  <si>
-    <t>29.1.2</t>
-  </si>
-  <si>
-    <t>29.1.3</t>
-  </si>
-  <si>
-    <t>Taxonomy-eligible proportion of CapEx substantially contributing to climate change mitigation</t>
-  </si>
-  <si>
-    <t>Taxonomy-aligned proportion of CapEx substantially contributing to climate change mitigation</t>
-  </si>
-  <si>
-    <t>Taxonomy-aligned and enabling proportion of CapEx substantially contributing to climate change mitigation</t>
-  </si>
-  <si>
-    <t>Taxonomy-aligned and transitional proportion of CapEx substantially contributing to climate change mitigation</t>
-  </si>
-  <si>
-    <t>30.1</t>
-  </si>
-  <si>
-    <t>30.1.1</t>
-  </si>
-  <si>
-    <t>30.1.2</t>
-  </si>
-  <si>
-    <t>Taxonomy-eligible proportion of CapEx substantially contributing to climate change adaptation</t>
-  </si>
-  <si>
-    <t>Taxonomy-aligned proportion of CapEx substantially contributing to climate change adaptation</t>
-  </si>
-  <si>
-    <t>Taxonomy-aligned and enabling proportion of CapEx substantially contributing to climate change adaptation</t>
-  </si>
-  <si>
-    <t>31.1</t>
-  </si>
-  <si>
-    <t>31.1.1</t>
-  </si>
-  <si>
-    <t>31.1.2</t>
-  </si>
-  <si>
-    <t>Taxonomy-eligible proportion of CapEx substantially contributing to sustainable use and protection of water and marine resources</t>
-  </si>
-  <si>
-    <t>Taxonomy-aligned proportion of CapEx substantially contributing to sustainable use and protection of water and marine resources</t>
-  </si>
-  <si>
-    <t>Taxonomy-aligned and enabling proportion of CapEx substantially contributing to sustainable use and protection of water and marine resources</t>
-  </si>
-  <si>
-    <t>32.1</t>
-  </si>
-  <si>
-    <t>32.1.1</t>
-  </si>
-  <si>
-    <t>32.1.2</t>
-  </si>
-  <si>
-    <t>Taxonomy-eligible proportion of CapEx substantially contributing to circular economy</t>
-  </si>
-  <si>
-    <t>Taxonomy-aligned proportion of CapEx substantially contributing to circular economy</t>
-  </si>
-  <si>
-    <t>Taxonomy-aligned and enabling proportion of CapEx substantially contributing to circular economy</t>
-  </si>
-  <si>
-    <t>Taxonomy-eligible proportion of CapEx substantially contributing to pollution prevention and control</t>
-  </si>
-  <si>
-    <t>Taxonomy-aligned proportion of CapEx substantially contributing to pollution prevention and control</t>
-  </si>
-  <si>
-    <t>Taxonomy-aligned and enabling proportion of CapEx substantially contributing to pollution prevention and control</t>
-  </si>
-  <si>
-    <t>Taxonomy-eligible proportion of CapEx substantially contributing to protection and restoration of biodiversity and ecosystems</t>
-  </si>
-  <si>
-    <t>Taxonomy-aligned proportion of CapEx substantially contributing to protection and restoration of biodiversity and ecosystems</t>
-  </si>
-  <si>
-    <t>Taxonomy-aligned and enabling proportion of CapEx substantially contributing to protection and restoration of biodiversity and ecosystems</t>
-  </si>
-  <si>
-    <t>33.1</t>
-  </si>
-  <si>
-    <t>33.1.1</t>
-  </si>
-  <si>
-    <t>33.1.2</t>
-  </si>
-  <si>
-    <t>34.1</t>
-  </si>
-  <si>
-    <t>34.1.1</t>
-  </si>
-  <si>
-    <t>34.1.2</t>
-  </si>
-  <si>
-    <t>Taxonomy-aligned proportion of OpEx substantially contributing to climate change mitigation</t>
-  </si>
-  <si>
-    <t>Taxonomy-aligned proportion of OpEx substantially contributing to climate change adaptation</t>
-  </si>
-  <si>
-    <t>Taxonomy-aligned proportion of OpEx substantially contributing to sustainable use and protection of water and marine resources</t>
-  </si>
-  <si>
-    <t>Taxonomy-aligned proportion of OpEx substantially contributing to circular economy</t>
-  </si>
-  <si>
-    <t>Taxonomy-aligned proportion of OpEx substantially contributing to pollution prevention and control</t>
-  </si>
-  <si>
-    <t>Taxonomy-aligned proportion of OpEx substantially contributing to protection and restoration of biodiversity and ecosystems</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -848,6 +872,18 @@
       <name val="Calibri"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="2" tint="-0.749992370372631"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="11">
     <fill>
@@ -911,7 +947,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -1065,12 +1101,44 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -1122,9 +1190,18 @@
     <xf numFmtId="0" fontId="11" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{438AC724-B8E1-4701-895E-04EF1113570C}"/>
     <cellStyle name="Normal 3" xfId="1" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1388,23 +1465,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L104"/>
+  <dimension ref="A1:L108"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14:F95"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="20.28515625" customWidth="1"/>
-    <col min="4" max="4" width="95.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="77.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="44.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="26.28515625" customWidth="1"/>
-    <col min="8" max="12" width="14.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.26953125" customWidth="1"/>
+    <col min="4" max="4" width="95.1796875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="77.81640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="44.7265625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="26.26953125" customWidth="1"/>
+    <col min="8" max="12" width="14.26953125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1442,7 +1519,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="7">
         <v>0</v>
       </c>
@@ -1460,7 +1537,7 @@
         <v>17</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="H2" s="11"/>
       <c r="I2" s="12" t="s">
@@ -1470,7 +1547,7 @@
       <c r="K2" s="12"/>
       <c r="L2" s="12"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="7"/>
       <c r="B3" s="8" t="s">
         <v>12</v>
@@ -1494,7 +1571,7 @@
       <c r="K3" s="12"/>
       <c r="L3" s="12"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="7">
         <v>1</v>
       </c>
@@ -1522,7 +1599,7 @@
       <c r="K4" s="11"/>
       <c r="L4" s="12"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="7">
         <v>2</v>
       </c>
@@ -1550,7 +1627,7 @@
       <c r="K5" s="12"/>
       <c r="L5" s="12"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="7">
         <v>3</v>
       </c>
@@ -1578,7 +1655,7 @@
       <c r="K6" s="12"/>
       <c r="L6" s="12"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="7">
         <v>4</v>
       </c>
@@ -1593,7 +1670,7 @@
         <v>32</v>
       </c>
       <c r="F7" s="27" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="G7" s="26" t="s">
         <v>14</v>
@@ -1604,7 +1681,7 @@
       <c r="K7" s="12"/>
       <c r="L7" s="12"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="7">
         <v>5</v>
       </c>
@@ -1612,14 +1689,14 @@
         <v>12</v>
       </c>
       <c r="C8" s="8"/>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="37" t="s">
         <v>26</v>
       </c>
       <c r="E8" s="12" t="s">
         <v>27</v>
       </c>
       <c r="F8" s="20" t="s">
-        <v>77</v>
+        <v>55</v>
       </c>
       <c r="G8" s="22"/>
       <c r="H8" s="12"/>
@@ -1630,7 +1707,7 @@
       <c r="K8" s="12"/>
       <c r="L8" s="12"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" s="7">
         <v>6</v>
       </c>
@@ -1638,38 +1715,40 @@
         <v>12</v>
       </c>
       <c r="C9" s="8"/>
-      <c r="D9" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="E9" s="12"/>
+      <c r="D9" s="38" t="s">
+        <v>196</v>
+      </c>
+      <c r="E9" s="34" t="s">
+        <v>203</v>
+      </c>
       <c r="F9" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="G9" s="23" t="s">
-        <v>14</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="G9" s="22"/>
       <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
+      <c r="I9" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J9" s="12"/>
       <c r="K9" s="12"/>
       <c r="L9" s="12"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" s="7">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="C10" s="8"/>
-      <c r="D10" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="E10" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="F10" s="21" t="s">
-        <v>37</v>
+      <c r="D10" s="33" t="s">
+        <v>197</v>
+      </c>
+      <c r="E10" s="35" t="s">
+        <v>198</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>25</v>
       </c>
       <c r="G10" s="22"/>
       <c r="H10" s="12"/>
@@ -1680,22 +1759,22 @@
       <c r="K10" s="12"/>
       <c r="L10" s="12"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="18" t="s">
-        <v>42</v>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A11" s="7">
+        <v>8</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="E11" s="19"/>
-      <c r="F11" s="21" t="s">
-        <v>28</v>
+        <v>12</v>
+      </c>
+      <c r="C11" s="8"/>
+      <c r="D11" s="38" t="s">
+        <v>199</v>
+      </c>
+      <c r="E11" s="36" t="s">
+        <v>200</v>
+      </c>
+      <c r="F11" s="20" t="s">
+        <v>25</v>
       </c>
       <c r="G11" s="22"/>
       <c r="H11" s="12"/>
@@ -1706,24 +1785,22 @@
       <c r="K11" s="12"/>
       <c r="L11" s="12"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="18" t="s">
-        <v>43</v>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A12" s="7">
+        <v>9</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D12" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="E12" s="28" t="s">
-        <v>84</v>
-      </c>
-      <c r="F12" s="21" t="s">
-        <v>37</v>
+        <v>12</v>
+      </c>
+      <c r="C12" s="8"/>
+      <c r="D12" s="38" t="s">
+        <v>201</v>
+      </c>
+      <c r="E12" s="35" t="s">
+        <v>202</v>
+      </c>
+      <c r="F12" s="20" t="s">
+        <v>25</v>
       </c>
       <c r="G12" s="22"/>
       <c r="H12" s="12"/>
@@ -1734,49 +1811,43 @@
       <c r="K12" s="12"/>
       <c r="L12" s="12"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="18" t="s">
-        <v>45</v>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A13" s="7">
+        <v>10</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="E13" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="F13" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="G13" s="22"/>
+        <v>12</v>
+      </c>
+      <c r="C13" s="8"/>
+      <c r="D13" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="E13" s="12"/>
+      <c r="F13" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="G13" s="23" t="s">
+        <v>14</v>
+      </c>
       <c r="H13" s="12"/>
-      <c r="I13" s="12" t="s">
-        <v>34</v>
-      </c>
+      <c r="I13" s="12"/>
       <c r="J13" s="12"/>
       <c r="K13" s="12"/>
       <c r="L13" s="12"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="18" t="s">
-        <v>46</v>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A14" s="7">
+        <v>11</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="8" t="s">
-        <v>44</v>
-      </c>
+      <c r="C14" s="8"/>
       <c r="D14" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="E14" s="12" t="s">
-        <v>107</v>
+        <v>38</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>59</v>
       </c>
       <c r="F14" s="21" t="s">
         <v>37</v>
@@ -1790,22 +1861,20 @@
       <c r="K14" s="12"/>
       <c r="L14" s="12"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" s="18" t="s">
-        <v>48</v>
+        <v>204</v>
       </c>
       <c r="B15" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="D15" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="E15" s="28" t="s">
-        <v>109</v>
-      </c>
+      <c r="E15" s="19"/>
       <c r="F15" s="21" t="s">
         <v>28</v>
       </c>
@@ -1818,21 +1887,21 @@
       <c r="K15" s="12"/>
       <c r="L15" s="12"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" s="18" t="s">
-        <v>49</v>
+        <v>205</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="D16" s="15" t="s">
         <v>41</v>
       </c>
       <c r="E16" s="28" t="s">
-        <v>106</v>
+        <v>62</v>
       </c>
       <c r="F16" s="21" t="s">
         <v>37</v>
@@ -1846,48 +1915,52 @@
       <c r="K16" s="12"/>
       <c r="L16" s="12"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" s="18" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="8"/>
+      <c r="C17" s="8" t="s">
+        <v>42</v>
+      </c>
       <c r="D17" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="E17" s="28" t="s">
-        <v>83</v>
+        <v>40</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>86</v>
       </c>
       <c r="F17" s="21" t="s">
-        <v>119</v>
+        <v>28</v>
       </c>
       <c r="G17" s="22"/>
       <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
+      <c r="I17" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J17" s="12"/>
       <c r="K17" s="12"/>
       <c r="L17" s="12"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18" s="18" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B18" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>110</v>
+        <v>85</v>
       </c>
       <c r="F18" s="21" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="G18" s="22"/>
       <c r="H18" s="12"/>
@@ -1898,24 +1971,24 @@
       <c r="K18" s="12"/>
       <c r="L18" s="12"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19" s="18" t="s">
-        <v>57</v>
+        <v>109</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="E19" s="12" t="s">
-        <v>105</v>
+        <v>40</v>
+      </c>
+      <c r="E19" s="28" t="s">
+        <v>87</v>
       </c>
       <c r="F19" s="21" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="G19" s="22"/>
       <c r="H19" s="12"/>
@@ -1926,22 +1999,24 @@
       <c r="K19" s="12"/>
       <c r="L19" s="12"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="7">
-        <v>14</v>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A20" s="18" t="s">
+        <v>206</v>
       </c>
       <c r="B20" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C20" s="8"/>
-      <c r="D20" s="29" t="s">
-        <v>121</v>
-      </c>
-      <c r="E20" s="30" t="s">
-        <v>122</v>
+      <c r="C20" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="E20" s="28" t="s">
+        <v>84</v>
       </c>
       <c r="F20" s="21" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="G20" s="22"/>
       <c r="H20" s="12"/>
@@ -1952,45 +2027,45 @@
       <c r="K20" s="12"/>
       <c r="L20" s="12"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A21" s="18" t="s">
-        <v>131</v>
+        <v>207</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C21" s="8"/>
-      <c r="D21" s="29" t="s">
-        <v>123</v>
-      </c>
-      <c r="E21" s="30" t="s">
-        <v>124</v>
+      <c r="D21" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="E21" s="28" t="s">
+        <v>61</v>
       </c>
       <c r="F21" s="21" t="s">
-        <v>28</v>
+        <v>97</v>
       </c>
       <c r="G21" s="22"/>
       <c r="H21" s="12"/>
-      <c r="I21" s="12" t="s">
-        <v>34</v>
-      </c>
+      <c r="I21" s="12"/>
       <c r="J21" s="12"/>
       <c r="K21" s="12"/>
       <c r="L21" s="12"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A22" s="18" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C22" s="8"/>
-      <c r="D22" s="31" t="s">
-        <v>125</v>
-      </c>
-      <c r="E22" s="30" t="s">
-        <v>126</v>
+      <c r="C22" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>88</v>
       </c>
       <c r="F22" s="21" t="s">
         <v>28</v>
@@ -2004,22 +2079,24 @@
       <c r="K22" s="12"/>
       <c r="L22" s="12"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A23" s="18" t="s">
-        <v>133</v>
+        <v>208</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C23" s="8"/>
-      <c r="D23" s="29" t="s">
-        <v>127</v>
-      </c>
-      <c r="E23" s="30" t="s">
-        <v>128</v>
+      <c r="C23" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>83</v>
       </c>
       <c r="F23" s="21" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="G23" s="22"/>
       <c r="H23" s="12"/>
@@ -2030,19 +2107,19 @@
       <c r="K23" s="12"/>
       <c r="L23" s="12"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="18" t="s">
-        <v>134</v>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A24" s="7">
+        <v>17</v>
       </c>
       <c r="B24" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C24" s="8"/>
       <c r="D24" s="29" t="s">
-        <v>129</v>
+        <v>99</v>
       </c>
       <c r="E24" s="30" t="s">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="F24" s="21" t="s">
         <v>28</v>
@@ -2056,19 +2133,19 @@
       <c r="K24" s="12"/>
       <c r="L24" s="12"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="7">
-        <v>15</v>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A25" s="18" t="s">
+        <v>127</v>
       </c>
       <c r="B25" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C25" s="8"/>
-      <c r="D25" s="32" t="s">
-        <v>138</v>
+      <c r="D25" s="29" t="s">
+        <v>101</v>
       </c>
       <c r="E25" s="30" t="s">
-        <v>139</v>
+        <v>102</v>
       </c>
       <c r="F25" s="21" t="s">
         <v>28</v>
@@ -2082,19 +2159,19 @@
       <c r="K25" s="12"/>
       <c r="L25" s="12"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A26" s="18" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="B26" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C26" s="8"/>
-      <c r="D26" s="32" t="s">
-        <v>140</v>
+      <c r="D26" s="31" t="s">
+        <v>103</v>
       </c>
       <c r="E26" s="30" t="s">
-        <v>141</v>
+        <v>104</v>
       </c>
       <c r="F26" s="21" t="s">
         <v>28</v>
@@ -2108,19 +2185,19 @@
       <c r="K26" s="12"/>
       <c r="L26" s="12"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A27" s="18" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="B27" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C27" s="8"/>
-      <c r="D27" s="31" t="s">
-        <v>142</v>
+      <c r="D27" s="29" t="s">
+        <v>105</v>
       </c>
       <c r="E27" s="30" t="s">
-        <v>143</v>
+        <v>106</v>
       </c>
       <c r="F27" s="21" t="s">
         <v>28</v>
@@ -2134,19 +2211,19 @@
       <c r="K27" s="12"/>
       <c r="L27" s="12"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A28" s="18" t="s">
-        <v>137</v>
+        <v>209</v>
       </c>
       <c r="B28" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C28" s="8"/>
-      <c r="D28" s="31" t="s">
-        <v>144</v>
+      <c r="D28" s="29" t="s">
+        <v>107</v>
       </c>
       <c r="E28" s="30" t="s">
-        <v>145</v>
+        <v>108</v>
       </c>
       <c r="F28" s="21" t="s">
         <v>28</v>
@@ -2160,19 +2237,19 @@
       <c r="K28" s="12"/>
       <c r="L28" s="12"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A29" s="7">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B29" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C29" s="8"/>
-      <c r="D29" s="31" t="s">
-        <v>149</v>
+      <c r="D29" s="32" t="s">
+        <v>110</v>
       </c>
       <c r="E29" s="30" t="s">
-        <v>150</v>
+        <v>111</v>
       </c>
       <c r="F29" s="21" t="s">
         <v>28</v>
@@ -2186,19 +2263,19 @@
       <c r="K29" s="12"/>
       <c r="L29" s="12"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A30" s="18" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="B30" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C30" s="8"/>
-      <c r="D30" s="31" t="s">
-        <v>151</v>
+      <c r="D30" s="32" t="s">
+        <v>112</v>
       </c>
       <c r="E30" s="30" t="s">
-        <v>152</v>
+        <v>113</v>
       </c>
       <c r="F30" s="21" t="s">
         <v>28</v>
@@ -2212,19 +2289,19 @@
       <c r="K30" s="12"/>
       <c r="L30" s="12"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A31" s="18" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="B31" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C31" s="8"/>
       <c r="D31" s="31" t="s">
-        <v>153</v>
+        <v>114</v>
       </c>
       <c r="E31" s="30" t="s">
-        <v>154</v>
+        <v>115</v>
       </c>
       <c r="F31" s="21" t="s">
         <v>28</v>
@@ -2238,19 +2315,19 @@
       <c r="K31" s="12"/>
       <c r="L31" s="12"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A32" s="18" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="B32" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C32" s="8"/>
       <c r="D32" s="31" t="s">
-        <v>155</v>
+        <v>116</v>
       </c>
       <c r="E32" s="30" t="s">
-        <v>156</v>
+        <v>117</v>
       </c>
       <c r="F32" s="21" t="s">
         <v>28</v>
@@ -2264,19 +2341,19 @@
       <c r="K32" s="12"/>
       <c r="L32" s="12"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A33" s="7">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B33" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C33" s="8"/>
       <c r="D33" s="31" t="s">
-        <v>160</v>
+        <v>119</v>
       </c>
       <c r="E33" s="30" t="s">
-        <v>161</v>
+        <v>120</v>
       </c>
       <c r="F33" s="21" t="s">
         <v>28</v>
@@ -2290,19 +2367,19 @@
       <c r="K33" s="12"/>
       <c r="L33" s="12"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A34" s="18" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="B34" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C34" s="8"/>
       <c r="D34" s="31" t="s">
-        <v>162</v>
+        <v>121</v>
       </c>
       <c r="E34" s="30" t="s">
-        <v>163</v>
+        <v>122</v>
       </c>
       <c r="F34" s="21" t="s">
         <v>28</v>
@@ -2316,19 +2393,19 @@
       <c r="K34" s="12"/>
       <c r="L34" s="12"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A35" s="18" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="B35" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C35" s="8"/>
       <c r="D35" s="31" t="s">
-        <v>164</v>
+        <v>123</v>
       </c>
       <c r="E35" s="30" t="s">
-        <v>165</v>
+        <v>124</v>
       </c>
       <c r="F35" s="21" t="s">
         <v>28</v>
@@ -2342,19 +2419,19 @@
       <c r="K35" s="12"/>
       <c r="L35" s="12"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A36" s="18" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B36" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C36" s="8"/>
       <c r="D36" s="31" t="s">
-        <v>166</v>
+        <v>125</v>
       </c>
       <c r="E36" s="30" t="s">
-        <v>167</v>
+        <v>126</v>
       </c>
       <c r="F36" s="21" t="s">
         <v>28</v>
@@ -2368,19 +2445,19 @@
       <c r="K36" s="12"/>
       <c r="L36" s="12"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A37" s="7">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B37" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C37" s="8"/>
       <c r="D37" s="31" t="s">
-        <v>171</v>
+        <v>130</v>
       </c>
       <c r="E37" s="30" t="s">
-        <v>172</v>
+        <v>131</v>
       </c>
       <c r="F37" s="21" t="s">
         <v>28</v>
@@ -2394,19 +2471,19 @@
       <c r="K37" s="12"/>
       <c r="L37" s="12"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A38" s="18" t="s">
-        <v>168</v>
+        <v>210</v>
       </c>
       <c r="B38" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C38" s="8"/>
       <c r="D38" s="31" t="s">
-        <v>173</v>
+        <v>132</v>
       </c>
       <c r="E38" s="30" t="s">
-        <v>174</v>
+        <v>133</v>
       </c>
       <c r="F38" s="21" t="s">
         <v>28</v>
@@ -2420,19 +2497,19 @@
       <c r="K38" s="12"/>
       <c r="L38" s="12"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A39" s="18" t="s">
-        <v>169</v>
+        <v>211</v>
       </c>
       <c r="B39" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C39" s="8"/>
       <c r="D39" s="31" t="s">
-        <v>175</v>
+        <v>134</v>
       </c>
       <c r="E39" s="30" t="s">
-        <v>176</v>
+        <v>135</v>
       </c>
       <c r="F39" s="21" t="s">
         <v>28</v>
@@ -2446,19 +2523,19 @@
       <c r="K39" s="12"/>
       <c r="L39" s="12"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A40" s="18" t="s">
-        <v>170</v>
+        <v>212</v>
       </c>
       <c r="B40" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C40" s="8"/>
       <c r="D40" s="31" t="s">
-        <v>177</v>
+        <v>136</v>
       </c>
       <c r="E40" s="30" t="s">
-        <v>178</v>
+        <v>137</v>
       </c>
       <c r="F40" s="21" t="s">
         <v>28</v>
@@ -2472,19 +2549,19 @@
       <c r="K40" s="12"/>
       <c r="L40" s="12"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A41" s="7">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B41" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C41" s="8"/>
       <c r="D41" s="31" t="s">
-        <v>182</v>
+        <v>141</v>
       </c>
       <c r="E41" s="30" t="s">
-        <v>183</v>
+        <v>142</v>
       </c>
       <c r="F41" s="21" t="s">
         <v>28</v>
@@ -2498,19 +2575,19 @@
       <c r="K41" s="12"/>
       <c r="L41" s="12"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A42" s="18" t="s">
-        <v>179</v>
+        <v>213</v>
       </c>
       <c r="B42" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C42" s="8"/>
       <c r="D42" s="31" t="s">
-        <v>184</v>
+        <v>143</v>
       </c>
       <c r="E42" s="30" t="s">
-        <v>185</v>
+        <v>144</v>
       </c>
       <c r="F42" s="21" t="s">
         <v>28</v>
@@ -2524,19 +2601,19 @@
       <c r="K42" s="12"/>
       <c r="L42" s="12"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A43" s="18" t="s">
-        <v>180</v>
+        <v>214</v>
       </c>
       <c r="B43" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C43" s="8"/>
       <c r="D43" s="31" t="s">
-        <v>186</v>
+        <v>145</v>
       </c>
       <c r="E43" s="30" t="s">
-        <v>187</v>
+        <v>146</v>
       </c>
       <c r="F43" s="21" t="s">
         <v>28</v>
@@ -2550,19 +2627,19 @@
       <c r="K43" s="12"/>
       <c r="L43" s="12"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A44" s="18" t="s">
-        <v>181</v>
+        <v>215</v>
       </c>
       <c r="B44" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C44" s="8"/>
       <c r="D44" s="31" t="s">
-        <v>188</v>
+        <v>147</v>
       </c>
       <c r="E44" s="30" t="s">
-        <v>189</v>
+        <v>148</v>
       </c>
       <c r="F44" s="21" t="s">
         <v>28</v>
@@ -2576,43 +2653,45 @@
       <c r="K44" s="12"/>
       <c r="L44" s="12"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A45" s="7">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B45" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C45" s="8"/>
-      <c r="D45" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="E45" s="28" t="s">
-        <v>82</v>
+      <c r="D45" s="31" t="s">
+        <v>152</v>
+      </c>
+      <c r="E45" s="30" t="s">
+        <v>153</v>
       </c>
       <c r="F45" s="21" t="s">
-        <v>120</v>
+        <v>28</v>
       </c>
       <c r="G45" s="22"/>
       <c r="H45" s="12"/>
-      <c r="I45" s="12"/>
+      <c r="I45" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J45" s="12"/>
       <c r="K45" s="12"/>
       <c r="L45" s="12"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A46" s="7">
-        <v>21</v>
-      </c>
-      <c r="B46" s="16" t="s">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A46" s="18" t="s">
+        <v>216</v>
+      </c>
+      <c r="B46" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C46" s="16"/>
-      <c r="D46" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="E46" s="28" t="s">
-        <v>85</v>
+      <c r="C46" s="8"/>
+      <c r="D46" s="31" t="s">
+        <v>154</v>
+      </c>
+      <c r="E46" s="30" t="s">
+        <v>155</v>
       </c>
       <c r="F46" s="21" t="s">
         <v>28</v>
@@ -2626,19 +2705,19 @@
       <c r="K46" s="12"/>
       <c r="L46" s="12"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A47" s="7">
-        <v>22</v>
-      </c>
-      <c r="B47" s="16" t="s">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A47" s="18" t="s">
+        <v>217</v>
+      </c>
+      <c r="B47" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C47" s="16"/>
-      <c r="D47" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="E47" s="28" t="s">
-        <v>86</v>
+      <c r="C47" s="8"/>
+      <c r="D47" s="31" t="s">
+        <v>156</v>
+      </c>
+      <c r="E47" s="30" t="s">
+        <v>157</v>
       </c>
       <c r="F47" s="21" t="s">
         <v>28</v>
@@ -2652,22 +2731,22 @@
       <c r="K47" s="12"/>
       <c r="L47" s="12"/>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A48" s="7">
-        <v>23</v>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A48" s="18" t="s">
+        <v>218</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C48" s="8"/>
-      <c r="D48" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="E48" s="28" t="s">
-        <v>87</v>
+      <c r="D48" s="31" t="s">
+        <v>158</v>
+      </c>
+      <c r="E48" s="30" t="s">
+        <v>159</v>
       </c>
       <c r="F48" s="21" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="G48" s="22"/>
       <c r="H48" s="12"/>
@@ -2678,52 +2757,46 @@
       <c r="K48" s="12"/>
       <c r="L48" s="12"/>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A49" s="18" t="s">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A49" s="7">
+        <v>23</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C49" s="8"/>
+      <c r="D49" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="E49" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="B49" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C49" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D49" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="E49" s="28" t="s">
-        <v>111</v>
-      </c>
       <c r="F49" s="21" t="s">
-        <v>28</v>
+        <v>98</v>
       </c>
       <c r="G49" s="22"/>
       <c r="H49" s="12"/>
-      <c r="I49" s="12" t="s">
-        <v>34</v>
-      </c>
+      <c r="I49" s="12"/>
       <c r="J49" s="12"/>
       <c r="K49" s="12"/>
       <c r="L49" s="12"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A50" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="B50" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C50" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D50" s="15" t="s">
-        <v>41</v>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A50" s="7">
+        <v>24</v>
+      </c>
+      <c r="B50" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C50" s="16"/>
+      <c r="D50" s="17" t="s">
+        <v>47</v>
       </c>
       <c r="E50" s="28" t="s">
-        <v>100</v>
+        <v>63</v>
       </c>
       <c r="F50" s="21" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="G50" s="22"/>
       <c r="H50" s="12"/>
@@ -2734,21 +2807,19 @@
       <c r="K50" s="12"/>
       <c r="L50" s="12"/>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A51" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="B51" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C51" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="D51" s="15" t="s">
-        <v>40</v>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A51" s="7">
+        <v>25</v>
+      </c>
+      <c r="B51" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C51" s="16"/>
+      <c r="D51" s="17" t="s">
+        <v>48</v>
       </c>
       <c r="E51" s="28" t="s">
-        <v>112</v>
+        <v>64</v>
       </c>
       <c r="F51" s="21" t="s">
         <v>28</v>
@@ -2762,21 +2833,19 @@
       <c r="K51" s="12"/>
       <c r="L51" s="12"/>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A52" s="18" t="s">
-        <v>59</v>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A52" s="7">
+        <v>26</v>
       </c>
       <c r="B52" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C52" s="8" t="s">
-        <v>44</v>
-      </c>
+      <c r="C52" s="8"/>
       <c r="D52" s="15" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E52" s="28" t="s">
-        <v>95</v>
+        <v>65</v>
       </c>
       <c r="F52" s="21" t="s">
         <v>37</v>
@@ -2790,21 +2859,21 @@
       <c r="K52" s="12"/>
       <c r="L52" s="12"/>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A53" s="18" t="s">
-        <v>62</v>
+        <v>219</v>
       </c>
       <c r="B53" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="D53" s="15" t="s">
         <v>40</v>
       </c>
       <c r="E53" s="28" t="s">
-        <v>113</v>
+        <v>89</v>
       </c>
       <c r="F53" s="21" t="s">
         <v>28</v>
@@ -2818,21 +2887,21 @@
       <c r="K53" s="12"/>
       <c r="L53" s="12"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A54" s="18" t="s">
-        <v>63</v>
+        <v>220</v>
       </c>
       <c r="B54" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="D54" s="15" t="s">
         <v>41</v>
       </c>
       <c r="E54" s="28" t="s">
-        <v>99</v>
+        <v>78</v>
       </c>
       <c r="F54" s="21" t="s">
         <v>37</v>
@@ -2846,48 +2915,52 @@
       <c r="K54" s="12"/>
       <c r="L54" s="12"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A55" s="18" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="B55" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C55" s="8"/>
+      <c r="C55" s="8" t="s">
+        <v>42</v>
+      </c>
       <c r="D55" s="15" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="E55" s="28" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="F55" s="21" t="s">
-        <v>119</v>
+        <v>28</v>
       </c>
       <c r="G55" s="22"/>
       <c r="H55" s="12"/>
-      <c r="I55" s="12"/>
+      <c r="I55" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J55" s="12"/>
       <c r="K55" s="12"/>
       <c r="L55" s="12"/>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A56" s="18" t="s">
-        <v>65</v>
+        <v>241</v>
       </c>
       <c r="B56" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="D56" s="15" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E56" s="28" t="s">
-        <v>114</v>
+        <v>73</v>
       </c>
       <c r="F56" s="21" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="G56" s="22"/>
       <c r="H56" s="12"/>
@@ -2898,24 +2971,24 @@
       <c r="K56" s="12"/>
       <c r="L56" s="12"/>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A57" s="18" t="s">
-        <v>66</v>
+        <v>160</v>
       </c>
       <c r="B57" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="D57" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E57" s="28" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="F57" s="21" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="G57" s="22"/>
       <c r="H57" s="12"/>
@@ -2926,22 +2999,24 @@
       <c r="K57" s="12"/>
       <c r="L57" s="12"/>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A58" s="7">
-        <v>29</v>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A58" s="18" t="s">
+        <v>221</v>
       </c>
       <c r="B58" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C58" s="8"/>
-      <c r="D58" s="29" t="s">
-        <v>121</v>
-      </c>
-      <c r="E58" s="30" t="s">
-        <v>194</v>
+      <c r="C58" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D58" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="E58" s="28" t="s">
+        <v>77</v>
       </c>
       <c r="F58" s="21" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="G58" s="22"/>
       <c r="H58" s="12"/>
@@ -2952,45 +3027,45 @@
       <c r="K58" s="12"/>
       <c r="L58" s="12"/>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A59" s="18" t="s">
-        <v>190</v>
+        <v>222</v>
       </c>
       <c r="B59" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C59" s="8"/>
-      <c r="D59" s="29" t="s">
-        <v>123</v>
-      </c>
-      <c r="E59" s="30" t="s">
-        <v>195</v>
+      <c r="D59" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="E59" s="28" t="s">
+        <v>76</v>
       </c>
       <c r="F59" s="21" t="s">
-        <v>28</v>
+        <v>97</v>
       </c>
       <c r="G59" s="22"/>
       <c r="H59" s="12"/>
-      <c r="I59" s="12" t="s">
-        <v>34</v>
-      </c>
+      <c r="I59" s="12"/>
       <c r="J59" s="12"/>
       <c r="K59" s="12"/>
       <c r="L59" s="12"/>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A60" s="18" t="s">
-        <v>191</v>
+        <v>168</v>
       </c>
       <c r="B60" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C60" s="8"/>
-      <c r="D60" s="31" t="s">
-        <v>125</v>
-      </c>
-      <c r="E60" s="30" t="s">
-        <v>126</v>
+      <c r="C60" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D60" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="E60" s="28" t="s">
+        <v>92</v>
       </c>
       <c r="F60" s="21" t="s">
         <v>28</v>
@@ -3004,22 +3079,24 @@
       <c r="K60" s="12"/>
       <c r="L60" s="12"/>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A61" s="18" t="s">
-        <v>192</v>
+        <v>223</v>
       </c>
       <c r="B61" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C61" s="8"/>
-      <c r="D61" s="29" t="s">
-        <v>127</v>
-      </c>
-      <c r="E61" s="30" t="s">
-        <v>196</v>
+      <c r="C61" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D61" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="E61" s="28" t="s">
+        <v>74</v>
       </c>
       <c r="F61" s="21" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="G61" s="22"/>
       <c r="H61" s="12"/>
@@ -3030,19 +3107,19 @@
       <c r="K61" s="12"/>
       <c r="L61" s="12"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A62" s="18" t="s">
-        <v>193</v>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A62" s="7">
+        <v>32</v>
       </c>
       <c r="B62" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C62" s="8"/>
       <c r="D62" s="29" t="s">
-        <v>129</v>
+        <v>99</v>
       </c>
       <c r="E62" s="30" t="s">
-        <v>197</v>
+        <v>161</v>
       </c>
       <c r="F62" s="21" t="s">
         <v>28</v>
@@ -3056,19 +3133,19 @@
       <c r="K62" s="12"/>
       <c r="L62" s="12"/>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A63" s="7">
-        <v>30</v>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A63" s="18" t="s">
+        <v>172</v>
       </c>
       <c r="B63" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C63" s="8"/>
-      <c r="D63" s="32" t="s">
-        <v>138</v>
+      <c r="D63" s="29" t="s">
+        <v>101</v>
       </c>
       <c r="E63" s="30" t="s">
-        <v>201</v>
+        <v>162</v>
       </c>
       <c r="F63" s="21" t="s">
         <v>28</v>
@@ -3082,19 +3159,19 @@
       <c r="K63" s="12"/>
       <c r="L63" s="12"/>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A64" s="18" t="s">
-        <v>198</v>
+        <v>173</v>
       </c>
       <c r="B64" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C64" s="8"/>
-      <c r="D64" s="32" t="s">
-        <v>140</v>
+      <c r="D64" s="31" t="s">
+        <v>103</v>
       </c>
       <c r="E64" s="30" t="s">
-        <v>202</v>
+        <v>104</v>
       </c>
       <c r="F64" s="21" t="s">
         <v>28</v>
@@ -3108,19 +3185,19 @@
       <c r="K64" s="12"/>
       <c r="L64" s="12"/>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A65" s="18" t="s">
-        <v>199</v>
+        <v>174</v>
       </c>
       <c r="B65" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C65" s="8"/>
-      <c r="D65" s="31" t="s">
-        <v>142</v>
+      <c r="D65" s="29" t="s">
+        <v>105</v>
       </c>
       <c r="E65" s="30" t="s">
-        <v>143</v>
+        <v>163</v>
       </c>
       <c r="F65" s="21" t="s">
         <v>28</v>
@@ -3134,19 +3211,19 @@
       <c r="K65" s="12"/>
       <c r="L65" s="12"/>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A66" s="18" t="s">
-        <v>200</v>
+        <v>224</v>
       </c>
       <c r="B66" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C66" s="8"/>
-      <c r="D66" s="31" t="s">
-        <v>144</v>
+      <c r="D66" s="29" t="s">
+        <v>107</v>
       </c>
       <c r="E66" s="30" t="s">
-        <v>203</v>
+        <v>164</v>
       </c>
       <c r="F66" s="21" t="s">
         <v>28</v>
@@ -3160,19 +3237,19 @@
       <c r="K66" s="12"/>
       <c r="L66" s="12"/>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A67" s="7">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B67" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C67" s="8"/>
-      <c r="D67" s="31" t="s">
-        <v>149</v>
+      <c r="D67" s="32" t="s">
+        <v>110</v>
       </c>
       <c r="E67" s="30" t="s">
-        <v>207</v>
+        <v>165</v>
       </c>
       <c r="F67" s="21" t="s">
         <v>28</v>
@@ -3186,19 +3263,19 @@
       <c r="K67" s="12"/>
       <c r="L67" s="12"/>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A68" s="18" t="s">
-        <v>204</v>
+        <v>184</v>
       </c>
       <c r="B68" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C68" s="8"/>
-      <c r="D68" s="31" t="s">
-        <v>151</v>
+      <c r="D68" s="32" t="s">
+        <v>112</v>
       </c>
       <c r="E68" s="30" t="s">
-        <v>208</v>
+        <v>166</v>
       </c>
       <c r="F68" s="21" t="s">
         <v>28</v>
@@ -3212,19 +3289,19 @@
       <c r="K68" s="12"/>
       <c r="L68" s="12"/>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A69" s="18" t="s">
-        <v>205</v>
+        <v>185</v>
       </c>
       <c r="B69" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C69" s="8"/>
       <c r="D69" s="31" t="s">
-        <v>153</v>
+        <v>114</v>
       </c>
       <c r="E69" s="30" t="s">
-        <v>154</v>
+        <v>115</v>
       </c>
       <c r="F69" s="21" t="s">
         <v>28</v>
@@ -3238,19 +3315,19 @@
       <c r="K69" s="12"/>
       <c r="L69" s="12"/>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A70" s="18" t="s">
-        <v>206</v>
+        <v>186</v>
       </c>
       <c r="B70" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C70" s="8"/>
       <c r="D70" s="31" t="s">
-        <v>155</v>
+        <v>116</v>
       </c>
       <c r="E70" s="30" t="s">
-        <v>209</v>
+        <v>167</v>
       </c>
       <c r="F70" s="21" t="s">
         <v>28</v>
@@ -3264,19 +3341,19 @@
       <c r="K70" s="12"/>
       <c r="L70" s="12"/>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A71" s="7">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B71" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C71" s="8"/>
       <c r="D71" s="31" t="s">
-        <v>160</v>
+        <v>119</v>
       </c>
       <c r="E71" s="30" t="s">
-        <v>213</v>
+        <v>169</v>
       </c>
       <c r="F71" s="21" t="s">
         <v>28</v>
@@ -3290,19 +3367,19 @@
       <c r="K71" s="12"/>
       <c r="L71" s="12"/>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A72" s="18" t="s">
-        <v>210</v>
+        <v>187</v>
       </c>
       <c r="B72" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C72" s="8"/>
       <c r="D72" s="31" t="s">
-        <v>162</v>
+        <v>121</v>
       </c>
       <c r="E72" s="30" t="s">
-        <v>214</v>
+        <v>170</v>
       </c>
       <c r="F72" s="21" t="s">
         <v>28</v>
@@ -3316,19 +3393,19 @@
       <c r="K72" s="12"/>
       <c r="L72" s="12"/>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A73" s="18" t="s">
-        <v>211</v>
+        <v>188</v>
       </c>
       <c r="B73" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C73" s="8"/>
       <c r="D73" s="31" t="s">
-        <v>164</v>
+        <v>123</v>
       </c>
       <c r="E73" s="30" t="s">
-        <v>165</v>
+        <v>124</v>
       </c>
       <c r="F73" s="21" t="s">
         <v>28</v>
@@ -3342,19 +3419,19 @@
       <c r="K73" s="12"/>
       <c r="L73" s="12"/>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A74" s="18" t="s">
-        <v>212</v>
+        <v>189</v>
       </c>
       <c r="B74" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C74" s="8"/>
       <c r="D74" s="31" t="s">
-        <v>166</v>
+        <v>125</v>
       </c>
       <c r="E74" s="30" t="s">
-        <v>215</v>
+        <v>171</v>
       </c>
       <c r="F74" s="21" t="s">
         <v>28</v>
@@ -3368,19 +3445,19 @@
       <c r="K74" s="12"/>
       <c r="L74" s="12"/>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A75" s="7">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B75" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C75" s="8"/>
       <c r="D75" s="31" t="s">
-        <v>171</v>
+        <v>130</v>
       </c>
       <c r="E75" s="30" t="s">
-        <v>216</v>
+        <v>175</v>
       </c>
       <c r="F75" s="21" t="s">
         <v>28</v>
@@ -3394,19 +3471,19 @@
       <c r="K75" s="12"/>
       <c r="L75" s="12"/>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A76" s="18" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="B76" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C76" s="8"/>
       <c r="D76" s="31" t="s">
-        <v>173</v>
+        <v>132</v>
       </c>
       <c r="E76" s="30" t="s">
-        <v>217</v>
+        <v>176</v>
       </c>
       <c r="F76" s="21" t="s">
         <v>28</v>
@@ -3420,19 +3497,19 @@
       <c r="K76" s="12"/>
       <c r="L76" s="12"/>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A77" s="18" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="B77" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C77" s="8"/>
       <c r="D77" s="31" t="s">
-        <v>175</v>
+        <v>134</v>
       </c>
       <c r="E77" s="30" t="s">
-        <v>176</v>
+        <v>135</v>
       </c>
       <c r="F77" s="21" t="s">
         <v>28</v>
@@ -3446,19 +3523,19 @@
       <c r="K77" s="12"/>
       <c r="L77" s="12"/>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A78" s="18" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="B78" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C78" s="8"/>
       <c r="D78" s="31" t="s">
+        <v>136</v>
+      </c>
+      <c r="E78" s="30" t="s">
         <v>177</v>
-      </c>
-      <c r="E78" s="30" t="s">
-        <v>218</v>
       </c>
       <c r="F78" s="21" t="s">
         <v>28</v>
@@ -3472,19 +3549,19 @@
       <c r="K78" s="12"/>
       <c r="L78" s="12"/>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A79" s="7">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B79" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C79" s="8"/>
       <c r="D79" s="31" t="s">
-        <v>182</v>
+        <v>141</v>
       </c>
       <c r="E79" s="30" t="s">
-        <v>219</v>
+        <v>178</v>
       </c>
       <c r="F79" s="21" t="s">
         <v>28</v>
@@ -3498,19 +3575,19 @@
       <c r="K79" s="12"/>
       <c r="L79" s="12"/>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A80" s="18" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="B80" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C80" s="8"/>
       <c r="D80" s="31" t="s">
-        <v>184</v>
+        <v>143</v>
       </c>
       <c r="E80" s="30" t="s">
-        <v>220</v>
+        <v>179</v>
       </c>
       <c r="F80" s="21" t="s">
         <v>28</v>
@@ -3524,19 +3601,19 @@
       <c r="K80" s="12"/>
       <c r="L80" s="12"/>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A81" s="18" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="B81" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C81" s="8"/>
       <c r="D81" s="31" t="s">
-        <v>186</v>
+        <v>145</v>
       </c>
       <c r="E81" s="30" t="s">
-        <v>187</v>
+        <v>146</v>
       </c>
       <c r="F81" s="21" t="s">
         <v>28</v>
@@ -3550,19 +3627,19 @@
       <c r="K81" s="12"/>
       <c r="L81" s="12"/>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A82" s="18" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="B82" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C82" s="8"/>
       <c r="D82" s="31" t="s">
-        <v>188</v>
+        <v>147</v>
       </c>
       <c r="E82" s="30" t="s">
-        <v>221</v>
+        <v>180</v>
       </c>
       <c r="F82" s="21" t="s">
         <v>28</v>
@@ -3576,43 +3653,45 @@
       <c r="K82" s="12"/>
       <c r="L82" s="12"/>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A83" s="7">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B83" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C83" s="8"/>
-      <c r="D83" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="E83" s="28" t="s">
-        <v>97</v>
+      <c r="D83" s="31" t="s">
+        <v>152</v>
+      </c>
+      <c r="E83" s="30" t="s">
+        <v>181</v>
       </c>
       <c r="F83" s="21" t="s">
-        <v>120</v>
+        <v>28</v>
       </c>
       <c r="G83" s="22"/>
       <c r="H83" s="12"/>
-      <c r="I83" s="12"/>
+      <c r="I83" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J83" s="12"/>
       <c r="K83" s="12"/>
       <c r="L83" s="12"/>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A84" s="7">
-        <v>36</v>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A84" s="18" t="s">
+        <v>231</v>
       </c>
       <c r="B84" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C84" s="16"/>
-      <c r="D84" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="E84" s="28" t="s">
-        <v>88</v>
+      <c r="C84" s="8"/>
+      <c r="D84" s="31" t="s">
+        <v>154</v>
+      </c>
+      <c r="E84" s="30" t="s">
+        <v>182</v>
       </c>
       <c r="F84" s="21" t="s">
         <v>28</v>
@@ -3626,19 +3705,19 @@
       <c r="K84" s="12"/>
       <c r="L84" s="12"/>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A85" s="7">
-        <v>37</v>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A85" s="18" t="s">
+        <v>232</v>
       </c>
       <c r="B85" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C85" s="16"/>
-      <c r="D85" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="E85" s="28" t="s">
-        <v>89</v>
+      <c r="C85" s="8"/>
+      <c r="D85" s="31" t="s">
+        <v>156</v>
+      </c>
+      <c r="E85" s="30" t="s">
+        <v>157</v>
       </c>
       <c r="F85" s="21" t="s">
         <v>28</v>
@@ -3652,22 +3731,22 @@
       <c r="K85" s="12"/>
       <c r="L85" s="12"/>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A86" s="7">
-        <v>38</v>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A86" s="18" t="s">
+        <v>233</v>
       </c>
       <c r="B86" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C86" s="8"/>
-      <c r="D86" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="E86" s="28" t="s">
-        <v>90</v>
+      <c r="D86" s="31" t="s">
+        <v>158</v>
+      </c>
+      <c r="E86" s="30" t="s">
+        <v>183</v>
       </c>
       <c r="F86" s="21" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="G86" s="22"/>
       <c r="H86" s="12"/>
@@ -3678,52 +3757,46 @@
       <c r="K86" s="12"/>
       <c r="L86" s="12"/>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A87" s="18" t="s">
-        <v>67</v>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A87" s="7">
+        <v>38</v>
       </c>
       <c r="B87" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C87" s="8" t="s">
-        <v>39</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="C87" s="8"/>
       <c r="D87" s="15" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="E87" s="28" t="s">
-        <v>115</v>
+        <v>75</v>
       </c>
       <c r="F87" s="21" t="s">
-        <v>28</v>
+        <v>98</v>
       </c>
       <c r="G87" s="22"/>
       <c r="H87" s="12"/>
-      <c r="I87" s="12" t="s">
-        <v>34</v>
-      </c>
+      <c r="I87" s="12"/>
       <c r="J87" s="12"/>
       <c r="K87" s="12"/>
       <c r="L87" s="12"/>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A88" s="18" t="s">
-        <v>68</v>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A88" s="7">
+        <v>39</v>
       </c>
       <c r="B88" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C88" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D88" s="15" t="s">
-        <v>41</v>
+        <v>35</v>
+      </c>
+      <c r="C88" s="16"/>
+      <c r="D88" s="17" t="s">
+        <v>47</v>
       </c>
       <c r="E88" s="28" t="s">
-        <v>101</v>
+        <v>66</v>
       </c>
       <c r="F88" s="21" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="G88" s="22"/>
       <c r="H88" s="12"/>
@@ -3734,21 +3807,19 @@
       <c r="K88" s="12"/>
       <c r="L88" s="12"/>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A89" s="18" t="s">
-        <v>69</v>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A89" s="7">
+        <v>40</v>
       </c>
       <c r="B89" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C89" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="D89" s="15" t="s">
-        <v>40</v>
+        <v>35</v>
+      </c>
+      <c r="C89" s="16"/>
+      <c r="D89" s="17" t="s">
+        <v>48</v>
       </c>
       <c r="E89" s="28" t="s">
-        <v>116</v>
+        <v>67</v>
       </c>
       <c r="F89" s="21" t="s">
         <v>28</v>
@@ -3762,21 +3833,19 @@
       <c r="K89" s="12"/>
       <c r="L89" s="12"/>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A90" s="18" t="s">
-        <v>70</v>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A90" s="7">
+        <v>41</v>
       </c>
       <c r="B90" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C90" s="8" t="s">
-        <v>44</v>
-      </c>
+      <c r="C90" s="8"/>
       <c r="D90" s="15" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E90" s="28" t="s">
-        <v>102</v>
+        <v>68</v>
       </c>
       <c r="F90" s="21" t="s">
         <v>37</v>
@@ -3790,21 +3859,21 @@
       <c r="K90" s="12"/>
       <c r="L90" s="12"/>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A91" s="18" t="s">
-        <v>71</v>
+        <v>234</v>
       </c>
       <c r="B91" s="8" t="s">
         <v>36</v>
       </c>
       <c r="C91" s="8" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="D91" s="15" t="s">
         <v>40</v>
       </c>
       <c r="E91" s="28" t="s">
-        <v>117</v>
+        <v>93</v>
       </c>
       <c r="F91" s="21" t="s">
         <v>28</v>
@@ -3818,21 +3887,21 @@
       <c r="K91" s="12"/>
       <c r="L91" s="12"/>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A92" s="18" t="s">
-        <v>72</v>
+        <v>235</v>
       </c>
       <c r="B92" s="8" t="s">
         <v>36</v>
       </c>
       <c r="C92" s="8" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="D92" s="15" t="s">
         <v>41</v>
       </c>
       <c r="E92" s="28" t="s">
-        <v>103</v>
+        <v>79</v>
       </c>
       <c r="F92" s="21" t="s">
         <v>37</v>
@@ -3846,48 +3915,52 @@
       <c r="K92" s="12"/>
       <c r="L92" s="12"/>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A93" s="18" t="s">
-        <v>73</v>
+        <v>52</v>
       </c>
       <c r="B93" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C93" s="8"/>
+      <c r="C93" s="8" t="s">
+        <v>42</v>
+      </c>
       <c r="D93" s="15" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="E93" s="28" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="F93" s="21" t="s">
-        <v>119</v>
+        <v>28</v>
       </c>
       <c r="G93" s="22"/>
       <c r="H93" s="12"/>
-      <c r="I93" s="12"/>
+      <c r="I93" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J93" s="12"/>
       <c r="K93" s="12"/>
       <c r="L93" s="12"/>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A94" s="18" t="s">
-        <v>74</v>
+        <v>53</v>
       </c>
       <c r="B94" s="8" t="s">
         <v>36</v>
       </c>
       <c r="C94" s="8" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="D94" s="15" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E94" s="28" t="s">
-        <v>118</v>
+        <v>80</v>
       </c>
       <c r="F94" s="21" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="G94" s="22"/>
       <c r="H94" s="12"/>
@@ -3898,24 +3971,24 @@
       <c r="K94" s="12"/>
       <c r="L94" s="12"/>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A95" s="18" t="s">
-        <v>75</v>
+        <v>236</v>
       </c>
       <c r="B95" s="8" t="s">
         <v>36</v>
       </c>
       <c r="C95" s="8" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="D95" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E95" s="28" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="F95" s="21" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="G95" s="22"/>
       <c r="H95" s="12"/>
@@ -3926,123 +3999,127 @@
       <c r="K95" s="12"/>
       <c r="L95" s="12"/>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A96" s="7">
-        <v>44</v>
+    <row r="96" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A96" s="18" t="s">
+        <v>237</v>
       </c>
       <c r="B96" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C96" s="8"/>
-      <c r="D96" s="29" t="s">
-        <v>123</v>
-      </c>
-      <c r="E96" s="30" t="s">
-        <v>228</v>
+      <c r="C96" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D96" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="E96" s="28" t="s">
+        <v>81</v>
       </c>
       <c r="F96" s="21" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="G96" s="22"/>
-      <c r="H96" s="19"/>
+      <c r="H96" s="12"/>
       <c r="I96" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="J96" s="19"/>
-      <c r="K96" s="19"/>
-      <c r="L96" s="19"/>
-    </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A97" s="7">
-        <v>45</v>
+      <c r="J96" s="12"/>
+      <c r="K96" s="12"/>
+      <c r="L96" s="12"/>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A97" s="18" t="s">
+        <v>238</v>
       </c>
       <c r="B97" s="8" t="s">
         <v>36</v>
       </c>
       <c r="C97" s="8"/>
-      <c r="D97" s="32" t="s">
-        <v>140</v>
-      </c>
-      <c r="E97" s="30" t="s">
-        <v>229</v>
+      <c r="D97" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="E97" s="28" t="s">
+        <v>70</v>
       </c>
       <c r="F97" s="21" t="s">
-        <v>28</v>
+        <v>97</v>
       </c>
       <c r="G97" s="22"/>
-      <c r="H97" s="19"/>
-      <c r="I97" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="J97" s="19"/>
-      <c r="K97" s="19"/>
-      <c r="L97" s="19"/>
-    </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A98" s="7">
-        <v>46</v>
+      <c r="H97" s="12"/>
+      <c r="I97" s="12"/>
+      <c r="J97" s="12"/>
+      <c r="K97" s="12"/>
+      <c r="L97" s="12"/>
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A98" s="18" t="s">
+        <v>239</v>
       </c>
       <c r="B98" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C98" s="8"/>
-      <c r="D98" s="31" t="s">
-        <v>151</v>
-      </c>
-      <c r="E98" s="30" t="s">
-        <v>230</v>
+      <c r="C98" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D98" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="E98" s="28" t="s">
+        <v>96</v>
       </c>
       <c r="F98" s="21" t="s">
         <v>28</v>
       </c>
       <c r="G98" s="22"/>
-      <c r="H98" s="19"/>
+      <c r="H98" s="12"/>
       <c r="I98" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="J98" s="19"/>
-      <c r="K98" s="19"/>
-      <c r="L98" s="19"/>
-    </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A99" s="7">
-        <v>47</v>
+      <c r="J98" s="12"/>
+      <c r="K98" s="12"/>
+      <c r="L98" s="12"/>
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A99" s="18" t="s">
+        <v>240</v>
       </c>
       <c r="B99" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C99" s="8"/>
-      <c r="D99" s="31" t="s">
-        <v>162</v>
-      </c>
-      <c r="E99" s="30" t="s">
-        <v>231</v>
+      <c r="C99" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D99" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="E99" s="28" t="s">
+        <v>82</v>
       </c>
       <c r="F99" s="21" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="G99" s="22"/>
-      <c r="H99" s="19"/>
+      <c r="H99" s="12"/>
       <c r="I99" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="J99" s="19"/>
-      <c r="K99" s="19"/>
-      <c r="L99" s="19"/>
-    </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J99" s="12"/>
+      <c r="K99" s="12"/>
+      <c r="L99" s="12"/>
+    </row>
+    <row r="100" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A100" s="7">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B100" s="8" t="s">
         <v>36</v>
       </c>
       <c r="C100" s="8"/>
-      <c r="D100" s="31" t="s">
-        <v>173</v>
+      <c r="D100" s="29" t="s">
+        <v>101</v>
       </c>
       <c r="E100" s="30" t="s">
-        <v>232</v>
+        <v>190</v>
       </c>
       <c r="F100" s="21" t="s">
         <v>28</v>
@@ -4056,19 +4133,19 @@
       <c r="K100" s="19"/>
       <c r="L100" s="19"/>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A101" s="7">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B101" s="8" t="s">
         <v>36</v>
       </c>
       <c r="C101" s="8"/>
-      <c r="D101" s="31" t="s">
-        <v>184</v>
+      <c r="D101" s="32" t="s">
+        <v>112</v>
       </c>
       <c r="E101" s="30" t="s">
-        <v>233</v>
+        <v>191</v>
       </c>
       <c r="F101" s="21" t="s">
         <v>28</v>
@@ -4082,43 +4159,45 @@
       <c r="K101" s="19"/>
       <c r="L101" s="19"/>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A102" s="7">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B102" s="8" t="s">
         <v>36</v>
       </c>
       <c r="C102" s="8"/>
-      <c r="D102" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="E102" s="28" t="s">
-        <v>91</v>
+      <c r="D102" s="31" t="s">
+        <v>121</v>
+      </c>
+      <c r="E102" s="30" t="s">
+        <v>192</v>
       </c>
       <c r="F102" s="21" t="s">
-        <v>120</v>
+        <v>28</v>
       </c>
       <c r="G102" s="22"/>
       <c r="H102" s="19"/>
-      <c r="I102" s="19"/>
+      <c r="I102" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="J102" s="19"/>
       <c r="K102" s="19"/>
       <c r="L102" s="19"/>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A103" s="7">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B103" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C103" s="16"/>
-      <c r="D103" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="E103" s="28" t="s">
-        <v>93</v>
+      <c r="C103" s="8"/>
+      <c r="D103" s="31" t="s">
+        <v>132</v>
+      </c>
+      <c r="E103" s="30" t="s">
+        <v>193</v>
       </c>
       <c r="F103" s="21" t="s">
         <v>28</v>
@@ -4132,19 +4211,19 @@
       <c r="K103" s="19"/>
       <c r="L103" s="19"/>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A104" s="7">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B104" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C104" s="16"/>
-      <c r="D104" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="E104" s="28" t="s">
-        <v>94</v>
+      <c r="C104" s="8"/>
+      <c r="D104" s="31" t="s">
+        <v>143</v>
+      </c>
+      <c r="E104" s="30" t="s">
+        <v>194</v>
       </c>
       <c r="F104" s="21" t="s">
         <v>28</v>
@@ -4158,8 +4237,110 @@
       <c r="K104" s="19"/>
       <c r="L104" s="19"/>
     </row>
+    <row r="105" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A105" s="7">
+        <v>52</v>
+      </c>
+      <c r="B105" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C105" s="8"/>
+      <c r="D105" s="31" t="s">
+        <v>154</v>
+      </c>
+      <c r="E105" s="30" t="s">
+        <v>195</v>
+      </c>
+      <c r="F105" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G105" s="22"/>
+      <c r="H105" s="19"/>
+      <c r="I105" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="J105" s="19"/>
+      <c r="K105" s="19"/>
+      <c r="L105" s="19"/>
+    </row>
+    <row r="106" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A106" s="7">
+        <v>53</v>
+      </c>
+      <c r="B106" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C106" s="8"/>
+      <c r="D106" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="E106" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="F106" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="G106" s="22"/>
+      <c r="H106" s="19"/>
+      <c r="I106" s="19"/>
+      <c r="J106" s="19"/>
+      <c r="K106" s="19"/>
+      <c r="L106" s="19"/>
+    </row>
+    <row r="107" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A107" s="7">
+        <v>54</v>
+      </c>
+      <c r="B107" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C107" s="16"/>
+      <c r="D107" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="E107" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="F107" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G107" s="22"/>
+      <c r="H107" s="19"/>
+      <c r="I107" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="J107" s="19"/>
+      <c r="K107" s="19"/>
+      <c r="L107" s="19"/>
+    </row>
+    <row r="108" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A108" s="7">
+        <v>55</v>
+      </c>
+      <c r="B108" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C108" s="16"/>
+      <c r="D108" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="E108" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="F108" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G108" s="22"/>
+      <c r="H108" s="19"/>
+      <c r="I108" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="J108" s="19"/>
+      <c r="K108" s="19"/>
+      <c r="L108" s="19"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:L104" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:L108" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
WIP Non-Financials to Lego
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/euTaxonomyNonFinancials/EutaxonomyNonFinancials.xlsx
+++ b/dataland-framework-toolbox/inputs/euTaxonomyNonFinancials/EutaxonomyNonFinancials.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dataland\Dataland\dataland-framework-toolbox\inputs\euTaxonomyNonFinancials\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d93401\Projects\Dataland\dataland-framework-toolbox\inputs\euTaxonomyNonFinancials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C67B78E9-299A-43AD-B2BD-B46716BA59B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D016372D-DEB1-4F57-AAF6-9FAB0981C7AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Framework Data Model" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="246">
   <si>
     <t>Field Identifier</t>
   </si>
@@ -117,9 +117,6 @@
     <t>Fiscal Year End</t>
   </si>
   <si>
-    <t>The date at which the fiscal year ends.</t>
-  </si>
-  <si>
     <t>Scope Of Entities</t>
   </si>
   <si>
@@ -156,9 +153,6 @@
     <t>Assurance</t>
   </si>
   <si>
-    <t>Level of assurance of the EU Taxonomy disclosure (Reasonable Assurance, Limited Assurance, None)</t>
-  </si>
-  <si>
     <t>Revenue</t>
   </si>
   <si>
@@ -669,9 +663,6 @@
     <t>Existence of due diligence processes to identify, prevent, mitigate and address adverse human rights impacts.</t>
   </si>
   <si>
-    <t>Existence of a policy to monitor compliance with the UNGC principles.</t>
-  </si>
-  <si>
     <t>12.1</t>
   </si>
   <si>
@@ -784,6 +775,27 @@
   </si>
   <si>
     <t>28.2</t>
+  </si>
+  <si>
+    <t>The date the fiscal year ends.</t>
+  </si>
+  <si>
+    <t>Level of Assurance of the EU Taxonomy Disclosure (Reasonable Assurance, Limited Assurance, None)</t>
+  </si>
+  <si>
+    <t>Include Category in Type Name</t>
+  </si>
+  <si>
+    <t>Include Sub-Category in Type Name</t>
+  </si>
+  <si>
+    <t>Data Point Type Name Overwrite</t>
+  </si>
+  <si>
+    <t>Number of Employees</t>
+  </si>
+  <si>
+    <t>Existence of a policy to monitor compliance with the UNGC principles or OECD Guidelines for Multinational Enterprises. See Regulation (EU) 2022/1288, Annex I, top (22) and table 1, indicator nr. 11.</t>
   </si>
 </sst>
 </file>
@@ -1465,23 +1477,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L108"/>
+  <dimension ref="A1:O108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A56" sqref="A56"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="20.26953125" customWidth="1"/>
-    <col min="4" max="4" width="95.1796875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="77.81640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="44.7265625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="26.26953125" customWidth="1"/>
-    <col min="8" max="12" width="14.26953125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" customWidth="1"/>
+    <col min="4" max="4" width="95.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="77.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="44.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="26.28515625" customWidth="1"/>
+    <col min="8" max="14" width="14.28515625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1518,8 +1531,17 @@
       <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M1" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
         <v>0</v>
       </c>
@@ -1537,17 +1559,20 @@
         <v>17</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H2" s="11"/>
       <c r="I2" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J2" s="12"/>
       <c r="K2" s="12"/>
       <c r="L2" s="12"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M2" s="12"/>
+      <c r="N2" s="12"/>
+      <c r="O2" s="12"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
       <c r="B3" s="8" t="s">
         <v>12</v>
@@ -1557,7 +1582,7 @@
         <v>18</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>19</v>
+        <v>239</v>
       </c>
       <c r="F3" s="10" t="s">
         <v>13</v>
@@ -1565,13 +1590,16 @@
       <c r="G3" s="10"/>
       <c r="H3" s="11"/>
       <c r="I3" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J3" s="12"/>
       <c r="K3" s="12"/>
       <c r="L3" s="12"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M3" s="12"/>
+      <c r="N3" s="12"/>
+      <c r="O3" s="12"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>1</v>
       </c>
@@ -1580,26 +1608,29 @@
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="19" t="s">
+      <c r="F4" s="10" t="s">
         <v>21</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>22</v>
       </c>
       <c r="G4" s="10" t="s">
         <v>14</v>
       </c>
       <c r="H4" s="12"/>
       <c r="I4" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J4" s="11"/>
       <c r="K4" s="11"/>
       <c r="L4" s="12"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M4" s="12"/>
+      <c r="N4" s="12"/>
+      <c r="O4" s="12"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>2</v>
       </c>
@@ -1608,26 +1639,29 @@
       </c>
       <c r="C5" s="8"/>
       <c r="D5" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="12" t="s">
-        <v>30</v>
-      </c>
       <c r="F5" s="20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G5" s="23" t="s">
         <v>14</v>
       </c>
       <c r="H5" s="12"/>
       <c r="I5" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J5" s="12"/>
       <c r="K5" s="12"/>
       <c r="L5" s="12"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M5" s="12"/>
+      <c r="N5" s="12"/>
+      <c r="O5" s="12"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>3</v>
       </c>
@@ -1636,26 +1670,29 @@
       </c>
       <c r="C6" s="8"/>
       <c r="D6" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="19" t="s">
+      <c r="F6" s="20" t="s">
         <v>24</v>
-      </c>
-      <c r="F6" s="20" t="s">
-        <v>25</v>
       </c>
       <c r="G6" s="26" t="s">
         <v>14</v>
       </c>
       <c r="H6" s="12"/>
       <c r="I6" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J6" s="12"/>
       <c r="K6" s="12"/>
       <c r="L6" s="12"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M6" s="12"/>
+      <c r="N6" s="12"/>
+      <c r="O6" s="12"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>4</v>
       </c>
@@ -1664,13 +1701,13 @@
       </c>
       <c r="C7" s="8"/>
       <c r="D7" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>32</v>
+        <v>240</v>
       </c>
       <c r="F7" s="27" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G7" s="26" t="s">
         <v>14</v>
@@ -1680,8 +1717,11 @@
       <c r="J7" s="12"/>
       <c r="K7" s="12"/>
       <c r="L7" s="12"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M7" s="12"/>
+      <c r="N7" s="12"/>
+      <c r="O7" s="12"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>5</v>
       </c>
@@ -1690,24 +1730,29 @@
       </c>
       <c r="C8" s="8"/>
       <c r="D8" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="12" t="s">
-        <v>27</v>
-      </c>
       <c r="F8" s="20" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G8" s="22"/>
       <c r="H8" s="12"/>
       <c r="I8" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J8" s="12"/>
       <c r="K8" s="12"/>
       <c r="L8" s="12"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M8" s="12"/>
+      <c r="N8" s="12"/>
+      <c r="O8" s="12" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>6</v>
       </c>
@@ -1716,24 +1761,27 @@
       </c>
       <c r="C9" s="8"/>
       <c r="D9" s="38" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E9" s="34" t="s">
-        <v>203</v>
+        <v>245</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G9" s="22"/>
       <c r="H9" s="12"/>
       <c r="I9" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J9" s="12"/>
       <c r="K9" s="12"/>
       <c r="L9" s="12"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M9" s="12"/>
+      <c r="N9" s="12"/>
+      <c r="O9" s="12"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>7</v>
       </c>
@@ -1742,24 +1790,27 @@
       </c>
       <c r="C10" s="8"/>
       <c r="D10" s="33" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E10" s="35" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="F10" s="20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G10" s="22"/>
       <c r="H10" s="12"/>
       <c r="I10" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J10" s="12"/>
       <c r="K10" s="12"/>
       <c r="L10" s="12"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M10" s="12"/>
+      <c r="N10" s="12"/>
+      <c r="O10" s="12"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>8</v>
       </c>
@@ -1768,24 +1819,27 @@
       </c>
       <c r="C11" s="8"/>
       <c r="D11" s="38" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E11" s="36" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="F11" s="20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G11" s="22"/>
       <c r="H11" s="12"/>
       <c r="I11" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J11" s="12"/>
       <c r="K11" s="12"/>
       <c r="L11" s="12"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M11" s="12"/>
+      <c r="N11" s="12"/>
+      <c r="O11" s="12"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>9</v>
       </c>
@@ -1794,24 +1848,27 @@
       </c>
       <c r="C12" s="8"/>
       <c r="D12" s="38" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E12" s="35" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="F12" s="20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G12" s="22"/>
       <c r="H12" s="12"/>
       <c r="I12" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J12" s="12"/>
       <c r="K12" s="12"/>
       <c r="L12" s="12"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M12" s="12"/>
+      <c r="N12" s="12"/>
+      <c r="O12" s="12"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>10</v>
       </c>
@@ -1820,11 +1877,11 @@
       </c>
       <c r="C13" s="8"/>
       <c r="D13" s="14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E13" s="12"/>
       <c r="F13" s="20" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G13" s="23" t="s">
         <v>14</v>
@@ -1834,215 +1891,239 @@
       <c r="J13" s="12"/>
       <c r="K13" s="12"/>
       <c r="L13" s="12"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M13" s="12"/>
+      <c r="N13" s="12"/>
+      <c r="O13" s="12"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>11</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C14" s="8"/>
       <c r="D14" s="15" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E14" s="19" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F14" s="21" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G14" s="22"/>
       <c r="H14" s="12"/>
       <c r="I14" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J14" s="12"/>
       <c r="K14" s="12"/>
       <c r="L14" s="12"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M14" s="12"/>
+      <c r="N14" s="12"/>
+      <c r="O14" s="12"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E15" s="19"/>
       <c r="F15" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G15" s="22"/>
       <c r="H15" s="12"/>
       <c r="I15" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J15" s="12"/>
       <c r="K15" s="12"/>
       <c r="L15" s="12"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M15" s="12"/>
+      <c r="N15" s="12"/>
+      <c r="O15" s="12"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C16" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="D16" s="15" t="s">
-        <v>41</v>
-      </c>
       <c r="E16" s="28" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F16" s="21" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G16" s="22"/>
       <c r="H16" s="12"/>
       <c r="I16" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J16" s="12"/>
       <c r="K16" s="12"/>
       <c r="L16" s="12"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M16" s="12"/>
+      <c r="N16" s="12"/>
+      <c r="O16" s="12"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F17" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G17" s="22"/>
       <c r="H17" s="12"/>
       <c r="I17" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J17" s="12"/>
       <c r="K17" s="12"/>
       <c r="L17" s="12"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M17" s="12"/>
+      <c r="N17" s="12"/>
+      <c r="O17" s="12"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F18" s="21" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G18" s="22"/>
       <c r="H18" s="12"/>
       <c r="I18" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J18" s="12"/>
       <c r="K18" s="12"/>
       <c r="L18" s="12"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M18" s="12"/>
+      <c r="N18" s="12"/>
+      <c r="O18" s="12"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="18" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E19" s="28" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F19" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G19" s="22"/>
       <c r="H19" s="12"/>
       <c r="I19" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J19" s="12"/>
       <c r="K19" s="12"/>
       <c r="L19" s="12"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M19" s="12"/>
+      <c r="N19" s="12"/>
+      <c r="O19" s="12"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E20" s="28" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F20" s="21" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G20" s="22"/>
       <c r="H20" s="12"/>
       <c r="I20" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J20" s="12"/>
       <c r="K20" s="12"/>
       <c r="L20" s="12"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M20" s="12"/>
+      <c r="N20" s="12"/>
+      <c r="O20" s="12"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="18" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C21" s="8"/>
       <c r="D21" s="15" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E21" s="28" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F21" s="21" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G21" s="22"/>
       <c r="H21" s="12"/>
@@ -2050,729 +2131,813 @@
       <c r="J21" s="12"/>
       <c r="K21" s="12"/>
       <c r="L21" s="12"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M21" s="12"/>
+      <c r="N21" s="12"/>
+      <c r="O21" s="12"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F22" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G22" s="22"/>
       <c r="H22" s="12"/>
       <c r="I22" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J22" s="12"/>
       <c r="K22" s="12"/>
       <c r="L22" s="12"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M22" s="12"/>
+      <c r="N22" s="12"/>
+      <c r="O22" s="12"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="18" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F23" s="21" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G23" s="22"/>
       <c r="H23" s="12"/>
       <c r="I23" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J23" s="12"/>
       <c r="K23" s="12"/>
       <c r="L23" s="12"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M23" s="12"/>
+      <c r="N23" s="12"/>
+      <c r="O23" s="12"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
         <v>17</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C24" s="8"/>
       <c r="D24" s="29" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E24" s="30" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F24" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G24" s="22"/>
       <c r="H24" s="12"/>
       <c r="I24" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J24" s="12"/>
       <c r="K24" s="12"/>
       <c r="L24" s="12"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M24" s="12"/>
+      <c r="N24" s="12"/>
+      <c r="O24" s="12"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="18" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C25" s="8"/>
       <c r="D25" s="29" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E25" s="30" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F25" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G25" s="22"/>
       <c r="H25" s="12"/>
       <c r="I25" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J25" s="12"/>
       <c r="K25" s="12"/>
       <c r="L25" s="12"/>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M25" s="12"/>
+      <c r="N25" s="12"/>
+      <c r="O25" s="12"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="18" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C26" s="8"/>
       <c r="D26" s="31" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E26" s="30" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F26" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G26" s="22"/>
       <c r="H26" s="12"/>
       <c r="I26" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J26" s="12"/>
       <c r="K26" s="12"/>
       <c r="L26" s="12"/>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M26" s="12"/>
+      <c r="N26" s="12"/>
+      <c r="O26" s="12"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="18" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C27" s="8"/>
       <c r="D27" s="29" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E27" s="30" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F27" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G27" s="22"/>
       <c r="H27" s="12"/>
       <c r="I27" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J27" s="12"/>
       <c r="K27" s="12"/>
       <c r="L27" s="12"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M27" s="12"/>
+      <c r="N27" s="12"/>
+      <c r="O27" s="12"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="18" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C28" s="8"/>
       <c r="D28" s="29" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E28" s="30" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F28" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G28" s="22"/>
       <c r="H28" s="12"/>
       <c r="I28" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J28" s="12"/>
       <c r="K28" s="12"/>
       <c r="L28" s="12"/>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M28" s="12"/>
+      <c r="N28" s="12"/>
+      <c r="O28" s="12"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="7">
         <v>18</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C29" s="8"/>
       <c r="D29" s="32" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E29" s="30" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F29" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G29" s="22"/>
       <c r="H29" s="12"/>
       <c r="I29" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J29" s="12"/>
       <c r="K29" s="12"/>
       <c r="L29" s="12"/>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M29" s="12"/>
+      <c r="N29" s="12"/>
+      <c r="O29" s="12"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="18" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C30" s="8"/>
       <c r="D30" s="32" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E30" s="30" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F30" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G30" s="22"/>
       <c r="H30" s="12"/>
       <c r="I30" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J30" s="12"/>
       <c r="K30" s="12"/>
       <c r="L30" s="12"/>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M30" s="12"/>
+      <c r="N30" s="12"/>
+      <c r="O30" s="12"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="18" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C31" s="8"/>
       <c r="D31" s="31" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E31" s="30" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F31" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G31" s="22"/>
       <c r="H31" s="12"/>
       <c r="I31" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J31" s="12"/>
       <c r="K31" s="12"/>
       <c r="L31" s="12"/>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M31" s="12"/>
+      <c r="N31" s="12"/>
+      <c r="O31" s="12"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="18" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C32" s="8"/>
       <c r="D32" s="31" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E32" s="30" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F32" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G32" s="22"/>
       <c r="H32" s="12"/>
       <c r="I32" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J32" s="12"/>
       <c r="K32" s="12"/>
       <c r="L32" s="12"/>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M32" s="12"/>
+      <c r="N32" s="12"/>
+      <c r="O32" s="12"/>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="7">
         <v>19</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C33" s="8"/>
       <c r="D33" s="31" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E33" s="30" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F33" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G33" s="22"/>
       <c r="H33" s="12"/>
       <c r="I33" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J33" s="12"/>
       <c r="K33" s="12"/>
       <c r="L33" s="12"/>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M33" s="12"/>
+      <c r="N33" s="12"/>
+      <c r="O33" s="12"/>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="18" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C34" s="8"/>
       <c r="D34" s="31" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E34" s="30" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F34" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G34" s="22"/>
       <c r="H34" s="12"/>
       <c r="I34" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J34" s="12"/>
       <c r="K34" s="12"/>
       <c r="L34" s="12"/>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M34" s="12"/>
+      <c r="N34" s="12"/>
+      <c r="O34" s="12"/>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="18" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C35" s="8"/>
       <c r="D35" s="31" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E35" s="30" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F35" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G35" s="22"/>
       <c r="H35" s="12"/>
       <c r="I35" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J35" s="12"/>
       <c r="K35" s="12"/>
       <c r="L35" s="12"/>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M35" s="12"/>
+      <c r="N35" s="12"/>
+      <c r="O35" s="12"/>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" s="18" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C36" s="8"/>
       <c r="D36" s="31" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E36" s="30" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F36" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G36" s="22"/>
       <c r="H36" s="12"/>
       <c r="I36" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J36" s="12"/>
       <c r="K36" s="12"/>
       <c r="L36" s="12"/>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M36" s="12"/>
+      <c r="N36" s="12"/>
+      <c r="O36" s="12"/>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="7">
         <v>20</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C37" s="8"/>
       <c r="D37" s="31" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E37" s="30" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F37" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G37" s="22"/>
       <c r="H37" s="12"/>
       <c r="I37" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J37" s="12"/>
       <c r="K37" s="12"/>
       <c r="L37" s="12"/>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M37" s="12"/>
+      <c r="N37" s="12"/>
+      <c r="O37" s="12"/>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" s="18" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C38" s="8"/>
       <c r="D38" s="31" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E38" s="30" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F38" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G38" s="22"/>
       <c r="H38" s="12"/>
       <c r="I38" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J38" s="12"/>
       <c r="K38" s="12"/>
       <c r="L38" s="12"/>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M38" s="12"/>
+      <c r="N38" s="12"/>
+      <c r="O38" s="12"/>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" s="18" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C39" s="8"/>
       <c r="D39" s="31" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E39" s="30" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F39" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G39" s="22"/>
       <c r="H39" s="12"/>
       <c r="I39" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J39" s="12"/>
       <c r="K39" s="12"/>
       <c r="L39" s="12"/>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M39" s="12"/>
+      <c r="N39" s="12"/>
+      <c r="O39" s="12"/>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" s="18" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C40" s="8"/>
       <c r="D40" s="31" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E40" s="30" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F40" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G40" s="22"/>
       <c r="H40" s="12"/>
       <c r="I40" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J40" s="12"/>
       <c r="K40" s="12"/>
       <c r="L40" s="12"/>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M40" s="12"/>
+      <c r="N40" s="12"/>
+      <c r="O40" s="12"/>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" s="7">
         <v>21</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C41" s="8"/>
       <c r="D41" s="31" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E41" s="30" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F41" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G41" s="22"/>
       <c r="H41" s="12"/>
       <c r="I41" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J41" s="12"/>
       <c r="K41" s="12"/>
       <c r="L41" s="12"/>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M41" s="12"/>
+      <c r="N41" s="12"/>
+      <c r="O41" s="12"/>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" s="18" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C42" s="8"/>
       <c r="D42" s="31" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E42" s="30" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F42" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G42" s="22"/>
       <c r="H42" s="12"/>
       <c r="I42" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J42" s="12"/>
       <c r="K42" s="12"/>
       <c r="L42" s="12"/>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M42" s="12"/>
+      <c r="N42" s="12"/>
+      <c r="O42" s="12"/>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" s="18" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C43" s="8"/>
       <c r="D43" s="31" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E43" s="30" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F43" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G43" s="22"/>
       <c r="H43" s="12"/>
       <c r="I43" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J43" s="12"/>
       <c r="K43" s="12"/>
       <c r="L43" s="12"/>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M43" s="12"/>
+      <c r="N43" s="12"/>
+      <c r="O43" s="12"/>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" s="18" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C44" s="8"/>
       <c r="D44" s="31" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E44" s="30" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F44" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G44" s="22"/>
       <c r="H44" s="12"/>
       <c r="I44" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J44" s="12"/>
       <c r="K44" s="12"/>
       <c r="L44" s="12"/>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M44" s="12"/>
+      <c r="N44" s="12"/>
+      <c r="O44" s="12"/>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" s="7">
         <v>22</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C45" s="8"/>
       <c r="D45" s="31" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E45" s="30" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F45" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G45" s="22"/>
       <c r="H45" s="12"/>
       <c r="I45" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J45" s="12"/>
       <c r="K45" s="12"/>
       <c r="L45" s="12"/>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M45" s="12"/>
+      <c r="N45" s="12"/>
+      <c r="O45" s="12"/>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" s="18" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C46" s="8"/>
       <c r="D46" s="31" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E46" s="30" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F46" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G46" s="22"/>
       <c r="H46" s="12"/>
       <c r="I46" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J46" s="12"/>
       <c r="K46" s="12"/>
       <c r="L46" s="12"/>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M46" s="12"/>
+      <c r="N46" s="12"/>
+      <c r="O46" s="12"/>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" s="18" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C47" s="8"/>
       <c r="D47" s="31" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E47" s="30" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F47" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G47" s="22"/>
       <c r="H47" s="12"/>
       <c r="I47" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J47" s="12"/>
       <c r="K47" s="12"/>
       <c r="L47" s="12"/>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M47" s="12"/>
+      <c r="N47" s="12"/>
+      <c r="O47" s="12"/>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" s="18" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C48" s="8"/>
       <c r="D48" s="31" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E48" s="30" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F48" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G48" s="22"/>
       <c r="H48" s="12"/>
       <c r="I48" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J48" s="12"/>
       <c r="K48" s="12"/>
       <c r="L48" s="12"/>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M48" s="12"/>
+      <c r="N48" s="12"/>
+      <c r="O48" s="12"/>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
         <v>23</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C49" s="8"/>
       <c r="D49" s="15" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E49" s="28" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F49" s="21" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G49" s="22"/>
       <c r="H49" s="12"/>
@@ -2780,269 +2945,299 @@
       <c r="J49" s="12"/>
       <c r="K49" s="12"/>
       <c r="L49" s="12"/>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M49" s="12"/>
+      <c r="N49" s="12"/>
+      <c r="O49" s="12"/>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" s="7">
         <v>24</v>
       </c>
       <c r="B50" s="16" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C50" s="16"/>
       <c r="D50" s="17" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E50" s="28" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F50" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G50" s="22"/>
       <c r="H50" s="12"/>
       <c r="I50" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J50" s="12"/>
       <c r="K50" s="12"/>
       <c r="L50" s="12"/>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M50" s="12"/>
+      <c r="N50" s="12"/>
+      <c r="O50" s="12"/>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" s="7">
         <v>25</v>
       </c>
       <c r="B51" s="16" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C51" s="16"/>
       <c r="D51" s="17" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E51" s="28" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F51" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G51" s="22"/>
       <c r="H51" s="12"/>
       <c r="I51" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J51" s="12"/>
       <c r="K51" s="12"/>
       <c r="L51" s="12"/>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M51" s="12"/>
+      <c r="N51" s="12"/>
+      <c r="O51" s="12"/>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" s="7">
         <v>26</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C52" s="8"/>
       <c r="D52" s="15" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E52" s="28" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F52" s="21" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G52" s="22"/>
       <c r="H52" s="12"/>
       <c r="I52" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J52" s="12"/>
       <c r="K52" s="12"/>
       <c r="L52" s="12"/>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M52" s="12"/>
+      <c r="N52" s="12"/>
+      <c r="O52" s="12"/>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" s="18" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D53" s="15" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E53" s="28" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F53" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G53" s="22"/>
       <c r="H53" s="12"/>
       <c r="I53" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J53" s="12"/>
       <c r="K53" s="12"/>
       <c r="L53" s="12"/>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M53" s="12"/>
+      <c r="N53" s="12"/>
+      <c r="O53" s="12"/>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" s="18" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B54" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C54" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D54" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="E54" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="F54" s="21" t="s">
         <v>35</v>
-      </c>
-      <c r="C54" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D54" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="E54" s="28" t="s">
-        <v>78</v>
-      </c>
-      <c r="F54" s="21" t="s">
-        <v>37</v>
       </c>
       <c r="G54" s="22"/>
       <c r="H54" s="12"/>
       <c r="I54" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J54" s="12"/>
       <c r="K54" s="12"/>
       <c r="L54" s="12"/>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M54" s="12"/>
+      <c r="N54" s="12"/>
+      <c r="O54" s="12"/>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" s="18" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D55" s="15" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E55" s="28" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F55" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G55" s="22"/>
       <c r="H55" s="12"/>
       <c r="I55" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J55" s="12"/>
       <c r="K55" s="12"/>
       <c r="L55" s="12"/>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M55" s="12"/>
+      <c r="N55" s="12"/>
+      <c r="O55" s="12"/>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" s="18" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="B56" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C56" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D56" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="E56" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="F56" s="21" t="s">
         <v>35</v>
-      </c>
-      <c r="C56" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="D56" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="E56" s="28" t="s">
-        <v>73</v>
-      </c>
-      <c r="F56" s="21" t="s">
-        <v>37</v>
       </c>
       <c r="G56" s="22"/>
       <c r="H56" s="12"/>
       <c r="I56" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J56" s="12"/>
       <c r="K56" s="12"/>
       <c r="L56" s="12"/>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M56" s="12"/>
+      <c r="N56" s="12"/>
+      <c r="O56" s="12"/>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" s="18" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D57" s="15" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E57" s="28" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F57" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G57" s="22"/>
       <c r="H57" s="12"/>
       <c r="I57" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J57" s="12"/>
       <c r="K57" s="12"/>
       <c r="L57" s="12"/>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M57" s="12"/>
+      <c r="N57" s="12"/>
+      <c r="O57" s="12"/>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" s="18" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B58" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C58" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D58" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="E58" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="F58" s="21" t="s">
         <v>35</v>
-      </c>
-      <c r="C58" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="D58" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="E58" s="28" t="s">
-        <v>77</v>
-      </c>
-      <c r="F58" s="21" t="s">
-        <v>37</v>
       </c>
       <c r="G58" s="22"/>
       <c r="H58" s="12"/>
       <c r="I58" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J58" s="12"/>
       <c r="K58" s="12"/>
       <c r="L58" s="12"/>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M58" s="12"/>
+      <c r="N58" s="12"/>
+      <c r="O58" s="12"/>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59" s="18" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C59" s="8"/>
       <c r="D59" s="15" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E59" s="28" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F59" s="21" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G59" s="22"/>
       <c r="H59" s="12"/>
@@ -3050,729 +3245,813 @@
       <c r="J59" s="12"/>
       <c r="K59" s="12"/>
       <c r="L59" s="12"/>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M59" s="12"/>
+      <c r="N59" s="12"/>
+      <c r="O59" s="12"/>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60" s="18" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D60" s="15" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E60" s="28" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F60" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G60" s="22"/>
       <c r="H60" s="12"/>
       <c r="I60" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J60" s="12"/>
       <c r="K60" s="12"/>
       <c r="L60" s="12"/>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M60" s="12"/>
+      <c r="N60" s="12"/>
+      <c r="O60" s="12"/>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61" s="18" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B61" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C61" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D61" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="E61" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="F61" s="21" t="s">
         <v>35</v>
-      </c>
-      <c r="C61" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="D61" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="E61" s="28" t="s">
-        <v>74</v>
-      </c>
-      <c r="F61" s="21" t="s">
-        <v>37</v>
       </c>
       <c r="G61" s="22"/>
       <c r="H61" s="12"/>
       <c r="I61" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J61" s="12"/>
       <c r="K61" s="12"/>
       <c r="L61" s="12"/>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M61" s="12"/>
+      <c r="N61" s="12"/>
+      <c r="O61" s="12"/>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A62" s="7">
         <v>32</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C62" s="8"/>
       <c r="D62" s="29" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E62" s="30" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F62" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G62" s="22"/>
       <c r="H62" s="12"/>
       <c r="I62" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J62" s="12"/>
       <c r="K62" s="12"/>
       <c r="L62" s="12"/>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M62" s="12"/>
+      <c r="N62" s="12"/>
+      <c r="O62" s="12"/>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A63" s="18" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C63" s="8"/>
       <c r="D63" s="29" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E63" s="30" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F63" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G63" s="22"/>
       <c r="H63" s="12"/>
       <c r="I63" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J63" s="12"/>
       <c r="K63" s="12"/>
       <c r="L63" s="12"/>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M63" s="12"/>
+      <c r="N63" s="12"/>
+      <c r="O63" s="12"/>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A64" s="18" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B64" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C64" s="8"/>
       <c r="D64" s="31" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E64" s="30" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F64" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G64" s="22"/>
       <c r="H64" s="12"/>
       <c r="I64" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J64" s="12"/>
       <c r="K64" s="12"/>
       <c r="L64" s="12"/>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M64" s="12"/>
+      <c r="N64" s="12"/>
+      <c r="O64" s="12"/>
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A65" s="18" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C65" s="8"/>
       <c r="D65" s="29" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E65" s="30" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F65" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G65" s="22"/>
       <c r="H65" s="12"/>
       <c r="I65" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J65" s="12"/>
       <c r="K65" s="12"/>
       <c r="L65" s="12"/>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M65" s="12"/>
+      <c r="N65" s="12"/>
+      <c r="O65" s="12"/>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A66" s="18" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B66" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C66" s="8"/>
       <c r="D66" s="29" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E66" s="30" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F66" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G66" s="22"/>
       <c r="H66" s="12"/>
       <c r="I66" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J66" s="12"/>
       <c r="K66" s="12"/>
       <c r="L66" s="12"/>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M66" s="12"/>
+      <c r="N66" s="12"/>
+      <c r="O66" s="12"/>
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A67" s="7">
         <v>33</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C67" s="8"/>
       <c r="D67" s="32" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E67" s="30" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F67" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G67" s="22"/>
       <c r="H67" s="12"/>
       <c r="I67" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J67" s="12"/>
       <c r="K67" s="12"/>
       <c r="L67" s="12"/>
-    </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M67" s="12"/>
+      <c r="N67" s="12"/>
+      <c r="O67" s="12"/>
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A68" s="18" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B68" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C68" s="8"/>
       <c r="D68" s="32" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E68" s="30" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F68" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G68" s="22"/>
       <c r="H68" s="12"/>
       <c r="I68" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J68" s="12"/>
       <c r="K68" s="12"/>
       <c r="L68" s="12"/>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M68" s="12"/>
+      <c r="N68" s="12"/>
+      <c r="O68" s="12"/>
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A69" s="18" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C69" s="8"/>
       <c r="D69" s="31" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E69" s="30" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F69" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G69" s="22"/>
       <c r="H69" s="12"/>
       <c r="I69" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J69" s="12"/>
       <c r="K69" s="12"/>
       <c r="L69" s="12"/>
-    </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M69" s="12"/>
+      <c r="N69" s="12"/>
+      <c r="O69" s="12"/>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A70" s="18" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B70" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C70" s="8"/>
       <c r="D70" s="31" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E70" s="30" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F70" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G70" s="22"/>
       <c r="H70" s="12"/>
       <c r="I70" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J70" s="12"/>
       <c r="K70" s="12"/>
       <c r="L70" s="12"/>
-    </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M70" s="12"/>
+      <c r="N70" s="12"/>
+      <c r="O70" s="12"/>
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A71" s="7">
         <v>34</v>
       </c>
       <c r="B71" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C71" s="8"/>
       <c r="D71" s="31" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E71" s="30" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F71" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G71" s="22"/>
       <c r="H71" s="12"/>
       <c r="I71" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J71" s="12"/>
       <c r="K71" s="12"/>
       <c r="L71" s="12"/>
-    </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M71" s="12"/>
+      <c r="N71" s="12"/>
+      <c r="O71" s="12"/>
+    </row>
+    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A72" s="18" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B72" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C72" s="8"/>
       <c r="D72" s="31" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E72" s="30" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F72" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G72" s="22"/>
       <c r="H72" s="12"/>
       <c r="I72" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J72" s="12"/>
       <c r="K72" s="12"/>
       <c r="L72" s="12"/>
-    </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M72" s="12"/>
+      <c r="N72" s="12"/>
+      <c r="O72" s="12"/>
+    </row>
+    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A73" s="18" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B73" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C73" s="8"/>
       <c r="D73" s="31" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E73" s="30" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F73" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G73" s="22"/>
       <c r="H73" s="12"/>
       <c r="I73" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J73" s="12"/>
       <c r="K73" s="12"/>
       <c r="L73" s="12"/>
-    </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M73" s="12"/>
+      <c r="N73" s="12"/>
+      <c r="O73" s="12"/>
+    </row>
+    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A74" s="18" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B74" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C74" s="8"/>
       <c r="D74" s="31" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E74" s="30" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F74" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G74" s="22"/>
       <c r="H74" s="12"/>
       <c r="I74" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J74" s="12"/>
       <c r="K74" s="12"/>
       <c r="L74" s="12"/>
-    </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M74" s="12"/>
+      <c r="N74" s="12"/>
+      <c r="O74" s="12"/>
+    </row>
+    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A75" s="7">
         <v>35</v>
       </c>
       <c r="B75" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C75" s="8"/>
       <c r="D75" s="31" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E75" s="30" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F75" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G75" s="22"/>
       <c r="H75" s="12"/>
       <c r="I75" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J75" s="12"/>
       <c r="K75" s="12"/>
       <c r="L75" s="12"/>
-    </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M75" s="12"/>
+      <c r="N75" s="12"/>
+      <c r="O75" s="12"/>
+    </row>
+    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A76" s="18" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B76" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C76" s="8"/>
       <c r="D76" s="31" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E76" s="30" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F76" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G76" s="22"/>
       <c r="H76" s="12"/>
       <c r="I76" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J76" s="12"/>
       <c r="K76" s="12"/>
       <c r="L76" s="12"/>
-    </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M76" s="12"/>
+      <c r="N76" s="12"/>
+      <c r="O76" s="12"/>
+    </row>
+    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A77" s="18" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C77" s="8"/>
       <c r="D77" s="31" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E77" s="30" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F77" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G77" s="22"/>
       <c r="H77" s="12"/>
       <c r="I77" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J77" s="12"/>
       <c r="K77" s="12"/>
       <c r="L77" s="12"/>
-    </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M77" s="12"/>
+      <c r="N77" s="12"/>
+      <c r="O77" s="12"/>
+    </row>
+    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A78" s="18" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B78" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C78" s="8"/>
       <c r="D78" s="31" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E78" s="30" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F78" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G78" s="22"/>
       <c r="H78" s="12"/>
       <c r="I78" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J78" s="12"/>
       <c r="K78" s="12"/>
       <c r="L78" s="12"/>
-    </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M78" s="12"/>
+      <c r="N78" s="12"/>
+      <c r="O78" s="12"/>
+    </row>
+    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A79" s="7">
         <v>36</v>
       </c>
       <c r="B79" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C79" s="8"/>
       <c r="D79" s="31" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E79" s="30" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F79" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G79" s="22"/>
       <c r="H79" s="12"/>
       <c r="I79" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J79" s="12"/>
       <c r="K79" s="12"/>
       <c r="L79" s="12"/>
-    </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M79" s="12"/>
+      <c r="N79" s="12"/>
+      <c r="O79" s="12"/>
+    </row>
+    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A80" s="18" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B80" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C80" s="8"/>
       <c r="D80" s="31" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E80" s="30" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F80" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G80" s="22"/>
       <c r="H80" s="12"/>
       <c r="I80" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J80" s="12"/>
       <c r="K80" s="12"/>
       <c r="L80" s="12"/>
-    </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M80" s="12"/>
+      <c r="N80" s="12"/>
+      <c r="O80" s="12"/>
+    </row>
+    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A81" s="18" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B81" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C81" s="8"/>
       <c r="D81" s="31" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E81" s="30" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F81" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G81" s="22"/>
       <c r="H81" s="12"/>
       <c r="I81" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J81" s="12"/>
       <c r="K81" s="12"/>
       <c r="L81" s="12"/>
-    </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M81" s="12"/>
+      <c r="N81" s="12"/>
+      <c r="O81" s="12"/>
+    </row>
+    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A82" s="18" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B82" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C82" s="8"/>
       <c r="D82" s="31" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E82" s="30" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F82" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G82" s="22"/>
       <c r="H82" s="12"/>
       <c r="I82" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J82" s="12"/>
       <c r="K82" s="12"/>
       <c r="L82" s="12"/>
-    </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M82" s="12"/>
+      <c r="N82" s="12"/>
+      <c r="O82" s="12"/>
+    </row>
+    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A83" s="7">
         <v>37</v>
       </c>
       <c r="B83" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C83" s="8"/>
       <c r="D83" s="31" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E83" s="30" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F83" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G83" s="22"/>
       <c r="H83" s="12"/>
       <c r="I83" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J83" s="12"/>
       <c r="K83" s="12"/>
       <c r="L83" s="12"/>
-    </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M83" s="12"/>
+      <c r="N83" s="12"/>
+      <c r="O83" s="12"/>
+    </row>
+    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A84" s="18" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B84" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C84" s="8"/>
       <c r="D84" s="31" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E84" s="30" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F84" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G84" s="22"/>
       <c r="H84" s="12"/>
       <c r="I84" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J84" s="12"/>
       <c r="K84" s="12"/>
       <c r="L84" s="12"/>
-    </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M84" s="12"/>
+      <c r="N84" s="12"/>
+      <c r="O84" s="12"/>
+    </row>
+    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A85" s="18" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="B85" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C85" s="8"/>
       <c r="D85" s="31" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E85" s="30" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F85" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G85" s="22"/>
       <c r="H85" s="12"/>
       <c r="I85" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J85" s="12"/>
       <c r="K85" s="12"/>
       <c r="L85" s="12"/>
-    </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M85" s="12"/>
+      <c r="N85" s="12"/>
+      <c r="O85" s="12"/>
+    </row>
+    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A86" s="18" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B86" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C86" s="8"/>
       <c r="D86" s="31" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E86" s="30" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F86" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G86" s="22"/>
       <c r="H86" s="12"/>
       <c r="I86" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J86" s="12"/>
       <c r="K86" s="12"/>
       <c r="L86" s="12"/>
-    </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M86" s="12"/>
+      <c r="N86" s="12"/>
+      <c r="O86" s="12"/>
+    </row>
+    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A87" s="7">
         <v>38</v>
       </c>
       <c r="B87" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C87" s="8"/>
       <c r="D87" s="15" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E87" s="28" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F87" s="21" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G87" s="22"/>
       <c r="H87" s="12"/>
@@ -3780,269 +4059,299 @@
       <c r="J87" s="12"/>
       <c r="K87" s="12"/>
       <c r="L87" s="12"/>
-    </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M87" s="12"/>
+      <c r="N87" s="12"/>
+      <c r="O87" s="12"/>
+    </row>
+    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A88" s="7">
         <v>39</v>
       </c>
       <c r="B88" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C88" s="16"/>
       <c r="D88" s="17" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E88" s="28" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F88" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G88" s="22"/>
       <c r="H88" s="12"/>
       <c r="I88" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J88" s="12"/>
       <c r="K88" s="12"/>
       <c r="L88" s="12"/>
-    </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M88" s="12"/>
+      <c r="N88" s="12"/>
+      <c r="O88" s="12"/>
+    </row>
+    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A89" s="7">
         <v>40</v>
       </c>
       <c r="B89" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C89" s="16"/>
       <c r="D89" s="17" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E89" s="28" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F89" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G89" s="22"/>
       <c r="H89" s="12"/>
       <c r="I89" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J89" s="12"/>
       <c r="K89" s="12"/>
       <c r="L89" s="12"/>
-    </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M89" s="12"/>
+      <c r="N89" s="12"/>
+      <c r="O89" s="12"/>
+    </row>
+    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A90" s="7">
         <v>41</v>
       </c>
       <c r="B90" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C90" s="8"/>
       <c r="D90" s="15" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E90" s="28" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F90" s="21" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G90" s="22"/>
       <c r="H90" s="12"/>
       <c r="I90" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J90" s="12"/>
       <c r="K90" s="12"/>
       <c r="L90" s="12"/>
-    </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M90" s="12"/>
+      <c r="N90" s="12"/>
+      <c r="O90" s="12"/>
+    </row>
+    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A91" s="18" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B91" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C91" s="8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D91" s="15" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E91" s="28" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F91" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G91" s="22"/>
       <c r="H91" s="12"/>
       <c r="I91" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J91" s="12"/>
       <c r="K91" s="12"/>
       <c r="L91" s="12"/>
-    </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M91" s="12"/>
+      <c r="N91" s="12"/>
+      <c r="O91" s="12"/>
+    </row>
+    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A92" s="18" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="B92" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C92" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D92" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="D92" s="15" t="s">
-        <v>41</v>
-      </c>
       <c r="E92" s="28" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F92" s="21" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G92" s="22"/>
       <c r="H92" s="12"/>
       <c r="I92" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J92" s="12"/>
       <c r="K92" s="12"/>
       <c r="L92" s="12"/>
-    </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M92" s="12"/>
+      <c r="N92" s="12"/>
+      <c r="O92" s="12"/>
+    </row>
+    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A93" s="18" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B93" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C93" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D93" s="15" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E93" s="28" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F93" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G93" s="22"/>
       <c r="H93" s="12"/>
       <c r="I93" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J93" s="12"/>
       <c r="K93" s="12"/>
       <c r="L93" s="12"/>
-    </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M93" s="12"/>
+      <c r="N93" s="12"/>
+      <c r="O93" s="12"/>
+    </row>
+    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A94" s="18" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B94" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C94" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D94" s="15" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E94" s="28" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F94" s="21" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G94" s="22"/>
       <c r="H94" s="12"/>
       <c r="I94" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J94" s="12"/>
       <c r="K94" s="12"/>
       <c r="L94" s="12"/>
-    </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M94" s="12"/>
+      <c r="N94" s="12"/>
+      <c r="O94" s="12"/>
+    </row>
+    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A95" s="18" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="B95" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C95" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D95" s="15" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E95" s="28" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F95" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G95" s="22"/>
       <c r="H95" s="12"/>
       <c r="I95" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J95" s="12"/>
       <c r="K95" s="12"/>
       <c r="L95" s="12"/>
-    </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M95" s="12"/>
+      <c r="N95" s="12"/>
+      <c r="O95" s="12"/>
+    </row>
+    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A96" s="18" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="B96" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C96" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D96" s="15" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E96" s="28" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F96" s="21" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G96" s="22"/>
       <c r="H96" s="12"/>
       <c r="I96" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J96" s="12"/>
       <c r="K96" s="12"/>
       <c r="L96" s="12"/>
-    </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M96" s="12"/>
+      <c r="N96" s="12"/>
+      <c r="O96" s="12"/>
+    </row>
+    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A97" s="18" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="B97" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C97" s="8"/>
       <c r="D97" s="15" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E97" s="28" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F97" s="21" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G97" s="22"/>
       <c r="H97" s="12"/>
@@ -4050,235 +4359,262 @@
       <c r="J97" s="12"/>
       <c r="K97" s="12"/>
       <c r="L97" s="12"/>
-    </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M97" s="12"/>
+      <c r="N97" s="12"/>
+      <c r="O97" s="12"/>
+    </row>
+    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A98" s="18" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="B98" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C98" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D98" s="15" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E98" s="28" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F98" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G98" s="22"/>
       <c r="H98" s="12"/>
       <c r="I98" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J98" s="12"/>
       <c r="K98" s="12"/>
       <c r="L98" s="12"/>
-    </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M98" s="12"/>
+      <c r="N98" s="12"/>
+      <c r="O98" s="12"/>
+    </row>
+    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A99" s="18" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="B99" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C99" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D99" s="15" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E99" s="28" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F99" s="21" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G99" s="22"/>
       <c r="H99" s="12"/>
       <c r="I99" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J99" s="12"/>
       <c r="K99" s="12"/>
       <c r="L99" s="12"/>
-    </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M99" s="12"/>
+      <c r="N99" s="12"/>
+      <c r="O99" s="12"/>
+    </row>
+    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A100" s="7">
         <v>47</v>
       </c>
       <c r="B100" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C100" s="8"/>
       <c r="D100" s="29" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E100" s="30" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F100" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G100" s="22"/>
       <c r="H100" s="19"/>
       <c r="I100" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J100" s="19"/>
       <c r="K100" s="19"/>
       <c r="L100" s="19"/>
-    </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M100" s="19"/>
+      <c r="N100" s="19"/>
+      <c r="O100" s="19"/>
+    </row>
+    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A101" s="7">
         <v>48</v>
       </c>
       <c r="B101" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C101" s="8"/>
       <c r="D101" s="32" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E101" s="30" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F101" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G101" s="22"/>
       <c r="H101" s="19"/>
       <c r="I101" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J101" s="19"/>
       <c r="K101" s="19"/>
       <c r="L101" s="19"/>
-    </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M101" s="19"/>
+      <c r="N101" s="19"/>
+      <c r="O101" s="19"/>
+    </row>
+    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A102" s="7">
         <v>49</v>
       </c>
       <c r="B102" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C102" s="8"/>
       <c r="D102" s="31" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E102" s="30" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F102" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G102" s="22"/>
       <c r="H102" s="19"/>
       <c r="I102" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J102" s="19"/>
       <c r="K102" s="19"/>
       <c r="L102" s="19"/>
-    </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M102" s="19"/>
+      <c r="N102" s="19"/>
+      <c r="O102" s="19"/>
+    </row>
+    <row r="103" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A103" s="7">
         <v>50</v>
       </c>
       <c r="B103" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C103" s="8"/>
       <c r="D103" s="31" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E103" s="30" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="F103" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G103" s="22"/>
       <c r="H103" s="19"/>
       <c r="I103" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J103" s="19"/>
       <c r="K103" s="19"/>
       <c r="L103" s="19"/>
-    </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M103" s="19"/>
+      <c r="N103" s="19"/>
+      <c r="O103" s="19"/>
+    </row>
+    <row r="104" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A104" s="7">
         <v>51</v>
       </c>
       <c r="B104" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C104" s="8"/>
       <c r="D104" s="31" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E104" s="30" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F104" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G104" s="22"/>
       <c r="H104" s="19"/>
       <c r="I104" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J104" s="19"/>
       <c r="K104" s="19"/>
       <c r="L104" s="19"/>
-    </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M104" s="19"/>
+      <c r="N104" s="19"/>
+      <c r="O104" s="19"/>
+    </row>
+    <row r="105" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A105" s="7">
         <v>52</v>
       </c>
       <c r="B105" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C105" s="8"/>
       <c r="D105" s="31" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E105" s="30" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F105" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G105" s="22"/>
       <c r="H105" s="19"/>
       <c r="I105" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J105" s="19"/>
       <c r="K105" s="19"/>
       <c r="L105" s="19"/>
-    </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M105" s="19"/>
+      <c r="N105" s="19"/>
+      <c r="O105" s="19"/>
+    </row>
+    <row r="106" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A106" s="7">
         <v>53</v>
       </c>
       <c r="B106" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C106" s="8"/>
       <c r="D106" s="15" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E106" s="28" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F106" s="21" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G106" s="22"/>
       <c r="H106" s="19"/>
@@ -4286,58 +4622,67 @@
       <c r="J106" s="19"/>
       <c r="K106" s="19"/>
       <c r="L106" s="19"/>
-    </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M106" s="19"/>
+      <c r="N106" s="19"/>
+      <c r="O106" s="19"/>
+    </row>
+    <row r="107" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A107" s="7">
         <v>54</v>
       </c>
       <c r="B107" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C107" s="16"/>
       <c r="D107" s="17" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E107" s="28" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F107" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G107" s="22"/>
       <c r="H107" s="19"/>
       <c r="I107" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J107" s="19"/>
       <c r="K107" s="19"/>
       <c r="L107" s="19"/>
-    </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M107" s="19"/>
+      <c r="N107" s="19"/>
+      <c r="O107" s="19"/>
+    </row>
+    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A108" s="7">
         <v>55</v>
       </c>
       <c r="B108" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C108" s="16"/>
       <c r="D108" s="17" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E108" s="28" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F108" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G108" s="22"/>
       <c r="H108" s="19"/>
       <c r="I108" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J108" s="19"/>
       <c r="K108" s="19"/>
       <c r="L108" s="19"/>
+      <c r="M108" s="19"/>
+      <c r="N108" s="19"/>
+      <c r="O108" s="19"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:L108" xr:uid="{00000000-0001-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
add extendedEuTaxonomyNonAlignedActivitiesComponent, adapt excel file for eu non-financials
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/euTaxonomyNonFinancials/EutaxonomyNonFinancials.xlsx
+++ b/dataland-framework-toolbox/inputs/euTaxonomyNonFinancials/EutaxonomyNonFinancials.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d93401\Projects\Dataland\dataland-framework-toolbox\inputs\euTaxonomyNonFinancials\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d91596\Dataland\dataland-framework-toolbox\inputs\euTaxonomyNonFinancials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A51A04C-B41B-4769-81F3-48093961F2E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13560" yWindow="0" windowWidth="15345" windowHeight="15585" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13560" yWindow="0" windowWidth="15345" windowHeight="15585" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Framework Data Model" sheetId="1" r:id="rId1"/>
@@ -58,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="826" uniqueCount="248">
   <si>
     <t>Field Identifier</t>
   </si>
@@ -237,9 +236,6 @@
     <t>Absolute value and share of the revenue per activity that is not taxonomy-aligned but eligible</t>
   </si>
   <si>
-    <t>Absolute value and share of the revenue that is not part of a plan to meet the DNSH criteria and make substantial contribution to any environmental objective</t>
-  </si>
-  <si>
     <t>Share of the taxonomy-aligned revenue from total aligned revenue that is linked to activities that enable reduction of GHG in other sectors</t>
   </si>
   <si>
@@ -796,12 +792,21 @@
   </si>
   <si>
     <t>Existence of grievance/complaints handling mechanisms to address violations of the UNGC principles or OECD Guidelines for Multinational Enterprises. See Regulation (EU) 2022/1288, Annex I, top (22) and table 1, indicator nr. 11.</t>
+  </si>
+  <si>
+    <t>Absolute value of the revenue that is not part of a plan to meet the DNSH criteria and make substantial contribution to any environmental objective</t>
+  </si>
+  <si>
+    <t>Relative share of the revenue that is not part of a plan to meet the DNSH criteria and make substantial contribution to any environmental objective</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1213,8 +1218,8 @@
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2" xr:uid="{438AC724-B8E1-4701-895E-04EF1113570C}"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Normal 2" xfId="2"/>
+    <cellStyle name="Normal 3" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1476,18 +1481,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="20.28515625" customWidth="1"/>
-    <col min="4" max="4" width="43.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="88.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="75.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" style="1" customWidth="1"/>
     <col min="6" max="6" width="44.7109375" style="1" customWidth="1"/>
     <col min="7" max="7" width="26.28515625" customWidth="1"/>
     <col min="8" max="14" width="14.28515625" style="1" customWidth="1"/>
@@ -1532,13 +1537,13 @@
         <v>11</v>
       </c>
       <c r="M1" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>239</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -1582,7 +1587,7 @@
         <v>18</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F3" s="10" t="s">
         <v>13</v>
@@ -1704,7 +1709,7 @@
         <v>29</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F7" s="27" t="s">
         <v>55</v>
@@ -1733,7 +1738,7 @@
         <v>25</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F8" s="20" t="s">
         <v>52</v>
@@ -1749,7 +1754,7 @@
       <c r="M8" s="12"/>
       <c r="N8" s="12"/>
       <c r="O8" s="12" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -1761,10 +1766,10 @@
       </c>
       <c r="C9" s="8"/>
       <c r="D9" s="38" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E9" s="34" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F9" s="20" t="s">
         <v>24</v>
@@ -1790,10 +1795,10 @@
       </c>
       <c r="C10" s="8"/>
       <c r="D10" s="33" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E10" s="35" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F10" s="20" t="s">
         <v>24</v>
@@ -1819,10 +1824,10 @@
       </c>
       <c r="C11" s="8"/>
       <c r="D11" s="38" t="s">
+        <v>194</v>
+      </c>
+      <c r="E11" s="36" t="s">
         <v>195</v>
-      </c>
-      <c r="E11" s="36" t="s">
-        <v>196</v>
       </c>
       <c r="F11" s="20" t="s">
         <v>24</v>
@@ -1848,10 +1853,10 @@
       </c>
       <c r="C12" s="8"/>
       <c r="D12" s="38" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E12" s="35" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F12" s="20" t="s">
         <v>24</v>
@@ -1926,7 +1931,7 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B15" s="8" t="s">
         <v>30</v>
@@ -1937,7 +1942,9 @@
       <c r="D15" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="E15" s="19"/>
+      <c r="E15" s="28" t="s">
+        <v>246</v>
+      </c>
       <c r="F15" s="21" t="s">
         <v>26</v>
       </c>
@@ -1949,13 +1956,17 @@
       <c r="J15" s="12"/>
       <c r="K15" s="12"/>
       <c r="L15" s="12"/>
-      <c r="M15" s="12"/>
-      <c r="N15" s="12"/>
+      <c r="M15" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N15" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O15" s="12"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>30</v>
@@ -1967,7 +1978,7 @@
         <v>38</v>
       </c>
       <c r="E16" s="28" t="s">
-        <v>59</v>
+        <v>245</v>
       </c>
       <c r="F16" s="21" t="s">
         <v>34</v>
@@ -1980,8 +1991,12 @@
       <c r="J16" s="12"/>
       <c r="K16" s="12"/>
       <c r="L16" s="12"/>
-      <c r="M16" s="12"/>
-      <c r="N16" s="12"/>
+      <c r="M16" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N16" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O16" s="12"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
@@ -1998,7 +2013,7 @@
         <v>37</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F17" s="21" t="s">
         <v>26</v>
@@ -2011,8 +2026,12 @@
       <c r="J17" s="12"/>
       <c r="K17" s="12"/>
       <c r="L17" s="12"/>
-      <c r="M17" s="12"/>
-      <c r="N17" s="12"/>
+      <c r="M17" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N17" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O17" s="12"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
@@ -2029,7 +2048,7 @@
         <v>38</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F18" s="21" t="s">
         <v>34</v>
@@ -2042,13 +2061,17 @@
       <c r="J18" s="12"/>
       <c r="K18" s="12"/>
       <c r="L18" s="12"/>
-      <c r="M18" s="12"/>
-      <c r="N18" s="12"/>
+      <c r="M18" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N18" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O18" s="12"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="18" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>30</v>
@@ -2060,7 +2083,7 @@
         <v>37</v>
       </c>
       <c r="E19" s="28" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F19" s="21" t="s">
         <v>26</v>
@@ -2073,13 +2096,17 @@
       <c r="J19" s="12"/>
       <c r="K19" s="12"/>
       <c r="L19" s="12"/>
-      <c r="M19" s="12"/>
-      <c r="N19" s="12"/>
+      <c r="M19" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N19" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O19" s="12"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B20" s="8" t="s">
         <v>30</v>
@@ -2091,7 +2118,7 @@
         <v>38</v>
       </c>
       <c r="E20" s="28" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F20" s="21" t="s">
         <v>34</v>
@@ -2104,13 +2131,17 @@
       <c r="J20" s="12"/>
       <c r="K20" s="12"/>
       <c r="L20" s="12"/>
-      <c r="M20" s="12"/>
-      <c r="N20" s="12"/>
+      <c r="M20" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N20" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O20" s="12"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>30</v>
@@ -2123,21 +2154,27 @@
         <v>58</v>
       </c>
       <c r="F21" s="21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G21" s="22"/>
       <c r="H21" s="12"/>
-      <c r="I21" s="12"/>
+      <c r="I21" s="12" t="s">
+        <v>31</v>
+      </c>
       <c r="J21" s="12"/>
       <c r="K21" s="12"/>
       <c r="L21" s="12"/>
-      <c r="M21" s="12"/>
-      <c r="N21" s="12"/>
+      <c r="M21" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N21" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O21" s="12"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>30</v>
@@ -2149,7 +2186,7 @@
         <v>37</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F22" s="21" t="s">
         <v>26</v>
@@ -2162,13 +2199,17 @@
       <c r="J22" s="12"/>
       <c r="K22" s="12"/>
       <c r="L22" s="12"/>
-      <c r="M22" s="12"/>
-      <c r="N22" s="12"/>
+      <c r="M22" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N22" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O22" s="12"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="18" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>30</v>
@@ -2180,7 +2221,7 @@
         <v>38</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F23" s="21" t="s">
         <v>34</v>
@@ -2193,8 +2234,12 @@
       <c r="J23" s="12"/>
       <c r="K23" s="12"/>
       <c r="L23" s="12"/>
-      <c r="M23" s="12"/>
-      <c r="N23" s="12"/>
+      <c r="M23" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N23" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O23" s="12"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
@@ -2206,10 +2251,10 @@
       </c>
       <c r="C24" s="8"/>
       <c r="D24" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="E24" s="30" t="s">
         <v>96</v>
-      </c>
-      <c r="E24" s="30" t="s">
-        <v>97</v>
       </c>
       <c r="F24" s="21" t="s">
         <v>26</v>
@@ -2222,23 +2267,27 @@
       <c r="J24" s="12"/>
       <c r="K24" s="12"/>
       <c r="L24" s="12"/>
-      <c r="M24" s="12"/>
-      <c r="N24" s="12"/>
+      <c r="M24" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N24" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O24" s="12"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="18" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B25" s="8" t="s">
         <v>30</v>
       </c>
       <c r="C25" s="8"/>
       <c r="D25" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="E25" s="30" t="s">
         <v>98</v>
-      </c>
-      <c r="E25" s="30" t="s">
-        <v>99</v>
       </c>
       <c r="F25" s="21" t="s">
         <v>26</v>
@@ -2251,23 +2300,27 @@
       <c r="J25" s="12"/>
       <c r="K25" s="12"/>
       <c r="L25" s="12"/>
-      <c r="M25" s="12"/>
-      <c r="N25" s="12"/>
+      <c r="M25" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N25" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O25" s="12"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="18" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B26" s="8" t="s">
         <v>30</v>
       </c>
       <c r="C26" s="8"/>
       <c r="D26" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="E26" s="30" t="s">
         <v>100</v>
-      </c>
-      <c r="E26" s="30" t="s">
-        <v>101</v>
       </c>
       <c r="F26" s="21" t="s">
         <v>26</v>
@@ -2280,23 +2333,27 @@
       <c r="J26" s="12"/>
       <c r="K26" s="12"/>
       <c r="L26" s="12"/>
-      <c r="M26" s="12"/>
-      <c r="N26" s="12"/>
+      <c r="M26" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N26" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O26" s="12"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B27" s="8" t="s">
         <v>30</v>
       </c>
       <c r="C27" s="8"/>
       <c r="D27" s="29" t="s">
+        <v>101</v>
+      </c>
+      <c r="E27" s="30" t="s">
         <v>102</v>
-      </c>
-      <c r="E27" s="30" t="s">
-        <v>103</v>
       </c>
       <c r="F27" s="21" t="s">
         <v>26</v>
@@ -2309,23 +2366,27 @@
       <c r="J27" s="12"/>
       <c r="K27" s="12"/>
       <c r="L27" s="12"/>
-      <c r="M27" s="12"/>
-      <c r="N27" s="12"/>
+      <c r="M27" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N27" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O27" s="12"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="18" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B28" s="8" t="s">
         <v>30</v>
       </c>
       <c r="C28" s="8"/>
       <c r="D28" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="E28" s="30" t="s">
         <v>104</v>
-      </c>
-      <c r="E28" s="30" t="s">
-        <v>105</v>
       </c>
       <c r="F28" s="21" t="s">
         <v>26</v>
@@ -2338,8 +2399,12 @@
       <c r="J28" s="12"/>
       <c r="K28" s="12"/>
       <c r="L28" s="12"/>
-      <c r="M28" s="12"/>
-      <c r="N28" s="12"/>
+      <c r="M28" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N28" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O28" s="12"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
@@ -2351,10 +2416,10 @@
       </c>
       <c r="C29" s="8"/>
       <c r="D29" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="E29" s="30" t="s">
         <v>107</v>
-      </c>
-      <c r="E29" s="30" t="s">
-        <v>108</v>
       </c>
       <c r="F29" s="21" t="s">
         <v>26</v>
@@ -2367,23 +2432,27 @@
       <c r="J29" s="12"/>
       <c r="K29" s="12"/>
       <c r="L29" s="12"/>
-      <c r="M29" s="12"/>
-      <c r="N29" s="12"/>
+      <c r="M29" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N29" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O29" s="12"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="18" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B30" s="8" t="s">
         <v>30</v>
       </c>
       <c r="C30" s="8"/>
       <c r="D30" s="32" t="s">
+        <v>108</v>
+      </c>
+      <c r="E30" s="30" t="s">
         <v>109</v>
-      </c>
-      <c r="E30" s="30" t="s">
-        <v>110</v>
       </c>
       <c r="F30" s="21" t="s">
         <v>26</v>
@@ -2396,23 +2465,27 @@
       <c r="J30" s="12"/>
       <c r="K30" s="12"/>
       <c r="L30" s="12"/>
-      <c r="M30" s="12"/>
-      <c r="N30" s="12"/>
+      <c r="M30" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N30" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O30" s="12"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="18" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B31" s="8" t="s">
         <v>30</v>
       </c>
       <c r="C31" s="8"/>
       <c r="D31" s="31" t="s">
+        <v>110</v>
+      </c>
+      <c r="E31" s="30" t="s">
         <v>111</v>
-      </c>
-      <c r="E31" s="30" t="s">
-        <v>112</v>
       </c>
       <c r="F31" s="21" t="s">
         <v>26</v>
@@ -2425,23 +2498,27 @@
       <c r="J31" s="12"/>
       <c r="K31" s="12"/>
       <c r="L31" s="12"/>
-      <c r="M31" s="12"/>
-      <c r="N31" s="12"/>
+      <c r="M31" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N31" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O31" s="12"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="18" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B32" s="8" t="s">
         <v>30</v>
       </c>
       <c r="C32" s="8"/>
       <c r="D32" s="31" t="s">
+        <v>112</v>
+      </c>
+      <c r="E32" s="30" t="s">
         <v>113</v>
-      </c>
-      <c r="E32" s="30" t="s">
-        <v>114</v>
       </c>
       <c r="F32" s="21" t="s">
         <v>26</v>
@@ -2454,8 +2531,12 @@
       <c r="J32" s="12"/>
       <c r="K32" s="12"/>
       <c r="L32" s="12"/>
-      <c r="M32" s="12"/>
-      <c r="N32" s="12"/>
+      <c r="M32" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N32" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O32" s="12"/>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
@@ -2467,10 +2548,10 @@
       </c>
       <c r="C33" s="8"/>
       <c r="D33" s="31" t="s">
+        <v>115</v>
+      </c>
+      <c r="E33" s="30" t="s">
         <v>116</v>
-      </c>
-      <c r="E33" s="30" t="s">
-        <v>117</v>
       </c>
       <c r="F33" s="21" t="s">
         <v>26</v>
@@ -2483,23 +2564,27 @@
       <c r="J33" s="12"/>
       <c r="K33" s="12"/>
       <c r="L33" s="12"/>
-      <c r="M33" s="12"/>
-      <c r="N33" s="12"/>
+      <c r="M33" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N33" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O33" s="12"/>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="18" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B34" s="8" t="s">
         <v>30</v>
       </c>
       <c r="C34" s="8"/>
       <c r="D34" s="31" t="s">
+        <v>117</v>
+      </c>
+      <c r="E34" s="30" t="s">
         <v>118</v>
-      </c>
-      <c r="E34" s="30" t="s">
-        <v>119</v>
       </c>
       <c r="F34" s="21" t="s">
         <v>26</v>
@@ -2512,23 +2597,27 @@
       <c r="J34" s="12"/>
       <c r="K34" s="12"/>
       <c r="L34" s="12"/>
-      <c r="M34" s="12"/>
-      <c r="N34" s="12"/>
+      <c r="M34" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N34" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O34" s="12"/>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="18" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B35" s="8" t="s">
         <v>30</v>
       </c>
       <c r="C35" s="8"/>
       <c r="D35" s="31" t="s">
+        <v>119</v>
+      </c>
+      <c r="E35" s="30" t="s">
         <v>120</v>
-      </c>
-      <c r="E35" s="30" t="s">
-        <v>121</v>
       </c>
       <c r="F35" s="21" t="s">
         <v>26</v>
@@ -2541,23 +2630,27 @@
       <c r="J35" s="12"/>
       <c r="K35" s="12"/>
       <c r="L35" s="12"/>
-      <c r="M35" s="12"/>
-      <c r="N35" s="12"/>
+      <c r="M35" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N35" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O35" s="12"/>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" s="18" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B36" s="8" t="s">
         <v>30</v>
       </c>
       <c r="C36" s="8"/>
       <c r="D36" s="31" t="s">
+        <v>121</v>
+      </c>
+      <c r="E36" s="30" t="s">
         <v>122</v>
-      </c>
-      <c r="E36" s="30" t="s">
-        <v>123</v>
       </c>
       <c r="F36" s="21" t="s">
         <v>26</v>
@@ -2570,8 +2663,12 @@
       <c r="J36" s="12"/>
       <c r="K36" s="12"/>
       <c r="L36" s="12"/>
-      <c r="M36" s="12"/>
-      <c r="N36" s="12"/>
+      <c r="M36" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N36" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O36" s="12"/>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
@@ -2583,10 +2680,10 @@
       </c>
       <c r="C37" s="8"/>
       <c r="D37" s="31" t="s">
+        <v>126</v>
+      </c>
+      <c r="E37" s="30" t="s">
         <v>127</v>
-      </c>
-      <c r="E37" s="30" t="s">
-        <v>128</v>
       </c>
       <c r="F37" s="21" t="s">
         <v>26</v>
@@ -2599,23 +2696,27 @@
       <c r="J37" s="12"/>
       <c r="K37" s="12"/>
       <c r="L37" s="12"/>
-      <c r="M37" s="12"/>
-      <c r="N37" s="12"/>
+      <c r="M37" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N37" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O37" s="12"/>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" s="18" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B38" s="8" t="s">
         <v>30</v>
       </c>
       <c r="C38" s="8"/>
       <c r="D38" s="31" t="s">
+        <v>128</v>
+      </c>
+      <c r="E38" s="30" t="s">
         <v>129</v>
-      </c>
-      <c r="E38" s="30" t="s">
-        <v>130</v>
       </c>
       <c r="F38" s="21" t="s">
         <v>26</v>
@@ -2628,23 +2729,27 @@
       <c r="J38" s="12"/>
       <c r="K38" s="12"/>
       <c r="L38" s="12"/>
-      <c r="M38" s="12"/>
-      <c r="N38" s="12"/>
+      <c r="M38" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N38" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O38" s="12"/>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" s="18" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B39" s="8" t="s">
         <v>30</v>
       </c>
       <c r="C39" s="8"/>
       <c r="D39" s="31" t="s">
+        <v>130</v>
+      </c>
+      <c r="E39" s="30" t="s">
         <v>131</v>
-      </c>
-      <c r="E39" s="30" t="s">
-        <v>132</v>
       </c>
       <c r="F39" s="21" t="s">
         <v>26</v>
@@ -2657,23 +2762,27 @@
       <c r="J39" s="12"/>
       <c r="K39" s="12"/>
       <c r="L39" s="12"/>
-      <c r="M39" s="12"/>
-      <c r="N39" s="12"/>
+      <c r="M39" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N39" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O39" s="12"/>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" s="18" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B40" s="8" t="s">
         <v>30</v>
       </c>
       <c r="C40" s="8"/>
       <c r="D40" s="31" t="s">
+        <v>132</v>
+      </c>
+      <c r="E40" s="30" t="s">
         <v>133</v>
-      </c>
-      <c r="E40" s="30" t="s">
-        <v>134</v>
       </c>
       <c r="F40" s="21" t="s">
         <v>26</v>
@@ -2686,8 +2795,12 @@
       <c r="J40" s="12"/>
       <c r="K40" s="12"/>
       <c r="L40" s="12"/>
-      <c r="M40" s="12"/>
-      <c r="N40" s="12"/>
+      <c r="M40" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N40" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O40" s="12"/>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
@@ -2699,10 +2812,10 @@
       </c>
       <c r="C41" s="8"/>
       <c r="D41" s="31" t="s">
+        <v>137</v>
+      </c>
+      <c r="E41" s="30" t="s">
         <v>138</v>
-      </c>
-      <c r="E41" s="30" t="s">
-        <v>139</v>
       </c>
       <c r="F41" s="21" t="s">
         <v>26</v>
@@ -2715,23 +2828,27 @@
       <c r="J41" s="12"/>
       <c r="K41" s="12"/>
       <c r="L41" s="12"/>
-      <c r="M41" s="12"/>
-      <c r="N41" s="12"/>
+      <c r="M41" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N41" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O41" s="12"/>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" s="18" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B42" s="8" t="s">
         <v>30</v>
       </c>
       <c r="C42" s="8"/>
       <c r="D42" s="31" t="s">
+        <v>139</v>
+      </c>
+      <c r="E42" s="30" t="s">
         <v>140</v>
-      </c>
-      <c r="E42" s="30" t="s">
-        <v>141</v>
       </c>
       <c r="F42" s="21" t="s">
         <v>26</v>
@@ -2744,23 +2861,27 @@
       <c r="J42" s="12"/>
       <c r="K42" s="12"/>
       <c r="L42" s="12"/>
-      <c r="M42" s="12"/>
-      <c r="N42" s="12"/>
+      <c r="M42" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N42" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O42" s="12"/>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" s="18" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B43" s="8" t="s">
         <v>30</v>
       </c>
       <c r="C43" s="8"/>
       <c r="D43" s="31" t="s">
+        <v>141</v>
+      </c>
+      <c r="E43" s="30" t="s">
         <v>142</v>
-      </c>
-      <c r="E43" s="30" t="s">
-        <v>143</v>
       </c>
       <c r="F43" s="21" t="s">
         <v>26</v>
@@ -2773,23 +2894,27 @@
       <c r="J43" s="12"/>
       <c r="K43" s="12"/>
       <c r="L43" s="12"/>
-      <c r="M43" s="12"/>
-      <c r="N43" s="12"/>
+      <c r="M43" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N43" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O43" s="12"/>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" s="18" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B44" s="8" t="s">
         <v>30</v>
       </c>
       <c r="C44" s="8"/>
       <c r="D44" s="31" t="s">
+        <v>143</v>
+      </c>
+      <c r="E44" s="30" t="s">
         <v>144</v>
-      </c>
-      <c r="E44" s="30" t="s">
-        <v>145</v>
       </c>
       <c r="F44" s="21" t="s">
         <v>26</v>
@@ -2802,8 +2927,12 @@
       <c r="J44" s="12"/>
       <c r="K44" s="12"/>
       <c r="L44" s="12"/>
-      <c r="M44" s="12"/>
-      <c r="N44" s="12"/>
+      <c r="M44" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N44" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O44" s="12"/>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
@@ -2815,10 +2944,10 @@
       </c>
       <c r="C45" s="8"/>
       <c r="D45" s="31" t="s">
+        <v>148</v>
+      </c>
+      <c r="E45" s="30" t="s">
         <v>149</v>
-      </c>
-      <c r="E45" s="30" t="s">
-        <v>150</v>
       </c>
       <c r="F45" s="21" t="s">
         <v>26</v>
@@ -2831,23 +2960,27 @@
       <c r="J45" s="12"/>
       <c r="K45" s="12"/>
       <c r="L45" s="12"/>
-      <c r="M45" s="12"/>
-      <c r="N45" s="12"/>
+      <c r="M45" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N45" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O45" s="12"/>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" s="18" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B46" s="8" t="s">
         <v>30</v>
       </c>
       <c r="C46" s="8"/>
       <c r="D46" s="31" t="s">
+        <v>150</v>
+      </c>
+      <c r="E46" s="30" t="s">
         <v>151</v>
-      </c>
-      <c r="E46" s="30" t="s">
-        <v>152</v>
       </c>
       <c r="F46" s="21" t="s">
         <v>26</v>
@@ -2860,23 +2993,27 @@
       <c r="J46" s="12"/>
       <c r="K46" s="12"/>
       <c r="L46" s="12"/>
-      <c r="M46" s="12"/>
-      <c r="N46" s="12"/>
+      <c r="M46" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N46" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O46" s="12"/>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" s="18" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B47" s="8" t="s">
         <v>30</v>
       </c>
       <c r="C47" s="8"/>
       <c r="D47" s="31" t="s">
+        <v>152</v>
+      </c>
+      <c r="E47" s="30" t="s">
         <v>153</v>
-      </c>
-      <c r="E47" s="30" t="s">
-        <v>154</v>
       </c>
       <c r="F47" s="21" t="s">
         <v>26</v>
@@ -2889,23 +3026,27 @@
       <c r="J47" s="12"/>
       <c r="K47" s="12"/>
       <c r="L47" s="12"/>
-      <c r="M47" s="12"/>
-      <c r="N47" s="12"/>
+      <c r="M47" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N47" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O47" s="12"/>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" s="18" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B48" s="8" t="s">
         <v>30</v>
       </c>
       <c r="C48" s="8"/>
       <c r="D48" s="31" t="s">
+        <v>154</v>
+      </c>
+      <c r="E48" s="30" t="s">
         <v>155</v>
-      </c>
-      <c r="E48" s="30" t="s">
-        <v>156</v>
       </c>
       <c r="F48" s="21" t="s">
         <v>26</v>
@@ -2918,8 +3059,12 @@
       <c r="J48" s="12"/>
       <c r="K48" s="12"/>
       <c r="L48" s="12"/>
-      <c r="M48" s="12"/>
-      <c r="N48" s="12"/>
+      <c r="M48" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N48" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O48" s="12"/>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.25">
@@ -2937,7 +3082,7 @@
         <v>57</v>
       </c>
       <c r="F49" s="21" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G49" s="22"/>
       <c r="H49" s="12"/>
@@ -2945,8 +3090,12 @@
       <c r="J49" s="12"/>
       <c r="K49" s="12"/>
       <c r="L49" s="12"/>
-      <c r="M49" s="12"/>
-      <c r="N49" s="12"/>
+      <c r="M49" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N49" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O49" s="12"/>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.25">
@@ -2961,7 +3110,7 @@
         <v>44</v>
       </c>
       <c r="E50" s="28" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F50" s="21" t="s">
         <v>26</v>
@@ -2974,8 +3123,12 @@
       <c r="J50" s="12"/>
       <c r="K50" s="12"/>
       <c r="L50" s="12"/>
-      <c r="M50" s="12"/>
-      <c r="N50" s="12"/>
+      <c r="M50" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N50" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O50" s="12"/>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.25">
@@ -2990,7 +3143,7 @@
         <v>45</v>
       </c>
       <c r="E51" s="28" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F51" s="21" t="s">
         <v>26</v>
@@ -3003,8 +3156,12 @@
       <c r="J51" s="12"/>
       <c r="K51" s="12"/>
       <c r="L51" s="12"/>
-      <c r="M51" s="12"/>
-      <c r="N51" s="12"/>
+      <c r="M51" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N51" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O51" s="12"/>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.25">
@@ -3019,7 +3176,7 @@
         <v>35</v>
       </c>
       <c r="E52" s="28" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F52" s="21" t="s">
         <v>34</v>
@@ -3032,13 +3189,17 @@
       <c r="J52" s="12"/>
       <c r="K52" s="12"/>
       <c r="L52" s="12"/>
-      <c r="M52" s="12"/>
-      <c r="N52" s="12"/>
+      <c r="M52" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N52" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O52" s="12"/>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" s="18" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B53" s="8" t="s">
         <v>32</v>
@@ -3050,7 +3211,7 @@
         <v>37</v>
       </c>
       <c r="E53" s="28" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F53" s="21" t="s">
         <v>26</v>
@@ -3063,13 +3224,17 @@
       <c r="J53" s="12"/>
       <c r="K53" s="12"/>
       <c r="L53" s="12"/>
-      <c r="M53" s="12"/>
-      <c r="N53" s="12"/>
+      <c r="M53" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N53" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O53" s="12"/>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" s="18" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B54" s="8" t="s">
         <v>32</v>
@@ -3081,7 +3246,7 @@
         <v>38</v>
       </c>
       <c r="E54" s="28" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F54" s="21" t="s">
         <v>34</v>
@@ -3094,8 +3259,12 @@
       <c r="J54" s="12"/>
       <c r="K54" s="12"/>
       <c r="L54" s="12"/>
-      <c r="M54" s="12"/>
-      <c r="N54" s="12"/>
+      <c r="M54" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N54" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O54" s="12"/>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.25">
@@ -3112,7 +3281,7 @@
         <v>37</v>
       </c>
       <c r="E55" s="28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F55" s="21" t="s">
         <v>26</v>
@@ -3125,13 +3294,17 @@
       <c r="J55" s="12"/>
       <c r="K55" s="12"/>
       <c r="L55" s="12"/>
-      <c r="M55" s="12"/>
-      <c r="N55" s="12"/>
+      <c r="M55" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N55" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O55" s="12"/>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" s="18" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B56" s="8" t="s">
         <v>32</v>
@@ -3143,7 +3316,7 @@
         <v>38</v>
       </c>
       <c r="E56" s="28" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F56" s="21" t="s">
         <v>34</v>
@@ -3156,13 +3329,17 @@
       <c r="J56" s="12"/>
       <c r="K56" s="12"/>
       <c r="L56" s="12"/>
-      <c r="M56" s="12"/>
-      <c r="N56" s="12"/>
+      <c r="M56" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N56" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O56" s="12"/>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" s="18" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B57" s="8" t="s">
         <v>32</v>
@@ -3174,7 +3351,7 @@
         <v>37</v>
       </c>
       <c r="E57" s="28" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F57" s="21" t="s">
         <v>26</v>
@@ -3187,13 +3364,17 @@
       <c r="J57" s="12"/>
       <c r="K57" s="12"/>
       <c r="L57" s="12"/>
-      <c r="M57" s="12"/>
-      <c r="N57" s="12"/>
+      <c r="M57" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N57" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O57" s="12"/>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" s="18" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B58" s="8" t="s">
         <v>32</v>
@@ -3205,7 +3386,7 @@
         <v>38</v>
       </c>
       <c r="E58" s="28" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F58" s="21" t="s">
         <v>34</v>
@@ -3218,13 +3399,17 @@
       <c r="J58" s="12"/>
       <c r="K58" s="12"/>
       <c r="L58" s="12"/>
-      <c r="M58" s="12"/>
-      <c r="N58" s="12"/>
+      <c r="M58" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N58" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O58" s="12"/>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B59" s="8" t="s">
         <v>32</v>
@@ -3234,10 +3419,10 @@
         <v>41</v>
       </c>
       <c r="E59" s="28" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F59" s="21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G59" s="22"/>
       <c r="H59" s="12"/>
@@ -3245,13 +3430,17 @@
       <c r="J59" s="12"/>
       <c r="K59" s="12"/>
       <c r="L59" s="12"/>
-      <c r="M59" s="12"/>
-      <c r="N59" s="12"/>
+      <c r="M59" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N59" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O59" s="12"/>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60" s="18" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B60" s="8" t="s">
         <v>32</v>
@@ -3263,7 +3452,7 @@
         <v>37</v>
       </c>
       <c r="E60" s="28" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F60" s="21" t="s">
         <v>26</v>
@@ -3276,13 +3465,17 @@
       <c r="J60" s="12"/>
       <c r="K60" s="12"/>
       <c r="L60" s="12"/>
-      <c r="M60" s="12"/>
-      <c r="N60" s="12"/>
+      <c r="M60" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N60" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O60" s="12"/>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61" s="18" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B61" s="8" t="s">
         <v>32</v>
@@ -3294,7 +3487,7 @@
         <v>38</v>
       </c>
       <c r="E61" s="28" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F61" s="21" t="s">
         <v>34</v>
@@ -3307,8 +3500,12 @@
       <c r="J61" s="12"/>
       <c r="K61" s="12"/>
       <c r="L61" s="12"/>
-      <c r="M61" s="12"/>
-      <c r="N61" s="12"/>
+      <c r="M61" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N61" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O61" s="12"/>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.25">
@@ -3320,10 +3517,10 @@
       </c>
       <c r="C62" s="8"/>
       <c r="D62" s="29" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E62" s="30" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F62" s="21" t="s">
         <v>26</v>
@@ -3336,23 +3533,27 @@
       <c r="J62" s="12"/>
       <c r="K62" s="12"/>
       <c r="L62" s="12"/>
-      <c r="M62" s="12"/>
-      <c r="N62" s="12"/>
+      <c r="M62" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N62" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O62" s="12"/>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A63" s="18" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B63" s="8" t="s">
         <v>32</v>
       </c>
       <c r="C63" s="8"/>
       <c r="D63" s="29" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E63" s="30" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F63" s="21" t="s">
         <v>26</v>
@@ -3365,23 +3566,27 @@
       <c r="J63" s="12"/>
       <c r="K63" s="12"/>
       <c r="L63" s="12"/>
-      <c r="M63" s="12"/>
-      <c r="N63" s="12"/>
+      <c r="M63" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N63" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O63" s="12"/>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A64" s="18" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B64" s="8" t="s">
         <v>32</v>
       </c>
       <c r="C64" s="8"/>
       <c r="D64" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="E64" s="30" t="s">
         <v>100</v>
-      </c>
-      <c r="E64" s="30" t="s">
-        <v>101</v>
       </c>
       <c r="F64" s="21" t="s">
         <v>26</v>
@@ -3394,23 +3599,27 @@
       <c r="J64" s="12"/>
       <c r="K64" s="12"/>
       <c r="L64" s="12"/>
-      <c r="M64" s="12"/>
-      <c r="N64" s="12"/>
+      <c r="M64" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N64" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O64" s="12"/>
     </row>
     <row r="65" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A65" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B65" s="8" t="s">
         <v>32</v>
       </c>
       <c r="C65" s="8"/>
       <c r="D65" s="29" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E65" s="30" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F65" s="21" t="s">
         <v>26</v>
@@ -3423,23 +3632,27 @@
       <c r="J65" s="12"/>
       <c r="K65" s="12"/>
       <c r="L65" s="12"/>
-      <c r="M65" s="12"/>
-      <c r="N65" s="12"/>
+      <c r="M65" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N65" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O65" s="12"/>
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A66" s="18" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B66" s="8" t="s">
         <v>32</v>
       </c>
       <c r="C66" s="8"/>
       <c r="D66" s="29" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E66" s="30" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F66" s="21" t="s">
         <v>26</v>
@@ -3452,8 +3665,12 @@
       <c r="J66" s="12"/>
       <c r="K66" s="12"/>
       <c r="L66" s="12"/>
-      <c r="M66" s="12"/>
-      <c r="N66" s="12"/>
+      <c r="M66" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N66" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O66" s="12"/>
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.25">
@@ -3465,10 +3682,10 @@
       </c>
       <c r="C67" s="8"/>
       <c r="D67" s="32" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E67" s="30" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F67" s="21" t="s">
         <v>26</v>
@@ -3481,23 +3698,27 @@
       <c r="J67" s="12"/>
       <c r="K67" s="12"/>
       <c r="L67" s="12"/>
-      <c r="M67" s="12"/>
-      <c r="N67" s="12"/>
+      <c r="M67" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N67" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O67" s="12"/>
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A68" s="18" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B68" s="8" t="s">
         <v>32</v>
       </c>
       <c r="C68" s="8"/>
       <c r="D68" s="32" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E68" s="30" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F68" s="21" t="s">
         <v>26</v>
@@ -3510,23 +3731,27 @@
       <c r="J68" s="12"/>
       <c r="K68" s="12"/>
       <c r="L68" s="12"/>
-      <c r="M68" s="12"/>
-      <c r="N68" s="12"/>
+      <c r="M68" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N68" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O68" s="12"/>
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A69" s="18" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B69" s="8" t="s">
         <v>32</v>
       </c>
       <c r="C69" s="8"/>
       <c r="D69" s="31" t="s">
+        <v>110</v>
+      </c>
+      <c r="E69" s="30" t="s">
         <v>111</v>
-      </c>
-      <c r="E69" s="30" t="s">
-        <v>112</v>
       </c>
       <c r="F69" s="21" t="s">
         <v>26</v>
@@ -3539,23 +3764,27 @@
       <c r="J69" s="12"/>
       <c r="K69" s="12"/>
       <c r="L69" s="12"/>
-      <c r="M69" s="12"/>
-      <c r="N69" s="12"/>
+      <c r="M69" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N69" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O69" s="12"/>
     </row>
     <row r="70" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A70" s="18" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B70" s="8" t="s">
         <v>32</v>
       </c>
       <c r="C70" s="8"/>
       <c r="D70" s="31" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E70" s="30" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F70" s="21" t="s">
         <v>26</v>
@@ -3568,8 +3797,12 @@
       <c r="J70" s="12"/>
       <c r="K70" s="12"/>
       <c r="L70" s="12"/>
-      <c r="M70" s="12"/>
-      <c r="N70" s="12"/>
+      <c r="M70" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N70" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O70" s="12"/>
     </row>
     <row r="71" spans="1:15" x14ac:dyDescent="0.25">
@@ -3581,10 +3814,10 @@
       </c>
       <c r="C71" s="8"/>
       <c r="D71" s="31" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E71" s="30" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F71" s="21" t="s">
         <v>26</v>
@@ -3597,23 +3830,27 @@
       <c r="J71" s="12"/>
       <c r="K71" s="12"/>
       <c r="L71" s="12"/>
-      <c r="M71" s="12"/>
-      <c r="N71" s="12"/>
+      <c r="M71" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N71" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O71" s="12"/>
     </row>
     <row r="72" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A72" s="18" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B72" s="8" t="s">
         <v>32</v>
       </c>
       <c r="C72" s="8"/>
       <c r="D72" s="31" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E72" s="30" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F72" s="21" t="s">
         <v>26</v>
@@ -3626,23 +3863,27 @@
       <c r="J72" s="12"/>
       <c r="K72" s="12"/>
       <c r="L72" s="12"/>
-      <c r="M72" s="12"/>
-      <c r="N72" s="12"/>
+      <c r="M72" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N72" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O72" s="12"/>
     </row>
     <row r="73" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A73" s="18" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B73" s="8" t="s">
         <v>32</v>
       </c>
       <c r="C73" s="8"/>
       <c r="D73" s="31" t="s">
+        <v>119</v>
+      </c>
+      <c r="E73" s="30" t="s">
         <v>120</v>
-      </c>
-      <c r="E73" s="30" t="s">
-        <v>121</v>
       </c>
       <c r="F73" s="21" t="s">
         <v>26</v>
@@ -3655,23 +3896,27 @@
       <c r="J73" s="12"/>
       <c r="K73" s="12"/>
       <c r="L73" s="12"/>
-      <c r="M73" s="12"/>
-      <c r="N73" s="12"/>
+      <c r="M73" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N73" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O73" s="12"/>
     </row>
     <row r="74" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A74" s="18" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B74" s="8" t="s">
         <v>32</v>
       </c>
       <c r="C74" s="8"/>
       <c r="D74" s="31" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E74" s="30" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F74" s="21" t="s">
         <v>26</v>
@@ -3684,8 +3929,12 @@
       <c r="J74" s="12"/>
       <c r="K74" s="12"/>
       <c r="L74" s="12"/>
-      <c r="M74" s="12"/>
-      <c r="N74" s="12"/>
+      <c r="M74" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N74" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O74" s="12"/>
     </row>
     <row r="75" spans="1:15" x14ac:dyDescent="0.25">
@@ -3697,10 +3946,10 @@
       </c>
       <c r="C75" s="8"/>
       <c r="D75" s="31" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E75" s="30" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F75" s="21" t="s">
         <v>26</v>
@@ -3713,23 +3962,27 @@
       <c r="J75" s="12"/>
       <c r="K75" s="12"/>
       <c r="L75" s="12"/>
-      <c r="M75" s="12"/>
-      <c r="N75" s="12"/>
+      <c r="M75" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N75" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O75" s="12"/>
     </row>
     <row r="76" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A76" s="18" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B76" s="8" t="s">
         <v>32</v>
       </c>
       <c r="C76" s="8"/>
       <c r="D76" s="31" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E76" s="30" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F76" s="21" t="s">
         <v>26</v>
@@ -3742,23 +3995,27 @@
       <c r="J76" s="12"/>
       <c r="K76" s="12"/>
       <c r="L76" s="12"/>
-      <c r="M76" s="12"/>
-      <c r="N76" s="12"/>
+      <c r="M76" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N76" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O76" s="12"/>
     </row>
     <row r="77" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A77" s="18" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B77" s="8" t="s">
         <v>32</v>
       </c>
       <c r="C77" s="8"/>
       <c r="D77" s="31" t="s">
+        <v>130</v>
+      </c>
+      <c r="E77" s="30" t="s">
         <v>131</v>
-      </c>
-      <c r="E77" s="30" t="s">
-        <v>132</v>
       </c>
       <c r="F77" s="21" t="s">
         <v>26</v>
@@ -3771,23 +4028,27 @@
       <c r="J77" s="12"/>
       <c r="K77" s="12"/>
       <c r="L77" s="12"/>
-      <c r="M77" s="12"/>
-      <c r="N77" s="12"/>
+      <c r="M77" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N77" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O77" s="12"/>
     </row>
     <row r="78" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A78" s="18" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B78" s="8" t="s">
         <v>32</v>
       </c>
       <c r="C78" s="8"/>
       <c r="D78" s="31" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E78" s="30" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F78" s="21" t="s">
         <v>26</v>
@@ -3800,8 +4061,12 @@
       <c r="J78" s="12"/>
       <c r="K78" s="12"/>
       <c r="L78" s="12"/>
-      <c r="M78" s="12"/>
-      <c r="N78" s="12"/>
+      <c r="M78" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N78" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O78" s="12"/>
     </row>
     <row r="79" spans="1:15" x14ac:dyDescent="0.25">
@@ -3813,10 +4078,10 @@
       </c>
       <c r="C79" s="8"/>
       <c r="D79" s="31" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E79" s="30" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F79" s="21" t="s">
         <v>26</v>
@@ -3829,23 +4094,27 @@
       <c r="J79" s="12"/>
       <c r="K79" s="12"/>
       <c r="L79" s="12"/>
-      <c r="M79" s="12"/>
-      <c r="N79" s="12"/>
+      <c r="M79" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N79" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O79" s="12"/>
     </row>
     <row r="80" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A80" s="18" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B80" s="8" t="s">
         <v>32</v>
       </c>
       <c r="C80" s="8"/>
       <c r="D80" s="31" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E80" s="30" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F80" s="21" t="s">
         <v>26</v>
@@ -3858,23 +4127,27 @@
       <c r="J80" s="12"/>
       <c r="K80" s="12"/>
       <c r="L80" s="12"/>
-      <c r="M80" s="12"/>
-      <c r="N80" s="12"/>
+      <c r="M80" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N80" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O80" s="12"/>
     </row>
     <row r="81" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A81" s="18" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B81" s="8" t="s">
         <v>32</v>
       </c>
       <c r="C81" s="8"/>
       <c r="D81" s="31" t="s">
+        <v>141</v>
+      </c>
+      <c r="E81" s="30" t="s">
         <v>142</v>
-      </c>
-      <c r="E81" s="30" t="s">
-        <v>143</v>
       </c>
       <c r="F81" s="21" t="s">
         <v>26</v>
@@ -3887,23 +4160,27 @@
       <c r="J81" s="12"/>
       <c r="K81" s="12"/>
       <c r="L81" s="12"/>
-      <c r="M81" s="12"/>
-      <c r="N81" s="12"/>
+      <c r="M81" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N81" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O81" s="12"/>
     </row>
     <row r="82" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A82" s="18" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B82" s="8" t="s">
         <v>32</v>
       </c>
       <c r="C82" s="8"/>
       <c r="D82" s="31" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E82" s="30" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F82" s="21" t="s">
         <v>26</v>
@@ -3916,8 +4193,12 @@
       <c r="J82" s="12"/>
       <c r="K82" s="12"/>
       <c r="L82" s="12"/>
-      <c r="M82" s="12"/>
-      <c r="N82" s="12"/>
+      <c r="M82" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N82" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O82" s="12"/>
     </row>
     <row r="83" spans="1:15" x14ac:dyDescent="0.25">
@@ -3929,10 +4210,10 @@
       </c>
       <c r="C83" s="8"/>
       <c r="D83" s="31" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E83" s="30" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F83" s="21" t="s">
         <v>26</v>
@@ -3945,23 +4226,27 @@
       <c r="J83" s="12"/>
       <c r="K83" s="12"/>
       <c r="L83" s="12"/>
-      <c r="M83" s="12"/>
-      <c r="N83" s="12"/>
+      <c r="M83" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N83" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O83" s="12"/>
     </row>
     <row r="84" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A84" s="18" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B84" s="8" t="s">
         <v>32</v>
       </c>
       <c r="C84" s="8"/>
       <c r="D84" s="31" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E84" s="30" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F84" s="21" t="s">
         <v>26</v>
@@ -3974,23 +4259,27 @@
       <c r="J84" s="12"/>
       <c r="K84" s="12"/>
       <c r="L84" s="12"/>
-      <c r="M84" s="12"/>
-      <c r="N84" s="12"/>
+      <c r="M84" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N84" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O84" s="12"/>
     </row>
     <row r="85" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A85" s="18" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B85" s="8" t="s">
         <v>32</v>
       </c>
       <c r="C85" s="8"/>
       <c r="D85" s="31" t="s">
+        <v>152</v>
+      </c>
+      <c r="E85" s="30" t="s">
         <v>153</v>
-      </c>
-      <c r="E85" s="30" t="s">
-        <v>154</v>
       </c>
       <c r="F85" s="21" t="s">
         <v>26</v>
@@ -4003,23 +4292,27 @@
       <c r="J85" s="12"/>
       <c r="K85" s="12"/>
       <c r="L85" s="12"/>
-      <c r="M85" s="12"/>
-      <c r="N85" s="12"/>
+      <c r="M85" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N85" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O85" s="12"/>
     </row>
     <row r="86" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A86" s="18" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B86" s="8" t="s">
         <v>32</v>
       </c>
       <c r="C86" s="8"/>
       <c r="D86" s="31" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E86" s="30" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F86" s="21" t="s">
         <v>26</v>
@@ -4032,8 +4325,12 @@
       <c r="J86" s="12"/>
       <c r="K86" s="12"/>
       <c r="L86" s="12"/>
-      <c r="M86" s="12"/>
-      <c r="N86" s="12"/>
+      <c r="M86" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N86" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O86" s="12"/>
     </row>
     <row r="87" spans="1:15" x14ac:dyDescent="0.25">
@@ -4048,10 +4345,10 @@
         <v>43</v>
       </c>
       <c r="E87" s="28" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F87" s="21" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G87" s="22"/>
       <c r="H87" s="12"/>
@@ -4059,8 +4356,12 @@
       <c r="J87" s="12"/>
       <c r="K87" s="12"/>
       <c r="L87" s="12"/>
-      <c r="M87" s="12"/>
-      <c r="N87" s="12"/>
+      <c r="M87" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N87" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O87" s="12"/>
     </row>
     <row r="88" spans="1:15" x14ac:dyDescent="0.25">
@@ -4075,7 +4376,7 @@
         <v>44</v>
       </c>
       <c r="E88" s="28" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F88" s="21" t="s">
         <v>26</v>
@@ -4088,8 +4389,12 @@
       <c r="J88" s="12"/>
       <c r="K88" s="12"/>
       <c r="L88" s="12"/>
-      <c r="M88" s="12"/>
-      <c r="N88" s="12"/>
+      <c r="M88" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N88" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O88" s="12"/>
     </row>
     <row r="89" spans="1:15" x14ac:dyDescent="0.25">
@@ -4104,7 +4409,7 @@
         <v>45</v>
       </c>
       <c r="E89" s="28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F89" s="21" t="s">
         <v>26</v>
@@ -4117,8 +4422,12 @@
       <c r="J89" s="12"/>
       <c r="K89" s="12"/>
       <c r="L89" s="12"/>
-      <c r="M89" s="12"/>
-      <c r="N89" s="12"/>
+      <c r="M89" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N89" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O89" s="12"/>
     </row>
     <row r="90" spans="1:15" x14ac:dyDescent="0.25">
@@ -4133,7 +4442,7 @@
         <v>35</v>
       </c>
       <c r="E90" s="28" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F90" s="21" t="s">
         <v>34</v>
@@ -4146,13 +4455,17 @@
       <c r="J90" s="12"/>
       <c r="K90" s="12"/>
       <c r="L90" s="12"/>
-      <c r="M90" s="12"/>
-      <c r="N90" s="12"/>
+      <c r="M90" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N90" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O90" s="12"/>
     </row>
     <row r="91" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A91" s="18" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B91" s="8" t="s">
         <v>33</v>
@@ -4164,7 +4477,7 @@
         <v>37</v>
       </c>
       <c r="E91" s="28" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F91" s="21" t="s">
         <v>26</v>
@@ -4177,13 +4490,17 @@
       <c r="J91" s="12"/>
       <c r="K91" s="12"/>
       <c r="L91" s="12"/>
-      <c r="M91" s="12"/>
-      <c r="N91" s="12"/>
+      <c r="M91" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N91" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O91" s="12"/>
     </row>
     <row r="92" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A92" s="18" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B92" s="8" t="s">
         <v>33</v>
@@ -4195,7 +4512,7 @@
         <v>38</v>
       </c>
       <c r="E92" s="28" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F92" s="21" t="s">
         <v>34</v>
@@ -4208,8 +4525,12 @@
       <c r="J92" s="12"/>
       <c r="K92" s="12"/>
       <c r="L92" s="12"/>
-      <c r="M92" s="12"/>
-      <c r="N92" s="12"/>
+      <c r="M92" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N92" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O92" s="12"/>
     </row>
     <row r="93" spans="1:15" x14ac:dyDescent="0.25">
@@ -4226,7 +4547,7 @@
         <v>37</v>
       </c>
       <c r="E93" s="28" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F93" s="21" t="s">
         <v>26</v>
@@ -4239,8 +4560,12 @@
       <c r="J93" s="12"/>
       <c r="K93" s="12"/>
       <c r="L93" s="12"/>
-      <c r="M93" s="12"/>
-      <c r="N93" s="12"/>
+      <c r="M93" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N93" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O93" s="12"/>
     </row>
     <row r="94" spans="1:15" x14ac:dyDescent="0.25">
@@ -4257,7 +4582,7 @@
         <v>38</v>
       </c>
       <c r="E94" s="28" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F94" s="21" t="s">
         <v>34</v>
@@ -4270,13 +4595,17 @@
       <c r="J94" s="12"/>
       <c r="K94" s="12"/>
       <c r="L94" s="12"/>
-      <c r="M94" s="12"/>
-      <c r="N94" s="12"/>
+      <c r="M94" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N94" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O94" s="12"/>
     </row>
     <row r="95" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A95" s="18" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B95" s="8" t="s">
         <v>33</v>
@@ -4288,7 +4617,7 @@
         <v>37</v>
       </c>
       <c r="E95" s="28" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F95" s="21" t="s">
         <v>26</v>
@@ -4301,13 +4630,17 @@
       <c r="J95" s="12"/>
       <c r="K95" s="12"/>
       <c r="L95" s="12"/>
-      <c r="M95" s="12"/>
-      <c r="N95" s="12"/>
+      <c r="M95" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N95" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O95" s="12"/>
     </row>
     <row r="96" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A96" s="18" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B96" s="8" t="s">
         <v>33</v>
@@ -4319,7 +4652,7 @@
         <v>38</v>
       </c>
       <c r="E96" s="28" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F96" s="21" t="s">
         <v>34</v>
@@ -4332,13 +4665,17 @@
       <c r="J96" s="12"/>
       <c r="K96" s="12"/>
       <c r="L96" s="12"/>
-      <c r="M96" s="12"/>
-      <c r="N96" s="12"/>
+      <c r="M96" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N96" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O96" s="12"/>
     </row>
     <row r="97" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A97" s="18" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B97" s="8" t="s">
         <v>33</v>
@@ -4348,10 +4685,10 @@
         <v>41</v>
       </c>
       <c r="E97" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F97" s="21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G97" s="22"/>
       <c r="H97" s="12"/>
@@ -4359,13 +4696,17 @@
       <c r="J97" s="12"/>
       <c r="K97" s="12"/>
       <c r="L97" s="12"/>
-      <c r="M97" s="12"/>
-      <c r="N97" s="12"/>
+      <c r="M97" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N97" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O97" s="12"/>
     </row>
     <row r="98" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A98" s="18" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B98" s="8" t="s">
         <v>33</v>
@@ -4377,7 +4718,7 @@
         <v>37</v>
       </c>
       <c r="E98" s="28" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F98" s="21" t="s">
         <v>26</v>
@@ -4390,13 +4731,17 @@
       <c r="J98" s="12"/>
       <c r="K98" s="12"/>
       <c r="L98" s="12"/>
-      <c r="M98" s="12"/>
-      <c r="N98" s="12"/>
+      <c r="M98" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N98" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O98" s="12"/>
     </row>
     <row r="99" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A99" s="18" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B99" s="8" t="s">
         <v>33</v>
@@ -4408,7 +4753,7 @@
         <v>38</v>
       </c>
       <c r="E99" s="28" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F99" s="21" t="s">
         <v>34</v>
@@ -4421,8 +4766,12 @@
       <c r="J99" s="12"/>
       <c r="K99" s="12"/>
       <c r="L99" s="12"/>
-      <c r="M99" s="12"/>
-      <c r="N99" s="12"/>
+      <c r="M99" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N99" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O99" s="12"/>
     </row>
     <row r="100" spans="1:15" x14ac:dyDescent="0.25">
@@ -4434,10 +4783,10 @@
       </c>
       <c r="C100" s="8"/>
       <c r="D100" s="29" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E100" s="30" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F100" s="21" t="s">
         <v>26</v>
@@ -4450,8 +4799,12 @@
       <c r="J100" s="19"/>
       <c r="K100" s="19"/>
       <c r="L100" s="19"/>
-      <c r="M100" s="19"/>
-      <c r="N100" s="19"/>
+      <c r="M100" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N100" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O100" s="19"/>
     </row>
     <row r="101" spans="1:15" x14ac:dyDescent="0.25">
@@ -4463,10 +4816,10 @@
       </c>
       <c r="C101" s="8"/>
       <c r="D101" s="32" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E101" s="30" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F101" s="21" t="s">
         <v>26</v>
@@ -4479,8 +4832,12 @@
       <c r="J101" s="19"/>
       <c r="K101" s="19"/>
       <c r="L101" s="19"/>
-      <c r="M101" s="19"/>
-      <c r="N101" s="19"/>
+      <c r="M101" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N101" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O101" s="19"/>
     </row>
     <row r="102" spans="1:15" x14ac:dyDescent="0.25">
@@ -4492,10 +4849,10 @@
       </c>
       <c r="C102" s="8"/>
       <c r="D102" s="31" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E102" s="30" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F102" s="21" t="s">
         <v>26</v>
@@ -4508,8 +4865,12 @@
       <c r="J102" s="19"/>
       <c r="K102" s="19"/>
       <c r="L102" s="19"/>
-      <c r="M102" s="19"/>
-      <c r="N102" s="19"/>
+      <c r="M102" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N102" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O102" s="19"/>
     </row>
     <row r="103" spans="1:15" x14ac:dyDescent="0.25">
@@ -4521,10 +4882,10 @@
       </c>
       <c r="C103" s="8"/>
       <c r="D103" s="31" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E103" s="30" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F103" s="21" t="s">
         <v>26</v>
@@ -4537,8 +4898,12 @@
       <c r="J103" s="19"/>
       <c r="K103" s="19"/>
       <c r="L103" s="19"/>
-      <c r="M103" s="19"/>
-      <c r="N103" s="19"/>
+      <c r="M103" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N103" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O103" s="19"/>
     </row>
     <row r="104" spans="1:15" x14ac:dyDescent="0.25">
@@ -4550,10 +4915,10 @@
       </c>
       <c r="C104" s="8"/>
       <c r="D104" s="31" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E104" s="30" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F104" s="21" t="s">
         <v>26</v>
@@ -4566,8 +4931,12 @@
       <c r="J104" s="19"/>
       <c r="K104" s="19"/>
       <c r="L104" s="19"/>
-      <c r="M104" s="19"/>
-      <c r="N104" s="19"/>
+      <c r="M104" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N104" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O104" s="19"/>
     </row>
     <row r="105" spans="1:15" x14ac:dyDescent="0.25">
@@ -4579,10 +4948,10 @@
       </c>
       <c r="C105" s="8"/>
       <c r="D105" s="31" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E105" s="30" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F105" s="21" t="s">
         <v>26</v>
@@ -4595,8 +4964,12 @@
       <c r="J105" s="19"/>
       <c r="K105" s="19"/>
       <c r="L105" s="19"/>
-      <c r="M105" s="19"/>
-      <c r="N105" s="19"/>
+      <c r="M105" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N105" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O105" s="19"/>
     </row>
     <row r="106" spans="1:15" x14ac:dyDescent="0.25">
@@ -4611,10 +4984,10 @@
         <v>43</v>
       </c>
       <c r="E106" s="28" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F106" s="21" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G106" s="22"/>
       <c r="H106" s="19"/>
@@ -4622,8 +4995,12 @@
       <c r="J106" s="19"/>
       <c r="K106" s="19"/>
       <c r="L106" s="19"/>
-      <c r="M106" s="19"/>
-      <c r="N106" s="19"/>
+      <c r="M106" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N106" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O106" s="19"/>
     </row>
     <row r="107" spans="1:15" x14ac:dyDescent="0.25">
@@ -4638,7 +5015,7 @@
         <v>44</v>
       </c>
       <c r="E107" s="28" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F107" s="21" t="s">
         <v>26</v>
@@ -4651,8 +5028,12 @@
       <c r="J107" s="19"/>
       <c r="K107" s="19"/>
       <c r="L107" s="19"/>
-      <c r="M107" s="19"/>
-      <c r="N107" s="19"/>
+      <c r="M107" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N107" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O107" s="19"/>
     </row>
     <row r="108" spans="1:15" x14ac:dyDescent="0.25">
@@ -4667,7 +5048,7 @@
         <v>45</v>
       </c>
       <c r="E108" s="28" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F108" s="21" t="s">
         <v>26</v>
@@ -4680,12 +5061,16 @@
       <c r="J108" s="19"/>
       <c r="K108" s="19"/>
       <c r="L108" s="19"/>
-      <c r="M108" s="19"/>
-      <c r="N108" s="19"/>
+      <c r="M108" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N108" s="12" t="s">
+        <v>247</v>
+      </c>
       <c r="O108" s="19"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L108" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:L108"/>
   <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
WIP add custom component for aligned activities
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/euTaxonomyNonFinancials/EutaxonomyNonFinancials.xlsx
+++ b/dataland-framework-toolbox/inputs/euTaxonomyNonFinancials/EutaxonomyNonFinancials.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d91596\Dataland\dataland-framework-toolbox\inputs\euTaxonomyNonFinancials\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2F24FD6-3C69-4ED3-A374-8F2B1B21123C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13560" yWindow="0" windowWidth="15345" windowHeight="15585" tabRatio="500"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Framework Data Model" sheetId="1" r:id="rId1"/>
@@ -57,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="826" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="248">
   <si>
     <t>Field Identifier</t>
   </si>
@@ -806,7 +807,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1218,8 +1219,8 @@
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2"/>
-    <cellStyle name="Normal 3" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1481,25 +1482,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O108"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" topLeftCell="D98" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H110" sqref="H110"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="3" max="3" width="20.28515625" customWidth="1"/>
-    <col min="4" max="4" width="75.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="44.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="26.28515625" customWidth="1"/>
-    <col min="8" max="14" width="14.28515625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.265625" customWidth="1"/>
+    <col min="4" max="4" width="75.73046875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.59765625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="44.73046875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="26.265625" customWidth="1"/>
+    <col min="8" max="14" width="14.265625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="18.86328125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1546,7 +1547,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A2" s="7">
         <v>0</v>
       </c>
@@ -1577,7 +1578,7 @@
       <c r="N2" s="12"/>
       <c r="O2" s="12"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A3" s="7"/>
       <c r="B3" s="8" t="s">
         <v>12</v>
@@ -1604,7 +1605,7 @@
       <c r="N3" s="12"/>
       <c r="O3" s="12"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A4" s="7">
         <v>1</v>
       </c>
@@ -1635,7 +1636,7 @@
       <c r="N4" s="12"/>
       <c r="O4" s="12"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A5" s="7">
         <v>2</v>
       </c>
@@ -1666,7 +1667,7 @@
       <c r="N5" s="12"/>
       <c r="O5" s="12"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A6" s="7">
         <v>3</v>
       </c>
@@ -1697,7 +1698,7 @@
       <c r="N6" s="12"/>
       <c r="O6" s="12"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A7" s="7">
         <v>4</v>
       </c>
@@ -1726,7 +1727,7 @@
       <c r="N7" s="12"/>
       <c r="O7" s="12"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A8" s="7">
         <v>5</v>
       </c>
@@ -1757,7 +1758,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A9" s="7">
         <v>6</v>
       </c>
@@ -1786,7 +1787,7 @@
       <c r="N9" s="12"/>
       <c r="O9" s="12"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A10" s="7">
         <v>7</v>
       </c>
@@ -1815,7 +1816,7 @@
       <c r="N10" s="12"/>
       <c r="O10" s="12"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" ht="35.65" x14ac:dyDescent="0.45">
       <c r="A11" s="7">
         <v>8</v>
       </c>
@@ -1844,7 +1845,7 @@
       <c r="N11" s="12"/>
       <c r="O11" s="12"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A12" s="7">
         <v>9</v>
       </c>
@@ -1873,7 +1874,7 @@
       <c r="N12" s="12"/>
       <c r="O12" s="12"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A13" s="7">
         <v>10</v>
       </c>
@@ -1900,7 +1901,7 @@
       <c r="N13" s="12"/>
       <c r="O13" s="12"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A14" s="7">
         <v>11</v>
       </c>
@@ -1929,7 +1930,7 @@
       <c r="N14" s="12"/>
       <c r="O14" s="12"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A15" s="18" t="s">
         <v>197</v>
       </c>
@@ -1964,7 +1965,7 @@
       </c>
       <c r="O15" s="12"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A16" s="18" t="s">
         <v>198</v>
       </c>
@@ -1999,7 +2000,7 @@
       </c>
       <c r="O16" s="12"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A17" s="18" t="s">
         <v>46</v>
       </c>
@@ -2034,7 +2035,7 @@
       </c>
       <c r="O17" s="12"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A18" s="18" t="s">
         <v>47</v>
       </c>
@@ -2069,7 +2070,7 @@
       </c>
       <c r="O18" s="12"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A19" s="18" t="s">
         <v>105</v>
       </c>
@@ -2104,7 +2105,7 @@
       </c>
       <c r="O19" s="12"/>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A20" s="18" t="s">
         <v>199</v>
       </c>
@@ -2139,7 +2140,7 @@
       </c>
       <c r="O20" s="12"/>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A21" s="18" t="s">
         <v>200</v>
       </c>
@@ -2172,7 +2173,7 @@
       </c>
       <c r="O21" s="12"/>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A22" s="18" t="s">
         <v>114</v>
       </c>
@@ -2207,7 +2208,7 @@
       </c>
       <c r="O22" s="12"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A23" s="18" t="s">
         <v>201</v>
       </c>
@@ -2242,7 +2243,7 @@
       </c>
       <c r="O23" s="12"/>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A24" s="7">
         <v>17</v>
       </c>
@@ -2275,7 +2276,7 @@
       </c>
       <c r="O24" s="12"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A25" s="18" t="s">
         <v>123</v>
       </c>
@@ -2308,7 +2309,7 @@
       </c>
       <c r="O25" s="12"/>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A26" s="18" t="s">
         <v>124</v>
       </c>
@@ -2341,7 +2342,7 @@
       </c>
       <c r="O26" s="12"/>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A27" s="18" t="s">
         <v>125</v>
       </c>
@@ -2374,7 +2375,7 @@
       </c>
       <c r="O27" s="12"/>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A28" s="18" t="s">
         <v>202</v>
       </c>
@@ -2407,7 +2408,7 @@
       </c>
       <c r="O28" s="12"/>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A29" s="7">
         <v>18</v>
       </c>
@@ -2440,7 +2441,7 @@
       </c>
       <c r="O29" s="12"/>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A30" s="18" t="s">
         <v>134</v>
       </c>
@@ -2473,7 +2474,7 @@
       </c>
       <c r="O30" s="12"/>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A31" s="18" t="s">
         <v>135</v>
       </c>
@@ -2506,7 +2507,7 @@
       </c>
       <c r="O31" s="12"/>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A32" s="18" t="s">
         <v>136</v>
       </c>
@@ -2539,7 +2540,7 @@
       </c>
       <c r="O32" s="12"/>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A33" s="7">
         <v>19</v>
       </c>
@@ -2572,7 +2573,7 @@
       </c>
       <c r="O33" s="12"/>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A34" s="18" t="s">
         <v>145</v>
       </c>
@@ -2605,7 +2606,7 @@
       </c>
       <c r="O34" s="12"/>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A35" s="18" t="s">
         <v>146</v>
       </c>
@@ -2638,7 +2639,7 @@
       </c>
       <c r="O35" s="12"/>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A36" s="18" t="s">
         <v>147</v>
       </c>
@@ -2671,7 +2672,7 @@
       </c>
       <c r="O36" s="12"/>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A37" s="7">
         <v>20</v>
       </c>
@@ -2704,7 +2705,7 @@
       </c>
       <c r="O37" s="12"/>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A38" s="18" t="s">
         <v>203</v>
       </c>
@@ -2737,7 +2738,7 @@
       </c>
       <c r="O38" s="12"/>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A39" s="18" t="s">
         <v>204</v>
       </c>
@@ -2770,7 +2771,7 @@
       </c>
       <c r="O39" s="12"/>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A40" s="18" t="s">
         <v>205</v>
       </c>
@@ -2803,7 +2804,7 @@
       </c>
       <c r="O40" s="12"/>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A41" s="7">
         <v>21</v>
       </c>
@@ -2836,7 +2837,7 @@
       </c>
       <c r="O41" s="12"/>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A42" s="18" t="s">
         <v>206</v>
       </c>
@@ -2869,7 +2870,7 @@
       </c>
       <c r="O42" s="12"/>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A43" s="18" t="s">
         <v>207</v>
       </c>
@@ -2902,7 +2903,7 @@
       </c>
       <c r="O43" s="12"/>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A44" s="18" t="s">
         <v>208</v>
       </c>
@@ -2935,7 +2936,7 @@
       </c>
       <c r="O44" s="12"/>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A45" s="7">
         <v>22</v>
       </c>
@@ -2968,7 +2969,7 @@
       </c>
       <c r="O45" s="12"/>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A46" s="18" t="s">
         <v>209</v>
       </c>
@@ -3001,7 +3002,7 @@
       </c>
       <c r="O46" s="12"/>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A47" s="18" t="s">
         <v>210</v>
       </c>
@@ -3034,7 +3035,7 @@
       </c>
       <c r="O47" s="12"/>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A48" s="18" t="s">
         <v>211</v>
       </c>
@@ -3067,7 +3068,7 @@
       </c>
       <c r="O48" s="12"/>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A49" s="7">
         <v>23</v>
       </c>
@@ -3086,7 +3087,9 @@
       </c>
       <c r="G49" s="22"/>
       <c r="H49" s="12"/>
-      <c r="I49" s="12"/>
+      <c r="I49" s="12" t="s">
+        <v>31</v>
+      </c>
       <c r="J49" s="12"/>
       <c r="K49" s="12"/>
       <c r="L49" s="12"/>
@@ -3098,7 +3101,7 @@
       </c>
       <c r="O49" s="12"/>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A50" s="7">
         <v>24</v>
       </c>
@@ -3131,7 +3134,7 @@
       </c>
       <c r="O50" s="12"/>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A51" s="7">
         <v>25</v>
       </c>
@@ -3164,7 +3167,7 @@
       </c>
       <c r="O51" s="12"/>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A52" s="7">
         <v>26</v>
       </c>
@@ -3197,7 +3200,7 @@
       </c>
       <c r="O52" s="12"/>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A53" s="18" t="s">
         <v>212</v>
       </c>
@@ -3232,7 +3235,7 @@
       </c>
       <c r="O53" s="12"/>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A54" s="18" t="s">
         <v>213</v>
       </c>
@@ -3267,7 +3270,7 @@
       </c>
       <c r="O54" s="12"/>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A55" s="18" t="s">
         <v>48</v>
       </c>
@@ -3302,7 +3305,7 @@
       </c>
       <c r="O55" s="12"/>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A56" s="18" t="s">
         <v>234</v>
       </c>
@@ -3337,7 +3340,7 @@
       </c>
       <c r="O56" s="12"/>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A57" s="18" t="s">
         <v>156</v>
       </c>
@@ -3372,7 +3375,7 @@
       </c>
       <c r="O57" s="12"/>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A58" s="18" t="s">
         <v>214</v>
       </c>
@@ -3407,7 +3410,7 @@
       </c>
       <c r="O58" s="12"/>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A59" s="18" t="s">
         <v>215</v>
       </c>
@@ -3426,7 +3429,9 @@
       </c>
       <c r="G59" s="22"/>
       <c r="H59" s="12"/>
-      <c r="I59" s="12"/>
+      <c r="I59" s="12" t="s">
+        <v>31</v>
+      </c>
       <c r="J59" s="12"/>
       <c r="K59" s="12"/>
       <c r="L59" s="12"/>
@@ -3438,7 +3443,7 @@
       </c>
       <c r="O59" s="12"/>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A60" s="18" t="s">
         <v>164</v>
       </c>
@@ -3473,7 +3478,7 @@
       </c>
       <c r="O60" s="12"/>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A61" s="18" t="s">
         <v>216</v>
       </c>
@@ -3508,7 +3513,7 @@
       </c>
       <c r="O61" s="12"/>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A62" s="7">
         <v>32</v>
       </c>
@@ -3541,7 +3546,7 @@
       </c>
       <c r="O62" s="12"/>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A63" s="18" t="s">
         <v>168</v>
       </c>
@@ -3574,7 +3579,7 @@
       </c>
       <c r="O63" s="12"/>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A64" s="18" t="s">
         <v>169</v>
       </c>
@@ -3607,7 +3612,7 @@
       </c>
       <c r="O64" s="12"/>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A65" s="18" t="s">
         <v>170</v>
       </c>
@@ -3640,7 +3645,7 @@
       </c>
       <c r="O65" s="12"/>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A66" s="18" t="s">
         <v>217</v>
       </c>
@@ -3673,7 +3678,7 @@
       </c>
       <c r="O66" s="12"/>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A67" s="7">
         <v>33</v>
       </c>
@@ -3706,7 +3711,7 @@
       </c>
       <c r="O67" s="12"/>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A68" s="18" t="s">
         <v>180</v>
       </c>
@@ -3739,7 +3744,7 @@
       </c>
       <c r="O68" s="12"/>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A69" s="18" t="s">
         <v>181</v>
       </c>
@@ -3772,7 +3777,7 @@
       </c>
       <c r="O69" s="12"/>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A70" s="18" t="s">
         <v>182</v>
       </c>
@@ -3805,7 +3810,7 @@
       </c>
       <c r="O70" s="12"/>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A71" s="7">
         <v>34</v>
       </c>
@@ -3838,7 +3843,7 @@
       </c>
       <c r="O71" s="12"/>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A72" s="18" t="s">
         <v>183</v>
       </c>
@@ -3871,7 +3876,7 @@
       </c>
       <c r="O72" s="12"/>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A73" s="18" t="s">
         <v>184</v>
       </c>
@@ -3904,7 +3909,7 @@
       </c>
       <c r="O73" s="12"/>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A74" s="18" t="s">
         <v>185</v>
       </c>
@@ -3937,7 +3942,7 @@
       </c>
       <c r="O74" s="12"/>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A75" s="7">
         <v>35</v>
       </c>
@@ -3970,7 +3975,7 @@
       </c>
       <c r="O75" s="12"/>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A76" s="18" t="s">
         <v>218</v>
       </c>
@@ -4003,7 +4008,7 @@
       </c>
       <c r="O76" s="12"/>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A77" s="18" t="s">
         <v>219</v>
       </c>
@@ -4036,7 +4041,7 @@
       </c>
       <c r="O77" s="12"/>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A78" s="18" t="s">
         <v>220</v>
       </c>
@@ -4069,7 +4074,7 @@
       </c>
       <c r="O78" s="12"/>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A79" s="7">
         <v>36</v>
       </c>
@@ -4102,7 +4107,7 @@
       </c>
       <c r="O79" s="12"/>
     </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A80" s="18" t="s">
         <v>221</v>
       </c>
@@ -4135,7 +4140,7 @@
       </c>
       <c r="O80" s="12"/>
     </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A81" s="18" t="s">
         <v>222</v>
       </c>
@@ -4168,7 +4173,7 @@
       </c>
       <c r="O81" s="12"/>
     </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A82" s="18" t="s">
         <v>223</v>
       </c>
@@ -4201,7 +4206,7 @@
       </c>
       <c r="O82" s="12"/>
     </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A83" s="7">
         <v>37</v>
       </c>
@@ -4234,7 +4239,7 @@
       </c>
       <c r="O83" s="12"/>
     </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A84" s="18" t="s">
         <v>224</v>
       </c>
@@ -4267,7 +4272,7 @@
       </c>
       <c r="O84" s="12"/>
     </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A85" s="18" t="s">
         <v>225</v>
       </c>
@@ -4300,7 +4305,7 @@
       </c>
       <c r="O85" s="12"/>
     </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A86" s="18" t="s">
         <v>226</v>
       </c>
@@ -4333,7 +4338,7 @@
       </c>
       <c r="O86" s="12"/>
     </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A87" s="7">
         <v>38</v>
       </c>
@@ -4352,7 +4357,9 @@
       </c>
       <c r="G87" s="22"/>
       <c r="H87" s="12"/>
-      <c r="I87" s="12"/>
+      <c r="I87" s="12" t="s">
+        <v>31</v>
+      </c>
       <c r="J87" s="12"/>
       <c r="K87" s="12"/>
       <c r="L87" s="12"/>
@@ -4364,7 +4371,7 @@
       </c>
       <c r="O87" s="12"/>
     </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A88" s="7">
         <v>39</v>
       </c>
@@ -4397,7 +4404,7 @@
       </c>
       <c r="O88" s="12"/>
     </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A89" s="7">
         <v>40</v>
       </c>
@@ -4430,7 +4437,7 @@
       </c>
       <c r="O89" s="12"/>
     </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A90" s="7">
         <v>41</v>
       </c>
@@ -4463,7 +4470,7 @@
       </c>
       <c r="O90" s="12"/>
     </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A91" s="18" t="s">
         <v>227</v>
       </c>
@@ -4498,7 +4505,7 @@
       </c>
       <c r="O91" s="12"/>
     </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A92" s="18" t="s">
         <v>228</v>
       </c>
@@ -4533,7 +4540,7 @@
       </c>
       <c r="O92" s="12"/>
     </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A93" s="18" t="s">
         <v>49</v>
       </c>
@@ -4568,7 +4575,7 @@
       </c>
       <c r="O93" s="12"/>
     </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A94" s="18" t="s">
         <v>50</v>
       </c>
@@ -4603,7 +4610,7 @@
       </c>
       <c r="O94" s="12"/>
     </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A95" s="18" t="s">
         <v>229</v>
       </c>
@@ -4638,7 +4645,7 @@
       </c>
       <c r="O95" s="12"/>
     </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A96" s="18" t="s">
         <v>230</v>
       </c>
@@ -4673,7 +4680,7 @@
       </c>
       <c r="O96" s="12"/>
     </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A97" s="18" t="s">
         <v>231</v>
       </c>
@@ -4692,7 +4699,9 @@
       </c>
       <c r="G97" s="22"/>
       <c r="H97" s="12"/>
-      <c r="I97" s="12"/>
+      <c r="I97" s="12" t="s">
+        <v>31</v>
+      </c>
       <c r="J97" s="12"/>
       <c r="K97" s="12"/>
       <c r="L97" s="12"/>
@@ -4704,7 +4713,7 @@
       </c>
       <c r="O97" s="12"/>
     </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A98" s="18" t="s">
         <v>232</v>
       </c>
@@ -4739,7 +4748,7 @@
       </c>
       <c r="O98" s="12"/>
     </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A99" s="18" t="s">
         <v>233</v>
       </c>
@@ -4774,7 +4783,7 @@
       </c>
       <c r="O99" s="12"/>
     </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A100" s="7">
         <v>47</v>
       </c>
@@ -4807,7 +4816,7 @@
       </c>
       <c r="O100" s="19"/>
     </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A101" s="7">
         <v>48</v>
       </c>
@@ -4840,7 +4849,7 @@
       </c>
       <c r="O101" s="19"/>
     </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A102" s="7">
         <v>49</v>
       </c>
@@ -4873,7 +4882,7 @@
       </c>
       <c r="O102" s="19"/>
     </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A103" s="7">
         <v>50</v>
       </c>
@@ -4906,7 +4915,7 @@
       </c>
       <c r="O103" s="19"/>
     </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A104" s="7">
         <v>51</v>
       </c>
@@ -4939,7 +4948,7 @@
       </c>
       <c r="O104" s="19"/>
     </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A105" s="7">
         <v>52</v>
       </c>
@@ -4972,7 +4981,7 @@
       </c>
       <c r="O105" s="19"/>
     </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A106" s="7">
         <v>53</v>
       </c>
@@ -4991,7 +5000,9 @@
       </c>
       <c r="G106" s="22"/>
       <c r="H106" s="19"/>
-      <c r="I106" s="19"/>
+      <c r="I106" s="12" t="s">
+        <v>31</v>
+      </c>
       <c r="J106" s="19"/>
       <c r="K106" s="19"/>
       <c r="L106" s="19"/>
@@ -5003,7 +5014,7 @@
       </c>
       <c r="O106" s="19"/>
     </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A107" s="7">
         <v>54</v>
       </c>
@@ -5036,7 +5047,7 @@
       </c>
       <c r="O107" s="19"/>
     </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A108" s="7">
         <v>55</v>
       </c>
@@ -5070,7 +5081,7 @@
       <c r="O108" s="19"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L108"/>
+  <autoFilter ref="A1:L108" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
adapt excel, add aligned activities custom component
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/euTaxonomyNonFinancials/EutaxonomyNonFinancials.xlsx
+++ b/dataland-framework-toolbox/inputs/euTaxonomyNonFinancials/EutaxonomyNonFinancials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d91596\Dataland\dataland-framework-toolbox\inputs\euTaxonomyNonFinancials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2F24FD6-3C69-4ED3-A374-8F2B1B21123C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81A18272-0AEA-45CF-A66E-EF746785C060}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -135,9 +135,6 @@
     <t>Yes/No</t>
   </si>
   <si>
-    <t>Number Of Employees</t>
-  </si>
-  <si>
     <t>Percentage</t>
   </si>
   <si>
@@ -802,6 +799,9 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>Allowed Range: [0, INF]</t>
   </si>
 </sst>
 </file>
@@ -1485,15 +1485,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D98" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H110" sqref="H110"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="3" max="3" width="20.265625" customWidth="1"/>
     <col min="4" max="4" width="75.73046875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.59765625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="255.59765625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="44.73046875" style="1" customWidth="1"/>
     <col min="7" max="7" width="26.265625" customWidth="1"/>
     <col min="8" max="14" width="14.265625" style="1" customWidth="1"/>
@@ -1538,13 +1538,13 @@
         <v>11</v>
       </c>
       <c r="M1" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>238</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.45">
@@ -1565,11 +1565,11 @@
         <v>17</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H2" s="11"/>
       <c r="I2" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J2" s="12"/>
       <c r="K2" s="12"/>
@@ -1588,7 +1588,7 @@
         <v>18</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F3" s="10" t="s">
         <v>13</v>
@@ -1596,7 +1596,7 @@
       <c r="G3" s="10"/>
       <c r="H3" s="11"/>
       <c r="I3" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J3" s="12"/>
       <c r="K3" s="12"/>
@@ -1627,7 +1627,7 @@
       </c>
       <c r="H4" s="12"/>
       <c r="I4" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J4" s="11"/>
       <c r="K4" s="11"/>
@@ -1645,10 +1645,10 @@
       </c>
       <c r="C5" s="8"/>
       <c r="D5" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="12" t="s">
         <v>27</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>28</v>
       </c>
       <c r="F5" s="20" t="s">
         <v>24</v>
@@ -1658,7 +1658,7 @@
       </c>
       <c r="H5" s="12"/>
       <c r="I5" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J5" s="12"/>
       <c r="K5" s="12"/>
@@ -1689,7 +1689,7 @@
       </c>
       <c r="H6" s="12"/>
       <c r="I6" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J6" s="12"/>
       <c r="K6" s="12"/>
@@ -1707,13 +1707,13 @@
       </c>
       <c r="C7" s="8"/>
       <c r="D7" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F7" s="27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G7" s="26" t="s">
         <v>14</v>
@@ -1736,27 +1736,27 @@
       </c>
       <c r="C8" s="8"/>
       <c r="D8" s="37" t="s">
-        <v>25</v>
+        <v>239</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F8" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="G8" s="22"/>
+        <v>51</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>247</v>
+      </c>
       <c r="H8" s="12"/>
       <c r="I8" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J8" s="12"/>
       <c r="K8" s="12"/>
       <c r="L8" s="12"/>
       <c r="M8" s="12"/>
       <c r="N8" s="12"/>
-      <c r="O8" s="12" t="s">
-        <v>240</v>
-      </c>
+      <c r="O8" s="12"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A9" s="7">
@@ -1767,10 +1767,10 @@
       </c>
       <c r="C9" s="8"/>
       <c r="D9" s="38" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E9" s="34" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F9" s="20" t="s">
         <v>24</v>
@@ -1778,7 +1778,7 @@
       <c r="G9" s="22"/>
       <c r="H9" s="12"/>
       <c r="I9" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J9" s="12"/>
       <c r="K9" s="12"/>
@@ -1796,10 +1796,10 @@
       </c>
       <c r="C10" s="8"/>
       <c r="D10" s="33" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E10" s="35" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F10" s="20" t="s">
         <v>24</v>
@@ -1807,7 +1807,7 @@
       <c r="G10" s="22"/>
       <c r="H10" s="12"/>
       <c r="I10" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J10" s="12"/>
       <c r="K10" s="12"/>
@@ -1816,7 +1816,7 @@
       <c r="N10" s="12"/>
       <c r="O10" s="12"/>
     </row>
-    <row r="11" spans="1:15" ht="35.65" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A11" s="7">
         <v>8</v>
       </c>
@@ -1825,10 +1825,10 @@
       </c>
       <c r="C11" s="8"/>
       <c r="D11" s="38" t="s">
+        <v>193</v>
+      </c>
+      <c r="E11" s="36" t="s">
         <v>194</v>
-      </c>
-      <c r="E11" s="36" t="s">
-        <v>195</v>
       </c>
       <c r="F11" s="20" t="s">
         <v>24</v>
@@ -1836,7 +1836,7 @@
       <c r="G11" s="22"/>
       <c r="H11" s="12"/>
       <c r="I11" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J11" s="12"/>
       <c r="K11" s="12"/>
@@ -1854,10 +1854,10 @@
       </c>
       <c r="C12" s="8"/>
       <c r="D12" s="38" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E12" s="35" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F12" s="20" t="s">
         <v>24</v>
@@ -1865,7 +1865,7 @@
       <c r="G12" s="22"/>
       <c r="H12" s="12"/>
       <c r="I12" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J12" s="12"/>
       <c r="K12" s="12"/>
@@ -1883,11 +1883,11 @@
       </c>
       <c r="C13" s="8"/>
       <c r="D13" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E13" s="12"/>
       <c r="F13" s="20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G13" s="23" t="s">
         <v>14</v>
@@ -1906,22 +1906,22 @@
         <v>11</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C14" s="8"/>
       <c r="D14" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E14" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F14" s="21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G14" s="22"/>
       <c r="H14" s="12"/>
       <c r="I14" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J14" s="12"/>
       <c r="K14" s="12"/>
@@ -1932,314 +1932,314 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A15" s="18" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C15" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D15" s="15" t="s">
-        <v>37</v>
-      </c>
       <c r="E15" s="28" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F15" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G15" s="22"/>
       <c r="H15" s="12"/>
       <c r="I15" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J15" s="12"/>
       <c r="K15" s="12"/>
       <c r="L15" s="12"/>
       <c r="M15" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N15" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O15" s="12"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A16" s="18" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E16" s="28" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F16" s="21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G16" s="22"/>
       <c r="H16" s="12"/>
       <c r="I16" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J16" s="12"/>
       <c r="K16" s="12"/>
       <c r="L16" s="12"/>
       <c r="M16" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N16" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O16" s="12"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A17" s="18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F17" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G17" s="22"/>
       <c r="H17" s="12"/>
       <c r="I17" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J17" s="12"/>
       <c r="K17" s="12"/>
       <c r="L17" s="12"/>
       <c r="M17" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N17" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O17" s="12"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A18" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F18" s="21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G18" s="22"/>
       <c r="H18" s="12"/>
       <c r="I18" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J18" s="12"/>
       <c r="K18" s="12"/>
       <c r="L18" s="12"/>
       <c r="M18" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N18" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O18" s="12"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A19" s="18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E19" s="28" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F19" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G19" s="22"/>
       <c r="H19" s="12"/>
       <c r="I19" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J19" s="12"/>
       <c r="K19" s="12"/>
       <c r="L19" s="12"/>
       <c r="M19" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N19" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O19" s="12"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A20" s="18" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E20" s="28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F20" s="21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G20" s="22"/>
       <c r="H20" s="12"/>
       <c r="I20" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J20" s="12"/>
       <c r="K20" s="12"/>
       <c r="L20" s="12"/>
       <c r="M20" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N20" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O20" s="12"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A21" s="18" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C21" s="8"/>
       <c r="D21" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E21" s="28" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F21" s="21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G21" s="22"/>
       <c r="H21" s="12"/>
       <c r="I21" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J21" s="12"/>
       <c r="K21" s="12"/>
       <c r="L21" s="12"/>
       <c r="M21" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N21" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O21" s="12"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A22" s="18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F22" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G22" s="22"/>
       <c r="H22" s="12"/>
       <c r="I22" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J22" s="12"/>
       <c r="K22" s="12"/>
       <c r="L22" s="12"/>
       <c r="M22" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N22" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O22" s="12"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A23" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F23" s="21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G23" s="22"/>
       <c r="H23" s="12"/>
       <c r="I23" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J23" s="12"/>
       <c r="K23" s="12"/>
       <c r="L23" s="12"/>
       <c r="M23" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N23" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O23" s="12"/>
     </row>
@@ -2248,163 +2248,163 @@
         <v>17</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C24" s="8"/>
       <c r="D24" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="E24" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="E24" s="30" t="s">
-        <v>96</v>
-      </c>
       <c r="F24" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G24" s="22"/>
       <c r="H24" s="12"/>
       <c r="I24" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J24" s="12"/>
       <c r="K24" s="12"/>
       <c r="L24" s="12"/>
       <c r="M24" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N24" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O24" s="12"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A25" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C25" s="8"/>
       <c r="D25" s="29" t="s">
+        <v>96</v>
+      </c>
+      <c r="E25" s="30" t="s">
         <v>97</v>
       </c>
-      <c r="E25" s="30" t="s">
-        <v>98</v>
-      </c>
       <c r="F25" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G25" s="22"/>
       <c r="H25" s="12"/>
       <c r="I25" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J25" s="12"/>
       <c r="K25" s="12"/>
       <c r="L25" s="12"/>
       <c r="M25" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N25" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O25" s="12"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A26" s="18" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C26" s="8"/>
       <c r="D26" s="31" t="s">
+        <v>98</v>
+      </c>
+      <c r="E26" s="30" t="s">
         <v>99</v>
       </c>
-      <c r="E26" s="30" t="s">
-        <v>100</v>
-      </c>
       <c r="F26" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G26" s="22"/>
       <c r="H26" s="12"/>
       <c r="I26" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J26" s="12"/>
       <c r="K26" s="12"/>
       <c r="L26" s="12"/>
       <c r="M26" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N26" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O26" s="12"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A27" s="18" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C27" s="8"/>
       <c r="D27" s="29" t="s">
+        <v>100</v>
+      </c>
+      <c r="E27" s="30" t="s">
         <v>101</v>
       </c>
-      <c r="E27" s="30" t="s">
-        <v>102</v>
-      </c>
       <c r="F27" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G27" s="22"/>
       <c r="H27" s="12"/>
       <c r="I27" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J27" s="12"/>
       <c r="K27" s="12"/>
       <c r="L27" s="12"/>
       <c r="M27" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N27" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O27" s="12"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A28" s="18" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C28" s="8"/>
       <c r="D28" s="29" t="s">
+        <v>102</v>
+      </c>
+      <c r="E28" s="30" t="s">
         <v>103</v>
       </c>
-      <c r="E28" s="30" t="s">
-        <v>104</v>
-      </c>
       <c r="F28" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G28" s="22"/>
       <c r="H28" s="12"/>
       <c r="I28" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J28" s="12"/>
       <c r="K28" s="12"/>
       <c r="L28" s="12"/>
       <c r="M28" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N28" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O28" s="12"/>
     </row>
@@ -2413,130 +2413,130 @@
         <v>18</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C29" s="8"/>
       <c r="D29" s="32" t="s">
+        <v>105</v>
+      </c>
+      <c r="E29" s="30" t="s">
         <v>106</v>
       </c>
-      <c r="E29" s="30" t="s">
-        <v>107</v>
-      </c>
       <c r="F29" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G29" s="22"/>
       <c r="H29" s="12"/>
       <c r="I29" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J29" s="12"/>
       <c r="K29" s="12"/>
       <c r="L29" s="12"/>
       <c r="M29" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N29" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O29" s="12"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A30" s="18" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C30" s="8"/>
       <c r="D30" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="E30" s="30" t="s">
         <v>108</v>
       </c>
-      <c r="E30" s="30" t="s">
-        <v>109</v>
-      </c>
       <c r="F30" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G30" s="22"/>
       <c r="H30" s="12"/>
       <c r="I30" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J30" s="12"/>
       <c r="K30" s="12"/>
       <c r="L30" s="12"/>
       <c r="M30" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N30" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O30" s="12"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A31" s="18" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C31" s="8"/>
       <c r="D31" s="31" t="s">
+        <v>109</v>
+      </c>
+      <c r="E31" s="30" t="s">
         <v>110</v>
       </c>
-      <c r="E31" s="30" t="s">
-        <v>111</v>
-      </c>
       <c r="F31" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G31" s="22"/>
       <c r="H31" s="12"/>
       <c r="I31" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J31" s="12"/>
       <c r="K31" s="12"/>
       <c r="L31" s="12"/>
       <c r="M31" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N31" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O31" s="12"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A32" s="18" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C32" s="8"/>
       <c r="D32" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="E32" s="30" t="s">
         <v>112</v>
       </c>
-      <c r="E32" s="30" t="s">
-        <v>113</v>
-      </c>
       <c r="F32" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G32" s="22"/>
       <c r="H32" s="12"/>
       <c r="I32" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J32" s="12"/>
       <c r="K32" s="12"/>
       <c r="L32" s="12"/>
       <c r="M32" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N32" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O32" s="12"/>
     </row>
@@ -2545,130 +2545,130 @@
         <v>19</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C33" s="8"/>
       <c r="D33" s="31" t="s">
+        <v>114</v>
+      </c>
+      <c r="E33" s="30" t="s">
         <v>115</v>
       </c>
-      <c r="E33" s="30" t="s">
-        <v>116</v>
-      </c>
       <c r="F33" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G33" s="22"/>
       <c r="H33" s="12"/>
       <c r="I33" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J33" s="12"/>
       <c r="K33" s="12"/>
       <c r="L33" s="12"/>
       <c r="M33" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N33" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O33" s="12"/>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A34" s="18" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C34" s="8"/>
       <c r="D34" s="31" t="s">
+        <v>116</v>
+      </c>
+      <c r="E34" s="30" t="s">
         <v>117</v>
       </c>
-      <c r="E34" s="30" t="s">
-        <v>118</v>
-      </c>
       <c r="F34" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G34" s="22"/>
       <c r="H34" s="12"/>
       <c r="I34" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J34" s="12"/>
       <c r="K34" s="12"/>
       <c r="L34" s="12"/>
       <c r="M34" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N34" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O34" s="12"/>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A35" s="18" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C35" s="8"/>
       <c r="D35" s="31" t="s">
+        <v>118</v>
+      </c>
+      <c r="E35" s="30" t="s">
         <v>119</v>
       </c>
-      <c r="E35" s="30" t="s">
-        <v>120</v>
-      </c>
       <c r="F35" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G35" s="22"/>
       <c r="H35" s="12"/>
       <c r="I35" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J35" s="12"/>
       <c r="K35" s="12"/>
       <c r="L35" s="12"/>
       <c r="M35" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N35" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O35" s="12"/>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A36" s="18" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C36" s="8"/>
       <c r="D36" s="31" t="s">
+        <v>120</v>
+      </c>
+      <c r="E36" s="30" t="s">
         <v>121</v>
       </c>
-      <c r="E36" s="30" t="s">
-        <v>122</v>
-      </c>
       <c r="F36" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G36" s="22"/>
       <c r="H36" s="12"/>
       <c r="I36" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J36" s="12"/>
       <c r="K36" s="12"/>
       <c r="L36" s="12"/>
       <c r="M36" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N36" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O36" s="12"/>
     </row>
@@ -2677,130 +2677,130 @@
         <v>20</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C37" s="8"/>
       <c r="D37" s="31" t="s">
+        <v>125</v>
+      </c>
+      <c r="E37" s="30" t="s">
         <v>126</v>
       </c>
-      <c r="E37" s="30" t="s">
-        <v>127</v>
-      </c>
       <c r="F37" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G37" s="22"/>
       <c r="H37" s="12"/>
       <c r="I37" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J37" s="12"/>
       <c r="K37" s="12"/>
       <c r="L37" s="12"/>
       <c r="M37" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N37" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O37" s="12"/>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A38" s="18" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C38" s="8"/>
       <c r="D38" s="31" t="s">
+        <v>127</v>
+      </c>
+      <c r="E38" s="30" t="s">
         <v>128</v>
       </c>
-      <c r="E38" s="30" t="s">
-        <v>129</v>
-      </c>
       <c r="F38" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G38" s="22"/>
       <c r="H38" s="12"/>
       <c r="I38" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J38" s="12"/>
       <c r="K38" s="12"/>
       <c r="L38" s="12"/>
       <c r="M38" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N38" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O38" s="12"/>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A39" s="18" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C39" s="8"/>
       <c r="D39" s="31" t="s">
+        <v>129</v>
+      </c>
+      <c r="E39" s="30" t="s">
         <v>130</v>
       </c>
-      <c r="E39" s="30" t="s">
-        <v>131</v>
-      </c>
       <c r="F39" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G39" s="22"/>
       <c r="H39" s="12"/>
       <c r="I39" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J39" s="12"/>
       <c r="K39" s="12"/>
       <c r="L39" s="12"/>
       <c r="M39" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N39" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O39" s="12"/>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A40" s="18" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C40" s="8"/>
       <c r="D40" s="31" t="s">
+        <v>131</v>
+      </c>
+      <c r="E40" s="30" t="s">
         <v>132</v>
       </c>
-      <c r="E40" s="30" t="s">
-        <v>133</v>
-      </c>
       <c r="F40" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G40" s="22"/>
       <c r="H40" s="12"/>
       <c r="I40" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J40" s="12"/>
       <c r="K40" s="12"/>
       <c r="L40" s="12"/>
       <c r="M40" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N40" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O40" s="12"/>
     </row>
@@ -2809,130 +2809,130 @@
         <v>21</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C41" s="8"/>
       <c r="D41" s="31" t="s">
+        <v>136</v>
+      </c>
+      <c r="E41" s="30" t="s">
         <v>137</v>
       </c>
-      <c r="E41" s="30" t="s">
-        <v>138</v>
-      </c>
       <c r="F41" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G41" s="22"/>
       <c r="H41" s="12"/>
       <c r="I41" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J41" s="12"/>
       <c r="K41" s="12"/>
       <c r="L41" s="12"/>
       <c r="M41" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N41" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O41" s="12"/>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A42" s="18" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C42" s="8"/>
       <c r="D42" s="31" t="s">
+        <v>138</v>
+      </c>
+      <c r="E42" s="30" t="s">
         <v>139</v>
       </c>
-      <c r="E42" s="30" t="s">
-        <v>140</v>
-      </c>
       <c r="F42" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G42" s="22"/>
       <c r="H42" s="12"/>
       <c r="I42" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J42" s="12"/>
       <c r="K42" s="12"/>
       <c r="L42" s="12"/>
       <c r="M42" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N42" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O42" s="12"/>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A43" s="18" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C43" s="8"/>
       <c r="D43" s="31" t="s">
+        <v>140</v>
+      </c>
+      <c r="E43" s="30" t="s">
         <v>141</v>
       </c>
-      <c r="E43" s="30" t="s">
-        <v>142</v>
-      </c>
       <c r="F43" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G43" s="22"/>
       <c r="H43" s="12"/>
       <c r="I43" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J43" s="12"/>
       <c r="K43" s="12"/>
       <c r="L43" s="12"/>
       <c r="M43" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N43" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O43" s="12"/>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A44" s="18" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C44" s="8"/>
       <c r="D44" s="31" t="s">
+        <v>142</v>
+      </c>
+      <c r="E44" s="30" t="s">
         <v>143</v>
       </c>
-      <c r="E44" s="30" t="s">
-        <v>144</v>
-      </c>
       <c r="F44" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G44" s="22"/>
       <c r="H44" s="12"/>
       <c r="I44" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J44" s="12"/>
       <c r="K44" s="12"/>
       <c r="L44" s="12"/>
       <c r="M44" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N44" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O44" s="12"/>
     </row>
@@ -2941,130 +2941,130 @@
         <v>22</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C45" s="8"/>
       <c r="D45" s="31" t="s">
+        <v>147</v>
+      </c>
+      <c r="E45" s="30" t="s">
         <v>148</v>
       </c>
-      <c r="E45" s="30" t="s">
-        <v>149</v>
-      </c>
       <c r="F45" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G45" s="22"/>
       <c r="H45" s="12"/>
       <c r="I45" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J45" s="12"/>
       <c r="K45" s="12"/>
       <c r="L45" s="12"/>
       <c r="M45" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N45" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O45" s="12"/>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A46" s="18" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C46" s="8"/>
       <c r="D46" s="31" t="s">
+        <v>149</v>
+      </c>
+      <c r="E46" s="30" t="s">
         <v>150</v>
       </c>
-      <c r="E46" s="30" t="s">
-        <v>151</v>
-      </c>
       <c r="F46" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G46" s="22"/>
       <c r="H46" s="12"/>
       <c r="I46" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J46" s="12"/>
       <c r="K46" s="12"/>
       <c r="L46" s="12"/>
       <c r="M46" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N46" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O46" s="12"/>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A47" s="18" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C47" s="8"/>
       <c r="D47" s="31" t="s">
+        <v>151</v>
+      </c>
+      <c r="E47" s="30" t="s">
         <v>152</v>
       </c>
-      <c r="E47" s="30" t="s">
-        <v>153</v>
-      </c>
       <c r="F47" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G47" s="22"/>
       <c r="H47" s="12"/>
       <c r="I47" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J47" s="12"/>
       <c r="K47" s="12"/>
       <c r="L47" s="12"/>
       <c r="M47" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N47" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O47" s="12"/>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A48" s="18" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C48" s="8"/>
       <c r="D48" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="E48" s="30" t="s">
         <v>154</v>
       </c>
-      <c r="E48" s="30" t="s">
-        <v>155</v>
-      </c>
       <c r="F48" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G48" s="22"/>
       <c r="H48" s="12"/>
       <c r="I48" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J48" s="12"/>
       <c r="K48" s="12"/>
       <c r="L48" s="12"/>
       <c r="M48" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N48" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O48" s="12"/>
     </row>
@@ -3073,31 +3073,31 @@
         <v>23</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C49" s="8"/>
       <c r="D49" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E49" s="28" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F49" s="21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G49" s="22"/>
       <c r="H49" s="12"/>
       <c r="I49" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J49" s="12"/>
       <c r="K49" s="12"/>
       <c r="L49" s="12"/>
       <c r="M49" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N49" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O49" s="12"/>
     </row>
@@ -3106,31 +3106,31 @@
         <v>24</v>
       </c>
       <c r="B50" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C50" s="16"/>
       <c r="D50" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E50" s="28" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F50" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G50" s="22"/>
       <c r="H50" s="12"/>
       <c r="I50" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J50" s="12"/>
       <c r="K50" s="12"/>
       <c r="L50" s="12"/>
       <c r="M50" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N50" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O50" s="12"/>
     </row>
@@ -3139,31 +3139,31 @@
         <v>25</v>
       </c>
       <c r="B51" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C51" s="16"/>
       <c r="D51" s="17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E51" s="28" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F51" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G51" s="22"/>
       <c r="H51" s="12"/>
       <c r="I51" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J51" s="12"/>
       <c r="K51" s="12"/>
       <c r="L51" s="12"/>
       <c r="M51" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N51" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O51" s="12"/>
     </row>
@@ -3172,344 +3172,344 @@
         <v>26</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C52" s="8"/>
       <c r="D52" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E52" s="28" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F52" s="21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G52" s="22"/>
       <c r="H52" s="12"/>
       <c r="I52" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J52" s="12"/>
       <c r="K52" s="12"/>
       <c r="L52" s="12"/>
       <c r="M52" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N52" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O52" s="12"/>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A53" s="18" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C53" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D53" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D53" s="15" t="s">
-        <v>37</v>
-      </c>
       <c r="E53" s="28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F53" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G53" s="22"/>
       <c r="H53" s="12"/>
       <c r="I53" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J53" s="12"/>
       <c r="K53" s="12"/>
       <c r="L53" s="12"/>
       <c r="M53" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N53" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O53" s="12"/>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A54" s="18" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D54" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E54" s="28" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F54" s="21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G54" s="22"/>
       <c r="H54" s="12"/>
       <c r="I54" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J54" s="12"/>
       <c r="K54" s="12"/>
       <c r="L54" s="12"/>
       <c r="M54" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N54" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O54" s="12"/>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A55" s="18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D55" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E55" s="28" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F55" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G55" s="22"/>
       <c r="H55" s="12"/>
       <c r="I55" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J55" s="12"/>
       <c r="K55" s="12"/>
       <c r="L55" s="12"/>
       <c r="M55" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N55" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O55" s="12"/>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A56" s="18" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D56" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E56" s="28" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F56" s="21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G56" s="22"/>
       <c r="H56" s="12"/>
       <c r="I56" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J56" s="12"/>
       <c r="K56" s="12"/>
       <c r="L56" s="12"/>
       <c r="M56" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N56" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O56" s="12"/>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A57" s="18" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D57" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E57" s="28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F57" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G57" s="22"/>
       <c r="H57" s="12"/>
       <c r="I57" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J57" s="12"/>
       <c r="K57" s="12"/>
       <c r="L57" s="12"/>
       <c r="M57" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N57" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O57" s="12"/>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A58" s="18" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D58" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E58" s="28" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F58" s="21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G58" s="22"/>
       <c r="H58" s="12"/>
       <c r="I58" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J58" s="12"/>
       <c r="K58" s="12"/>
       <c r="L58" s="12"/>
       <c r="M58" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N58" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O58" s="12"/>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A59" s="18" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C59" s="8"/>
       <c r="D59" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E59" s="28" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F59" s="21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G59" s="22"/>
       <c r="H59" s="12"/>
       <c r="I59" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J59" s="12"/>
       <c r="K59" s="12"/>
       <c r="L59" s="12"/>
       <c r="M59" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N59" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O59" s="12"/>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A60" s="18" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D60" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E60" s="28" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F60" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G60" s="22"/>
       <c r="H60" s="12"/>
       <c r="I60" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J60" s="12"/>
       <c r="K60" s="12"/>
       <c r="L60" s="12"/>
       <c r="M60" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N60" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O60" s="12"/>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A61" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D61" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E61" s="28" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F61" s="21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G61" s="22"/>
       <c r="H61" s="12"/>
       <c r="I61" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J61" s="12"/>
       <c r="K61" s="12"/>
       <c r="L61" s="12"/>
       <c r="M61" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N61" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O61" s="12"/>
     </row>
@@ -3518,163 +3518,163 @@
         <v>32</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C62" s="8"/>
       <c r="D62" s="29" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E62" s="30" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F62" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G62" s="22"/>
       <c r="H62" s="12"/>
       <c r="I62" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J62" s="12"/>
       <c r="K62" s="12"/>
       <c r="L62" s="12"/>
       <c r="M62" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N62" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O62" s="12"/>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A63" s="18" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C63" s="8"/>
       <c r="D63" s="29" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E63" s="30" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F63" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G63" s="22"/>
       <c r="H63" s="12"/>
       <c r="I63" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J63" s="12"/>
       <c r="K63" s="12"/>
       <c r="L63" s="12"/>
       <c r="M63" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N63" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O63" s="12"/>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A64" s="18" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B64" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C64" s="8"/>
       <c r="D64" s="31" t="s">
+        <v>98</v>
+      </c>
+      <c r="E64" s="30" t="s">
         <v>99</v>
       </c>
-      <c r="E64" s="30" t="s">
-        <v>100</v>
-      </c>
       <c r="F64" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G64" s="22"/>
       <c r="H64" s="12"/>
       <c r="I64" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J64" s="12"/>
       <c r="K64" s="12"/>
       <c r="L64" s="12"/>
       <c r="M64" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N64" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O64" s="12"/>
     </row>
     <row r="65" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A65" s="18" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C65" s="8"/>
       <c r="D65" s="29" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E65" s="30" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F65" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G65" s="22"/>
       <c r="H65" s="12"/>
       <c r="I65" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J65" s="12"/>
       <c r="K65" s="12"/>
       <c r="L65" s="12"/>
       <c r="M65" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N65" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O65" s="12"/>
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A66" s="18" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B66" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C66" s="8"/>
       <c r="D66" s="29" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E66" s="30" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F66" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G66" s="22"/>
       <c r="H66" s="12"/>
       <c r="I66" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J66" s="12"/>
       <c r="K66" s="12"/>
       <c r="L66" s="12"/>
       <c r="M66" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N66" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O66" s="12"/>
     </row>
@@ -3683,130 +3683,130 @@
         <v>33</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C67" s="8"/>
       <c r="D67" s="32" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E67" s="30" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F67" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G67" s="22"/>
       <c r="H67" s="12"/>
       <c r="I67" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J67" s="12"/>
       <c r="K67" s="12"/>
       <c r="L67" s="12"/>
       <c r="M67" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N67" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O67" s="12"/>
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A68" s="18" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B68" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C68" s="8"/>
       <c r="D68" s="32" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E68" s="30" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F68" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G68" s="22"/>
       <c r="H68" s="12"/>
       <c r="I68" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J68" s="12"/>
       <c r="K68" s="12"/>
       <c r="L68" s="12"/>
       <c r="M68" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N68" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O68" s="12"/>
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A69" s="18" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C69" s="8"/>
       <c r="D69" s="31" t="s">
+        <v>109</v>
+      </c>
+      <c r="E69" s="30" t="s">
         <v>110</v>
       </c>
-      <c r="E69" s="30" t="s">
-        <v>111</v>
-      </c>
       <c r="F69" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G69" s="22"/>
       <c r="H69" s="12"/>
       <c r="I69" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J69" s="12"/>
       <c r="K69" s="12"/>
       <c r="L69" s="12"/>
       <c r="M69" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N69" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O69" s="12"/>
     </row>
     <row r="70" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A70" s="18" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B70" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C70" s="8"/>
       <c r="D70" s="31" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E70" s="30" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F70" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G70" s="22"/>
       <c r="H70" s="12"/>
       <c r="I70" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J70" s="12"/>
       <c r="K70" s="12"/>
       <c r="L70" s="12"/>
       <c r="M70" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N70" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O70" s="12"/>
     </row>
@@ -3815,130 +3815,130 @@
         <v>34</v>
       </c>
       <c r="B71" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C71" s="8"/>
       <c r="D71" s="31" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E71" s="30" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F71" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G71" s="22"/>
       <c r="H71" s="12"/>
       <c r="I71" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J71" s="12"/>
       <c r="K71" s="12"/>
       <c r="L71" s="12"/>
       <c r="M71" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N71" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O71" s="12"/>
     </row>
     <row r="72" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A72" s="18" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B72" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C72" s="8"/>
       <c r="D72" s="31" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E72" s="30" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F72" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G72" s="22"/>
       <c r="H72" s="12"/>
       <c r="I72" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J72" s="12"/>
       <c r="K72" s="12"/>
       <c r="L72" s="12"/>
       <c r="M72" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N72" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O72" s="12"/>
     </row>
     <row r="73" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A73" s="18" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B73" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C73" s="8"/>
       <c r="D73" s="31" t="s">
+        <v>118</v>
+      </c>
+      <c r="E73" s="30" t="s">
         <v>119</v>
       </c>
-      <c r="E73" s="30" t="s">
-        <v>120</v>
-      </c>
       <c r="F73" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G73" s="22"/>
       <c r="H73" s="12"/>
       <c r="I73" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J73" s="12"/>
       <c r="K73" s="12"/>
       <c r="L73" s="12"/>
       <c r="M73" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N73" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O73" s="12"/>
     </row>
     <row r="74" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A74" s="18" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B74" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C74" s="8"/>
       <c r="D74" s="31" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E74" s="30" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F74" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G74" s="22"/>
       <c r="H74" s="12"/>
       <c r="I74" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J74" s="12"/>
       <c r="K74" s="12"/>
       <c r="L74" s="12"/>
       <c r="M74" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N74" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O74" s="12"/>
     </row>
@@ -3947,130 +3947,130 @@
         <v>35</v>
       </c>
       <c r="B75" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C75" s="8"/>
       <c r="D75" s="31" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E75" s="30" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F75" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G75" s="22"/>
       <c r="H75" s="12"/>
       <c r="I75" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J75" s="12"/>
       <c r="K75" s="12"/>
       <c r="L75" s="12"/>
       <c r="M75" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N75" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O75" s="12"/>
     </row>
     <row r="76" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A76" s="18" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B76" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C76" s="8"/>
       <c r="D76" s="31" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E76" s="30" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F76" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G76" s="22"/>
       <c r="H76" s="12"/>
       <c r="I76" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J76" s="12"/>
       <c r="K76" s="12"/>
       <c r="L76" s="12"/>
       <c r="M76" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N76" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O76" s="12"/>
     </row>
     <row r="77" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A77" s="18" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C77" s="8"/>
       <c r="D77" s="31" t="s">
+        <v>129</v>
+      </c>
+      <c r="E77" s="30" t="s">
         <v>130</v>
       </c>
-      <c r="E77" s="30" t="s">
-        <v>131</v>
-      </c>
       <c r="F77" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G77" s="22"/>
       <c r="H77" s="12"/>
       <c r="I77" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J77" s="12"/>
       <c r="K77" s="12"/>
       <c r="L77" s="12"/>
       <c r="M77" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N77" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O77" s="12"/>
     </row>
     <row r="78" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A78" s="18" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B78" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C78" s="8"/>
       <c r="D78" s="31" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E78" s="30" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F78" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G78" s="22"/>
       <c r="H78" s="12"/>
       <c r="I78" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J78" s="12"/>
       <c r="K78" s="12"/>
       <c r="L78" s="12"/>
       <c r="M78" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N78" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O78" s="12"/>
     </row>
@@ -4079,130 +4079,130 @@
         <v>36</v>
       </c>
       <c r="B79" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C79" s="8"/>
       <c r="D79" s="31" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E79" s="30" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F79" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G79" s="22"/>
       <c r="H79" s="12"/>
       <c r="I79" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J79" s="12"/>
       <c r="K79" s="12"/>
       <c r="L79" s="12"/>
       <c r="M79" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N79" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O79" s="12"/>
     </row>
     <row r="80" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A80" s="18" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B80" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C80" s="8"/>
       <c r="D80" s="31" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E80" s="30" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F80" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G80" s="22"/>
       <c r="H80" s="12"/>
       <c r="I80" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J80" s="12"/>
       <c r="K80" s="12"/>
       <c r="L80" s="12"/>
       <c r="M80" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N80" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O80" s="12"/>
     </row>
     <row r="81" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A81" s="18" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B81" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C81" s="8"/>
       <c r="D81" s="31" t="s">
+        <v>140</v>
+      </c>
+      <c r="E81" s="30" t="s">
         <v>141</v>
       </c>
-      <c r="E81" s="30" t="s">
-        <v>142</v>
-      </c>
       <c r="F81" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G81" s="22"/>
       <c r="H81" s="12"/>
       <c r="I81" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J81" s="12"/>
       <c r="K81" s="12"/>
       <c r="L81" s="12"/>
       <c r="M81" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N81" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O81" s="12"/>
     </row>
     <row r="82" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A82" s="18" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B82" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C82" s="8"/>
       <c r="D82" s="31" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E82" s="30" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F82" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G82" s="22"/>
       <c r="H82" s="12"/>
       <c r="I82" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J82" s="12"/>
       <c r="K82" s="12"/>
       <c r="L82" s="12"/>
       <c r="M82" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N82" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O82" s="12"/>
     </row>
@@ -4211,130 +4211,130 @@
         <v>37</v>
       </c>
       <c r="B83" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C83" s="8"/>
       <c r="D83" s="31" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E83" s="30" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F83" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G83" s="22"/>
       <c r="H83" s="12"/>
       <c r="I83" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J83" s="12"/>
       <c r="K83" s="12"/>
       <c r="L83" s="12"/>
       <c r="M83" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N83" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O83" s="12"/>
     </row>
     <row r="84" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A84" s="18" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B84" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C84" s="8"/>
       <c r="D84" s="31" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E84" s="30" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F84" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G84" s="22"/>
       <c r="H84" s="12"/>
       <c r="I84" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J84" s="12"/>
       <c r="K84" s="12"/>
       <c r="L84" s="12"/>
       <c r="M84" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N84" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O84" s="12"/>
     </row>
     <row r="85" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A85" s="18" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B85" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C85" s="8"/>
       <c r="D85" s="31" t="s">
+        <v>151</v>
+      </c>
+      <c r="E85" s="30" t="s">
         <v>152</v>
       </c>
-      <c r="E85" s="30" t="s">
-        <v>153</v>
-      </c>
       <c r="F85" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G85" s="22"/>
       <c r="H85" s="12"/>
       <c r="I85" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J85" s="12"/>
       <c r="K85" s="12"/>
       <c r="L85" s="12"/>
       <c r="M85" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N85" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O85" s="12"/>
     </row>
     <row r="86" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A86" s="18" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B86" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C86" s="8"/>
       <c r="D86" s="31" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E86" s="30" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F86" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G86" s="22"/>
       <c r="H86" s="12"/>
       <c r="I86" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J86" s="12"/>
       <c r="K86" s="12"/>
       <c r="L86" s="12"/>
       <c r="M86" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N86" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O86" s="12"/>
     </row>
@@ -4343,31 +4343,31 @@
         <v>38</v>
       </c>
       <c r="B87" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C87" s="8"/>
       <c r="D87" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E87" s="28" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F87" s="21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G87" s="22"/>
       <c r="H87" s="12"/>
       <c r="I87" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J87" s="12"/>
       <c r="K87" s="12"/>
       <c r="L87" s="12"/>
       <c r="M87" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N87" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O87" s="12"/>
     </row>
@@ -4376,31 +4376,31 @@
         <v>39</v>
       </c>
       <c r="B88" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C88" s="16"/>
       <c r="D88" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E88" s="28" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F88" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G88" s="22"/>
       <c r="H88" s="12"/>
       <c r="I88" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J88" s="12"/>
       <c r="K88" s="12"/>
       <c r="L88" s="12"/>
       <c r="M88" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N88" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O88" s="12"/>
     </row>
@@ -4409,31 +4409,31 @@
         <v>40</v>
       </c>
       <c r="B89" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C89" s="16"/>
       <c r="D89" s="17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E89" s="28" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F89" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G89" s="22"/>
       <c r="H89" s="12"/>
       <c r="I89" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J89" s="12"/>
       <c r="K89" s="12"/>
       <c r="L89" s="12"/>
       <c r="M89" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N89" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O89" s="12"/>
     </row>
@@ -4442,344 +4442,344 @@
         <v>41</v>
       </c>
       <c r="B90" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C90" s="8"/>
       <c r="D90" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E90" s="28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F90" s="21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G90" s="22"/>
       <c r="H90" s="12"/>
       <c r="I90" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J90" s="12"/>
       <c r="K90" s="12"/>
       <c r="L90" s="12"/>
       <c r="M90" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N90" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O90" s="12"/>
     </row>
     <row r="91" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A91" s="18" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B91" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C91" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D91" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D91" s="15" t="s">
-        <v>37</v>
-      </c>
       <c r="E91" s="28" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F91" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G91" s="22"/>
       <c r="H91" s="12"/>
       <c r="I91" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J91" s="12"/>
       <c r="K91" s="12"/>
       <c r="L91" s="12"/>
       <c r="M91" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N91" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O91" s="12"/>
     </row>
     <row r="92" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A92" s="18" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B92" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C92" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D92" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="E92" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="F92" s="21" t="s">
         <v>33</v>
-      </c>
-      <c r="C92" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D92" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="E92" s="28" t="s">
-        <v>75</v>
-      </c>
-      <c r="F92" s="21" t="s">
-        <v>34</v>
       </c>
       <c r="G92" s="22"/>
       <c r="H92" s="12"/>
       <c r="I92" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J92" s="12"/>
       <c r="K92" s="12"/>
       <c r="L92" s="12"/>
       <c r="M92" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N92" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O92" s="12"/>
     </row>
     <row r="93" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A93" s="18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B93" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C93" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D93" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E93" s="28" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F93" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G93" s="22"/>
       <c r="H93" s="12"/>
       <c r="I93" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J93" s="12"/>
       <c r="K93" s="12"/>
       <c r="L93" s="12"/>
       <c r="M93" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N93" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O93" s="12"/>
     </row>
     <row r="94" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A94" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B94" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C94" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D94" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="E94" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="F94" s="21" t="s">
         <v>33</v>
-      </c>
-      <c r="C94" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D94" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="E94" s="28" t="s">
-        <v>76</v>
-      </c>
-      <c r="F94" s="21" t="s">
-        <v>34</v>
       </c>
       <c r="G94" s="22"/>
       <c r="H94" s="12"/>
       <c r="I94" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J94" s="12"/>
       <c r="K94" s="12"/>
       <c r="L94" s="12"/>
       <c r="M94" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N94" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O94" s="12"/>
     </row>
     <row r="95" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A95" s="18" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B95" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C95" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D95" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E95" s="28" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F95" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G95" s="22"/>
       <c r="H95" s="12"/>
       <c r="I95" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J95" s="12"/>
       <c r="K95" s="12"/>
       <c r="L95" s="12"/>
       <c r="M95" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N95" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O95" s="12"/>
     </row>
     <row r="96" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A96" s="18" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B96" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C96" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D96" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="E96" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="F96" s="21" t="s">
         <v>33</v>
-      </c>
-      <c r="C96" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="D96" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="E96" s="28" t="s">
-        <v>77</v>
-      </c>
-      <c r="F96" s="21" t="s">
-        <v>34</v>
       </c>
       <c r="G96" s="22"/>
       <c r="H96" s="12"/>
       <c r="I96" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J96" s="12"/>
       <c r="K96" s="12"/>
       <c r="L96" s="12"/>
       <c r="M96" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N96" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O96" s="12"/>
     </row>
     <row r="97" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A97" s="18" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B97" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C97" s="8"/>
       <c r="D97" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E97" s="28" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F97" s="21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G97" s="22"/>
       <c r="H97" s="12"/>
       <c r="I97" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J97" s="12"/>
       <c r="K97" s="12"/>
       <c r="L97" s="12"/>
       <c r="M97" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N97" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O97" s="12"/>
     </row>
     <row r="98" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A98" s="18" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B98" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C98" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D98" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E98" s="28" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F98" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G98" s="22"/>
       <c r="H98" s="12"/>
       <c r="I98" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J98" s="12"/>
       <c r="K98" s="12"/>
       <c r="L98" s="12"/>
       <c r="M98" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N98" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O98" s="12"/>
     </row>
     <row r="99" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A99" s="18" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B99" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C99" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D99" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="E99" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="F99" s="21" t="s">
         <v>33</v>
-      </c>
-      <c r="C99" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="D99" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="E99" s="28" t="s">
-        <v>78</v>
-      </c>
-      <c r="F99" s="21" t="s">
-        <v>34</v>
       </c>
       <c r="G99" s="22"/>
       <c r="H99" s="12"/>
       <c r="I99" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J99" s="12"/>
       <c r="K99" s="12"/>
       <c r="L99" s="12"/>
       <c r="M99" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N99" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O99" s="12"/>
     </row>
@@ -4788,31 +4788,31 @@
         <v>47</v>
       </c>
       <c r="B100" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C100" s="8"/>
       <c r="D100" s="29" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E100" s="30" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F100" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G100" s="22"/>
       <c r="H100" s="19"/>
       <c r="I100" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J100" s="19"/>
       <c r="K100" s="19"/>
       <c r="L100" s="19"/>
       <c r="M100" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N100" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O100" s="19"/>
     </row>
@@ -4821,31 +4821,31 @@
         <v>48</v>
       </c>
       <c r="B101" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C101" s="8"/>
       <c r="D101" s="32" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E101" s="30" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F101" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G101" s="22"/>
       <c r="H101" s="19"/>
       <c r="I101" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J101" s="19"/>
       <c r="K101" s="19"/>
       <c r="L101" s="19"/>
       <c r="M101" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N101" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O101" s="19"/>
     </row>
@@ -4854,31 +4854,31 @@
         <v>49</v>
       </c>
       <c r="B102" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C102" s="8"/>
       <c r="D102" s="31" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E102" s="30" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F102" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G102" s="22"/>
       <c r="H102" s="19"/>
       <c r="I102" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J102" s="19"/>
       <c r="K102" s="19"/>
       <c r="L102" s="19"/>
       <c r="M102" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N102" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O102" s="19"/>
     </row>
@@ -4887,31 +4887,31 @@
         <v>50</v>
       </c>
       <c r="B103" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C103" s="8"/>
       <c r="D103" s="31" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E103" s="30" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F103" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G103" s="22"/>
       <c r="H103" s="19"/>
       <c r="I103" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J103" s="19"/>
       <c r="K103" s="19"/>
       <c r="L103" s="19"/>
       <c r="M103" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N103" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O103" s="19"/>
     </row>
@@ -4920,31 +4920,31 @@
         <v>51</v>
       </c>
       <c r="B104" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C104" s="8"/>
       <c r="D104" s="31" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E104" s="30" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F104" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G104" s="22"/>
       <c r="H104" s="19"/>
       <c r="I104" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J104" s="19"/>
       <c r="K104" s="19"/>
       <c r="L104" s="19"/>
       <c r="M104" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N104" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O104" s="19"/>
     </row>
@@ -4953,31 +4953,31 @@
         <v>52</v>
       </c>
       <c r="B105" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C105" s="8"/>
       <c r="D105" s="31" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E105" s="30" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F105" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G105" s="22"/>
       <c r="H105" s="19"/>
       <c r="I105" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J105" s="19"/>
       <c r="K105" s="19"/>
       <c r="L105" s="19"/>
       <c r="M105" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N105" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O105" s="19"/>
     </row>
@@ -4986,31 +4986,31 @@
         <v>53</v>
       </c>
       <c r="B106" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C106" s="8"/>
       <c r="D106" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E106" s="28" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F106" s="21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G106" s="22"/>
       <c r="H106" s="19"/>
       <c r="I106" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J106" s="19"/>
       <c r="K106" s="19"/>
       <c r="L106" s="19"/>
       <c r="M106" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N106" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O106" s="19"/>
     </row>
@@ -5019,31 +5019,31 @@
         <v>54</v>
       </c>
       <c r="B107" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C107" s="16"/>
       <c r="D107" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E107" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F107" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G107" s="22"/>
       <c r="H107" s="19"/>
       <c r="I107" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J107" s="19"/>
       <c r="K107" s="19"/>
       <c r="L107" s="19"/>
       <c r="M107" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N107" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O107" s="19"/>
     </row>
@@ -5052,31 +5052,31 @@
         <v>55</v>
       </c>
       <c r="B108" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C108" s="16"/>
       <c r="D108" s="17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E108" s="28" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F108" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G108" s="22"/>
       <c r="H108" s="19"/>
       <c r="I108" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J108" s="19"/>
       <c r="K108" s="19"/>
       <c r="L108" s="19"/>
       <c r="M108" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N108" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O108" s="19"/>
     </row>

</xml_diff>

<commit_message>
DALA-5777: Migrate EU-Taxonomy Non-Financials to DataPoints (#1213)
Migrate EU-Taxonomy Non-Financials to DataPoints

---------

Co-authored-by: Wiebke Luenemann <208935942+WiebkeLuenemann-df@users.noreply.github.com>
Co-authored-by: SiegfriedSobkowiak <71646830+SiegfriedSobkowiak@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/euTaxonomyNonFinancials/EutaxonomyNonFinancials.xlsx
+++ b/dataland-framework-toolbox/inputs/euTaxonomyNonFinancials/EutaxonomyNonFinancials.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dataland\Dataland\dataland-framework-toolbox\inputs\euTaxonomyNonFinancials\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d91596\Dataland\dataland-framework-toolbox\inputs\euTaxonomyNonFinancials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C67B78E9-299A-43AD-B2BD-B46716BA59B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81A18272-0AEA-45CF-A66E-EF746785C060}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Framework Data Model" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="248">
   <si>
     <t>Field Identifier</t>
   </si>
@@ -117,9 +117,6 @@
     <t>Fiscal Year End</t>
   </si>
   <si>
-    <t>The date at which the fiscal year ends.</t>
-  </si>
-  <si>
     <t>Scope Of Entities</t>
   </si>
   <si>
@@ -138,12 +135,6 @@
     <t>Yes/No</t>
   </si>
   <si>
-    <t>Number Of Employees</t>
-  </si>
-  <si>
-    <t>Total number of employees (including temporary workers with assignment duration &gt;6 months)</t>
-  </si>
-  <si>
     <t>Percentage</t>
   </si>
   <si>
@@ -156,9 +147,6 @@
     <t>Assurance</t>
   </si>
   <si>
-    <t>Level of assurance of the EU Taxonomy disclosure (Reasonable Assurance, Limited Assurance, None)</t>
-  </si>
-  <si>
     <t>Revenue</t>
   </si>
   <si>
@@ -246,9 +234,6 @@
     <t>Absolute value and share of the revenue per activity that is not taxonomy-aligned but eligible</t>
   </si>
   <si>
-    <t>Absolute value and share of the revenue that is not part of a plan to meet the DNSH criteria and make substantial contribution to any environmental objective</t>
-  </si>
-  <si>
     <t>Share of the taxonomy-aligned revenue from total aligned revenue that is linked to activities that enable reduction of GHG in other sectors</t>
   </si>
   <si>
@@ -654,9 +639,6 @@
     <t>OECD Guidelines for Multinational Enterprises Compliance Policy</t>
   </si>
   <si>
-    <t>Existence of a policy to monitor compliance with the OECD Guidelines for Multinational Enterprises.</t>
-  </si>
-  <si>
     <t>ILO Core Labour Standards</t>
   </si>
   <si>
@@ -666,12 +648,6 @@
     <t>Human Rights Due Diligence</t>
   </si>
   <si>
-    <t>Existence of due diligence processes to identify, prevent, mitigate and address adverse human rights impacts.</t>
-  </si>
-  <si>
-    <t>Existence of a policy to monitor compliance with the UNGC principles.</t>
-  </si>
-  <si>
     <t>12.1</t>
   </si>
   <si>
@@ -784,6 +760,48 @@
   </si>
   <si>
     <t>28.2</t>
+  </si>
+  <si>
+    <t>The date the fiscal year ends.</t>
+  </si>
+  <si>
+    <t>Level of Assurance of the EU Taxonomy Disclosure (Reasonable Assurance, Limited Assurance, None)</t>
+  </si>
+  <si>
+    <t>Include Category in Type Name</t>
+  </si>
+  <si>
+    <t>Include Sub-Category in Type Name</t>
+  </si>
+  <si>
+    <t>Data Point Type Name Overwrite</t>
+  </si>
+  <si>
+    <t>Number of Employees</t>
+  </si>
+  <si>
+    <t>Existence of a policy to monitor compliance with the UNGC principles or OECD Guidelines for Multinational Enterprises. See Regulation (EU) 2022/1288, Annex I, top (22) and table 1, indicator nr. 11.</t>
+  </si>
+  <si>
+    <t>Total Number of Employees (including temporary workers with assignment duration longer than 6 months)</t>
+  </si>
+  <si>
+    <t>Existence of due diligence processes to identify, prevent, mitigate and address adverse human rights impacts. See Regulation (EU) 2022/1288, Annex I, table 3, indicator nr. 10.</t>
+  </si>
+  <si>
+    <t>Existence of grievance/complaints handling mechanisms to address violations of the UNGC principles or OECD Guidelines for Multinational Enterprises. See Regulation (EU) 2022/1288, Annex I, top (22) and table 1, indicator nr. 11.</t>
+  </si>
+  <si>
+    <t>Absolute value of the revenue that is not part of a plan to meet the DNSH criteria and make substantial contribution to any environmental objective</t>
+  </si>
+  <si>
+    <t>Relative share of the revenue that is not part of a plan to meet the DNSH criteria and make substantial contribution to any environmental objective</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Allowed Range: [0, INF]</t>
   </si>
 </sst>
 </file>
@@ -1201,8 +1219,8 @@
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2" xr:uid="{438AC724-B8E1-4701-895E-04EF1113570C}"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1465,23 +1483,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L108"/>
+  <dimension ref="A1:O108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A56" sqref="A56"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="3" max="3" width="20.26953125" customWidth="1"/>
-    <col min="4" max="4" width="95.1796875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="77.81640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="44.7265625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="26.26953125" customWidth="1"/>
-    <col min="8" max="12" width="14.26953125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.265625" customWidth="1"/>
+    <col min="4" max="4" width="75.73046875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="255.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="44.73046875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="26.265625" customWidth="1"/>
+    <col min="8" max="14" width="14.265625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="18.86328125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1518,8 +1537,17 @@
       <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M1" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A2" s="7">
         <v>0</v>
       </c>
@@ -1537,17 +1565,20 @@
         <v>17</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="H2" s="11"/>
       <c r="I2" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J2" s="12"/>
       <c r="K2" s="12"/>
       <c r="L2" s="12"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M2" s="12"/>
+      <c r="N2" s="12"/>
+      <c r="O2" s="12"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A3" s="7"/>
       <c r="B3" s="8" t="s">
         <v>12</v>
@@ -1557,7 +1588,7 @@
         <v>18</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>19</v>
+        <v>234</v>
       </c>
       <c r="F3" s="10" t="s">
         <v>13</v>
@@ -1565,13 +1596,16 @@
       <c r="G3" s="10"/>
       <c r="H3" s="11"/>
       <c r="I3" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J3" s="12"/>
       <c r="K3" s="12"/>
       <c r="L3" s="12"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M3" s="12"/>
+      <c r="N3" s="12"/>
+      <c r="O3" s="12"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A4" s="7">
         <v>1</v>
       </c>
@@ -1580,26 +1614,29 @@
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="19" t="s">
+      <c r="F4" s="10" t="s">
         <v>21</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>22</v>
       </c>
       <c r="G4" s="10" t="s">
         <v>14</v>
       </c>
       <c r="H4" s="12"/>
       <c r="I4" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J4" s="11"/>
       <c r="K4" s="11"/>
       <c r="L4" s="12"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M4" s="12"/>
+      <c r="N4" s="12"/>
+      <c r="O4" s="12"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A5" s="7">
         <v>2</v>
       </c>
@@ -1608,26 +1645,29 @@
       </c>
       <c r="C5" s="8"/>
       <c r="D5" s="14" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F5" s="20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G5" s="23" t="s">
         <v>14</v>
       </c>
       <c r="H5" s="12"/>
       <c r="I5" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J5" s="12"/>
       <c r="K5" s="12"/>
       <c r="L5" s="12"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M5" s="12"/>
+      <c r="N5" s="12"/>
+      <c r="O5" s="12"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A6" s="7">
         <v>3</v>
       </c>
@@ -1636,26 +1676,29 @@
       </c>
       <c r="C6" s="8"/>
       <c r="D6" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="19" t="s">
+      <c r="F6" s="20" t="s">
         <v>24</v>
-      </c>
-      <c r="F6" s="20" t="s">
-        <v>25</v>
       </c>
       <c r="G6" s="26" t="s">
         <v>14</v>
       </c>
       <c r="H6" s="12"/>
       <c r="I6" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J6" s="12"/>
       <c r="K6" s="12"/>
       <c r="L6" s="12"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M6" s="12"/>
+      <c r="N6" s="12"/>
+      <c r="O6" s="12"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A7" s="7">
         <v>4</v>
       </c>
@@ -1664,13 +1707,13 @@
       </c>
       <c r="C7" s="8"/>
       <c r="D7" s="14" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>32</v>
+        <v>235</v>
       </c>
       <c r="F7" s="27" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G7" s="26" t="s">
         <v>14</v>
@@ -1680,8 +1723,11 @@
       <c r="J7" s="12"/>
       <c r="K7" s="12"/>
       <c r="L7" s="12"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M7" s="12"/>
+      <c r="N7" s="12"/>
+      <c r="O7" s="12"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A8" s="7">
         <v>5</v>
       </c>
@@ -1690,24 +1736,29 @@
       </c>
       <c r="C8" s="8"/>
       <c r="D8" s="37" t="s">
-        <v>26</v>
+        <v>239</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>27</v>
+        <v>241</v>
       </c>
       <c r="F8" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="G8" s="22"/>
+        <v>51</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>247</v>
+      </c>
       <c r="H8" s="12"/>
       <c r="I8" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J8" s="12"/>
       <c r="K8" s="12"/>
       <c r="L8" s="12"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M8" s="12"/>
+      <c r="N8" s="12"/>
+      <c r="O8" s="12"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A9" s="7">
         <v>6</v>
       </c>
@@ -1716,24 +1767,27 @@
       </c>
       <c r="C9" s="8"/>
       <c r="D9" s="38" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="E9" s="34" t="s">
-        <v>203</v>
+        <v>240</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G9" s="22"/>
       <c r="H9" s="12"/>
       <c r="I9" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J9" s="12"/>
       <c r="K9" s="12"/>
       <c r="L9" s="12"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M9" s="12"/>
+      <c r="N9" s="12"/>
+      <c r="O9" s="12"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A10" s="7">
         <v>7</v>
       </c>
@@ -1742,24 +1796,27 @@
       </c>
       <c r="C10" s="8"/>
       <c r="D10" s="33" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="E10" s="35" t="s">
-        <v>198</v>
+        <v>243</v>
       </c>
       <c r="F10" s="20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G10" s="22"/>
       <c r="H10" s="12"/>
       <c r="I10" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J10" s="12"/>
       <c r="K10" s="12"/>
       <c r="L10" s="12"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M10" s="12"/>
+      <c r="N10" s="12"/>
+      <c r="O10" s="12"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A11" s="7">
         <v>8</v>
       </c>
@@ -1768,24 +1825,27 @@
       </c>
       <c r="C11" s="8"/>
       <c r="D11" s="38" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="E11" s="36" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="F11" s="20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G11" s="22"/>
       <c r="H11" s="12"/>
       <c r="I11" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J11" s="12"/>
       <c r="K11" s="12"/>
       <c r="L11" s="12"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M11" s="12"/>
+      <c r="N11" s="12"/>
+      <c r="O11" s="12"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A12" s="7">
         <v>9</v>
       </c>
@@ -1794,24 +1854,27 @@
       </c>
       <c r="C12" s="8"/>
       <c r="D12" s="38" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="E12" s="35" t="s">
-        <v>202</v>
+        <v>242</v>
       </c>
       <c r="F12" s="20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G12" s="22"/>
       <c r="H12" s="12"/>
       <c r="I12" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J12" s="12"/>
       <c r="K12" s="12"/>
       <c r="L12" s="12"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M12" s="12"/>
+      <c r="N12" s="12"/>
+      <c r="O12" s="12"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A13" s="7">
         <v>10</v>
       </c>
@@ -1820,11 +1883,11 @@
       </c>
       <c r="C13" s="8"/>
       <c r="D13" s="14" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E13" s="12"/>
       <c r="F13" s="20" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="G13" s="23" t="s">
         <v>14</v>
@@ -1834,2513 +1897,3191 @@
       <c r="J13" s="12"/>
       <c r="K13" s="12"/>
       <c r="L13" s="12"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M13" s="12"/>
+      <c r="N13" s="12"/>
+      <c r="O13" s="12"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A14" s="7">
         <v>11</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C14" s="8"/>
       <c r="D14" s="15" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E14" s="19" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F14" s="21" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G14" s="22"/>
       <c r="H14" s="12"/>
       <c r="I14" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J14" s="12"/>
       <c r="K14" s="12"/>
       <c r="L14" s="12"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M14" s="12"/>
+      <c r="N14" s="12"/>
+      <c r="O14" s="12"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A15" s="18" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="E15" s="19"/>
+        <v>36</v>
+      </c>
+      <c r="E15" s="28" t="s">
+        <v>245</v>
+      </c>
       <c r="F15" s="21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G15" s="22"/>
       <c r="H15" s="12"/>
       <c r="I15" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J15" s="12"/>
       <c r="K15" s="12"/>
       <c r="L15" s="12"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M15" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N15" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O15" s="12"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A16" s="18" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="B16" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" s="28" t="s">
+        <v>244</v>
+      </c>
+      <c r="F16" s="21" t="s">
         <v>33</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D16" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="E16" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="F16" s="21" t="s">
-        <v>37</v>
       </c>
       <c r="G16" s="22"/>
       <c r="H16" s="12"/>
       <c r="I16" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J16" s="12"/>
       <c r="K16" s="12"/>
       <c r="L16" s="12"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M16" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N16" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O16" s="12"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A17" s="18" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="F17" s="21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G17" s="22"/>
       <c r="H17" s="12"/>
       <c r="I17" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J17" s="12"/>
       <c r="K17" s="12"/>
       <c r="L17" s="12"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M17" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N17" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O17" s="12"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A18" s="18" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B18" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="F18" s="21" t="s">
         <v>33</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="D18" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="E18" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="F18" s="21" t="s">
-        <v>37</v>
       </c>
       <c r="G18" s="22"/>
       <c r="H18" s="12"/>
       <c r="I18" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J18" s="12"/>
       <c r="K18" s="12"/>
       <c r="L18" s="12"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M18" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N18" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O18" s="12"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A19" s="18" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E19" s="28" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F19" s="21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G19" s="22"/>
       <c r="H19" s="12"/>
       <c r="I19" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J19" s="12"/>
       <c r="K19" s="12"/>
       <c r="L19" s="12"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M19" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N19" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O19" s="12"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A20" s="18" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="B20" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="E20" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="F20" s="21" t="s">
         <v>33</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="D20" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="E20" s="28" t="s">
-        <v>84</v>
-      </c>
-      <c r="F20" s="21" t="s">
-        <v>37</v>
       </c>
       <c r="G20" s="22"/>
       <c r="H20" s="12"/>
       <c r="I20" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J20" s="12"/>
       <c r="K20" s="12"/>
       <c r="L20" s="12"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M20" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N20" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O20" s="12"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A21" s="18" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C21" s="8"/>
       <c r="D21" s="15" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E21" s="28" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F21" s="21" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="G21" s="22"/>
       <c r="H21" s="12"/>
-      <c r="I21" s="12"/>
+      <c r="I21" s="12" t="s">
+        <v>30</v>
+      </c>
       <c r="J21" s="12"/>
       <c r="K21" s="12"/>
       <c r="L21" s="12"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M21" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N21" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O21" s="12"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A22" s="18" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="F22" s="21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G22" s="22"/>
       <c r="H22" s="12"/>
       <c r="I22" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J22" s="12"/>
       <c r="K22" s="12"/>
       <c r="L22" s="12"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M22" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N22" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O22" s="12"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A23" s="18" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="B23" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="F23" s="21" t="s">
         <v>33</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="D23" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="E23" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="F23" s="21" t="s">
-        <v>37</v>
       </c>
       <c r="G23" s="22"/>
       <c r="H23" s="12"/>
       <c r="I23" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J23" s="12"/>
       <c r="K23" s="12"/>
       <c r="L23" s="12"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M23" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N23" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O23" s="12"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A24" s="7">
         <v>17</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C24" s="8"/>
       <c r="D24" s="29" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E24" s="30" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F24" s="21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G24" s="22"/>
       <c r="H24" s="12"/>
       <c r="I24" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J24" s="12"/>
       <c r="K24" s="12"/>
       <c r="L24" s="12"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M24" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N24" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O24" s="12"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A25" s="18" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C25" s="8"/>
       <c r="D25" s="29" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="E25" s="30" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="F25" s="21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G25" s="22"/>
       <c r="H25" s="12"/>
       <c r="I25" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J25" s="12"/>
       <c r="K25" s="12"/>
       <c r="L25" s="12"/>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M25" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N25" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O25" s="12"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A26" s="18" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C26" s="8"/>
       <c r="D26" s="31" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="E26" s="30" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="F26" s="21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G26" s="22"/>
       <c r="H26" s="12"/>
       <c r="I26" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J26" s="12"/>
       <c r="K26" s="12"/>
       <c r="L26" s="12"/>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M26" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N26" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O26" s="12"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A27" s="18" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C27" s="8"/>
       <c r="D27" s="29" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E27" s="30" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="F27" s="21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G27" s="22"/>
       <c r="H27" s="12"/>
       <c r="I27" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J27" s="12"/>
       <c r="K27" s="12"/>
       <c r="L27" s="12"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M27" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N27" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O27" s="12"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A28" s="18" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C28" s="8"/>
       <c r="D28" s="29" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E28" s="30" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F28" s="21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G28" s="22"/>
       <c r="H28" s="12"/>
       <c r="I28" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J28" s="12"/>
       <c r="K28" s="12"/>
       <c r="L28" s="12"/>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M28" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N28" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O28" s="12"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A29" s="7">
         <v>18</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C29" s="8"/>
       <c r="D29" s="32" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="E29" s="30" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="F29" s="21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G29" s="22"/>
       <c r="H29" s="12"/>
       <c r="I29" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J29" s="12"/>
       <c r="K29" s="12"/>
       <c r="L29" s="12"/>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M29" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N29" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O29" s="12"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A30" s="18" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C30" s="8"/>
       <c r="D30" s="32" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E30" s="30" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="F30" s="21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G30" s="22"/>
       <c r="H30" s="12"/>
       <c r="I30" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J30" s="12"/>
       <c r="K30" s="12"/>
       <c r="L30" s="12"/>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M30" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N30" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O30" s="12"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A31" s="18" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C31" s="8"/>
       <c r="D31" s="31" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="E31" s="30" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="F31" s="21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G31" s="22"/>
       <c r="H31" s="12"/>
       <c r="I31" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J31" s="12"/>
       <c r="K31" s="12"/>
       <c r="L31" s="12"/>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M31" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N31" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O31" s="12"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A32" s="18" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C32" s="8"/>
       <c r="D32" s="31" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="E32" s="30" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="F32" s="21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G32" s="22"/>
       <c r="H32" s="12"/>
       <c r="I32" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J32" s="12"/>
       <c r="K32" s="12"/>
       <c r="L32" s="12"/>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M32" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N32" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O32" s="12"/>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A33" s="7">
         <v>19</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C33" s="8"/>
       <c r="D33" s="31" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="E33" s="30" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="F33" s="21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G33" s="22"/>
       <c r="H33" s="12"/>
       <c r="I33" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J33" s="12"/>
       <c r="K33" s="12"/>
       <c r="L33" s="12"/>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M33" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N33" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O33" s="12"/>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A34" s="18" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C34" s="8"/>
       <c r="D34" s="31" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="E34" s="30" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="F34" s="21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G34" s="22"/>
       <c r="H34" s="12"/>
       <c r="I34" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J34" s="12"/>
       <c r="K34" s="12"/>
       <c r="L34" s="12"/>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M34" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N34" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O34" s="12"/>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A35" s="18" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C35" s="8"/>
       <c r="D35" s="31" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="E35" s="30" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="F35" s="21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G35" s="22"/>
       <c r="H35" s="12"/>
       <c r="I35" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J35" s="12"/>
       <c r="K35" s="12"/>
       <c r="L35" s="12"/>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M35" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N35" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O35" s="12"/>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A36" s="18" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C36" s="8"/>
       <c r="D36" s="31" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="E36" s="30" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="F36" s="21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G36" s="22"/>
       <c r="H36" s="12"/>
       <c r="I36" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J36" s="12"/>
       <c r="K36" s="12"/>
       <c r="L36" s="12"/>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M36" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N36" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O36" s="12"/>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A37" s="7">
         <v>20</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C37" s="8"/>
       <c r="D37" s="31" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="E37" s="30" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="F37" s="21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G37" s="22"/>
       <c r="H37" s="12"/>
       <c r="I37" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J37" s="12"/>
       <c r="K37" s="12"/>
       <c r="L37" s="12"/>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M37" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N37" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O37" s="12"/>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A38" s="18" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C38" s="8"/>
       <c r="D38" s="31" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="E38" s="30" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="F38" s="21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G38" s="22"/>
       <c r="H38" s="12"/>
       <c r="I38" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J38" s="12"/>
       <c r="K38" s="12"/>
       <c r="L38" s="12"/>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M38" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N38" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O38" s="12"/>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A39" s="18" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C39" s="8"/>
       <c r="D39" s="31" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="E39" s="30" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="F39" s="21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G39" s="22"/>
       <c r="H39" s="12"/>
       <c r="I39" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J39" s="12"/>
       <c r="K39" s="12"/>
       <c r="L39" s="12"/>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M39" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N39" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O39" s="12"/>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A40" s="18" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C40" s="8"/>
       <c r="D40" s="31" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="E40" s="30" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="F40" s="21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G40" s="22"/>
       <c r="H40" s="12"/>
       <c r="I40" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J40" s="12"/>
       <c r="K40" s="12"/>
       <c r="L40" s="12"/>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M40" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N40" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O40" s="12"/>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A41" s="7">
         <v>21</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C41" s="8"/>
       <c r="D41" s="31" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="E41" s="30" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="F41" s="21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G41" s="22"/>
       <c r="H41" s="12"/>
       <c r="I41" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J41" s="12"/>
       <c r="K41" s="12"/>
       <c r="L41" s="12"/>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M41" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N41" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O41" s="12"/>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A42" s="18" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C42" s="8"/>
       <c r="D42" s="31" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="E42" s="30" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="F42" s="21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G42" s="22"/>
       <c r="H42" s="12"/>
       <c r="I42" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J42" s="12"/>
       <c r="K42" s="12"/>
       <c r="L42" s="12"/>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M42" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N42" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O42" s="12"/>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A43" s="18" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C43" s="8"/>
       <c r="D43" s="31" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="E43" s="30" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="F43" s="21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G43" s="22"/>
       <c r="H43" s="12"/>
       <c r="I43" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J43" s="12"/>
       <c r="K43" s="12"/>
       <c r="L43" s="12"/>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M43" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N43" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O43" s="12"/>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A44" s="18" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C44" s="8"/>
       <c r="D44" s="31" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="E44" s="30" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="F44" s="21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G44" s="22"/>
       <c r="H44" s="12"/>
       <c r="I44" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J44" s="12"/>
       <c r="K44" s="12"/>
       <c r="L44" s="12"/>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M44" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N44" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O44" s="12"/>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A45" s="7">
         <v>22</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C45" s="8"/>
       <c r="D45" s="31" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="E45" s="30" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="F45" s="21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G45" s="22"/>
       <c r="H45" s="12"/>
       <c r="I45" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J45" s="12"/>
       <c r="K45" s="12"/>
       <c r="L45" s="12"/>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M45" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N45" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O45" s="12"/>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A46" s="18" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C46" s="8"/>
       <c r="D46" s="31" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="E46" s="30" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="F46" s="21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G46" s="22"/>
       <c r="H46" s="12"/>
       <c r="I46" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J46" s="12"/>
       <c r="K46" s="12"/>
       <c r="L46" s="12"/>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M46" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N46" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O46" s="12"/>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A47" s="18" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C47" s="8"/>
       <c r="D47" s="31" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="E47" s="30" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="F47" s="21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G47" s="22"/>
       <c r="H47" s="12"/>
       <c r="I47" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J47" s="12"/>
       <c r="K47" s="12"/>
       <c r="L47" s="12"/>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M47" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N47" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O47" s="12"/>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A48" s="18" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C48" s="8"/>
       <c r="D48" s="31" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="E48" s="30" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="F48" s="21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G48" s="22"/>
       <c r="H48" s="12"/>
       <c r="I48" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J48" s="12"/>
       <c r="K48" s="12"/>
       <c r="L48" s="12"/>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M48" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N48" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O48" s="12"/>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A49" s="7">
         <v>23</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C49" s="8"/>
       <c r="D49" s="15" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E49" s="28" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="F49" s="21" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="G49" s="22"/>
       <c r="H49" s="12"/>
-      <c r="I49" s="12"/>
+      <c r="I49" s="12" t="s">
+        <v>30</v>
+      </c>
       <c r="J49" s="12"/>
       <c r="K49" s="12"/>
       <c r="L49" s="12"/>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M49" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N49" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O49" s="12"/>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A50" s="7">
         <v>24</v>
       </c>
       <c r="B50" s="16" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C50" s="16"/>
       <c r="D50" s="17" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E50" s="28" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="F50" s="21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G50" s="22"/>
       <c r="H50" s="12"/>
       <c r="I50" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J50" s="12"/>
       <c r="K50" s="12"/>
       <c r="L50" s="12"/>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M50" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N50" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O50" s="12"/>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A51" s="7">
         <v>25</v>
       </c>
       <c r="B51" s="16" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C51" s="16"/>
       <c r="D51" s="17" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E51" s="28" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="F51" s="21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G51" s="22"/>
       <c r="H51" s="12"/>
       <c r="I51" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J51" s="12"/>
       <c r="K51" s="12"/>
       <c r="L51" s="12"/>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M51" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N51" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O51" s="12"/>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A52" s="7">
         <v>26</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C52" s="8"/>
       <c r="D52" s="15" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E52" s="28" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F52" s="21" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G52" s="22"/>
       <c r="H52" s="12"/>
       <c r="I52" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J52" s="12"/>
       <c r="K52" s="12"/>
       <c r="L52" s="12"/>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M52" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N52" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O52" s="12"/>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A53" s="18" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="B53" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C53" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C53" s="8" t="s">
-        <v>39</v>
-      </c>
       <c r="D53" s="15" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E53" s="28" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="F53" s="21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G53" s="22"/>
       <c r="H53" s="12"/>
       <c r="I53" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J53" s="12"/>
       <c r="K53" s="12"/>
       <c r="L53" s="12"/>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M53" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N53" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O53" s="12"/>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A54" s="18" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="B54" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C54" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C54" s="8" t="s">
-        <v>39</v>
-      </c>
       <c r="D54" s="15" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E54" s="28" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="F54" s="21" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G54" s="22"/>
       <c r="H54" s="12"/>
       <c r="I54" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J54" s="12"/>
       <c r="K54" s="12"/>
       <c r="L54" s="12"/>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M54" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N54" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O54" s="12"/>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A55" s="18" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D55" s="15" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E55" s="28" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="F55" s="21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G55" s="22"/>
       <c r="H55" s="12"/>
       <c r="I55" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J55" s="12"/>
       <c r="K55" s="12"/>
       <c r="L55" s="12"/>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M55" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N55" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O55" s="12"/>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A56" s="18" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D56" s="15" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E56" s="28" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="F56" s="21" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G56" s="22"/>
       <c r="H56" s="12"/>
       <c r="I56" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J56" s="12"/>
       <c r="K56" s="12"/>
       <c r="L56" s="12"/>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M56" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N56" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O56" s="12"/>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A57" s="18" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D57" s="15" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E57" s="28" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="F57" s="21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G57" s="22"/>
       <c r="H57" s="12"/>
       <c r="I57" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J57" s="12"/>
       <c r="K57" s="12"/>
       <c r="L57" s="12"/>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M57" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N57" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O57" s="12"/>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A58" s="18" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D58" s="15" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E58" s="28" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="F58" s="21" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G58" s="22"/>
       <c r="H58" s="12"/>
       <c r="I58" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J58" s="12"/>
       <c r="K58" s="12"/>
       <c r="L58" s="12"/>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M58" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N58" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O58" s="12"/>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A59" s="18" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C59" s="8"/>
       <c r="D59" s="15" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E59" s="28" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="F59" s="21" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="G59" s="22"/>
       <c r="H59" s="12"/>
-      <c r="I59" s="12"/>
+      <c r="I59" s="12" t="s">
+        <v>30</v>
+      </c>
       <c r="J59" s="12"/>
       <c r="K59" s="12"/>
       <c r="L59" s="12"/>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M59" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N59" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O59" s="12"/>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A60" s="18" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D60" s="15" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E60" s="28" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="F60" s="21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G60" s="22"/>
       <c r="H60" s="12"/>
       <c r="I60" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J60" s="12"/>
       <c r="K60" s="12"/>
       <c r="L60" s="12"/>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M60" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N60" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O60" s="12"/>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A61" s="18" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D61" s="15" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E61" s="28" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F61" s="21" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G61" s="22"/>
       <c r="H61" s="12"/>
       <c r="I61" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J61" s="12"/>
       <c r="K61" s="12"/>
       <c r="L61" s="12"/>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M61" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N61" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O61" s="12"/>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A62" s="7">
         <v>32</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C62" s="8"/>
       <c r="D62" s="29" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E62" s="30" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="F62" s="21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G62" s="22"/>
       <c r="H62" s="12"/>
       <c r="I62" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J62" s="12"/>
       <c r="K62" s="12"/>
       <c r="L62" s="12"/>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M62" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N62" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O62" s="12"/>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A63" s="18" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C63" s="8"/>
       <c r="D63" s="29" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="E63" s="30" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="F63" s="21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G63" s="22"/>
       <c r="H63" s="12"/>
       <c r="I63" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J63" s="12"/>
       <c r="K63" s="12"/>
       <c r="L63" s="12"/>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M63" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N63" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O63" s="12"/>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A64" s="18" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="B64" s="8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C64" s="8"/>
       <c r="D64" s="31" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="E64" s="30" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="F64" s="21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G64" s="22"/>
       <c r="H64" s="12"/>
       <c r="I64" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J64" s="12"/>
       <c r="K64" s="12"/>
       <c r="L64" s="12"/>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M64" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N64" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O64" s="12"/>
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A65" s="18" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C65" s="8"/>
       <c r="D65" s="29" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E65" s="30" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="F65" s="21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G65" s="22"/>
       <c r="H65" s="12"/>
       <c r="I65" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J65" s="12"/>
       <c r="K65" s="12"/>
       <c r="L65" s="12"/>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M65" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N65" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O65" s="12"/>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A66" s="18" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="B66" s="8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C66" s="8"/>
       <c r="D66" s="29" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E66" s="30" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="F66" s="21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G66" s="22"/>
       <c r="H66" s="12"/>
       <c r="I66" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J66" s="12"/>
       <c r="K66" s="12"/>
       <c r="L66" s="12"/>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M66" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N66" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O66" s="12"/>
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A67" s="7">
         <v>33</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C67" s="8"/>
       <c r="D67" s="32" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="E67" s="30" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="F67" s="21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G67" s="22"/>
       <c r="H67" s="12"/>
       <c r="I67" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J67" s="12"/>
       <c r="K67" s="12"/>
       <c r="L67" s="12"/>
-    </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M67" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N67" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O67" s="12"/>
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A68" s="18" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="B68" s="8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C68" s="8"/>
       <c r="D68" s="32" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E68" s="30" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="F68" s="21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G68" s="22"/>
       <c r="H68" s="12"/>
       <c r="I68" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J68" s="12"/>
       <c r="K68" s="12"/>
       <c r="L68" s="12"/>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M68" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N68" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O68" s="12"/>
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A69" s="18" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C69" s="8"/>
       <c r="D69" s="31" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="E69" s="30" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="F69" s="21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G69" s="22"/>
       <c r="H69" s="12"/>
       <c r="I69" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J69" s="12"/>
       <c r="K69" s="12"/>
       <c r="L69" s="12"/>
-    </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M69" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N69" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O69" s="12"/>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A70" s="18" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="B70" s="8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C70" s="8"/>
       <c r="D70" s="31" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="E70" s="30" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="F70" s="21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G70" s="22"/>
       <c r="H70" s="12"/>
       <c r="I70" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J70" s="12"/>
       <c r="K70" s="12"/>
       <c r="L70" s="12"/>
-    </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M70" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N70" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O70" s="12"/>
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A71" s="7">
         <v>34</v>
       </c>
       <c r="B71" s="8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C71" s="8"/>
       <c r="D71" s="31" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="E71" s="30" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="F71" s="21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G71" s="22"/>
       <c r="H71" s="12"/>
       <c r="I71" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J71" s="12"/>
       <c r="K71" s="12"/>
       <c r="L71" s="12"/>
-    </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M71" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N71" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O71" s="12"/>
+    </row>
+    <row r="72" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A72" s="18" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="B72" s="8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C72" s="8"/>
       <c r="D72" s="31" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="E72" s="30" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="F72" s="21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G72" s="22"/>
       <c r="H72" s="12"/>
       <c r="I72" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J72" s="12"/>
       <c r="K72" s="12"/>
       <c r="L72" s="12"/>
-    </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M72" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N72" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O72" s="12"/>
+    </row>
+    <row r="73" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A73" s="18" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="B73" s="8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C73" s="8"/>
       <c r="D73" s="31" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="E73" s="30" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="F73" s="21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G73" s="22"/>
       <c r="H73" s="12"/>
       <c r="I73" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J73" s="12"/>
       <c r="K73" s="12"/>
       <c r="L73" s="12"/>
-    </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M73" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N73" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O73" s="12"/>
+    </row>
+    <row r="74" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A74" s="18" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="B74" s="8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C74" s="8"/>
       <c r="D74" s="31" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="E74" s="30" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="F74" s="21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G74" s="22"/>
       <c r="H74" s="12"/>
       <c r="I74" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J74" s="12"/>
       <c r="K74" s="12"/>
       <c r="L74" s="12"/>
-    </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M74" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N74" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O74" s="12"/>
+    </row>
+    <row r="75" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A75" s="7">
         <v>35</v>
       </c>
       <c r="B75" s="8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C75" s="8"/>
       <c r="D75" s="31" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="E75" s="30" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="F75" s="21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G75" s="22"/>
       <c r="H75" s="12"/>
       <c r="I75" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J75" s="12"/>
       <c r="K75" s="12"/>
       <c r="L75" s="12"/>
-    </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M75" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N75" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O75" s="12"/>
+    </row>
+    <row r="76" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A76" s="18" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="B76" s="8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C76" s="8"/>
       <c r="D76" s="31" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="E76" s="30" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="F76" s="21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G76" s="22"/>
       <c r="H76" s="12"/>
       <c r="I76" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J76" s="12"/>
       <c r="K76" s="12"/>
       <c r="L76" s="12"/>
-    </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M76" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N76" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O76" s="12"/>
+    </row>
+    <row r="77" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A77" s="18" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C77" s="8"/>
       <c r="D77" s="31" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="E77" s="30" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="F77" s="21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G77" s="22"/>
       <c r="H77" s="12"/>
       <c r="I77" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J77" s="12"/>
       <c r="K77" s="12"/>
       <c r="L77" s="12"/>
-    </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M77" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N77" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O77" s="12"/>
+    </row>
+    <row r="78" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A78" s="18" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="B78" s="8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C78" s="8"/>
       <c r="D78" s="31" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="E78" s="30" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="F78" s="21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G78" s="22"/>
       <c r="H78" s="12"/>
       <c r="I78" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J78" s="12"/>
       <c r="K78" s="12"/>
       <c r="L78" s="12"/>
-    </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M78" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N78" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O78" s="12"/>
+    </row>
+    <row r="79" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A79" s="7">
         <v>36</v>
       </c>
       <c r="B79" s="8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C79" s="8"/>
       <c r="D79" s="31" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="E79" s="30" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="F79" s="21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G79" s="22"/>
       <c r="H79" s="12"/>
       <c r="I79" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J79" s="12"/>
       <c r="K79" s="12"/>
       <c r="L79" s="12"/>
-    </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M79" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N79" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O79" s="12"/>
+    </row>
+    <row r="80" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A80" s="18" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="B80" s="8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C80" s="8"/>
       <c r="D80" s="31" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="E80" s="30" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="F80" s="21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G80" s="22"/>
       <c r="H80" s="12"/>
       <c r="I80" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J80" s="12"/>
       <c r="K80" s="12"/>
       <c r="L80" s="12"/>
-    </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M80" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N80" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O80" s="12"/>
+    </row>
+    <row r="81" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A81" s="18" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="B81" s="8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C81" s="8"/>
       <c r="D81" s="31" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="E81" s="30" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="F81" s="21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G81" s="22"/>
       <c r="H81" s="12"/>
       <c r="I81" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J81" s="12"/>
       <c r="K81" s="12"/>
       <c r="L81" s="12"/>
-    </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M81" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N81" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O81" s="12"/>
+    </row>
+    <row r="82" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A82" s="18" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="B82" s="8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C82" s="8"/>
       <c r="D82" s="31" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="E82" s="30" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="F82" s="21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G82" s="22"/>
       <c r="H82" s="12"/>
       <c r="I82" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J82" s="12"/>
       <c r="K82" s="12"/>
       <c r="L82" s="12"/>
-    </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M82" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N82" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O82" s="12"/>
+    </row>
+    <row r="83" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A83" s="7">
         <v>37</v>
       </c>
       <c r="B83" s="8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C83" s="8"/>
       <c r="D83" s="31" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="E83" s="30" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="F83" s="21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G83" s="22"/>
       <c r="H83" s="12"/>
       <c r="I83" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J83" s="12"/>
       <c r="K83" s="12"/>
       <c r="L83" s="12"/>
-    </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M83" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N83" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O83" s="12"/>
+    </row>
+    <row r="84" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A84" s="18" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="B84" s="8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C84" s="8"/>
       <c r="D84" s="31" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="E84" s="30" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="F84" s="21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G84" s="22"/>
       <c r="H84" s="12"/>
       <c r="I84" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J84" s="12"/>
       <c r="K84" s="12"/>
       <c r="L84" s="12"/>
-    </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M84" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N84" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O84" s="12"/>
+    </row>
+    <row r="85" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A85" s="18" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="B85" s="8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C85" s="8"/>
       <c r="D85" s="31" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="E85" s="30" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="F85" s="21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G85" s="22"/>
       <c r="H85" s="12"/>
       <c r="I85" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J85" s="12"/>
       <c r="K85" s="12"/>
       <c r="L85" s="12"/>
-    </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M85" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N85" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O85" s="12"/>
+    </row>
+    <row r="86" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A86" s="18" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="B86" s="8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C86" s="8"/>
       <c r="D86" s="31" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="E86" s="30" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="F86" s="21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G86" s="22"/>
       <c r="H86" s="12"/>
       <c r="I86" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J86" s="12"/>
       <c r="K86" s="12"/>
       <c r="L86" s="12"/>
-    </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M86" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N86" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O86" s="12"/>
+    </row>
+    <row r="87" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A87" s="7">
         <v>38</v>
       </c>
       <c r="B87" s="8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C87" s="8"/>
       <c r="D87" s="15" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E87" s="28" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F87" s="21" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="G87" s="22"/>
       <c r="H87" s="12"/>
-      <c r="I87" s="12"/>
+      <c r="I87" s="12" t="s">
+        <v>30</v>
+      </c>
       <c r="J87" s="12"/>
       <c r="K87" s="12"/>
       <c r="L87" s="12"/>
-    </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M87" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N87" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O87" s="12"/>
+    </row>
+    <row r="88" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A88" s="7">
         <v>39</v>
       </c>
       <c r="B88" s="8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C88" s="16"/>
       <c r="D88" s="17" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E88" s="28" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="F88" s="21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G88" s="22"/>
       <c r="H88" s="12"/>
       <c r="I88" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J88" s="12"/>
       <c r="K88" s="12"/>
       <c r="L88" s="12"/>
-    </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M88" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N88" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O88" s="12"/>
+    </row>
+    <row r="89" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A89" s="7">
         <v>40</v>
       </c>
       <c r="B89" s="8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C89" s="16"/>
       <c r="D89" s="17" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E89" s="28" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="F89" s="21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G89" s="22"/>
       <c r="H89" s="12"/>
       <c r="I89" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J89" s="12"/>
       <c r="K89" s="12"/>
       <c r="L89" s="12"/>
-    </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M89" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N89" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O89" s="12"/>
+    </row>
+    <row r="90" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A90" s="7">
         <v>41</v>
       </c>
       <c r="B90" s="8" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C90" s="8"/>
       <c r="D90" s="15" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E90" s="28" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="F90" s="21" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G90" s="22"/>
       <c r="H90" s="12"/>
       <c r="I90" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J90" s="12"/>
       <c r="K90" s="12"/>
       <c r="L90" s="12"/>
-    </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M90" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N90" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O90" s="12"/>
+    </row>
+    <row r="91" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A91" s="18" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="B91" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C91" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D91" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C91" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D91" s="15" t="s">
-        <v>40</v>
-      </c>
       <c r="E91" s="28" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="F91" s="21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G91" s="22"/>
       <c r="H91" s="12"/>
       <c r="I91" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J91" s="12"/>
       <c r="K91" s="12"/>
       <c r="L91" s="12"/>
-    </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M91" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N91" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O91" s="12"/>
+    </row>
+    <row r="92" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A92" s="18" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="B92" s="8" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C92" s="8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D92" s="15" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E92" s="28" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F92" s="21" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G92" s="22"/>
       <c r="H92" s="12"/>
       <c r="I92" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J92" s="12"/>
       <c r="K92" s="12"/>
       <c r="L92" s="12"/>
-    </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M92" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N92" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O92" s="12"/>
+    </row>
+    <row r="93" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A93" s="18" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B93" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C93" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D93" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C93" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="D93" s="15" t="s">
-        <v>40</v>
-      </c>
       <c r="E93" s="28" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="F93" s="21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G93" s="22"/>
       <c r="H93" s="12"/>
       <c r="I93" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J93" s="12"/>
       <c r="K93" s="12"/>
       <c r="L93" s="12"/>
-    </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M93" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N93" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O93" s="12"/>
+    </row>
+    <row r="94" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A94" s="18" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B94" s="8" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C94" s="8" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D94" s="15" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E94" s="28" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F94" s="21" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G94" s="22"/>
       <c r="H94" s="12"/>
       <c r="I94" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J94" s="12"/>
       <c r="K94" s="12"/>
       <c r="L94" s="12"/>
-    </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M94" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N94" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O94" s="12"/>
+    </row>
+    <row r="95" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A95" s="18" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="B95" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C95" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D95" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C95" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="D95" s="15" t="s">
-        <v>40</v>
-      </c>
       <c r="E95" s="28" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="F95" s="21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G95" s="22"/>
       <c r="H95" s="12"/>
       <c r="I95" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J95" s="12"/>
       <c r="K95" s="12"/>
       <c r="L95" s="12"/>
-    </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M95" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N95" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O95" s="12"/>
+    </row>
+    <row r="96" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A96" s="18" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="B96" s="8" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C96" s="8" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D96" s="15" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E96" s="28" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="F96" s="21" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G96" s="22"/>
       <c r="H96" s="12"/>
       <c r="I96" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J96" s="12"/>
       <c r="K96" s="12"/>
       <c r="L96" s="12"/>
-    </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M96" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N96" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O96" s="12"/>
+    </row>
+    <row r="97" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A97" s="18" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="B97" s="8" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C97" s="8"/>
       <c r="D97" s="15" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E97" s="28" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="F97" s="21" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="G97" s="22"/>
       <c r="H97" s="12"/>
-      <c r="I97" s="12"/>
+      <c r="I97" s="12" t="s">
+        <v>30</v>
+      </c>
       <c r="J97" s="12"/>
       <c r="K97" s="12"/>
       <c r="L97" s="12"/>
-    </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M97" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N97" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O97" s="12"/>
+    </row>
+    <row r="98" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A98" s="18" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="B98" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C98" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D98" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C98" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="D98" s="15" t="s">
-        <v>40</v>
-      </c>
       <c r="E98" s="28" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="F98" s="21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G98" s="22"/>
       <c r="H98" s="12"/>
       <c r="I98" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J98" s="12"/>
       <c r="K98" s="12"/>
       <c r="L98" s="12"/>
-    </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M98" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N98" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O98" s="12"/>
+    </row>
+    <row r="99" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A99" s="18" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="B99" s="8" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C99" s="8" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D99" s="15" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E99" s="28" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F99" s="21" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G99" s="22"/>
       <c r="H99" s="12"/>
       <c r="I99" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J99" s="12"/>
       <c r="K99" s="12"/>
       <c r="L99" s="12"/>
-    </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M99" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N99" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O99" s="12"/>
+    </row>
+    <row r="100" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A100" s="7">
         <v>47</v>
       </c>
       <c r="B100" s="8" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C100" s="8"/>
       <c r="D100" s="29" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="E100" s="30" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="F100" s="21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G100" s="22"/>
       <c r="H100" s="19"/>
       <c r="I100" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J100" s="19"/>
       <c r="K100" s="19"/>
       <c r="L100" s="19"/>
-    </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M100" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N100" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O100" s="19"/>
+    </row>
+    <row r="101" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A101" s="7">
         <v>48</v>
       </c>
       <c r="B101" s="8" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C101" s="8"/>
       <c r="D101" s="32" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E101" s="30" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="F101" s="21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G101" s="22"/>
       <c r="H101" s="19"/>
       <c r="I101" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J101" s="19"/>
       <c r="K101" s="19"/>
       <c r="L101" s="19"/>
-    </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M101" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N101" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O101" s="19"/>
+    </row>
+    <row r="102" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A102" s="7">
         <v>49</v>
       </c>
       <c r="B102" s="8" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C102" s="8"/>
       <c r="D102" s="31" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="E102" s="30" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="F102" s="21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G102" s="22"/>
       <c r="H102" s="19"/>
       <c r="I102" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J102" s="19"/>
       <c r="K102" s="19"/>
       <c r="L102" s="19"/>
-    </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M102" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N102" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O102" s="19"/>
+    </row>
+    <row r="103" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A103" s="7">
         <v>50</v>
       </c>
       <c r="B103" s="8" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C103" s="8"/>
       <c r="D103" s="31" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="E103" s="30" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="F103" s="21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G103" s="22"/>
       <c r="H103" s="19"/>
       <c r="I103" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J103" s="19"/>
       <c r="K103" s="19"/>
       <c r="L103" s="19"/>
-    </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M103" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N103" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O103" s="19"/>
+    </row>
+    <row r="104" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A104" s="7">
         <v>51</v>
       </c>
       <c r="B104" s="8" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C104" s="8"/>
       <c r="D104" s="31" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="E104" s="30" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="F104" s="21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G104" s="22"/>
       <c r="H104" s="19"/>
       <c r="I104" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J104" s="19"/>
       <c r="K104" s="19"/>
       <c r="L104" s="19"/>
-    </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M104" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N104" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O104" s="19"/>
+    </row>
+    <row r="105" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A105" s="7">
         <v>52</v>
       </c>
       <c r="B105" s="8" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C105" s="8"/>
       <c r="D105" s="31" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="E105" s="30" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="F105" s="21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G105" s="22"/>
       <c r="H105" s="19"/>
       <c r="I105" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J105" s="19"/>
       <c r="K105" s="19"/>
       <c r="L105" s="19"/>
-    </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M105" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N105" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O105" s="19"/>
+    </row>
+    <row r="106" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A106" s="7">
         <v>53</v>
       </c>
       <c r="B106" s="8" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C106" s="8"/>
       <c r="D106" s="15" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E106" s="28" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="F106" s="21" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="G106" s="22"/>
       <c r="H106" s="19"/>
-      <c r="I106" s="19"/>
+      <c r="I106" s="12" t="s">
+        <v>30</v>
+      </c>
       <c r="J106" s="19"/>
       <c r="K106" s="19"/>
       <c r="L106" s="19"/>
-    </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M106" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N106" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O106" s="19"/>
+    </row>
+    <row r="107" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A107" s="7">
         <v>54</v>
       </c>
       <c r="B107" s="8" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C107" s="16"/>
       <c r="D107" s="17" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E107" s="28" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="F107" s="21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G107" s="22"/>
       <c r="H107" s="19"/>
       <c r="I107" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J107" s="19"/>
       <c r="K107" s="19"/>
       <c r="L107" s="19"/>
-    </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M107" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N107" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O107" s="19"/>
+    </row>
+    <row r="108" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A108" s="7">
         <v>55</v>
       </c>
       <c r="B108" s="8" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C108" s="16"/>
       <c r="D108" s="17" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E108" s="28" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="F108" s="21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G108" s="22"/>
       <c r="H108" s="19"/>
       <c r="I108" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J108" s="19"/>
       <c r="K108" s="19"/>
       <c r="L108" s="19"/>
+      <c r="M108" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N108" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="O108" s="19"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L108" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:L108" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
update eu non financial tooltips to match sfdr tooltips
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/euTaxonomyNonFinancials/EutaxonomyNonFinancials.xlsx
+++ b/dataland-framework-toolbox/inputs/euTaxonomyNonFinancials/EutaxonomyNonFinancials.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d91596\Dataland\dataland-framework-toolbox\inputs\euTaxonomyNonFinancials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81A18272-0AEA-45CF-A66E-EF746785C060}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22C2C080-4880-461E-9FD9-4D88C39F14B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Framework Data Model" sheetId="1" r:id="rId1"/>
@@ -48,8 +48,19 @@
     <definedName name="IQ_YTD">3000</definedName>
     <definedName name="IQ_YTDMONTH">130000</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -642,9 +653,6 @@
     <t>ILO Core Labour Standards</t>
   </si>
   <si>
-    <t>Abidance by the ILO Core Labour Standards.</t>
-  </si>
-  <si>
     <t>Human Rights Due Diligence</t>
   </si>
   <si>
@@ -780,15 +788,9 @@
     <t>Number of Employees</t>
   </si>
   <si>
-    <t>Existence of a policy to monitor compliance with the UNGC principles or OECD Guidelines for Multinational Enterprises. See Regulation (EU) 2022/1288, Annex I, top (22) and table 1, indicator nr. 11.</t>
-  </si>
-  <si>
     <t>Total Number of Employees (including temporary workers with assignment duration longer than 6 months)</t>
   </si>
   <si>
-    <t>Existence of due diligence processes to identify, prevent, mitigate and address adverse human rights impacts. See Regulation (EU) 2022/1288, Annex I, table 3, indicator nr. 10.</t>
-  </si>
-  <si>
     <t>Existence of grievance/complaints handling mechanisms to address violations of the UNGC principles or OECD Guidelines for Multinational Enterprises. See Regulation (EU) 2022/1288, Annex I, top (22) and table 1, indicator nr. 11.</t>
   </si>
   <si>
@@ -802,6 +804,15 @@
   </si>
   <si>
     <t>Allowed Range: [0, INF]</t>
+  </si>
+  <si>
+    <t>Does the company have a policy to monitor compliance with the UNGC principles or OECD Guidelines for Multinational Enterprises? (See Regulation (EU) 2022/1288, Annex I, top (22) and table 1, indicator nr. 11.) If yes, please share the relevant documents with us.</t>
+  </si>
+  <si>
+    <t>Does the company abide by the ILO Core Labour Standards?</t>
+  </si>
+  <si>
+    <t>Does the company have due diligence processes to identify, prevent, mitigate and address adverse human rights impacts? See Regulation (EU) 2022/1288, Annex I, table 3, indicator nr. 10.</t>
   </si>
 </sst>
 </file>
@@ -1485,19 +1496,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="3" max="3" width="20.265625" customWidth="1"/>
     <col min="4" max="4" width="75.73046875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="255.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="255.59765625" style="1" customWidth="1"/>
     <col min="6" max="6" width="44.73046875" style="1" customWidth="1"/>
     <col min="7" max="7" width="26.265625" customWidth="1"/>
     <col min="8" max="14" width="14.265625" style="1" customWidth="1"/>
     <col min="15" max="15" width="18.86328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.73046875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.45">
@@ -1538,13 +1550,13 @@
         <v>11</v>
       </c>
       <c r="M1" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>237</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.45">
@@ -1588,7 +1600,7 @@
         <v>18</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F3" s="10" t="s">
         <v>13</v>
@@ -1710,7 +1722,7 @@
         <v>28</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F7" s="27" t="s">
         <v>54</v>
@@ -1736,16 +1748,16 @@
       </c>
       <c r="C8" s="8"/>
       <c r="D8" s="37" t="s">
+        <v>238</v>
+      </c>
+      <c r="E8" s="12" t="s">
         <v>239</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>241</v>
       </c>
       <c r="F8" s="20" t="s">
         <v>51</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="H8" s="12"/>
       <c r="I8" s="12" t="s">
@@ -1770,7 +1782,7 @@
         <v>191</v>
       </c>
       <c r="E9" s="34" t="s">
-        <v>240</v>
+        <v>245</v>
       </c>
       <c r="F9" s="20" t="s">
         <v>24</v>
@@ -1799,7 +1811,7 @@
         <v>192</v>
       </c>
       <c r="E10" s="35" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="F10" s="20" t="s">
         <v>24</v>
@@ -1828,7 +1840,7 @@
         <v>193</v>
       </c>
       <c r="E11" s="36" t="s">
-        <v>194</v>
+        <v>246</v>
       </c>
       <c r="F11" s="20" t="s">
         <v>24</v>
@@ -1854,10 +1866,10 @@
       </c>
       <c r="C12" s="8"/>
       <c r="D12" s="38" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E12" s="35" t="s">
-        <v>242</v>
+        <v>247</v>
       </c>
       <c r="F12" s="20" t="s">
         <v>24</v>
@@ -1932,7 +1944,7 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A15" s="18" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B15" s="8" t="s">
         <v>29</v>
@@ -1944,7 +1956,7 @@
         <v>36</v>
       </c>
       <c r="E15" s="28" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="F15" s="21" t="s">
         <v>25</v>
@@ -1958,16 +1970,16 @@
       <c r="K15" s="12"/>
       <c r="L15" s="12"/>
       <c r="M15" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N15" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O15" s="12"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A16" s="18" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>29</v>
@@ -1979,7 +1991,7 @@
         <v>37</v>
       </c>
       <c r="E16" s="28" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="F16" s="21" t="s">
         <v>33</v>
@@ -1993,10 +2005,10 @@
       <c r="K16" s="12"/>
       <c r="L16" s="12"/>
       <c r="M16" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N16" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O16" s="12"/>
     </row>
@@ -2028,10 +2040,10 @@
       <c r="K17" s="12"/>
       <c r="L17" s="12"/>
       <c r="M17" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N17" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O17" s="12"/>
     </row>
@@ -2063,10 +2075,10 @@
       <c r="K18" s="12"/>
       <c r="L18" s="12"/>
       <c r="M18" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N18" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O18" s="12"/>
     </row>
@@ -2098,16 +2110,16 @@
       <c r="K19" s="12"/>
       <c r="L19" s="12"/>
       <c r="M19" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N19" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O19" s="12"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A20" s="18" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B20" s="8" t="s">
         <v>29</v>
@@ -2133,16 +2145,16 @@
       <c r="K20" s="12"/>
       <c r="L20" s="12"/>
       <c r="M20" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N20" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O20" s="12"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A21" s="18" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>29</v>
@@ -2166,10 +2178,10 @@
       <c r="K21" s="12"/>
       <c r="L21" s="12"/>
       <c r="M21" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N21" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O21" s="12"/>
     </row>
@@ -2201,16 +2213,16 @@
       <c r="K22" s="12"/>
       <c r="L22" s="12"/>
       <c r="M22" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N22" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O22" s="12"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A23" s="18" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>29</v>
@@ -2236,10 +2248,10 @@
       <c r="K23" s="12"/>
       <c r="L23" s="12"/>
       <c r="M23" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N23" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O23" s="12"/>
     </row>
@@ -2269,10 +2281,10 @@
       <c r="K24" s="12"/>
       <c r="L24" s="12"/>
       <c r="M24" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N24" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O24" s="12"/>
     </row>
@@ -2302,10 +2314,10 @@
       <c r="K25" s="12"/>
       <c r="L25" s="12"/>
       <c r="M25" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N25" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O25" s="12"/>
     </row>
@@ -2335,10 +2347,10 @@
       <c r="K26" s="12"/>
       <c r="L26" s="12"/>
       <c r="M26" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N26" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O26" s="12"/>
     </row>
@@ -2368,16 +2380,16 @@
       <c r="K27" s="12"/>
       <c r="L27" s="12"/>
       <c r="M27" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N27" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O27" s="12"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A28" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B28" s="8" t="s">
         <v>29</v>
@@ -2401,10 +2413,10 @@
       <c r="K28" s="12"/>
       <c r="L28" s="12"/>
       <c r="M28" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N28" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O28" s="12"/>
     </row>
@@ -2434,10 +2446,10 @@
       <c r="K29" s="12"/>
       <c r="L29" s="12"/>
       <c r="M29" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N29" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O29" s="12"/>
     </row>
@@ -2467,10 +2479,10 @@
       <c r="K30" s="12"/>
       <c r="L30" s="12"/>
       <c r="M30" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N30" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O30" s="12"/>
     </row>
@@ -2500,10 +2512,10 @@
       <c r="K31" s="12"/>
       <c r="L31" s="12"/>
       <c r="M31" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N31" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O31" s="12"/>
     </row>
@@ -2533,10 +2545,10 @@
       <c r="K32" s="12"/>
       <c r="L32" s="12"/>
       <c r="M32" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N32" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O32" s="12"/>
     </row>
@@ -2566,10 +2578,10 @@
       <c r="K33" s="12"/>
       <c r="L33" s="12"/>
       <c r="M33" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N33" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O33" s="12"/>
     </row>
@@ -2599,10 +2611,10 @@
       <c r="K34" s="12"/>
       <c r="L34" s="12"/>
       <c r="M34" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N34" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O34" s="12"/>
     </row>
@@ -2632,10 +2644,10 @@
       <c r="K35" s="12"/>
       <c r="L35" s="12"/>
       <c r="M35" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N35" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O35" s="12"/>
     </row>
@@ -2665,10 +2677,10 @@
       <c r="K36" s="12"/>
       <c r="L36" s="12"/>
       <c r="M36" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N36" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O36" s="12"/>
     </row>
@@ -2698,16 +2710,16 @@
       <c r="K37" s="12"/>
       <c r="L37" s="12"/>
       <c r="M37" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N37" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O37" s="12"/>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A38" s="18" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B38" s="8" t="s">
         <v>29</v>
@@ -2731,16 +2743,16 @@
       <c r="K38" s="12"/>
       <c r="L38" s="12"/>
       <c r="M38" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N38" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O38" s="12"/>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A39" s="18" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B39" s="8" t="s">
         <v>29</v>
@@ -2764,16 +2776,16 @@
       <c r="K39" s="12"/>
       <c r="L39" s="12"/>
       <c r="M39" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N39" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O39" s="12"/>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A40" s="18" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B40" s="8" t="s">
         <v>29</v>
@@ -2797,10 +2809,10 @@
       <c r="K40" s="12"/>
       <c r="L40" s="12"/>
       <c r="M40" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N40" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O40" s="12"/>
     </row>
@@ -2830,16 +2842,16 @@
       <c r="K41" s="12"/>
       <c r="L41" s="12"/>
       <c r="M41" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N41" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O41" s="12"/>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A42" s="18" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B42" s="8" t="s">
         <v>29</v>
@@ -2863,16 +2875,16 @@
       <c r="K42" s="12"/>
       <c r="L42" s="12"/>
       <c r="M42" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N42" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O42" s="12"/>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A43" s="18" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B43" s="8" t="s">
         <v>29</v>
@@ -2896,16 +2908,16 @@
       <c r="K43" s="12"/>
       <c r="L43" s="12"/>
       <c r="M43" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N43" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O43" s="12"/>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A44" s="18" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B44" s="8" t="s">
         <v>29</v>
@@ -2929,10 +2941,10 @@
       <c r="K44" s="12"/>
       <c r="L44" s="12"/>
       <c r="M44" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N44" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O44" s="12"/>
     </row>
@@ -2962,16 +2974,16 @@
       <c r="K45" s="12"/>
       <c r="L45" s="12"/>
       <c r="M45" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N45" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O45" s="12"/>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A46" s="18" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B46" s="8" t="s">
         <v>29</v>
@@ -2995,16 +3007,16 @@
       <c r="K46" s="12"/>
       <c r="L46" s="12"/>
       <c r="M46" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N46" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O46" s="12"/>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A47" s="18" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B47" s="8" t="s">
         <v>29</v>
@@ -3028,16 +3040,16 @@
       <c r="K47" s="12"/>
       <c r="L47" s="12"/>
       <c r="M47" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N47" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O47" s="12"/>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A48" s="18" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B48" s="8" t="s">
         <v>29</v>
@@ -3061,10 +3073,10 @@
       <c r="K48" s="12"/>
       <c r="L48" s="12"/>
       <c r="M48" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N48" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O48" s="12"/>
     </row>
@@ -3094,10 +3106,10 @@
       <c r="K49" s="12"/>
       <c r="L49" s="12"/>
       <c r="M49" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N49" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O49" s="12"/>
     </row>
@@ -3127,10 +3139,10 @@
       <c r="K50" s="12"/>
       <c r="L50" s="12"/>
       <c r="M50" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N50" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O50" s="12"/>
     </row>
@@ -3160,10 +3172,10 @@
       <c r="K51" s="12"/>
       <c r="L51" s="12"/>
       <c r="M51" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N51" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O51" s="12"/>
     </row>
@@ -3193,16 +3205,16 @@
       <c r="K52" s="12"/>
       <c r="L52" s="12"/>
       <c r="M52" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N52" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O52" s="12"/>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A53" s="18" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B53" s="8" t="s">
         <v>31</v>
@@ -3228,16 +3240,16 @@
       <c r="K53" s="12"/>
       <c r="L53" s="12"/>
       <c r="M53" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N53" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O53" s="12"/>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A54" s="18" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B54" s="8" t="s">
         <v>31</v>
@@ -3263,10 +3275,10 @@
       <c r="K54" s="12"/>
       <c r="L54" s="12"/>
       <c r="M54" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N54" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O54" s="12"/>
     </row>
@@ -3298,16 +3310,16 @@
       <c r="K55" s="12"/>
       <c r="L55" s="12"/>
       <c r="M55" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N55" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O55" s="12"/>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A56" s="18" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B56" s="8" t="s">
         <v>31</v>
@@ -3333,10 +3345,10 @@
       <c r="K56" s="12"/>
       <c r="L56" s="12"/>
       <c r="M56" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N56" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O56" s="12"/>
     </row>
@@ -3368,16 +3380,16 @@
       <c r="K57" s="12"/>
       <c r="L57" s="12"/>
       <c r="M57" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N57" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O57" s="12"/>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A58" s="18" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B58" s="8" t="s">
         <v>31</v>
@@ -3403,16 +3415,16 @@
       <c r="K58" s="12"/>
       <c r="L58" s="12"/>
       <c r="M58" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N58" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O58" s="12"/>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A59" s="18" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B59" s="8" t="s">
         <v>31</v>
@@ -3436,10 +3448,10 @@
       <c r="K59" s="12"/>
       <c r="L59" s="12"/>
       <c r="M59" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N59" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O59" s="12"/>
     </row>
@@ -3471,16 +3483,16 @@
       <c r="K60" s="12"/>
       <c r="L60" s="12"/>
       <c r="M60" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N60" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O60" s="12"/>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A61" s="18" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B61" s="8" t="s">
         <v>31</v>
@@ -3506,10 +3518,10 @@
       <c r="K61" s="12"/>
       <c r="L61" s="12"/>
       <c r="M61" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N61" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O61" s="12"/>
     </row>
@@ -3539,10 +3551,10 @@
       <c r="K62" s="12"/>
       <c r="L62" s="12"/>
       <c r="M62" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N62" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O62" s="12"/>
     </row>
@@ -3572,10 +3584,10 @@
       <c r="K63" s="12"/>
       <c r="L63" s="12"/>
       <c r="M63" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N63" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O63" s="12"/>
     </row>
@@ -3605,10 +3617,10 @@
       <c r="K64" s="12"/>
       <c r="L64" s="12"/>
       <c r="M64" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N64" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O64" s="12"/>
     </row>
@@ -3638,16 +3650,16 @@
       <c r="K65" s="12"/>
       <c r="L65" s="12"/>
       <c r="M65" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N65" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O65" s="12"/>
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A66" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B66" s="8" t="s">
         <v>31</v>
@@ -3671,10 +3683,10 @@
       <c r="K66" s="12"/>
       <c r="L66" s="12"/>
       <c r="M66" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N66" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O66" s="12"/>
     </row>
@@ -3704,10 +3716,10 @@
       <c r="K67" s="12"/>
       <c r="L67" s="12"/>
       <c r="M67" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N67" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O67" s="12"/>
     </row>
@@ -3737,10 +3749,10 @@
       <c r="K68" s="12"/>
       <c r="L68" s="12"/>
       <c r="M68" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N68" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O68" s="12"/>
     </row>
@@ -3770,10 +3782,10 @@
       <c r="K69" s="12"/>
       <c r="L69" s="12"/>
       <c r="M69" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N69" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O69" s="12"/>
     </row>
@@ -3803,10 +3815,10 @@
       <c r="K70" s="12"/>
       <c r="L70" s="12"/>
       <c r="M70" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N70" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O70" s="12"/>
     </row>
@@ -3836,10 +3848,10 @@
       <c r="K71" s="12"/>
       <c r="L71" s="12"/>
       <c r="M71" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N71" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O71" s="12"/>
     </row>
@@ -3869,10 +3881,10 @@
       <c r="K72" s="12"/>
       <c r="L72" s="12"/>
       <c r="M72" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N72" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O72" s="12"/>
     </row>
@@ -3902,10 +3914,10 @@
       <c r="K73" s="12"/>
       <c r="L73" s="12"/>
       <c r="M73" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N73" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O73" s="12"/>
     </row>
@@ -3935,10 +3947,10 @@
       <c r="K74" s="12"/>
       <c r="L74" s="12"/>
       <c r="M74" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N74" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O74" s="12"/>
     </row>
@@ -3968,16 +3980,16 @@
       <c r="K75" s="12"/>
       <c r="L75" s="12"/>
       <c r="M75" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N75" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O75" s="12"/>
     </row>
     <row r="76" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A76" s="18" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B76" s="8" t="s">
         <v>31</v>
@@ -4001,16 +4013,16 @@
       <c r="K76" s="12"/>
       <c r="L76" s="12"/>
       <c r="M76" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N76" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O76" s="12"/>
     </row>
     <row r="77" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A77" s="18" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B77" s="8" t="s">
         <v>31</v>
@@ -4034,16 +4046,16 @@
       <c r="K77" s="12"/>
       <c r="L77" s="12"/>
       <c r="M77" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N77" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O77" s="12"/>
     </row>
     <row r="78" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A78" s="18" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B78" s="8" t="s">
         <v>31</v>
@@ -4067,10 +4079,10 @@
       <c r="K78" s="12"/>
       <c r="L78" s="12"/>
       <c r="M78" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N78" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O78" s="12"/>
     </row>
@@ -4100,16 +4112,16 @@
       <c r="K79" s="12"/>
       <c r="L79" s="12"/>
       <c r="M79" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N79" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O79" s="12"/>
     </row>
     <row r="80" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A80" s="18" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B80" s="8" t="s">
         <v>31</v>
@@ -4133,16 +4145,16 @@
       <c r="K80" s="12"/>
       <c r="L80" s="12"/>
       <c r="M80" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N80" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O80" s="12"/>
     </row>
     <row r="81" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A81" s="18" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B81" s="8" t="s">
         <v>31</v>
@@ -4166,16 +4178,16 @@
       <c r="K81" s="12"/>
       <c r="L81" s="12"/>
       <c r="M81" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N81" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O81" s="12"/>
     </row>
     <row r="82" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A82" s="18" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B82" s="8" t="s">
         <v>31</v>
@@ -4199,10 +4211,10 @@
       <c r="K82" s="12"/>
       <c r="L82" s="12"/>
       <c r="M82" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N82" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O82" s="12"/>
     </row>
@@ -4232,16 +4244,16 @@
       <c r="K83" s="12"/>
       <c r="L83" s="12"/>
       <c r="M83" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N83" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O83" s="12"/>
     </row>
     <row r="84" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A84" s="18" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B84" s="8" t="s">
         <v>31</v>
@@ -4265,16 +4277,16 @@
       <c r="K84" s="12"/>
       <c r="L84" s="12"/>
       <c r="M84" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N84" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O84" s="12"/>
     </row>
     <row r="85" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A85" s="18" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B85" s="8" t="s">
         <v>31</v>
@@ -4298,16 +4310,16 @@
       <c r="K85" s="12"/>
       <c r="L85" s="12"/>
       <c r="M85" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N85" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O85" s="12"/>
     </row>
     <row r="86" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A86" s="18" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B86" s="8" t="s">
         <v>31</v>
@@ -4331,10 +4343,10 @@
       <c r="K86" s="12"/>
       <c r="L86" s="12"/>
       <c r="M86" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N86" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O86" s="12"/>
     </row>
@@ -4364,10 +4376,10 @@
       <c r="K87" s="12"/>
       <c r="L87" s="12"/>
       <c r="M87" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N87" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O87" s="12"/>
     </row>
@@ -4397,10 +4409,10 @@
       <c r="K88" s="12"/>
       <c r="L88" s="12"/>
       <c r="M88" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N88" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O88" s="12"/>
     </row>
@@ -4430,10 +4442,10 @@
       <c r="K89" s="12"/>
       <c r="L89" s="12"/>
       <c r="M89" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N89" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O89" s="12"/>
     </row>
@@ -4463,16 +4475,16 @@
       <c r="K90" s="12"/>
       <c r="L90" s="12"/>
       <c r="M90" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N90" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O90" s="12"/>
     </row>
     <row r="91" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A91" s="18" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B91" s="8" t="s">
         <v>32</v>
@@ -4498,16 +4510,16 @@
       <c r="K91" s="12"/>
       <c r="L91" s="12"/>
       <c r="M91" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N91" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O91" s="12"/>
     </row>
     <row r="92" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A92" s="18" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B92" s="8" t="s">
         <v>32</v>
@@ -4533,10 +4545,10 @@
       <c r="K92" s="12"/>
       <c r="L92" s="12"/>
       <c r="M92" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N92" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O92" s="12"/>
     </row>
@@ -4568,10 +4580,10 @@
       <c r="K93" s="12"/>
       <c r="L93" s="12"/>
       <c r="M93" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N93" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O93" s="12"/>
     </row>
@@ -4603,16 +4615,16 @@
       <c r="K94" s="12"/>
       <c r="L94" s="12"/>
       <c r="M94" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N94" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O94" s="12"/>
     </row>
     <row r="95" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A95" s="18" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B95" s="8" t="s">
         <v>32</v>
@@ -4638,16 +4650,16 @@
       <c r="K95" s="12"/>
       <c r="L95" s="12"/>
       <c r="M95" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N95" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O95" s="12"/>
     </row>
     <row r="96" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A96" s="18" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B96" s="8" t="s">
         <v>32</v>
@@ -4673,16 +4685,16 @@
       <c r="K96" s="12"/>
       <c r="L96" s="12"/>
       <c r="M96" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N96" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O96" s="12"/>
     </row>
     <row r="97" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A97" s="18" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B97" s="8" t="s">
         <v>32</v>
@@ -4706,16 +4718,16 @@
       <c r="K97" s="12"/>
       <c r="L97" s="12"/>
       <c r="M97" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N97" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O97" s="12"/>
     </row>
     <row r="98" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A98" s="18" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B98" s="8" t="s">
         <v>32</v>
@@ -4741,16 +4753,16 @@
       <c r="K98" s="12"/>
       <c r="L98" s="12"/>
       <c r="M98" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N98" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O98" s="12"/>
     </row>
     <row r="99" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A99" s="18" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B99" s="8" t="s">
         <v>32</v>
@@ -4776,10 +4788,10 @@
       <c r="K99" s="12"/>
       <c r="L99" s="12"/>
       <c r="M99" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N99" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O99" s="12"/>
     </row>
@@ -4809,10 +4821,10 @@
       <c r="K100" s="19"/>
       <c r="L100" s="19"/>
       <c r="M100" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N100" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O100" s="19"/>
     </row>
@@ -4842,10 +4854,10 @@
       <c r="K101" s="19"/>
       <c r="L101" s="19"/>
       <c r="M101" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N101" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O101" s="19"/>
     </row>
@@ -4875,10 +4887,10 @@
       <c r="K102" s="19"/>
       <c r="L102" s="19"/>
       <c r="M102" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N102" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O102" s="19"/>
     </row>
@@ -4908,10 +4920,10 @@
       <c r="K103" s="19"/>
       <c r="L103" s="19"/>
       <c r="M103" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N103" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O103" s="19"/>
     </row>
@@ -4941,10 +4953,10 @@
       <c r="K104" s="19"/>
       <c r="L104" s="19"/>
       <c r="M104" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N104" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O104" s="19"/>
     </row>
@@ -4974,10 +4986,10 @@
       <c r="K105" s="19"/>
       <c r="L105" s="19"/>
       <c r="M105" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N105" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O105" s="19"/>
     </row>
@@ -5007,10 +5019,10 @@
       <c r="K106" s="19"/>
       <c r="L106" s="19"/>
       <c r="M106" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N106" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O106" s="19"/>
     </row>
@@ -5040,10 +5052,10 @@
       <c r="K107" s="19"/>
       <c r="L107" s="19"/>
       <c r="M107" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N107" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O107" s="19"/>
     </row>
@@ -5073,10 +5085,10 @@
       <c r="K108" s="19"/>
       <c r="L108" s="19"/>
       <c r="M108" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N108" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O108" s="19"/>
     </row>

</xml_diff>

<commit_message>
DALA-5634: Display currency related fields with respect to EUR (#1216)
---------

Co-authored-by: AlexanderBors <137779015+AlexanderBors@users.noreply.github.com>
Co-authored-by: S-Hofmann1 <192322604+SimonHofmann12@users.noreply.github.com>
Co-authored-by: Fabian-dfine <Fabian-dfine@users.noreply.github.com>
Co-authored-by: Wiebke Luenemann <208935942+WiebkeLuenemann-df@users.noreply.github.com>
Co-authored-by: Dennis Groh <173401487+dennis-dfine@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/euTaxonomyNonFinancials/EutaxonomyNonFinancials.xlsx
+++ b/dataland-framework-toolbox/inputs/euTaxonomyNonFinancials/EutaxonomyNonFinancials.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d91596\Dataland\dataland-framework-toolbox\inputs\euTaxonomyNonFinancials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81A18272-0AEA-45CF-A66E-EF746785C060}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22C2C080-4880-461E-9FD9-4D88C39F14B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Framework Data Model" sheetId="1" r:id="rId1"/>
@@ -48,8 +48,19 @@
     <definedName name="IQ_YTD">3000</definedName>
     <definedName name="IQ_YTDMONTH">130000</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -642,9 +653,6 @@
     <t>ILO Core Labour Standards</t>
   </si>
   <si>
-    <t>Abidance by the ILO Core Labour Standards.</t>
-  </si>
-  <si>
     <t>Human Rights Due Diligence</t>
   </si>
   <si>
@@ -780,15 +788,9 @@
     <t>Number of Employees</t>
   </si>
   <si>
-    <t>Existence of a policy to monitor compliance with the UNGC principles or OECD Guidelines for Multinational Enterprises. See Regulation (EU) 2022/1288, Annex I, top (22) and table 1, indicator nr. 11.</t>
-  </si>
-  <si>
     <t>Total Number of Employees (including temporary workers with assignment duration longer than 6 months)</t>
   </si>
   <si>
-    <t>Existence of due diligence processes to identify, prevent, mitigate and address adverse human rights impacts. See Regulation (EU) 2022/1288, Annex I, table 3, indicator nr. 10.</t>
-  </si>
-  <si>
     <t>Existence of grievance/complaints handling mechanisms to address violations of the UNGC principles or OECD Guidelines for Multinational Enterprises. See Regulation (EU) 2022/1288, Annex I, top (22) and table 1, indicator nr. 11.</t>
   </si>
   <si>
@@ -802,6 +804,15 @@
   </si>
   <si>
     <t>Allowed Range: [0, INF]</t>
+  </si>
+  <si>
+    <t>Does the company have a policy to monitor compliance with the UNGC principles or OECD Guidelines for Multinational Enterprises? (See Regulation (EU) 2022/1288, Annex I, top (22) and table 1, indicator nr. 11.) If yes, please share the relevant documents with us.</t>
+  </si>
+  <si>
+    <t>Does the company abide by the ILO Core Labour Standards?</t>
+  </si>
+  <si>
+    <t>Does the company have due diligence processes to identify, prevent, mitigate and address adverse human rights impacts? See Regulation (EU) 2022/1288, Annex I, table 3, indicator nr. 10.</t>
   </si>
 </sst>
 </file>
@@ -1485,19 +1496,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="3" max="3" width="20.265625" customWidth="1"/>
     <col min="4" max="4" width="75.73046875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="255.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="255.59765625" style="1" customWidth="1"/>
     <col min="6" max="6" width="44.73046875" style="1" customWidth="1"/>
     <col min="7" max="7" width="26.265625" customWidth="1"/>
     <col min="8" max="14" width="14.265625" style="1" customWidth="1"/>
     <col min="15" max="15" width="18.86328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.73046875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.45">
@@ -1538,13 +1550,13 @@
         <v>11</v>
       </c>
       <c r="M1" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>237</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.45">
@@ -1588,7 +1600,7 @@
         <v>18</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F3" s="10" t="s">
         <v>13</v>
@@ -1710,7 +1722,7 @@
         <v>28</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F7" s="27" t="s">
         <v>54</v>
@@ -1736,16 +1748,16 @@
       </c>
       <c r="C8" s="8"/>
       <c r="D8" s="37" t="s">
+        <v>238</v>
+      </c>
+      <c r="E8" s="12" t="s">
         <v>239</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>241</v>
       </c>
       <c r="F8" s="20" t="s">
         <v>51</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="H8" s="12"/>
       <c r="I8" s="12" t="s">
@@ -1770,7 +1782,7 @@
         <v>191</v>
       </c>
       <c r="E9" s="34" t="s">
-        <v>240</v>
+        <v>245</v>
       </c>
       <c r="F9" s="20" t="s">
         <v>24</v>
@@ -1799,7 +1811,7 @@
         <v>192</v>
       </c>
       <c r="E10" s="35" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="F10" s="20" t="s">
         <v>24</v>
@@ -1828,7 +1840,7 @@
         <v>193</v>
       </c>
       <c r="E11" s="36" t="s">
-        <v>194</v>
+        <v>246</v>
       </c>
       <c r="F11" s="20" t="s">
         <v>24</v>
@@ -1854,10 +1866,10 @@
       </c>
       <c r="C12" s="8"/>
       <c r="D12" s="38" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E12" s="35" t="s">
-        <v>242</v>
+        <v>247</v>
       </c>
       <c r="F12" s="20" t="s">
         <v>24</v>
@@ -1932,7 +1944,7 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A15" s="18" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B15" s="8" t="s">
         <v>29</v>
@@ -1944,7 +1956,7 @@
         <v>36</v>
       </c>
       <c r="E15" s="28" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="F15" s="21" t="s">
         <v>25</v>
@@ -1958,16 +1970,16 @@
       <c r="K15" s="12"/>
       <c r="L15" s="12"/>
       <c r="M15" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N15" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O15" s="12"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A16" s="18" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>29</v>
@@ -1979,7 +1991,7 @@
         <v>37</v>
       </c>
       <c r="E16" s="28" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="F16" s="21" t="s">
         <v>33</v>
@@ -1993,10 +2005,10 @@
       <c r="K16" s="12"/>
       <c r="L16" s="12"/>
       <c r="M16" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N16" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O16" s="12"/>
     </row>
@@ -2028,10 +2040,10 @@
       <c r="K17" s="12"/>
       <c r="L17" s="12"/>
       <c r="M17" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N17" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O17" s="12"/>
     </row>
@@ -2063,10 +2075,10 @@
       <c r="K18" s="12"/>
       <c r="L18" s="12"/>
       <c r="M18" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N18" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O18" s="12"/>
     </row>
@@ -2098,16 +2110,16 @@
       <c r="K19" s="12"/>
       <c r="L19" s="12"/>
       <c r="M19" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N19" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O19" s="12"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A20" s="18" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B20" s="8" t="s">
         <v>29</v>
@@ -2133,16 +2145,16 @@
       <c r="K20" s="12"/>
       <c r="L20" s="12"/>
       <c r="M20" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N20" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O20" s="12"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A21" s="18" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>29</v>
@@ -2166,10 +2178,10 @@
       <c r="K21" s="12"/>
       <c r="L21" s="12"/>
       <c r="M21" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N21" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O21" s="12"/>
     </row>
@@ -2201,16 +2213,16 @@
       <c r="K22" s="12"/>
       <c r="L22" s="12"/>
       <c r="M22" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N22" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O22" s="12"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A23" s="18" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>29</v>
@@ -2236,10 +2248,10 @@
       <c r="K23" s="12"/>
       <c r="L23" s="12"/>
       <c r="M23" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N23" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O23" s="12"/>
     </row>
@@ -2269,10 +2281,10 @@
       <c r="K24" s="12"/>
       <c r="L24" s="12"/>
       <c r="M24" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N24" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O24" s="12"/>
     </row>
@@ -2302,10 +2314,10 @@
       <c r="K25" s="12"/>
       <c r="L25" s="12"/>
       <c r="M25" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N25" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O25" s="12"/>
     </row>
@@ -2335,10 +2347,10 @@
       <c r="K26" s="12"/>
       <c r="L26" s="12"/>
       <c r="M26" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N26" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O26" s="12"/>
     </row>
@@ -2368,16 +2380,16 @@
       <c r="K27" s="12"/>
       <c r="L27" s="12"/>
       <c r="M27" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N27" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O27" s="12"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A28" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B28" s="8" t="s">
         <v>29</v>
@@ -2401,10 +2413,10 @@
       <c r="K28" s="12"/>
       <c r="L28" s="12"/>
       <c r="M28" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N28" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O28" s="12"/>
     </row>
@@ -2434,10 +2446,10 @@
       <c r="K29" s="12"/>
       <c r="L29" s="12"/>
       <c r="M29" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N29" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O29" s="12"/>
     </row>
@@ -2467,10 +2479,10 @@
       <c r="K30" s="12"/>
       <c r="L30" s="12"/>
       <c r="M30" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N30" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O30" s="12"/>
     </row>
@@ -2500,10 +2512,10 @@
       <c r="K31" s="12"/>
       <c r="L31" s="12"/>
       <c r="M31" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N31" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O31" s="12"/>
     </row>
@@ -2533,10 +2545,10 @@
       <c r="K32" s="12"/>
       <c r="L32" s="12"/>
       <c r="M32" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N32" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O32" s="12"/>
     </row>
@@ -2566,10 +2578,10 @@
       <c r="K33" s="12"/>
       <c r="L33" s="12"/>
       <c r="M33" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N33" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O33" s="12"/>
     </row>
@@ -2599,10 +2611,10 @@
       <c r="K34" s="12"/>
       <c r="L34" s="12"/>
       <c r="M34" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N34" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O34" s="12"/>
     </row>
@@ -2632,10 +2644,10 @@
       <c r="K35" s="12"/>
       <c r="L35" s="12"/>
       <c r="M35" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N35" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O35" s="12"/>
     </row>
@@ -2665,10 +2677,10 @@
       <c r="K36" s="12"/>
       <c r="L36" s="12"/>
       <c r="M36" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N36" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O36" s="12"/>
     </row>
@@ -2698,16 +2710,16 @@
       <c r="K37" s="12"/>
       <c r="L37" s="12"/>
       <c r="M37" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N37" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O37" s="12"/>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A38" s="18" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B38" s="8" t="s">
         <v>29</v>
@@ -2731,16 +2743,16 @@
       <c r="K38" s="12"/>
       <c r="L38" s="12"/>
       <c r="M38" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N38" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O38" s="12"/>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A39" s="18" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B39" s="8" t="s">
         <v>29</v>
@@ -2764,16 +2776,16 @@
       <c r="K39" s="12"/>
       <c r="L39" s="12"/>
       <c r="M39" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N39" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O39" s="12"/>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A40" s="18" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B40" s="8" t="s">
         <v>29</v>
@@ -2797,10 +2809,10 @@
       <c r="K40" s="12"/>
       <c r="L40" s="12"/>
       <c r="M40" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N40" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O40" s="12"/>
     </row>
@@ -2830,16 +2842,16 @@
       <c r="K41" s="12"/>
       <c r="L41" s="12"/>
       <c r="M41" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N41" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O41" s="12"/>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A42" s="18" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B42" s="8" t="s">
         <v>29</v>
@@ -2863,16 +2875,16 @@
       <c r="K42" s="12"/>
       <c r="L42" s="12"/>
       <c r="M42" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N42" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O42" s="12"/>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A43" s="18" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B43" s="8" t="s">
         <v>29</v>
@@ -2896,16 +2908,16 @@
       <c r="K43" s="12"/>
       <c r="L43" s="12"/>
       <c r="M43" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N43" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O43" s="12"/>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A44" s="18" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B44" s="8" t="s">
         <v>29</v>
@@ -2929,10 +2941,10 @@
       <c r="K44" s="12"/>
       <c r="L44" s="12"/>
       <c r="M44" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N44" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O44" s="12"/>
     </row>
@@ -2962,16 +2974,16 @@
       <c r="K45" s="12"/>
       <c r="L45" s="12"/>
       <c r="M45" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N45" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O45" s="12"/>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A46" s="18" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B46" s="8" t="s">
         <v>29</v>
@@ -2995,16 +3007,16 @@
       <c r="K46" s="12"/>
       <c r="L46" s="12"/>
       <c r="M46" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N46" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O46" s="12"/>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A47" s="18" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B47" s="8" t="s">
         <v>29</v>
@@ -3028,16 +3040,16 @@
       <c r="K47" s="12"/>
       <c r="L47" s="12"/>
       <c r="M47" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N47" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O47" s="12"/>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A48" s="18" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B48" s="8" t="s">
         <v>29</v>
@@ -3061,10 +3073,10 @@
       <c r="K48" s="12"/>
       <c r="L48" s="12"/>
       <c r="M48" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N48" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O48" s="12"/>
     </row>
@@ -3094,10 +3106,10 @@
       <c r="K49" s="12"/>
       <c r="L49" s="12"/>
       <c r="M49" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N49" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O49" s="12"/>
     </row>
@@ -3127,10 +3139,10 @@
       <c r="K50" s="12"/>
       <c r="L50" s="12"/>
       <c r="M50" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N50" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O50" s="12"/>
     </row>
@@ -3160,10 +3172,10 @@
       <c r="K51" s="12"/>
       <c r="L51" s="12"/>
       <c r="M51" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N51" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O51" s="12"/>
     </row>
@@ -3193,16 +3205,16 @@
       <c r="K52" s="12"/>
       <c r="L52" s="12"/>
       <c r="M52" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N52" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O52" s="12"/>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A53" s="18" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B53" s="8" t="s">
         <v>31</v>
@@ -3228,16 +3240,16 @@
       <c r="K53" s="12"/>
       <c r="L53" s="12"/>
       <c r="M53" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N53" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O53" s="12"/>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A54" s="18" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B54" s="8" t="s">
         <v>31</v>
@@ -3263,10 +3275,10 @@
       <c r="K54" s="12"/>
       <c r="L54" s="12"/>
       <c r="M54" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N54" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O54" s="12"/>
     </row>
@@ -3298,16 +3310,16 @@
       <c r="K55" s="12"/>
       <c r="L55" s="12"/>
       <c r="M55" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N55" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O55" s="12"/>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A56" s="18" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B56" s="8" t="s">
         <v>31</v>
@@ -3333,10 +3345,10 @@
       <c r="K56" s="12"/>
       <c r="L56" s="12"/>
       <c r="M56" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N56" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O56" s="12"/>
     </row>
@@ -3368,16 +3380,16 @@
       <c r="K57" s="12"/>
       <c r="L57" s="12"/>
       <c r="M57" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N57" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O57" s="12"/>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A58" s="18" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B58" s="8" t="s">
         <v>31</v>
@@ -3403,16 +3415,16 @@
       <c r="K58" s="12"/>
       <c r="L58" s="12"/>
       <c r="M58" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N58" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O58" s="12"/>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A59" s="18" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B59" s="8" t="s">
         <v>31</v>
@@ -3436,10 +3448,10 @@
       <c r="K59" s="12"/>
       <c r="L59" s="12"/>
       <c r="M59" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N59" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O59" s="12"/>
     </row>
@@ -3471,16 +3483,16 @@
       <c r="K60" s="12"/>
       <c r="L60" s="12"/>
       <c r="M60" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N60" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O60" s="12"/>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A61" s="18" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B61" s="8" t="s">
         <v>31</v>
@@ -3506,10 +3518,10 @@
       <c r="K61" s="12"/>
       <c r="L61" s="12"/>
       <c r="M61" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N61" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O61" s="12"/>
     </row>
@@ -3539,10 +3551,10 @@
       <c r="K62" s="12"/>
       <c r="L62" s="12"/>
       <c r="M62" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N62" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O62" s="12"/>
     </row>
@@ -3572,10 +3584,10 @@
       <c r="K63" s="12"/>
       <c r="L63" s="12"/>
       <c r="M63" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N63" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O63" s="12"/>
     </row>
@@ -3605,10 +3617,10 @@
       <c r="K64" s="12"/>
       <c r="L64" s="12"/>
       <c r="M64" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N64" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O64" s="12"/>
     </row>
@@ -3638,16 +3650,16 @@
       <c r="K65" s="12"/>
       <c r="L65" s="12"/>
       <c r="M65" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N65" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O65" s="12"/>
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A66" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B66" s="8" t="s">
         <v>31</v>
@@ -3671,10 +3683,10 @@
       <c r="K66" s="12"/>
       <c r="L66" s="12"/>
       <c r="M66" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N66" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O66" s="12"/>
     </row>
@@ -3704,10 +3716,10 @@
       <c r="K67" s="12"/>
       <c r="L67" s="12"/>
       <c r="M67" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N67" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O67" s="12"/>
     </row>
@@ -3737,10 +3749,10 @@
       <c r="K68" s="12"/>
       <c r="L68" s="12"/>
       <c r="M68" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N68" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O68" s="12"/>
     </row>
@@ -3770,10 +3782,10 @@
       <c r="K69" s="12"/>
       <c r="L69" s="12"/>
       <c r="M69" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N69" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O69" s="12"/>
     </row>
@@ -3803,10 +3815,10 @@
       <c r="K70" s="12"/>
       <c r="L70" s="12"/>
       <c r="M70" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N70" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O70" s="12"/>
     </row>
@@ -3836,10 +3848,10 @@
       <c r="K71" s="12"/>
       <c r="L71" s="12"/>
       <c r="M71" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N71" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O71" s="12"/>
     </row>
@@ -3869,10 +3881,10 @@
       <c r="K72" s="12"/>
       <c r="L72" s="12"/>
       <c r="M72" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N72" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O72" s="12"/>
     </row>
@@ -3902,10 +3914,10 @@
       <c r="K73" s="12"/>
       <c r="L73" s="12"/>
       <c r="M73" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N73" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O73" s="12"/>
     </row>
@@ -3935,10 +3947,10 @@
       <c r="K74" s="12"/>
       <c r="L74" s="12"/>
       <c r="M74" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N74" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O74" s="12"/>
     </row>
@@ -3968,16 +3980,16 @@
       <c r="K75" s="12"/>
       <c r="L75" s="12"/>
       <c r="M75" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N75" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O75" s="12"/>
     </row>
     <row r="76" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A76" s="18" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B76" s="8" t="s">
         <v>31</v>
@@ -4001,16 +4013,16 @@
       <c r="K76" s="12"/>
       <c r="L76" s="12"/>
       <c r="M76" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N76" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O76" s="12"/>
     </row>
     <row r="77" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A77" s="18" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B77" s="8" t="s">
         <v>31</v>
@@ -4034,16 +4046,16 @@
       <c r="K77" s="12"/>
       <c r="L77" s="12"/>
       <c r="M77" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N77" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O77" s="12"/>
     </row>
     <row r="78" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A78" s="18" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B78" s="8" t="s">
         <v>31</v>
@@ -4067,10 +4079,10 @@
       <c r="K78" s="12"/>
       <c r="L78" s="12"/>
       <c r="M78" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N78" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O78" s="12"/>
     </row>
@@ -4100,16 +4112,16 @@
       <c r="K79" s="12"/>
       <c r="L79" s="12"/>
       <c r="M79" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N79" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O79" s="12"/>
     </row>
     <row r="80" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A80" s="18" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B80" s="8" t="s">
         <v>31</v>
@@ -4133,16 +4145,16 @@
       <c r="K80" s="12"/>
       <c r="L80" s="12"/>
       <c r="M80" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N80" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O80" s="12"/>
     </row>
     <row r="81" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A81" s="18" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B81" s="8" t="s">
         <v>31</v>
@@ -4166,16 +4178,16 @@
       <c r="K81" s="12"/>
       <c r="L81" s="12"/>
       <c r="M81" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N81" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O81" s="12"/>
     </row>
     <row r="82" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A82" s="18" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B82" s="8" t="s">
         <v>31</v>
@@ -4199,10 +4211,10 @@
       <c r="K82" s="12"/>
       <c r="L82" s="12"/>
       <c r="M82" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N82" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O82" s="12"/>
     </row>
@@ -4232,16 +4244,16 @@
       <c r="K83" s="12"/>
       <c r="L83" s="12"/>
       <c r="M83" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N83" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O83" s="12"/>
     </row>
     <row r="84" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A84" s="18" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B84" s="8" t="s">
         <v>31</v>
@@ -4265,16 +4277,16 @@
       <c r="K84" s="12"/>
       <c r="L84" s="12"/>
       <c r="M84" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N84" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O84" s="12"/>
     </row>
     <row r="85" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A85" s="18" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B85" s="8" t="s">
         <v>31</v>
@@ -4298,16 +4310,16 @@
       <c r="K85" s="12"/>
       <c r="L85" s="12"/>
       <c r="M85" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N85" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O85" s="12"/>
     </row>
     <row r="86" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A86" s="18" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B86" s="8" t="s">
         <v>31</v>
@@ -4331,10 +4343,10 @@
       <c r="K86" s="12"/>
       <c r="L86" s="12"/>
       <c r="M86" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N86" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O86" s="12"/>
     </row>
@@ -4364,10 +4376,10 @@
       <c r="K87" s="12"/>
       <c r="L87" s="12"/>
       <c r="M87" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N87" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O87" s="12"/>
     </row>
@@ -4397,10 +4409,10 @@
       <c r="K88" s="12"/>
       <c r="L88" s="12"/>
       <c r="M88" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N88" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O88" s="12"/>
     </row>
@@ -4430,10 +4442,10 @@
       <c r="K89" s="12"/>
       <c r="L89" s="12"/>
       <c r="M89" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N89" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O89" s="12"/>
     </row>
@@ -4463,16 +4475,16 @@
       <c r="K90" s="12"/>
       <c r="L90" s="12"/>
       <c r="M90" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N90" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O90" s="12"/>
     </row>
     <row r="91" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A91" s="18" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B91" s="8" t="s">
         <v>32</v>
@@ -4498,16 +4510,16 @@
       <c r="K91" s="12"/>
       <c r="L91" s="12"/>
       <c r="M91" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N91" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O91" s="12"/>
     </row>
     <row r="92" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A92" s="18" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B92" s="8" t="s">
         <v>32</v>
@@ -4533,10 +4545,10 @@
       <c r="K92" s="12"/>
       <c r="L92" s="12"/>
       <c r="M92" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N92" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O92" s="12"/>
     </row>
@@ -4568,10 +4580,10 @@
       <c r="K93" s="12"/>
       <c r="L93" s="12"/>
       <c r="M93" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N93" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O93" s="12"/>
     </row>
@@ -4603,16 +4615,16 @@
       <c r="K94" s="12"/>
       <c r="L94" s="12"/>
       <c r="M94" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N94" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O94" s="12"/>
     </row>
     <row r="95" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A95" s="18" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B95" s="8" t="s">
         <v>32</v>
@@ -4638,16 +4650,16 @@
       <c r="K95" s="12"/>
       <c r="L95" s="12"/>
       <c r="M95" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N95" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O95" s="12"/>
     </row>
     <row r="96" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A96" s="18" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B96" s="8" t="s">
         <v>32</v>
@@ -4673,16 +4685,16 @@
       <c r="K96" s="12"/>
       <c r="L96" s="12"/>
       <c r="M96" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N96" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O96" s="12"/>
     </row>
     <row r="97" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A97" s="18" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B97" s="8" t="s">
         <v>32</v>
@@ -4706,16 +4718,16 @@
       <c r="K97" s="12"/>
       <c r="L97" s="12"/>
       <c r="M97" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N97" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O97" s="12"/>
     </row>
     <row r="98" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A98" s="18" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B98" s="8" t="s">
         <v>32</v>
@@ -4741,16 +4753,16 @@
       <c r="K98" s="12"/>
       <c r="L98" s="12"/>
       <c r="M98" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N98" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O98" s="12"/>
     </row>
     <row r="99" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A99" s="18" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B99" s="8" t="s">
         <v>32</v>
@@ -4776,10 +4788,10 @@
       <c r="K99" s="12"/>
       <c r="L99" s="12"/>
       <c r="M99" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N99" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O99" s="12"/>
     </row>
@@ -4809,10 +4821,10 @@
       <c r="K100" s="19"/>
       <c r="L100" s="19"/>
       <c r="M100" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N100" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O100" s="19"/>
     </row>
@@ -4842,10 +4854,10 @@
       <c r="K101" s="19"/>
       <c r="L101" s="19"/>
       <c r="M101" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N101" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O101" s="19"/>
     </row>
@@ -4875,10 +4887,10 @@
       <c r="K102" s="19"/>
       <c r="L102" s="19"/>
       <c r="M102" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N102" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O102" s="19"/>
     </row>
@@ -4908,10 +4920,10 @@
       <c r="K103" s="19"/>
       <c r="L103" s="19"/>
       <c r="M103" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N103" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O103" s="19"/>
     </row>
@@ -4941,10 +4953,10 @@
       <c r="K104" s="19"/>
       <c r="L104" s="19"/>
       <c r="M104" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N104" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O104" s="19"/>
     </row>
@@ -4974,10 +4986,10 @@
       <c r="K105" s="19"/>
       <c r="L105" s="19"/>
       <c r="M105" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N105" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O105" s="19"/>
     </row>
@@ -5007,10 +5019,10 @@
       <c r="K106" s="19"/>
       <c r="L106" s="19"/>
       <c r="M106" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N106" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O106" s="19"/>
     </row>
@@ -5040,10 +5052,10 @@
       <c r="K107" s="19"/>
       <c r="L107" s="19"/>
       <c r="M107" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N107" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O107" s="19"/>
     </row>
@@ -5073,10 +5085,10 @@
       <c r="K108" s="19"/>
       <c r="L108" s="19"/>
       <c r="M108" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N108" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O108" s="19"/>
     </row>

</xml_diff>

<commit_message>
Reset field name to original value and used Data Point Type Name Overwrite instead. Added a customization for NFRD.
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/euTaxonomyNonFinancials/EutaxonomyNonFinancials.xlsx
+++ b/dataland-framework-toolbox/inputs/euTaxonomyNonFinancials/EutaxonomyNonFinancials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d40006\Documents\Dataland Project\Dataland\dataland-framework-toolbox\inputs\euTaxonomyNonFinancials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0529B90B-08B3-42EA-8231-C49EB940A2D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEFA05E6-A4D9-4CE9-BF4A-EF8BE9180EB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="1650" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="249">
   <si>
     <t>Field Identifier</t>
   </si>
@@ -149,6 +149,9 @@
     <t>Percentage</t>
   </si>
   <si>
+    <t>NFRD Mandatory</t>
+  </si>
+  <si>
     <t>Is the NFRD mandatory for your company?</t>
   </si>
   <si>
@@ -812,7 +815,7 @@
     <t>Does the company have due diligence processes to identify, prevent, mitigate and address adverse human rights impacts? See Regulation (EU) 2022/1288, Annex I, table 3, indicator nr. 10.</t>
   </si>
   <si>
-    <t>Is NFRD mandatory?</t>
+    <t>IsNfrdMandatory</t>
   </si>
 </sst>
 </file>
@@ -1495,8 +1498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O108"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1549,13 +1552,13 @@
         <v>11</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
@@ -1576,11 +1579,11 @@
         <v>17</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H2" s="10"/>
       <c r="I2" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J2" s="11"/>
       <c r="K2" s="11"/>
@@ -1599,7 +1602,7 @@
         <v>18</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="F3" s="9" t="s">
         <v>13</v>
@@ -1607,7 +1610,7 @@
       <c r="G3" s="9"/>
       <c r="H3" s="10"/>
       <c r="I3" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J3" s="11"/>
       <c r="K3" s="11"/>
@@ -1638,7 +1641,7 @@
       </c>
       <c r="H4" s="11"/>
       <c r="I4" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J4" s="10"/>
       <c r="K4" s="10"/>
@@ -1656,10 +1659,10 @@
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="13" t="s">
-        <v>247</v>
+        <v>26</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F5" s="19" t="s">
         <v>24</v>
@@ -1669,14 +1672,16 @@
       </c>
       <c r="H5" s="11"/>
       <c r="I5" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J5" s="11"/>
       <c r="K5" s="11"/>
       <c r="L5" s="11"/>
       <c r="M5" s="11"/>
       <c r="N5" s="11"/>
-      <c r="O5" s="11"/>
+      <c r="O5" s="11" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" s="6">
@@ -1700,7 +1705,7 @@
       </c>
       <c r="H6" s="11"/>
       <c r="I6" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J6" s="11"/>
       <c r="K6" s="11"/>
@@ -1718,13 +1723,13 @@
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="13" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="F7" s="26" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G7" s="25" t="s">
         <v>14</v>
@@ -1747,20 +1752,20 @@
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="36" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="H8" s="11"/>
       <c r="I8" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J8" s="11"/>
       <c r="K8" s="11"/>
@@ -1778,10 +1783,10 @@
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="37" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E9" s="33" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="F9" s="19" t="s">
         <v>24</v>
@@ -1789,7 +1794,7 @@
       <c r="G9" s="21"/>
       <c r="H9" s="11"/>
       <c r="I9" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J9" s="11"/>
       <c r="K9" s="11"/>
@@ -1807,10 +1812,10 @@
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="32" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E10" s="34" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F10" s="19" t="s">
         <v>24</v>
@@ -1818,7 +1823,7 @@
       <c r="G10" s="21"/>
       <c r="H10" s="11"/>
       <c r="I10" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J10" s="11"/>
       <c r="K10" s="11"/>
@@ -1836,10 +1841,10 @@
       </c>
       <c r="C11" s="7"/>
       <c r="D11" s="37" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="E11" s="35" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="F11" s="19" t="s">
         <v>24</v>
@@ -1847,7 +1852,7 @@
       <c r="G11" s="21"/>
       <c r="H11" s="11"/>
       <c r="I11" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J11" s="11"/>
       <c r="K11" s="11"/>
@@ -1865,10 +1870,10 @@
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="37" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="E12" s="34" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="F12" s="19" t="s">
         <v>24</v>
@@ -1876,7 +1881,7 @@
       <c r="G12" s="21"/>
       <c r="H12" s="11"/>
       <c r="I12" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J12" s="11"/>
       <c r="K12" s="11"/>
@@ -1894,11 +1899,11 @@
       </c>
       <c r="C13" s="7"/>
       <c r="D13" s="13" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E13" s="11"/>
       <c r="F13" s="19" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G13" s="22" t="s">
         <v>14</v>
@@ -1917,22 +1922,22 @@
         <v>11</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C14" s="7"/>
       <c r="D14" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="F14" s="20" t="s">
         <v>33</v>
-      </c>
-      <c r="E14" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="F14" s="20" t="s">
-        <v>32</v>
       </c>
       <c r="G14" s="21"/>
       <c r="H14" s="11"/>
       <c r="I14" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J14" s="11"/>
       <c r="K14" s="11"/>
@@ -1943,19 +1948,19 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A15" s="17" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E15" s="27" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="F15" s="20" t="s">
         <v>25</v>
@@ -1963,69 +1968,69 @@
       <c r="G15" s="21"/>
       <c r="H15" s="11"/>
       <c r="I15" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J15" s="11"/>
       <c r="K15" s="11"/>
       <c r="L15" s="11"/>
       <c r="M15" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N15" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O15" s="11"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16" s="17" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E16" s="27" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="F16" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G16" s="21"/>
       <c r="H16" s="11"/>
       <c r="I16" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J16" s="11"/>
       <c r="K16" s="11"/>
       <c r="L16" s="11"/>
       <c r="M16" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N16" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O16" s="11"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A17" s="17" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F17" s="20" t="s">
         <v>25</v>
@@ -2033,69 +2038,69 @@
       <c r="G17" s="21"/>
       <c r="H17" s="11"/>
       <c r="I17" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J17" s="11"/>
       <c r="K17" s="11"/>
       <c r="L17" s="11"/>
       <c r="M17" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N17" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O17" s="11"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A18" s="17" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C18" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="D18" s="14" t="s">
-        <v>36</v>
-      </c>
       <c r="E18" s="11" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F18" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G18" s="21"/>
       <c r="H18" s="11"/>
       <c r="I18" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J18" s="11"/>
       <c r="K18" s="11"/>
       <c r="L18" s="11"/>
       <c r="M18" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N18" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O18" s="11"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A19" s="17" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E19" s="27" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F19" s="20" t="s">
         <v>25</v>
@@ -2103,102 +2108,102 @@
       <c r="G19" s="21"/>
       <c r="H19" s="11"/>
       <c r="I19" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J19" s="11"/>
       <c r="K19" s="11"/>
       <c r="L19" s="11"/>
       <c r="M19" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N19" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O19" s="11"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A20" s="17" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E20" s="27" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F20" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G20" s="21"/>
       <c r="H20" s="11"/>
       <c r="I20" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J20" s="11"/>
       <c r="K20" s="11"/>
       <c r="L20" s="11"/>
       <c r="M20" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N20" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O20" s="11"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A21" s="17" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C21" s="7"/>
       <c r="D21" s="14" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E21" s="27" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F21" s="20" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G21" s="21"/>
       <c r="H21" s="11"/>
       <c r="I21" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J21" s="11"/>
       <c r="K21" s="11"/>
       <c r="L21" s="11"/>
       <c r="M21" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N21" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O21" s="11"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A22" s="17" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D22" s="14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F22" s="20" t="s">
         <v>25</v>
@@ -2206,51 +2211,51 @@
       <c r="G22" s="21"/>
       <c r="H22" s="11"/>
       <c r="I22" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J22" s="11"/>
       <c r="K22" s="11"/>
       <c r="L22" s="11"/>
       <c r="M22" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N22" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O22" s="11"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A23" s="17" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D23" s="14" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F23" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G23" s="21"/>
       <c r="H23" s="11"/>
       <c r="I23" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J23" s="11"/>
       <c r="K23" s="11"/>
       <c r="L23" s="11"/>
       <c r="M23" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N23" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O23" s="11"/>
     </row>
@@ -2259,14 +2264,14 @@
         <v>17</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C24" s="7"/>
       <c r="D24" s="28" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E24" s="29" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F24" s="20" t="s">
         <v>25</v>
@@ -2274,32 +2279,32 @@
       <c r="G24" s="21"/>
       <c r="H24" s="11"/>
       <c r="I24" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J24" s="11"/>
       <c r="K24" s="11"/>
       <c r="L24" s="11"/>
       <c r="M24" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N24" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O24" s="11"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A25" s="17" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C25" s="7"/>
       <c r="D25" s="28" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E25" s="29" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F25" s="20" t="s">
         <v>25</v>
@@ -2307,32 +2312,32 @@
       <c r="G25" s="21"/>
       <c r="H25" s="11"/>
       <c r="I25" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J25" s="11"/>
       <c r="K25" s="11"/>
       <c r="L25" s="11"/>
       <c r="M25" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N25" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O25" s="11"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A26" s="17" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C26" s="7"/>
       <c r="D26" s="30" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E26" s="29" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F26" s="20" t="s">
         <v>25</v>
@@ -2340,32 +2345,32 @@
       <c r="G26" s="21"/>
       <c r="H26" s="11"/>
       <c r="I26" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J26" s="11"/>
       <c r="K26" s="11"/>
       <c r="L26" s="11"/>
       <c r="M26" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N26" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O26" s="11"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A27" s="17" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C27" s="7"/>
       <c r="D27" s="28" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E27" s="29" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F27" s="20" t="s">
         <v>25</v>
@@ -2373,32 +2378,32 @@
       <c r="G27" s="21"/>
       <c r="H27" s="11"/>
       <c r="I27" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J27" s="11"/>
       <c r="K27" s="11"/>
       <c r="L27" s="11"/>
       <c r="M27" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N27" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O27" s="11"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A28" s="17" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C28" s="7"/>
       <c r="D28" s="28" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E28" s="29" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F28" s="20" t="s">
         <v>25</v>
@@ -2406,16 +2411,16 @@
       <c r="G28" s="21"/>
       <c r="H28" s="11"/>
       <c r="I28" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J28" s="11"/>
       <c r="K28" s="11"/>
       <c r="L28" s="11"/>
       <c r="M28" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N28" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O28" s="11"/>
     </row>
@@ -2424,14 +2429,14 @@
         <v>18</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C29" s="7"/>
       <c r="D29" s="31" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E29" s="29" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F29" s="20" t="s">
         <v>25</v>
@@ -2439,32 +2444,32 @@
       <c r="G29" s="21"/>
       <c r="H29" s="11"/>
       <c r="I29" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J29" s="11"/>
       <c r="K29" s="11"/>
       <c r="L29" s="11"/>
       <c r="M29" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N29" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O29" s="11"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A30" s="17" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C30" s="7"/>
       <c r="D30" s="31" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E30" s="29" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F30" s="20" t="s">
         <v>25</v>
@@ -2472,32 +2477,32 @@
       <c r="G30" s="21"/>
       <c r="H30" s="11"/>
       <c r="I30" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J30" s="11"/>
       <c r="K30" s="11"/>
       <c r="L30" s="11"/>
       <c r="M30" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N30" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O30" s="11"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A31" s="17" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C31" s="7"/>
       <c r="D31" s="30" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E31" s="29" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F31" s="20" t="s">
         <v>25</v>
@@ -2505,32 +2510,32 @@
       <c r="G31" s="21"/>
       <c r="H31" s="11"/>
       <c r="I31" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J31" s="11"/>
       <c r="K31" s="11"/>
       <c r="L31" s="11"/>
       <c r="M31" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N31" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O31" s="11"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A32" s="17" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C32" s="7"/>
       <c r="D32" s="30" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E32" s="29" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F32" s="20" t="s">
         <v>25</v>
@@ -2538,16 +2543,16 @@
       <c r="G32" s="21"/>
       <c r="H32" s="11"/>
       <c r="I32" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J32" s="11"/>
       <c r="K32" s="11"/>
       <c r="L32" s="11"/>
       <c r="M32" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N32" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O32" s="11"/>
     </row>
@@ -2556,14 +2561,14 @@
         <v>19</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C33" s="7"/>
       <c r="D33" s="30" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E33" s="29" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F33" s="20" t="s">
         <v>25</v>
@@ -2571,32 +2576,32 @@
       <c r="G33" s="21"/>
       <c r="H33" s="11"/>
       <c r="I33" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J33" s="11"/>
       <c r="K33" s="11"/>
       <c r="L33" s="11"/>
       <c r="M33" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N33" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O33" s="11"/>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A34" s="17" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C34" s="7"/>
       <c r="D34" s="30" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E34" s="29" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F34" s="20" t="s">
         <v>25</v>
@@ -2604,32 +2609,32 @@
       <c r="G34" s="21"/>
       <c r="H34" s="11"/>
       <c r="I34" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J34" s="11"/>
       <c r="K34" s="11"/>
       <c r="L34" s="11"/>
       <c r="M34" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N34" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O34" s="11"/>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A35" s="17" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C35" s="7"/>
       <c r="D35" s="30" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E35" s="29" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F35" s="20" t="s">
         <v>25</v>
@@ -2637,32 +2642,32 @@
       <c r="G35" s="21"/>
       <c r="H35" s="11"/>
       <c r="I35" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J35" s="11"/>
       <c r="K35" s="11"/>
       <c r="L35" s="11"/>
       <c r="M35" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N35" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O35" s="11"/>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A36" s="17" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C36" s="7"/>
       <c r="D36" s="30" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E36" s="29" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F36" s="20" t="s">
         <v>25</v>
@@ -2670,16 +2675,16 @@
       <c r="G36" s="21"/>
       <c r="H36" s="11"/>
       <c r="I36" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J36" s="11"/>
       <c r="K36" s="11"/>
       <c r="L36" s="11"/>
       <c r="M36" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N36" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O36" s="11"/>
     </row>
@@ -2688,14 +2693,14 @@
         <v>20</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C37" s="7"/>
       <c r="D37" s="30" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E37" s="29" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F37" s="20" t="s">
         <v>25</v>
@@ -2703,32 +2708,32 @@
       <c r="G37" s="21"/>
       <c r="H37" s="11"/>
       <c r="I37" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J37" s="11"/>
       <c r="K37" s="11"/>
       <c r="L37" s="11"/>
       <c r="M37" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N37" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O37" s="11"/>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A38" s="17" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C38" s="7"/>
       <c r="D38" s="30" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E38" s="29" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="F38" s="20" t="s">
         <v>25</v>
@@ -2736,32 +2741,32 @@
       <c r="G38" s="21"/>
       <c r="H38" s="11"/>
       <c r="I38" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J38" s="11"/>
       <c r="K38" s="11"/>
       <c r="L38" s="11"/>
       <c r="M38" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N38" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O38" s="11"/>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A39" s="17" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C39" s="7"/>
       <c r="D39" s="30" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E39" s="29" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F39" s="20" t="s">
         <v>25</v>
@@ -2769,32 +2774,32 @@
       <c r="G39" s="21"/>
       <c r="H39" s="11"/>
       <c r="I39" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J39" s="11"/>
       <c r="K39" s="11"/>
       <c r="L39" s="11"/>
       <c r="M39" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N39" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O39" s="11"/>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A40" s="17" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C40" s="7"/>
       <c r="D40" s="30" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E40" s="29" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F40" s="20" t="s">
         <v>25</v>
@@ -2802,16 +2807,16 @@
       <c r="G40" s="21"/>
       <c r="H40" s="11"/>
       <c r="I40" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J40" s="11"/>
       <c r="K40" s="11"/>
       <c r="L40" s="11"/>
       <c r="M40" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N40" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O40" s="11"/>
     </row>
@@ -2820,14 +2825,14 @@
         <v>21</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C41" s="7"/>
       <c r="D41" s="30" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E41" s="29" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F41" s="20" t="s">
         <v>25</v>
@@ -2835,32 +2840,32 @@
       <c r="G41" s="21"/>
       <c r="H41" s="11"/>
       <c r="I41" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J41" s="11"/>
       <c r="K41" s="11"/>
       <c r="L41" s="11"/>
       <c r="M41" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N41" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O41" s="11"/>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A42" s="17" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C42" s="7"/>
       <c r="D42" s="30" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E42" s="29" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F42" s="20" t="s">
         <v>25</v>
@@ -2868,32 +2873,32 @@
       <c r="G42" s="21"/>
       <c r="H42" s="11"/>
       <c r="I42" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J42" s="11"/>
       <c r="K42" s="11"/>
       <c r="L42" s="11"/>
       <c r="M42" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N42" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O42" s="11"/>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A43" s="17" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C43" s="7"/>
       <c r="D43" s="30" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E43" s="29" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="F43" s="20" t="s">
         <v>25</v>
@@ -2901,32 +2906,32 @@
       <c r="G43" s="21"/>
       <c r="H43" s="11"/>
       <c r="I43" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J43" s="11"/>
       <c r="K43" s="11"/>
       <c r="L43" s="11"/>
       <c r="M43" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N43" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O43" s="11"/>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A44" s="17" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C44" s="7"/>
       <c r="D44" s="30" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E44" s="29" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F44" s="20" t="s">
         <v>25</v>
@@ -2934,16 +2939,16 @@
       <c r="G44" s="21"/>
       <c r="H44" s="11"/>
       <c r="I44" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J44" s="11"/>
       <c r="K44" s="11"/>
       <c r="L44" s="11"/>
       <c r="M44" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N44" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O44" s="11"/>
     </row>
@@ -2952,14 +2957,14 @@
         <v>22</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C45" s="7"/>
       <c r="D45" s="30" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E45" s="29" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="F45" s="20" t="s">
         <v>25</v>
@@ -2967,32 +2972,32 @@
       <c r="G45" s="21"/>
       <c r="H45" s="11"/>
       <c r="I45" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J45" s="11"/>
       <c r="K45" s="11"/>
       <c r="L45" s="11"/>
       <c r="M45" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N45" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O45" s="11"/>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A46" s="17" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C46" s="7"/>
       <c r="D46" s="30" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E46" s="29" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="F46" s="20" t="s">
         <v>25</v>
@@ -3000,32 +3005,32 @@
       <c r="G46" s="21"/>
       <c r="H46" s="11"/>
       <c r="I46" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J46" s="11"/>
       <c r="K46" s="11"/>
       <c r="L46" s="11"/>
       <c r="M46" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N46" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O46" s="11"/>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A47" s="17" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C47" s="7"/>
       <c r="D47" s="30" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E47" s="29" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F47" s="20" t="s">
         <v>25</v>
@@ -3033,32 +3038,32 @@
       <c r="G47" s="21"/>
       <c r="H47" s="11"/>
       <c r="I47" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J47" s="11"/>
       <c r="K47" s="11"/>
       <c r="L47" s="11"/>
       <c r="M47" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N47" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O47" s="11"/>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A48" s="17" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C48" s="7"/>
       <c r="D48" s="30" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E48" s="29" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="F48" s="20" t="s">
         <v>25</v>
@@ -3066,16 +3071,16 @@
       <c r="G48" s="21"/>
       <c r="H48" s="11"/>
       <c r="I48" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J48" s="11"/>
       <c r="K48" s="11"/>
       <c r="L48" s="11"/>
       <c r="M48" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N48" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O48" s="11"/>
     </row>
@@ -3084,31 +3089,31 @@
         <v>23</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C49" s="7"/>
       <c r="D49" s="14" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E49" s="27" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F49" s="20" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G49" s="21"/>
       <c r="H49" s="11"/>
       <c r="I49" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J49" s="11"/>
       <c r="K49" s="11"/>
       <c r="L49" s="11"/>
       <c r="M49" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N49" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O49" s="11"/>
     </row>
@@ -3117,14 +3122,14 @@
         <v>24</v>
       </c>
       <c r="B50" s="15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C50" s="15"/>
       <c r="D50" s="16" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E50" s="27" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F50" s="20" t="s">
         <v>25</v>
@@ -3132,16 +3137,16 @@
       <c r="G50" s="21"/>
       <c r="H50" s="11"/>
       <c r="I50" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J50" s="11"/>
       <c r="K50" s="11"/>
       <c r="L50" s="11"/>
       <c r="M50" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N50" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O50" s="11"/>
     </row>
@@ -3150,14 +3155,14 @@
         <v>25</v>
       </c>
       <c r="B51" s="15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C51" s="15"/>
       <c r="D51" s="16" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E51" s="27" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F51" s="20" t="s">
         <v>25</v>
@@ -3165,16 +3170,16 @@
       <c r="G51" s="21"/>
       <c r="H51" s="11"/>
       <c r="I51" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J51" s="11"/>
       <c r="K51" s="11"/>
       <c r="L51" s="11"/>
       <c r="M51" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N51" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O51" s="11"/>
     </row>
@@ -3183,49 +3188,49 @@
         <v>26</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C52" s="7"/>
       <c r="D52" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E52" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="F52" s="20" t="s">
         <v>33</v>
-      </c>
-      <c r="E52" s="27" t="s">
-        <v>59</v>
-      </c>
-      <c r="F52" s="20" t="s">
-        <v>32</v>
       </c>
       <c r="G52" s="21"/>
       <c r="H52" s="11"/>
       <c r="I52" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J52" s="11"/>
       <c r="K52" s="11"/>
       <c r="L52" s="11"/>
       <c r="M52" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N52" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O52" s="11"/>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A53" s="17" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D53" s="14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E53" s="27" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F53" s="20" t="s">
         <v>25</v>
@@ -3233,69 +3238,69 @@
       <c r="G53" s="21"/>
       <c r="H53" s="11"/>
       <c r="I53" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J53" s="11"/>
       <c r="K53" s="11"/>
       <c r="L53" s="11"/>
       <c r="M53" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N53" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O53" s="11"/>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A54" s="17" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D54" s="14" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E54" s="27" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F54" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G54" s="21"/>
       <c r="H54" s="11"/>
       <c r="I54" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J54" s="11"/>
       <c r="K54" s="11"/>
       <c r="L54" s="11"/>
       <c r="M54" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N54" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O54" s="11"/>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A55" s="17" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D55" s="14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E55" s="27" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F55" s="20" t="s">
         <v>25</v>
@@ -3303,69 +3308,69 @@
       <c r="G55" s="21"/>
       <c r="H55" s="11"/>
       <c r="I55" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J55" s="11"/>
       <c r="K55" s="11"/>
       <c r="L55" s="11"/>
       <c r="M55" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N55" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O55" s="11"/>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A56" s="17" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C56" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D56" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="D56" s="14" t="s">
-        <v>36</v>
-      </c>
       <c r="E56" s="27" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F56" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G56" s="21"/>
       <c r="H56" s="11"/>
       <c r="I56" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J56" s="11"/>
       <c r="K56" s="11"/>
       <c r="L56" s="11"/>
       <c r="M56" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N56" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O56" s="11"/>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A57" s="17" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D57" s="14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E57" s="27" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F57" s="20" t="s">
         <v>25</v>
@@ -3373,102 +3378,102 @@
       <c r="G57" s="21"/>
       <c r="H57" s="11"/>
       <c r="I57" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J57" s="11"/>
       <c r="K57" s="11"/>
       <c r="L57" s="11"/>
       <c r="M57" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N57" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O57" s="11"/>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A58" s="17" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D58" s="14" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E58" s="27" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F58" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G58" s="21"/>
       <c r="H58" s="11"/>
       <c r="I58" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J58" s="11"/>
       <c r="K58" s="11"/>
       <c r="L58" s="11"/>
       <c r="M58" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N58" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O58" s="11"/>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A59" s="17" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C59" s="7"/>
       <c r="D59" s="14" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E59" s="27" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F59" s="20" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G59" s="21"/>
       <c r="H59" s="11"/>
       <c r="I59" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J59" s="11"/>
       <c r="K59" s="11"/>
       <c r="L59" s="11"/>
       <c r="M59" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N59" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O59" s="11"/>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A60" s="17" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D60" s="14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E60" s="27" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F60" s="20" t="s">
         <v>25</v>
@@ -3476,51 +3481,51 @@
       <c r="G60" s="21"/>
       <c r="H60" s="11"/>
       <c r="I60" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J60" s="11"/>
       <c r="K60" s="11"/>
       <c r="L60" s="11"/>
       <c r="M60" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N60" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O60" s="11"/>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A61" s="17" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D61" s="14" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E61" s="27" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F61" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G61" s="21"/>
       <c r="H61" s="11"/>
       <c r="I61" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J61" s="11"/>
       <c r="K61" s="11"/>
       <c r="L61" s="11"/>
       <c r="M61" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N61" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O61" s="11"/>
     </row>
@@ -3529,14 +3534,14 @@
         <v>32</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C62" s="7"/>
       <c r="D62" s="28" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E62" s="29" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="F62" s="20" t="s">
         <v>25</v>
@@ -3544,32 +3549,32 @@
       <c r="G62" s="21"/>
       <c r="H62" s="11"/>
       <c r="I62" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J62" s="11"/>
       <c r="K62" s="11"/>
       <c r="L62" s="11"/>
       <c r="M62" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N62" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O62" s="11"/>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A63" s="17" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C63" s="7"/>
       <c r="D63" s="28" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E63" s="29" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="F63" s="20" t="s">
         <v>25</v>
@@ -3577,32 +3582,32 @@
       <c r="G63" s="21"/>
       <c r="H63" s="11"/>
       <c r="I63" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J63" s="11"/>
       <c r="K63" s="11"/>
       <c r="L63" s="11"/>
       <c r="M63" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N63" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O63" s="11"/>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A64" s="17" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C64" s="7"/>
       <c r="D64" s="30" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E64" s="29" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F64" s="20" t="s">
         <v>25</v>
@@ -3610,32 +3615,32 @@
       <c r="G64" s="21"/>
       <c r="H64" s="11"/>
       <c r="I64" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J64" s="11"/>
       <c r="K64" s="11"/>
       <c r="L64" s="11"/>
       <c r="M64" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N64" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O64" s="11"/>
     </row>
     <row r="65" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A65" s="17" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C65" s="7"/>
       <c r="D65" s="28" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E65" s="29" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F65" s="20" t="s">
         <v>25</v>
@@ -3643,32 +3648,32 @@
       <c r="G65" s="21"/>
       <c r="H65" s="11"/>
       <c r="I65" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J65" s="11"/>
       <c r="K65" s="11"/>
       <c r="L65" s="11"/>
       <c r="M65" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N65" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O65" s="11"/>
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A66" s="17" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C66" s="7"/>
       <c r="D66" s="28" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E66" s="29" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F66" s="20" t="s">
         <v>25</v>
@@ -3676,16 +3681,16 @@
       <c r="G66" s="21"/>
       <c r="H66" s="11"/>
       <c r="I66" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J66" s="11"/>
       <c r="K66" s="11"/>
       <c r="L66" s="11"/>
       <c r="M66" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N66" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O66" s="11"/>
     </row>
@@ -3694,14 +3699,14 @@
         <v>33</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C67" s="7"/>
       <c r="D67" s="31" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E67" s="29" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F67" s="20" t="s">
         <v>25</v>
@@ -3709,32 +3714,32 @@
       <c r="G67" s="21"/>
       <c r="H67" s="11"/>
       <c r="I67" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J67" s="11"/>
       <c r="K67" s="11"/>
       <c r="L67" s="11"/>
       <c r="M67" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N67" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O67" s="11"/>
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A68" s="17" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C68" s="7"/>
       <c r="D68" s="31" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E68" s="29" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="F68" s="20" t="s">
         <v>25</v>
@@ -3742,32 +3747,32 @@
       <c r="G68" s="21"/>
       <c r="H68" s="11"/>
       <c r="I68" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J68" s="11"/>
       <c r="K68" s="11"/>
       <c r="L68" s="11"/>
       <c r="M68" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N68" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O68" s="11"/>
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A69" s="17" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C69" s="7"/>
       <c r="D69" s="30" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E69" s="29" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F69" s="20" t="s">
         <v>25</v>
@@ -3775,32 +3780,32 @@
       <c r="G69" s="21"/>
       <c r="H69" s="11"/>
       <c r="I69" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J69" s="11"/>
       <c r="K69" s="11"/>
       <c r="L69" s="11"/>
       <c r="M69" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N69" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O69" s="11"/>
     </row>
     <row r="70" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A70" s="17" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C70" s="7"/>
       <c r="D70" s="30" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E70" s="29" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="F70" s="20" t="s">
         <v>25</v>
@@ -3808,16 +3813,16 @@
       <c r="G70" s="21"/>
       <c r="H70" s="11"/>
       <c r="I70" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J70" s="11"/>
       <c r="K70" s="11"/>
       <c r="L70" s="11"/>
       <c r="M70" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N70" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O70" s="11"/>
     </row>
@@ -3826,14 +3831,14 @@
         <v>34</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C71" s="7"/>
       <c r="D71" s="30" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E71" s="29" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="F71" s="20" t="s">
         <v>25</v>
@@ -3841,32 +3846,32 @@
       <c r="G71" s="21"/>
       <c r="H71" s="11"/>
       <c r="I71" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J71" s="11"/>
       <c r="K71" s="11"/>
       <c r="L71" s="11"/>
       <c r="M71" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N71" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O71" s="11"/>
     </row>
     <row r="72" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A72" s="17" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C72" s="7"/>
       <c r="D72" s="30" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E72" s="29" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="F72" s="20" t="s">
         <v>25</v>
@@ -3874,32 +3879,32 @@
       <c r="G72" s="21"/>
       <c r="H72" s="11"/>
       <c r="I72" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J72" s="11"/>
       <c r="K72" s="11"/>
       <c r="L72" s="11"/>
       <c r="M72" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N72" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O72" s="11"/>
     </row>
     <row r="73" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A73" s="17" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C73" s="7"/>
       <c r="D73" s="30" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E73" s="29" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F73" s="20" t="s">
         <v>25</v>
@@ -3907,32 +3912,32 @@
       <c r="G73" s="21"/>
       <c r="H73" s="11"/>
       <c r="I73" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J73" s="11"/>
       <c r="K73" s="11"/>
       <c r="L73" s="11"/>
       <c r="M73" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N73" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O73" s="11"/>
     </row>
     <row r="74" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A74" s="17" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C74" s="7"/>
       <c r="D74" s="30" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E74" s="29" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F74" s="20" t="s">
         <v>25</v>
@@ -3940,16 +3945,16 @@
       <c r="G74" s="21"/>
       <c r="H74" s="11"/>
       <c r="I74" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J74" s="11"/>
       <c r="K74" s="11"/>
       <c r="L74" s="11"/>
       <c r="M74" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N74" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O74" s="11"/>
     </row>
@@ -3958,14 +3963,14 @@
         <v>35</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C75" s="7"/>
       <c r="D75" s="30" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E75" s="29" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F75" s="20" t="s">
         <v>25</v>
@@ -3973,32 +3978,32 @@
       <c r="G75" s="21"/>
       <c r="H75" s="11"/>
       <c r="I75" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J75" s="11"/>
       <c r="K75" s="11"/>
       <c r="L75" s="11"/>
       <c r="M75" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N75" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O75" s="11"/>
     </row>
     <row r="76" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A76" s="17" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C76" s="7"/>
       <c r="D76" s="30" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E76" s="29" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="F76" s="20" t="s">
         <v>25</v>
@@ -4006,32 +4011,32 @@
       <c r="G76" s="21"/>
       <c r="H76" s="11"/>
       <c r="I76" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J76" s="11"/>
       <c r="K76" s="11"/>
       <c r="L76" s="11"/>
       <c r="M76" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N76" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O76" s="11"/>
     </row>
     <row r="77" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A77" s="17" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C77" s="7"/>
       <c r="D77" s="30" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E77" s="29" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F77" s="20" t="s">
         <v>25</v>
@@ -4039,32 +4044,32 @@
       <c r="G77" s="21"/>
       <c r="H77" s="11"/>
       <c r="I77" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J77" s="11"/>
       <c r="K77" s="11"/>
       <c r="L77" s="11"/>
       <c r="M77" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N77" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O77" s="11"/>
     </row>
     <row r="78" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A78" s="17" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C78" s="7"/>
       <c r="D78" s="30" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E78" s="29" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="F78" s="20" t="s">
         <v>25</v>
@@ -4072,16 +4077,16 @@
       <c r="G78" s="21"/>
       <c r="H78" s="11"/>
       <c r="I78" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J78" s="11"/>
       <c r="K78" s="11"/>
       <c r="L78" s="11"/>
       <c r="M78" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N78" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O78" s="11"/>
     </row>
@@ -4090,14 +4095,14 @@
         <v>36</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C79" s="7"/>
       <c r="D79" s="30" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E79" s="29" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F79" s="20" t="s">
         <v>25</v>
@@ -4105,32 +4110,32 @@
       <c r="G79" s="21"/>
       <c r="H79" s="11"/>
       <c r="I79" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J79" s="11"/>
       <c r="K79" s="11"/>
       <c r="L79" s="11"/>
       <c r="M79" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N79" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O79" s="11"/>
     </row>
     <row r="80" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A80" s="17" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B80" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C80" s="7"/>
       <c r="D80" s="30" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E80" s="29" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="F80" s="20" t="s">
         <v>25</v>
@@ -4138,32 +4143,32 @@
       <c r="G80" s="21"/>
       <c r="H80" s="11"/>
       <c r="I80" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J80" s="11"/>
       <c r="K80" s="11"/>
       <c r="L80" s="11"/>
       <c r="M80" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N80" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O80" s="11"/>
     </row>
     <row r="81" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A81" s="17" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B81" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C81" s="7"/>
       <c r="D81" s="30" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E81" s="29" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="F81" s="20" t="s">
         <v>25</v>
@@ -4171,32 +4176,32 @@
       <c r="G81" s="21"/>
       <c r="H81" s="11"/>
       <c r="I81" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J81" s="11"/>
       <c r="K81" s="11"/>
       <c r="L81" s="11"/>
       <c r="M81" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N81" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O81" s="11"/>
     </row>
     <row r="82" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A82" s="17" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B82" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C82" s="7"/>
       <c r="D82" s="30" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E82" s="29" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F82" s="20" t="s">
         <v>25</v>
@@ -4204,16 +4209,16 @@
       <c r="G82" s="21"/>
       <c r="H82" s="11"/>
       <c r="I82" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J82" s="11"/>
       <c r="K82" s="11"/>
       <c r="L82" s="11"/>
       <c r="M82" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N82" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O82" s="11"/>
     </row>
@@ -4222,14 +4227,14 @@
         <v>37</v>
       </c>
       <c r="B83" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C83" s="7"/>
       <c r="D83" s="30" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E83" s="29" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="F83" s="20" t="s">
         <v>25</v>
@@ -4237,32 +4242,32 @@
       <c r="G83" s="21"/>
       <c r="H83" s="11"/>
       <c r="I83" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J83" s="11"/>
       <c r="K83" s="11"/>
       <c r="L83" s="11"/>
       <c r="M83" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N83" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O83" s="11"/>
     </row>
     <row r="84" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A84" s="17" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B84" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C84" s="7"/>
       <c r="D84" s="30" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E84" s="29" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="F84" s="20" t="s">
         <v>25</v>
@@ -4270,32 +4275,32 @@
       <c r="G84" s="21"/>
       <c r="H84" s="11"/>
       <c r="I84" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J84" s="11"/>
       <c r="K84" s="11"/>
       <c r="L84" s="11"/>
       <c r="M84" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N84" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O84" s="11"/>
     </row>
     <row r="85" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A85" s="17" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C85" s="7"/>
       <c r="D85" s="30" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E85" s="29" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F85" s="20" t="s">
         <v>25</v>
@@ -4303,32 +4308,32 @@
       <c r="G85" s="21"/>
       <c r="H85" s="11"/>
       <c r="I85" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J85" s="11"/>
       <c r="K85" s="11"/>
       <c r="L85" s="11"/>
       <c r="M85" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N85" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O85" s="11"/>
     </row>
     <row r="86" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A86" s="17" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B86" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C86" s="7"/>
       <c r="D86" s="30" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E86" s="29" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="F86" s="20" t="s">
         <v>25</v>
@@ -4336,16 +4341,16 @@
       <c r="G86" s="21"/>
       <c r="H86" s="11"/>
       <c r="I86" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J86" s="11"/>
       <c r="K86" s="11"/>
       <c r="L86" s="11"/>
       <c r="M86" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N86" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O86" s="11"/>
     </row>
@@ -4354,31 +4359,31 @@
         <v>38</v>
       </c>
       <c r="B87" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C87" s="7"/>
       <c r="D87" s="14" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E87" s="27" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F87" s="20" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G87" s="21"/>
       <c r="H87" s="11"/>
       <c r="I87" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J87" s="11"/>
       <c r="K87" s="11"/>
       <c r="L87" s="11"/>
       <c r="M87" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N87" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O87" s="11"/>
     </row>
@@ -4387,14 +4392,14 @@
         <v>39</v>
       </c>
       <c r="B88" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C88" s="15"/>
       <c r="D88" s="16" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E88" s="27" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F88" s="20" t="s">
         <v>25</v>
@@ -4402,16 +4407,16 @@
       <c r="G88" s="21"/>
       <c r="H88" s="11"/>
       <c r="I88" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J88" s="11"/>
       <c r="K88" s="11"/>
       <c r="L88" s="11"/>
       <c r="M88" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N88" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O88" s="11"/>
     </row>
@@ -4420,14 +4425,14 @@
         <v>40</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C89" s="15"/>
       <c r="D89" s="16" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E89" s="27" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F89" s="20" t="s">
         <v>25</v>
@@ -4435,16 +4440,16 @@
       <c r="G89" s="21"/>
       <c r="H89" s="11"/>
       <c r="I89" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J89" s="11"/>
       <c r="K89" s="11"/>
       <c r="L89" s="11"/>
       <c r="M89" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N89" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O89" s="11"/>
     </row>
@@ -4453,49 +4458,49 @@
         <v>41</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C90" s="7"/>
       <c r="D90" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E90" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="F90" s="20" t="s">
         <v>33</v>
-      </c>
-      <c r="E90" s="27" t="s">
-        <v>62</v>
-      </c>
-      <c r="F90" s="20" t="s">
-        <v>32</v>
       </c>
       <c r="G90" s="21"/>
       <c r="H90" s="11"/>
       <c r="I90" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J90" s="11"/>
       <c r="K90" s="11"/>
       <c r="L90" s="11"/>
       <c r="M90" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N90" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O90" s="11"/>
     </row>
     <row r="91" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A91" s="17" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C91" s="7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D91" s="14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E91" s="27" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F91" s="20" t="s">
         <v>25</v>
@@ -4503,69 +4508,69 @@
       <c r="G91" s="21"/>
       <c r="H91" s="11"/>
       <c r="I91" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J91" s="11"/>
       <c r="K91" s="11"/>
       <c r="L91" s="11"/>
       <c r="M91" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N91" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O91" s="11"/>
     </row>
     <row r="92" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A92" s="17" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B92" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C92" s="7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D92" s="14" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E92" s="27" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F92" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G92" s="21"/>
       <c r="H92" s="11"/>
       <c r="I92" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J92" s="11"/>
       <c r="K92" s="11"/>
       <c r="L92" s="11"/>
       <c r="M92" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N92" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O92" s="11"/>
     </row>
     <row r="93" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A93" s="17" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B93" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C93" s="7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D93" s="14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E93" s="27" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F93" s="20" t="s">
         <v>25</v>
@@ -4573,69 +4578,69 @@
       <c r="G93" s="21"/>
       <c r="H93" s="11"/>
       <c r="I93" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J93" s="11"/>
       <c r="K93" s="11"/>
       <c r="L93" s="11"/>
       <c r="M93" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N93" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O93" s="11"/>
     </row>
     <row r="94" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A94" s="17" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B94" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C94" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D94" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="D94" s="14" t="s">
-        <v>36</v>
-      </c>
       <c r="E94" s="27" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F94" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G94" s="21"/>
       <c r="H94" s="11"/>
       <c r="I94" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J94" s="11"/>
       <c r="K94" s="11"/>
       <c r="L94" s="11"/>
       <c r="M94" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N94" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O94" s="11"/>
     </row>
     <row r="95" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A95" s="17" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B95" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C95" s="7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D95" s="14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E95" s="27" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F95" s="20" t="s">
         <v>25</v>
@@ -4643,102 +4648,102 @@
       <c r="G95" s="21"/>
       <c r="H95" s="11"/>
       <c r="I95" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J95" s="11"/>
       <c r="K95" s="11"/>
       <c r="L95" s="11"/>
       <c r="M95" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N95" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O95" s="11"/>
     </row>
     <row r="96" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A96" s="17" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B96" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C96" s="7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D96" s="14" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E96" s="27" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F96" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G96" s="21"/>
       <c r="H96" s="11"/>
       <c r="I96" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J96" s="11"/>
       <c r="K96" s="11"/>
       <c r="L96" s="11"/>
       <c r="M96" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N96" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O96" s="11"/>
     </row>
     <row r="97" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A97" s="17" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C97" s="7"/>
       <c r="D97" s="14" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E97" s="27" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F97" s="20" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G97" s="21"/>
       <c r="H97" s="11"/>
       <c r="I97" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J97" s="11"/>
       <c r="K97" s="11"/>
       <c r="L97" s="11"/>
       <c r="M97" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N97" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O97" s="11"/>
     </row>
     <row r="98" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A98" s="17" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B98" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C98" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D98" s="14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E98" s="27" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F98" s="20" t="s">
         <v>25</v>
@@ -4746,51 +4751,51 @@
       <c r="G98" s="21"/>
       <c r="H98" s="11"/>
       <c r="I98" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J98" s="11"/>
       <c r="K98" s="11"/>
       <c r="L98" s="11"/>
       <c r="M98" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N98" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O98" s="11"/>
     </row>
     <row r="99" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A99" s="17" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B99" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C99" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D99" s="14" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E99" s="27" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F99" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G99" s="21"/>
       <c r="H99" s="11"/>
       <c r="I99" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J99" s="11"/>
       <c r="K99" s="11"/>
       <c r="L99" s="11"/>
       <c r="M99" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N99" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O99" s="11"/>
     </row>
@@ -4799,14 +4804,14 @@
         <v>47</v>
       </c>
       <c r="B100" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C100" s="7"/>
       <c r="D100" s="28" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E100" s="29" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="F100" s="20" t="s">
         <v>25</v>
@@ -4814,16 +4819,16 @@
       <c r="G100" s="21"/>
       <c r="H100" s="18"/>
       <c r="I100" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J100" s="18"/>
       <c r="K100" s="18"/>
       <c r="L100" s="18"/>
       <c r="M100" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N100" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O100" s="18"/>
     </row>
@@ -4832,14 +4837,14 @@
         <v>48</v>
       </c>
       <c r="B101" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C101" s="7"/>
       <c r="D101" s="31" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E101" s="29" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="F101" s="20" t="s">
         <v>25</v>
@@ -4847,16 +4852,16 @@
       <c r="G101" s="21"/>
       <c r="H101" s="18"/>
       <c r="I101" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J101" s="18"/>
       <c r="K101" s="18"/>
       <c r="L101" s="18"/>
       <c r="M101" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N101" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O101" s="18"/>
     </row>
@@ -4865,14 +4870,14 @@
         <v>49</v>
       </c>
       <c r="B102" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C102" s="7"/>
       <c r="D102" s="30" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E102" s="29" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="F102" s="20" t="s">
         <v>25</v>
@@ -4880,16 +4885,16 @@
       <c r="G102" s="21"/>
       <c r="H102" s="18"/>
       <c r="I102" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J102" s="18"/>
       <c r="K102" s="18"/>
       <c r="L102" s="18"/>
       <c r="M102" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N102" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O102" s="18"/>
     </row>
@@ -4898,14 +4903,14 @@
         <v>50</v>
       </c>
       <c r="B103" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C103" s="7"/>
       <c r="D103" s="30" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E103" s="29" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="F103" s="20" t="s">
         <v>25</v>
@@ -4913,16 +4918,16 @@
       <c r="G103" s="21"/>
       <c r="H103" s="18"/>
       <c r="I103" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J103" s="18"/>
       <c r="K103" s="18"/>
       <c r="L103" s="18"/>
       <c r="M103" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N103" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O103" s="18"/>
     </row>
@@ -4931,14 +4936,14 @@
         <v>51</v>
       </c>
       <c r="B104" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C104" s="7"/>
       <c r="D104" s="30" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E104" s="29" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="F104" s="20" t="s">
         <v>25</v>
@@ -4946,16 +4951,16 @@
       <c r="G104" s="21"/>
       <c r="H104" s="18"/>
       <c r="I104" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J104" s="18"/>
       <c r="K104" s="18"/>
       <c r="L104" s="18"/>
       <c r="M104" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N104" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O104" s="18"/>
     </row>
@@ -4964,14 +4969,14 @@
         <v>52</v>
       </c>
       <c r="B105" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C105" s="7"/>
       <c r="D105" s="30" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E105" s="29" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="F105" s="20" t="s">
         <v>25</v>
@@ -4979,16 +4984,16 @@
       <c r="G105" s="21"/>
       <c r="H105" s="18"/>
       <c r="I105" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J105" s="18"/>
       <c r="K105" s="18"/>
       <c r="L105" s="18"/>
       <c r="M105" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N105" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O105" s="18"/>
     </row>
@@ -4997,31 +5002,31 @@
         <v>53</v>
       </c>
       <c r="B106" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C106" s="7"/>
       <c r="D106" s="14" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E106" s="27" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F106" s="20" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G106" s="21"/>
       <c r="H106" s="18"/>
       <c r="I106" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J106" s="18"/>
       <c r="K106" s="18"/>
       <c r="L106" s="18"/>
       <c r="M106" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N106" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O106" s="18"/>
     </row>
@@ -5030,14 +5035,14 @@
         <v>54</v>
       </c>
       <c r="B107" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C107" s="15"/>
       <c r="D107" s="16" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E107" s="27" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F107" s="20" t="s">
         <v>25</v>
@@ -5045,16 +5050,16 @@
       <c r="G107" s="21"/>
       <c r="H107" s="18"/>
       <c r="I107" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J107" s="18"/>
       <c r="K107" s="18"/>
       <c r="L107" s="18"/>
       <c r="M107" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N107" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O107" s="18"/>
     </row>
@@ -5063,14 +5068,14 @@
         <v>55</v>
       </c>
       <c r="B108" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C108" s="15"/>
       <c r="D108" s="16" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E108" s="27" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F108" s="20" t="s">
         <v>25</v>
@@ -5078,16 +5083,16 @@
       <c r="G108" s="21"/>
       <c r="H108" s="18"/>
       <c r="I108" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J108" s="18"/>
       <c r="K108" s="18"/>
       <c r="L108" s="18"/>
       <c r="M108" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N108" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O108" s="18"/>
     </row>

</xml_diff>